<commit_message>
master config changes and read pickle
</commit_message>
<xml_diff>
--- a/config/master_config.xlsx
+++ b/config/master_config.xlsx
@@ -5,12 +5,12 @@
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\APERC\9th_edition_visualisation\config\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\hyuga.kasai\Documents\Github\9th_Visualization\9th_edition_visualisation\config\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A60323E7-A1F5-46D2-BBD4-78F1CDCBD2E2}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{8612EEE1-723F-4FBB-8891-8FA4E6557CBE}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="1755" yWindow="-16320" windowWidth="29040" windowHeight="15840" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" tabRatio="812" firstSheet="1" activeTab="7" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="9th_EBT_schema" sheetId="7" r:id="rId1"/>
@@ -196,7 +196,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1489" uniqueCount="492">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1489" uniqueCount="494">
   <si>
     <t>chart_type</t>
   </si>
@@ -1672,13 +1672,19 @@
   </si>
   <si>
     <t>['2000', '2010', '2018', '2020', '2030', '2040', '2050', '2060', '2070']</t>
+  </si>
+  <si>
+    <t>Gas?</t>
+  </si>
+  <si>
+    <t>16_others_dummy</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="8" x14ac:knownFonts="1">
+  <fonts count="9" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -1735,8 +1741,15 @@
       <name val="Tahoma"/>
       <family val="2"/>
     </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF9C0006"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
   </fonts>
-  <fills count="9">
+  <fills count="10">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -1783,6 +1796,11 @@
       <patternFill patternType="solid">
         <fgColor rgb="FF00B050"/>
         <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFC7CE"/>
       </patternFill>
     </fill>
   </fills>
@@ -1847,10 +1865,11 @@
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="1">
+  <cellStyleXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="8" fillId="9" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="16">
+  <cellXfs count="17">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="top"/>
@@ -1879,8 +1898,10 @@
     <xf numFmtId="0" fontId="2" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="top"/>
     </xf>
+    <xf numFmtId="0" fontId="8" fillId="9" borderId="0" xfId="1"/>
   </cellXfs>
-  <cellStyles count="1">
+  <cellStyles count="2">
+    <cellStyle name="Bad" xfId="1" builtinId="27"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
@@ -3080,29 +3101,29 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{A000B41E-5923-4013-B542-E4247E89557C}">
   <dimension ref="A1:I102"/>
   <sheetViews>
-    <sheetView showGridLines="0" tabSelected="1" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <selection activeCell="D38" sqref="D38"/>
+    <sheetView showGridLines="0" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
+      <selection activeCell="C45" sqref="C45"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="12.81640625" customWidth="1"/>
+    <col min="1" max="1" width="12.85546875" customWidth="1"/>
     <col min="2" max="2" width="11" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="26.1796875" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="42.453125" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="33.54296875" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="45.1796875" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="41.1796875" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="28.54296875" bestFit="1" customWidth="1"/>
-    <col min="9" max="9" width="40.81640625" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="26.140625" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="42.42578125" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="33.5703125" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="45.140625" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="41.140625" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="28.5703125" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="40.85546875" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:9" x14ac:dyDescent="0.35">
+    <row r="1" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A1" s="8" t="s">
         <v>214</v>
       </c>
     </row>
-    <row r="3" spans="1:9" x14ac:dyDescent="0.35">
+    <row r="3" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A3" s="9" t="s">
         <v>215</v>
       </c>
@@ -3131,7 +3152,7 @@
         <v>218</v>
       </c>
     </row>
-    <row r="4" spans="1:9" x14ac:dyDescent="0.35">
+    <row r="4" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
         <v>219</v>
       </c>
@@ -3160,7 +3181,7 @@
         <v>224</v>
       </c>
     </row>
-    <row r="5" spans="1:9" x14ac:dyDescent="0.35">
+    <row r="5" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
         <v>225</v>
       </c>
@@ -3189,7 +3210,7 @@
         <v>230</v>
       </c>
     </row>
-    <row r="6" spans="1:9" x14ac:dyDescent="0.35">
+    <row r="6" spans="1:9" x14ac:dyDescent="0.25">
       <c r="B6" t="s">
         <v>231</v>
       </c>
@@ -3215,7 +3236,7 @@
         <v>234</v>
       </c>
     </row>
-    <row r="7" spans="1:9" x14ac:dyDescent="0.35">
+    <row r="7" spans="1:9" x14ac:dyDescent="0.25">
       <c r="B7" t="s">
         <v>235</v>
       </c>
@@ -3241,7 +3262,7 @@
         <v>239</v>
       </c>
     </row>
-    <row r="8" spans="1:9" x14ac:dyDescent="0.35">
+    <row r="8" spans="1:9" x14ac:dyDescent="0.25">
       <c r="B8" t="s">
         <v>240</v>
       </c>
@@ -3267,7 +3288,7 @@
         <v>244</v>
       </c>
     </row>
-    <row r="9" spans="1:9" x14ac:dyDescent="0.35">
+    <row r="9" spans="1:9" x14ac:dyDescent="0.25">
       <c r="B9" t="s">
         <v>245</v>
       </c>
@@ -3293,7 +3314,7 @@
         <v>250</v>
       </c>
     </row>
-    <row r="10" spans="1:9" x14ac:dyDescent="0.35">
+    <row r="10" spans="1:9" x14ac:dyDescent="0.25">
       <c r="B10" t="s">
         <v>251</v>
       </c>
@@ -3319,7 +3340,7 @@
         <v>254</v>
       </c>
     </row>
-    <row r="11" spans="1:9" x14ac:dyDescent="0.35">
+    <row r="11" spans="1:9" x14ac:dyDescent="0.25">
       <c r="B11" t="s">
         <v>255</v>
       </c>
@@ -3345,7 +3366,7 @@
         <v>258</v>
       </c>
     </row>
-    <row r="12" spans="1:9" x14ac:dyDescent="0.35">
+    <row r="12" spans="1:9" x14ac:dyDescent="0.25">
       <c r="B12" t="s">
         <v>259</v>
       </c>
@@ -3371,7 +3392,7 @@
         <v>262</v>
       </c>
     </row>
-    <row r="13" spans="1:9" x14ac:dyDescent="0.35">
+    <row r="13" spans="1:9" x14ac:dyDescent="0.25">
       <c r="B13" t="s">
         <v>263</v>
       </c>
@@ -3397,7 +3418,7 @@
         <v>266</v>
       </c>
     </row>
-    <row r="14" spans="1:9" x14ac:dyDescent="0.35">
+    <row r="14" spans="1:9" x14ac:dyDescent="0.25">
       <c r="B14" t="s">
         <v>267</v>
       </c>
@@ -3423,7 +3444,7 @@
         <v>270</v>
       </c>
     </row>
-    <row r="15" spans="1:9" x14ac:dyDescent="0.35">
+    <row r="15" spans="1:9" x14ac:dyDescent="0.25">
       <c r="B15" t="s">
         <v>271</v>
       </c>
@@ -3449,7 +3470,7 @@
         <v>274</v>
       </c>
     </row>
-    <row r="16" spans="1:9" x14ac:dyDescent="0.35">
+    <row r="16" spans="1:9" x14ac:dyDescent="0.25">
       <c r="B16" t="s">
         <v>275</v>
       </c>
@@ -3475,7 +3496,7 @@
         <v>278</v>
       </c>
     </row>
-    <row r="17" spans="2:9" x14ac:dyDescent="0.35">
+    <row r="17" spans="2:9" x14ac:dyDescent="0.25">
       <c r="B17" t="s">
         <v>279</v>
       </c>
@@ -3501,7 +3522,7 @@
         <v>282</v>
       </c>
     </row>
-    <row r="18" spans="2:9" x14ac:dyDescent="0.35">
+    <row r="18" spans="2:9" x14ac:dyDescent="0.25">
       <c r="B18" t="s">
         <v>283</v>
       </c>
@@ -3527,11 +3548,11 @@
         <v>286</v>
       </c>
     </row>
-    <row r="19" spans="2:9" x14ac:dyDescent="0.35">
+    <row r="19" spans="2:9" x14ac:dyDescent="0.25">
       <c r="B19" t="s">
         <v>287</v>
       </c>
-      <c r="C19" t="s">
+      <c r="C19" s="4" t="s">
         <v>100</v>
       </c>
       <c r="D19" t="s">
@@ -3553,7 +3574,7 @@
         <v>291</v>
       </c>
     </row>
-    <row r="20" spans="2:9" x14ac:dyDescent="0.35">
+    <row r="20" spans="2:9" x14ac:dyDescent="0.25">
       <c r="B20" t="s">
         <v>292</v>
       </c>
@@ -3579,7 +3600,7 @@
         <v>296</v>
       </c>
     </row>
-    <row r="21" spans="2:9" x14ac:dyDescent="0.35">
+    <row r="21" spans="2:9" x14ac:dyDescent="0.25">
       <c r="B21" t="s">
         <v>297</v>
       </c>
@@ -3605,7 +3626,7 @@
         <v>302</v>
       </c>
     </row>
-    <row r="22" spans="2:9" x14ac:dyDescent="0.35">
+    <row r="22" spans="2:9" x14ac:dyDescent="0.25">
       <c r="B22" t="s">
         <v>303</v>
       </c>
@@ -3631,7 +3652,7 @@
         <v>306</v>
       </c>
     </row>
-    <row r="23" spans="2:9" x14ac:dyDescent="0.35">
+    <row r="23" spans="2:9" x14ac:dyDescent="0.25">
       <c r="B23" t="s">
         <v>307</v>
       </c>
@@ -3654,7 +3675,7 @@
         <v>311</v>
       </c>
     </row>
-    <row r="24" spans="2:9" x14ac:dyDescent="0.35">
+    <row r="24" spans="2:9" x14ac:dyDescent="0.25">
       <c r="B24" t="s">
         <v>312</v>
       </c>
@@ -3677,7 +3698,7 @@
         <v>316</v>
       </c>
     </row>
-    <row r="25" spans="2:9" x14ac:dyDescent="0.35">
+    <row r="25" spans="2:9" x14ac:dyDescent="0.25">
       <c r="B25" t="s">
         <v>317</v>
       </c>
@@ -3697,7 +3718,7 @@
         <v>321</v>
       </c>
     </row>
-    <row r="26" spans="2:9" x14ac:dyDescent="0.35">
+    <row r="26" spans="2:9" x14ac:dyDescent="0.25">
       <c r="B26" t="s">
         <v>322</v>
       </c>
@@ -3717,7 +3738,7 @@
         <v>326</v>
       </c>
     </row>
-    <row r="27" spans="2:9" x14ac:dyDescent="0.35">
+    <row r="27" spans="2:9" x14ac:dyDescent="0.25">
       <c r="B27" t="s">
         <v>327</v>
       </c>
@@ -3737,7 +3758,7 @@
         <v>331</v>
       </c>
     </row>
-    <row r="28" spans="2:9" x14ac:dyDescent="0.35">
+    <row r="28" spans="2:9" x14ac:dyDescent="0.25">
       <c r="B28" t="s">
         <v>332</v>
       </c>
@@ -3757,7 +3778,7 @@
         <v>336</v>
       </c>
     </row>
-    <row r="29" spans="2:9" x14ac:dyDescent="0.35">
+    <row r="29" spans="2:9" x14ac:dyDescent="0.25">
       <c r="B29" t="s">
         <v>337</v>
       </c>
@@ -3777,7 +3798,7 @@
         <v>341</v>
       </c>
     </row>
-    <row r="30" spans="2:9" x14ac:dyDescent="0.35">
+    <row r="30" spans="2:9" x14ac:dyDescent="0.25">
       <c r="B30" t="s">
         <v>342</v>
       </c>
@@ -3797,7 +3818,7 @@
         <v>346</v>
       </c>
     </row>
-    <row r="31" spans="2:9" x14ac:dyDescent="0.35">
+    <row r="31" spans="2:9" x14ac:dyDescent="0.25">
       <c r="B31" t="s">
         <v>347</v>
       </c>
@@ -3817,7 +3838,7 @@
         <v>350</v>
       </c>
     </row>
-    <row r="32" spans="2:9" x14ac:dyDescent="0.35">
+    <row r="32" spans="2:9" x14ac:dyDescent="0.25">
       <c r="D32" t="s">
         <v>114</v>
       </c>
@@ -3834,7 +3855,7 @@
         <v>353</v>
       </c>
     </row>
-    <row r="33" spans="4:9" x14ac:dyDescent="0.35">
+    <row r="33" spans="4:9" x14ac:dyDescent="0.25">
       <c r="D33" t="s">
         <v>115</v>
       </c>
@@ -3851,7 +3872,7 @@
         <v>356</v>
       </c>
     </row>
-    <row r="34" spans="4:9" x14ac:dyDescent="0.35">
+    <row r="34" spans="4:9" x14ac:dyDescent="0.25">
       <c r="D34" t="s">
         <v>116</v>
       </c>
@@ -3868,7 +3889,7 @@
         <v>360</v>
       </c>
     </row>
-    <row r="35" spans="4:9" x14ac:dyDescent="0.35">
+    <row r="35" spans="4:9" x14ac:dyDescent="0.25">
       <c r="D35" t="s">
         <v>117</v>
       </c>
@@ -3885,7 +3906,7 @@
         <v>364</v>
       </c>
     </row>
-    <row r="36" spans="4:9" x14ac:dyDescent="0.35">
+    <row r="36" spans="4:9" x14ac:dyDescent="0.25">
       <c r="D36" t="s">
         <v>118</v>
       </c>
@@ -3902,7 +3923,7 @@
         <v>368</v>
       </c>
     </row>
-    <row r="37" spans="4:9" x14ac:dyDescent="0.35">
+    <row r="37" spans="4:9" x14ac:dyDescent="0.25">
       <c r="D37" t="s">
         <v>119</v>
       </c>
@@ -3919,7 +3940,7 @@
         <v>372</v>
       </c>
     </row>
-    <row r="38" spans="4:9" x14ac:dyDescent="0.35">
+    <row r="38" spans="4:9" x14ac:dyDescent="0.25">
       <c r="D38" t="s">
         <v>120</v>
       </c>
@@ -3936,7 +3957,7 @@
         <v>376</v>
       </c>
     </row>
-    <row r="39" spans="4:9" x14ac:dyDescent="0.35">
+    <row r="39" spans="4:9" x14ac:dyDescent="0.25">
       <c r="D39" t="s">
         <v>101</v>
       </c>
@@ -3953,7 +3974,7 @@
         <v>380</v>
       </c>
     </row>
-    <row r="40" spans="4:9" x14ac:dyDescent="0.35">
+    <row r="40" spans="4:9" x14ac:dyDescent="0.25">
       <c r="D40" t="s">
         <v>125</v>
       </c>
@@ -3970,7 +3991,7 @@
         <v>384</v>
       </c>
     </row>
-    <row r="41" spans="4:9" x14ac:dyDescent="0.35">
+    <row r="41" spans="4:9" x14ac:dyDescent="0.25">
       <c r="D41" t="s">
         <v>126</v>
       </c>
@@ -3987,7 +4008,7 @@
         <v>388</v>
       </c>
     </row>
-    <row r="42" spans="4:9" x14ac:dyDescent="0.35">
+    <row r="42" spans="4:9" x14ac:dyDescent="0.25">
       <c r="D42" t="s">
         <v>389</v>
       </c>
@@ -4004,7 +4025,7 @@
         <v>392</v>
       </c>
     </row>
-    <row r="43" spans="4:9" x14ac:dyDescent="0.35">
+    <row r="43" spans="4:9" x14ac:dyDescent="0.25">
       <c r="G43" t="s">
         <v>393</v>
       </c>
@@ -4015,7 +4036,7 @@
         <v>395</v>
       </c>
     </row>
-    <row r="44" spans="4:9" x14ac:dyDescent="0.35">
+    <row r="44" spans="4:9" x14ac:dyDescent="0.25">
       <c r="G44" t="s">
         <v>396</v>
       </c>
@@ -4026,7 +4047,7 @@
         <v>398</v>
       </c>
     </row>
-    <row r="45" spans="4:9" x14ac:dyDescent="0.35">
+    <row r="45" spans="4:9" x14ac:dyDescent="0.25">
       <c r="G45" t="s">
         <v>399</v>
       </c>
@@ -4037,7 +4058,7 @@
         <v>401</v>
       </c>
     </row>
-    <row r="46" spans="4:9" x14ac:dyDescent="0.35">
+    <row r="46" spans="4:9" x14ac:dyDescent="0.25">
       <c r="G46" t="s">
         <v>402</v>
       </c>
@@ -4048,7 +4069,7 @@
         <v>404</v>
       </c>
     </row>
-    <row r="47" spans="4:9" x14ac:dyDescent="0.35">
+    <row r="47" spans="4:9" x14ac:dyDescent="0.25">
       <c r="G47" t="s">
         <v>405</v>
       </c>
@@ -4059,7 +4080,7 @@
         <v>407</v>
       </c>
     </row>
-    <row r="48" spans="4:9" x14ac:dyDescent="0.35">
+    <row r="48" spans="4:9" x14ac:dyDescent="0.25">
       <c r="G48" t="s">
         <v>408</v>
       </c>
@@ -4070,7 +4091,7 @@
         <v>410</v>
       </c>
     </row>
-    <row r="49" spans="7:9" x14ac:dyDescent="0.35">
+    <row r="49" spans="7:9" x14ac:dyDescent="0.25">
       <c r="G49" t="s">
         <v>411</v>
       </c>
@@ -4081,7 +4102,7 @@
         <v>413</v>
       </c>
     </row>
-    <row r="50" spans="7:9" x14ac:dyDescent="0.35">
+    <row r="50" spans="7:9" x14ac:dyDescent="0.25">
       <c r="G50" t="s">
         <v>414</v>
       </c>
@@ -4092,7 +4113,7 @@
         <v>416</v>
       </c>
     </row>
-    <row r="51" spans="7:9" x14ac:dyDescent="0.35">
+    <row r="51" spans="7:9" x14ac:dyDescent="0.25">
       <c r="G51" t="s">
         <v>417</v>
       </c>
@@ -4103,7 +4124,7 @@
         <v>418</v>
       </c>
     </row>
-    <row r="52" spans="7:9" x14ac:dyDescent="0.35">
+    <row r="52" spans="7:9" x14ac:dyDescent="0.25">
       <c r="G52" t="s">
         <v>419</v>
       </c>
@@ -4111,252 +4132,252 @@
         <v>389</v>
       </c>
     </row>
-    <row r="53" spans="7:9" x14ac:dyDescent="0.35">
+    <row r="53" spans="7:9" x14ac:dyDescent="0.25">
       <c r="G53" t="s">
         <v>420</v>
       </c>
     </row>
-    <row r="54" spans="7:9" x14ac:dyDescent="0.35">
+    <row r="54" spans="7:9" x14ac:dyDescent="0.25">
       <c r="G54" t="s">
         <v>421</v>
       </c>
     </row>
-    <row r="55" spans="7:9" x14ac:dyDescent="0.35">
+    <row r="55" spans="7:9" x14ac:dyDescent="0.25">
       <c r="G55" t="s">
         <v>182</v>
       </c>
     </row>
-    <row r="56" spans="7:9" x14ac:dyDescent="0.35">
+    <row r="56" spans="7:9" x14ac:dyDescent="0.25">
       <c r="G56" t="s">
         <v>180</v>
       </c>
     </row>
-    <row r="57" spans="7:9" x14ac:dyDescent="0.35">
+    <row r="57" spans="7:9" x14ac:dyDescent="0.25">
       <c r="G57" t="s">
         <v>178</v>
       </c>
     </row>
-    <row r="58" spans="7:9" x14ac:dyDescent="0.35">
+    <row r="58" spans="7:9" x14ac:dyDescent="0.25">
       <c r="G58" t="s">
         <v>186</v>
       </c>
     </row>
-    <row r="59" spans="7:9" x14ac:dyDescent="0.35">
+    <row r="59" spans="7:9" x14ac:dyDescent="0.25">
       <c r="G59" t="s">
         <v>190</v>
       </c>
     </row>
-    <row r="60" spans="7:9" x14ac:dyDescent="0.35">
+    <row r="60" spans="7:9" x14ac:dyDescent="0.25">
       <c r="G60" t="s">
         <v>191</v>
       </c>
     </row>
-    <row r="61" spans="7:9" x14ac:dyDescent="0.35">
+    <row r="61" spans="7:9" x14ac:dyDescent="0.25">
       <c r="G61" t="s">
         <v>192</v>
       </c>
     </row>
-    <row r="62" spans="7:9" x14ac:dyDescent="0.35">
+    <row r="62" spans="7:9" x14ac:dyDescent="0.25">
       <c r="G62" t="s">
         <v>188</v>
       </c>
     </row>
-    <row r="63" spans="7:9" x14ac:dyDescent="0.35">
+    <row r="63" spans="7:9" x14ac:dyDescent="0.25">
       <c r="G63" t="s">
         <v>193</v>
       </c>
     </row>
-    <row r="64" spans="7:9" x14ac:dyDescent="0.35">
+    <row r="64" spans="7:9" x14ac:dyDescent="0.25">
       <c r="G64" t="s">
         <v>194</v>
       </c>
     </row>
-    <row r="65" spans="7:7" x14ac:dyDescent="0.35">
+    <row r="65" spans="7:7" x14ac:dyDescent="0.25">
       <c r="G65" t="s">
         <v>196</v>
       </c>
     </row>
-    <row r="66" spans="7:7" x14ac:dyDescent="0.35">
+    <row r="66" spans="7:7" x14ac:dyDescent="0.25">
       <c r="G66" t="s">
         <v>422</v>
       </c>
     </row>
-    <row r="67" spans="7:7" x14ac:dyDescent="0.35">
+    <row r="67" spans="7:7" x14ac:dyDescent="0.25">
       <c r="G67" t="s">
         <v>423</v>
       </c>
     </row>
-    <row r="68" spans="7:7" x14ac:dyDescent="0.35">
+    <row r="68" spans="7:7" x14ac:dyDescent="0.25">
       <c r="G68" t="s">
         <v>207</v>
       </c>
     </row>
-    <row r="69" spans="7:7" x14ac:dyDescent="0.35">
+    <row r="69" spans="7:7" x14ac:dyDescent="0.25">
       <c r="G69" t="s">
         <v>205</v>
       </c>
     </row>
-    <row r="70" spans="7:7" x14ac:dyDescent="0.35">
+    <row r="70" spans="7:7" x14ac:dyDescent="0.25">
       <c r="G70" t="s">
         <v>424</v>
       </c>
     </row>
-    <row r="71" spans="7:7" x14ac:dyDescent="0.35">
+    <row r="71" spans="7:7" x14ac:dyDescent="0.25">
       <c r="G71" t="s">
         <v>425</v>
       </c>
     </row>
-    <row r="72" spans="7:7" x14ac:dyDescent="0.35">
+    <row r="72" spans="7:7" x14ac:dyDescent="0.25">
       <c r="G72" t="s">
         <v>426</v>
       </c>
     </row>
-    <row r="73" spans="7:7" x14ac:dyDescent="0.35">
+    <row r="73" spans="7:7" x14ac:dyDescent="0.25">
       <c r="G73" t="s">
         <v>427</v>
       </c>
     </row>
-    <row r="74" spans="7:7" x14ac:dyDescent="0.35">
+    <row r="74" spans="7:7" x14ac:dyDescent="0.25">
       <c r="G74" t="s">
         <v>169</v>
       </c>
     </row>
-    <row r="75" spans="7:7" x14ac:dyDescent="0.35">
+    <row r="75" spans="7:7" x14ac:dyDescent="0.25">
       <c r="G75" t="s">
         <v>170</v>
       </c>
     </row>
-    <row r="76" spans="7:7" x14ac:dyDescent="0.35">
+    <row r="76" spans="7:7" x14ac:dyDescent="0.25">
       <c r="G76" t="s">
         <v>428</v>
       </c>
     </row>
-    <row r="77" spans="7:7" x14ac:dyDescent="0.35">
+    <row r="77" spans="7:7" x14ac:dyDescent="0.25">
       <c r="G77" t="s">
         <v>429</v>
       </c>
     </row>
-    <row r="78" spans="7:7" x14ac:dyDescent="0.35">
+    <row r="78" spans="7:7" x14ac:dyDescent="0.25">
       <c r="G78" t="s">
         <v>430</v>
       </c>
     </row>
-    <row r="79" spans="7:7" x14ac:dyDescent="0.35">
+    <row r="79" spans="7:7" x14ac:dyDescent="0.25">
       <c r="G79" t="s">
         <v>431</v>
       </c>
     </row>
-    <row r="80" spans="7:7" x14ac:dyDescent="0.35">
+    <row r="80" spans="7:7" x14ac:dyDescent="0.25">
       <c r="G80" t="s">
         <v>432</v>
       </c>
     </row>
-    <row r="81" spans="7:7" x14ac:dyDescent="0.35">
+    <row r="81" spans="7:7" x14ac:dyDescent="0.25">
       <c r="G81" t="s">
         <v>433</v>
       </c>
     </row>
-    <row r="82" spans="7:7" x14ac:dyDescent="0.35">
+    <row r="82" spans="7:7" x14ac:dyDescent="0.25">
       <c r="G82" t="s">
         <v>434</v>
       </c>
     </row>
-    <row r="83" spans="7:7" x14ac:dyDescent="0.35">
+    <row r="83" spans="7:7" x14ac:dyDescent="0.25">
       <c r="G83" t="s">
         <v>435</v>
       </c>
     </row>
-    <row r="84" spans="7:7" x14ac:dyDescent="0.35">
+    <row r="84" spans="7:7" x14ac:dyDescent="0.25">
       <c r="G84" t="s">
         <v>436</v>
       </c>
     </row>
-    <row r="85" spans="7:7" x14ac:dyDescent="0.35">
+    <row r="85" spans="7:7" x14ac:dyDescent="0.25">
       <c r="G85" t="s">
         <v>437</v>
       </c>
     </row>
-    <row r="86" spans="7:7" x14ac:dyDescent="0.35">
+    <row r="86" spans="7:7" x14ac:dyDescent="0.25">
       <c r="G86" t="s">
         <v>438</v>
       </c>
     </row>
-    <row r="87" spans="7:7" x14ac:dyDescent="0.35">
+    <row r="87" spans="7:7" x14ac:dyDescent="0.25">
       <c r="G87" t="s">
         <v>439</v>
       </c>
     </row>
-    <row r="88" spans="7:7" x14ac:dyDescent="0.35">
+    <row r="88" spans="7:7" x14ac:dyDescent="0.25">
       <c r="G88" t="s">
         <v>440</v>
       </c>
     </row>
-    <row r="89" spans="7:7" x14ac:dyDescent="0.35">
+    <row r="89" spans="7:7" x14ac:dyDescent="0.25">
       <c r="G89" t="s">
         <v>441</v>
       </c>
     </row>
-    <row r="90" spans="7:7" x14ac:dyDescent="0.35">
+    <row r="90" spans="7:7" x14ac:dyDescent="0.25">
       <c r="G90" t="s">
         <v>442</v>
       </c>
     </row>
-    <row r="91" spans="7:7" x14ac:dyDescent="0.35">
+    <row r="91" spans="7:7" x14ac:dyDescent="0.25">
       <c r="G91" t="s">
         <v>443</v>
       </c>
     </row>
-    <row r="92" spans="7:7" x14ac:dyDescent="0.35">
+    <row r="92" spans="7:7" x14ac:dyDescent="0.25">
       <c r="G92" t="s">
         <v>444</v>
       </c>
     </row>
-    <row r="93" spans="7:7" x14ac:dyDescent="0.35">
+    <row r="93" spans="7:7" x14ac:dyDescent="0.25">
       <c r="G93" t="s">
         <v>445</v>
       </c>
     </row>
-    <row r="94" spans="7:7" x14ac:dyDescent="0.35">
+    <row r="94" spans="7:7" x14ac:dyDescent="0.25">
       <c r="G94" t="s">
         <v>446</v>
       </c>
     </row>
-    <row r="95" spans="7:7" x14ac:dyDescent="0.35">
+    <row r="95" spans="7:7" x14ac:dyDescent="0.25">
       <c r="G95" t="s">
         <v>447</v>
       </c>
     </row>
-    <row r="96" spans="7:7" x14ac:dyDescent="0.35">
+    <row r="96" spans="7:7" x14ac:dyDescent="0.25">
       <c r="G96" t="s">
         <v>448</v>
       </c>
     </row>
-    <row r="97" spans="7:7" x14ac:dyDescent="0.35">
+    <row r="97" spans="7:7" x14ac:dyDescent="0.25">
       <c r="G97" t="s">
         <v>449</v>
       </c>
     </row>
-    <row r="98" spans="7:7" x14ac:dyDescent="0.35">
+    <row r="98" spans="7:7" x14ac:dyDescent="0.25">
       <c r="G98" t="s">
         <v>450</v>
       </c>
     </row>
-    <row r="99" spans="7:7" x14ac:dyDescent="0.35">
+    <row r="99" spans="7:7" x14ac:dyDescent="0.25">
       <c r="G99" t="s">
         <v>451</v>
       </c>
     </row>
-    <row r="100" spans="7:7" x14ac:dyDescent="0.35">
+    <row r="100" spans="7:7" x14ac:dyDescent="0.25">
       <c r="G100" t="s">
         <v>452</v>
       </c>
     </row>
-    <row r="101" spans="7:7" x14ac:dyDescent="0.35">
+    <row r="101" spans="7:7" x14ac:dyDescent="0.25">
       <c r="G101" t="s">
         <v>453</v>
       </c>
     </row>
-    <row r="102" spans="7:7" x14ac:dyDescent="0.35">
+    <row r="102" spans="7:7" x14ac:dyDescent="0.25">
       <c r="G102" t="s">
         <v>389</v>
       </c>
@@ -4375,20 +4396,20 @@
   <dimension ref="A1:D51"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="B34" sqref="B34"/>
+      <selection activeCell="C17" sqref="C17"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="62.1796875" customWidth="1"/>
-    <col min="2" max="2" width="64.81640625" customWidth="1"/>
-    <col min="3" max="3" width="43.81640625" customWidth="1"/>
-    <col min="12" max="12" width="19.81640625" customWidth="1"/>
-    <col min="13" max="13" width="27.1796875" customWidth="1"/>
+    <col min="1" max="1" width="62.140625" customWidth="1"/>
+    <col min="2" max="2" width="64.85546875" customWidth="1"/>
+    <col min="3" max="3" width="43.85546875" customWidth="1"/>
+    <col min="12" max="12" width="19.85546875" customWidth="1"/>
+    <col min="13" max="13" width="27.140625" customWidth="1"/>
     <col min="14" max="14" width="25" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="1" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
         <v>57</v>
       </c>
@@ -4402,7 +4423,7 @@
         <v>147</v>
       </c>
     </row>
-    <row r="2" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="2" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
         <v>21</v>
       </c>
@@ -4410,7 +4431,7 @@
         <v>148</v>
       </c>
     </row>
-    <row r="3" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="3" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
         <v>20</v>
       </c>
@@ -4418,7 +4439,7 @@
         <v>149</v>
       </c>
     </row>
-    <row r="4" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="4" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
         <v>19</v>
       </c>
@@ -4426,7 +4447,7 @@
         <v>150</v>
       </c>
     </row>
-    <row r="5" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="5" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
         <v>35</v>
       </c>
@@ -4434,7 +4455,7 @@
         <v>151</v>
       </c>
     </row>
-    <row r="6" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="6" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
         <v>35</v>
       </c>
@@ -4442,7 +4463,7 @@
         <v>152</v>
       </c>
     </row>
-    <row r="7" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="7" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
         <v>22</v>
       </c>
@@ -4450,7 +4471,7 @@
         <v>153</v>
       </c>
     </row>
-    <row r="8" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="8" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A8" t="s">
         <v>23</v>
       </c>
@@ -4458,7 +4479,7 @@
         <v>154</v>
       </c>
     </row>
-    <row r="9" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="9" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A9" t="s">
         <v>155</v>
       </c>
@@ -4466,7 +4487,7 @@
         <v>156</v>
       </c>
     </row>
-    <row r="10" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="10" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A10" t="s">
         <v>157</v>
       </c>
@@ -4474,7 +4495,7 @@
         <v>61</v>
       </c>
     </row>
-    <row r="11" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="11" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A11" t="s">
         <v>27</v>
       </c>
@@ -4482,7 +4503,7 @@
         <v>158</v>
       </c>
     </row>
-    <row r="12" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="12" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A12" t="s">
         <v>159</v>
       </c>
@@ -4490,7 +4511,7 @@
         <v>160</v>
       </c>
     </row>
-    <row r="13" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="13" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A13" t="s">
         <v>161</v>
       </c>
@@ -4498,7 +4519,7 @@
         <v>162</v>
       </c>
     </row>
-    <row r="14" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="14" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A14" t="s">
         <v>163</v>
       </c>
@@ -4506,7 +4527,7 @@
         <v>164</v>
       </c>
     </row>
-    <row r="15" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="15" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A15" t="s">
         <v>25</v>
       </c>
@@ -4514,7 +4535,7 @@
         <v>165</v>
       </c>
     </row>
-    <row r="16" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="16" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A16" t="s">
         <v>28</v>
       </c>
@@ -4522,23 +4543,23 @@
         <v>166</v>
       </c>
     </row>
-    <row r="17" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="17" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A17" t="s">
         <v>1</v>
       </c>
-      <c r="B17" t="s">
-        <v>100</v>
+      <c r="B17" s="16" t="s">
+        <v>493</v>
       </c>
       <c r="C17" t="s">
         <v>167</v>
       </c>
     </row>
-    <row r="18" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="18" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A18" t="s">
         <v>14</v>
       </c>
-      <c r="B18" t="s">
-        <v>100</v>
+      <c r="B18" s="16" t="s">
+        <v>493</v>
       </c>
       <c r="C18" t="s">
         <v>168</v>
@@ -4547,12 +4568,12 @@
         <v>169</v>
       </c>
     </row>
-    <row r="19" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="19" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A19" t="s">
         <v>13</v>
       </c>
-      <c r="B19" t="s">
-        <v>100</v>
+      <c r="B19" s="16" t="s">
+        <v>493</v>
       </c>
       <c r="C19" t="s">
         <v>168</v>
@@ -4561,29 +4582,29 @@
         <v>170</v>
       </c>
     </row>
-    <row r="20" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="20" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A20" t="s">
         <v>9</v>
       </c>
-      <c r="B20" t="s">
-        <v>100</v>
+      <c r="B20" s="16" t="s">
+        <v>493</v>
       </c>
       <c r="C20" t="s">
         <v>168</v>
       </c>
     </row>
-    <row r="21" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="21" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A21" s="4" t="s">
         <v>26</v>
       </c>
-      <c r="B21" t="s">
-        <v>100</v>
+      <c r="B21" s="16" t="s">
+        <v>493</v>
       </c>
       <c r="C21" t="s">
         <v>171</v>
       </c>
     </row>
-    <row r="22" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="22" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A22" s="4" t="s">
         <v>33</v>
       </c>
@@ -4591,7 +4612,7 @@
         <v>172</v>
       </c>
     </row>
-    <row r="23" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="23" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A23" t="s">
         <v>173</v>
       </c>
@@ -4599,7 +4620,7 @@
         <v>174</v>
       </c>
     </row>
-    <row r="24" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="24" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A24" t="s">
         <v>175</v>
       </c>
@@ -4607,7 +4628,7 @@
         <v>146</v>
       </c>
     </row>
-    <row r="25" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="25" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A25" t="s">
         <v>176</v>
       </c>
@@ -4621,7 +4642,7 @@
         <v>178</v>
       </c>
     </row>
-    <row r="26" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="26" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A26" t="s">
         <v>179</v>
       </c>
@@ -4635,7 +4656,7 @@
         <v>180</v>
       </c>
     </row>
-    <row r="27" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="27" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A27" t="s">
         <v>181</v>
       </c>
@@ -4649,7 +4670,7 @@
         <v>182</v>
       </c>
     </row>
-    <row r="28" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="28" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A28" t="s">
         <v>183</v>
       </c>
@@ -4660,7 +4681,7 @@
         <v>184</v>
       </c>
     </row>
-    <row r="29" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="29" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A29" t="s">
         <v>185</v>
       </c>
@@ -4674,7 +4695,7 @@
         <v>186</v>
       </c>
     </row>
-    <row r="30" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="30" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A30" t="s">
         <v>187</v>
       </c>
@@ -4688,7 +4709,7 @@
         <v>188</v>
       </c>
     </row>
-    <row r="31" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="31" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A31" t="s">
         <v>189</v>
       </c>
@@ -4702,7 +4723,7 @@
         <v>190</v>
       </c>
     </row>
-    <row r="32" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="32" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A32" t="s">
         <v>189</v>
       </c>
@@ -4716,7 +4737,7 @@
         <v>191</v>
       </c>
     </row>
-    <row r="33" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="33" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A33" t="s">
         <v>189</v>
       </c>
@@ -4730,7 +4751,7 @@
         <v>192</v>
       </c>
     </row>
-    <row r="34" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="34" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A34" t="s">
         <v>189</v>
       </c>
@@ -4744,7 +4765,7 @@
         <v>188</v>
       </c>
     </row>
-    <row r="35" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="35" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A35" t="s">
         <v>189</v>
       </c>
@@ -4758,7 +4779,7 @@
         <v>193</v>
       </c>
     </row>
-    <row r="36" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="36" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A36" t="s">
         <v>189</v>
       </c>
@@ -4772,7 +4793,7 @@
         <v>194</v>
       </c>
     </row>
-    <row r="37" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="37" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A37" s="7" t="s">
         <v>195</v>
       </c>
@@ -4786,7 +4807,7 @@
         <v>196</v>
       </c>
     </row>
-    <row r="38" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="38" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A38" t="s">
         <v>197</v>
       </c>
@@ -4797,7 +4818,7 @@
         <v>198</v>
       </c>
     </row>
-    <row r="39" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="39" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A39" t="s">
         <v>48</v>
       </c>
@@ -4808,7 +4829,7 @@
         <v>199</v>
       </c>
     </row>
-    <row r="40" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="40" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A40" t="s">
         <v>47</v>
       </c>
@@ -4819,7 +4840,7 @@
         <v>200</v>
       </c>
     </row>
-    <row r="41" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="41" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A41" t="s">
         <v>49</v>
       </c>
@@ -4830,7 +4851,7 @@
         <v>201</v>
       </c>
     </row>
-    <row r="42" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="42" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A42" t="s">
         <v>50</v>
       </c>
@@ -4841,7 +4862,7 @@
         <v>202</v>
       </c>
     </row>
-    <row r="43" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="43" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A43" t="s">
         <v>203</v>
       </c>
@@ -4855,7 +4876,7 @@
         <v>205</v>
       </c>
     </row>
-    <row r="44" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="44" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A44" t="s">
         <v>206</v>
       </c>
@@ -4869,7 +4890,7 @@
         <v>207</v>
       </c>
     </row>
-    <row r="45" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="45" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A45" t="s">
         <v>208</v>
       </c>
@@ -4880,7 +4901,7 @@
         <v>209</v>
       </c>
     </row>
-    <row r="46" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="46" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A46" t="s">
         <v>488</v>
       </c>
@@ -4888,7 +4909,7 @@
         <v>164</v>
       </c>
     </row>
-    <row r="47" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="47" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A47" t="s">
         <v>41</v>
       </c>
@@ -4896,7 +4917,7 @@
         <v>149</v>
       </c>
     </row>
-    <row r="48" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="48" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A48" t="s">
         <v>41</v>
       </c>
@@ -4904,7 +4925,7 @@
         <v>150</v>
       </c>
     </row>
-    <row r="49" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="49" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A49" t="s">
         <v>51</v>
       </c>
@@ -4915,7 +4936,7 @@
         <v>204</v>
       </c>
     </row>
-    <row r="50" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="50" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A50" t="s">
         <v>210</v>
       </c>
@@ -4923,7 +4944,7 @@
         <v>211</v>
       </c>
     </row>
-    <row r="51" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="51" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A51" t="s">
         <v>212</v>
       </c>
@@ -4947,17 +4968,17 @@
   <dimension ref="A1:C89"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="D20" sqref="D20:D21"/>
+      <selection activeCell="C21" sqref="C21"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="57.81640625" customWidth="1"/>
-    <col min="2" max="2" width="36.54296875" customWidth="1"/>
-    <col min="3" max="3" width="29.1796875" customWidth="1"/>
+    <col min="1" max="1" width="57.85546875" customWidth="1"/>
+    <col min="2" max="2" width="36.5703125" customWidth="1"/>
+    <col min="3" max="3" width="29.140625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="1" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
         <v>76</v>
       </c>
@@ -4968,7 +4989,7 @@
         <v>78</v>
       </c>
     </row>
-    <row r="2" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="2" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
         <v>11</v>
       </c>
@@ -4976,7 +4997,7 @@
         <v>79</v>
       </c>
     </row>
-    <row r="3" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="3" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
         <v>11</v>
       </c>
@@ -4984,7 +5005,7 @@
         <v>80</v>
       </c>
     </row>
-    <row r="4" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="4" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
         <v>11</v>
       </c>
@@ -4992,7 +5013,7 @@
         <v>81</v>
       </c>
     </row>
-    <row r="5" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="5" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
         <v>11</v>
       </c>
@@ -5000,7 +5021,7 @@
         <v>82</v>
       </c>
     </row>
-    <row r="6" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="6" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
         <v>5</v>
       </c>
@@ -5008,7 +5029,7 @@
         <v>83</v>
       </c>
     </row>
-    <row r="7" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="7" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
         <v>5</v>
       </c>
@@ -5016,7 +5037,7 @@
         <v>84</v>
       </c>
     </row>
-    <row r="8" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="8" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A8" t="s">
         <v>5</v>
       </c>
@@ -5024,7 +5045,7 @@
         <v>85</v>
       </c>
     </row>
-    <row r="9" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="9" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A9" t="s">
         <v>4</v>
       </c>
@@ -5032,7 +5053,7 @@
         <v>86</v>
       </c>
     </row>
-    <row r="10" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="10" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A10" t="s">
         <v>87</v>
       </c>
@@ -5040,7 +5061,7 @@
         <v>88</v>
       </c>
     </row>
-    <row r="11" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="11" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A11" t="s">
         <v>89</v>
       </c>
@@ -5048,7 +5069,7 @@
         <v>90</v>
       </c>
     </row>
-    <row r="12" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="12" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A12" t="s">
         <v>91</v>
       </c>
@@ -5056,7 +5077,7 @@
         <v>92</v>
       </c>
     </row>
-    <row r="13" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="13" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A13" t="s">
         <v>93</v>
       </c>
@@ -5064,7 +5085,7 @@
         <v>94</v>
       </c>
     </row>
-    <row r="14" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="14" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A14" t="s">
         <v>95</v>
       </c>
@@ -5072,7 +5093,7 @@
         <v>96</v>
       </c>
     </row>
-    <row r="15" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="15" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A15" t="s">
         <v>97</v>
       </c>
@@ -5080,7 +5101,7 @@
         <v>98</v>
       </c>
     </row>
-    <row r="16" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="16" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A16" t="s">
         <v>10</v>
       </c>
@@ -5088,7 +5109,7 @@
         <v>99</v>
       </c>
     </row>
-    <row r="17" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="17" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A17" t="s">
         <v>31</v>
       </c>
@@ -5099,7 +5120,7 @@
         <v>101</v>
       </c>
     </row>
-    <row r="18" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="18" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A18" t="s">
         <v>3</v>
       </c>
@@ -5107,7 +5128,7 @@
         <v>102</v>
       </c>
     </row>
-    <row r="19" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="19" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A19" t="s">
         <v>103</v>
       </c>
@@ -5115,7 +5136,7 @@
         <v>104</v>
       </c>
     </row>
-    <row r="20" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="20" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A20" t="s">
         <v>487</v>
       </c>
@@ -5123,7 +5144,7 @@
         <v>105</v>
       </c>
     </row>
-    <row r="21" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="21" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A21" t="s">
         <v>106</v>
       </c>
@@ -5131,7 +5152,7 @@
         <v>107</v>
       </c>
     </row>
-    <row r="22" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="22" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A22" t="s">
         <v>108</v>
       </c>
@@ -5139,7 +5160,7 @@
         <v>109</v>
       </c>
     </row>
-    <row r="23" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="23" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A23" t="s">
         <v>110</v>
       </c>
@@ -5147,7 +5168,7 @@
         <v>99</v>
       </c>
     </row>
-    <row r="24" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="24" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A24" t="s">
         <v>111</v>
       </c>
@@ -5155,7 +5176,7 @@
         <v>102</v>
       </c>
     </row>
-    <row r="25" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="25" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A25" t="s">
         <v>111</v>
       </c>
@@ -5163,7 +5184,7 @@
         <v>104</v>
       </c>
     </row>
-    <row r="26" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="26" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A26" s="4" t="s">
         <v>112</v>
       </c>
@@ -5171,7 +5192,7 @@
         <v>99</v>
       </c>
     </row>
-    <row r="27" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="27" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A27" s="4" t="s">
         <v>112</v>
       </c>
@@ -5182,7 +5203,7 @@
         <v>113</v>
       </c>
     </row>
-    <row r="28" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="28" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A28" s="4" t="s">
         <v>112</v>
       </c>
@@ -5193,7 +5214,7 @@
         <v>114</v>
       </c>
     </row>
-    <row r="29" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="29" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A29" s="4" t="s">
         <v>112</v>
       </c>
@@ -5204,7 +5225,7 @@
         <v>115</v>
       </c>
     </row>
-    <row r="30" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="30" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A30" s="4" t="s">
         <v>112</v>
       </c>
@@ -5215,7 +5236,7 @@
         <v>116</v>
       </c>
     </row>
-    <row r="31" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="31" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A31" s="4" t="s">
         <v>112</v>
       </c>
@@ -5226,7 +5247,7 @@
         <v>117</v>
       </c>
     </row>
-    <row r="32" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="32" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A32" s="4" t="s">
         <v>112</v>
       </c>
@@ -5237,7 +5258,7 @@
         <v>118</v>
       </c>
     </row>
-    <row r="33" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="33" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A33" s="4" t="s">
         <v>112</v>
       </c>
@@ -5248,7 +5269,7 @@
         <v>119</v>
       </c>
     </row>
-    <row r="34" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="34" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A34" s="4" t="s">
         <v>112</v>
       </c>
@@ -5259,7 +5280,7 @@
         <v>120</v>
       </c>
     </row>
-    <row r="35" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="35" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A35" s="4" t="s">
         <v>112</v>
       </c>
@@ -5270,7 +5291,7 @@
         <v>101</v>
       </c>
     </row>
-    <row r="36" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="36" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A36" t="s">
         <v>17</v>
       </c>
@@ -5281,7 +5302,7 @@
         <v>121</v>
       </c>
     </row>
-    <row r="37" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="37" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A37" t="s">
         <v>18</v>
       </c>
@@ -5292,7 +5313,7 @@
         <v>122</v>
       </c>
     </row>
-    <row r="38" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="38" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A38" t="s">
         <v>16</v>
       </c>
@@ -5303,7 +5324,7 @@
         <v>123</v>
       </c>
     </row>
-    <row r="39" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="39" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A39" t="s">
         <v>42</v>
       </c>
@@ -5311,7 +5332,7 @@
         <v>84</v>
       </c>
     </row>
-    <row r="40" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="40" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A40" t="s">
         <v>124</v>
       </c>
@@ -5319,7 +5340,7 @@
         <v>84</v>
       </c>
     </row>
-    <row r="41" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="41" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A41" t="s">
         <v>12</v>
       </c>
@@ -5330,7 +5351,7 @@
         <v>113</v>
       </c>
     </row>
-    <row r="42" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="42" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A42" t="s">
         <v>12</v>
       </c>
@@ -5341,7 +5362,7 @@
         <v>114</v>
       </c>
     </row>
-    <row r="43" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="43" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A43" t="s">
         <v>12</v>
       </c>
@@ -5352,7 +5373,7 @@
         <v>115</v>
       </c>
     </row>
-    <row r="44" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="44" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A44" t="s">
         <v>12</v>
       </c>
@@ -5363,7 +5384,7 @@
         <v>116</v>
       </c>
     </row>
-    <row r="45" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="45" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A45" t="s">
         <v>12</v>
       </c>
@@ -5374,7 +5395,7 @@
         <v>117</v>
       </c>
     </row>
-    <row r="46" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="46" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A46" t="s">
         <v>12</v>
       </c>
@@ -5385,7 +5406,7 @@
         <v>118</v>
       </c>
     </row>
-    <row r="47" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="47" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A47" t="s">
         <v>12</v>
       </c>
@@ -5396,7 +5417,7 @@
         <v>119</v>
       </c>
     </row>
-    <row r="48" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="48" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A48" t="s">
         <v>12</v>
       </c>
@@ -5407,7 +5428,7 @@
         <v>120</v>
       </c>
     </row>
-    <row r="49" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="49" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A49" t="s">
         <v>12</v>
       </c>
@@ -5418,7 +5439,7 @@
         <v>101</v>
       </c>
     </row>
-    <row r="50" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="50" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A50" t="s">
         <v>30</v>
       </c>
@@ -5429,7 +5450,7 @@
         <v>125</v>
       </c>
     </row>
-    <row r="51" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="51" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A51" t="s">
         <v>30</v>
       </c>
@@ -5440,7 +5461,7 @@
         <v>126</v>
       </c>
     </row>
-    <row r="52" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="52" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A52" t="s">
         <v>127</v>
       </c>
@@ -5451,7 +5472,7 @@
         <v>128</v>
       </c>
     </row>
-    <row r="53" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="53" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A53" t="s">
         <v>129</v>
       </c>
@@ -5462,7 +5483,7 @@
         <v>130</v>
       </c>
     </row>
-    <row r="54" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="54" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A54" t="s">
         <v>131</v>
       </c>
@@ -5473,9 +5494,9 @@
         <v>132</v>
       </c>
     </row>
-    <row r="55" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="55" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A55" s="4" t="s">
-        <v>4</v>
+        <v>492</v>
       </c>
       <c r="B55" t="s">
         <v>85</v>
@@ -5484,7 +5505,7 @@
         <v>133</v>
       </c>
     </row>
-    <row r="56" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="56" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A56" t="s">
         <v>134</v>
       </c>
@@ -5495,7 +5516,7 @@
         <v>135</v>
       </c>
     </row>
-    <row r="57" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="57" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A57" t="s">
         <v>134</v>
       </c>
@@ -5506,7 +5527,7 @@
         <v>136</v>
       </c>
     </row>
-    <row r="58" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="58" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A58" s="5" t="s">
         <v>37</v>
       </c>
@@ -5517,7 +5538,7 @@
         <v>125</v>
       </c>
     </row>
-    <row r="59" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="59" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A59" s="12" t="s">
         <v>30</v>
       </c>
@@ -5528,7 +5549,7 @@
         <v>126</v>
       </c>
     </row>
-    <row r="60" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="60" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A60" t="s">
         <v>43</v>
       </c>
@@ -5539,7 +5560,7 @@
         <v>130</v>
       </c>
     </row>
-    <row r="61" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="61" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A61" t="s">
         <v>43</v>
       </c>
@@ -5550,7 +5571,7 @@
         <v>135</v>
       </c>
     </row>
-    <row r="62" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="62" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A62" t="s">
         <v>43</v>
       </c>
@@ -5561,7 +5582,7 @@
         <v>137</v>
       </c>
     </row>
-    <row r="63" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="63" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A63" t="s">
         <v>43</v>
       </c>
@@ -5572,7 +5593,7 @@
         <v>136</v>
       </c>
     </row>
-    <row r="64" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="64" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A64" t="s">
         <v>43</v>
       </c>
@@ -5583,7 +5604,7 @@
         <v>138</v>
       </c>
     </row>
-    <row r="65" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="65" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A65" t="s">
         <v>43</v>
       </c>
@@ -5594,7 +5615,7 @@
         <v>128</v>
       </c>
     </row>
-    <row r="66" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="66" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A66" t="s">
         <v>43</v>
       </c>
@@ -5605,7 +5626,7 @@
         <v>139</v>
       </c>
     </row>
-    <row r="67" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="67" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A67" t="s">
         <v>43</v>
       </c>
@@ -5616,7 +5637,7 @@
         <v>132</v>
       </c>
     </row>
-    <row r="68" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="68" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A68" t="s">
         <v>43</v>
       </c>
@@ -5627,7 +5648,7 @@
         <v>140</v>
       </c>
     </row>
-    <row r="69" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="69" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A69" t="s">
         <v>43</v>
       </c>
@@ -5638,7 +5659,7 @@
         <v>141</v>
       </c>
     </row>
-    <row r="70" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="70" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A70" t="s">
         <v>43</v>
       </c>
@@ -5649,7 +5670,7 @@
         <v>142</v>
       </c>
     </row>
-    <row r="71" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="71" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A71" t="s">
         <v>143</v>
       </c>
@@ -5660,7 +5681,7 @@
         <v>139</v>
       </c>
     </row>
-    <row r="72" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="72" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A72" t="s">
         <v>144</v>
       </c>
@@ -5671,7 +5692,7 @@
         <v>119</v>
       </c>
     </row>
-    <row r="73" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="73" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A73" t="s">
         <v>145</v>
       </c>
@@ -5679,7 +5700,7 @@
         <v>99</v>
       </c>
     </row>
-    <row r="74" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="74" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A74" t="s">
         <v>145</v>
       </c>
@@ -5690,7 +5711,7 @@
         <v>113</v>
       </c>
     </row>
-    <row r="75" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="75" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A75" t="s">
         <v>145</v>
       </c>
@@ -5701,7 +5722,7 @@
         <v>115</v>
       </c>
     </row>
-    <row r="76" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="76" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A76" t="s">
         <v>145</v>
       </c>
@@ -5712,7 +5733,7 @@
         <v>117</v>
       </c>
     </row>
-    <row r="77" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="77" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A77" t="s">
         <v>145</v>
       </c>
@@ -5723,7 +5744,7 @@
         <v>118</v>
       </c>
     </row>
-    <row r="78" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="78" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A78" t="s">
         <v>145</v>
       </c>
@@ -5734,7 +5755,7 @@
         <v>119</v>
       </c>
     </row>
-    <row r="79" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="79" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A79" t="s">
         <v>145</v>
       </c>
@@ -5745,13 +5766,13 @@
         <v>120</v>
       </c>
     </row>
-    <row r="87" spans="2:2" x14ac:dyDescent="0.35">
+    <row r="87" spans="2:2" x14ac:dyDescent="0.25">
       <c r="B87" s="6"/>
     </row>
-    <row r="88" spans="2:2" x14ac:dyDescent="0.35">
+    <row r="88" spans="2:2" x14ac:dyDescent="0.25">
       <c r="B88" s="6"/>
     </row>
-    <row r="89" spans="2:2" x14ac:dyDescent="0.35">
+    <row r="89" spans="2:2" x14ac:dyDescent="0.25">
       <c r="B89" s="6"/>
     </row>
   </sheetData>
@@ -5773,15 +5794,15 @@
       <selection activeCell="B13" activeCellId="1" sqref="B26 B13"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="33.453125" customWidth="1"/>
-    <col min="2" max="2" width="47.1796875" customWidth="1"/>
-    <col min="3" max="3" width="50.1796875" customWidth="1"/>
+    <col min="1" max="1" width="33.42578125" customWidth="1"/>
+    <col min="2" max="2" width="47.140625" customWidth="1"/>
+    <col min="3" max="3" width="50.140625" customWidth="1"/>
     <col min="4" max="4" width="69" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="1" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
         <v>56</v>
       </c>
@@ -5795,7 +5816,7 @@
         <v>59</v>
       </c>
     </row>
-    <row r="2" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="2" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A2" t="b">
         <v>1</v>
       </c>
@@ -5809,7 +5830,7 @@
         <v>62</v>
       </c>
     </row>
-    <row r="3" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="3" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A3" t="b">
         <v>1</v>
       </c>
@@ -5823,7 +5844,7 @@
         <v>63</v>
       </c>
     </row>
-    <row r="4" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="4" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A4" t="b">
         <v>1</v>
       </c>
@@ -5837,7 +5858,7 @@
         <v>64</v>
       </c>
     </row>
-    <row r="5" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="5" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A5" t="b">
         <v>1</v>
       </c>
@@ -5851,7 +5872,7 @@
         <v>65</v>
       </c>
     </row>
-    <row r="6" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="6" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A6" t="b">
         <v>1</v>
       </c>
@@ -5865,7 +5886,7 @@
         <v>67</v>
       </c>
     </row>
-    <row r="7" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="7" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A7" t="b">
         <v>1</v>
       </c>
@@ -5879,7 +5900,7 @@
         <v>68</v>
       </c>
     </row>
-    <row r="8" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="8" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A8" t="b">
         <v>1</v>
       </c>
@@ -5893,7 +5914,7 @@
         <v>69</v>
       </c>
     </row>
-    <row r="9" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="9" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A9" t="b">
         <v>1</v>
       </c>
@@ -5907,7 +5928,7 @@
         <v>70</v>
       </c>
     </row>
-    <row r="10" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="10" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A10" t="b">
         <v>1</v>
       </c>
@@ -5921,7 +5942,7 @@
         <v>71</v>
       </c>
     </row>
-    <row r="11" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="11" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A11" t="b">
         <v>1</v>
       </c>
@@ -5935,7 +5956,7 @@
         <v>72</v>
       </c>
     </row>
-    <row r="12" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="12" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A12" t="b">
         <v>1</v>
       </c>
@@ -5949,7 +5970,7 @@
         <v>73</v>
       </c>
     </row>
-    <row r="13" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="13" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A13" t="b">
         <v>1</v>
       </c>
@@ -5963,7 +5984,7 @@
         <v>74</v>
       </c>
     </row>
-    <row r="14" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="14" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A14" t="b">
         <v>1</v>
       </c>
@@ -5977,7 +5998,7 @@
         <v>75</v>
       </c>
     </row>
-    <row r="15" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="15" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A15" t="b">
         <v>0</v>
       </c>
@@ -5991,7 +6012,7 @@
         <v>62</v>
       </c>
     </row>
-    <row r="16" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="16" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A16" t="b">
         <v>0</v>
       </c>
@@ -6005,7 +6026,7 @@
         <v>63</v>
       </c>
     </row>
-    <row r="17" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="17" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A17" t="b">
         <v>0</v>
       </c>
@@ -6019,7 +6040,7 @@
         <v>64</v>
       </c>
     </row>
-    <row r="18" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="18" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A18" t="b">
         <v>0</v>
       </c>
@@ -6033,7 +6054,7 @@
         <v>65</v>
       </c>
     </row>
-    <row r="19" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="19" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A19" t="b">
         <v>0</v>
       </c>
@@ -6047,7 +6068,7 @@
         <v>67</v>
       </c>
     </row>
-    <row r="20" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="20" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A20" t="b">
         <v>0</v>
       </c>
@@ -6061,7 +6082,7 @@
         <v>68</v>
       </c>
     </row>
-    <row r="21" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="21" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A21" t="b">
         <v>0</v>
       </c>
@@ -6075,7 +6096,7 @@
         <v>69</v>
       </c>
     </row>
-    <row r="22" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="22" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A22" t="b">
         <v>0</v>
       </c>
@@ -6089,7 +6110,7 @@
         <v>70</v>
       </c>
     </row>
-    <row r="23" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="23" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A23" t="b">
         <v>0</v>
       </c>
@@ -6103,7 +6124,7 @@
         <v>71</v>
       </c>
     </row>
-    <row r="24" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="24" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A24" t="b">
         <v>0</v>
       </c>
@@ -6117,7 +6138,7 @@
         <v>72</v>
       </c>
     </row>
-    <row r="25" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="25" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A25" t="b">
         <v>0</v>
       </c>
@@ -6131,7 +6152,7 @@
         <v>73</v>
       </c>
     </row>
-    <row r="26" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="26" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A26" t="b">
         <v>0</v>
       </c>
@@ -6145,7 +6166,7 @@
         <v>74</v>
       </c>
     </row>
-    <row r="27" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="27" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A27" t="b">
         <v>0</v>
       </c>
@@ -6171,15 +6192,15 @@
   <dimension ref="A1:B29"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="A28" sqref="A28"/>
+      <selection activeCell="A21" sqref="A21"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="19.81640625" customWidth="1"/>
+    <col min="1" max="1" width="19.85546875" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="1" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
         <v>474</v>
       </c>
@@ -6187,7 +6208,7 @@
         <v>477</v>
       </c>
     </row>
-    <row r="2" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="2" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
         <v>481</v>
       </c>
@@ -6195,7 +6216,7 @@
         <v>60</v>
       </c>
     </row>
-    <row r="3" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="3" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
         <v>481</v>
       </c>
@@ -6203,7 +6224,7 @@
         <v>60</v>
       </c>
     </row>
-    <row r="4" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="4" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
         <v>481</v>
       </c>
@@ -6211,7 +6232,7 @@
         <v>60</v>
       </c>
     </row>
-    <row r="5" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="5" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
         <v>481</v>
       </c>
@@ -6219,7 +6240,7 @@
         <v>60</v>
       </c>
     </row>
-    <row r="6" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="6" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
         <v>482</v>
       </c>
@@ -6227,7 +6248,7 @@
         <v>66</v>
       </c>
     </row>
-    <row r="7" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="7" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
         <v>482</v>
       </c>
@@ -6235,7 +6256,7 @@
         <v>66</v>
       </c>
     </row>
-    <row r="8" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="8" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A8" t="s">
         <v>482</v>
       </c>
@@ -6243,7 +6264,7 @@
         <v>66</v>
       </c>
     </row>
-    <row r="9" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="9" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A9" t="s">
         <v>482</v>
       </c>
@@ -6251,7 +6272,7 @@
         <v>66</v>
       </c>
     </row>
-    <row r="10" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="10" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A10" t="s">
         <v>482</v>
       </c>
@@ -6259,7 +6280,7 @@
         <v>66</v>
       </c>
     </row>
-    <row r="11" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="11" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A11" t="s">
         <v>482</v>
       </c>
@@ -6267,7 +6288,7 @@
         <v>66</v>
       </c>
     </row>
-    <row r="12" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="12" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A12" t="s">
         <v>482</v>
       </c>
@@ -6275,7 +6296,7 @@
         <v>66</v>
       </c>
     </row>
-    <row r="13" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="13" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A13" t="s">
         <v>483</v>
       </c>
@@ -6283,7 +6304,7 @@
         <v>30</v>
       </c>
     </row>
-    <row r="14" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="14" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A14" t="s">
         <v>486</v>
       </c>
@@ -6291,7 +6312,7 @@
         <v>60</v>
       </c>
     </row>
-    <row r="15" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="15" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A15" t="s">
         <v>478</v>
       </c>
@@ -6299,7 +6320,7 @@
         <v>60</v>
       </c>
     </row>
-    <row r="16" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="16" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A16" t="s">
         <v>478</v>
       </c>
@@ -6307,7 +6328,7 @@
         <v>60</v>
       </c>
     </row>
-    <row r="17" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="17" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A17" t="s">
         <v>478</v>
       </c>
@@ -6315,7 +6336,7 @@
         <v>60</v>
       </c>
     </row>
-    <row r="18" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="18" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A18" t="s">
         <v>478</v>
       </c>
@@ -6323,7 +6344,7 @@
         <v>60</v>
       </c>
     </row>
-    <row r="19" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="19" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A19" t="s">
         <v>479</v>
       </c>
@@ -6331,7 +6352,7 @@
         <v>66</v>
       </c>
     </row>
-    <row r="20" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="20" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A20" t="s">
         <v>479</v>
       </c>
@@ -6339,7 +6360,7 @@
         <v>66</v>
       </c>
     </row>
-    <row r="21" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="21" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A21" t="s">
         <v>479</v>
       </c>
@@ -6347,7 +6368,7 @@
         <v>66</v>
       </c>
     </row>
-    <row r="22" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="22" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A22" t="s">
         <v>479</v>
       </c>
@@ -6355,7 +6376,7 @@
         <v>66</v>
       </c>
     </row>
-    <row r="23" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="23" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A23" t="s">
         <v>479</v>
       </c>
@@ -6363,7 +6384,7 @@
         <v>66</v>
       </c>
     </row>
-    <row r="24" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="24" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A24" t="s">
         <v>479</v>
       </c>
@@ -6371,7 +6392,7 @@
         <v>66</v>
       </c>
     </row>
-    <row r="25" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="25" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A25" t="s">
         <v>479</v>
       </c>
@@ -6379,7 +6400,7 @@
         <v>66</v>
       </c>
     </row>
-    <row r="26" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="26" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A26" t="s">
         <v>480</v>
       </c>
@@ -6387,7 +6408,7 @@
         <v>30</v>
       </c>
     </row>
-    <row r="27" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="27" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A27" t="s">
         <v>478</v>
       </c>
@@ -6395,7 +6416,7 @@
         <v>60</v>
       </c>
     </row>
-    <row r="28" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="28" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A28" t="s">
         <v>487</v>
       </c>
@@ -6403,7 +6424,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="29" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="29" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A29" t="s">
         <v>488</v>
       </c>
@@ -6429,9 +6450,9 @@
       <selection activeCell="D73" sqref="D73"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <sheetData>
-    <row r="1" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="1" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
         <v>474</v>
       </c>
@@ -6439,7 +6460,7 @@
         <v>475</v>
       </c>
     </row>
-    <row r="2" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="2" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
         <v>11</v>
       </c>
@@ -6447,7 +6468,7 @@
         <v>454</v>
       </c>
     </row>
-    <row r="3" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="3" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
         <v>5</v>
       </c>
@@ -6455,7 +6476,7 @@
         <v>455</v>
       </c>
     </row>
-    <row r="4" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="4" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
         <v>4</v>
       </c>
@@ -6463,7 +6484,7 @@
         <v>456</v>
       </c>
     </row>
-    <row r="5" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="5" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
         <v>12</v>
       </c>
@@ -6471,7 +6492,7 @@
         <v>457</v>
       </c>
     </row>
-    <row r="6" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="6" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
         <v>10</v>
       </c>
@@ -6479,7 +6500,7 @@
         <v>458</v>
       </c>
     </row>
-    <row r="7" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="7" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
         <v>30</v>
       </c>
@@ -6487,7 +6508,7 @@
         <v>459</v>
       </c>
     </row>
-    <row r="8" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="8" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A8" t="s">
         <v>3</v>
       </c>
@@ -6495,7 +6516,7 @@
         <v>460</v>
       </c>
     </row>
-    <row r="9" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="9" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A9" t="s">
         <v>103</v>
       </c>
@@ -6503,7 +6524,7 @@
         <v>461</v>
       </c>
     </row>
-    <row r="10" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="10" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A10" t="s">
         <v>31</v>
       </c>
@@ -6511,7 +6532,7 @@
         <v>462</v>
       </c>
     </row>
-    <row r="11" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="11" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A11" t="s">
         <v>25</v>
       </c>
@@ -6519,7 +6540,7 @@
         <v>463</v>
       </c>
     </row>
-    <row r="12" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="12" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A12" t="s">
         <v>28</v>
       </c>
@@ -6527,7 +6548,7 @@
         <v>464</v>
       </c>
     </row>
-    <row r="13" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="13" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A13" t="s">
         <v>9</v>
       </c>
@@ -6535,7 +6556,7 @@
         <v>455</v>
       </c>
     </row>
-    <row r="14" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="14" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A14" t="s">
         <v>1</v>
       </c>
@@ -6543,7 +6564,7 @@
         <v>456</v>
       </c>
     </row>
-    <row r="15" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="15" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A15" t="s">
         <v>33</v>
       </c>
@@ -6551,7 +6572,7 @@
         <v>457</v>
       </c>
     </row>
-    <row r="16" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="16" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A16" t="s">
         <v>26</v>
       </c>
@@ -6559,7 +6580,7 @@
         <v>465</v>
       </c>
     </row>
-    <row r="17" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="17" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A17" t="s">
         <v>14</v>
       </c>
@@ -6567,7 +6588,7 @@
         <v>456</v>
       </c>
     </row>
-    <row r="18" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="18" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A18" t="s">
         <v>13</v>
       </c>
@@ -6575,7 +6596,7 @@
         <v>457</v>
       </c>
     </row>
-    <row r="19" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="19" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A19" t="s">
         <v>181</v>
       </c>
@@ -6583,7 +6604,7 @@
         <v>464</v>
       </c>
     </row>
-    <row r="20" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="20" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A20" t="s">
         <v>179</v>
       </c>
@@ -6591,7 +6612,7 @@
         <v>456</v>
       </c>
     </row>
-    <row r="21" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="21" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A21" t="s">
         <v>176</v>
       </c>
@@ -6599,7 +6620,7 @@
         <v>455</v>
       </c>
     </row>
-    <row r="22" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="22" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A22" t="s">
         <v>185</v>
       </c>
@@ -6607,7 +6628,7 @@
         <v>454</v>
       </c>
     </row>
-    <row r="23" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="23" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A23" t="s">
         <v>183</v>
       </c>
@@ -6615,7 +6636,7 @@
         <v>457</v>
       </c>
     </row>
-    <row r="24" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="24" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A24" t="s">
         <v>187</v>
       </c>
@@ -6623,7 +6644,7 @@
         <v>459</v>
       </c>
     </row>
-    <row r="25" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="25" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A25" t="s">
         <v>134</v>
       </c>
@@ -6631,7 +6652,7 @@
         <v>455</v>
       </c>
     </row>
-    <row r="26" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="26" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A26" t="s">
         <v>131</v>
       </c>
@@ -6639,7 +6660,7 @@
         <v>466</v>
       </c>
     </row>
-    <row r="27" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="27" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A27" t="s">
         <v>129</v>
       </c>
@@ -6647,7 +6668,7 @@
         <v>465</v>
       </c>
     </row>
-    <row r="28" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="28" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A28" t="s">
         <v>127</v>
       </c>
@@ -6655,7 +6676,7 @@
         <v>454</v>
       </c>
     </row>
-    <row r="29" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="29" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A29" t="s">
         <v>37</v>
       </c>
@@ -6663,7 +6684,7 @@
         <v>457</v>
       </c>
     </row>
-    <row r="30" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="30" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A30" t="s">
         <v>47</v>
       </c>
@@ -6671,7 +6692,7 @@
         <v>465</v>
       </c>
     </row>
-    <row r="31" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="31" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A31" t="s">
         <v>51</v>
       </c>
@@ -6679,7 +6700,7 @@
         <v>464</v>
       </c>
     </row>
-    <row r="32" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="32" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A32" t="s">
         <v>50</v>
       </c>
@@ -6687,7 +6708,7 @@
         <v>455</v>
       </c>
     </row>
-    <row r="33" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="33" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A33" t="s">
         <v>48</v>
       </c>
@@ -6695,7 +6716,7 @@
         <v>457</v>
       </c>
     </row>
-    <row r="34" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="34" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A34" t="s">
         <v>49</v>
       </c>
@@ -6703,7 +6724,7 @@
         <v>466</v>
       </c>
     </row>
-    <row r="35" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="35" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A35" t="s">
         <v>91</v>
       </c>
@@ -6711,7 +6732,7 @@
         <v>464</v>
       </c>
     </row>
-    <row r="36" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="36" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A36" t="s">
         <v>89</v>
       </c>
@@ -6719,7 +6740,7 @@
         <v>467</v>
       </c>
     </row>
-    <row r="37" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="37" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A37" t="s">
         <v>16</v>
       </c>
@@ -6727,7 +6748,7 @@
         <v>468</v>
       </c>
     </row>
-    <row r="38" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="38" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A38" t="s">
         <v>87</v>
       </c>
@@ -6735,7 +6756,7 @@
         <v>466</v>
       </c>
     </row>
-    <row r="39" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="39" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A39" t="s">
         <v>93</v>
       </c>
@@ -6743,7 +6764,7 @@
         <v>459</v>
       </c>
     </row>
-    <row r="40" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="40" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A40" t="s">
         <v>97</v>
       </c>
@@ -6751,7 +6772,7 @@
         <v>465</v>
       </c>
     </row>
-    <row r="41" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="41" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A41" t="s">
         <v>20</v>
       </c>
@@ -6759,7 +6780,7 @@
         <v>463</v>
       </c>
     </row>
-    <row r="42" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="42" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A42" t="s">
         <v>19</v>
       </c>
@@ -6767,7 +6788,7 @@
         <v>465</v>
       </c>
     </row>
-    <row r="43" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="43" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A43" t="s">
         <v>143</v>
       </c>
@@ -6775,7 +6796,7 @@
         <v>465</v>
       </c>
     </row>
-    <row r="44" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="44" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A44" t="s">
         <v>60</v>
       </c>
@@ -6783,7 +6804,7 @@
         <v>462</v>
       </c>
     </row>
-    <row r="45" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="45" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A45" t="s">
         <v>66</v>
       </c>
@@ -6791,7 +6812,7 @@
         <v>468</v>
       </c>
     </row>
-    <row r="46" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="46" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A46" t="s">
         <v>21</v>
       </c>
@@ -6799,7 +6820,7 @@
         <v>464</v>
       </c>
     </row>
-    <row r="47" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="47" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A47" t="s">
         <v>22</v>
       </c>
@@ -6807,7 +6828,7 @@
         <v>455</v>
       </c>
     </row>
-    <row r="48" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="48" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A48" t="s">
         <v>41</v>
       </c>
@@ -6815,7 +6836,7 @@
         <v>456</v>
       </c>
     </row>
-    <row r="49" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="49" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A49" t="s">
         <v>35</v>
       </c>
@@ -6823,7 +6844,7 @@
         <v>457</v>
       </c>
     </row>
-    <row r="50" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="50" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A50" t="s">
         <v>42</v>
       </c>
@@ -6831,7 +6852,7 @@
         <v>468</v>
       </c>
     </row>
-    <row r="51" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="51" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A51" t="s">
         <v>108</v>
       </c>
@@ -6839,7 +6860,7 @@
         <v>459</v>
       </c>
     </row>
-    <row r="52" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="52" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A52" t="s">
         <v>110</v>
       </c>
@@ -6847,7 +6868,7 @@
         <v>456</v>
       </c>
     </row>
-    <row r="53" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="53" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A53" t="s">
         <v>27</v>
       </c>
@@ -6855,7 +6876,7 @@
         <v>460</v>
       </c>
     </row>
-    <row r="54" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="54" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A54" t="s">
         <v>144</v>
       </c>
@@ -6863,7 +6884,7 @@
         <v>462</v>
       </c>
     </row>
-    <row r="55" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="55" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A55" t="s">
         <v>6</v>
       </c>
@@ -6871,7 +6892,7 @@
         <v>454</v>
       </c>
     </row>
-    <row r="56" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="56" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A56" t="s">
         <v>17</v>
       </c>
@@ -6879,7 +6900,7 @@
         <v>457</v>
       </c>
     </row>
-    <row r="57" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="57" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A57" t="s">
         <v>18</v>
       </c>
@@ -6887,7 +6908,7 @@
         <v>454</v>
       </c>
     </row>
-    <row r="58" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="58" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A58" t="s">
         <v>43</v>
       </c>
@@ -6895,7 +6916,7 @@
         <v>465</v>
       </c>
     </row>
-    <row r="59" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="59" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A59" t="s">
         <v>112</v>
       </c>
@@ -6903,7 +6924,7 @@
         <v>458</v>
       </c>
     </row>
-    <row r="60" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="60" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A60" t="s">
         <v>124</v>
       </c>
@@ -6911,7 +6932,7 @@
         <v>468</v>
       </c>
     </row>
-    <row r="61" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="61" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A61" t="s">
         <v>111</v>
       </c>
@@ -6919,7 +6940,7 @@
         <v>460</v>
       </c>
     </row>
-    <row r="62" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="62" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A62" t="s">
         <v>145</v>
       </c>
@@ -6927,7 +6948,7 @@
         <v>458</v>
       </c>
     </row>
-    <row r="63" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="63" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A63" t="s">
         <v>106</v>
       </c>
@@ -6935,7 +6956,7 @@
         <v>459</v>
       </c>
     </row>
-    <row r="64" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="64" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A64" t="s">
         <v>95</v>
       </c>
@@ -6943,7 +6964,7 @@
         <v>464</v>
       </c>
     </row>
-    <row r="65" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="65" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A65" t="s">
         <v>197</v>
       </c>
@@ -6951,7 +6972,7 @@
         <v>468</v>
       </c>
     </row>
-    <row r="66" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="66" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A66" t="s">
         <v>173</v>
       </c>
@@ -6959,7 +6980,7 @@
         <v>460</v>
       </c>
     </row>
-    <row r="67" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="67" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A67" t="s">
         <v>203</v>
       </c>
@@ -6967,7 +6988,7 @@
         <v>465</v>
       </c>
     </row>
-    <row r="68" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="68" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A68" t="s">
         <v>175</v>
       </c>
@@ -6975,7 +6996,7 @@
         <v>461</v>
       </c>
     </row>
-    <row r="69" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="69" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A69" t="s">
         <v>195</v>
       </c>
@@ -6983,7 +7004,7 @@
         <v>460</v>
       </c>
     </row>
-    <row r="70" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="70" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A70" t="s">
         <v>208</v>
       </c>
@@ -6991,7 +7012,7 @@
         <v>460</v>
       </c>
     </row>
-    <row r="71" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="71" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A71" t="s">
         <v>189</v>
       </c>
@@ -6999,7 +7020,7 @@
         <v>462</v>
       </c>
     </row>
-    <row r="72" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="72" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A72" t="s">
         <v>206</v>
       </c>
@@ -7007,7 +7028,7 @@
         <v>467</v>
       </c>
     </row>
-    <row r="73" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="73" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A73" t="s">
         <v>159</v>
       </c>
@@ -7015,7 +7036,7 @@
         <v>465</v>
       </c>
     </row>
-    <row r="74" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="74" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A74" t="s">
         <v>161</v>
       </c>
@@ -7023,7 +7044,7 @@
         <v>464</v>
       </c>
     </row>
-    <row r="75" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="75" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A75" t="s">
         <v>163</v>
       </c>
@@ -7031,7 +7052,7 @@
         <v>469</v>
       </c>
     </row>
-    <row r="76" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="76" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A76" t="s">
         <v>23</v>
       </c>
@@ -7039,7 +7060,7 @@
         <v>470</v>
       </c>
     </row>
-    <row r="77" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="77" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A77" t="s">
         <v>155</v>
       </c>
@@ -7047,7 +7068,7 @@
         <v>471</v>
       </c>
     </row>
-    <row r="78" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="78" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A78" t="s">
         <v>157</v>
       </c>
@@ -7055,7 +7076,7 @@
         <v>460</v>
       </c>
     </row>
-    <row r="79" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="79" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A79" t="s">
         <v>481</v>
       </c>
@@ -7063,7 +7084,7 @@
         <v>462</v>
       </c>
     </row>
-    <row r="80" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="80" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A80" t="s">
         <v>482</v>
       </c>
@@ -7071,7 +7092,7 @@
         <v>468</v>
       </c>
     </row>
-    <row r="81" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="81" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A81" t="s">
         <v>478</v>
       </c>
@@ -7079,7 +7100,7 @@
         <v>462</v>
       </c>
     </row>
-    <row r="82" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="82" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A82" t="s">
         <v>479</v>
       </c>
@@ -7087,7 +7108,7 @@
         <v>468</v>
       </c>
     </row>
-    <row r="83" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="83" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A83" t="s">
         <v>483</v>
       </c>
@@ -7095,7 +7116,7 @@
         <v>459</v>
       </c>
     </row>
-    <row r="84" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="84" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A84" t="s">
         <v>480</v>
       </c>
@@ -7103,7 +7124,7 @@
         <v>459</v>
       </c>
     </row>
-    <row r="85" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="85" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A85" t="s">
         <v>487</v>
       </c>
@@ -7111,7 +7132,7 @@
         <v>454</v>
       </c>
     </row>
-    <row r="86" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="86" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A86" t="s">
         <v>488</v>
       </c>
@@ -7133,12 +7154,12 @@
       <selection activeCell="I25" sqref="I25"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="19" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="1" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A1" s="1" t="s">
         <v>473</v>
       </c>
@@ -7146,7 +7167,7 @@
         <v>472</v>
       </c>
     </row>
-    <row r="2" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="2" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
         <v>52</v>
       </c>
@@ -7154,7 +7175,7 @@
         <v>18</v>
       </c>
     </row>
-    <row r="3" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="3" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
         <v>53</v>
       </c>
@@ -7162,7 +7183,7 @@
         <v>491</v>
       </c>
     </row>
-    <row r="4" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="4" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
         <v>54</v>
       </c>
@@ -7170,7 +7191,7 @@
         <v>500</v>
       </c>
     </row>
-    <row r="5" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="5" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
         <v>55</v>
       </c>
@@ -7191,26 +7212,26 @@
   </sheetPr>
   <dimension ref="A1:N56"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="H30" sqref="H30"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="F14" sqref="F14"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="25.1796875" customWidth="1"/>
+    <col min="1" max="1" width="25.140625" customWidth="1"/>
     <col min="2" max="5" width="25" customWidth="1"/>
-    <col min="6" max="6" width="20.1796875" customWidth="1"/>
-    <col min="7" max="7" width="25.1796875" customWidth="1"/>
-    <col min="8" max="8" width="28.1796875" customWidth="1"/>
-    <col min="9" max="9" width="34.1796875" customWidth="1"/>
-    <col min="10" max="10" width="20.81640625" customWidth="1"/>
-    <col min="11" max="11" width="20.1796875" customWidth="1"/>
-    <col min="12" max="12" width="22.81640625" customWidth="1"/>
-    <col min="13" max="13" width="21.81640625" customWidth="1"/>
-    <col min="14" max="14" width="24.81640625" customWidth="1"/>
+    <col min="6" max="6" width="20.140625" customWidth="1"/>
+    <col min="7" max="7" width="25.140625" customWidth="1"/>
+    <col min="8" max="8" width="28.140625" customWidth="1"/>
+    <col min="9" max="9" width="34.140625" customWidth="1"/>
+    <col min="10" max="10" width="20.85546875" customWidth="1"/>
+    <col min="11" max="11" width="20.140625" customWidth="1"/>
+    <col min="12" max="12" width="22.85546875" customWidth="1"/>
+    <col min="13" max="13" width="21.85546875" customWidth="1"/>
+    <col min="14" max="14" width="24.85546875" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:14" x14ac:dyDescent="0.35">
+    <row r="1" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A1" s="1"/>
       <c r="B1" s="1"/>
       <c r="D1" s="13" t="s">
@@ -7229,7 +7250,7 @@
       <c r="M1" s="14"/>
       <c r="N1" s="15"/>
     </row>
-    <row r="2" spans="1:14" x14ac:dyDescent="0.35">
+    <row r="2" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A2" s="1" t="s">
         <v>485</v>
       </c>
@@ -7273,7 +7294,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="3" spans="1:14" x14ac:dyDescent="0.35">
+    <row r="3" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
         <v>1</v>
       </c>
@@ -7299,7 +7320,7 @@
         <v>163</v>
       </c>
     </row>
-    <row r="4" spans="1:14" x14ac:dyDescent="0.35">
+    <row r="4" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
         <v>1</v>
       </c>
@@ -7325,7 +7346,7 @@
         <v>163</v>
       </c>
     </row>
-    <row r="5" spans="1:14" x14ac:dyDescent="0.35">
+    <row r="5" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
         <v>1</v>
       </c>
@@ -7351,7 +7372,7 @@
         <v>163</v>
       </c>
     </row>
-    <row r="6" spans="1:14" x14ac:dyDescent="0.35">
+    <row r="6" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
         <v>9</v>
       </c>
@@ -7386,7 +7407,7 @@
         <v>163</v>
       </c>
     </row>
-    <row r="7" spans="1:14" x14ac:dyDescent="0.35">
+    <row r="7" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
         <v>9</v>
       </c>
@@ -7409,7 +7430,7 @@
         <v>14</v>
       </c>
     </row>
-    <row r="8" spans="1:14" x14ac:dyDescent="0.35">
+    <row r="8" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A8" t="s">
         <v>15</v>
       </c>
@@ -7432,7 +7453,7 @@
         <v>18</v>
       </c>
     </row>
-    <row r="9" spans="1:14" x14ac:dyDescent="0.35">
+    <row r="9" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A9" t="s">
         <v>15</v>
       </c>
@@ -7452,7 +7473,7 @@
         <v>18</v>
       </c>
     </row>
-    <row r="10" spans="1:14" x14ac:dyDescent="0.35">
+    <row r="10" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A10" t="s">
         <v>15</v>
       </c>
@@ -7472,7 +7493,7 @@
         <v>18</v>
       </c>
     </row>
-    <row r="11" spans="1:14" x14ac:dyDescent="0.35">
+    <row r="11" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A11" t="s">
         <v>11</v>
       </c>
@@ -7501,7 +7522,7 @@
         <v>23</v>
       </c>
     </row>
-    <row r="12" spans="1:14" x14ac:dyDescent="0.35">
+    <row r="12" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A12" t="s">
         <v>11</v>
       </c>
@@ -7530,7 +7551,7 @@
         <v>23</v>
       </c>
     </row>
-    <row r="13" spans="1:14" x14ac:dyDescent="0.35">
+    <row r="13" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A13" t="s">
         <v>24</v>
       </c>
@@ -7559,7 +7580,7 @@
         <v>23</v>
       </c>
     </row>
-    <row r="14" spans="1:14" x14ac:dyDescent="0.35">
+    <row r="14" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A14" t="s">
         <v>24</v>
       </c>
@@ -7588,7 +7609,7 @@
         <v>23</v>
       </c>
     </row>
-    <row r="15" spans="1:14" x14ac:dyDescent="0.35">
+    <row r="15" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A15" t="s">
         <v>3</v>
       </c>
@@ -7623,7 +7644,7 @@
         <v>163</v>
       </c>
     </row>
-    <row r="16" spans="1:14" x14ac:dyDescent="0.35">
+    <row r="16" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A16" t="s">
         <v>29</v>
       </c>
@@ -7664,7 +7685,7 @@
         <v>163</v>
       </c>
     </row>
-    <row r="17" spans="1:13" x14ac:dyDescent="0.35">
+    <row r="17" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A17" t="s">
         <v>32</v>
       </c>
@@ -7699,7 +7720,7 @@
         <v>28</v>
       </c>
     </row>
-    <row r="18" spans="1:13" x14ac:dyDescent="0.35">
+    <row r="18" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A18" t="s">
         <v>32</v>
       </c>
@@ -7734,7 +7755,7 @@
         <v>28</v>
       </c>
     </row>
-    <row r="19" spans="1:13" x14ac:dyDescent="0.35">
+    <row r="19" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A19" t="s">
         <v>30</v>
       </c>
@@ -7757,7 +7778,7 @@
         <v>28</v>
       </c>
     </row>
-    <row r="20" spans="1:13" x14ac:dyDescent="0.35">
+    <row r="20" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A20" t="s">
         <v>30</v>
       </c>
@@ -7780,7 +7801,7 @@
         <v>28</v>
       </c>
     </row>
-    <row r="21" spans="1:13" x14ac:dyDescent="0.35">
+    <row r="21" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A21" t="s">
         <v>30</v>
       </c>
@@ -7803,7 +7824,7 @@
         <v>28</v>
       </c>
     </row>
-    <row r="22" spans="1:13" x14ac:dyDescent="0.35">
+    <row r="22" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A22" t="s">
         <v>25</v>
       </c>
@@ -7841,7 +7862,7 @@
         <v>163</v>
       </c>
     </row>
-    <row r="23" spans="1:13" x14ac:dyDescent="0.35">
+    <row r="23" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A23" t="s">
         <v>34</v>
       </c>
@@ -7858,7 +7879,7 @@
         <v>21</v>
       </c>
     </row>
-    <row r="24" spans="1:13" x14ac:dyDescent="0.35">
+    <row r="24" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A24" t="s">
         <v>34</v>
       </c>
@@ -7887,7 +7908,7 @@
         <v>23</v>
       </c>
     </row>
-    <row r="25" spans="1:13" x14ac:dyDescent="0.35">
+    <row r="25" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A25" t="s">
         <v>34</v>
       </c>
@@ -7919,7 +7940,7 @@
         <v>23</v>
       </c>
     </row>
-    <row r="26" spans="1:13" x14ac:dyDescent="0.35">
+    <row r="26" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A26" t="s">
         <v>36</v>
       </c>
@@ -7936,7 +7957,7 @@
         <v>21</v>
       </c>
     </row>
-    <row r="27" spans="1:13" x14ac:dyDescent="0.35">
+    <row r="27" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A27" t="s">
         <v>36</v>
       </c>
@@ -7965,7 +7986,7 @@
         <v>23</v>
       </c>
     </row>
-    <row r="28" spans="1:13" x14ac:dyDescent="0.35">
+    <row r="28" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A28" t="s">
         <v>36</v>
       </c>
@@ -7997,7 +8018,7 @@
         <v>23</v>
       </c>
     </row>
-    <row r="29" spans="1:13" x14ac:dyDescent="0.35">
+    <row r="29" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A29" t="s">
         <v>21</v>
       </c>
@@ -8029,7 +8050,7 @@
         <v>23</v>
       </c>
     </row>
-    <row r="30" spans="1:13" x14ac:dyDescent="0.35">
+    <row r="30" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A30" t="s">
         <v>21</v>
       </c>
@@ -8061,7 +8082,7 @@
         <v>23</v>
       </c>
     </row>
-    <row r="31" spans="1:13" x14ac:dyDescent="0.35">
+    <row r="31" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A31" t="s">
         <v>21</v>
       </c>
@@ -8093,7 +8114,7 @@
         <v>23</v>
       </c>
     </row>
-    <row r="32" spans="1:13" x14ac:dyDescent="0.35">
+    <row r="32" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A32" t="s">
         <v>38</v>
       </c>
@@ -8125,7 +8146,7 @@
         <v>23</v>
       </c>
     </row>
-    <row r="33" spans="1:13" x14ac:dyDescent="0.35">
+    <row r="33" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A33" t="s">
         <v>38</v>
       </c>
@@ -8157,7 +8178,7 @@
         <v>23</v>
       </c>
     </row>
-    <row r="34" spans="1:13" x14ac:dyDescent="0.35">
+    <row r="34" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A34" t="s">
         <v>39</v>
       </c>
@@ -8189,7 +8210,7 @@
         <v>23</v>
       </c>
     </row>
-    <row r="35" spans="1:13" x14ac:dyDescent="0.35">
+    <row r="35" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A35" t="s">
         <v>39</v>
       </c>
@@ -8221,7 +8242,7 @@
         <v>23</v>
       </c>
     </row>
-    <row r="36" spans="1:13" x14ac:dyDescent="0.35">
+    <row r="36" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A36" t="s">
         <v>40</v>
       </c>
@@ -8247,7 +8268,7 @@
         <v>22</v>
       </c>
     </row>
-    <row r="37" spans="1:13" x14ac:dyDescent="0.35">
+    <row r="37" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A37" t="s">
         <v>40</v>
       </c>
@@ -8273,7 +8294,7 @@
         <v>22</v>
       </c>
     </row>
-    <row r="38" spans="1:13" x14ac:dyDescent="0.35">
+    <row r="38" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A38" t="s">
         <v>40</v>
       </c>
@@ -8305,7 +8326,7 @@
         <v>23</v>
       </c>
     </row>
-    <row r="39" spans="1:13" x14ac:dyDescent="0.35">
+    <row r="39" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A39" t="s">
         <v>40</v>
       </c>
@@ -8337,7 +8358,7 @@
         <v>23</v>
       </c>
     </row>
-    <row r="40" spans="1:13" x14ac:dyDescent="0.35">
+    <row r="40" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A40" t="s">
         <v>40</v>
       </c>
@@ -8372,7 +8393,7 @@
         <v>23</v>
       </c>
     </row>
-    <row r="41" spans="1:13" x14ac:dyDescent="0.35">
+    <row r="41" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A41" t="s">
         <v>40</v>
       </c>
@@ -8407,7 +8428,7 @@
         <v>23</v>
       </c>
     </row>
-    <row r="42" spans="1:13" x14ac:dyDescent="0.35">
+    <row r="42" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A42" t="s">
         <v>40</v>
       </c>
@@ -8445,7 +8466,7 @@
         <v>44</v>
       </c>
     </row>
-    <row r="43" spans="1:13" x14ac:dyDescent="0.35">
+    <row r="43" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A43" t="s">
         <v>40</v>
       </c>
@@ -8483,7 +8504,7 @@
         <v>44</v>
       </c>
     </row>
-    <row r="44" spans="1:13" x14ac:dyDescent="0.35">
+    <row r="44" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A44" t="s">
         <v>45</v>
       </c>
@@ -8509,7 +8530,7 @@
         <v>22</v>
       </c>
     </row>
-    <row r="45" spans="1:13" x14ac:dyDescent="0.35">
+    <row r="45" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A45" t="s">
         <v>45</v>
       </c>
@@ -8535,7 +8556,7 @@
         <v>22</v>
       </c>
     </row>
-    <row r="46" spans="1:13" x14ac:dyDescent="0.35">
+    <row r="46" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A46" t="s">
         <v>45</v>
       </c>
@@ -8567,7 +8588,7 @@
         <v>23</v>
       </c>
     </row>
-    <row r="47" spans="1:13" x14ac:dyDescent="0.35">
+    <row r="47" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A47" t="s">
         <v>45</v>
       </c>
@@ -8599,7 +8620,7 @@
         <v>23</v>
       </c>
     </row>
-    <row r="48" spans="1:13" x14ac:dyDescent="0.35">
+    <row r="48" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A48" t="s">
         <v>45</v>
       </c>
@@ -8634,7 +8655,7 @@
         <v>23</v>
       </c>
     </row>
-    <row r="49" spans="1:13" x14ac:dyDescent="0.35">
+    <row r="49" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A49" t="s">
         <v>45</v>
       </c>
@@ -8669,7 +8690,7 @@
         <v>23</v>
       </c>
     </row>
-    <row r="50" spans="1:13" x14ac:dyDescent="0.35">
+    <row r="50" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A50" t="s">
         <v>45</v>
       </c>
@@ -8707,7 +8728,7 @@
         <v>44</v>
       </c>
     </row>
-    <row r="51" spans="1:13" x14ac:dyDescent="0.35">
+    <row r="51" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A51" t="s">
         <v>45</v>
       </c>
@@ -8745,7 +8766,7 @@
         <v>44</v>
       </c>
     </row>
-    <row r="52" spans="1:13" x14ac:dyDescent="0.35">
+    <row r="52" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A52" t="s">
         <v>46</v>
       </c>
@@ -8777,7 +8798,7 @@
         <v>23</v>
       </c>
     </row>
-    <row r="53" spans="1:13" x14ac:dyDescent="0.35">
+    <row r="53" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A53" t="s">
         <v>46</v>
       </c>
@@ -8809,7 +8830,7 @@
         <v>23</v>
       </c>
     </row>
-    <row r="54" spans="1:13" x14ac:dyDescent="0.35">
+    <row r="54" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A54" t="s">
         <v>46</v>
       </c>
@@ -8829,7 +8850,7 @@
         <v>480</v>
       </c>
     </row>
-    <row r="55" spans="1:13" x14ac:dyDescent="0.35">
+    <row r="55" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A55" t="s">
         <v>28</v>
       </c>
@@ -8864,7 +8885,7 @@
         <v>163</v>
       </c>
     </row>
-    <row r="56" spans="1:13" x14ac:dyDescent="0.35">
+    <row r="56" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A56" t="s">
         <v>28</v>
       </c>

</xml_diff>

<commit_message>
master config file changes
</commit_message>
<xml_diff>
--- a/config/master_config.xlsx
+++ b/config/master_config.xlsx
@@ -5,12 +5,12 @@
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\APERC\9th_edition_visualisation\config\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\hyuga.kasai\Documents\Github\9th_Visualization\9th_edition_visualisation\config\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A60323E7-A1F5-46D2-BBD4-78F1CDCBD2E2}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{8612EEE1-723F-4FBB-8891-8FA4E6557CBE}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="1755" yWindow="-16320" windowWidth="29040" windowHeight="15840" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" tabRatio="812" firstSheet="1" activeTab="7" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="9th_EBT_schema" sheetId="7" r:id="rId1"/>
@@ -196,7 +196,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1489" uniqueCount="492">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1489" uniqueCount="494">
   <si>
     <t>chart_type</t>
   </si>
@@ -1672,13 +1672,19 @@
   </si>
   <si>
     <t>['2000', '2010', '2018', '2020', '2030', '2040', '2050', '2060', '2070']</t>
+  </si>
+  <si>
+    <t>Gas?</t>
+  </si>
+  <si>
+    <t>16_others_dummy</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="8" x14ac:knownFonts="1">
+  <fonts count="9" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -1735,8 +1741,15 @@
       <name val="Tahoma"/>
       <family val="2"/>
     </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF9C0006"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
   </fonts>
-  <fills count="9">
+  <fills count="10">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -1783,6 +1796,11 @@
       <patternFill patternType="solid">
         <fgColor rgb="FF00B050"/>
         <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFC7CE"/>
       </patternFill>
     </fill>
   </fills>
@@ -1847,10 +1865,11 @@
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="1">
+  <cellStyleXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="8" fillId="9" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="16">
+  <cellXfs count="17">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="top"/>
@@ -1879,8 +1898,10 @@
     <xf numFmtId="0" fontId="2" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="top"/>
     </xf>
+    <xf numFmtId="0" fontId="8" fillId="9" borderId="0" xfId="1"/>
   </cellXfs>
-  <cellStyles count="1">
+  <cellStyles count="2">
+    <cellStyle name="Bad" xfId="1" builtinId="27"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
@@ -3080,29 +3101,29 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{A000B41E-5923-4013-B542-E4247E89557C}">
   <dimension ref="A1:I102"/>
   <sheetViews>
-    <sheetView showGridLines="0" tabSelected="1" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <selection activeCell="D38" sqref="D38"/>
+    <sheetView showGridLines="0" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
+      <selection activeCell="C45" sqref="C45"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="12.81640625" customWidth="1"/>
+    <col min="1" max="1" width="12.85546875" customWidth="1"/>
     <col min="2" max="2" width="11" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="26.1796875" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="42.453125" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="33.54296875" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="45.1796875" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="41.1796875" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="28.54296875" bestFit="1" customWidth="1"/>
-    <col min="9" max="9" width="40.81640625" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="26.140625" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="42.42578125" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="33.5703125" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="45.140625" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="41.140625" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="28.5703125" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="40.85546875" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:9" x14ac:dyDescent="0.35">
+    <row r="1" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A1" s="8" t="s">
         <v>214</v>
       </c>
     </row>
-    <row r="3" spans="1:9" x14ac:dyDescent="0.35">
+    <row r="3" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A3" s="9" t="s">
         <v>215</v>
       </c>
@@ -3131,7 +3152,7 @@
         <v>218</v>
       </c>
     </row>
-    <row r="4" spans="1:9" x14ac:dyDescent="0.35">
+    <row r="4" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
         <v>219</v>
       </c>
@@ -3160,7 +3181,7 @@
         <v>224</v>
       </c>
     </row>
-    <row r="5" spans="1:9" x14ac:dyDescent="0.35">
+    <row r="5" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
         <v>225</v>
       </c>
@@ -3189,7 +3210,7 @@
         <v>230</v>
       </c>
     </row>
-    <row r="6" spans="1:9" x14ac:dyDescent="0.35">
+    <row r="6" spans="1:9" x14ac:dyDescent="0.25">
       <c r="B6" t="s">
         <v>231</v>
       </c>
@@ -3215,7 +3236,7 @@
         <v>234</v>
       </c>
     </row>
-    <row r="7" spans="1:9" x14ac:dyDescent="0.35">
+    <row r="7" spans="1:9" x14ac:dyDescent="0.25">
       <c r="B7" t="s">
         <v>235</v>
       </c>
@@ -3241,7 +3262,7 @@
         <v>239</v>
       </c>
     </row>
-    <row r="8" spans="1:9" x14ac:dyDescent="0.35">
+    <row r="8" spans="1:9" x14ac:dyDescent="0.25">
       <c r="B8" t="s">
         <v>240</v>
       </c>
@@ -3267,7 +3288,7 @@
         <v>244</v>
       </c>
     </row>
-    <row r="9" spans="1:9" x14ac:dyDescent="0.35">
+    <row r="9" spans="1:9" x14ac:dyDescent="0.25">
       <c r="B9" t="s">
         <v>245</v>
       </c>
@@ -3293,7 +3314,7 @@
         <v>250</v>
       </c>
     </row>
-    <row r="10" spans="1:9" x14ac:dyDescent="0.35">
+    <row r="10" spans="1:9" x14ac:dyDescent="0.25">
       <c r="B10" t="s">
         <v>251</v>
       </c>
@@ -3319,7 +3340,7 @@
         <v>254</v>
       </c>
     </row>
-    <row r="11" spans="1:9" x14ac:dyDescent="0.35">
+    <row r="11" spans="1:9" x14ac:dyDescent="0.25">
       <c r="B11" t="s">
         <v>255</v>
       </c>
@@ -3345,7 +3366,7 @@
         <v>258</v>
       </c>
     </row>
-    <row r="12" spans="1:9" x14ac:dyDescent="0.35">
+    <row r="12" spans="1:9" x14ac:dyDescent="0.25">
       <c r="B12" t="s">
         <v>259</v>
       </c>
@@ -3371,7 +3392,7 @@
         <v>262</v>
       </c>
     </row>
-    <row r="13" spans="1:9" x14ac:dyDescent="0.35">
+    <row r="13" spans="1:9" x14ac:dyDescent="0.25">
       <c r="B13" t="s">
         <v>263</v>
       </c>
@@ -3397,7 +3418,7 @@
         <v>266</v>
       </c>
     </row>
-    <row r="14" spans="1:9" x14ac:dyDescent="0.35">
+    <row r="14" spans="1:9" x14ac:dyDescent="0.25">
       <c r="B14" t="s">
         <v>267</v>
       </c>
@@ -3423,7 +3444,7 @@
         <v>270</v>
       </c>
     </row>
-    <row r="15" spans="1:9" x14ac:dyDescent="0.35">
+    <row r="15" spans="1:9" x14ac:dyDescent="0.25">
       <c r="B15" t="s">
         <v>271</v>
       </c>
@@ -3449,7 +3470,7 @@
         <v>274</v>
       </c>
     </row>
-    <row r="16" spans="1:9" x14ac:dyDescent="0.35">
+    <row r="16" spans="1:9" x14ac:dyDescent="0.25">
       <c r="B16" t="s">
         <v>275</v>
       </c>
@@ -3475,7 +3496,7 @@
         <v>278</v>
       </c>
     </row>
-    <row r="17" spans="2:9" x14ac:dyDescent="0.35">
+    <row r="17" spans="2:9" x14ac:dyDescent="0.25">
       <c r="B17" t="s">
         <v>279</v>
       </c>
@@ -3501,7 +3522,7 @@
         <v>282</v>
       </c>
     </row>
-    <row r="18" spans="2:9" x14ac:dyDescent="0.35">
+    <row r="18" spans="2:9" x14ac:dyDescent="0.25">
       <c r="B18" t="s">
         <v>283</v>
       </c>
@@ -3527,11 +3548,11 @@
         <v>286</v>
       </c>
     </row>
-    <row r="19" spans="2:9" x14ac:dyDescent="0.35">
+    <row r="19" spans="2:9" x14ac:dyDescent="0.25">
       <c r="B19" t="s">
         <v>287</v>
       </c>
-      <c r="C19" t="s">
+      <c r="C19" s="4" t="s">
         <v>100</v>
       </c>
       <c r="D19" t="s">
@@ -3553,7 +3574,7 @@
         <v>291</v>
       </c>
     </row>
-    <row r="20" spans="2:9" x14ac:dyDescent="0.35">
+    <row r="20" spans="2:9" x14ac:dyDescent="0.25">
       <c r="B20" t="s">
         <v>292</v>
       </c>
@@ -3579,7 +3600,7 @@
         <v>296</v>
       </c>
     </row>
-    <row r="21" spans="2:9" x14ac:dyDescent="0.35">
+    <row r="21" spans="2:9" x14ac:dyDescent="0.25">
       <c r="B21" t="s">
         <v>297</v>
       </c>
@@ -3605,7 +3626,7 @@
         <v>302</v>
       </c>
     </row>
-    <row r="22" spans="2:9" x14ac:dyDescent="0.35">
+    <row r="22" spans="2:9" x14ac:dyDescent="0.25">
       <c r="B22" t="s">
         <v>303</v>
       </c>
@@ -3631,7 +3652,7 @@
         <v>306</v>
       </c>
     </row>
-    <row r="23" spans="2:9" x14ac:dyDescent="0.35">
+    <row r="23" spans="2:9" x14ac:dyDescent="0.25">
       <c r="B23" t="s">
         <v>307</v>
       </c>
@@ -3654,7 +3675,7 @@
         <v>311</v>
       </c>
     </row>
-    <row r="24" spans="2:9" x14ac:dyDescent="0.35">
+    <row r="24" spans="2:9" x14ac:dyDescent="0.25">
       <c r="B24" t="s">
         <v>312</v>
       </c>
@@ -3677,7 +3698,7 @@
         <v>316</v>
       </c>
     </row>
-    <row r="25" spans="2:9" x14ac:dyDescent="0.35">
+    <row r="25" spans="2:9" x14ac:dyDescent="0.25">
       <c r="B25" t="s">
         <v>317</v>
       </c>
@@ -3697,7 +3718,7 @@
         <v>321</v>
       </c>
     </row>
-    <row r="26" spans="2:9" x14ac:dyDescent="0.35">
+    <row r="26" spans="2:9" x14ac:dyDescent="0.25">
       <c r="B26" t="s">
         <v>322</v>
       </c>
@@ -3717,7 +3738,7 @@
         <v>326</v>
       </c>
     </row>
-    <row r="27" spans="2:9" x14ac:dyDescent="0.35">
+    <row r="27" spans="2:9" x14ac:dyDescent="0.25">
       <c r="B27" t="s">
         <v>327</v>
       </c>
@@ -3737,7 +3758,7 @@
         <v>331</v>
       </c>
     </row>
-    <row r="28" spans="2:9" x14ac:dyDescent="0.35">
+    <row r="28" spans="2:9" x14ac:dyDescent="0.25">
       <c r="B28" t="s">
         <v>332</v>
       </c>
@@ -3757,7 +3778,7 @@
         <v>336</v>
       </c>
     </row>
-    <row r="29" spans="2:9" x14ac:dyDescent="0.35">
+    <row r="29" spans="2:9" x14ac:dyDescent="0.25">
       <c r="B29" t="s">
         <v>337</v>
       </c>
@@ -3777,7 +3798,7 @@
         <v>341</v>
       </c>
     </row>
-    <row r="30" spans="2:9" x14ac:dyDescent="0.35">
+    <row r="30" spans="2:9" x14ac:dyDescent="0.25">
       <c r="B30" t="s">
         <v>342</v>
       </c>
@@ -3797,7 +3818,7 @@
         <v>346</v>
       </c>
     </row>
-    <row r="31" spans="2:9" x14ac:dyDescent="0.35">
+    <row r="31" spans="2:9" x14ac:dyDescent="0.25">
       <c r="B31" t="s">
         <v>347</v>
       </c>
@@ -3817,7 +3838,7 @@
         <v>350</v>
       </c>
     </row>
-    <row r="32" spans="2:9" x14ac:dyDescent="0.35">
+    <row r="32" spans="2:9" x14ac:dyDescent="0.25">
       <c r="D32" t="s">
         <v>114</v>
       </c>
@@ -3834,7 +3855,7 @@
         <v>353</v>
       </c>
     </row>
-    <row r="33" spans="4:9" x14ac:dyDescent="0.35">
+    <row r="33" spans="4:9" x14ac:dyDescent="0.25">
       <c r="D33" t="s">
         <v>115</v>
       </c>
@@ -3851,7 +3872,7 @@
         <v>356</v>
       </c>
     </row>
-    <row r="34" spans="4:9" x14ac:dyDescent="0.35">
+    <row r="34" spans="4:9" x14ac:dyDescent="0.25">
       <c r="D34" t="s">
         <v>116</v>
       </c>
@@ -3868,7 +3889,7 @@
         <v>360</v>
       </c>
     </row>
-    <row r="35" spans="4:9" x14ac:dyDescent="0.35">
+    <row r="35" spans="4:9" x14ac:dyDescent="0.25">
       <c r="D35" t="s">
         <v>117</v>
       </c>
@@ -3885,7 +3906,7 @@
         <v>364</v>
       </c>
     </row>
-    <row r="36" spans="4:9" x14ac:dyDescent="0.35">
+    <row r="36" spans="4:9" x14ac:dyDescent="0.25">
       <c r="D36" t="s">
         <v>118</v>
       </c>
@@ -3902,7 +3923,7 @@
         <v>368</v>
       </c>
     </row>
-    <row r="37" spans="4:9" x14ac:dyDescent="0.35">
+    <row r="37" spans="4:9" x14ac:dyDescent="0.25">
       <c r="D37" t="s">
         <v>119</v>
       </c>
@@ -3919,7 +3940,7 @@
         <v>372</v>
       </c>
     </row>
-    <row r="38" spans="4:9" x14ac:dyDescent="0.35">
+    <row r="38" spans="4:9" x14ac:dyDescent="0.25">
       <c r="D38" t="s">
         <v>120</v>
       </c>
@@ -3936,7 +3957,7 @@
         <v>376</v>
       </c>
     </row>
-    <row r="39" spans="4:9" x14ac:dyDescent="0.35">
+    <row r="39" spans="4:9" x14ac:dyDescent="0.25">
       <c r="D39" t="s">
         <v>101</v>
       </c>
@@ -3953,7 +3974,7 @@
         <v>380</v>
       </c>
     </row>
-    <row r="40" spans="4:9" x14ac:dyDescent="0.35">
+    <row r="40" spans="4:9" x14ac:dyDescent="0.25">
       <c r="D40" t="s">
         <v>125</v>
       </c>
@@ -3970,7 +3991,7 @@
         <v>384</v>
       </c>
     </row>
-    <row r="41" spans="4:9" x14ac:dyDescent="0.35">
+    <row r="41" spans="4:9" x14ac:dyDescent="0.25">
       <c r="D41" t="s">
         <v>126</v>
       </c>
@@ -3987,7 +4008,7 @@
         <v>388</v>
       </c>
     </row>
-    <row r="42" spans="4:9" x14ac:dyDescent="0.35">
+    <row r="42" spans="4:9" x14ac:dyDescent="0.25">
       <c r="D42" t="s">
         <v>389</v>
       </c>
@@ -4004,7 +4025,7 @@
         <v>392</v>
       </c>
     </row>
-    <row r="43" spans="4:9" x14ac:dyDescent="0.35">
+    <row r="43" spans="4:9" x14ac:dyDescent="0.25">
       <c r="G43" t="s">
         <v>393</v>
       </c>
@@ -4015,7 +4036,7 @@
         <v>395</v>
       </c>
     </row>
-    <row r="44" spans="4:9" x14ac:dyDescent="0.35">
+    <row r="44" spans="4:9" x14ac:dyDescent="0.25">
       <c r="G44" t="s">
         <v>396</v>
       </c>
@@ -4026,7 +4047,7 @@
         <v>398</v>
       </c>
     </row>
-    <row r="45" spans="4:9" x14ac:dyDescent="0.35">
+    <row r="45" spans="4:9" x14ac:dyDescent="0.25">
       <c r="G45" t="s">
         <v>399</v>
       </c>
@@ -4037,7 +4058,7 @@
         <v>401</v>
       </c>
     </row>
-    <row r="46" spans="4:9" x14ac:dyDescent="0.35">
+    <row r="46" spans="4:9" x14ac:dyDescent="0.25">
       <c r="G46" t="s">
         <v>402</v>
       </c>
@@ -4048,7 +4069,7 @@
         <v>404</v>
       </c>
     </row>
-    <row r="47" spans="4:9" x14ac:dyDescent="0.35">
+    <row r="47" spans="4:9" x14ac:dyDescent="0.25">
       <c r="G47" t="s">
         <v>405</v>
       </c>
@@ -4059,7 +4080,7 @@
         <v>407</v>
       </c>
     </row>
-    <row r="48" spans="4:9" x14ac:dyDescent="0.35">
+    <row r="48" spans="4:9" x14ac:dyDescent="0.25">
       <c r="G48" t="s">
         <v>408</v>
       </c>
@@ -4070,7 +4091,7 @@
         <v>410</v>
       </c>
     </row>
-    <row r="49" spans="7:9" x14ac:dyDescent="0.35">
+    <row r="49" spans="7:9" x14ac:dyDescent="0.25">
       <c r="G49" t="s">
         <v>411</v>
       </c>
@@ -4081,7 +4102,7 @@
         <v>413</v>
       </c>
     </row>
-    <row r="50" spans="7:9" x14ac:dyDescent="0.35">
+    <row r="50" spans="7:9" x14ac:dyDescent="0.25">
       <c r="G50" t="s">
         <v>414</v>
       </c>
@@ -4092,7 +4113,7 @@
         <v>416</v>
       </c>
     </row>
-    <row r="51" spans="7:9" x14ac:dyDescent="0.35">
+    <row r="51" spans="7:9" x14ac:dyDescent="0.25">
       <c r="G51" t="s">
         <v>417</v>
       </c>
@@ -4103,7 +4124,7 @@
         <v>418</v>
       </c>
     </row>
-    <row r="52" spans="7:9" x14ac:dyDescent="0.35">
+    <row r="52" spans="7:9" x14ac:dyDescent="0.25">
       <c r="G52" t="s">
         <v>419</v>
       </c>
@@ -4111,252 +4132,252 @@
         <v>389</v>
       </c>
     </row>
-    <row r="53" spans="7:9" x14ac:dyDescent="0.35">
+    <row r="53" spans="7:9" x14ac:dyDescent="0.25">
       <c r="G53" t="s">
         <v>420</v>
       </c>
     </row>
-    <row r="54" spans="7:9" x14ac:dyDescent="0.35">
+    <row r="54" spans="7:9" x14ac:dyDescent="0.25">
       <c r="G54" t="s">
         <v>421</v>
       </c>
     </row>
-    <row r="55" spans="7:9" x14ac:dyDescent="0.35">
+    <row r="55" spans="7:9" x14ac:dyDescent="0.25">
       <c r="G55" t="s">
         <v>182</v>
       </c>
     </row>
-    <row r="56" spans="7:9" x14ac:dyDescent="0.35">
+    <row r="56" spans="7:9" x14ac:dyDescent="0.25">
       <c r="G56" t="s">
         <v>180</v>
       </c>
     </row>
-    <row r="57" spans="7:9" x14ac:dyDescent="0.35">
+    <row r="57" spans="7:9" x14ac:dyDescent="0.25">
       <c r="G57" t="s">
         <v>178</v>
       </c>
     </row>
-    <row r="58" spans="7:9" x14ac:dyDescent="0.35">
+    <row r="58" spans="7:9" x14ac:dyDescent="0.25">
       <c r="G58" t="s">
         <v>186</v>
       </c>
     </row>
-    <row r="59" spans="7:9" x14ac:dyDescent="0.35">
+    <row r="59" spans="7:9" x14ac:dyDescent="0.25">
       <c r="G59" t="s">
         <v>190</v>
       </c>
     </row>
-    <row r="60" spans="7:9" x14ac:dyDescent="0.35">
+    <row r="60" spans="7:9" x14ac:dyDescent="0.25">
       <c r="G60" t="s">
         <v>191</v>
       </c>
     </row>
-    <row r="61" spans="7:9" x14ac:dyDescent="0.35">
+    <row r="61" spans="7:9" x14ac:dyDescent="0.25">
       <c r="G61" t="s">
         <v>192</v>
       </c>
     </row>
-    <row r="62" spans="7:9" x14ac:dyDescent="0.35">
+    <row r="62" spans="7:9" x14ac:dyDescent="0.25">
       <c r="G62" t="s">
         <v>188</v>
       </c>
     </row>
-    <row r="63" spans="7:9" x14ac:dyDescent="0.35">
+    <row r="63" spans="7:9" x14ac:dyDescent="0.25">
       <c r="G63" t="s">
         <v>193</v>
       </c>
     </row>
-    <row r="64" spans="7:9" x14ac:dyDescent="0.35">
+    <row r="64" spans="7:9" x14ac:dyDescent="0.25">
       <c r="G64" t="s">
         <v>194</v>
       </c>
     </row>
-    <row r="65" spans="7:7" x14ac:dyDescent="0.35">
+    <row r="65" spans="7:7" x14ac:dyDescent="0.25">
       <c r="G65" t="s">
         <v>196</v>
       </c>
     </row>
-    <row r="66" spans="7:7" x14ac:dyDescent="0.35">
+    <row r="66" spans="7:7" x14ac:dyDescent="0.25">
       <c r="G66" t="s">
         <v>422</v>
       </c>
     </row>
-    <row r="67" spans="7:7" x14ac:dyDescent="0.35">
+    <row r="67" spans="7:7" x14ac:dyDescent="0.25">
       <c r="G67" t="s">
         <v>423</v>
       </c>
     </row>
-    <row r="68" spans="7:7" x14ac:dyDescent="0.35">
+    <row r="68" spans="7:7" x14ac:dyDescent="0.25">
       <c r="G68" t="s">
         <v>207</v>
       </c>
     </row>
-    <row r="69" spans="7:7" x14ac:dyDescent="0.35">
+    <row r="69" spans="7:7" x14ac:dyDescent="0.25">
       <c r="G69" t="s">
         <v>205</v>
       </c>
     </row>
-    <row r="70" spans="7:7" x14ac:dyDescent="0.35">
+    <row r="70" spans="7:7" x14ac:dyDescent="0.25">
       <c r="G70" t="s">
         <v>424</v>
       </c>
     </row>
-    <row r="71" spans="7:7" x14ac:dyDescent="0.35">
+    <row r="71" spans="7:7" x14ac:dyDescent="0.25">
       <c r="G71" t="s">
         <v>425</v>
       </c>
     </row>
-    <row r="72" spans="7:7" x14ac:dyDescent="0.35">
+    <row r="72" spans="7:7" x14ac:dyDescent="0.25">
       <c r="G72" t="s">
         <v>426</v>
       </c>
     </row>
-    <row r="73" spans="7:7" x14ac:dyDescent="0.35">
+    <row r="73" spans="7:7" x14ac:dyDescent="0.25">
       <c r="G73" t="s">
         <v>427</v>
       </c>
     </row>
-    <row r="74" spans="7:7" x14ac:dyDescent="0.35">
+    <row r="74" spans="7:7" x14ac:dyDescent="0.25">
       <c r="G74" t="s">
         <v>169</v>
       </c>
     </row>
-    <row r="75" spans="7:7" x14ac:dyDescent="0.35">
+    <row r="75" spans="7:7" x14ac:dyDescent="0.25">
       <c r="G75" t="s">
         <v>170</v>
       </c>
     </row>
-    <row r="76" spans="7:7" x14ac:dyDescent="0.35">
+    <row r="76" spans="7:7" x14ac:dyDescent="0.25">
       <c r="G76" t="s">
         <v>428</v>
       </c>
     </row>
-    <row r="77" spans="7:7" x14ac:dyDescent="0.35">
+    <row r="77" spans="7:7" x14ac:dyDescent="0.25">
       <c r="G77" t="s">
         <v>429</v>
       </c>
     </row>
-    <row r="78" spans="7:7" x14ac:dyDescent="0.35">
+    <row r="78" spans="7:7" x14ac:dyDescent="0.25">
       <c r="G78" t="s">
         <v>430</v>
       </c>
     </row>
-    <row r="79" spans="7:7" x14ac:dyDescent="0.35">
+    <row r="79" spans="7:7" x14ac:dyDescent="0.25">
       <c r="G79" t="s">
         <v>431</v>
       </c>
     </row>
-    <row r="80" spans="7:7" x14ac:dyDescent="0.35">
+    <row r="80" spans="7:7" x14ac:dyDescent="0.25">
       <c r="G80" t="s">
         <v>432</v>
       </c>
     </row>
-    <row r="81" spans="7:7" x14ac:dyDescent="0.35">
+    <row r="81" spans="7:7" x14ac:dyDescent="0.25">
       <c r="G81" t="s">
         <v>433</v>
       </c>
     </row>
-    <row r="82" spans="7:7" x14ac:dyDescent="0.35">
+    <row r="82" spans="7:7" x14ac:dyDescent="0.25">
       <c r="G82" t="s">
         <v>434</v>
       </c>
     </row>
-    <row r="83" spans="7:7" x14ac:dyDescent="0.35">
+    <row r="83" spans="7:7" x14ac:dyDescent="0.25">
       <c r="G83" t="s">
         <v>435</v>
       </c>
     </row>
-    <row r="84" spans="7:7" x14ac:dyDescent="0.35">
+    <row r="84" spans="7:7" x14ac:dyDescent="0.25">
       <c r="G84" t="s">
         <v>436</v>
       </c>
     </row>
-    <row r="85" spans="7:7" x14ac:dyDescent="0.35">
+    <row r="85" spans="7:7" x14ac:dyDescent="0.25">
       <c r="G85" t="s">
         <v>437</v>
       </c>
     </row>
-    <row r="86" spans="7:7" x14ac:dyDescent="0.35">
+    <row r="86" spans="7:7" x14ac:dyDescent="0.25">
       <c r="G86" t="s">
         <v>438</v>
       </c>
     </row>
-    <row r="87" spans="7:7" x14ac:dyDescent="0.35">
+    <row r="87" spans="7:7" x14ac:dyDescent="0.25">
       <c r="G87" t="s">
         <v>439</v>
       </c>
     </row>
-    <row r="88" spans="7:7" x14ac:dyDescent="0.35">
+    <row r="88" spans="7:7" x14ac:dyDescent="0.25">
       <c r="G88" t="s">
         <v>440</v>
       </c>
     </row>
-    <row r="89" spans="7:7" x14ac:dyDescent="0.35">
+    <row r="89" spans="7:7" x14ac:dyDescent="0.25">
       <c r="G89" t="s">
         <v>441</v>
       </c>
     </row>
-    <row r="90" spans="7:7" x14ac:dyDescent="0.35">
+    <row r="90" spans="7:7" x14ac:dyDescent="0.25">
       <c r="G90" t="s">
         <v>442</v>
       </c>
     </row>
-    <row r="91" spans="7:7" x14ac:dyDescent="0.35">
+    <row r="91" spans="7:7" x14ac:dyDescent="0.25">
       <c r="G91" t="s">
         <v>443</v>
       </c>
     </row>
-    <row r="92" spans="7:7" x14ac:dyDescent="0.35">
+    <row r="92" spans="7:7" x14ac:dyDescent="0.25">
       <c r="G92" t="s">
         <v>444</v>
       </c>
     </row>
-    <row r="93" spans="7:7" x14ac:dyDescent="0.35">
+    <row r="93" spans="7:7" x14ac:dyDescent="0.25">
       <c r="G93" t="s">
         <v>445</v>
       </c>
     </row>
-    <row r="94" spans="7:7" x14ac:dyDescent="0.35">
+    <row r="94" spans="7:7" x14ac:dyDescent="0.25">
       <c r="G94" t="s">
         <v>446</v>
       </c>
     </row>
-    <row r="95" spans="7:7" x14ac:dyDescent="0.35">
+    <row r="95" spans="7:7" x14ac:dyDescent="0.25">
       <c r="G95" t="s">
         <v>447</v>
       </c>
     </row>
-    <row r="96" spans="7:7" x14ac:dyDescent="0.35">
+    <row r="96" spans="7:7" x14ac:dyDescent="0.25">
       <c r="G96" t="s">
         <v>448</v>
       </c>
     </row>
-    <row r="97" spans="7:7" x14ac:dyDescent="0.35">
+    <row r="97" spans="7:7" x14ac:dyDescent="0.25">
       <c r="G97" t="s">
         <v>449</v>
       </c>
     </row>
-    <row r="98" spans="7:7" x14ac:dyDescent="0.35">
+    <row r="98" spans="7:7" x14ac:dyDescent="0.25">
       <c r="G98" t="s">
         <v>450</v>
       </c>
     </row>
-    <row r="99" spans="7:7" x14ac:dyDescent="0.35">
+    <row r="99" spans="7:7" x14ac:dyDescent="0.25">
       <c r="G99" t="s">
         <v>451</v>
       </c>
     </row>
-    <row r="100" spans="7:7" x14ac:dyDescent="0.35">
+    <row r="100" spans="7:7" x14ac:dyDescent="0.25">
       <c r="G100" t="s">
         <v>452</v>
       </c>
     </row>
-    <row r="101" spans="7:7" x14ac:dyDescent="0.35">
+    <row r="101" spans="7:7" x14ac:dyDescent="0.25">
       <c r="G101" t="s">
         <v>453</v>
       </c>
     </row>
-    <row r="102" spans="7:7" x14ac:dyDescent="0.35">
+    <row r="102" spans="7:7" x14ac:dyDescent="0.25">
       <c r="G102" t="s">
         <v>389</v>
       </c>
@@ -4375,20 +4396,20 @@
   <dimension ref="A1:D51"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="B34" sqref="B34"/>
+      <selection activeCell="C17" sqref="C17"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="62.1796875" customWidth="1"/>
-    <col min="2" max="2" width="64.81640625" customWidth="1"/>
-    <col min="3" max="3" width="43.81640625" customWidth="1"/>
-    <col min="12" max="12" width="19.81640625" customWidth="1"/>
-    <col min="13" max="13" width="27.1796875" customWidth="1"/>
+    <col min="1" max="1" width="62.140625" customWidth="1"/>
+    <col min="2" max="2" width="64.85546875" customWidth="1"/>
+    <col min="3" max="3" width="43.85546875" customWidth="1"/>
+    <col min="12" max="12" width="19.85546875" customWidth="1"/>
+    <col min="13" max="13" width="27.140625" customWidth="1"/>
     <col min="14" max="14" width="25" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="1" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
         <v>57</v>
       </c>
@@ -4402,7 +4423,7 @@
         <v>147</v>
       </c>
     </row>
-    <row r="2" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="2" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
         <v>21</v>
       </c>
@@ -4410,7 +4431,7 @@
         <v>148</v>
       </c>
     </row>
-    <row r="3" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="3" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
         <v>20</v>
       </c>
@@ -4418,7 +4439,7 @@
         <v>149</v>
       </c>
     </row>
-    <row r="4" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="4" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
         <v>19</v>
       </c>
@@ -4426,7 +4447,7 @@
         <v>150</v>
       </c>
     </row>
-    <row r="5" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="5" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
         <v>35</v>
       </c>
@@ -4434,7 +4455,7 @@
         <v>151</v>
       </c>
     </row>
-    <row r="6" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="6" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
         <v>35</v>
       </c>
@@ -4442,7 +4463,7 @@
         <v>152</v>
       </c>
     </row>
-    <row r="7" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="7" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
         <v>22</v>
       </c>
@@ -4450,7 +4471,7 @@
         <v>153</v>
       </c>
     </row>
-    <row r="8" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="8" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A8" t="s">
         <v>23</v>
       </c>
@@ -4458,7 +4479,7 @@
         <v>154</v>
       </c>
     </row>
-    <row r="9" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="9" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A9" t="s">
         <v>155</v>
       </c>
@@ -4466,7 +4487,7 @@
         <v>156</v>
       </c>
     </row>
-    <row r="10" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="10" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A10" t="s">
         <v>157</v>
       </c>
@@ -4474,7 +4495,7 @@
         <v>61</v>
       </c>
     </row>
-    <row r="11" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="11" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A11" t="s">
         <v>27</v>
       </c>
@@ -4482,7 +4503,7 @@
         <v>158</v>
       </c>
     </row>
-    <row r="12" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="12" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A12" t="s">
         <v>159</v>
       </c>
@@ -4490,7 +4511,7 @@
         <v>160</v>
       </c>
     </row>
-    <row r="13" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="13" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A13" t="s">
         <v>161</v>
       </c>
@@ -4498,7 +4519,7 @@
         <v>162</v>
       </c>
     </row>
-    <row r="14" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="14" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A14" t="s">
         <v>163</v>
       </c>
@@ -4506,7 +4527,7 @@
         <v>164</v>
       </c>
     </row>
-    <row r="15" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="15" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A15" t="s">
         <v>25</v>
       </c>
@@ -4514,7 +4535,7 @@
         <v>165</v>
       </c>
     </row>
-    <row r="16" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="16" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A16" t="s">
         <v>28</v>
       </c>
@@ -4522,23 +4543,23 @@
         <v>166</v>
       </c>
     </row>
-    <row r="17" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="17" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A17" t="s">
         <v>1</v>
       </c>
-      <c r="B17" t="s">
-        <v>100</v>
+      <c r="B17" s="16" t="s">
+        <v>493</v>
       </c>
       <c r="C17" t="s">
         <v>167</v>
       </c>
     </row>
-    <row r="18" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="18" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A18" t="s">
         <v>14</v>
       </c>
-      <c r="B18" t="s">
-        <v>100</v>
+      <c r="B18" s="16" t="s">
+        <v>493</v>
       </c>
       <c r="C18" t="s">
         <v>168</v>
@@ -4547,12 +4568,12 @@
         <v>169</v>
       </c>
     </row>
-    <row r="19" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="19" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A19" t="s">
         <v>13</v>
       </c>
-      <c r="B19" t="s">
-        <v>100</v>
+      <c r="B19" s="16" t="s">
+        <v>493</v>
       </c>
       <c r="C19" t="s">
         <v>168</v>
@@ -4561,29 +4582,29 @@
         <v>170</v>
       </c>
     </row>
-    <row r="20" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="20" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A20" t="s">
         <v>9</v>
       </c>
-      <c r="B20" t="s">
-        <v>100</v>
+      <c r="B20" s="16" t="s">
+        <v>493</v>
       </c>
       <c r="C20" t="s">
         <v>168</v>
       </c>
     </row>
-    <row r="21" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="21" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A21" s="4" t="s">
         <v>26</v>
       </c>
-      <c r="B21" t="s">
-        <v>100</v>
+      <c r="B21" s="16" t="s">
+        <v>493</v>
       </c>
       <c r="C21" t="s">
         <v>171</v>
       </c>
     </row>
-    <row r="22" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="22" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A22" s="4" t="s">
         <v>33</v>
       </c>
@@ -4591,7 +4612,7 @@
         <v>172</v>
       </c>
     </row>
-    <row r="23" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="23" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A23" t="s">
         <v>173</v>
       </c>
@@ -4599,7 +4620,7 @@
         <v>174</v>
       </c>
     </row>
-    <row r="24" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="24" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A24" t="s">
         <v>175</v>
       </c>
@@ -4607,7 +4628,7 @@
         <v>146</v>
       </c>
     </row>
-    <row r="25" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="25" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A25" t="s">
         <v>176</v>
       </c>
@@ -4621,7 +4642,7 @@
         <v>178</v>
       </c>
     </row>
-    <row r="26" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="26" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A26" t="s">
         <v>179</v>
       </c>
@@ -4635,7 +4656,7 @@
         <v>180</v>
       </c>
     </row>
-    <row r="27" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="27" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A27" t="s">
         <v>181</v>
       </c>
@@ -4649,7 +4670,7 @@
         <v>182</v>
       </c>
     </row>
-    <row r="28" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="28" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A28" t="s">
         <v>183</v>
       </c>
@@ -4660,7 +4681,7 @@
         <v>184</v>
       </c>
     </row>
-    <row r="29" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="29" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A29" t="s">
         <v>185</v>
       </c>
@@ -4674,7 +4695,7 @@
         <v>186</v>
       </c>
     </row>
-    <row r="30" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="30" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A30" t="s">
         <v>187</v>
       </c>
@@ -4688,7 +4709,7 @@
         <v>188</v>
       </c>
     </row>
-    <row r="31" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="31" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A31" t="s">
         <v>189</v>
       </c>
@@ -4702,7 +4723,7 @@
         <v>190</v>
       </c>
     </row>
-    <row r="32" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="32" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A32" t="s">
         <v>189</v>
       </c>
@@ -4716,7 +4737,7 @@
         <v>191</v>
       </c>
     </row>
-    <row r="33" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="33" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A33" t="s">
         <v>189</v>
       </c>
@@ -4730,7 +4751,7 @@
         <v>192</v>
       </c>
     </row>
-    <row r="34" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="34" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A34" t="s">
         <v>189</v>
       </c>
@@ -4744,7 +4765,7 @@
         <v>188</v>
       </c>
     </row>
-    <row r="35" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="35" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A35" t="s">
         <v>189</v>
       </c>
@@ -4758,7 +4779,7 @@
         <v>193</v>
       </c>
     </row>
-    <row r="36" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="36" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A36" t="s">
         <v>189</v>
       </c>
@@ -4772,7 +4793,7 @@
         <v>194</v>
       </c>
     </row>
-    <row r="37" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="37" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A37" s="7" t="s">
         <v>195</v>
       </c>
@@ -4786,7 +4807,7 @@
         <v>196</v>
       </c>
     </row>
-    <row r="38" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="38" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A38" t="s">
         <v>197</v>
       </c>
@@ -4797,7 +4818,7 @@
         <v>198</v>
       </c>
     </row>
-    <row r="39" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="39" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A39" t="s">
         <v>48</v>
       </c>
@@ -4808,7 +4829,7 @@
         <v>199</v>
       </c>
     </row>
-    <row r="40" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="40" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A40" t="s">
         <v>47</v>
       </c>
@@ -4819,7 +4840,7 @@
         <v>200</v>
       </c>
     </row>
-    <row r="41" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="41" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A41" t="s">
         <v>49</v>
       </c>
@@ -4830,7 +4851,7 @@
         <v>201</v>
       </c>
     </row>
-    <row r="42" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="42" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A42" t="s">
         <v>50</v>
       </c>
@@ -4841,7 +4862,7 @@
         <v>202</v>
       </c>
     </row>
-    <row r="43" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="43" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A43" t="s">
         <v>203</v>
       </c>
@@ -4855,7 +4876,7 @@
         <v>205</v>
       </c>
     </row>
-    <row r="44" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="44" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A44" t="s">
         <v>206</v>
       </c>
@@ -4869,7 +4890,7 @@
         <v>207</v>
       </c>
     </row>
-    <row r="45" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="45" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A45" t="s">
         <v>208</v>
       </c>
@@ -4880,7 +4901,7 @@
         <v>209</v>
       </c>
     </row>
-    <row r="46" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="46" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A46" t="s">
         <v>488</v>
       </c>
@@ -4888,7 +4909,7 @@
         <v>164</v>
       </c>
     </row>
-    <row r="47" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="47" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A47" t="s">
         <v>41</v>
       </c>
@@ -4896,7 +4917,7 @@
         <v>149</v>
       </c>
     </row>
-    <row r="48" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="48" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A48" t="s">
         <v>41</v>
       </c>
@@ -4904,7 +4925,7 @@
         <v>150</v>
       </c>
     </row>
-    <row r="49" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="49" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A49" t="s">
         <v>51</v>
       </c>
@@ -4915,7 +4936,7 @@
         <v>204</v>
       </c>
     </row>
-    <row r="50" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="50" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A50" t="s">
         <v>210</v>
       </c>
@@ -4923,7 +4944,7 @@
         <v>211</v>
       </c>
     </row>
-    <row r="51" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="51" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A51" t="s">
         <v>212</v>
       </c>
@@ -4947,17 +4968,17 @@
   <dimension ref="A1:C89"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="D20" sqref="D20:D21"/>
+      <selection activeCell="C21" sqref="C21"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="57.81640625" customWidth="1"/>
-    <col min="2" max="2" width="36.54296875" customWidth="1"/>
-    <col min="3" max="3" width="29.1796875" customWidth="1"/>
+    <col min="1" max="1" width="57.85546875" customWidth="1"/>
+    <col min="2" max="2" width="36.5703125" customWidth="1"/>
+    <col min="3" max="3" width="29.140625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="1" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
         <v>76</v>
       </c>
@@ -4968,7 +4989,7 @@
         <v>78</v>
       </c>
     </row>
-    <row r="2" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="2" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
         <v>11</v>
       </c>
@@ -4976,7 +4997,7 @@
         <v>79</v>
       </c>
     </row>
-    <row r="3" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="3" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
         <v>11</v>
       </c>
@@ -4984,7 +5005,7 @@
         <v>80</v>
       </c>
     </row>
-    <row r="4" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="4" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
         <v>11</v>
       </c>
@@ -4992,7 +5013,7 @@
         <v>81</v>
       </c>
     </row>
-    <row r="5" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="5" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
         <v>11</v>
       </c>
@@ -5000,7 +5021,7 @@
         <v>82</v>
       </c>
     </row>
-    <row r="6" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="6" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
         <v>5</v>
       </c>
@@ -5008,7 +5029,7 @@
         <v>83</v>
       </c>
     </row>
-    <row r="7" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="7" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
         <v>5</v>
       </c>
@@ -5016,7 +5037,7 @@
         <v>84</v>
       </c>
     </row>
-    <row r="8" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="8" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A8" t="s">
         <v>5</v>
       </c>
@@ -5024,7 +5045,7 @@
         <v>85</v>
       </c>
     </row>
-    <row r="9" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="9" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A9" t="s">
         <v>4</v>
       </c>
@@ -5032,7 +5053,7 @@
         <v>86</v>
       </c>
     </row>
-    <row r="10" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="10" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A10" t="s">
         <v>87</v>
       </c>
@@ -5040,7 +5061,7 @@
         <v>88</v>
       </c>
     </row>
-    <row r="11" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="11" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A11" t="s">
         <v>89</v>
       </c>
@@ -5048,7 +5069,7 @@
         <v>90</v>
       </c>
     </row>
-    <row r="12" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="12" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A12" t="s">
         <v>91</v>
       </c>
@@ -5056,7 +5077,7 @@
         <v>92</v>
       </c>
     </row>
-    <row r="13" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="13" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A13" t="s">
         <v>93</v>
       </c>
@@ -5064,7 +5085,7 @@
         <v>94</v>
       </c>
     </row>
-    <row r="14" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="14" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A14" t="s">
         <v>95</v>
       </c>
@@ -5072,7 +5093,7 @@
         <v>96</v>
       </c>
     </row>
-    <row r="15" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="15" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A15" t="s">
         <v>97</v>
       </c>
@@ -5080,7 +5101,7 @@
         <v>98</v>
       </c>
     </row>
-    <row r="16" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="16" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A16" t="s">
         <v>10</v>
       </c>
@@ -5088,7 +5109,7 @@
         <v>99</v>
       </c>
     </row>
-    <row r="17" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="17" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A17" t="s">
         <v>31</v>
       </c>
@@ -5099,7 +5120,7 @@
         <v>101</v>
       </c>
     </row>
-    <row r="18" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="18" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A18" t="s">
         <v>3</v>
       </c>
@@ -5107,7 +5128,7 @@
         <v>102</v>
       </c>
     </row>
-    <row r="19" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="19" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A19" t="s">
         <v>103</v>
       </c>
@@ -5115,7 +5136,7 @@
         <v>104</v>
       </c>
     </row>
-    <row r="20" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="20" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A20" t="s">
         <v>487</v>
       </c>
@@ -5123,7 +5144,7 @@
         <v>105</v>
       </c>
     </row>
-    <row r="21" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="21" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A21" t="s">
         <v>106</v>
       </c>
@@ -5131,7 +5152,7 @@
         <v>107</v>
       </c>
     </row>
-    <row r="22" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="22" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A22" t="s">
         <v>108</v>
       </c>
@@ -5139,7 +5160,7 @@
         <v>109</v>
       </c>
     </row>
-    <row r="23" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="23" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A23" t="s">
         <v>110</v>
       </c>
@@ -5147,7 +5168,7 @@
         <v>99</v>
       </c>
     </row>
-    <row r="24" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="24" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A24" t="s">
         <v>111</v>
       </c>
@@ -5155,7 +5176,7 @@
         <v>102</v>
       </c>
     </row>
-    <row r="25" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="25" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A25" t="s">
         <v>111</v>
       </c>
@@ -5163,7 +5184,7 @@
         <v>104</v>
       </c>
     </row>
-    <row r="26" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="26" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A26" s="4" t="s">
         <v>112</v>
       </c>
@@ -5171,7 +5192,7 @@
         <v>99</v>
       </c>
     </row>
-    <row r="27" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="27" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A27" s="4" t="s">
         <v>112</v>
       </c>
@@ -5182,7 +5203,7 @@
         <v>113</v>
       </c>
     </row>
-    <row r="28" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="28" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A28" s="4" t="s">
         <v>112</v>
       </c>
@@ -5193,7 +5214,7 @@
         <v>114</v>
       </c>
     </row>
-    <row r="29" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="29" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A29" s="4" t="s">
         <v>112</v>
       </c>
@@ -5204,7 +5225,7 @@
         <v>115</v>
       </c>
     </row>
-    <row r="30" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="30" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A30" s="4" t="s">
         <v>112</v>
       </c>
@@ -5215,7 +5236,7 @@
         <v>116</v>
       </c>
     </row>
-    <row r="31" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="31" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A31" s="4" t="s">
         <v>112</v>
       </c>
@@ -5226,7 +5247,7 @@
         <v>117</v>
       </c>
     </row>
-    <row r="32" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="32" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A32" s="4" t="s">
         <v>112</v>
       </c>
@@ -5237,7 +5258,7 @@
         <v>118</v>
       </c>
     </row>
-    <row r="33" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="33" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A33" s="4" t="s">
         <v>112</v>
       </c>
@@ -5248,7 +5269,7 @@
         <v>119</v>
       </c>
     </row>
-    <row r="34" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="34" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A34" s="4" t="s">
         <v>112</v>
       </c>
@@ -5259,7 +5280,7 @@
         <v>120</v>
       </c>
     </row>
-    <row r="35" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="35" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A35" s="4" t="s">
         <v>112</v>
       </c>
@@ -5270,7 +5291,7 @@
         <v>101</v>
       </c>
     </row>
-    <row r="36" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="36" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A36" t="s">
         <v>17</v>
       </c>
@@ -5281,7 +5302,7 @@
         <v>121</v>
       </c>
     </row>
-    <row r="37" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="37" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A37" t="s">
         <v>18</v>
       </c>
@@ -5292,7 +5313,7 @@
         <v>122</v>
       </c>
     </row>
-    <row r="38" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="38" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A38" t="s">
         <v>16</v>
       </c>
@@ -5303,7 +5324,7 @@
         <v>123</v>
       </c>
     </row>
-    <row r="39" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="39" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A39" t="s">
         <v>42</v>
       </c>
@@ -5311,7 +5332,7 @@
         <v>84</v>
       </c>
     </row>
-    <row r="40" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="40" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A40" t="s">
         <v>124</v>
       </c>
@@ -5319,7 +5340,7 @@
         <v>84</v>
       </c>
     </row>
-    <row r="41" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="41" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A41" t="s">
         <v>12</v>
       </c>
@@ -5330,7 +5351,7 @@
         <v>113</v>
       </c>
     </row>
-    <row r="42" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="42" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A42" t="s">
         <v>12</v>
       </c>
@@ -5341,7 +5362,7 @@
         <v>114</v>
       </c>
     </row>
-    <row r="43" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="43" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A43" t="s">
         <v>12</v>
       </c>
@@ -5352,7 +5373,7 @@
         <v>115</v>
       </c>
     </row>
-    <row r="44" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="44" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A44" t="s">
         <v>12</v>
       </c>
@@ -5363,7 +5384,7 @@
         <v>116</v>
       </c>
     </row>
-    <row r="45" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="45" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A45" t="s">
         <v>12</v>
       </c>
@@ -5374,7 +5395,7 @@
         <v>117</v>
       </c>
     </row>
-    <row r="46" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="46" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A46" t="s">
         <v>12</v>
       </c>
@@ -5385,7 +5406,7 @@
         <v>118</v>
       </c>
     </row>
-    <row r="47" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="47" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A47" t="s">
         <v>12</v>
       </c>
@@ -5396,7 +5417,7 @@
         <v>119</v>
       </c>
     </row>
-    <row r="48" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="48" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A48" t="s">
         <v>12</v>
       </c>
@@ -5407,7 +5428,7 @@
         <v>120</v>
       </c>
     </row>
-    <row r="49" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="49" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A49" t="s">
         <v>12</v>
       </c>
@@ -5418,7 +5439,7 @@
         <v>101</v>
       </c>
     </row>
-    <row r="50" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="50" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A50" t="s">
         <v>30</v>
       </c>
@@ -5429,7 +5450,7 @@
         <v>125</v>
       </c>
     </row>
-    <row r="51" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="51" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A51" t="s">
         <v>30</v>
       </c>
@@ -5440,7 +5461,7 @@
         <v>126</v>
       </c>
     </row>
-    <row r="52" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="52" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A52" t="s">
         <v>127</v>
       </c>
@@ -5451,7 +5472,7 @@
         <v>128</v>
       </c>
     </row>
-    <row r="53" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="53" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A53" t="s">
         <v>129</v>
       </c>
@@ -5462,7 +5483,7 @@
         <v>130</v>
       </c>
     </row>
-    <row r="54" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="54" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A54" t="s">
         <v>131</v>
       </c>
@@ -5473,9 +5494,9 @@
         <v>132</v>
       </c>
     </row>
-    <row r="55" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="55" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A55" s="4" t="s">
-        <v>4</v>
+        <v>492</v>
       </c>
       <c r="B55" t="s">
         <v>85</v>
@@ -5484,7 +5505,7 @@
         <v>133</v>
       </c>
     </row>
-    <row r="56" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="56" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A56" t="s">
         <v>134</v>
       </c>
@@ -5495,7 +5516,7 @@
         <v>135</v>
       </c>
     </row>
-    <row r="57" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="57" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A57" t="s">
         <v>134</v>
       </c>
@@ -5506,7 +5527,7 @@
         <v>136</v>
       </c>
     </row>
-    <row r="58" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="58" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A58" s="5" t="s">
         <v>37</v>
       </c>
@@ -5517,7 +5538,7 @@
         <v>125</v>
       </c>
     </row>
-    <row r="59" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="59" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A59" s="12" t="s">
         <v>30</v>
       </c>
@@ -5528,7 +5549,7 @@
         <v>126</v>
       </c>
     </row>
-    <row r="60" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="60" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A60" t="s">
         <v>43</v>
       </c>
@@ -5539,7 +5560,7 @@
         <v>130</v>
       </c>
     </row>
-    <row r="61" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="61" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A61" t="s">
         <v>43</v>
       </c>
@@ -5550,7 +5571,7 @@
         <v>135</v>
       </c>
     </row>
-    <row r="62" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="62" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A62" t="s">
         <v>43</v>
       </c>
@@ -5561,7 +5582,7 @@
         <v>137</v>
       </c>
     </row>
-    <row r="63" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="63" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A63" t="s">
         <v>43</v>
       </c>
@@ -5572,7 +5593,7 @@
         <v>136</v>
       </c>
     </row>
-    <row r="64" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="64" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A64" t="s">
         <v>43</v>
       </c>
@@ -5583,7 +5604,7 @@
         <v>138</v>
       </c>
     </row>
-    <row r="65" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="65" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A65" t="s">
         <v>43</v>
       </c>
@@ -5594,7 +5615,7 @@
         <v>128</v>
       </c>
     </row>
-    <row r="66" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="66" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A66" t="s">
         <v>43</v>
       </c>
@@ -5605,7 +5626,7 @@
         <v>139</v>
       </c>
     </row>
-    <row r="67" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="67" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A67" t="s">
         <v>43</v>
       </c>
@@ -5616,7 +5637,7 @@
         <v>132</v>
       </c>
     </row>
-    <row r="68" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="68" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A68" t="s">
         <v>43</v>
       </c>
@@ -5627,7 +5648,7 @@
         <v>140</v>
       </c>
     </row>
-    <row r="69" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="69" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A69" t="s">
         <v>43</v>
       </c>
@@ -5638,7 +5659,7 @@
         <v>141</v>
       </c>
     </row>
-    <row r="70" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="70" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A70" t="s">
         <v>43</v>
       </c>
@@ -5649,7 +5670,7 @@
         <v>142</v>
       </c>
     </row>
-    <row r="71" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="71" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A71" t="s">
         <v>143</v>
       </c>
@@ -5660,7 +5681,7 @@
         <v>139</v>
       </c>
     </row>
-    <row r="72" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="72" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A72" t="s">
         <v>144</v>
       </c>
@@ -5671,7 +5692,7 @@
         <v>119</v>
       </c>
     </row>
-    <row r="73" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="73" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A73" t="s">
         <v>145</v>
       </c>
@@ -5679,7 +5700,7 @@
         <v>99</v>
       </c>
     </row>
-    <row r="74" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="74" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A74" t="s">
         <v>145</v>
       </c>
@@ -5690,7 +5711,7 @@
         <v>113</v>
       </c>
     </row>
-    <row r="75" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="75" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A75" t="s">
         <v>145</v>
       </c>
@@ -5701,7 +5722,7 @@
         <v>115</v>
       </c>
     </row>
-    <row r="76" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="76" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A76" t="s">
         <v>145</v>
       </c>
@@ -5712,7 +5733,7 @@
         <v>117</v>
       </c>
     </row>
-    <row r="77" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="77" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A77" t="s">
         <v>145</v>
       </c>
@@ -5723,7 +5744,7 @@
         <v>118</v>
       </c>
     </row>
-    <row r="78" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="78" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A78" t="s">
         <v>145</v>
       </c>
@@ -5734,7 +5755,7 @@
         <v>119</v>
       </c>
     </row>
-    <row r="79" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="79" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A79" t="s">
         <v>145</v>
       </c>
@@ -5745,13 +5766,13 @@
         <v>120</v>
       </c>
     </row>
-    <row r="87" spans="2:2" x14ac:dyDescent="0.35">
+    <row r="87" spans="2:2" x14ac:dyDescent="0.25">
       <c r="B87" s="6"/>
     </row>
-    <row r="88" spans="2:2" x14ac:dyDescent="0.35">
+    <row r="88" spans="2:2" x14ac:dyDescent="0.25">
       <c r="B88" s="6"/>
     </row>
-    <row r="89" spans="2:2" x14ac:dyDescent="0.35">
+    <row r="89" spans="2:2" x14ac:dyDescent="0.25">
       <c r="B89" s="6"/>
     </row>
   </sheetData>
@@ -5773,15 +5794,15 @@
       <selection activeCell="B13" activeCellId="1" sqref="B26 B13"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="33.453125" customWidth="1"/>
-    <col min="2" max="2" width="47.1796875" customWidth="1"/>
-    <col min="3" max="3" width="50.1796875" customWidth="1"/>
+    <col min="1" max="1" width="33.42578125" customWidth="1"/>
+    <col min="2" max="2" width="47.140625" customWidth="1"/>
+    <col min="3" max="3" width="50.140625" customWidth="1"/>
     <col min="4" max="4" width="69" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="1" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
         <v>56</v>
       </c>
@@ -5795,7 +5816,7 @@
         <v>59</v>
       </c>
     </row>
-    <row r="2" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="2" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A2" t="b">
         <v>1</v>
       </c>
@@ -5809,7 +5830,7 @@
         <v>62</v>
       </c>
     </row>
-    <row r="3" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="3" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A3" t="b">
         <v>1</v>
       </c>
@@ -5823,7 +5844,7 @@
         <v>63</v>
       </c>
     </row>
-    <row r="4" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="4" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A4" t="b">
         <v>1</v>
       </c>
@@ -5837,7 +5858,7 @@
         <v>64</v>
       </c>
     </row>
-    <row r="5" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="5" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A5" t="b">
         <v>1</v>
       </c>
@@ -5851,7 +5872,7 @@
         <v>65</v>
       </c>
     </row>
-    <row r="6" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="6" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A6" t="b">
         <v>1</v>
       </c>
@@ -5865,7 +5886,7 @@
         <v>67</v>
       </c>
     </row>
-    <row r="7" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="7" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A7" t="b">
         <v>1</v>
       </c>
@@ -5879,7 +5900,7 @@
         <v>68</v>
       </c>
     </row>
-    <row r="8" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="8" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A8" t="b">
         <v>1</v>
       </c>
@@ -5893,7 +5914,7 @@
         <v>69</v>
       </c>
     </row>
-    <row r="9" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="9" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A9" t="b">
         <v>1</v>
       </c>
@@ -5907,7 +5928,7 @@
         <v>70</v>
       </c>
     </row>
-    <row r="10" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="10" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A10" t="b">
         <v>1</v>
       </c>
@@ -5921,7 +5942,7 @@
         <v>71</v>
       </c>
     </row>
-    <row r="11" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="11" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A11" t="b">
         <v>1</v>
       </c>
@@ -5935,7 +5956,7 @@
         <v>72</v>
       </c>
     </row>
-    <row r="12" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="12" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A12" t="b">
         <v>1</v>
       </c>
@@ -5949,7 +5970,7 @@
         <v>73</v>
       </c>
     </row>
-    <row r="13" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="13" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A13" t="b">
         <v>1</v>
       </c>
@@ -5963,7 +5984,7 @@
         <v>74</v>
       </c>
     </row>
-    <row r="14" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="14" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A14" t="b">
         <v>1</v>
       </c>
@@ -5977,7 +5998,7 @@
         <v>75</v>
       </c>
     </row>
-    <row r="15" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="15" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A15" t="b">
         <v>0</v>
       </c>
@@ -5991,7 +6012,7 @@
         <v>62</v>
       </c>
     </row>
-    <row r="16" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="16" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A16" t="b">
         <v>0</v>
       </c>
@@ -6005,7 +6026,7 @@
         <v>63</v>
       </c>
     </row>
-    <row r="17" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="17" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A17" t="b">
         <v>0</v>
       </c>
@@ -6019,7 +6040,7 @@
         <v>64</v>
       </c>
     </row>
-    <row r="18" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="18" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A18" t="b">
         <v>0</v>
       </c>
@@ -6033,7 +6054,7 @@
         <v>65</v>
       </c>
     </row>
-    <row r="19" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="19" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A19" t="b">
         <v>0</v>
       </c>
@@ -6047,7 +6068,7 @@
         <v>67</v>
       </c>
     </row>
-    <row r="20" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="20" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A20" t="b">
         <v>0</v>
       </c>
@@ -6061,7 +6082,7 @@
         <v>68</v>
       </c>
     </row>
-    <row r="21" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="21" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A21" t="b">
         <v>0</v>
       </c>
@@ -6075,7 +6096,7 @@
         <v>69</v>
       </c>
     </row>
-    <row r="22" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="22" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A22" t="b">
         <v>0</v>
       </c>
@@ -6089,7 +6110,7 @@
         <v>70</v>
       </c>
     </row>
-    <row r="23" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="23" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A23" t="b">
         <v>0</v>
       </c>
@@ -6103,7 +6124,7 @@
         <v>71</v>
       </c>
     </row>
-    <row r="24" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="24" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A24" t="b">
         <v>0</v>
       </c>
@@ -6117,7 +6138,7 @@
         <v>72</v>
       </c>
     </row>
-    <row r="25" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="25" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A25" t="b">
         <v>0</v>
       </c>
@@ -6131,7 +6152,7 @@
         <v>73</v>
       </c>
     </row>
-    <row r="26" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="26" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A26" t="b">
         <v>0</v>
       </c>
@@ -6145,7 +6166,7 @@
         <v>74</v>
       </c>
     </row>
-    <row r="27" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="27" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A27" t="b">
         <v>0</v>
       </c>
@@ -6171,15 +6192,15 @@
   <dimension ref="A1:B29"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="A28" sqref="A28"/>
+      <selection activeCell="A21" sqref="A21"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="19.81640625" customWidth="1"/>
+    <col min="1" max="1" width="19.85546875" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="1" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
         <v>474</v>
       </c>
@@ -6187,7 +6208,7 @@
         <v>477</v>
       </c>
     </row>
-    <row r="2" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="2" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
         <v>481</v>
       </c>
@@ -6195,7 +6216,7 @@
         <v>60</v>
       </c>
     </row>
-    <row r="3" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="3" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
         <v>481</v>
       </c>
@@ -6203,7 +6224,7 @@
         <v>60</v>
       </c>
     </row>
-    <row r="4" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="4" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
         <v>481</v>
       </c>
@@ -6211,7 +6232,7 @@
         <v>60</v>
       </c>
     </row>
-    <row r="5" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="5" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
         <v>481</v>
       </c>
@@ -6219,7 +6240,7 @@
         <v>60</v>
       </c>
     </row>
-    <row r="6" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="6" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
         <v>482</v>
       </c>
@@ -6227,7 +6248,7 @@
         <v>66</v>
       </c>
     </row>
-    <row r="7" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="7" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
         <v>482</v>
       </c>
@@ -6235,7 +6256,7 @@
         <v>66</v>
       </c>
     </row>
-    <row r="8" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="8" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A8" t="s">
         <v>482</v>
       </c>
@@ -6243,7 +6264,7 @@
         <v>66</v>
       </c>
     </row>
-    <row r="9" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="9" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A9" t="s">
         <v>482</v>
       </c>
@@ -6251,7 +6272,7 @@
         <v>66</v>
       </c>
     </row>
-    <row r="10" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="10" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A10" t="s">
         <v>482</v>
       </c>
@@ -6259,7 +6280,7 @@
         <v>66</v>
       </c>
     </row>
-    <row r="11" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="11" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A11" t="s">
         <v>482</v>
       </c>
@@ -6267,7 +6288,7 @@
         <v>66</v>
       </c>
     </row>
-    <row r="12" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="12" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A12" t="s">
         <v>482</v>
       </c>
@@ -6275,7 +6296,7 @@
         <v>66</v>
       </c>
     </row>
-    <row r="13" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="13" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A13" t="s">
         <v>483</v>
       </c>
@@ -6283,7 +6304,7 @@
         <v>30</v>
       </c>
     </row>
-    <row r="14" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="14" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A14" t="s">
         <v>486</v>
       </c>
@@ -6291,7 +6312,7 @@
         <v>60</v>
       </c>
     </row>
-    <row r="15" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="15" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A15" t="s">
         <v>478</v>
       </c>
@@ -6299,7 +6320,7 @@
         <v>60</v>
       </c>
     </row>
-    <row r="16" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="16" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A16" t="s">
         <v>478</v>
       </c>
@@ -6307,7 +6328,7 @@
         <v>60</v>
       </c>
     </row>
-    <row r="17" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="17" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A17" t="s">
         <v>478</v>
       </c>
@@ -6315,7 +6336,7 @@
         <v>60</v>
       </c>
     </row>
-    <row r="18" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="18" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A18" t="s">
         <v>478</v>
       </c>
@@ -6323,7 +6344,7 @@
         <v>60</v>
       </c>
     </row>
-    <row r="19" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="19" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A19" t="s">
         <v>479</v>
       </c>
@@ -6331,7 +6352,7 @@
         <v>66</v>
       </c>
     </row>
-    <row r="20" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="20" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A20" t="s">
         <v>479</v>
       </c>
@@ -6339,7 +6360,7 @@
         <v>66</v>
       </c>
     </row>
-    <row r="21" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="21" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A21" t="s">
         <v>479</v>
       </c>
@@ -6347,7 +6368,7 @@
         <v>66</v>
       </c>
     </row>
-    <row r="22" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="22" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A22" t="s">
         <v>479</v>
       </c>
@@ -6355,7 +6376,7 @@
         <v>66</v>
       </c>
     </row>
-    <row r="23" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="23" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A23" t="s">
         <v>479</v>
       </c>
@@ -6363,7 +6384,7 @@
         <v>66</v>
       </c>
     </row>
-    <row r="24" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="24" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A24" t="s">
         <v>479</v>
       </c>
@@ -6371,7 +6392,7 @@
         <v>66</v>
       </c>
     </row>
-    <row r="25" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="25" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A25" t="s">
         <v>479</v>
       </c>
@@ -6379,7 +6400,7 @@
         <v>66</v>
       </c>
     </row>
-    <row r="26" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="26" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A26" t="s">
         <v>480</v>
       </c>
@@ -6387,7 +6408,7 @@
         <v>30</v>
       </c>
     </row>
-    <row r="27" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="27" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A27" t="s">
         <v>478</v>
       </c>
@@ -6395,7 +6416,7 @@
         <v>60</v>
       </c>
     </row>
-    <row r="28" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="28" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A28" t="s">
         <v>487</v>
       </c>
@@ -6403,7 +6424,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="29" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="29" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A29" t="s">
         <v>488</v>
       </c>
@@ -6429,9 +6450,9 @@
       <selection activeCell="D73" sqref="D73"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <sheetData>
-    <row r="1" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="1" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
         <v>474</v>
       </c>
@@ -6439,7 +6460,7 @@
         <v>475</v>
       </c>
     </row>
-    <row r="2" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="2" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
         <v>11</v>
       </c>
@@ -6447,7 +6468,7 @@
         <v>454</v>
       </c>
     </row>
-    <row r="3" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="3" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
         <v>5</v>
       </c>
@@ -6455,7 +6476,7 @@
         <v>455</v>
       </c>
     </row>
-    <row r="4" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="4" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
         <v>4</v>
       </c>
@@ -6463,7 +6484,7 @@
         <v>456</v>
       </c>
     </row>
-    <row r="5" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="5" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
         <v>12</v>
       </c>
@@ -6471,7 +6492,7 @@
         <v>457</v>
       </c>
     </row>
-    <row r="6" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="6" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
         <v>10</v>
       </c>
@@ -6479,7 +6500,7 @@
         <v>458</v>
       </c>
     </row>
-    <row r="7" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="7" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
         <v>30</v>
       </c>
@@ -6487,7 +6508,7 @@
         <v>459</v>
       </c>
     </row>
-    <row r="8" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="8" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A8" t="s">
         <v>3</v>
       </c>
@@ -6495,7 +6516,7 @@
         <v>460</v>
       </c>
     </row>
-    <row r="9" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="9" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A9" t="s">
         <v>103</v>
       </c>
@@ -6503,7 +6524,7 @@
         <v>461</v>
       </c>
     </row>
-    <row r="10" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="10" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A10" t="s">
         <v>31</v>
       </c>
@@ -6511,7 +6532,7 @@
         <v>462</v>
       </c>
     </row>
-    <row r="11" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="11" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A11" t="s">
         <v>25</v>
       </c>
@@ -6519,7 +6540,7 @@
         <v>463</v>
       </c>
     </row>
-    <row r="12" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="12" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A12" t="s">
         <v>28</v>
       </c>
@@ -6527,7 +6548,7 @@
         <v>464</v>
       </c>
     </row>
-    <row r="13" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="13" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A13" t="s">
         <v>9</v>
       </c>
@@ -6535,7 +6556,7 @@
         <v>455</v>
       </c>
     </row>
-    <row r="14" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="14" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A14" t="s">
         <v>1</v>
       </c>
@@ -6543,7 +6564,7 @@
         <v>456</v>
       </c>
     </row>
-    <row r="15" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="15" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A15" t="s">
         <v>33</v>
       </c>
@@ -6551,7 +6572,7 @@
         <v>457</v>
       </c>
     </row>
-    <row r="16" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="16" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A16" t="s">
         <v>26</v>
       </c>
@@ -6559,7 +6580,7 @@
         <v>465</v>
       </c>
     </row>
-    <row r="17" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="17" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A17" t="s">
         <v>14</v>
       </c>
@@ -6567,7 +6588,7 @@
         <v>456</v>
       </c>
     </row>
-    <row r="18" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="18" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A18" t="s">
         <v>13</v>
       </c>
@@ -6575,7 +6596,7 @@
         <v>457</v>
       </c>
     </row>
-    <row r="19" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="19" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A19" t="s">
         <v>181</v>
       </c>
@@ -6583,7 +6604,7 @@
         <v>464</v>
       </c>
     </row>
-    <row r="20" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="20" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A20" t="s">
         <v>179</v>
       </c>
@@ -6591,7 +6612,7 @@
         <v>456</v>
       </c>
     </row>
-    <row r="21" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="21" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A21" t="s">
         <v>176</v>
       </c>
@@ -6599,7 +6620,7 @@
         <v>455</v>
       </c>
     </row>
-    <row r="22" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="22" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A22" t="s">
         <v>185</v>
       </c>
@@ -6607,7 +6628,7 @@
         <v>454</v>
       </c>
     </row>
-    <row r="23" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="23" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A23" t="s">
         <v>183</v>
       </c>
@@ -6615,7 +6636,7 @@
         <v>457</v>
       </c>
     </row>
-    <row r="24" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="24" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A24" t="s">
         <v>187</v>
       </c>
@@ -6623,7 +6644,7 @@
         <v>459</v>
       </c>
     </row>
-    <row r="25" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="25" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A25" t="s">
         <v>134</v>
       </c>
@@ -6631,7 +6652,7 @@
         <v>455</v>
       </c>
     </row>
-    <row r="26" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="26" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A26" t="s">
         <v>131</v>
       </c>
@@ -6639,7 +6660,7 @@
         <v>466</v>
       </c>
     </row>
-    <row r="27" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="27" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A27" t="s">
         <v>129</v>
       </c>
@@ -6647,7 +6668,7 @@
         <v>465</v>
       </c>
     </row>
-    <row r="28" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="28" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A28" t="s">
         <v>127</v>
       </c>
@@ -6655,7 +6676,7 @@
         <v>454</v>
       </c>
     </row>
-    <row r="29" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="29" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A29" t="s">
         <v>37</v>
       </c>
@@ -6663,7 +6684,7 @@
         <v>457</v>
       </c>
     </row>
-    <row r="30" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="30" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A30" t="s">
         <v>47</v>
       </c>
@@ -6671,7 +6692,7 @@
         <v>465</v>
       </c>
     </row>
-    <row r="31" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="31" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A31" t="s">
         <v>51</v>
       </c>
@@ -6679,7 +6700,7 @@
         <v>464</v>
       </c>
     </row>
-    <row r="32" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="32" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A32" t="s">
         <v>50</v>
       </c>
@@ -6687,7 +6708,7 @@
         <v>455</v>
       </c>
     </row>
-    <row r="33" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="33" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A33" t="s">
         <v>48</v>
       </c>
@@ -6695,7 +6716,7 @@
         <v>457</v>
       </c>
     </row>
-    <row r="34" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="34" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A34" t="s">
         <v>49</v>
       </c>
@@ -6703,7 +6724,7 @@
         <v>466</v>
       </c>
     </row>
-    <row r="35" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="35" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A35" t="s">
         <v>91</v>
       </c>
@@ -6711,7 +6732,7 @@
         <v>464</v>
       </c>
     </row>
-    <row r="36" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="36" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A36" t="s">
         <v>89</v>
       </c>
@@ -6719,7 +6740,7 @@
         <v>467</v>
       </c>
     </row>
-    <row r="37" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="37" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A37" t="s">
         <v>16</v>
       </c>
@@ -6727,7 +6748,7 @@
         <v>468</v>
       </c>
     </row>
-    <row r="38" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="38" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A38" t="s">
         <v>87</v>
       </c>
@@ -6735,7 +6756,7 @@
         <v>466</v>
       </c>
     </row>
-    <row r="39" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="39" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A39" t="s">
         <v>93</v>
       </c>
@@ -6743,7 +6764,7 @@
         <v>459</v>
       </c>
     </row>
-    <row r="40" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="40" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A40" t="s">
         <v>97</v>
       </c>
@@ -6751,7 +6772,7 @@
         <v>465</v>
       </c>
     </row>
-    <row r="41" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="41" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A41" t="s">
         <v>20</v>
       </c>
@@ -6759,7 +6780,7 @@
         <v>463</v>
       </c>
     </row>
-    <row r="42" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="42" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A42" t="s">
         <v>19</v>
       </c>
@@ -6767,7 +6788,7 @@
         <v>465</v>
       </c>
     </row>
-    <row r="43" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="43" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A43" t="s">
         <v>143</v>
       </c>
@@ -6775,7 +6796,7 @@
         <v>465</v>
       </c>
     </row>
-    <row r="44" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="44" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A44" t="s">
         <v>60</v>
       </c>
@@ -6783,7 +6804,7 @@
         <v>462</v>
       </c>
     </row>
-    <row r="45" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="45" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A45" t="s">
         <v>66</v>
       </c>
@@ -6791,7 +6812,7 @@
         <v>468</v>
       </c>
     </row>
-    <row r="46" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="46" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A46" t="s">
         <v>21</v>
       </c>
@@ -6799,7 +6820,7 @@
         <v>464</v>
       </c>
     </row>
-    <row r="47" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="47" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A47" t="s">
         <v>22</v>
       </c>
@@ -6807,7 +6828,7 @@
         <v>455</v>
       </c>
     </row>
-    <row r="48" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="48" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A48" t="s">
         <v>41</v>
       </c>
@@ -6815,7 +6836,7 @@
         <v>456</v>
       </c>
     </row>
-    <row r="49" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="49" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A49" t="s">
         <v>35</v>
       </c>
@@ -6823,7 +6844,7 @@
         <v>457</v>
       </c>
     </row>
-    <row r="50" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="50" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A50" t="s">
         <v>42</v>
       </c>
@@ -6831,7 +6852,7 @@
         <v>468</v>
       </c>
     </row>
-    <row r="51" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="51" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A51" t="s">
         <v>108</v>
       </c>
@@ -6839,7 +6860,7 @@
         <v>459</v>
       </c>
     </row>
-    <row r="52" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="52" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A52" t="s">
         <v>110</v>
       </c>
@@ -6847,7 +6868,7 @@
         <v>456</v>
       </c>
     </row>
-    <row r="53" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="53" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A53" t="s">
         <v>27</v>
       </c>
@@ -6855,7 +6876,7 @@
         <v>460</v>
       </c>
     </row>
-    <row r="54" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="54" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A54" t="s">
         <v>144</v>
       </c>
@@ -6863,7 +6884,7 @@
         <v>462</v>
       </c>
     </row>
-    <row r="55" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="55" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A55" t="s">
         <v>6</v>
       </c>
@@ -6871,7 +6892,7 @@
         <v>454</v>
       </c>
     </row>
-    <row r="56" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="56" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A56" t="s">
         <v>17</v>
       </c>
@@ -6879,7 +6900,7 @@
         <v>457</v>
       </c>
     </row>
-    <row r="57" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="57" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A57" t="s">
         <v>18</v>
       </c>
@@ -6887,7 +6908,7 @@
         <v>454</v>
       </c>
     </row>
-    <row r="58" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="58" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A58" t="s">
         <v>43</v>
       </c>
@@ -6895,7 +6916,7 @@
         <v>465</v>
       </c>
     </row>
-    <row r="59" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="59" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A59" t="s">
         <v>112</v>
       </c>
@@ -6903,7 +6924,7 @@
         <v>458</v>
       </c>
     </row>
-    <row r="60" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="60" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A60" t="s">
         <v>124</v>
       </c>
@@ -6911,7 +6932,7 @@
         <v>468</v>
       </c>
     </row>
-    <row r="61" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="61" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A61" t="s">
         <v>111</v>
       </c>
@@ -6919,7 +6940,7 @@
         <v>460</v>
       </c>
     </row>
-    <row r="62" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="62" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A62" t="s">
         <v>145</v>
       </c>
@@ -6927,7 +6948,7 @@
         <v>458</v>
       </c>
     </row>
-    <row r="63" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="63" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A63" t="s">
         <v>106</v>
       </c>
@@ -6935,7 +6956,7 @@
         <v>459</v>
       </c>
     </row>
-    <row r="64" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="64" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A64" t="s">
         <v>95</v>
       </c>
@@ -6943,7 +6964,7 @@
         <v>464</v>
       </c>
     </row>
-    <row r="65" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="65" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A65" t="s">
         <v>197</v>
       </c>
@@ -6951,7 +6972,7 @@
         <v>468</v>
       </c>
     </row>
-    <row r="66" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="66" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A66" t="s">
         <v>173</v>
       </c>
@@ -6959,7 +6980,7 @@
         <v>460</v>
       </c>
     </row>
-    <row r="67" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="67" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A67" t="s">
         <v>203</v>
       </c>
@@ -6967,7 +6988,7 @@
         <v>465</v>
       </c>
     </row>
-    <row r="68" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="68" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A68" t="s">
         <v>175</v>
       </c>
@@ -6975,7 +6996,7 @@
         <v>461</v>
       </c>
     </row>
-    <row r="69" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="69" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A69" t="s">
         <v>195</v>
       </c>
@@ -6983,7 +7004,7 @@
         <v>460</v>
       </c>
     </row>
-    <row r="70" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="70" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A70" t="s">
         <v>208</v>
       </c>
@@ -6991,7 +7012,7 @@
         <v>460</v>
       </c>
     </row>
-    <row r="71" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="71" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A71" t="s">
         <v>189</v>
       </c>
@@ -6999,7 +7020,7 @@
         <v>462</v>
       </c>
     </row>
-    <row r="72" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="72" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A72" t="s">
         <v>206</v>
       </c>
@@ -7007,7 +7028,7 @@
         <v>467</v>
       </c>
     </row>
-    <row r="73" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="73" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A73" t="s">
         <v>159</v>
       </c>
@@ -7015,7 +7036,7 @@
         <v>465</v>
       </c>
     </row>
-    <row r="74" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="74" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A74" t="s">
         <v>161</v>
       </c>
@@ -7023,7 +7044,7 @@
         <v>464</v>
       </c>
     </row>
-    <row r="75" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="75" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A75" t="s">
         <v>163</v>
       </c>
@@ -7031,7 +7052,7 @@
         <v>469</v>
       </c>
     </row>
-    <row r="76" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="76" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A76" t="s">
         <v>23</v>
       </c>
@@ -7039,7 +7060,7 @@
         <v>470</v>
       </c>
     </row>
-    <row r="77" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="77" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A77" t="s">
         <v>155</v>
       </c>
@@ -7047,7 +7068,7 @@
         <v>471</v>
       </c>
     </row>
-    <row r="78" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="78" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A78" t="s">
         <v>157</v>
       </c>
@@ -7055,7 +7076,7 @@
         <v>460</v>
       </c>
     </row>
-    <row r="79" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="79" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A79" t="s">
         <v>481</v>
       </c>
@@ -7063,7 +7084,7 @@
         <v>462</v>
       </c>
     </row>
-    <row r="80" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="80" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A80" t="s">
         <v>482</v>
       </c>
@@ -7071,7 +7092,7 @@
         <v>468</v>
       </c>
     </row>
-    <row r="81" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="81" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A81" t="s">
         <v>478</v>
       </c>
@@ -7079,7 +7100,7 @@
         <v>462</v>
       </c>
     </row>
-    <row r="82" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="82" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A82" t="s">
         <v>479</v>
       </c>
@@ -7087,7 +7108,7 @@
         <v>468</v>
       </c>
     </row>
-    <row r="83" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="83" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A83" t="s">
         <v>483</v>
       </c>
@@ -7095,7 +7116,7 @@
         <v>459</v>
       </c>
     </row>
-    <row r="84" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="84" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A84" t="s">
         <v>480</v>
       </c>
@@ -7103,7 +7124,7 @@
         <v>459</v>
       </c>
     </row>
-    <row r="85" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="85" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A85" t="s">
         <v>487</v>
       </c>
@@ -7111,7 +7132,7 @@
         <v>454</v>
       </c>
     </row>
-    <row r="86" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="86" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A86" t="s">
         <v>488</v>
       </c>
@@ -7133,12 +7154,12 @@
       <selection activeCell="I25" sqref="I25"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="19" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="1" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A1" s="1" t="s">
         <v>473</v>
       </c>
@@ -7146,7 +7167,7 @@
         <v>472</v>
       </c>
     </row>
-    <row r="2" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="2" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
         <v>52</v>
       </c>
@@ -7154,7 +7175,7 @@
         <v>18</v>
       </c>
     </row>
-    <row r="3" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="3" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
         <v>53</v>
       </c>
@@ -7162,7 +7183,7 @@
         <v>491</v>
       </c>
     </row>
-    <row r="4" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="4" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
         <v>54</v>
       </c>
@@ -7170,7 +7191,7 @@
         <v>500</v>
       </c>
     </row>
-    <row r="5" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="5" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
         <v>55</v>
       </c>
@@ -7191,26 +7212,26 @@
   </sheetPr>
   <dimension ref="A1:N56"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="H30" sqref="H30"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="F14" sqref="F14"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="25.1796875" customWidth="1"/>
+    <col min="1" max="1" width="25.140625" customWidth="1"/>
     <col min="2" max="5" width="25" customWidth="1"/>
-    <col min="6" max="6" width="20.1796875" customWidth="1"/>
-    <col min="7" max="7" width="25.1796875" customWidth="1"/>
-    <col min="8" max="8" width="28.1796875" customWidth="1"/>
-    <col min="9" max="9" width="34.1796875" customWidth="1"/>
-    <col min="10" max="10" width="20.81640625" customWidth="1"/>
-    <col min="11" max="11" width="20.1796875" customWidth="1"/>
-    <col min="12" max="12" width="22.81640625" customWidth="1"/>
-    <col min="13" max="13" width="21.81640625" customWidth="1"/>
-    <col min="14" max="14" width="24.81640625" customWidth="1"/>
+    <col min="6" max="6" width="20.140625" customWidth="1"/>
+    <col min="7" max="7" width="25.140625" customWidth="1"/>
+    <col min="8" max="8" width="28.140625" customWidth="1"/>
+    <col min="9" max="9" width="34.140625" customWidth="1"/>
+    <col min="10" max="10" width="20.85546875" customWidth="1"/>
+    <col min="11" max="11" width="20.140625" customWidth="1"/>
+    <col min="12" max="12" width="22.85546875" customWidth="1"/>
+    <col min="13" max="13" width="21.85546875" customWidth="1"/>
+    <col min="14" max="14" width="24.85546875" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:14" x14ac:dyDescent="0.35">
+    <row r="1" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A1" s="1"/>
       <c r="B1" s="1"/>
       <c r="D1" s="13" t="s">
@@ -7229,7 +7250,7 @@
       <c r="M1" s="14"/>
       <c r="N1" s="15"/>
     </row>
-    <row r="2" spans="1:14" x14ac:dyDescent="0.35">
+    <row r="2" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A2" s="1" t="s">
         <v>485</v>
       </c>
@@ -7273,7 +7294,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="3" spans="1:14" x14ac:dyDescent="0.35">
+    <row r="3" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
         <v>1</v>
       </c>
@@ -7299,7 +7320,7 @@
         <v>163</v>
       </c>
     </row>
-    <row r="4" spans="1:14" x14ac:dyDescent="0.35">
+    <row r="4" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
         <v>1</v>
       </c>
@@ -7325,7 +7346,7 @@
         <v>163</v>
       </c>
     </row>
-    <row r="5" spans="1:14" x14ac:dyDescent="0.35">
+    <row r="5" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
         <v>1</v>
       </c>
@@ -7351,7 +7372,7 @@
         <v>163</v>
       </c>
     </row>
-    <row r="6" spans="1:14" x14ac:dyDescent="0.35">
+    <row r="6" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
         <v>9</v>
       </c>
@@ -7386,7 +7407,7 @@
         <v>163</v>
       </c>
     </row>
-    <row r="7" spans="1:14" x14ac:dyDescent="0.35">
+    <row r="7" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
         <v>9</v>
       </c>
@@ -7409,7 +7430,7 @@
         <v>14</v>
       </c>
     </row>
-    <row r="8" spans="1:14" x14ac:dyDescent="0.35">
+    <row r="8" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A8" t="s">
         <v>15</v>
       </c>
@@ -7432,7 +7453,7 @@
         <v>18</v>
       </c>
     </row>
-    <row r="9" spans="1:14" x14ac:dyDescent="0.35">
+    <row r="9" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A9" t="s">
         <v>15</v>
       </c>
@@ -7452,7 +7473,7 @@
         <v>18</v>
       </c>
     </row>
-    <row r="10" spans="1:14" x14ac:dyDescent="0.35">
+    <row r="10" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A10" t="s">
         <v>15</v>
       </c>
@@ -7472,7 +7493,7 @@
         <v>18</v>
       </c>
     </row>
-    <row r="11" spans="1:14" x14ac:dyDescent="0.35">
+    <row r="11" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A11" t="s">
         <v>11</v>
       </c>
@@ -7501,7 +7522,7 @@
         <v>23</v>
       </c>
     </row>
-    <row r="12" spans="1:14" x14ac:dyDescent="0.35">
+    <row r="12" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A12" t="s">
         <v>11</v>
       </c>
@@ -7530,7 +7551,7 @@
         <v>23</v>
       </c>
     </row>
-    <row r="13" spans="1:14" x14ac:dyDescent="0.35">
+    <row r="13" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A13" t="s">
         <v>24</v>
       </c>
@@ -7559,7 +7580,7 @@
         <v>23</v>
       </c>
     </row>
-    <row r="14" spans="1:14" x14ac:dyDescent="0.35">
+    <row r="14" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A14" t="s">
         <v>24</v>
       </c>
@@ -7588,7 +7609,7 @@
         <v>23</v>
       </c>
     </row>
-    <row r="15" spans="1:14" x14ac:dyDescent="0.35">
+    <row r="15" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A15" t="s">
         <v>3</v>
       </c>
@@ -7623,7 +7644,7 @@
         <v>163</v>
       </c>
     </row>
-    <row r="16" spans="1:14" x14ac:dyDescent="0.35">
+    <row r="16" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A16" t="s">
         <v>29</v>
       </c>
@@ -7664,7 +7685,7 @@
         <v>163</v>
       </c>
     </row>
-    <row r="17" spans="1:13" x14ac:dyDescent="0.35">
+    <row r="17" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A17" t="s">
         <v>32</v>
       </c>
@@ -7699,7 +7720,7 @@
         <v>28</v>
       </c>
     </row>
-    <row r="18" spans="1:13" x14ac:dyDescent="0.35">
+    <row r="18" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A18" t="s">
         <v>32</v>
       </c>
@@ -7734,7 +7755,7 @@
         <v>28</v>
       </c>
     </row>
-    <row r="19" spans="1:13" x14ac:dyDescent="0.35">
+    <row r="19" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A19" t="s">
         <v>30</v>
       </c>
@@ -7757,7 +7778,7 @@
         <v>28</v>
       </c>
     </row>
-    <row r="20" spans="1:13" x14ac:dyDescent="0.35">
+    <row r="20" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A20" t="s">
         <v>30</v>
       </c>
@@ -7780,7 +7801,7 @@
         <v>28</v>
       </c>
     </row>
-    <row r="21" spans="1:13" x14ac:dyDescent="0.35">
+    <row r="21" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A21" t="s">
         <v>30</v>
       </c>
@@ -7803,7 +7824,7 @@
         <v>28</v>
       </c>
     </row>
-    <row r="22" spans="1:13" x14ac:dyDescent="0.35">
+    <row r="22" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A22" t="s">
         <v>25</v>
       </c>
@@ -7841,7 +7862,7 @@
         <v>163</v>
       </c>
     </row>
-    <row r="23" spans="1:13" x14ac:dyDescent="0.35">
+    <row r="23" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A23" t="s">
         <v>34</v>
       </c>
@@ -7858,7 +7879,7 @@
         <v>21</v>
       </c>
     </row>
-    <row r="24" spans="1:13" x14ac:dyDescent="0.35">
+    <row r="24" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A24" t="s">
         <v>34</v>
       </c>
@@ -7887,7 +7908,7 @@
         <v>23</v>
       </c>
     </row>
-    <row r="25" spans="1:13" x14ac:dyDescent="0.35">
+    <row r="25" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A25" t="s">
         <v>34</v>
       </c>
@@ -7919,7 +7940,7 @@
         <v>23</v>
       </c>
     </row>
-    <row r="26" spans="1:13" x14ac:dyDescent="0.35">
+    <row r="26" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A26" t="s">
         <v>36</v>
       </c>
@@ -7936,7 +7957,7 @@
         <v>21</v>
       </c>
     </row>
-    <row r="27" spans="1:13" x14ac:dyDescent="0.35">
+    <row r="27" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A27" t="s">
         <v>36</v>
       </c>
@@ -7965,7 +7986,7 @@
         <v>23</v>
       </c>
     </row>
-    <row r="28" spans="1:13" x14ac:dyDescent="0.35">
+    <row r="28" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A28" t="s">
         <v>36</v>
       </c>
@@ -7997,7 +8018,7 @@
         <v>23</v>
       </c>
     </row>
-    <row r="29" spans="1:13" x14ac:dyDescent="0.35">
+    <row r="29" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A29" t="s">
         <v>21</v>
       </c>
@@ -8029,7 +8050,7 @@
         <v>23</v>
       </c>
     </row>
-    <row r="30" spans="1:13" x14ac:dyDescent="0.35">
+    <row r="30" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A30" t="s">
         <v>21</v>
       </c>
@@ -8061,7 +8082,7 @@
         <v>23</v>
       </c>
     </row>
-    <row r="31" spans="1:13" x14ac:dyDescent="0.35">
+    <row r="31" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A31" t="s">
         <v>21</v>
       </c>
@@ -8093,7 +8114,7 @@
         <v>23</v>
       </c>
     </row>
-    <row r="32" spans="1:13" x14ac:dyDescent="0.35">
+    <row r="32" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A32" t="s">
         <v>38</v>
       </c>
@@ -8125,7 +8146,7 @@
         <v>23</v>
       </c>
     </row>
-    <row r="33" spans="1:13" x14ac:dyDescent="0.35">
+    <row r="33" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A33" t="s">
         <v>38</v>
       </c>
@@ -8157,7 +8178,7 @@
         <v>23</v>
       </c>
     </row>
-    <row r="34" spans="1:13" x14ac:dyDescent="0.35">
+    <row r="34" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A34" t="s">
         <v>39</v>
       </c>
@@ -8189,7 +8210,7 @@
         <v>23</v>
       </c>
     </row>
-    <row r="35" spans="1:13" x14ac:dyDescent="0.35">
+    <row r="35" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A35" t="s">
         <v>39</v>
       </c>
@@ -8221,7 +8242,7 @@
         <v>23</v>
       </c>
     </row>
-    <row r="36" spans="1:13" x14ac:dyDescent="0.35">
+    <row r="36" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A36" t="s">
         <v>40</v>
       </c>
@@ -8247,7 +8268,7 @@
         <v>22</v>
       </c>
     </row>
-    <row r="37" spans="1:13" x14ac:dyDescent="0.35">
+    <row r="37" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A37" t="s">
         <v>40</v>
       </c>
@@ -8273,7 +8294,7 @@
         <v>22</v>
       </c>
     </row>
-    <row r="38" spans="1:13" x14ac:dyDescent="0.35">
+    <row r="38" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A38" t="s">
         <v>40</v>
       </c>
@@ -8305,7 +8326,7 @@
         <v>23</v>
       </c>
     </row>
-    <row r="39" spans="1:13" x14ac:dyDescent="0.35">
+    <row r="39" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A39" t="s">
         <v>40</v>
       </c>
@@ -8337,7 +8358,7 @@
         <v>23</v>
       </c>
     </row>
-    <row r="40" spans="1:13" x14ac:dyDescent="0.35">
+    <row r="40" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A40" t="s">
         <v>40</v>
       </c>
@@ -8372,7 +8393,7 @@
         <v>23</v>
       </c>
     </row>
-    <row r="41" spans="1:13" x14ac:dyDescent="0.35">
+    <row r="41" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A41" t="s">
         <v>40</v>
       </c>
@@ -8407,7 +8428,7 @@
         <v>23</v>
       </c>
     </row>
-    <row r="42" spans="1:13" x14ac:dyDescent="0.35">
+    <row r="42" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A42" t="s">
         <v>40</v>
       </c>
@@ -8445,7 +8466,7 @@
         <v>44</v>
       </c>
     </row>
-    <row r="43" spans="1:13" x14ac:dyDescent="0.35">
+    <row r="43" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A43" t="s">
         <v>40</v>
       </c>
@@ -8483,7 +8504,7 @@
         <v>44</v>
       </c>
     </row>
-    <row r="44" spans="1:13" x14ac:dyDescent="0.35">
+    <row r="44" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A44" t="s">
         <v>45</v>
       </c>
@@ -8509,7 +8530,7 @@
         <v>22</v>
       </c>
     </row>
-    <row r="45" spans="1:13" x14ac:dyDescent="0.35">
+    <row r="45" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A45" t="s">
         <v>45</v>
       </c>
@@ -8535,7 +8556,7 @@
         <v>22</v>
       </c>
     </row>
-    <row r="46" spans="1:13" x14ac:dyDescent="0.35">
+    <row r="46" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A46" t="s">
         <v>45</v>
       </c>
@@ -8567,7 +8588,7 @@
         <v>23</v>
       </c>
     </row>
-    <row r="47" spans="1:13" x14ac:dyDescent="0.35">
+    <row r="47" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A47" t="s">
         <v>45</v>
       </c>
@@ -8599,7 +8620,7 @@
         <v>23</v>
       </c>
     </row>
-    <row r="48" spans="1:13" x14ac:dyDescent="0.35">
+    <row r="48" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A48" t="s">
         <v>45</v>
       </c>
@@ -8634,7 +8655,7 @@
         <v>23</v>
       </c>
     </row>
-    <row r="49" spans="1:13" x14ac:dyDescent="0.35">
+    <row r="49" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A49" t="s">
         <v>45</v>
       </c>
@@ -8669,7 +8690,7 @@
         <v>23</v>
       </c>
     </row>
-    <row r="50" spans="1:13" x14ac:dyDescent="0.35">
+    <row r="50" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A50" t="s">
         <v>45</v>
       </c>
@@ -8707,7 +8728,7 @@
         <v>44</v>
       </c>
     </row>
-    <row r="51" spans="1:13" x14ac:dyDescent="0.35">
+    <row r="51" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A51" t="s">
         <v>45</v>
       </c>
@@ -8745,7 +8766,7 @@
         <v>44</v>
       </c>
     </row>
-    <row r="52" spans="1:13" x14ac:dyDescent="0.35">
+    <row r="52" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A52" t="s">
         <v>46</v>
       </c>
@@ -8777,7 +8798,7 @@
         <v>23</v>
       </c>
     </row>
-    <row r="53" spans="1:13" x14ac:dyDescent="0.35">
+    <row r="53" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A53" t="s">
         <v>46</v>
       </c>
@@ -8809,7 +8830,7 @@
         <v>23</v>
       </c>
     </row>
-    <row r="54" spans="1:13" x14ac:dyDescent="0.35">
+    <row r="54" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A54" t="s">
         <v>46</v>
       </c>
@@ -8829,7 +8850,7 @@
         <v>480</v>
       </c>
     </row>
-    <row r="55" spans="1:13" x14ac:dyDescent="0.35">
+    <row r="55" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A55" t="s">
         <v>28</v>
       </c>
@@ -8864,7 +8885,7 @@
         <v>163</v>
       </c>
     </row>
-    <row r="56" spans="1:13" x14ac:dyDescent="0.35">
+    <row r="56" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A56" t="s">
         <v>28</v>
       </c>

</xml_diff>

<commit_message>
added fuels to transport
</commit_message>
<xml_diff>
--- a/config/master_config.xlsx
+++ b/config/master_config.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\hyuga.kasai\Documents\Github\9th_Visualization\9th_edition_visualisation\config\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{8612EEE1-723F-4FBB-8891-8FA4E6557CBE}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E37C6F56-FE28-46A6-96BC-50993CBADAF2}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" tabRatio="812" firstSheet="1" activeTab="7" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-14235" yWindow="-16320" windowWidth="29040" windowHeight="15840" tabRatio="812" firstSheet="1" activeTab="7" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="9th_EBT_schema" sheetId="7" r:id="rId1"/>
@@ -196,7 +196,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1489" uniqueCount="494">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1487" uniqueCount="494">
   <si>
     <t>chart_type</t>
   </si>
@@ -1684,7 +1684,7 @@
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="9" x14ac:knownFonts="1">
+  <fonts count="10" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -1748,8 +1748,15 @@
       <family val="2"/>
       <scheme val="minor"/>
     </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF9C5700"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
   </fonts>
-  <fills count="10">
+  <fills count="11">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -1801,6 +1808,11 @@
     <fill>
       <patternFill patternType="solid">
         <fgColor rgb="FFFFC7CE"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFEB9C"/>
       </patternFill>
     </fill>
   </fills>
@@ -1865,11 +1877,12 @@
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="2">
+  <cellStyleXfs count="3">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="8" fillId="9" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="9" fillId="10" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="17">
+  <cellXfs count="18">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="top"/>
@@ -1889,6 +1902,7 @@
     <xf numFmtId="0" fontId="1" fillId="6" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
     <xf numFmtId="0" fontId="1" fillId="7" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
     <xf numFmtId="0" fontId="0" fillId="8" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="8" fillId="9" borderId="0" xfId="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="top"/>
     </xf>
@@ -1898,10 +1912,11 @@
     <xf numFmtId="0" fontId="2" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="top"/>
     </xf>
-    <xf numFmtId="0" fontId="8" fillId="9" borderId="0" xfId="1"/>
+    <xf numFmtId="0" fontId="9" fillId="10" borderId="0" xfId="2"/>
   </cellXfs>
-  <cellStyles count="2">
+  <cellStyles count="3">
     <cellStyle name="Bad" xfId="1" builtinId="27"/>
+    <cellStyle name="Neutral" xfId="2" builtinId="28"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
@@ -4395,8 +4410,8 @@
   </sheetPr>
   <dimension ref="A1:D51"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="C17" sqref="C17"/>
+    <sheetView topLeftCell="A7" workbookViewId="0">
+      <selection activeCell="A16" sqref="A16"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -4547,7 +4562,7 @@
       <c r="A17" t="s">
         <v>1</v>
       </c>
-      <c r="B17" s="16" t="s">
+      <c r="B17" s="13" t="s">
         <v>493</v>
       </c>
       <c r="C17" t="s">
@@ -4558,7 +4573,7 @@
       <c r="A18" t="s">
         <v>14</v>
       </c>
-      <c r="B18" s="16" t="s">
+      <c r="B18" s="13" t="s">
         <v>493</v>
       </c>
       <c r="C18" t="s">
@@ -4572,7 +4587,7 @@
       <c r="A19" t="s">
         <v>13</v>
       </c>
-      <c r="B19" s="16" t="s">
+      <c r="B19" s="13" t="s">
         <v>493</v>
       </c>
       <c r="C19" t="s">
@@ -4586,7 +4601,7 @@
       <c r="A20" t="s">
         <v>9</v>
       </c>
-      <c r="B20" s="16" t="s">
+      <c r="B20" s="13" t="s">
         <v>493</v>
       </c>
       <c r="C20" t="s">
@@ -4597,7 +4612,7 @@
       <c r="A21" s="4" t="s">
         <v>26</v>
       </c>
-      <c r="B21" s="16" t="s">
+      <c r="B21" s="13" t="s">
         <v>493</v>
       </c>
       <c r="C21" t="s">
@@ -7212,8 +7227,8 @@
   </sheetPr>
   <dimension ref="A1:N56"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="F14" sqref="F14"/>
+    <sheetView tabSelected="1" topLeftCell="C20" workbookViewId="0">
+      <selection activeCell="K57" sqref="K57"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -7234,21 +7249,21 @@
     <row r="1" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A1" s="1"/>
       <c r="B1" s="1"/>
-      <c r="D1" s="13" t="s">
+      <c r="D1" s="14" t="s">
         <v>489</v>
       </c>
-      <c r="E1" s="15"/>
-      <c r="F1" s="13" t="s">
+      <c r="E1" s="16"/>
+      <c r="F1" s="14" t="s">
         <v>476</v>
       </c>
-      <c r="G1" s="14"/>
-      <c r="H1" s="14"/>
-      <c r="I1" s="14"/>
-      <c r="J1" s="14"/>
-      <c r="K1" s="14"/>
-      <c r="L1" s="14"/>
-      <c r="M1" s="14"/>
-      <c r="N1" s="15"/>
+      <c r="G1" s="15"/>
+      <c r="H1" s="15"/>
+      <c r="I1" s="15"/>
+      <c r="J1" s="15"/>
+      <c r="K1" s="15"/>
+      <c r="L1" s="15"/>
+      <c r="M1" s="15"/>
+      <c r="N1" s="16"/>
     </row>
     <row r="2" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A2" s="1" t="s">
@@ -8863,25 +8878,22 @@
       <c r="D55" t="s">
         <v>28</v>
       </c>
-      <c r="F55" t="s">
-        <v>47</v>
-      </c>
-      <c r="G55" t="s">
-        <v>48</v>
-      </c>
-      <c r="H55" t="s">
-        <v>26</v>
-      </c>
-      <c r="I55" t="s">
-        <v>49</v>
-      </c>
-      <c r="J55" t="s">
-        <v>50</v>
-      </c>
-      <c r="K55" t="s">
-        <v>51</v>
-      </c>
-      <c r="L55" t="s">
+      <c r="F55" s="17" t="s">
+        <v>11</v>
+      </c>
+      <c r="G55" s="17" t="s">
+        <v>5</v>
+      </c>
+      <c r="H55" s="17" t="s">
+        <v>4</v>
+      </c>
+      <c r="I55" s="17" t="s">
+        <v>3</v>
+      </c>
+      <c r="J55" s="17" t="s">
+        <v>31</v>
+      </c>
+      <c r="K55" s="17" t="s">
         <v>163</v>
       </c>
     </row>
@@ -8898,25 +8910,22 @@
       <c r="D56" t="s">
         <v>28</v>
       </c>
-      <c r="F56" t="s">
-        <v>47</v>
-      </c>
-      <c r="G56" t="s">
-        <v>48</v>
-      </c>
-      <c r="H56" t="s">
-        <v>26</v>
-      </c>
-      <c r="I56" t="s">
-        <v>49</v>
-      </c>
-      <c r="J56" t="s">
-        <v>50</v>
-      </c>
-      <c r="K56" t="s">
-        <v>51</v>
-      </c>
-      <c r="L56" t="s">
+      <c r="F56" s="17" t="s">
+        <v>11</v>
+      </c>
+      <c r="G56" s="17" t="s">
+        <v>5</v>
+      </c>
+      <c r="H56" s="17" t="s">
+        <v>4</v>
+      </c>
+      <c r="I56" s="17" t="s">
+        <v>3</v>
+      </c>
+      <c r="J56" s="17" t="s">
+        <v>31</v>
+      </c>
+      <c r="K56" s="17" t="s">
         <v>163</v>
       </c>
     </row>

</xml_diff>

<commit_message>
changed crossing (vertical dotted line)
</commit_message>
<xml_diff>
--- a/config/master_config.xlsx
+++ b/config/master_config.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="26529"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="26731"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\hyuga.kasai\Documents\Github\9th_Visualization\9th_edition_visualisation\config\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{8612EEE1-723F-4FBB-8891-8FA4E6557CBE}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{9491FA88-72D6-43DF-BF02-90E76F15DB4D}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" tabRatio="812" firstSheet="1" activeTab="7" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="22050" yWindow="-16395" windowWidth="29040" windowHeight="15840" tabRatio="812" firstSheet="1" activeTab="6" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="9th_EBT_schema" sheetId="7" r:id="rId1"/>
@@ -1671,13 +1671,13 @@
     <t>Other_fuels</t>
   </si>
   <si>
-    <t>['2000', '2010', '2018', '2020', '2030', '2040', '2050', '2060', '2070']</t>
-  </si>
-  <si>
     <t>Gas?</t>
   </si>
   <si>
     <t>16_others_dummy</t>
+  </si>
+  <si>
+    <t>['2000', '2010', '2020', '2030', '2040', '2050', '2060', '2070']</t>
   </si>
 </sst>
 </file>
@@ -1889,6 +1889,7 @@
     <xf numFmtId="0" fontId="1" fillId="6" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
     <xf numFmtId="0" fontId="1" fillId="7" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
     <xf numFmtId="0" fontId="0" fillId="8" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="8" fillId="9" borderId="0" xfId="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="top"/>
     </xf>
@@ -1898,7 +1899,6 @@
     <xf numFmtId="0" fontId="2" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="top"/>
     </xf>
-    <xf numFmtId="0" fontId="8" fillId="9" borderId="0" xfId="1"/>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="Bad" xfId="1" builtinId="27"/>
@@ -4547,8 +4547,8 @@
       <c r="A17" t="s">
         <v>1</v>
       </c>
-      <c r="B17" s="16" t="s">
-        <v>493</v>
+      <c r="B17" s="13" t="s">
+        <v>492</v>
       </c>
       <c r="C17" t="s">
         <v>167</v>
@@ -4558,8 +4558,8 @@
       <c r="A18" t="s">
         <v>14</v>
       </c>
-      <c r="B18" s="16" t="s">
-        <v>493</v>
+      <c r="B18" s="13" t="s">
+        <v>492</v>
       </c>
       <c r="C18" t="s">
         <v>168</v>
@@ -4572,8 +4572,8 @@
       <c r="A19" t="s">
         <v>13</v>
       </c>
-      <c r="B19" s="16" t="s">
-        <v>493</v>
+      <c r="B19" s="13" t="s">
+        <v>492</v>
       </c>
       <c r="C19" t="s">
         <v>168</v>
@@ -4586,8 +4586,8 @@
       <c r="A20" t="s">
         <v>9</v>
       </c>
-      <c r="B20" s="16" t="s">
-        <v>493</v>
+      <c r="B20" s="13" t="s">
+        <v>492</v>
       </c>
       <c r="C20" t="s">
         <v>168</v>
@@ -4597,8 +4597,8 @@
       <c r="A21" s="4" t="s">
         <v>26</v>
       </c>
-      <c r="B21" s="16" t="s">
-        <v>493</v>
+      <c r="B21" s="13" t="s">
+        <v>492</v>
       </c>
       <c r="C21" t="s">
         <v>171</v>
@@ -5496,7 +5496,7 @@
     </row>
     <row r="55" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A55" s="4" t="s">
-        <v>492</v>
+        <v>491</v>
       </c>
       <c r="B55" t="s">
         <v>85</v>
@@ -7150,8 +7150,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{8FD61665-6B06-460E-828D-1570B45BB2AE}">
   <dimension ref="A1:B5"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="I25" sqref="I25"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="B3" sqref="B3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -7180,7 +7180,7 @@
         <v>53</v>
       </c>
       <c r="B3" t="s">
-        <v>491</v>
+        <v>493</v>
       </c>
     </row>
     <row r="4" spans="1:2" x14ac:dyDescent="0.25">
@@ -7212,7 +7212,7 @@
   </sheetPr>
   <dimension ref="A1:N56"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="F14" sqref="F14"/>
     </sheetView>
   </sheetViews>
@@ -7234,21 +7234,21 @@
     <row r="1" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A1" s="1"/>
       <c r="B1" s="1"/>
-      <c r="D1" s="13" t="s">
+      <c r="D1" s="14" t="s">
         <v>489</v>
       </c>
-      <c r="E1" s="15"/>
-      <c r="F1" s="13" t="s">
+      <c r="E1" s="16"/>
+      <c r="F1" s="14" t="s">
         <v>476</v>
       </c>
-      <c r="G1" s="14"/>
-      <c r="H1" s="14"/>
-      <c r="I1" s="14"/>
-      <c r="J1" s="14"/>
-      <c r="K1" s="14"/>
-      <c r="L1" s="14"/>
-      <c r="M1" s="14"/>
-      <c r="N1" s="15"/>
+      <c r="G1" s="15"/>
+      <c r="H1" s="15"/>
+      <c r="I1" s="15"/>
+      <c r="J1" s="15"/>
+      <c r="K1" s="15"/>
+      <c r="L1" s="15"/>
+      <c r="M1" s="15"/>
+      <c r="N1" s="16"/>
     </row>
     <row r="2" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A2" s="1" t="s">

</xml_diff>

<commit_message>
cleaned up a heap
</commit_message>
<xml_diff>
--- a/config/master_config.xlsx
+++ b/config/master_config.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="26529"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="26731"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\hyuga.kasai\Documents\Github\9th_Visualization\9th_edition_visualisation\config\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\APERC\9th_edition_visualisation\config\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E37C6F56-FE28-46A6-96BC-50993CBADAF2}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{94194DB3-31BD-432C-AC60-49A8F9907E60}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-14235" yWindow="-16320" windowWidth="29040" windowHeight="15840" tabRatio="812" firstSheet="1" activeTab="7" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="1755" yWindow="-16320" windowWidth="29040" windowHeight="15840" tabRatio="812" activeTab="7" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="9th_EBT_schema" sheetId="7" r:id="rId1"/>
@@ -196,7 +196,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1487" uniqueCount="494">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1517" uniqueCount="494">
   <si>
     <t>chart_type</t>
   </si>
@@ -1903,6 +1903,7 @@
     <xf numFmtId="0" fontId="1" fillId="7" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
     <xf numFmtId="0" fontId="0" fillId="8" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="0" fontId="8" fillId="9" borderId="0" xfId="1"/>
+    <xf numFmtId="0" fontId="9" fillId="10" borderId="0" xfId="2"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="top"/>
     </xf>
@@ -1912,7 +1913,6 @@
     <xf numFmtId="0" fontId="2" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="top"/>
     </xf>
-    <xf numFmtId="0" fontId="9" fillId="10" borderId="0" xfId="2"/>
   </cellXfs>
   <cellStyles count="3">
     <cellStyle name="Bad" xfId="1" builtinId="27"/>
@@ -3116,29 +3116,29 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{A000B41E-5923-4013-B542-E4247E89557C}">
   <dimension ref="A1:I102"/>
   <sheetViews>
-    <sheetView showGridLines="0" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <selection activeCell="C45" sqref="C45"/>
+    <sheetView showGridLines="0" topLeftCell="A13" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
+      <selection activeCell="E45" sqref="E45"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <cols>
-    <col min="1" max="1" width="12.85546875" customWidth="1"/>
+    <col min="1" max="1" width="12.81640625" customWidth="1"/>
     <col min="2" max="2" width="11" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="26.140625" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="42.42578125" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="33.5703125" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="45.140625" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="41.140625" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="28.5703125" bestFit="1" customWidth="1"/>
-    <col min="9" max="9" width="40.85546875" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="26.1796875" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="42.453125" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="33.54296875" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="45.1796875" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="41.1796875" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="28.54296875" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="40.81640625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A1" s="8" t="s">
         <v>214</v>
       </c>
     </row>
-    <row r="3" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A3" s="9" t="s">
         <v>215</v>
       </c>
@@ -3167,7 +3167,7 @@
         <v>218</v>
       </c>
     </row>
-    <row r="4" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A4" t="s">
         <v>219</v>
       </c>
@@ -3196,7 +3196,7 @@
         <v>224</v>
       </c>
     </row>
-    <row r="5" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A5" t="s">
         <v>225</v>
       </c>
@@ -3225,7 +3225,7 @@
         <v>230</v>
       </c>
     </row>
-    <row r="6" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:9" x14ac:dyDescent="0.35">
       <c r="B6" t="s">
         <v>231</v>
       </c>
@@ -3251,7 +3251,7 @@
         <v>234</v>
       </c>
     </row>
-    <row r="7" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:9" x14ac:dyDescent="0.35">
       <c r="B7" t="s">
         <v>235</v>
       </c>
@@ -3277,7 +3277,7 @@
         <v>239</v>
       </c>
     </row>
-    <row r="8" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:9" x14ac:dyDescent="0.35">
       <c r="B8" t="s">
         <v>240</v>
       </c>
@@ -3303,7 +3303,7 @@
         <v>244</v>
       </c>
     </row>
-    <row r="9" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:9" x14ac:dyDescent="0.35">
       <c r="B9" t="s">
         <v>245</v>
       </c>
@@ -3329,7 +3329,7 @@
         <v>250</v>
       </c>
     </row>
-    <row r="10" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:9" x14ac:dyDescent="0.35">
       <c r="B10" t="s">
         <v>251</v>
       </c>
@@ -3355,7 +3355,7 @@
         <v>254</v>
       </c>
     </row>
-    <row r="11" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:9" x14ac:dyDescent="0.35">
       <c r="B11" t="s">
         <v>255</v>
       </c>
@@ -3381,7 +3381,7 @@
         <v>258</v>
       </c>
     </row>
-    <row r="12" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:9" x14ac:dyDescent="0.35">
       <c r="B12" t="s">
         <v>259</v>
       </c>
@@ -3407,7 +3407,7 @@
         <v>262</v>
       </c>
     </row>
-    <row r="13" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:9" x14ac:dyDescent="0.35">
       <c r="B13" t="s">
         <v>263</v>
       </c>
@@ -3433,7 +3433,7 @@
         <v>266</v>
       </c>
     </row>
-    <row r="14" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:9" x14ac:dyDescent="0.35">
       <c r="B14" t="s">
         <v>267</v>
       </c>
@@ -3459,7 +3459,7 @@
         <v>270</v>
       </c>
     </row>
-    <row r="15" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:9" x14ac:dyDescent="0.35">
       <c r="B15" t="s">
         <v>271</v>
       </c>
@@ -3485,7 +3485,7 @@
         <v>274</v>
       </c>
     </row>
-    <row r="16" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:9" x14ac:dyDescent="0.35">
       <c r="B16" t="s">
         <v>275</v>
       </c>
@@ -3511,7 +3511,7 @@
         <v>278</v>
       </c>
     </row>
-    <row r="17" spans="2:9" x14ac:dyDescent="0.25">
+    <row r="17" spans="2:9" x14ac:dyDescent="0.35">
       <c r="B17" t="s">
         <v>279</v>
       </c>
@@ -3537,7 +3537,7 @@
         <v>282</v>
       </c>
     </row>
-    <row r="18" spans="2:9" x14ac:dyDescent="0.25">
+    <row r="18" spans="2:9" x14ac:dyDescent="0.35">
       <c r="B18" t="s">
         <v>283</v>
       </c>
@@ -3563,7 +3563,7 @@
         <v>286</v>
       </c>
     </row>
-    <row r="19" spans="2:9" x14ac:dyDescent="0.25">
+    <row r="19" spans="2:9" x14ac:dyDescent="0.35">
       <c r="B19" t="s">
         <v>287</v>
       </c>
@@ -3589,7 +3589,7 @@
         <v>291</v>
       </c>
     </row>
-    <row r="20" spans="2:9" x14ac:dyDescent="0.25">
+    <row r="20" spans="2:9" x14ac:dyDescent="0.35">
       <c r="B20" t="s">
         <v>292</v>
       </c>
@@ -3615,7 +3615,7 @@
         <v>296</v>
       </c>
     </row>
-    <row r="21" spans="2:9" x14ac:dyDescent="0.25">
+    <row r="21" spans="2:9" x14ac:dyDescent="0.35">
       <c r="B21" t="s">
         <v>297</v>
       </c>
@@ -3641,7 +3641,7 @@
         <v>302</v>
       </c>
     </row>
-    <row r="22" spans="2:9" x14ac:dyDescent="0.25">
+    <row r="22" spans="2:9" x14ac:dyDescent="0.35">
       <c r="B22" t="s">
         <v>303</v>
       </c>
@@ -3667,7 +3667,7 @@
         <v>306</v>
       </c>
     </row>
-    <row r="23" spans="2:9" x14ac:dyDescent="0.25">
+    <row r="23" spans="2:9" x14ac:dyDescent="0.35">
       <c r="B23" t="s">
         <v>307</v>
       </c>
@@ -3690,7 +3690,7 @@
         <v>311</v>
       </c>
     </row>
-    <row r="24" spans="2:9" x14ac:dyDescent="0.25">
+    <row r="24" spans="2:9" x14ac:dyDescent="0.35">
       <c r="B24" t="s">
         <v>312</v>
       </c>
@@ -3713,7 +3713,7 @@
         <v>316</v>
       </c>
     </row>
-    <row r="25" spans="2:9" x14ac:dyDescent="0.25">
+    <row r="25" spans="2:9" x14ac:dyDescent="0.35">
       <c r="B25" t="s">
         <v>317</v>
       </c>
@@ -3733,7 +3733,7 @@
         <v>321</v>
       </c>
     </row>
-    <row r="26" spans="2:9" x14ac:dyDescent="0.25">
+    <row r="26" spans="2:9" x14ac:dyDescent="0.35">
       <c r="B26" t="s">
         <v>322</v>
       </c>
@@ -3753,7 +3753,7 @@
         <v>326</v>
       </c>
     </row>
-    <row r="27" spans="2:9" x14ac:dyDescent="0.25">
+    <row r="27" spans="2:9" x14ac:dyDescent="0.35">
       <c r="B27" t="s">
         <v>327</v>
       </c>
@@ -3773,7 +3773,7 @@
         <v>331</v>
       </c>
     </row>
-    <row r="28" spans="2:9" x14ac:dyDescent="0.25">
+    <row r="28" spans="2:9" x14ac:dyDescent="0.35">
       <c r="B28" t="s">
         <v>332</v>
       </c>
@@ -3793,7 +3793,7 @@
         <v>336</v>
       </c>
     </row>
-    <row r="29" spans="2:9" x14ac:dyDescent="0.25">
+    <row r="29" spans="2:9" x14ac:dyDescent="0.35">
       <c r="B29" t="s">
         <v>337</v>
       </c>
@@ -3813,7 +3813,7 @@
         <v>341</v>
       </c>
     </row>
-    <row r="30" spans="2:9" x14ac:dyDescent="0.25">
+    <row r="30" spans="2:9" x14ac:dyDescent="0.35">
       <c r="B30" t="s">
         <v>342</v>
       </c>
@@ -3833,7 +3833,7 @@
         <v>346</v>
       </c>
     </row>
-    <row r="31" spans="2:9" x14ac:dyDescent="0.25">
+    <row r="31" spans="2:9" x14ac:dyDescent="0.35">
       <c r="B31" t="s">
         <v>347</v>
       </c>
@@ -3853,7 +3853,7 @@
         <v>350</v>
       </c>
     </row>
-    <row r="32" spans="2:9" x14ac:dyDescent="0.25">
+    <row r="32" spans="2:9" x14ac:dyDescent="0.35">
       <c r="D32" t="s">
         <v>114</v>
       </c>
@@ -3870,7 +3870,7 @@
         <v>353</v>
       </c>
     </row>
-    <row r="33" spans="4:9" x14ac:dyDescent="0.25">
+    <row r="33" spans="4:9" x14ac:dyDescent="0.35">
       <c r="D33" t="s">
         <v>115</v>
       </c>
@@ -3887,7 +3887,7 @@
         <v>356</v>
       </c>
     </row>
-    <row r="34" spans="4:9" x14ac:dyDescent="0.25">
+    <row r="34" spans="4:9" x14ac:dyDescent="0.35">
       <c r="D34" t="s">
         <v>116</v>
       </c>
@@ -3904,7 +3904,7 @@
         <v>360</v>
       </c>
     </row>
-    <row r="35" spans="4:9" x14ac:dyDescent="0.25">
+    <row r="35" spans="4:9" x14ac:dyDescent="0.35">
       <c r="D35" t="s">
         <v>117</v>
       </c>
@@ -3921,7 +3921,7 @@
         <v>364</v>
       </c>
     </row>
-    <row r="36" spans="4:9" x14ac:dyDescent="0.25">
+    <row r="36" spans="4:9" x14ac:dyDescent="0.35">
       <c r="D36" t="s">
         <v>118</v>
       </c>
@@ -3938,7 +3938,7 @@
         <v>368</v>
       </c>
     </row>
-    <row r="37" spans="4:9" x14ac:dyDescent="0.25">
+    <row r="37" spans="4:9" x14ac:dyDescent="0.35">
       <c r="D37" t="s">
         <v>119</v>
       </c>
@@ -3955,7 +3955,7 @@
         <v>372</v>
       </c>
     </row>
-    <row r="38" spans="4:9" x14ac:dyDescent="0.25">
+    <row r="38" spans="4:9" x14ac:dyDescent="0.35">
       <c r="D38" t="s">
         <v>120</v>
       </c>
@@ -3972,7 +3972,7 @@
         <v>376</v>
       </c>
     </row>
-    <row r="39" spans="4:9" x14ac:dyDescent="0.25">
+    <row r="39" spans="4:9" x14ac:dyDescent="0.35">
       <c r="D39" t="s">
         <v>101</v>
       </c>
@@ -3989,7 +3989,7 @@
         <v>380</v>
       </c>
     </row>
-    <row r="40" spans="4:9" x14ac:dyDescent="0.25">
+    <row r="40" spans="4:9" x14ac:dyDescent="0.35">
       <c r="D40" t="s">
         <v>125</v>
       </c>
@@ -4006,7 +4006,7 @@
         <v>384</v>
       </c>
     </row>
-    <row r="41" spans="4:9" x14ac:dyDescent="0.25">
+    <row r="41" spans="4:9" x14ac:dyDescent="0.35">
       <c r="D41" t="s">
         <v>126</v>
       </c>
@@ -4023,7 +4023,7 @@
         <v>388</v>
       </c>
     </row>
-    <row r="42" spans="4:9" x14ac:dyDescent="0.25">
+    <row r="42" spans="4:9" x14ac:dyDescent="0.35">
       <c r="D42" t="s">
         <v>389</v>
       </c>
@@ -4040,7 +4040,7 @@
         <v>392</v>
       </c>
     </row>
-    <row r="43" spans="4:9" x14ac:dyDescent="0.25">
+    <row r="43" spans="4:9" x14ac:dyDescent="0.35">
       <c r="G43" t="s">
         <v>393</v>
       </c>
@@ -4051,7 +4051,7 @@
         <v>395</v>
       </c>
     </row>
-    <row r="44" spans="4:9" x14ac:dyDescent="0.25">
+    <row r="44" spans="4:9" x14ac:dyDescent="0.35">
       <c r="G44" t="s">
         <v>396</v>
       </c>
@@ -4062,7 +4062,7 @@
         <v>398</v>
       </c>
     </row>
-    <row r="45" spans="4:9" x14ac:dyDescent="0.25">
+    <row r="45" spans="4:9" x14ac:dyDescent="0.35">
       <c r="G45" t="s">
         <v>399</v>
       </c>
@@ -4073,7 +4073,7 @@
         <v>401</v>
       </c>
     </row>
-    <row r="46" spans="4:9" x14ac:dyDescent="0.25">
+    <row r="46" spans="4:9" x14ac:dyDescent="0.35">
       <c r="G46" t="s">
         <v>402</v>
       </c>
@@ -4084,7 +4084,7 @@
         <v>404</v>
       </c>
     </row>
-    <row r="47" spans="4:9" x14ac:dyDescent="0.25">
+    <row r="47" spans="4:9" x14ac:dyDescent="0.35">
       <c r="G47" t="s">
         <v>405</v>
       </c>
@@ -4095,7 +4095,7 @@
         <v>407</v>
       </c>
     </row>
-    <row r="48" spans="4:9" x14ac:dyDescent="0.25">
+    <row r="48" spans="4:9" x14ac:dyDescent="0.35">
       <c r="G48" t="s">
         <v>408</v>
       </c>
@@ -4106,7 +4106,7 @@
         <v>410</v>
       </c>
     </row>
-    <row r="49" spans="7:9" x14ac:dyDescent="0.25">
+    <row r="49" spans="7:9" x14ac:dyDescent="0.35">
       <c r="G49" t="s">
         <v>411</v>
       </c>
@@ -4117,7 +4117,7 @@
         <v>413</v>
       </c>
     </row>
-    <row r="50" spans="7:9" x14ac:dyDescent="0.25">
+    <row r="50" spans="7:9" x14ac:dyDescent="0.35">
       <c r="G50" t="s">
         <v>414</v>
       </c>
@@ -4128,7 +4128,7 @@
         <v>416</v>
       </c>
     </row>
-    <row r="51" spans="7:9" x14ac:dyDescent="0.25">
+    <row r="51" spans="7:9" x14ac:dyDescent="0.35">
       <c r="G51" t="s">
         <v>417</v>
       </c>
@@ -4139,7 +4139,7 @@
         <v>418</v>
       </c>
     </row>
-    <row r="52" spans="7:9" x14ac:dyDescent="0.25">
+    <row r="52" spans="7:9" x14ac:dyDescent="0.35">
       <c r="G52" t="s">
         <v>419</v>
       </c>
@@ -4147,252 +4147,252 @@
         <v>389</v>
       </c>
     </row>
-    <row r="53" spans="7:9" x14ac:dyDescent="0.25">
+    <row r="53" spans="7:9" x14ac:dyDescent="0.35">
       <c r="G53" t="s">
         <v>420</v>
       </c>
     </row>
-    <row r="54" spans="7:9" x14ac:dyDescent="0.25">
+    <row r="54" spans="7:9" x14ac:dyDescent="0.35">
       <c r="G54" t="s">
         <v>421</v>
       </c>
     </row>
-    <row r="55" spans="7:9" x14ac:dyDescent="0.25">
+    <row r="55" spans="7:9" x14ac:dyDescent="0.35">
       <c r="G55" t="s">
         <v>182</v>
       </c>
     </row>
-    <row r="56" spans="7:9" x14ac:dyDescent="0.25">
+    <row r="56" spans="7:9" x14ac:dyDescent="0.35">
       <c r="G56" t="s">
         <v>180</v>
       </c>
     </row>
-    <row r="57" spans="7:9" x14ac:dyDescent="0.25">
+    <row r="57" spans="7:9" x14ac:dyDescent="0.35">
       <c r="G57" t="s">
         <v>178</v>
       </c>
     </row>
-    <row r="58" spans="7:9" x14ac:dyDescent="0.25">
+    <row r="58" spans="7:9" x14ac:dyDescent="0.35">
       <c r="G58" t="s">
         <v>186</v>
       </c>
     </row>
-    <row r="59" spans="7:9" x14ac:dyDescent="0.25">
+    <row r="59" spans="7:9" x14ac:dyDescent="0.35">
       <c r="G59" t="s">
         <v>190</v>
       </c>
     </row>
-    <row r="60" spans="7:9" x14ac:dyDescent="0.25">
+    <row r="60" spans="7:9" x14ac:dyDescent="0.35">
       <c r="G60" t="s">
         <v>191</v>
       </c>
     </row>
-    <row r="61" spans="7:9" x14ac:dyDescent="0.25">
+    <row r="61" spans="7:9" x14ac:dyDescent="0.35">
       <c r="G61" t="s">
         <v>192</v>
       </c>
     </row>
-    <row r="62" spans="7:9" x14ac:dyDescent="0.25">
+    <row r="62" spans="7:9" x14ac:dyDescent="0.35">
       <c r="G62" t="s">
         <v>188</v>
       </c>
     </row>
-    <row r="63" spans="7:9" x14ac:dyDescent="0.25">
+    <row r="63" spans="7:9" x14ac:dyDescent="0.35">
       <c r="G63" t="s">
         <v>193</v>
       </c>
     </row>
-    <row r="64" spans="7:9" x14ac:dyDescent="0.25">
+    <row r="64" spans="7:9" x14ac:dyDescent="0.35">
       <c r="G64" t="s">
         <v>194</v>
       </c>
     </row>
-    <row r="65" spans="7:7" x14ac:dyDescent="0.25">
+    <row r="65" spans="7:7" x14ac:dyDescent="0.35">
       <c r="G65" t="s">
         <v>196</v>
       </c>
     </row>
-    <row r="66" spans="7:7" x14ac:dyDescent="0.25">
+    <row r="66" spans="7:7" x14ac:dyDescent="0.35">
       <c r="G66" t="s">
         <v>422</v>
       </c>
     </row>
-    <row r="67" spans="7:7" x14ac:dyDescent="0.25">
+    <row r="67" spans="7:7" x14ac:dyDescent="0.35">
       <c r="G67" t="s">
         <v>423</v>
       </c>
     </row>
-    <row r="68" spans="7:7" x14ac:dyDescent="0.25">
+    <row r="68" spans="7:7" x14ac:dyDescent="0.35">
       <c r="G68" t="s">
         <v>207</v>
       </c>
     </row>
-    <row r="69" spans="7:7" x14ac:dyDescent="0.25">
+    <row r="69" spans="7:7" x14ac:dyDescent="0.35">
       <c r="G69" t="s">
         <v>205</v>
       </c>
     </row>
-    <row r="70" spans="7:7" x14ac:dyDescent="0.25">
+    <row r="70" spans="7:7" x14ac:dyDescent="0.35">
       <c r="G70" t="s">
         <v>424</v>
       </c>
     </row>
-    <row r="71" spans="7:7" x14ac:dyDescent="0.25">
+    <row r="71" spans="7:7" x14ac:dyDescent="0.35">
       <c r="G71" t="s">
         <v>425</v>
       </c>
     </row>
-    <row r="72" spans="7:7" x14ac:dyDescent="0.25">
+    <row r="72" spans="7:7" x14ac:dyDescent="0.35">
       <c r="G72" t="s">
         <v>426</v>
       </c>
     </row>
-    <row r="73" spans="7:7" x14ac:dyDescent="0.25">
+    <row r="73" spans="7:7" x14ac:dyDescent="0.35">
       <c r="G73" t="s">
         <v>427</v>
       </c>
     </row>
-    <row r="74" spans="7:7" x14ac:dyDescent="0.25">
+    <row r="74" spans="7:7" x14ac:dyDescent="0.35">
       <c r="G74" t="s">
         <v>169</v>
       </c>
     </row>
-    <row r="75" spans="7:7" x14ac:dyDescent="0.25">
+    <row r="75" spans="7:7" x14ac:dyDescent="0.35">
       <c r="G75" t="s">
         <v>170</v>
       </c>
     </row>
-    <row r="76" spans="7:7" x14ac:dyDescent="0.25">
+    <row r="76" spans="7:7" x14ac:dyDescent="0.35">
       <c r="G76" t="s">
         <v>428</v>
       </c>
     </row>
-    <row r="77" spans="7:7" x14ac:dyDescent="0.25">
+    <row r="77" spans="7:7" x14ac:dyDescent="0.35">
       <c r="G77" t="s">
         <v>429</v>
       </c>
     </row>
-    <row r="78" spans="7:7" x14ac:dyDescent="0.25">
+    <row r="78" spans="7:7" x14ac:dyDescent="0.35">
       <c r="G78" t="s">
         <v>430</v>
       </c>
     </row>
-    <row r="79" spans="7:7" x14ac:dyDescent="0.25">
+    <row r="79" spans="7:7" x14ac:dyDescent="0.35">
       <c r="G79" t="s">
         <v>431</v>
       </c>
     </row>
-    <row r="80" spans="7:7" x14ac:dyDescent="0.25">
+    <row r="80" spans="7:7" x14ac:dyDescent="0.35">
       <c r="G80" t="s">
         <v>432</v>
       </c>
     </row>
-    <row r="81" spans="7:7" x14ac:dyDescent="0.25">
+    <row r="81" spans="7:7" x14ac:dyDescent="0.35">
       <c r="G81" t="s">
         <v>433</v>
       </c>
     </row>
-    <row r="82" spans="7:7" x14ac:dyDescent="0.25">
+    <row r="82" spans="7:7" x14ac:dyDescent="0.35">
       <c r="G82" t="s">
         <v>434</v>
       </c>
     </row>
-    <row r="83" spans="7:7" x14ac:dyDescent="0.25">
+    <row r="83" spans="7:7" x14ac:dyDescent="0.35">
       <c r="G83" t="s">
         <v>435</v>
       </c>
     </row>
-    <row r="84" spans="7:7" x14ac:dyDescent="0.25">
+    <row r="84" spans="7:7" x14ac:dyDescent="0.35">
       <c r="G84" t="s">
         <v>436</v>
       </c>
     </row>
-    <row r="85" spans="7:7" x14ac:dyDescent="0.25">
+    <row r="85" spans="7:7" x14ac:dyDescent="0.35">
       <c r="G85" t="s">
         <v>437</v>
       </c>
     </row>
-    <row r="86" spans="7:7" x14ac:dyDescent="0.25">
+    <row r="86" spans="7:7" x14ac:dyDescent="0.35">
       <c r="G86" t="s">
         <v>438</v>
       </c>
     </row>
-    <row r="87" spans="7:7" x14ac:dyDescent="0.25">
+    <row r="87" spans="7:7" x14ac:dyDescent="0.35">
       <c r="G87" t="s">
         <v>439</v>
       </c>
     </row>
-    <row r="88" spans="7:7" x14ac:dyDescent="0.25">
+    <row r="88" spans="7:7" x14ac:dyDescent="0.35">
       <c r="G88" t="s">
         <v>440</v>
       </c>
     </row>
-    <row r="89" spans="7:7" x14ac:dyDescent="0.25">
+    <row r="89" spans="7:7" x14ac:dyDescent="0.35">
       <c r="G89" t="s">
         <v>441</v>
       </c>
     </row>
-    <row r="90" spans="7:7" x14ac:dyDescent="0.25">
+    <row r="90" spans="7:7" x14ac:dyDescent="0.35">
       <c r="G90" t="s">
         <v>442</v>
       </c>
     </row>
-    <row r="91" spans="7:7" x14ac:dyDescent="0.25">
+    <row r="91" spans="7:7" x14ac:dyDescent="0.35">
       <c r="G91" t="s">
         <v>443</v>
       </c>
     </row>
-    <row r="92" spans="7:7" x14ac:dyDescent="0.25">
+    <row r="92" spans="7:7" x14ac:dyDescent="0.35">
       <c r="G92" t="s">
         <v>444</v>
       </c>
     </row>
-    <row r="93" spans="7:7" x14ac:dyDescent="0.25">
+    <row r="93" spans="7:7" x14ac:dyDescent="0.35">
       <c r="G93" t="s">
         <v>445</v>
       </c>
     </row>
-    <row r="94" spans="7:7" x14ac:dyDescent="0.25">
+    <row r="94" spans="7:7" x14ac:dyDescent="0.35">
       <c r="G94" t="s">
         <v>446</v>
       </c>
     </row>
-    <row r="95" spans="7:7" x14ac:dyDescent="0.25">
+    <row r="95" spans="7:7" x14ac:dyDescent="0.35">
       <c r="G95" t="s">
         <v>447</v>
       </c>
     </row>
-    <row r="96" spans="7:7" x14ac:dyDescent="0.25">
+    <row r="96" spans="7:7" x14ac:dyDescent="0.35">
       <c r="G96" t="s">
         <v>448</v>
       </c>
     </row>
-    <row r="97" spans="7:7" x14ac:dyDescent="0.25">
+    <row r="97" spans="7:7" x14ac:dyDescent="0.35">
       <c r="G97" t="s">
         <v>449</v>
       </c>
     </row>
-    <row r="98" spans="7:7" x14ac:dyDescent="0.25">
+    <row r="98" spans="7:7" x14ac:dyDescent="0.35">
       <c r="G98" t="s">
         <v>450</v>
       </c>
     </row>
-    <row r="99" spans="7:7" x14ac:dyDescent="0.25">
+    <row r="99" spans="7:7" x14ac:dyDescent="0.35">
       <c r="G99" t="s">
         <v>451</v>
       </c>
     </row>
-    <row r="100" spans="7:7" x14ac:dyDescent="0.25">
+    <row r="100" spans="7:7" x14ac:dyDescent="0.35">
       <c r="G100" t="s">
         <v>452</v>
       </c>
     </row>
-    <row r="101" spans="7:7" x14ac:dyDescent="0.25">
+    <row r="101" spans="7:7" x14ac:dyDescent="0.35">
       <c r="G101" t="s">
         <v>453</v>
       </c>
     </row>
-    <row r="102" spans="7:7" x14ac:dyDescent="0.25">
+    <row r="102" spans="7:7" x14ac:dyDescent="0.35">
       <c r="G102" t="s">
         <v>389</v>
       </c>
@@ -4410,21 +4410,21 @@
   </sheetPr>
   <dimension ref="A1:D51"/>
   <sheetViews>
-    <sheetView topLeftCell="A7" workbookViewId="0">
-      <selection activeCell="A16" sqref="A16"/>
+    <sheetView topLeftCell="A22" workbookViewId="0">
+      <selection activeCell="B49" sqref="B49"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <cols>
-    <col min="1" max="1" width="62.140625" customWidth="1"/>
-    <col min="2" max="2" width="64.85546875" customWidth="1"/>
-    <col min="3" max="3" width="43.85546875" customWidth="1"/>
-    <col min="12" max="12" width="19.85546875" customWidth="1"/>
-    <col min="13" max="13" width="27.140625" customWidth="1"/>
+    <col min="1" max="1" width="62.1796875" customWidth="1"/>
+    <col min="2" max="2" width="64.81640625" customWidth="1"/>
+    <col min="3" max="3" width="43.81640625" customWidth="1"/>
+    <col min="12" max="12" width="19.81640625" customWidth="1"/>
+    <col min="13" max="13" width="27.1796875" customWidth="1"/>
     <col min="14" max="14" width="25" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A1" t="s">
         <v>57</v>
       </c>
@@ -4438,7 +4438,7 @@
         <v>147</v>
       </c>
     </row>
-    <row r="2" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A2" t="s">
         <v>21</v>
       </c>
@@ -4446,7 +4446,7 @@
         <v>148</v>
       </c>
     </row>
-    <row r="3" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A3" t="s">
         <v>20</v>
       </c>
@@ -4454,7 +4454,7 @@
         <v>149</v>
       </c>
     </row>
-    <row r="4" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A4" t="s">
         <v>19</v>
       </c>
@@ -4462,7 +4462,7 @@
         <v>150</v>
       </c>
     </row>
-    <row r="5" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A5" t="s">
         <v>35</v>
       </c>
@@ -4470,7 +4470,7 @@
         <v>151</v>
       </c>
     </row>
-    <row r="6" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A6" t="s">
         <v>35</v>
       </c>
@@ -4478,7 +4478,7 @@
         <v>152</v>
       </c>
     </row>
-    <row r="7" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A7" t="s">
         <v>22</v>
       </c>
@@ -4486,7 +4486,7 @@
         <v>153</v>
       </c>
     </row>
-    <row r="8" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A8" t="s">
         <v>23</v>
       </c>
@@ -4494,7 +4494,7 @@
         <v>154</v>
       </c>
     </row>
-    <row r="9" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A9" t="s">
         <v>155</v>
       </c>
@@ -4502,7 +4502,7 @@
         <v>156</v>
       </c>
     </row>
-    <row r="10" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A10" t="s">
         <v>157</v>
       </c>
@@ -4510,7 +4510,7 @@
         <v>61</v>
       </c>
     </row>
-    <row r="11" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A11" t="s">
         <v>27</v>
       </c>
@@ -4518,7 +4518,7 @@
         <v>158</v>
       </c>
     </row>
-    <row r="12" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A12" t="s">
         <v>159</v>
       </c>
@@ -4526,7 +4526,7 @@
         <v>160</v>
       </c>
     </row>
-    <row r="13" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A13" t="s">
         <v>161</v>
       </c>
@@ -4534,7 +4534,7 @@
         <v>162</v>
       </c>
     </row>
-    <row r="14" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A14" t="s">
         <v>163</v>
       </c>
@@ -4542,7 +4542,7 @@
         <v>164</v>
       </c>
     </row>
-    <row r="15" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A15" t="s">
         <v>25</v>
       </c>
@@ -4550,7 +4550,7 @@
         <v>165</v>
       </c>
     </row>
-    <row r="16" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A16" t="s">
         <v>28</v>
       </c>
@@ -4558,7 +4558,7 @@
         <v>166</v>
       </c>
     </row>
-    <row r="17" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A17" t="s">
         <v>1</v>
       </c>
@@ -4569,7 +4569,7 @@
         <v>167</v>
       </c>
     </row>
-    <row r="18" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="18" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A18" t="s">
         <v>14</v>
       </c>
@@ -4583,7 +4583,7 @@
         <v>169</v>
       </c>
     </row>
-    <row r="19" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="19" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A19" t="s">
         <v>13</v>
       </c>
@@ -4597,7 +4597,7 @@
         <v>170</v>
       </c>
     </row>
-    <row r="20" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="20" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A20" t="s">
         <v>9</v>
       </c>
@@ -4608,7 +4608,7 @@
         <v>168</v>
       </c>
     </row>
-    <row r="21" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="21" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A21" s="4" t="s">
         <v>26</v>
       </c>
@@ -4619,7 +4619,7 @@
         <v>171</v>
       </c>
     </row>
-    <row r="22" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="22" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A22" s="4" t="s">
         <v>33</v>
       </c>
@@ -4627,7 +4627,7 @@
         <v>172</v>
       </c>
     </row>
-    <row r="23" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="23" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A23" t="s">
         <v>173</v>
       </c>
@@ -4635,7 +4635,7 @@
         <v>174</v>
       </c>
     </row>
-    <row r="24" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="24" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A24" t="s">
         <v>175</v>
       </c>
@@ -4643,7 +4643,7 @@
         <v>146</v>
       </c>
     </row>
-    <row r="25" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="25" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A25" t="s">
         <v>176</v>
       </c>
@@ -4657,7 +4657,7 @@
         <v>178</v>
       </c>
     </row>
-    <row r="26" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="26" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A26" t="s">
         <v>179</v>
       </c>
@@ -4671,7 +4671,7 @@
         <v>180</v>
       </c>
     </row>
-    <row r="27" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="27" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A27" t="s">
         <v>181</v>
       </c>
@@ -4685,7 +4685,7 @@
         <v>182</v>
       </c>
     </row>
-    <row r="28" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="28" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A28" t="s">
         <v>183</v>
       </c>
@@ -4696,7 +4696,7 @@
         <v>184</v>
       </c>
     </row>
-    <row r="29" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="29" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A29" t="s">
         <v>185</v>
       </c>
@@ -4710,7 +4710,7 @@
         <v>186</v>
       </c>
     </row>
-    <row r="30" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="30" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A30" t="s">
         <v>187</v>
       </c>
@@ -4724,7 +4724,7 @@
         <v>188</v>
       </c>
     </row>
-    <row r="31" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="31" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A31" t="s">
         <v>189</v>
       </c>
@@ -4738,7 +4738,7 @@
         <v>190</v>
       </c>
     </row>
-    <row r="32" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="32" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A32" t="s">
         <v>189</v>
       </c>
@@ -4752,7 +4752,7 @@
         <v>191</v>
       </c>
     </row>
-    <row r="33" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="33" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A33" t="s">
         <v>189</v>
       </c>
@@ -4766,7 +4766,7 @@
         <v>192</v>
       </c>
     </row>
-    <row r="34" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="34" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A34" t="s">
         <v>189</v>
       </c>
@@ -4780,7 +4780,7 @@
         <v>188</v>
       </c>
     </row>
-    <row r="35" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="35" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A35" t="s">
         <v>189</v>
       </c>
@@ -4794,7 +4794,7 @@
         <v>193</v>
       </c>
     </row>
-    <row r="36" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="36" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A36" t="s">
         <v>189</v>
       </c>
@@ -4808,7 +4808,7 @@
         <v>194</v>
       </c>
     </row>
-    <row r="37" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="37" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A37" s="7" t="s">
         <v>195</v>
       </c>
@@ -4822,7 +4822,7 @@
         <v>196</v>
       </c>
     </row>
-    <row r="38" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="38" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A38" t="s">
         <v>197</v>
       </c>
@@ -4833,7 +4833,7 @@
         <v>198</v>
       </c>
     </row>
-    <row r="39" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="39" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A39" t="s">
         <v>48</v>
       </c>
@@ -4844,7 +4844,7 @@
         <v>199</v>
       </c>
     </row>
-    <row r="40" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="40" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A40" t="s">
         <v>47</v>
       </c>
@@ -4855,7 +4855,7 @@
         <v>200</v>
       </c>
     </row>
-    <row r="41" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="41" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A41" t="s">
         <v>49</v>
       </c>
@@ -4866,7 +4866,7 @@
         <v>201</v>
       </c>
     </row>
-    <row r="42" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="42" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A42" t="s">
         <v>50</v>
       </c>
@@ -4877,7 +4877,7 @@
         <v>202</v>
       </c>
     </row>
-    <row r="43" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="43" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A43" t="s">
         <v>203</v>
       </c>
@@ -4891,7 +4891,7 @@
         <v>205</v>
       </c>
     </row>
-    <row r="44" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="44" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A44" t="s">
         <v>206</v>
       </c>
@@ -4905,7 +4905,7 @@
         <v>207</v>
       </c>
     </row>
-    <row r="45" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="45" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A45" t="s">
         <v>208</v>
       </c>
@@ -4916,7 +4916,7 @@
         <v>209</v>
       </c>
     </row>
-    <row r="46" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="46" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A46" t="s">
         <v>488</v>
       </c>
@@ -4924,7 +4924,7 @@
         <v>164</v>
       </c>
     </row>
-    <row r="47" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="47" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A47" t="s">
         <v>41</v>
       </c>
@@ -4932,7 +4932,7 @@
         <v>149</v>
       </c>
     </row>
-    <row r="48" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="48" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A48" t="s">
         <v>41</v>
       </c>
@@ -4940,7 +4940,7 @@
         <v>150</v>
       </c>
     </row>
-    <row r="49" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="49" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A49" t="s">
         <v>51</v>
       </c>
@@ -4951,7 +4951,7 @@
         <v>204</v>
       </c>
     </row>
-    <row r="50" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="50" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A50" t="s">
         <v>210</v>
       </c>
@@ -4959,7 +4959,7 @@
         <v>211</v>
       </c>
     </row>
-    <row r="51" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="51" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A51" t="s">
         <v>212</v>
       </c>
@@ -4986,14 +4986,14 @@
       <selection activeCell="C21" sqref="C21"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <cols>
-    <col min="1" max="1" width="57.85546875" customWidth="1"/>
-    <col min="2" max="2" width="36.5703125" customWidth="1"/>
-    <col min="3" max="3" width="29.140625" customWidth="1"/>
+    <col min="1" max="1" width="57.81640625" customWidth="1"/>
+    <col min="2" max="2" width="36.54296875" customWidth="1"/>
+    <col min="3" max="3" width="29.1796875" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A1" t="s">
         <v>76</v>
       </c>
@@ -5004,7 +5004,7 @@
         <v>78</v>
       </c>
     </row>
-    <row r="2" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A2" t="s">
         <v>11</v>
       </c>
@@ -5012,7 +5012,7 @@
         <v>79</v>
       </c>
     </row>
-    <row r="3" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A3" t="s">
         <v>11</v>
       </c>
@@ -5020,7 +5020,7 @@
         <v>80</v>
       </c>
     </row>
-    <row r="4" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A4" t="s">
         <v>11</v>
       </c>
@@ -5028,7 +5028,7 @@
         <v>81</v>
       </c>
     </row>
-    <row r="5" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A5" t="s">
         <v>11</v>
       </c>
@@ -5036,7 +5036,7 @@
         <v>82</v>
       </c>
     </row>
-    <row r="6" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A6" t="s">
         <v>5</v>
       </c>
@@ -5044,7 +5044,7 @@
         <v>83</v>
       </c>
     </row>
-    <row r="7" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A7" t="s">
         <v>5</v>
       </c>
@@ -5052,7 +5052,7 @@
         <v>84</v>
       </c>
     </row>
-    <row r="8" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A8" t="s">
         <v>5</v>
       </c>
@@ -5060,7 +5060,7 @@
         <v>85</v>
       </c>
     </row>
-    <row r="9" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A9" t="s">
         <v>4</v>
       </c>
@@ -5068,7 +5068,7 @@
         <v>86</v>
       </c>
     </row>
-    <row r="10" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A10" t="s">
         <v>87</v>
       </c>
@@ -5076,7 +5076,7 @@
         <v>88</v>
       </c>
     </row>
-    <row r="11" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A11" t="s">
         <v>89</v>
       </c>
@@ -5084,7 +5084,7 @@
         <v>90</v>
       </c>
     </row>
-    <row r="12" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A12" t="s">
         <v>91</v>
       </c>
@@ -5092,7 +5092,7 @@
         <v>92</v>
       </c>
     </row>
-    <row r="13" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A13" t="s">
         <v>93</v>
       </c>
@@ -5100,7 +5100,7 @@
         <v>94</v>
       </c>
     </row>
-    <row r="14" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A14" t="s">
         <v>95</v>
       </c>
@@ -5108,7 +5108,7 @@
         <v>96</v>
       </c>
     </row>
-    <row r="15" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A15" t="s">
         <v>97</v>
       </c>
@@ -5116,7 +5116,7 @@
         <v>98</v>
       </c>
     </row>
-    <row r="16" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A16" t="s">
         <v>10</v>
       </c>
@@ -5124,7 +5124,7 @@
         <v>99</v>
       </c>
     </row>
-    <row r="17" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A17" t="s">
         <v>31</v>
       </c>
@@ -5135,7 +5135,7 @@
         <v>101</v>
       </c>
     </row>
-    <row r="18" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="18" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A18" t="s">
         <v>3</v>
       </c>
@@ -5143,7 +5143,7 @@
         <v>102</v>
       </c>
     </row>
-    <row r="19" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="19" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A19" t="s">
         <v>103</v>
       </c>
@@ -5151,7 +5151,7 @@
         <v>104</v>
       </c>
     </row>
-    <row r="20" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="20" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A20" t="s">
         <v>487</v>
       </c>
@@ -5159,7 +5159,7 @@
         <v>105</v>
       </c>
     </row>
-    <row r="21" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="21" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A21" t="s">
         <v>106</v>
       </c>
@@ -5167,7 +5167,7 @@
         <v>107</v>
       </c>
     </row>
-    <row r="22" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="22" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A22" t="s">
         <v>108</v>
       </c>
@@ -5175,7 +5175,7 @@
         <v>109</v>
       </c>
     </row>
-    <row r="23" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="23" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A23" t="s">
         <v>110</v>
       </c>
@@ -5183,7 +5183,7 @@
         <v>99</v>
       </c>
     </row>
-    <row r="24" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="24" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A24" t="s">
         <v>111</v>
       </c>
@@ -5191,7 +5191,7 @@
         <v>102</v>
       </c>
     </row>
-    <row r="25" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="25" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A25" t="s">
         <v>111</v>
       </c>
@@ -5199,7 +5199,7 @@
         <v>104</v>
       </c>
     </row>
-    <row r="26" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="26" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A26" s="4" t="s">
         <v>112</v>
       </c>
@@ -5207,7 +5207,7 @@
         <v>99</v>
       </c>
     </row>
-    <row r="27" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="27" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A27" s="4" t="s">
         <v>112</v>
       </c>
@@ -5218,7 +5218,7 @@
         <v>113</v>
       </c>
     </row>
-    <row r="28" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="28" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A28" s="4" t="s">
         <v>112</v>
       </c>
@@ -5229,7 +5229,7 @@
         <v>114</v>
       </c>
     </row>
-    <row r="29" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="29" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A29" s="4" t="s">
         <v>112</v>
       </c>
@@ -5240,7 +5240,7 @@
         <v>115</v>
       </c>
     </row>
-    <row r="30" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="30" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A30" s="4" t="s">
         <v>112</v>
       </c>
@@ -5251,7 +5251,7 @@
         <v>116</v>
       </c>
     </row>
-    <row r="31" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="31" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A31" s="4" t="s">
         <v>112</v>
       </c>
@@ -5262,7 +5262,7 @@
         <v>117</v>
       </c>
     </row>
-    <row r="32" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="32" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A32" s="4" t="s">
         <v>112</v>
       </c>
@@ -5273,7 +5273,7 @@
         <v>118</v>
       </c>
     </row>
-    <row r="33" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="33" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A33" s="4" t="s">
         <v>112</v>
       </c>
@@ -5284,7 +5284,7 @@
         <v>119</v>
       </c>
     </row>
-    <row r="34" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="34" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A34" s="4" t="s">
         <v>112</v>
       </c>
@@ -5295,7 +5295,7 @@
         <v>120</v>
       </c>
     </row>
-    <row r="35" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="35" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A35" s="4" t="s">
         <v>112</v>
       </c>
@@ -5306,7 +5306,7 @@
         <v>101</v>
       </c>
     </row>
-    <row r="36" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="36" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A36" t="s">
         <v>17</v>
       </c>
@@ -5317,7 +5317,7 @@
         <v>121</v>
       </c>
     </row>
-    <row r="37" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="37" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A37" t="s">
         <v>18</v>
       </c>
@@ -5328,7 +5328,7 @@
         <v>122</v>
       </c>
     </row>
-    <row r="38" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="38" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A38" t="s">
         <v>16</v>
       </c>
@@ -5339,7 +5339,7 @@
         <v>123</v>
       </c>
     </row>
-    <row r="39" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="39" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A39" t="s">
         <v>42</v>
       </c>
@@ -5347,7 +5347,7 @@
         <v>84</v>
       </c>
     </row>
-    <row r="40" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="40" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A40" t="s">
         <v>124</v>
       </c>
@@ -5355,7 +5355,7 @@
         <v>84</v>
       </c>
     </row>
-    <row r="41" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="41" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A41" t="s">
         <v>12</v>
       </c>
@@ -5366,7 +5366,7 @@
         <v>113</v>
       </c>
     </row>
-    <row r="42" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="42" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A42" t="s">
         <v>12</v>
       </c>
@@ -5377,7 +5377,7 @@
         <v>114</v>
       </c>
     </row>
-    <row r="43" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="43" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A43" t="s">
         <v>12</v>
       </c>
@@ -5388,7 +5388,7 @@
         <v>115</v>
       </c>
     </row>
-    <row r="44" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="44" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A44" t="s">
         <v>12</v>
       </c>
@@ -5399,7 +5399,7 @@
         <v>116</v>
       </c>
     </row>
-    <row r="45" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="45" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A45" t="s">
         <v>12</v>
       </c>
@@ -5410,7 +5410,7 @@
         <v>117</v>
       </c>
     </row>
-    <row r="46" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="46" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A46" t="s">
         <v>12</v>
       </c>
@@ -5421,7 +5421,7 @@
         <v>118</v>
       </c>
     </row>
-    <row r="47" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="47" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A47" t="s">
         <v>12</v>
       </c>
@@ -5432,7 +5432,7 @@
         <v>119</v>
       </c>
     </row>
-    <row r="48" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="48" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A48" t="s">
         <v>12</v>
       </c>
@@ -5443,7 +5443,7 @@
         <v>120</v>
       </c>
     </row>
-    <row r="49" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="49" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A49" t="s">
         <v>12</v>
       </c>
@@ -5454,7 +5454,7 @@
         <v>101</v>
       </c>
     </row>
-    <row r="50" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="50" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A50" t="s">
         <v>30</v>
       </c>
@@ -5465,7 +5465,7 @@
         <v>125</v>
       </c>
     </row>
-    <row r="51" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="51" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A51" t="s">
         <v>30</v>
       </c>
@@ -5476,7 +5476,7 @@
         <v>126</v>
       </c>
     </row>
-    <row r="52" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="52" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A52" t="s">
         <v>127</v>
       </c>
@@ -5487,7 +5487,7 @@
         <v>128</v>
       </c>
     </row>
-    <row r="53" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="53" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A53" t="s">
         <v>129</v>
       </c>
@@ -5498,7 +5498,7 @@
         <v>130</v>
       </c>
     </row>
-    <row r="54" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="54" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A54" t="s">
         <v>131</v>
       </c>
@@ -5509,7 +5509,7 @@
         <v>132</v>
       </c>
     </row>
-    <row r="55" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="55" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A55" s="4" t="s">
         <v>492</v>
       </c>
@@ -5520,7 +5520,7 @@
         <v>133</v>
       </c>
     </row>
-    <row r="56" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="56" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A56" t="s">
         <v>134</v>
       </c>
@@ -5531,7 +5531,7 @@
         <v>135</v>
       </c>
     </row>
-    <row r="57" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="57" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A57" t="s">
         <v>134</v>
       </c>
@@ -5542,7 +5542,7 @@
         <v>136</v>
       </c>
     </row>
-    <row r="58" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="58" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A58" s="5" t="s">
         <v>37</v>
       </c>
@@ -5553,7 +5553,7 @@
         <v>125</v>
       </c>
     </row>
-    <row r="59" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="59" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A59" s="12" t="s">
         <v>30</v>
       </c>
@@ -5564,7 +5564,7 @@
         <v>126</v>
       </c>
     </row>
-    <row r="60" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="60" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A60" t="s">
         <v>43</v>
       </c>
@@ -5575,7 +5575,7 @@
         <v>130</v>
       </c>
     </row>
-    <row r="61" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="61" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A61" t="s">
         <v>43</v>
       </c>
@@ -5586,7 +5586,7 @@
         <v>135</v>
       </c>
     </row>
-    <row r="62" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="62" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A62" t="s">
         <v>43</v>
       </c>
@@ -5597,7 +5597,7 @@
         <v>137</v>
       </c>
     </row>
-    <row r="63" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="63" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A63" t="s">
         <v>43</v>
       </c>
@@ -5608,7 +5608,7 @@
         <v>136</v>
       </c>
     </row>
-    <row r="64" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="64" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A64" t="s">
         <v>43</v>
       </c>
@@ -5619,7 +5619,7 @@
         <v>138</v>
       </c>
     </row>
-    <row r="65" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="65" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A65" t="s">
         <v>43</v>
       </c>
@@ -5630,7 +5630,7 @@
         <v>128</v>
       </c>
     </row>
-    <row r="66" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="66" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A66" t="s">
         <v>43</v>
       </c>
@@ -5641,7 +5641,7 @@
         <v>139</v>
       </c>
     </row>
-    <row r="67" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="67" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A67" t="s">
         <v>43</v>
       </c>
@@ -5652,7 +5652,7 @@
         <v>132</v>
       </c>
     </row>
-    <row r="68" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="68" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A68" t="s">
         <v>43</v>
       </c>
@@ -5663,7 +5663,7 @@
         <v>140</v>
       </c>
     </row>
-    <row r="69" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="69" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A69" t="s">
         <v>43</v>
       </c>
@@ -5674,7 +5674,7 @@
         <v>141</v>
       </c>
     </row>
-    <row r="70" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="70" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A70" t="s">
         <v>43</v>
       </c>
@@ -5685,7 +5685,7 @@
         <v>142</v>
       </c>
     </row>
-    <row r="71" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="71" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A71" t="s">
         <v>143</v>
       </c>
@@ -5696,7 +5696,7 @@
         <v>139</v>
       </c>
     </row>
-    <row r="72" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="72" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A72" t="s">
         <v>144</v>
       </c>
@@ -5707,7 +5707,7 @@
         <v>119</v>
       </c>
     </row>
-    <row r="73" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="73" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A73" t="s">
         <v>145</v>
       </c>
@@ -5715,7 +5715,7 @@
         <v>99</v>
       </c>
     </row>
-    <row r="74" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="74" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A74" t="s">
         <v>145</v>
       </c>
@@ -5726,7 +5726,7 @@
         <v>113</v>
       </c>
     </row>
-    <row r="75" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="75" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A75" t="s">
         <v>145</v>
       </c>
@@ -5737,7 +5737,7 @@
         <v>115</v>
       </c>
     </row>
-    <row r="76" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="76" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A76" t="s">
         <v>145</v>
       </c>
@@ -5748,7 +5748,7 @@
         <v>117</v>
       </c>
     </row>
-    <row r="77" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="77" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A77" t="s">
         <v>145</v>
       </c>
@@ -5759,7 +5759,7 @@
         <v>118</v>
       </c>
     </row>
-    <row r="78" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="78" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A78" t="s">
         <v>145</v>
       </c>
@@ -5770,7 +5770,7 @@
         <v>119</v>
       </c>
     </row>
-    <row r="79" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="79" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A79" t="s">
         <v>145</v>
       </c>
@@ -5781,13 +5781,61 @@
         <v>120</v>
       </c>
     </row>
-    <row r="87" spans="2:2" x14ac:dyDescent="0.25">
+    <row r="80" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A80" t="s">
+        <v>28</v>
+      </c>
+      <c r="B80" t="s">
+        <v>105</v>
+      </c>
+    </row>
+    <row r="81" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A81" t="s">
+        <v>13</v>
+      </c>
+      <c r="B81" t="s">
+        <v>105</v>
+      </c>
+    </row>
+    <row r="82" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A82" t="s">
+        <v>25</v>
+      </c>
+      <c r="B82" t="s">
+        <v>105</v>
+      </c>
+    </row>
+    <row r="83" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A83" t="s">
+        <v>1</v>
+      </c>
+      <c r="B83" t="s">
+        <v>105</v>
+      </c>
+    </row>
+    <row r="84" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A84" t="s">
+        <v>23</v>
+      </c>
+      <c r="B84" t="s">
+        <v>105</v>
+      </c>
+    </row>
+    <row r="85" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A85" t="s">
+        <v>163</v>
+      </c>
+      <c r="B85" t="s">
+        <v>105</v>
+      </c>
+    </row>
+    <row r="87" spans="1:2" x14ac:dyDescent="0.35">
       <c r="B87" s="6"/>
     </row>
-    <row r="88" spans="2:2" x14ac:dyDescent="0.25">
+    <row r="88" spans="1:2" x14ac:dyDescent="0.35">
       <c r="B88" s="6"/>
     </row>
-    <row r="89" spans="2:2" x14ac:dyDescent="0.25">
+    <row r="89" spans="1:2" x14ac:dyDescent="0.35">
       <c r="B89" s="6"/>
     </row>
   </sheetData>
@@ -5809,15 +5857,15 @@
       <selection activeCell="B13" activeCellId="1" sqref="B26 B13"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <cols>
-    <col min="1" max="1" width="33.42578125" customWidth="1"/>
-    <col min="2" max="2" width="47.140625" customWidth="1"/>
-    <col min="3" max="3" width="50.140625" customWidth="1"/>
+    <col min="1" max="1" width="33.453125" customWidth="1"/>
+    <col min="2" max="2" width="47.1796875" customWidth="1"/>
+    <col min="3" max="3" width="50.1796875" customWidth="1"/>
     <col min="4" max="4" width="69" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A1" t="s">
         <v>56</v>
       </c>
@@ -5831,7 +5879,7 @@
         <v>59</v>
       </c>
     </row>
-    <row r="2" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A2" t="b">
         <v>1</v>
       </c>
@@ -5845,7 +5893,7 @@
         <v>62</v>
       </c>
     </row>
-    <row r="3" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A3" t="b">
         <v>1</v>
       </c>
@@ -5859,7 +5907,7 @@
         <v>63</v>
       </c>
     </row>
-    <row r="4" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A4" t="b">
         <v>1</v>
       </c>
@@ -5873,7 +5921,7 @@
         <v>64</v>
       </c>
     </row>
-    <row r="5" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A5" t="b">
         <v>1</v>
       </c>
@@ -5887,7 +5935,7 @@
         <v>65</v>
       </c>
     </row>
-    <row r="6" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A6" t="b">
         <v>1</v>
       </c>
@@ -5901,7 +5949,7 @@
         <v>67</v>
       </c>
     </row>
-    <row r="7" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A7" t="b">
         <v>1</v>
       </c>
@@ -5915,7 +5963,7 @@
         <v>68</v>
       </c>
     </row>
-    <row r="8" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A8" t="b">
         <v>1</v>
       </c>
@@ -5929,7 +5977,7 @@
         <v>69</v>
       </c>
     </row>
-    <row r="9" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A9" t="b">
         <v>1</v>
       </c>
@@ -5943,7 +5991,7 @@
         <v>70</v>
       </c>
     </row>
-    <row r="10" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A10" t="b">
         <v>1</v>
       </c>
@@ -5957,7 +6005,7 @@
         <v>71</v>
       </c>
     </row>
-    <row r="11" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A11" t="b">
         <v>1</v>
       </c>
@@ -5971,7 +6019,7 @@
         <v>72</v>
       </c>
     </row>
-    <row r="12" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A12" t="b">
         <v>1</v>
       </c>
@@ -5985,7 +6033,7 @@
         <v>73</v>
       </c>
     </row>
-    <row r="13" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A13" t="b">
         <v>1</v>
       </c>
@@ -5999,7 +6047,7 @@
         <v>74</v>
       </c>
     </row>
-    <row r="14" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A14" t="b">
         <v>1</v>
       </c>
@@ -6013,7 +6061,7 @@
         <v>75</v>
       </c>
     </row>
-    <row r="15" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A15" t="b">
         <v>0</v>
       </c>
@@ -6027,7 +6075,7 @@
         <v>62</v>
       </c>
     </row>
-    <row r="16" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A16" t="b">
         <v>0</v>
       </c>
@@ -6041,7 +6089,7 @@
         <v>63</v>
       </c>
     </row>
-    <row r="17" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A17" t="b">
         <v>0</v>
       </c>
@@ -6055,7 +6103,7 @@
         <v>64</v>
       </c>
     </row>
-    <row r="18" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="18" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A18" t="b">
         <v>0</v>
       </c>
@@ -6069,7 +6117,7 @@
         <v>65</v>
       </c>
     </row>
-    <row r="19" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="19" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A19" t="b">
         <v>0</v>
       </c>
@@ -6083,7 +6131,7 @@
         <v>67</v>
       </c>
     </row>
-    <row r="20" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="20" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A20" t="b">
         <v>0</v>
       </c>
@@ -6097,7 +6145,7 @@
         <v>68</v>
       </c>
     </row>
-    <row r="21" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="21" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A21" t="b">
         <v>0</v>
       </c>
@@ -6111,7 +6159,7 @@
         <v>69</v>
       </c>
     </row>
-    <row r="22" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="22" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A22" t="b">
         <v>0</v>
       </c>
@@ -6125,7 +6173,7 @@
         <v>70</v>
       </c>
     </row>
-    <row r="23" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="23" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A23" t="b">
         <v>0</v>
       </c>
@@ -6139,7 +6187,7 @@
         <v>71</v>
       </c>
     </row>
-    <row r="24" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="24" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A24" t="b">
         <v>0</v>
       </c>
@@ -6153,7 +6201,7 @@
         <v>72</v>
       </c>
     </row>
-    <row r="25" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="25" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A25" t="b">
         <v>0</v>
       </c>
@@ -6167,7 +6215,7 @@
         <v>73</v>
       </c>
     </row>
-    <row r="26" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="26" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A26" t="b">
         <v>0</v>
       </c>
@@ -6181,7 +6229,7 @@
         <v>74</v>
       </c>
     </row>
-    <row r="27" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="27" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A27" t="b">
         <v>0</v>
       </c>
@@ -6210,12 +6258,12 @@
       <selection activeCell="A21" sqref="A21"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <cols>
-    <col min="1" max="1" width="19.85546875" customWidth="1"/>
+    <col min="1" max="1" width="19.81640625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A1" t="s">
         <v>474</v>
       </c>
@@ -6223,7 +6271,7 @@
         <v>477</v>
       </c>
     </row>
-    <row r="2" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A2" t="s">
         <v>481</v>
       </c>
@@ -6231,7 +6279,7 @@
         <v>60</v>
       </c>
     </row>
-    <row r="3" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A3" t="s">
         <v>481</v>
       </c>
@@ -6239,7 +6287,7 @@
         <v>60</v>
       </c>
     </row>
-    <row r="4" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A4" t="s">
         <v>481</v>
       </c>
@@ -6247,7 +6295,7 @@
         <v>60</v>
       </c>
     </row>
-    <row r="5" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A5" t="s">
         <v>481</v>
       </c>
@@ -6255,7 +6303,7 @@
         <v>60</v>
       </c>
     </row>
-    <row r="6" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A6" t="s">
         <v>482</v>
       </c>
@@ -6263,7 +6311,7 @@
         <v>66</v>
       </c>
     </row>
-    <row r="7" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A7" t="s">
         <v>482</v>
       </c>
@@ -6271,7 +6319,7 @@
         <v>66</v>
       </c>
     </row>
-    <row r="8" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A8" t="s">
         <v>482</v>
       </c>
@@ -6279,7 +6327,7 @@
         <v>66</v>
       </c>
     </row>
-    <row r="9" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A9" t="s">
         <v>482</v>
       </c>
@@ -6287,7 +6335,7 @@
         <v>66</v>
       </c>
     </row>
-    <row r="10" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A10" t="s">
         <v>482</v>
       </c>
@@ -6295,7 +6343,7 @@
         <v>66</v>
       </c>
     </row>
-    <row r="11" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A11" t="s">
         <v>482</v>
       </c>
@@ -6303,7 +6351,7 @@
         <v>66</v>
       </c>
     </row>
-    <row r="12" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A12" t="s">
         <v>482</v>
       </c>
@@ -6311,7 +6359,7 @@
         <v>66</v>
       </c>
     </row>
-    <row r="13" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A13" t="s">
         <v>483</v>
       </c>
@@ -6319,7 +6367,7 @@
         <v>30</v>
       </c>
     </row>
-    <row r="14" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A14" t="s">
         <v>486</v>
       </c>
@@ -6327,7 +6375,7 @@
         <v>60</v>
       </c>
     </row>
-    <row r="15" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A15" t="s">
         <v>478</v>
       </c>
@@ -6335,7 +6383,7 @@
         <v>60</v>
       </c>
     </row>
-    <row r="16" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A16" t="s">
         <v>478</v>
       </c>
@@ -6343,7 +6391,7 @@
         <v>60</v>
       </c>
     </row>
-    <row r="17" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A17" t="s">
         <v>478</v>
       </c>
@@ -6351,7 +6399,7 @@
         <v>60</v>
       </c>
     </row>
-    <row r="18" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="18" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A18" t="s">
         <v>478</v>
       </c>
@@ -6359,7 +6407,7 @@
         <v>60</v>
       </c>
     </row>
-    <row r="19" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="19" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A19" t="s">
         <v>479</v>
       </c>
@@ -6367,7 +6415,7 @@
         <v>66</v>
       </c>
     </row>
-    <row r="20" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="20" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A20" t="s">
         <v>479</v>
       </c>
@@ -6375,7 +6423,7 @@
         <v>66</v>
       </c>
     </row>
-    <row r="21" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="21" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A21" t="s">
         <v>479</v>
       </c>
@@ -6383,7 +6431,7 @@
         <v>66</v>
       </c>
     </row>
-    <row r="22" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="22" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A22" t="s">
         <v>479</v>
       </c>
@@ -6391,7 +6439,7 @@
         <v>66</v>
       </c>
     </row>
-    <row r="23" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="23" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A23" t="s">
         <v>479</v>
       </c>
@@ -6399,7 +6447,7 @@
         <v>66</v>
       </c>
     </row>
-    <row r="24" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="24" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A24" t="s">
         <v>479</v>
       </c>
@@ -6407,7 +6455,7 @@
         <v>66</v>
       </c>
     </row>
-    <row r="25" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="25" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A25" t="s">
         <v>479</v>
       </c>
@@ -6415,7 +6463,7 @@
         <v>66</v>
       </c>
     </row>
-    <row r="26" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="26" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A26" t="s">
         <v>480</v>
       </c>
@@ -6423,7 +6471,7 @@
         <v>30</v>
       </c>
     </row>
-    <row r="27" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="27" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A27" t="s">
         <v>478</v>
       </c>
@@ -6431,7 +6479,7 @@
         <v>60</v>
       </c>
     </row>
-    <row r="28" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="28" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A28" t="s">
         <v>487</v>
       </c>
@@ -6439,7 +6487,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="29" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="29" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A29" t="s">
         <v>488</v>
       </c>
@@ -6465,9 +6513,9 @@
       <selection activeCell="D73" sqref="D73"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <sheetData>
-    <row r="1" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A1" t="s">
         <v>474</v>
       </c>
@@ -6475,7 +6523,7 @@
         <v>475</v>
       </c>
     </row>
-    <row r="2" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A2" t="s">
         <v>11</v>
       </c>
@@ -6483,7 +6531,7 @@
         <v>454</v>
       </c>
     </row>
-    <row r="3" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A3" t="s">
         <v>5</v>
       </c>
@@ -6491,7 +6539,7 @@
         <v>455</v>
       </c>
     </row>
-    <row r="4" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A4" t="s">
         <v>4</v>
       </c>
@@ -6499,7 +6547,7 @@
         <v>456</v>
       </c>
     </row>
-    <row r="5" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A5" t="s">
         <v>12</v>
       </c>
@@ -6507,7 +6555,7 @@
         <v>457</v>
       </c>
     </row>
-    <row r="6" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A6" t="s">
         <v>10</v>
       </c>
@@ -6515,7 +6563,7 @@
         <v>458</v>
       </c>
     </row>
-    <row r="7" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A7" t="s">
         <v>30</v>
       </c>
@@ -6523,7 +6571,7 @@
         <v>459</v>
       </c>
     </row>
-    <row r="8" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A8" t="s">
         <v>3</v>
       </c>
@@ -6531,7 +6579,7 @@
         <v>460</v>
       </c>
     </row>
-    <row r="9" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A9" t="s">
         <v>103</v>
       </c>
@@ -6539,7 +6587,7 @@
         <v>461</v>
       </c>
     </row>
-    <row r="10" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A10" t="s">
         <v>31</v>
       </c>
@@ -6547,7 +6595,7 @@
         <v>462</v>
       </c>
     </row>
-    <row r="11" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A11" t="s">
         <v>25</v>
       </c>
@@ -6555,7 +6603,7 @@
         <v>463</v>
       </c>
     </row>
-    <row r="12" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A12" t="s">
         <v>28</v>
       </c>
@@ -6563,7 +6611,7 @@
         <v>464</v>
       </c>
     </row>
-    <row r="13" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A13" t="s">
         <v>9</v>
       </c>
@@ -6571,7 +6619,7 @@
         <v>455</v>
       </c>
     </row>
-    <row r="14" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A14" t="s">
         <v>1</v>
       </c>
@@ -6579,7 +6627,7 @@
         <v>456</v>
       </c>
     </row>
-    <row r="15" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A15" t="s">
         <v>33</v>
       </c>
@@ -6587,7 +6635,7 @@
         <v>457</v>
       </c>
     </row>
-    <row r="16" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A16" t="s">
         <v>26</v>
       </c>
@@ -6595,7 +6643,7 @@
         <v>465</v>
       </c>
     </row>
-    <row r="17" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A17" t="s">
         <v>14</v>
       </c>
@@ -6603,7 +6651,7 @@
         <v>456</v>
       </c>
     </row>
-    <row r="18" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="18" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A18" t="s">
         <v>13</v>
       </c>
@@ -6611,7 +6659,7 @@
         <v>457</v>
       </c>
     </row>
-    <row r="19" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="19" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A19" t="s">
         <v>181</v>
       </c>
@@ -6619,7 +6667,7 @@
         <v>464</v>
       </c>
     </row>
-    <row r="20" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="20" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A20" t="s">
         <v>179</v>
       </c>
@@ -6627,7 +6675,7 @@
         <v>456</v>
       </c>
     </row>
-    <row r="21" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="21" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A21" t="s">
         <v>176</v>
       </c>
@@ -6635,7 +6683,7 @@
         <v>455</v>
       </c>
     </row>
-    <row r="22" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="22" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A22" t="s">
         <v>185</v>
       </c>
@@ -6643,7 +6691,7 @@
         <v>454</v>
       </c>
     </row>
-    <row r="23" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="23" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A23" t="s">
         <v>183</v>
       </c>
@@ -6651,7 +6699,7 @@
         <v>457</v>
       </c>
     </row>
-    <row r="24" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="24" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A24" t="s">
         <v>187</v>
       </c>
@@ -6659,7 +6707,7 @@
         <v>459</v>
       </c>
     </row>
-    <row r="25" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="25" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A25" t="s">
         <v>134</v>
       </c>
@@ -6667,7 +6715,7 @@
         <v>455</v>
       </c>
     </row>
-    <row r="26" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="26" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A26" t="s">
         <v>131</v>
       </c>
@@ -6675,7 +6723,7 @@
         <v>466</v>
       </c>
     </row>
-    <row r="27" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="27" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A27" t="s">
         <v>129</v>
       </c>
@@ -6683,7 +6731,7 @@
         <v>465</v>
       </c>
     </row>
-    <row r="28" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="28" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A28" t="s">
         <v>127</v>
       </c>
@@ -6691,7 +6739,7 @@
         <v>454</v>
       </c>
     </row>
-    <row r="29" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="29" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A29" t="s">
         <v>37</v>
       </c>
@@ -6699,7 +6747,7 @@
         <v>457</v>
       </c>
     </row>
-    <row r="30" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="30" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A30" t="s">
         <v>47</v>
       </c>
@@ -6707,7 +6755,7 @@
         <v>465</v>
       </c>
     </row>
-    <row r="31" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="31" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A31" t="s">
         <v>51</v>
       </c>
@@ -6715,7 +6763,7 @@
         <v>464</v>
       </c>
     </row>
-    <row r="32" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="32" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A32" t="s">
         <v>50</v>
       </c>
@@ -6723,7 +6771,7 @@
         <v>455</v>
       </c>
     </row>
-    <row r="33" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="33" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A33" t="s">
         <v>48</v>
       </c>
@@ -6731,7 +6779,7 @@
         <v>457</v>
       </c>
     </row>
-    <row r="34" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="34" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A34" t="s">
         <v>49</v>
       </c>
@@ -6739,7 +6787,7 @@
         <v>466</v>
       </c>
     </row>
-    <row r="35" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="35" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A35" t="s">
         <v>91</v>
       </c>
@@ -6747,7 +6795,7 @@
         <v>464</v>
       </c>
     </row>
-    <row r="36" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="36" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A36" t="s">
         <v>89</v>
       </c>
@@ -6755,7 +6803,7 @@
         <v>467</v>
       </c>
     </row>
-    <row r="37" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="37" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A37" t="s">
         <v>16</v>
       </c>
@@ -6763,7 +6811,7 @@
         <v>468</v>
       </c>
     </row>
-    <row r="38" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="38" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A38" t="s">
         <v>87</v>
       </c>
@@ -6771,7 +6819,7 @@
         <v>466</v>
       </c>
     </row>
-    <row r="39" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="39" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A39" t="s">
         <v>93</v>
       </c>
@@ -6779,7 +6827,7 @@
         <v>459</v>
       </c>
     </row>
-    <row r="40" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="40" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A40" t="s">
         <v>97</v>
       </c>
@@ -6787,7 +6835,7 @@
         <v>465</v>
       </c>
     </row>
-    <row r="41" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="41" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A41" t="s">
         <v>20</v>
       </c>
@@ -6795,7 +6843,7 @@
         <v>463</v>
       </c>
     </row>
-    <row r="42" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="42" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A42" t="s">
         <v>19</v>
       </c>
@@ -6803,7 +6851,7 @@
         <v>465</v>
       </c>
     </row>
-    <row r="43" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="43" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A43" t="s">
         <v>143</v>
       </c>
@@ -6811,7 +6859,7 @@
         <v>465</v>
       </c>
     </row>
-    <row r="44" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="44" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A44" t="s">
         <v>60</v>
       </c>
@@ -6819,7 +6867,7 @@
         <v>462</v>
       </c>
     </row>
-    <row r="45" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="45" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A45" t="s">
         <v>66</v>
       </c>
@@ -6827,7 +6875,7 @@
         <v>468</v>
       </c>
     </row>
-    <row r="46" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="46" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A46" t="s">
         <v>21</v>
       </c>
@@ -6835,7 +6883,7 @@
         <v>464</v>
       </c>
     </row>
-    <row r="47" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="47" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A47" t="s">
         <v>22</v>
       </c>
@@ -6843,7 +6891,7 @@
         <v>455</v>
       </c>
     </row>
-    <row r="48" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="48" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A48" t="s">
         <v>41</v>
       </c>
@@ -6851,7 +6899,7 @@
         <v>456</v>
       </c>
     </row>
-    <row r="49" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="49" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A49" t="s">
         <v>35</v>
       </c>
@@ -6859,7 +6907,7 @@
         <v>457</v>
       </c>
     </row>
-    <row r="50" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="50" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A50" t="s">
         <v>42</v>
       </c>
@@ -6867,7 +6915,7 @@
         <v>468</v>
       </c>
     </row>
-    <row r="51" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="51" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A51" t="s">
         <v>108</v>
       </c>
@@ -6875,7 +6923,7 @@
         <v>459</v>
       </c>
     </row>
-    <row r="52" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="52" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A52" t="s">
         <v>110</v>
       </c>
@@ -6883,7 +6931,7 @@
         <v>456</v>
       </c>
     </row>
-    <row r="53" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="53" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A53" t="s">
         <v>27</v>
       </c>
@@ -6891,7 +6939,7 @@
         <v>460</v>
       </c>
     </row>
-    <row r="54" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="54" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A54" t="s">
         <v>144</v>
       </c>
@@ -6899,7 +6947,7 @@
         <v>462</v>
       </c>
     </row>
-    <row r="55" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="55" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A55" t="s">
         <v>6</v>
       </c>
@@ -6907,7 +6955,7 @@
         <v>454</v>
       </c>
     </row>
-    <row r="56" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="56" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A56" t="s">
         <v>17</v>
       </c>
@@ -6915,7 +6963,7 @@
         <v>457</v>
       </c>
     </row>
-    <row r="57" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="57" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A57" t="s">
         <v>18</v>
       </c>
@@ -6923,7 +6971,7 @@
         <v>454</v>
       </c>
     </row>
-    <row r="58" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="58" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A58" t="s">
         <v>43</v>
       </c>
@@ -6931,7 +6979,7 @@
         <v>465</v>
       </c>
     </row>
-    <row r="59" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="59" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A59" t="s">
         <v>112</v>
       </c>
@@ -6939,7 +6987,7 @@
         <v>458</v>
       </c>
     </row>
-    <row r="60" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="60" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A60" t="s">
         <v>124</v>
       </c>
@@ -6947,7 +6995,7 @@
         <v>468</v>
       </c>
     </row>
-    <row r="61" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="61" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A61" t="s">
         <v>111</v>
       </c>
@@ -6955,7 +7003,7 @@
         <v>460</v>
       </c>
     </row>
-    <row r="62" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="62" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A62" t="s">
         <v>145</v>
       </c>
@@ -6963,7 +7011,7 @@
         <v>458</v>
       </c>
     </row>
-    <row r="63" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="63" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A63" t="s">
         <v>106</v>
       </c>
@@ -6971,7 +7019,7 @@
         <v>459</v>
       </c>
     </row>
-    <row r="64" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="64" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A64" t="s">
         <v>95</v>
       </c>
@@ -6979,7 +7027,7 @@
         <v>464</v>
       </c>
     </row>
-    <row r="65" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="65" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A65" t="s">
         <v>197</v>
       </c>
@@ -6987,7 +7035,7 @@
         <v>468</v>
       </c>
     </row>
-    <row r="66" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="66" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A66" t="s">
         <v>173</v>
       </c>
@@ -6995,7 +7043,7 @@
         <v>460</v>
       </c>
     </row>
-    <row r="67" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="67" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A67" t="s">
         <v>203</v>
       </c>
@@ -7003,7 +7051,7 @@
         <v>465</v>
       </c>
     </row>
-    <row r="68" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="68" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A68" t="s">
         <v>175</v>
       </c>
@@ -7011,7 +7059,7 @@
         <v>461</v>
       </c>
     </row>
-    <row r="69" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="69" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A69" t="s">
         <v>195</v>
       </c>
@@ -7019,7 +7067,7 @@
         <v>460</v>
       </c>
     </row>
-    <row r="70" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="70" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A70" t="s">
         <v>208</v>
       </c>
@@ -7027,7 +7075,7 @@
         <v>460</v>
       </c>
     </row>
-    <row r="71" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="71" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A71" t="s">
         <v>189</v>
       </c>
@@ -7035,7 +7083,7 @@
         <v>462</v>
       </c>
     </row>
-    <row r="72" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="72" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A72" t="s">
         <v>206</v>
       </c>
@@ -7043,7 +7091,7 @@
         <v>467</v>
       </c>
     </row>
-    <row r="73" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="73" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A73" t="s">
         <v>159</v>
       </c>
@@ -7051,7 +7099,7 @@
         <v>465</v>
       </c>
     </row>
-    <row r="74" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="74" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A74" t="s">
         <v>161</v>
       </c>
@@ -7059,7 +7107,7 @@
         <v>464</v>
       </c>
     </row>
-    <row r="75" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="75" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A75" t="s">
         <v>163</v>
       </c>
@@ -7067,7 +7115,7 @@
         <v>469</v>
       </c>
     </row>
-    <row r="76" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="76" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A76" t="s">
         <v>23</v>
       </c>
@@ -7075,7 +7123,7 @@
         <v>470</v>
       </c>
     </row>
-    <row r="77" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="77" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A77" t="s">
         <v>155</v>
       </c>
@@ -7083,7 +7131,7 @@
         <v>471</v>
       </c>
     </row>
-    <row r="78" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="78" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A78" t="s">
         <v>157</v>
       </c>
@@ -7091,7 +7139,7 @@
         <v>460</v>
       </c>
     </row>
-    <row r="79" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="79" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A79" t="s">
         <v>481</v>
       </c>
@@ -7099,7 +7147,7 @@
         <v>462</v>
       </c>
     </row>
-    <row r="80" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="80" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A80" t="s">
         <v>482</v>
       </c>
@@ -7107,7 +7155,7 @@
         <v>468</v>
       </c>
     </row>
-    <row r="81" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="81" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A81" t="s">
         <v>478</v>
       </c>
@@ -7115,7 +7163,7 @@
         <v>462</v>
       </c>
     </row>
-    <row r="82" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="82" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A82" t="s">
         <v>479</v>
       </c>
@@ -7123,7 +7171,7 @@
         <v>468</v>
       </c>
     </row>
-    <row r="83" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="83" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A83" t="s">
         <v>483</v>
       </c>
@@ -7131,7 +7179,7 @@
         <v>459</v>
       </c>
     </row>
-    <row r="84" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="84" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A84" t="s">
         <v>480</v>
       </c>
@@ -7139,7 +7187,7 @@
         <v>459</v>
       </c>
     </row>
-    <row r="85" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="85" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A85" t="s">
         <v>487</v>
       </c>
@@ -7147,7 +7195,7 @@
         <v>454</v>
       </c>
     </row>
-    <row r="86" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="86" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A86" t="s">
         <v>488</v>
       </c>
@@ -7169,12 +7217,12 @@
       <selection activeCell="I25" sqref="I25"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <cols>
     <col min="1" max="1" width="19" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A1" s="1" t="s">
         <v>473</v>
       </c>
@@ -7182,7 +7230,7 @@
         <v>472</v>
       </c>
     </row>
-    <row r="2" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A2" t="s">
         <v>52</v>
       </c>
@@ -7190,7 +7238,7 @@
         <v>18</v>
       </c>
     </row>
-    <row r="3" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A3" t="s">
         <v>53</v>
       </c>
@@ -7198,7 +7246,7 @@
         <v>491</v>
       </c>
     </row>
-    <row r="4" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A4" t="s">
         <v>54</v>
       </c>
@@ -7206,7 +7254,7 @@
         <v>500</v>
       </c>
     </row>
-    <row r="5" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A5" t="s">
         <v>55</v>
       </c>
@@ -7225,47 +7273,47 @@
   <sheetPr>
     <tabColor theme="8"/>
   </sheetPr>
-  <dimension ref="A1:N56"/>
+  <dimension ref="A1:N58"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="C20" workbookViewId="0">
-      <selection activeCell="K57" sqref="K57"/>
+    <sheetView tabSelected="1" topLeftCell="A34" workbookViewId="0">
+      <selection activeCell="D52" sqref="D52"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <cols>
-    <col min="1" max="1" width="25.140625" customWidth="1"/>
+    <col min="1" max="1" width="25.1796875" customWidth="1"/>
     <col min="2" max="5" width="25" customWidth="1"/>
-    <col min="6" max="6" width="20.140625" customWidth="1"/>
-    <col min="7" max="7" width="25.140625" customWidth="1"/>
-    <col min="8" max="8" width="28.140625" customWidth="1"/>
-    <col min="9" max="9" width="34.140625" customWidth="1"/>
-    <col min="10" max="10" width="20.85546875" customWidth="1"/>
-    <col min="11" max="11" width="20.140625" customWidth="1"/>
-    <col min="12" max="12" width="22.85546875" customWidth="1"/>
-    <col min="13" max="13" width="21.85546875" customWidth="1"/>
-    <col min="14" max="14" width="24.85546875" customWidth="1"/>
+    <col min="6" max="6" width="20.1796875" customWidth="1"/>
+    <col min="7" max="7" width="25.1796875" customWidth="1"/>
+    <col min="8" max="8" width="28.1796875" customWidth="1"/>
+    <col min="9" max="9" width="34.1796875" customWidth="1"/>
+    <col min="10" max="10" width="20.81640625" customWidth="1"/>
+    <col min="11" max="11" width="20.1796875" customWidth="1"/>
+    <col min="12" max="12" width="22.81640625" customWidth="1"/>
+    <col min="13" max="13" width="21.81640625" customWidth="1"/>
+    <col min="14" max="14" width="24.81640625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:14" x14ac:dyDescent="0.35">
       <c r="A1" s="1"/>
       <c r="B1" s="1"/>
-      <c r="D1" s="14" t="s">
+      <c r="D1" s="15" t="s">
         <v>489</v>
       </c>
-      <c r="E1" s="16"/>
-      <c r="F1" s="14" t="s">
+      <c r="E1" s="17"/>
+      <c r="F1" s="15" t="s">
         <v>476</v>
       </c>
-      <c r="G1" s="15"/>
-      <c r="H1" s="15"/>
-      <c r="I1" s="15"/>
-      <c r="J1" s="15"/>
-      <c r="K1" s="15"/>
-      <c r="L1" s="15"/>
-      <c r="M1" s="15"/>
-      <c r="N1" s="16"/>
-    </row>
-    <row r="2" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="G1" s="16"/>
+      <c r="H1" s="16"/>
+      <c r="I1" s="16"/>
+      <c r="J1" s="16"/>
+      <c r="K1" s="16"/>
+      <c r="L1" s="16"/>
+      <c r="M1" s="16"/>
+      <c r="N1" s="17"/>
+    </row>
+    <row r="2" spans="1:14" x14ac:dyDescent="0.35">
       <c r="A2" s="1" t="s">
         <v>485</v>
       </c>
@@ -7309,7 +7357,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="3" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:14" x14ac:dyDescent="0.35">
       <c r="A3" t="s">
         <v>1</v>
       </c>
@@ -7335,7 +7383,7 @@
         <v>163</v>
       </c>
     </row>
-    <row r="4" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:14" x14ac:dyDescent="0.35">
       <c r="A4" t="s">
         <v>1</v>
       </c>
@@ -7361,7 +7409,7 @@
         <v>163</v>
       </c>
     </row>
-    <row r="5" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:14" x14ac:dyDescent="0.35">
       <c r="A5" t="s">
         <v>1</v>
       </c>
@@ -7387,7 +7435,7 @@
         <v>163</v>
       </c>
     </row>
-    <row r="6" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:14" x14ac:dyDescent="0.35">
       <c r="A6" t="s">
         <v>9</v>
       </c>
@@ -7422,7 +7470,7 @@
         <v>163</v>
       </c>
     </row>
-    <row r="7" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:14" x14ac:dyDescent="0.35">
       <c r="A7" t="s">
         <v>9</v>
       </c>
@@ -7432,7 +7480,7 @@
       <c r="C7" t="s">
         <v>2</v>
       </c>
-      <c r="D7" t="s">
+      <c r="E7" t="s">
         <v>9</v>
       </c>
       <c r="F7" t="s">
@@ -7445,7 +7493,7 @@
         <v>14</v>
       </c>
     </row>
-    <row r="8" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:14" x14ac:dyDescent="0.35">
       <c r="A8" t="s">
         <v>15</v>
       </c>
@@ -7455,7 +7503,7 @@
       <c r="C8" t="s">
         <v>7</v>
       </c>
-      <c r="E8" t="s">
+      <c r="D8" t="s">
         <v>11</v>
       </c>
       <c r="F8" t="s">
@@ -7468,7 +7516,7 @@
         <v>18</v>
       </c>
     </row>
-    <row r="9" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:14" x14ac:dyDescent="0.35">
       <c r="A9" t="s">
         <v>15</v>
       </c>
@@ -7478,7 +7526,7 @@
       <c r="C9" t="s">
         <v>7</v>
       </c>
-      <c r="E9" t="s">
+      <c r="D9" t="s">
         <v>11</v>
       </c>
       <c r="F9" t="s">
@@ -7488,7 +7536,7 @@
         <v>18</v>
       </c>
     </row>
-    <row r="10" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:14" x14ac:dyDescent="0.35">
       <c r="A10" t="s">
         <v>15</v>
       </c>
@@ -7498,7 +7546,7 @@
       <c r="C10" t="s">
         <v>7</v>
       </c>
-      <c r="E10" t="s">
+      <c r="D10" t="s">
         <v>11</v>
       </c>
       <c r="F10" t="s">
@@ -7508,7 +7556,7 @@
         <v>18</v>
       </c>
     </row>
-    <row r="11" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:14" x14ac:dyDescent="0.35">
       <c r="A11" t="s">
         <v>11</v>
       </c>
@@ -7537,7 +7585,7 @@
         <v>23</v>
       </c>
     </row>
-    <row r="12" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:14" x14ac:dyDescent="0.35">
       <c r="A12" t="s">
         <v>11</v>
       </c>
@@ -7566,7 +7614,7 @@
         <v>23</v>
       </c>
     </row>
-    <row r="13" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:14" x14ac:dyDescent="0.35">
       <c r="A13" t="s">
         <v>24</v>
       </c>
@@ -7595,7 +7643,7 @@
         <v>23</v>
       </c>
     </row>
-    <row r="14" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:14" x14ac:dyDescent="0.35">
       <c r="A14" t="s">
         <v>24</v>
       </c>
@@ -7624,7 +7672,7 @@
         <v>23</v>
       </c>
     </row>
-    <row r="15" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:14" x14ac:dyDescent="0.35">
       <c r="A15" t="s">
         <v>3</v>
       </c>
@@ -7659,7 +7707,7 @@
         <v>163</v>
       </c>
     </row>
-    <row r="16" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:14" x14ac:dyDescent="0.35">
       <c r="A16" t="s">
         <v>29</v>
       </c>
@@ -7700,7 +7748,7 @@
         <v>163</v>
       </c>
     </row>
-    <row r="17" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:13" x14ac:dyDescent="0.35">
       <c r="A17" t="s">
         <v>32</v>
       </c>
@@ -7735,7 +7783,7 @@
         <v>28</v>
       </c>
     </row>
-    <row r="18" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="18" spans="1:13" x14ac:dyDescent="0.35">
       <c r="A18" t="s">
         <v>32</v>
       </c>
@@ -7770,7 +7818,7 @@
         <v>28</v>
       </c>
     </row>
-    <row r="19" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="19" spans="1:13" x14ac:dyDescent="0.35">
       <c r="A19" t="s">
         <v>30</v>
       </c>
@@ -7793,7 +7841,7 @@
         <v>28</v>
       </c>
     </row>
-    <row r="20" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="20" spans="1:13" x14ac:dyDescent="0.35">
       <c r="A20" t="s">
         <v>30</v>
       </c>
@@ -7816,7 +7864,7 @@
         <v>28</v>
       </c>
     </row>
-    <row r="21" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="21" spans="1:13" x14ac:dyDescent="0.35">
       <c r="A21" t="s">
         <v>30</v>
       </c>
@@ -7839,7 +7887,7 @@
         <v>28</v>
       </c>
     </row>
-    <row r="22" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="22" spans="1:13" x14ac:dyDescent="0.35">
       <c r="A22" t="s">
         <v>25</v>
       </c>
@@ -7877,7 +7925,7 @@
         <v>163</v>
       </c>
     </row>
-    <row r="23" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="23" spans="1:13" x14ac:dyDescent="0.35">
       <c r="A23" t="s">
         <v>34</v>
       </c>
@@ -7894,7 +7942,7 @@
         <v>21</v>
       </c>
     </row>
-    <row r="24" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="24" spans="1:13" x14ac:dyDescent="0.35">
       <c r="A24" t="s">
         <v>34</v>
       </c>
@@ -7923,7 +7971,7 @@
         <v>23</v>
       </c>
     </row>
-    <row r="25" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="25" spans="1:13" x14ac:dyDescent="0.35">
       <c r="A25" t="s">
         <v>34</v>
       </c>
@@ -7955,7 +8003,7 @@
         <v>23</v>
       </c>
     </row>
-    <row r="26" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="26" spans="1:13" x14ac:dyDescent="0.35">
       <c r="A26" t="s">
         <v>36</v>
       </c>
@@ -7972,7 +8020,7 @@
         <v>21</v>
       </c>
     </row>
-    <row r="27" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="27" spans="1:13" x14ac:dyDescent="0.35">
       <c r="A27" t="s">
         <v>36</v>
       </c>
@@ -8001,7 +8049,7 @@
         <v>23</v>
       </c>
     </row>
-    <row r="28" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="28" spans="1:13" x14ac:dyDescent="0.35">
       <c r="A28" t="s">
         <v>36</v>
       </c>
@@ -8033,7 +8081,7 @@
         <v>23</v>
       </c>
     </row>
-    <row r="29" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="29" spans="1:13" x14ac:dyDescent="0.35">
       <c r="A29" t="s">
         <v>21</v>
       </c>
@@ -8065,7 +8113,7 @@
         <v>23</v>
       </c>
     </row>
-    <row r="30" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="30" spans="1:13" x14ac:dyDescent="0.35">
       <c r="A30" t="s">
         <v>21</v>
       </c>
@@ -8097,7 +8145,7 @@
         <v>23</v>
       </c>
     </row>
-    <row r="31" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="31" spans="1:13" x14ac:dyDescent="0.35">
       <c r="A31" t="s">
         <v>21</v>
       </c>
@@ -8129,7 +8177,7 @@
         <v>23</v>
       </c>
     </row>
-    <row r="32" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="32" spans="1:13" x14ac:dyDescent="0.35">
       <c r="A32" t="s">
         <v>38</v>
       </c>
@@ -8161,7 +8209,7 @@
         <v>23</v>
       </c>
     </row>
-    <row r="33" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="33" spans="1:13" x14ac:dyDescent="0.35">
       <c r="A33" t="s">
         <v>38</v>
       </c>
@@ -8193,7 +8241,7 @@
         <v>23</v>
       </c>
     </row>
-    <row r="34" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="34" spans="1:13" x14ac:dyDescent="0.35">
       <c r="A34" t="s">
         <v>39</v>
       </c>
@@ -8225,7 +8273,7 @@
         <v>23</v>
       </c>
     </row>
-    <row r="35" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="35" spans="1:13" x14ac:dyDescent="0.35">
       <c r="A35" t="s">
         <v>39</v>
       </c>
@@ -8257,7 +8305,7 @@
         <v>23</v>
       </c>
     </row>
-    <row r="36" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="36" spans="1:13" x14ac:dyDescent="0.35">
       <c r="A36" t="s">
         <v>40</v>
       </c>
@@ -8283,7 +8331,7 @@
         <v>22</v>
       </c>
     </row>
-    <row r="37" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="37" spans="1:13" x14ac:dyDescent="0.35">
       <c r="A37" t="s">
         <v>40</v>
       </c>
@@ -8309,7 +8357,7 @@
         <v>22</v>
       </c>
     </row>
-    <row r="38" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="38" spans="1:13" x14ac:dyDescent="0.35">
       <c r="A38" t="s">
         <v>40</v>
       </c>
@@ -8319,7 +8367,7 @@
       <c r="C38" t="s">
         <v>2</v>
       </c>
-      <c r="E38" t="s">
+      <c r="D38" t="s">
         <v>23</v>
       </c>
       <c r="F38" t="s">
@@ -8341,7 +8389,7 @@
         <v>23</v>
       </c>
     </row>
-    <row r="39" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="39" spans="1:13" x14ac:dyDescent="0.35">
       <c r="A39" t="s">
         <v>40</v>
       </c>
@@ -8351,7 +8399,7 @@
       <c r="C39" t="s">
         <v>7</v>
       </c>
-      <c r="E39" t="s">
+      <c r="D39" t="s">
         <v>23</v>
       </c>
       <c r="F39" t="s">
@@ -8373,7 +8421,7 @@
         <v>23</v>
       </c>
     </row>
-    <row r="40" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="40" spans="1:13" x14ac:dyDescent="0.35">
       <c r="A40" t="s">
         <v>40</v>
       </c>
@@ -8383,7 +8431,7 @@
       <c r="C40" t="s">
         <v>2</v>
       </c>
-      <c r="E40" t="s">
+      <c r="D40" t="s">
         <v>23</v>
       </c>
       <c r="F40" t="s">
@@ -8408,7 +8456,7 @@
         <v>23</v>
       </c>
     </row>
-    <row r="41" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="41" spans="1:13" x14ac:dyDescent="0.35">
       <c r="A41" t="s">
         <v>40</v>
       </c>
@@ -8418,7 +8466,7 @@
       <c r="C41" t="s">
         <v>7</v>
       </c>
-      <c r="E41" t="s">
+      <c r="D41" t="s">
         <v>23</v>
       </c>
       <c r="F41" t="s">
@@ -8443,7 +8491,7 @@
         <v>23</v>
       </c>
     </row>
-    <row r="42" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="42" spans="1:13" x14ac:dyDescent="0.35">
       <c r="A42" t="s">
         <v>40</v>
       </c>
@@ -8453,7 +8501,7 @@
       <c r="C42" t="s">
         <v>2</v>
       </c>
-      <c r="E42" t="s">
+      <c r="D42" t="s">
         <v>23</v>
       </c>
       <c r="F42" t="s">
@@ -8481,7 +8529,7 @@
         <v>44</v>
       </c>
     </row>
-    <row r="43" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="43" spans="1:13" x14ac:dyDescent="0.35">
       <c r="A43" t="s">
         <v>40</v>
       </c>
@@ -8491,7 +8539,7 @@
       <c r="C43" t="s">
         <v>7</v>
       </c>
-      <c r="E43" t="s">
+      <c r="D43" t="s">
         <v>23</v>
       </c>
       <c r="F43" t="s">
@@ -8519,7 +8567,7 @@
         <v>44</v>
       </c>
     </row>
-    <row r="44" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="44" spans="1:13" x14ac:dyDescent="0.35">
       <c r="A44" t="s">
         <v>45</v>
       </c>
@@ -8545,7 +8593,7 @@
         <v>22</v>
       </c>
     </row>
-    <row r="45" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="45" spans="1:13" x14ac:dyDescent="0.35">
       <c r="A45" t="s">
         <v>45</v>
       </c>
@@ -8571,7 +8619,7 @@
         <v>22</v>
       </c>
     </row>
-    <row r="46" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="46" spans="1:13" x14ac:dyDescent="0.35">
       <c r="A46" t="s">
         <v>45</v>
       </c>
@@ -8581,7 +8629,7 @@
       <c r="C46" t="s">
         <v>2</v>
       </c>
-      <c r="E46" t="s">
+      <c r="D46" t="s">
         <v>23</v>
       </c>
       <c r="F46" t="s">
@@ -8603,7 +8651,7 @@
         <v>23</v>
       </c>
     </row>
-    <row r="47" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="47" spans="1:13" x14ac:dyDescent="0.35">
       <c r="A47" t="s">
         <v>45</v>
       </c>
@@ -8613,7 +8661,7 @@
       <c r="C47" t="s">
         <v>7</v>
       </c>
-      <c r="E47" t="s">
+      <c r="D47" t="s">
         <v>23</v>
       </c>
       <c r="F47" t="s">
@@ -8635,7 +8683,7 @@
         <v>23</v>
       </c>
     </row>
-    <row r="48" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="48" spans="1:13" x14ac:dyDescent="0.35">
       <c r="A48" t="s">
         <v>45</v>
       </c>
@@ -8645,7 +8693,7 @@
       <c r="C48" t="s">
         <v>2</v>
       </c>
-      <c r="E48" t="s">
+      <c r="D48" t="s">
         <v>23</v>
       </c>
       <c r="F48" t="s">
@@ -8670,7 +8718,7 @@
         <v>23</v>
       </c>
     </row>
-    <row r="49" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="49" spans="1:13" x14ac:dyDescent="0.35">
       <c r="A49" t="s">
         <v>45</v>
       </c>
@@ -8680,7 +8728,7 @@
       <c r="C49" t="s">
         <v>7</v>
       </c>
-      <c r="E49" t="s">
+      <c r="D49" t="s">
         <v>23</v>
       </c>
       <c r="F49" t="s">
@@ -8705,7 +8753,7 @@
         <v>23</v>
       </c>
     </row>
-    <row r="50" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="50" spans="1:13" x14ac:dyDescent="0.35">
       <c r="A50" t="s">
         <v>45</v>
       </c>
@@ -8715,7 +8763,7 @@
       <c r="C50" t="s">
         <v>2</v>
       </c>
-      <c r="E50" t="s">
+      <c r="D50" t="s">
         <v>23</v>
       </c>
       <c r="F50" t="s">
@@ -8743,7 +8791,7 @@
         <v>44</v>
       </c>
     </row>
-    <row r="51" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="51" spans="1:13" x14ac:dyDescent="0.35">
       <c r="A51" t="s">
         <v>45</v>
       </c>
@@ -8753,7 +8801,7 @@
       <c r="C51" t="s">
         <v>7</v>
       </c>
-      <c r="E51" t="s">
+      <c r="D51" t="s">
         <v>23</v>
       </c>
       <c r="F51" t="s">
@@ -8781,7 +8829,7 @@
         <v>44</v>
       </c>
     </row>
-    <row r="52" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="52" spans="1:13" x14ac:dyDescent="0.35">
       <c r="A52" t="s">
         <v>46</v>
       </c>
@@ -8791,7 +8839,7 @@
       <c r="C52" t="s">
         <v>2</v>
       </c>
-      <c r="E52" t="s">
+      <c r="D52" t="s">
         <v>23</v>
       </c>
       <c r="F52" t="s">
@@ -8813,7 +8861,7 @@
         <v>23</v>
       </c>
     </row>
-    <row r="53" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="53" spans="1:13" x14ac:dyDescent="0.35">
       <c r="A53" t="s">
         <v>46</v>
       </c>
@@ -8823,7 +8871,7 @@
       <c r="C53" t="s">
         <v>7</v>
       </c>
-      <c r="E53" t="s">
+      <c r="D53" t="s">
         <v>23</v>
       </c>
       <c r="F53" t="s">
@@ -8845,7 +8893,7 @@
         <v>23</v>
       </c>
     </row>
-    <row r="54" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="54" spans="1:13" x14ac:dyDescent="0.35">
       <c r="A54" t="s">
         <v>46</v>
       </c>
@@ -8865,7 +8913,7 @@
         <v>480</v>
       </c>
     </row>
-    <row r="55" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="55" spans="1:13" x14ac:dyDescent="0.35">
       <c r="A55" t="s">
         <v>28</v>
       </c>
@@ -8875,29 +8923,29 @@
       <c r="C55" t="s">
         <v>2</v>
       </c>
-      <c r="D55" t="s">
-        <v>28</v>
-      </c>
-      <c r="F55" s="17" t="s">
-        <v>11</v>
-      </c>
-      <c r="G55" s="17" t="s">
-        <v>5</v>
-      </c>
-      <c r="H55" s="17" t="s">
-        <v>4</v>
-      </c>
-      <c r="I55" s="17" t="s">
-        <v>3</v>
-      </c>
-      <c r="J55" s="17" t="s">
-        <v>31</v>
-      </c>
-      <c r="K55" s="17" t="s">
+      <c r="E55" t="s">
         <v>163</v>
       </c>
-    </row>
-    <row r="56" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="F55" t="s">
+        <v>51</v>
+      </c>
+      <c r="G55" s="14" t="s">
+        <v>50</v>
+      </c>
+      <c r="H55" t="s">
+        <v>47</v>
+      </c>
+      <c r="I55" t="s">
+        <v>49</v>
+      </c>
+      <c r="J55" t="s">
+        <v>48</v>
+      </c>
+      <c r="K55" s="14" t="s">
+        <v>163</v>
+      </c>
+    </row>
+    <row r="56" spans="1:13" x14ac:dyDescent="0.35">
       <c r="A56" t="s">
         <v>28</v>
       </c>
@@ -8907,25 +8955,89 @@
       <c r="C56" t="s">
         <v>8</v>
       </c>
-      <c r="D56" t="s">
+      <c r="E56" t="s">
+        <v>163</v>
+      </c>
+      <c r="F56" t="s">
+        <v>51</v>
+      </c>
+      <c r="G56" s="14" t="s">
+        <v>50</v>
+      </c>
+      <c r="H56" t="s">
+        <v>47</v>
+      </c>
+      <c r="I56" t="s">
+        <v>49</v>
+      </c>
+      <c r="J56" t="s">
+        <v>48</v>
+      </c>
+      <c r="K56" s="14" t="s">
+        <v>163</v>
+      </c>
+    </row>
+    <row r="57" spans="1:13" x14ac:dyDescent="0.35">
+      <c r="A57" t="s">
         <v>28</v>
       </c>
-      <c r="F56" s="17" t="s">
-        <v>11</v>
-      </c>
-      <c r="G56" s="17" t="s">
-        <v>5</v>
-      </c>
-      <c r="H56" s="17" t="s">
+      <c r="B57">
+        <v>3</v>
+      </c>
+      <c r="C57" t="s">
+        <v>2</v>
+      </c>
+      <c r="E57" t="s">
+        <v>28</v>
+      </c>
+      <c r="F57" t="s">
+        <v>51</v>
+      </c>
+      <c r="G57" s="14" t="s">
+        <v>50</v>
+      </c>
+      <c r="H57" t="s">
+        <v>47</v>
+      </c>
+      <c r="I57" t="s">
+        <v>49</v>
+      </c>
+      <c r="J57" t="s">
+        <v>48</v>
+      </c>
+      <c r="K57" s="14" t="s">
+        <v>163</v>
+      </c>
+    </row>
+    <row r="58" spans="1:13" x14ac:dyDescent="0.35">
+      <c r="A58" t="s">
+        <v>28</v>
+      </c>
+      <c r="B58">
         <v>4</v>
       </c>
-      <c r="I56" s="17" t="s">
-        <v>3</v>
-      </c>
-      <c r="J56" s="17" t="s">
-        <v>31</v>
-      </c>
-      <c r="K56" s="17" t="s">
+      <c r="C58" t="s">
+        <v>8</v>
+      </c>
+      <c r="E58" t="s">
+        <v>28</v>
+      </c>
+      <c r="F58" t="s">
+        <v>51</v>
+      </c>
+      <c r="G58" s="14" t="s">
+        <v>50</v>
+      </c>
+      <c r="H58" t="s">
+        <v>47</v>
+      </c>
+      <c r="I58" t="s">
+        <v>49</v>
+      </c>
+      <c r="J58" t="s">
+        <v>48</v>
+      </c>
+      <c r="K58" s="14" t="s">
         <v>163</v>
       </c>
     </row>

</xml_diff>

<commit_message>
changes. not done yet
</commit_message>
<xml_diff>
--- a/config/master_config.xlsx
+++ b/config/master_config.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\APERC\9th_edition_visualisation\config\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{9B300A1D-132B-43C4-8128-830E5EA83327}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="8_{2A65DEB6-F59B-4C28-91B9-2EDC9C976785}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-27045" yWindow="-16320" windowWidth="29040" windowHeight="15840" tabRatio="812" firstSheet="1" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -196,7 +196,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1501" uniqueCount="494">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1521" uniqueCount="494">
   <si>
     <t>chart_type</t>
   </si>
@@ -1903,6 +1903,7 @@
     <xf numFmtId="0" fontId="1" fillId="7" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
     <xf numFmtId="0" fontId="0" fillId="8" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="0" fontId="8" fillId="9" borderId="0" xfId="1"/>
+    <xf numFmtId="0" fontId="9" fillId="10" borderId="0" xfId="2"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="top"/>
     </xf>
@@ -1912,7 +1913,6 @@
     <xf numFmtId="0" fontId="2" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="top"/>
     </xf>
-    <xf numFmtId="0" fontId="9" fillId="10" borderId="0" xfId="2"/>
   </cellXfs>
   <cellStyles count="3">
     <cellStyle name="Bad" xfId="1" builtinId="27"/>
@@ -4410,8 +4410,8 @@
   </sheetPr>
   <dimension ref="A1:D52"/>
   <sheetViews>
-    <sheetView topLeftCell="A3" workbookViewId="0">
-      <selection activeCell="A19" sqref="A19:XFD19"/>
+    <sheetView topLeftCell="A25" workbookViewId="0">
+      <selection activeCell="B50" sqref="B50"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -4990,8 +4990,8 @@
   </sheetPr>
   <dimension ref="A1:C89"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A52" workbookViewId="0">
-      <selection activeCell="A80" sqref="A80"/>
+    <sheetView tabSelected="1" topLeftCell="A55" workbookViewId="0">
+      <selection activeCell="E70" sqref="E70"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -7281,12 +7281,12 @@
   <sheetPr>
     <tabColor theme="8"/>
   </sheetPr>
-  <dimension ref="A1:N56"/>
+  <dimension ref="A1:N58"/>
   <sheetViews>
-    <sheetView topLeftCell="B2" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A53" activePane="bottomLeft" state="frozen"/>
+    <sheetView topLeftCell="A2" workbookViewId="0">
+      <pane ySplit="1" topLeftCell="A38" activePane="bottomLeft" state="frozen"/>
       <selection activeCell="E2" sqref="E2"/>
-      <selection pane="bottomLeft" activeCell="D69" sqref="D69:D70"/>
+      <selection pane="bottomLeft" activeCell="C61" sqref="C61"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -7307,21 +7307,21 @@
     <row r="1" spans="1:14" x14ac:dyDescent="0.35">
       <c r="A1" s="1"/>
       <c r="B1" s="1"/>
-      <c r="D1" s="14" t="s">
+      <c r="D1" s="15" t="s">
         <v>488</v>
       </c>
-      <c r="E1" s="16"/>
-      <c r="F1" s="14" t="s">
+      <c r="E1" s="17"/>
+      <c r="F1" s="15" t="s">
         <v>475</v>
       </c>
-      <c r="G1" s="15"/>
-      <c r="H1" s="15"/>
-      <c r="I1" s="15"/>
-      <c r="J1" s="15"/>
-      <c r="K1" s="15"/>
-      <c r="L1" s="15"/>
-      <c r="M1" s="15"/>
-      <c r="N1" s="16"/>
+      <c r="G1" s="16"/>
+      <c r="H1" s="16"/>
+      <c r="I1" s="16"/>
+      <c r="J1" s="16"/>
+      <c r="K1" s="16"/>
+      <c r="L1" s="16"/>
+      <c r="M1" s="16"/>
+      <c r="N1" s="17"/>
     </row>
     <row r="2" spans="1:14" x14ac:dyDescent="0.35">
       <c r="A2" s="1" t="s">
@@ -8939,7 +8939,7 @@
       <c r="F55" t="s">
         <v>50</v>
       </c>
-      <c r="G55" s="17" t="s">
+      <c r="G55" s="14" t="s">
         <v>49</v>
       </c>
       <c r="H55" t="s">
@@ -8951,7 +8951,7 @@
       <c r="J55" t="s">
         <v>47</v>
       </c>
-      <c r="K55" s="17" t="s">
+      <c r="K55" s="14" t="s">
         <v>162</v>
       </c>
     </row>
@@ -8971,7 +8971,7 @@
       <c r="F56" t="s">
         <v>50</v>
       </c>
-      <c r="G56" s="17" t="s">
+      <c r="G56" s="14" t="s">
         <v>49</v>
       </c>
       <c r="H56" t="s">
@@ -8983,8 +8983,78 @@
       <c r="J56" t="s">
         <v>47</v>
       </c>
-      <c r="K56" s="17" t="s">
+      <c r="K56" s="14" t="s">
         <v>162</v>
+      </c>
+    </row>
+    <row r="57" spans="1:13" x14ac:dyDescent="0.35">
+      <c r="A57" t="s">
+        <v>24</v>
+      </c>
+      <c r="B57">
+        <v>3</v>
+      </c>
+      <c r="C57" t="s">
+        <v>2</v>
+      </c>
+      <c r="E57" t="s">
+        <v>24</v>
+      </c>
+      <c r="F57" t="s">
+        <v>175</v>
+      </c>
+      <c r="G57" t="s">
+        <v>178</v>
+      </c>
+      <c r="H57" t="s">
+        <v>180</v>
+      </c>
+      <c r="I57" t="s">
+        <v>182</v>
+      </c>
+      <c r="J57" t="s">
+        <v>184</v>
+      </c>
+      <c r="K57" t="s">
+        <v>186</v>
+      </c>
+      <c r="L57" t="s">
+        <v>188</v>
+      </c>
+    </row>
+    <row r="58" spans="1:13" x14ac:dyDescent="0.35">
+      <c r="A58" t="s">
+        <v>24</v>
+      </c>
+      <c r="B58">
+        <v>4</v>
+      </c>
+      <c r="C58" t="s">
+        <v>8</v>
+      </c>
+      <c r="E58" t="s">
+        <v>24</v>
+      </c>
+      <c r="F58" t="s">
+        <v>175</v>
+      </c>
+      <c r="G58" t="s">
+        <v>178</v>
+      </c>
+      <c r="H58" t="s">
+        <v>180</v>
+      </c>
+      <c r="I58" t="s">
+        <v>182</v>
+      </c>
+      <c r="J58" t="s">
+        <v>184</v>
+      </c>
+      <c r="K58" t="s">
+        <v>186</v>
+      </c>
+      <c r="L58" t="s">
+        <v>188</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
max value for y axis probably fixed
</commit_message>
<xml_diff>
--- a/config/master_config.xlsx
+++ b/config/master_config.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\hyuga.kasai\Documents\Github\9th_Visualization\9th_edition_visualisation\config\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F5C031F5-44BB-4B9E-B857-E28616D1A436}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C7BE17B4-AEE3-4CFA-A79C-24EA45E164C1}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="22050" yWindow="-16395" windowWidth="29040" windowHeight="15840" tabRatio="812" activeTab="7" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -23,7 +23,6 @@
     <sheet name="table_id_to_chart" sheetId="2" r:id="rId8"/>
   </sheets>
   <calcPr calcId="191029"/>
-  <fileRecoveryPr repairLoad="1"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
@@ -76,7 +75,7 @@
     Is lng equivalent to cng or do we need to add in a new fuel type? Should check balances</t>
       </text>
     </comment>
-    <comment ref="C58" authorId="1" shapeId="0" xr:uid="{89B88E45-46D2-4A21-AC6F-3EA3AEBCAB61}">
+    <comment ref="C62" authorId="1" shapeId="0" xr:uid="{89B88E45-46D2-4A21-AC6F-3EA3AEBCAB61}">
       <text>
         <r>
           <rPr>
@@ -197,7 +196,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1809" uniqueCount="494">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1882" uniqueCount="502">
   <si>
     <t>chart_type</t>
   </si>
@@ -1679,6 +1678,30 @@
   </si>
   <si>
     <t>TFC by fuel</t>
+  </si>
+  <si>
+    <t>Fuel consumption power sector</t>
+  </si>
+  <si>
+    <t>Crude oil</t>
+  </si>
+  <si>
+    <t>NGL</t>
+  </si>
+  <si>
+    <t>Other hydrocarbons</t>
+  </si>
+  <si>
+    <t>Naphtha</t>
+  </si>
+  <si>
+    <t>Kerosene</t>
+  </si>
+  <si>
+    <t>Other petroleum products</t>
+  </si>
+  <si>
+    <t>#b0bf1a</t>
   </si>
 </sst>
 </file>
@@ -4988,10 +5011,10 @@
   <sheetPr>
     <tabColor theme="8"/>
   </sheetPr>
-  <dimension ref="A1:C220"/>
+  <dimension ref="A1:C224"/>
   <sheetViews>
-    <sheetView topLeftCell="A21" workbookViewId="0">
-      <selection activeCell="A206" sqref="A206"/>
+    <sheetView topLeftCell="A7" workbookViewId="0">
+      <selection activeCell="A212" sqref="A212"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -5540,69 +5563,69 @@
       </c>
     </row>
     <row r="57" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A57" s="5" t="s">
-        <v>35</v>
+      <c r="A57" t="s">
+        <v>498</v>
       </c>
       <c r="B57" t="s">
-        <v>98</v>
+        <v>83</v>
       </c>
       <c r="C57" t="s">
-        <v>123</v>
+        <v>135</v>
       </c>
     </row>
     <row r="58" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A58" s="11" t="s">
-        <v>28</v>
-      </c>
-      <c r="B58" s="11" t="s">
-        <v>98</v>
-      </c>
-      <c r="C58" s="11" t="s">
-        <v>124</v>
+      <c r="A58" t="s">
+        <v>499</v>
+      </c>
+      <c r="B58" t="s">
+        <v>83</v>
+      </c>
+      <c r="C58" t="s">
+        <v>136</v>
       </c>
     </row>
     <row r="59" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A59" t="s">
-        <v>41</v>
+        <v>141</v>
       </c>
       <c r="B59" t="s">
         <v>83</v>
       </c>
       <c r="C59" t="s">
-        <v>128</v>
+        <v>137</v>
       </c>
     </row>
     <row r="60" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A60" t="s">
-        <v>41</v>
+        <v>500</v>
       </c>
       <c r="B60" t="s">
         <v>83</v>
       </c>
       <c r="C60" t="s">
-        <v>133</v>
+        <v>140</v>
       </c>
     </row>
     <row r="61" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A61" t="s">
-        <v>41</v>
+      <c r="A61" s="5" t="s">
+        <v>35</v>
       </c>
       <c r="B61" t="s">
-        <v>83</v>
+        <v>98</v>
       </c>
       <c r="C61" t="s">
-        <v>135</v>
+        <v>123</v>
       </c>
     </row>
     <row r="62" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A62" t="s">
-        <v>41</v>
-      </c>
-      <c r="B62" t="s">
-        <v>83</v>
-      </c>
-      <c r="C62" t="s">
-        <v>134</v>
+      <c r="A62" s="11" t="s">
+        <v>28</v>
+      </c>
+      <c r="B62" s="11" t="s">
+        <v>98</v>
+      </c>
+      <c r="C62" s="11" t="s">
+        <v>124</v>
       </c>
     </row>
     <row r="63" spans="1:3" x14ac:dyDescent="0.25">
@@ -5613,7 +5636,7 @@
         <v>83</v>
       </c>
       <c r="C63" t="s">
-        <v>136</v>
+        <v>128</v>
       </c>
     </row>
     <row r="64" spans="1:3" x14ac:dyDescent="0.25">
@@ -5624,7 +5647,7 @@
         <v>83</v>
       </c>
       <c r="C64" t="s">
-        <v>126</v>
+        <v>133</v>
       </c>
     </row>
     <row r="65" spans="1:3" x14ac:dyDescent="0.25">
@@ -5635,7 +5658,7 @@
         <v>83</v>
       </c>
       <c r="C65" t="s">
-        <v>137</v>
+        <v>135</v>
       </c>
     </row>
     <row r="66" spans="1:3" x14ac:dyDescent="0.25">
@@ -5646,7 +5669,7 @@
         <v>83</v>
       </c>
       <c r="C66" t="s">
-        <v>130</v>
+        <v>134</v>
       </c>
     </row>
     <row r="67" spans="1:3" x14ac:dyDescent="0.25">
@@ -5657,7 +5680,7 @@
         <v>83</v>
       </c>
       <c r="C67" t="s">
-        <v>138</v>
+        <v>136</v>
       </c>
     </row>
     <row r="68" spans="1:3" x14ac:dyDescent="0.25">
@@ -5668,7 +5691,7 @@
         <v>83</v>
       </c>
       <c r="C68" t="s">
-        <v>139</v>
+        <v>126</v>
       </c>
     </row>
     <row r="69" spans="1:3" x14ac:dyDescent="0.25">
@@ -5679,70 +5702,73 @@
         <v>83</v>
       </c>
       <c r="C69" t="s">
-        <v>140</v>
+        <v>137</v>
       </c>
     </row>
     <row r="70" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A70" t="s">
-        <v>141</v>
+        <v>41</v>
       </c>
       <c r="B70" t="s">
         <v>83</v>
       </c>
       <c r="C70" t="s">
-        <v>137</v>
+        <v>130</v>
       </c>
     </row>
     <row r="71" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A71" t="s">
-        <v>142</v>
+        <v>41</v>
       </c>
       <c r="B71" t="s">
-        <v>98</v>
+        <v>83</v>
       </c>
       <c r="C71" t="s">
-        <v>117</v>
+        <v>138</v>
       </c>
     </row>
     <row r="72" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A72" t="s">
-        <v>143</v>
+        <v>41</v>
       </c>
       <c r="B72" t="s">
-        <v>97</v>
+        <v>83</v>
+      </c>
+      <c r="C72" t="s">
+        <v>139</v>
       </c>
     </row>
     <row r="73" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A73" t="s">
-        <v>143</v>
+        <v>41</v>
       </c>
       <c r="B73" t="s">
-        <v>98</v>
+        <v>83</v>
       </c>
       <c r="C73" t="s">
-        <v>111</v>
+        <v>140</v>
       </c>
     </row>
     <row r="74" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A74" t="s">
-        <v>143</v>
+        <v>141</v>
       </c>
       <c r="B74" t="s">
-        <v>98</v>
+        <v>83</v>
       </c>
       <c r="C74" t="s">
-        <v>113</v>
+        <v>137</v>
       </c>
     </row>
     <row r="75" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A75" t="s">
-        <v>143</v>
+        <v>142</v>
       </c>
       <c r="B75" t="s">
         <v>98</v>
       </c>
       <c r="C75" t="s">
-        <v>115</v>
+        <v>117</v>
       </c>
     </row>
     <row r="76" spans="1:3" x14ac:dyDescent="0.25">
@@ -5750,10 +5776,7 @@
         <v>143</v>
       </c>
       <c r="B76" t="s">
-        <v>98</v>
-      </c>
-      <c r="C76" t="s">
-        <v>116</v>
+        <v>97</v>
       </c>
     </row>
     <row r="77" spans="1:3" x14ac:dyDescent="0.25">
@@ -5764,7 +5787,7 @@
         <v>98</v>
       </c>
       <c r="C77" t="s">
-        <v>117</v>
+        <v>111</v>
       </c>
     </row>
     <row r="78" spans="1:3" x14ac:dyDescent="0.25">
@@ -5775,183 +5798,195 @@
         <v>98</v>
       </c>
       <c r="C78" t="s">
-        <v>118</v>
+        <v>113</v>
       </c>
     </row>
     <row r="79" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A79" t="s">
-        <v>27</v>
+        <v>143</v>
       </c>
       <c r="B79" t="s">
-        <v>77</v>
+        <v>98</v>
+      </c>
+      <c r="C79" t="s">
+        <v>115</v>
       </c>
     </row>
     <row r="80" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A80" t="s">
-        <v>27</v>
+        <v>143</v>
       </c>
       <c r="B80" t="s">
-        <v>78</v>
-      </c>
-    </row>
-    <row r="81" spans="1:2" x14ac:dyDescent="0.25">
+        <v>98</v>
+      </c>
+      <c r="C80" t="s">
+        <v>116</v>
+      </c>
+    </row>
+    <row r="81" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A81" t="s">
-        <v>27</v>
+        <v>143</v>
       </c>
       <c r="B81" t="s">
-        <v>79</v>
-      </c>
-    </row>
-    <row r="82" spans="1:2" x14ac:dyDescent="0.25">
+        <v>98</v>
+      </c>
+      <c r="C81" t="s">
+        <v>117</v>
+      </c>
+    </row>
+    <row r="82" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A82" t="s">
-        <v>27</v>
+        <v>143</v>
       </c>
       <c r="B82" t="s">
-        <v>80</v>
-      </c>
-    </row>
-    <row r="83" spans="1:2" x14ac:dyDescent="0.25">
+        <v>98</v>
+      </c>
+      <c r="C82" t="s">
+        <v>118</v>
+      </c>
+    </row>
+    <row r="83" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A83" t="s">
         <v>27</v>
       </c>
       <c r="B83" t="s">
-        <v>81</v>
-      </c>
-    </row>
-    <row r="84" spans="1:2" x14ac:dyDescent="0.25">
+        <v>77</v>
+      </c>
+    </row>
+    <row r="84" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A84" t="s">
         <v>27</v>
       </c>
       <c r="B84" t="s">
-        <v>82</v>
-      </c>
-    </row>
-    <row r="85" spans="1:2" x14ac:dyDescent="0.25">
+        <v>78</v>
+      </c>
+    </row>
+    <row r="85" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A85" t="s">
         <v>27</v>
       </c>
       <c r="B85" t="s">
-        <v>83</v>
-      </c>
-    </row>
-    <row r="86" spans="1:2" x14ac:dyDescent="0.25">
+        <v>79</v>
+      </c>
+    </row>
+    <row r="86" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A86" t="s">
         <v>27</v>
       </c>
       <c r="B86" t="s">
-        <v>84</v>
-      </c>
-    </row>
-    <row r="87" spans="1:2" x14ac:dyDescent="0.25">
+        <v>80</v>
+      </c>
+    </row>
+    <row r="87" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A87" t="s">
         <v>27</v>
       </c>
       <c r="B87" t="s">
-        <v>86</v>
-      </c>
-    </row>
-    <row r="88" spans="1:2" x14ac:dyDescent="0.25">
+        <v>81</v>
+      </c>
+    </row>
+    <row r="88" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A88" t="s">
         <v>27</v>
       </c>
       <c r="B88" t="s">
-        <v>88</v>
-      </c>
-    </row>
-    <row r="89" spans="1:2" x14ac:dyDescent="0.25">
+        <v>82</v>
+      </c>
+    </row>
+    <row r="89" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A89" t="s">
         <v>27</v>
       </c>
       <c r="B89" t="s">
-        <v>90</v>
-      </c>
-    </row>
-    <row r="90" spans="1:2" x14ac:dyDescent="0.25">
+        <v>83</v>
+      </c>
+    </row>
+    <row r="90" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A90" t="s">
         <v>27</v>
       </c>
       <c r="B90" t="s">
-        <v>92</v>
-      </c>
-    </row>
-    <row r="91" spans="1:2" x14ac:dyDescent="0.25">
+        <v>84</v>
+      </c>
+    </row>
+    <row r="91" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A91" t="s">
         <v>27</v>
       </c>
       <c r="B91" t="s">
-        <v>94</v>
-      </c>
-    </row>
-    <row r="92" spans="1:2" x14ac:dyDescent="0.25">
+        <v>86</v>
+      </c>
+    </row>
+    <row r="92" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A92" t="s">
         <v>27</v>
       </c>
       <c r="B92" t="s">
-        <v>96</v>
-      </c>
-    </row>
-    <row r="93" spans="1:2" x14ac:dyDescent="0.25">
+        <v>88</v>
+      </c>
+    </row>
+    <row r="93" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A93" t="s">
         <v>27</v>
       </c>
       <c r="B93" t="s">
-        <v>97</v>
-      </c>
-    </row>
-    <row r="94" spans="1:2" x14ac:dyDescent="0.25">
+        <v>90</v>
+      </c>
+    </row>
+    <row r="94" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A94" t="s">
         <v>27</v>
       </c>
       <c r="B94" t="s">
-        <v>98</v>
-      </c>
-    </row>
-    <row r="95" spans="1:2" x14ac:dyDescent="0.25">
+        <v>92</v>
+      </c>
+    </row>
+    <row r="95" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A95" t="s">
         <v>27</v>
       </c>
       <c r="B95" t="s">
-        <v>100</v>
-      </c>
-    </row>
-    <row r="96" spans="1:2" x14ac:dyDescent="0.25">
+        <v>94</v>
+      </c>
+    </row>
+    <row r="96" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A96" t="s">
         <v>27</v>
       </c>
       <c r="B96" t="s">
-        <v>102</v>
+        <v>96</v>
       </c>
     </row>
     <row r="97" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A97" t="s">
-        <v>13</v>
+        <v>27</v>
       </c>
       <c r="B97" t="s">
-        <v>77</v>
+        <v>97</v>
       </c>
     </row>
     <row r="98" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A98" t="s">
-        <v>13</v>
+        <v>27</v>
       </c>
       <c r="B98" t="s">
-        <v>78</v>
+        <v>98</v>
       </c>
     </row>
     <row r="99" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A99" t="s">
-        <v>13</v>
+        <v>27</v>
       </c>
       <c r="B99" t="s">
-        <v>79</v>
+        <v>100</v>
       </c>
     </row>
     <row r="100" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A100" t="s">
-        <v>13</v>
+        <v>27</v>
       </c>
       <c r="B100" t="s">
-        <v>80</v>
+        <v>102</v>
       </c>
     </row>
     <row r="101" spans="1:2" x14ac:dyDescent="0.25">
@@ -5959,7 +5994,7 @@
         <v>13</v>
       </c>
       <c r="B101" t="s">
-        <v>81</v>
+        <v>77</v>
       </c>
     </row>
     <row r="102" spans="1:2" x14ac:dyDescent="0.25">
@@ -5967,7 +6002,7 @@
         <v>13</v>
       </c>
       <c r="B102" t="s">
-        <v>82</v>
+        <v>78</v>
       </c>
     </row>
     <row r="103" spans="1:2" x14ac:dyDescent="0.25">
@@ -5975,7 +6010,7 @@
         <v>13</v>
       </c>
       <c r="B103" t="s">
-        <v>83</v>
+        <v>79</v>
       </c>
     </row>
     <row r="104" spans="1:2" x14ac:dyDescent="0.25">
@@ -5983,7 +6018,7 @@
         <v>13</v>
       </c>
       <c r="B104" t="s">
-        <v>84</v>
+        <v>80</v>
       </c>
     </row>
     <row r="105" spans="1:2" x14ac:dyDescent="0.25">
@@ -5991,7 +6026,7 @@
         <v>13</v>
       </c>
       <c r="B105" t="s">
-        <v>86</v>
+        <v>81</v>
       </c>
     </row>
     <row r="106" spans="1:2" x14ac:dyDescent="0.25">
@@ -5999,7 +6034,7 @@
         <v>13</v>
       </c>
       <c r="B106" t="s">
-        <v>88</v>
+        <v>82</v>
       </c>
     </row>
     <row r="107" spans="1:2" x14ac:dyDescent="0.25">
@@ -6007,7 +6042,7 @@
         <v>13</v>
       </c>
       <c r="B107" t="s">
-        <v>90</v>
+        <v>83</v>
       </c>
     </row>
     <row r="108" spans="1:2" x14ac:dyDescent="0.25">
@@ -6015,7 +6050,7 @@
         <v>13</v>
       </c>
       <c r="B108" t="s">
-        <v>92</v>
+        <v>84</v>
       </c>
     </row>
     <row r="109" spans="1:2" x14ac:dyDescent="0.25">
@@ -6023,7 +6058,7 @@
         <v>13</v>
       </c>
       <c r="B109" t="s">
-        <v>94</v>
+        <v>86</v>
       </c>
     </row>
     <row r="110" spans="1:2" x14ac:dyDescent="0.25">
@@ -6031,7 +6066,7 @@
         <v>13</v>
       </c>
       <c r="B110" t="s">
-        <v>96</v>
+        <v>88</v>
       </c>
     </row>
     <row r="111" spans="1:2" x14ac:dyDescent="0.25">
@@ -6039,7 +6074,7 @@
         <v>13</v>
       </c>
       <c r="B111" t="s">
-        <v>97</v>
+        <v>90</v>
       </c>
     </row>
     <row r="112" spans="1:2" x14ac:dyDescent="0.25">
@@ -6047,7 +6082,7 @@
         <v>13</v>
       </c>
       <c r="B112" t="s">
-        <v>98</v>
+        <v>92</v>
       </c>
     </row>
     <row r="113" spans="1:2" x14ac:dyDescent="0.25">
@@ -6055,7 +6090,7 @@
         <v>13</v>
       </c>
       <c r="B113" t="s">
-        <v>100</v>
+        <v>94</v>
       </c>
     </row>
     <row r="114" spans="1:2" x14ac:dyDescent="0.25">
@@ -6063,39 +6098,39 @@
         <v>13</v>
       </c>
       <c r="B114" t="s">
-        <v>102</v>
+        <v>96</v>
       </c>
     </row>
     <row r="115" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A115" t="s">
-        <v>24</v>
+        <v>13</v>
       </c>
       <c r="B115" t="s">
-        <v>77</v>
+        <v>97</v>
       </c>
     </row>
     <row r="116" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A116" t="s">
-        <v>24</v>
+        <v>13</v>
       </c>
       <c r="B116" t="s">
-        <v>78</v>
+        <v>98</v>
       </c>
     </row>
     <row r="117" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A117" t="s">
-        <v>24</v>
+        <v>13</v>
       </c>
       <c r="B117" t="s">
-        <v>79</v>
+        <v>100</v>
       </c>
     </row>
     <row r="118" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A118" t="s">
-        <v>24</v>
+        <v>13</v>
       </c>
       <c r="B118" t="s">
-        <v>80</v>
+        <v>102</v>
       </c>
     </row>
     <row r="119" spans="1:2" x14ac:dyDescent="0.25">
@@ -6103,7 +6138,7 @@
         <v>24</v>
       </c>
       <c r="B119" t="s">
-        <v>81</v>
+        <v>77</v>
       </c>
     </row>
     <row r="120" spans="1:2" x14ac:dyDescent="0.25">
@@ -6111,7 +6146,7 @@
         <v>24</v>
       </c>
       <c r="B120" t="s">
-        <v>82</v>
+        <v>78</v>
       </c>
     </row>
     <row r="121" spans="1:2" x14ac:dyDescent="0.25">
@@ -6119,7 +6154,7 @@
         <v>24</v>
       </c>
       <c r="B121" t="s">
-        <v>83</v>
+        <v>79</v>
       </c>
     </row>
     <row r="122" spans="1:2" x14ac:dyDescent="0.25">
@@ -6127,7 +6162,7 @@
         <v>24</v>
       </c>
       <c r="B122" t="s">
-        <v>84</v>
+        <v>80</v>
       </c>
     </row>
     <row r="123" spans="1:2" x14ac:dyDescent="0.25">
@@ -6135,7 +6170,7 @@
         <v>24</v>
       </c>
       <c r="B123" t="s">
-        <v>86</v>
+        <v>81</v>
       </c>
     </row>
     <row r="124" spans="1:2" x14ac:dyDescent="0.25">
@@ -6143,7 +6178,7 @@
         <v>24</v>
       </c>
       <c r="B124" t="s">
-        <v>88</v>
+        <v>82</v>
       </c>
     </row>
     <row r="125" spans="1:2" x14ac:dyDescent="0.25">
@@ -6151,7 +6186,7 @@
         <v>24</v>
       </c>
       <c r="B125" t="s">
-        <v>90</v>
+        <v>83</v>
       </c>
     </row>
     <row r="126" spans="1:2" x14ac:dyDescent="0.25">
@@ -6159,7 +6194,7 @@
         <v>24</v>
       </c>
       <c r="B126" t="s">
-        <v>92</v>
+        <v>84</v>
       </c>
     </row>
     <row r="127" spans="1:2" x14ac:dyDescent="0.25">
@@ -6167,7 +6202,7 @@
         <v>24</v>
       </c>
       <c r="B127" t="s">
-        <v>94</v>
+        <v>86</v>
       </c>
     </row>
     <row r="128" spans="1:2" x14ac:dyDescent="0.25">
@@ -6175,7 +6210,7 @@
         <v>24</v>
       </c>
       <c r="B128" t="s">
-        <v>96</v>
+        <v>88</v>
       </c>
     </row>
     <row r="129" spans="1:2" x14ac:dyDescent="0.25">
@@ -6183,7 +6218,7 @@
         <v>24</v>
       </c>
       <c r="B129" t="s">
-        <v>97</v>
+        <v>90</v>
       </c>
     </row>
     <row r="130" spans="1:2" x14ac:dyDescent="0.25">
@@ -6191,7 +6226,7 @@
         <v>24</v>
       </c>
       <c r="B130" t="s">
-        <v>98</v>
+        <v>92</v>
       </c>
     </row>
     <row r="131" spans="1:2" x14ac:dyDescent="0.25">
@@ -6199,7 +6234,7 @@
         <v>24</v>
       </c>
       <c r="B131" t="s">
-        <v>100</v>
+        <v>94</v>
       </c>
     </row>
     <row r="132" spans="1:2" x14ac:dyDescent="0.25">
@@ -6207,39 +6242,39 @@
         <v>24</v>
       </c>
       <c r="B132" t="s">
-        <v>102</v>
+        <v>96</v>
       </c>
     </row>
     <row r="133" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A133" t="s">
-        <v>1</v>
+        <v>24</v>
       </c>
       <c r="B133" t="s">
-        <v>77</v>
+        <v>97</v>
       </c>
     </row>
     <row r="134" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A134" t="s">
-        <v>1</v>
+        <v>24</v>
       </c>
       <c r="B134" t="s">
-        <v>78</v>
+        <v>98</v>
       </c>
     </row>
     <row r="135" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A135" t="s">
-        <v>1</v>
+        <v>24</v>
       </c>
       <c r="B135" t="s">
-        <v>79</v>
+        <v>100</v>
       </c>
     </row>
     <row r="136" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A136" t="s">
-        <v>1</v>
+        <v>24</v>
       </c>
       <c r="B136" t="s">
-        <v>80</v>
+        <v>102</v>
       </c>
     </row>
     <row r="137" spans="1:2" x14ac:dyDescent="0.25">
@@ -6247,7 +6282,7 @@
         <v>1</v>
       </c>
       <c r="B137" t="s">
-        <v>81</v>
+        <v>77</v>
       </c>
     </row>
     <row r="138" spans="1:2" x14ac:dyDescent="0.25">
@@ -6255,7 +6290,7 @@
         <v>1</v>
       </c>
       <c r="B138" t="s">
-        <v>82</v>
+        <v>78</v>
       </c>
     </row>
     <row r="139" spans="1:2" x14ac:dyDescent="0.25">
@@ -6263,7 +6298,7 @@
         <v>1</v>
       </c>
       <c r="B139" t="s">
-        <v>83</v>
+        <v>79</v>
       </c>
     </row>
     <row r="140" spans="1:2" x14ac:dyDescent="0.25">
@@ -6271,7 +6306,7 @@
         <v>1</v>
       </c>
       <c r="B140" t="s">
-        <v>84</v>
+        <v>80</v>
       </c>
     </row>
     <row r="141" spans="1:2" x14ac:dyDescent="0.25">
@@ -6279,7 +6314,7 @@
         <v>1</v>
       </c>
       <c r="B141" t="s">
-        <v>86</v>
+        <v>81</v>
       </c>
     </row>
     <row r="142" spans="1:2" x14ac:dyDescent="0.25">
@@ -6287,7 +6322,7 @@
         <v>1</v>
       </c>
       <c r="B142" t="s">
-        <v>88</v>
+        <v>82</v>
       </c>
     </row>
     <row r="143" spans="1:2" x14ac:dyDescent="0.25">
@@ -6295,7 +6330,7 @@
         <v>1</v>
       </c>
       <c r="B143" t="s">
-        <v>90</v>
+        <v>83</v>
       </c>
     </row>
     <row r="144" spans="1:2" x14ac:dyDescent="0.25">
@@ -6303,7 +6338,7 @@
         <v>1</v>
       </c>
       <c r="B144" t="s">
-        <v>92</v>
+        <v>84</v>
       </c>
     </row>
     <row r="145" spans="1:2" x14ac:dyDescent="0.25">
@@ -6311,7 +6346,7 @@
         <v>1</v>
       </c>
       <c r="B145" t="s">
-        <v>94</v>
+        <v>86</v>
       </c>
     </row>
     <row r="146" spans="1:2" x14ac:dyDescent="0.25">
@@ -6319,7 +6354,7 @@
         <v>1</v>
       </c>
       <c r="B146" t="s">
-        <v>96</v>
+        <v>88</v>
       </c>
     </row>
     <row r="147" spans="1:2" x14ac:dyDescent="0.25">
@@ -6327,7 +6362,7 @@
         <v>1</v>
       </c>
       <c r="B147" t="s">
-        <v>97</v>
+        <v>90</v>
       </c>
     </row>
     <row r="148" spans="1:2" x14ac:dyDescent="0.25">
@@ -6335,7 +6370,7 @@
         <v>1</v>
       </c>
       <c r="B148" t="s">
-        <v>98</v>
+        <v>92</v>
       </c>
     </row>
     <row r="149" spans="1:2" x14ac:dyDescent="0.25">
@@ -6343,7 +6378,7 @@
         <v>1</v>
       </c>
       <c r="B149" t="s">
-        <v>100</v>
+        <v>94</v>
       </c>
     </row>
     <row r="150" spans="1:2" x14ac:dyDescent="0.25">
@@ -6351,39 +6386,39 @@
         <v>1</v>
       </c>
       <c r="B150" t="s">
-        <v>102</v>
+        <v>96</v>
       </c>
     </row>
     <row r="151" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A151" t="s">
-        <v>22</v>
+        <v>1</v>
       </c>
       <c r="B151" t="s">
-        <v>77</v>
+        <v>97</v>
       </c>
     </row>
     <row r="152" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A152" t="s">
-        <v>22</v>
+        <v>1</v>
       </c>
       <c r="B152" t="s">
-        <v>78</v>
+        <v>98</v>
       </c>
     </row>
     <row r="153" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A153" t="s">
-        <v>22</v>
+        <v>1</v>
       </c>
       <c r="B153" t="s">
-        <v>79</v>
+        <v>100</v>
       </c>
     </row>
     <row r="154" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A154" t="s">
-        <v>22</v>
+        <v>1</v>
       </c>
       <c r="B154" t="s">
-        <v>80</v>
+        <v>102</v>
       </c>
     </row>
     <row r="155" spans="1:2" x14ac:dyDescent="0.25">
@@ -6391,7 +6426,7 @@
         <v>22</v>
       </c>
       <c r="B155" t="s">
-        <v>81</v>
+        <v>77</v>
       </c>
     </row>
     <row r="156" spans="1:2" x14ac:dyDescent="0.25">
@@ -6399,7 +6434,7 @@
         <v>22</v>
       </c>
       <c r="B156" t="s">
-        <v>82</v>
+        <v>78</v>
       </c>
     </row>
     <row r="157" spans="1:2" x14ac:dyDescent="0.25">
@@ -6407,7 +6442,7 @@
         <v>22</v>
       </c>
       <c r="B157" t="s">
-        <v>83</v>
+        <v>79</v>
       </c>
     </row>
     <row r="158" spans="1:2" x14ac:dyDescent="0.25">
@@ -6415,7 +6450,7 @@
         <v>22</v>
       </c>
       <c r="B158" t="s">
-        <v>84</v>
+        <v>80</v>
       </c>
     </row>
     <row r="159" spans="1:2" x14ac:dyDescent="0.25">
@@ -6423,7 +6458,7 @@
         <v>22</v>
       </c>
       <c r="B159" t="s">
-        <v>86</v>
+        <v>81</v>
       </c>
     </row>
     <row r="160" spans="1:2" x14ac:dyDescent="0.25">
@@ -6431,7 +6466,7 @@
         <v>22</v>
       </c>
       <c r="B160" t="s">
-        <v>88</v>
+        <v>82</v>
       </c>
     </row>
     <row r="161" spans="1:2" x14ac:dyDescent="0.25">
@@ -6439,7 +6474,7 @@
         <v>22</v>
       </c>
       <c r="B161" t="s">
-        <v>90</v>
+        <v>83</v>
       </c>
     </row>
     <row r="162" spans="1:2" x14ac:dyDescent="0.25">
@@ -6447,7 +6482,7 @@
         <v>22</v>
       </c>
       <c r="B162" t="s">
-        <v>92</v>
+        <v>84</v>
       </c>
     </row>
     <row r="163" spans="1:2" x14ac:dyDescent="0.25">
@@ -6455,7 +6490,7 @@
         <v>22</v>
       </c>
       <c r="B163" t="s">
-        <v>94</v>
+        <v>86</v>
       </c>
     </row>
     <row r="164" spans="1:2" x14ac:dyDescent="0.25">
@@ -6463,7 +6498,7 @@
         <v>22</v>
       </c>
       <c r="B164" t="s">
-        <v>96</v>
+        <v>88</v>
       </c>
     </row>
     <row r="165" spans="1:2" x14ac:dyDescent="0.25">
@@ -6471,7 +6506,7 @@
         <v>22</v>
       </c>
       <c r="B165" t="s">
-        <v>97</v>
+        <v>90</v>
       </c>
     </row>
     <row r="166" spans="1:2" x14ac:dyDescent="0.25">
@@ -6479,7 +6514,7 @@
         <v>22</v>
       </c>
       <c r="B166" t="s">
-        <v>98</v>
+        <v>92</v>
       </c>
     </row>
     <row r="167" spans="1:2" x14ac:dyDescent="0.25">
@@ -6487,7 +6522,7 @@
         <v>22</v>
       </c>
       <c r="B167" t="s">
-        <v>100</v>
+        <v>94</v>
       </c>
     </row>
     <row r="168" spans="1:2" x14ac:dyDescent="0.25">
@@ -6495,39 +6530,39 @@
         <v>22</v>
       </c>
       <c r="B168" t="s">
-        <v>102</v>
+        <v>96</v>
       </c>
     </row>
     <row r="169" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A169" t="s">
-        <v>161</v>
+        <v>22</v>
       </c>
       <c r="B169" t="s">
-        <v>77</v>
+        <v>97</v>
       </c>
     </row>
     <row r="170" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A170" t="s">
-        <v>161</v>
+        <v>22</v>
       </c>
       <c r="B170" t="s">
-        <v>78</v>
+        <v>98</v>
       </c>
     </row>
     <row r="171" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A171" t="s">
-        <v>161</v>
+        <v>22</v>
       </c>
       <c r="B171" t="s">
-        <v>79</v>
+        <v>100</v>
       </c>
     </row>
     <row r="172" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A172" t="s">
-        <v>161</v>
+        <v>22</v>
       </c>
       <c r="B172" t="s">
-        <v>80</v>
+        <v>102</v>
       </c>
     </row>
     <row r="173" spans="1:2" x14ac:dyDescent="0.25">
@@ -6535,7 +6570,7 @@
         <v>161</v>
       </c>
       <c r="B173" t="s">
-        <v>81</v>
+        <v>77</v>
       </c>
     </row>
     <row r="174" spans="1:2" x14ac:dyDescent="0.25">
@@ -6543,7 +6578,7 @@
         <v>161</v>
       </c>
       <c r="B174" t="s">
-        <v>82</v>
+        <v>78</v>
       </c>
     </row>
     <row r="175" spans="1:2" x14ac:dyDescent="0.25">
@@ -6551,7 +6586,7 @@
         <v>161</v>
       </c>
       <c r="B175" t="s">
-        <v>83</v>
+        <v>79</v>
       </c>
     </row>
     <row r="176" spans="1:2" x14ac:dyDescent="0.25">
@@ -6559,7 +6594,7 @@
         <v>161</v>
       </c>
       <c r="B176" t="s">
-        <v>84</v>
+        <v>80</v>
       </c>
     </row>
     <row r="177" spans="1:2" x14ac:dyDescent="0.25">
@@ -6567,7 +6602,7 @@
         <v>161</v>
       </c>
       <c r="B177" t="s">
-        <v>86</v>
+        <v>81</v>
       </c>
     </row>
     <row r="178" spans="1:2" x14ac:dyDescent="0.25">
@@ -6575,7 +6610,7 @@
         <v>161</v>
       </c>
       <c r="B178" t="s">
-        <v>88</v>
+        <v>82</v>
       </c>
     </row>
     <row r="179" spans="1:2" x14ac:dyDescent="0.25">
@@ -6583,7 +6618,7 @@
         <v>161</v>
       </c>
       <c r="B179" t="s">
-        <v>90</v>
+        <v>83</v>
       </c>
     </row>
     <row r="180" spans="1:2" x14ac:dyDescent="0.25">
@@ -6591,7 +6626,7 @@
         <v>161</v>
       </c>
       <c r="B180" t="s">
-        <v>92</v>
+        <v>84</v>
       </c>
     </row>
     <row r="181" spans="1:2" x14ac:dyDescent="0.25">
@@ -6599,7 +6634,7 @@
         <v>161</v>
       </c>
       <c r="B181" t="s">
-        <v>94</v>
+        <v>86</v>
       </c>
     </row>
     <row r="182" spans="1:2" x14ac:dyDescent="0.25">
@@ -6607,7 +6642,7 @@
         <v>161</v>
       </c>
       <c r="B182" t="s">
-        <v>96</v>
+        <v>88</v>
       </c>
     </row>
     <row r="183" spans="1:2" x14ac:dyDescent="0.25">
@@ -6615,7 +6650,7 @@
         <v>161</v>
       </c>
       <c r="B183" t="s">
-        <v>97</v>
+        <v>90</v>
       </c>
     </row>
     <row r="184" spans="1:2" x14ac:dyDescent="0.25">
@@ -6623,7 +6658,7 @@
         <v>161</v>
       </c>
       <c r="B184" t="s">
-        <v>98</v>
+        <v>92</v>
       </c>
     </row>
     <row r="185" spans="1:2" x14ac:dyDescent="0.25">
@@ -6631,7 +6666,7 @@
         <v>161</v>
       </c>
       <c r="B185" t="s">
-        <v>100</v>
+        <v>94</v>
       </c>
     </row>
     <row r="186" spans="1:2" x14ac:dyDescent="0.25">
@@ -6639,39 +6674,39 @@
         <v>161</v>
       </c>
       <c r="B186" t="s">
-        <v>102</v>
+        <v>96</v>
       </c>
     </row>
     <row r="187" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A187" t="s">
-        <v>159</v>
+        <v>161</v>
       </c>
       <c r="B187" t="s">
-        <v>77</v>
+        <v>97</v>
       </c>
     </row>
     <row r="188" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A188" t="s">
-        <v>159</v>
+        <v>161</v>
       </c>
       <c r="B188" t="s">
-        <v>78</v>
+        <v>98</v>
       </c>
     </row>
     <row r="189" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A189" t="s">
-        <v>159</v>
+        <v>161</v>
       </c>
       <c r="B189" t="s">
-        <v>79</v>
+        <v>100</v>
       </c>
     </row>
     <row r="190" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A190" t="s">
-        <v>159</v>
+        <v>161</v>
       </c>
       <c r="B190" t="s">
-        <v>80</v>
+        <v>102</v>
       </c>
     </row>
     <row r="191" spans="1:2" x14ac:dyDescent="0.25">
@@ -6679,7 +6714,7 @@
         <v>159</v>
       </c>
       <c r="B191" t="s">
-        <v>81</v>
+        <v>77</v>
       </c>
     </row>
     <row r="192" spans="1:2" x14ac:dyDescent="0.25">
@@ -6687,7 +6722,7 @@
         <v>159</v>
       </c>
       <c r="B192" t="s">
-        <v>82</v>
+        <v>78</v>
       </c>
     </row>
     <row r="193" spans="1:2" x14ac:dyDescent="0.25">
@@ -6695,7 +6730,7 @@
         <v>159</v>
       </c>
       <c r="B193" t="s">
-        <v>83</v>
+        <v>79</v>
       </c>
     </row>
     <row r="194" spans="1:2" x14ac:dyDescent="0.25">
@@ -6703,7 +6738,7 @@
         <v>159</v>
       </c>
       <c r="B194" t="s">
-        <v>84</v>
+        <v>80</v>
       </c>
     </row>
     <row r="195" spans="1:2" x14ac:dyDescent="0.25">
@@ -6711,7 +6746,7 @@
         <v>159</v>
       </c>
       <c r="B195" t="s">
-        <v>86</v>
+        <v>81</v>
       </c>
     </row>
     <row r="196" spans="1:2" x14ac:dyDescent="0.25">
@@ -6719,7 +6754,7 @@
         <v>159</v>
       </c>
       <c r="B196" t="s">
-        <v>88</v>
+        <v>82</v>
       </c>
     </row>
     <row r="197" spans="1:2" x14ac:dyDescent="0.25">
@@ -6727,7 +6762,7 @@
         <v>159</v>
       </c>
       <c r="B197" t="s">
-        <v>90</v>
+        <v>83</v>
       </c>
     </row>
     <row r="198" spans="1:2" x14ac:dyDescent="0.25">
@@ -6735,7 +6770,7 @@
         <v>159</v>
       </c>
       <c r="B198" t="s">
-        <v>92</v>
+        <v>84</v>
       </c>
     </row>
     <row r="199" spans="1:2" x14ac:dyDescent="0.25">
@@ -6743,7 +6778,7 @@
         <v>159</v>
       </c>
       <c r="B199" t="s">
-        <v>94</v>
+        <v>86</v>
       </c>
     </row>
     <row r="200" spans="1:2" x14ac:dyDescent="0.25">
@@ -6751,7 +6786,7 @@
         <v>159</v>
       </c>
       <c r="B200" t="s">
-        <v>96</v>
+        <v>88</v>
       </c>
     </row>
     <row r="201" spans="1:2" x14ac:dyDescent="0.25">
@@ -6759,7 +6794,7 @@
         <v>159</v>
       </c>
       <c r="B201" t="s">
-        <v>97</v>
+        <v>90</v>
       </c>
     </row>
     <row r="202" spans="1:2" x14ac:dyDescent="0.25">
@@ -6767,7 +6802,7 @@
         <v>159</v>
       </c>
       <c r="B202" t="s">
-        <v>98</v>
+        <v>92</v>
       </c>
     </row>
     <row r="203" spans="1:2" x14ac:dyDescent="0.25">
@@ -6775,7 +6810,7 @@
         <v>159</v>
       </c>
       <c r="B203" t="s">
-        <v>100</v>
+        <v>94</v>
       </c>
     </row>
     <row r="204" spans="1:2" x14ac:dyDescent="0.25">
@@ -6783,11 +6818,76 @@
         <v>159</v>
       </c>
       <c r="B204" t="s">
+        <v>96</v>
+      </c>
+    </row>
+    <row r="205" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A205" t="s">
+        <v>159</v>
+      </c>
+      <c r="B205" t="s">
+        <v>97</v>
+      </c>
+    </row>
+    <row r="206" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A206" t="s">
+        <v>159</v>
+      </c>
+      <c r="B206" t="s">
+        <v>98</v>
+      </c>
+    </row>
+    <row r="207" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A207" t="s">
+        <v>159</v>
+      </c>
+      <c r="B207" t="s">
+        <v>100</v>
+      </c>
+    </row>
+    <row r="208" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A208" t="s">
+        <v>159</v>
+      </c>
+      <c r="B208" t="s">
         <v>102</v>
       </c>
     </row>
-    <row r="220" spans="2:2" x14ac:dyDescent="0.25">
-      <c r="B220" s="4"/>
+    <row r="209" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A209" t="s">
+        <v>495</v>
+      </c>
+      <c r="B209" t="s">
+        <v>82</v>
+      </c>
+      <c r="C209" t="s">
+        <v>234</v>
+      </c>
+    </row>
+    <row r="210" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A210" t="s">
+        <v>496</v>
+      </c>
+      <c r="B210" t="s">
+        <v>82</v>
+      </c>
+      <c r="C210" t="s">
+        <v>239</v>
+      </c>
+    </row>
+    <row r="211" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A211" t="s">
+        <v>497</v>
+      </c>
+      <c r="B211" t="s">
+        <v>82</v>
+      </c>
+      <c r="C211" t="s">
+        <v>244</v>
+      </c>
+    </row>
+    <row r="224" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="B224" s="4"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
@@ -6805,7 +6905,7 @@
   <dimension ref="A1:D27"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="B13" activeCellId="1" sqref="B26 B13"/>
+      <selection activeCell="A12" sqref="A12"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -7458,10 +7558,10 @@
   <sheetPr>
     <tabColor rgb="FFFFC000"/>
   </sheetPr>
-  <dimension ref="A1:B86"/>
+  <dimension ref="A1:B92"/>
   <sheetViews>
-    <sheetView topLeftCell="A51" workbookViewId="0">
-      <selection activeCell="A35" sqref="A35"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="H42" sqref="H42"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -8152,6 +8252,54 @@
       </c>
       <c r="B86" t="s">
         <v>452</v>
+      </c>
+    </row>
+    <row r="87" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A87" t="s">
+        <v>498</v>
+      </c>
+      <c r="B87" t="s">
+        <v>501</v>
+      </c>
+    </row>
+    <row r="88" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A88" t="s">
+        <v>499</v>
+      </c>
+      <c r="B88" t="s">
+        <v>460</v>
+      </c>
+    </row>
+    <row r="89" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A89" t="s">
+        <v>495</v>
+      </c>
+      <c r="B89" t="s">
+        <v>466</v>
+      </c>
+    </row>
+    <row r="90" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A90" t="s">
+        <v>496</v>
+      </c>
+      <c r="B90" t="s">
+        <v>454</v>
+      </c>
+    </row>
+    <row r="91" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A91" t="s">
+        <v>497</v>
+      </c>
+      <c r="B91" t="s">
+        <v>457</v>
+      </c>
+    </row>
+    <row r="92" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A92" t="s">
+        <v>500</v>
+      </c>
+      <c r="B92" t="s">
+        <v>457</v>
       </c>
     </row>
   </sheetData>
@@ -8224,12 +8372,12 @@
   <sheetPr>
     <tabColor theme="8"/>
   </sheetPr>
-  <dimension ref="A1:P62"/>
+  <dimension ref="A1:P66"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A2" zoomScale="80" zoomScaleNormal="80" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A3" activePane="bottomLeft" state="frozen"/>
+    <sheetView tabSelected="1" topLeftCell="B2" zoomScale="80" zoomScaleNormal="80" workbookViewId="0">
+      <pane ySplit="1" topLeftCell="A25" activePane="bottomLeft" state="frozen"/>
       <selection activeCell="E2" sqref="E2"/>
-      <selection pane="bottomLeft" activeCell="F16" sqref="F16:P16"/>
+      <selection pane="bottomLeft" activeCell="H68" sqref="H68"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -9725,7 +9873,7 @@
         <v>22</v>
       </c>
     </row>
-    <row r="49" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="49" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A49" t="s">
         <v>43</v>
       </c>
@@ -9760,7 +9908,7 @@
         <v>22</v>
       </c>
     </row>
-    <row r="50" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="50" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A50" t="s">
         <v>43</v>
       </c>
@@ -9798,7 +9946,7 @@
         <v>42</v>
       </c>
     </row>
-    <row r="51" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="51" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A51" t="s">
         <v>43</v>
       </c>
@@ -9836,7 +9984,7 @@
         <v>42</v>
       </c>
     </row>
-    <row r="52" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="52" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A52" t="s">
         <v>44</v>
       </c>
@@ -9868,7 +10016,7 @@
         <v>22</v>
       </c>
     </row>
-    <row r="53" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="53" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A53" t="s">
         <v>44</v>
       </c>
@@ -9900,7 +10048,7 @@
         <v>22</v>
       </c>
     </row>
-    <row r="54" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="54" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A54" t="s">
         <v>44</v>
       </c>
@@ -9920,7 +10068,7 @@
         <v>478</v>
       </c>
     </row>
-    <row r="55" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="55" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A55" t="s">
         <v>27</v>
       </c>
@@ -9952,7 +10100,7 @@
         <v>161</v>
       </c>
     </row>
-    <row r="56" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="56" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A56" t="s">
         <v>27</v>
       </c>
@@ -9984,7 +10132,7 @@
         <v>161</v>
       </c>
     </row>
-    <row r="57" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="57" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A57" t="s">
         <v>27</v>
       </c>
@@ -10016,7 +10164,7 @@
         <v>161</v>
       </c>
     </row>
-    <row r="58" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="58" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A58" t="s">
         <v>27</v>
       </c>
@@ -10048,7 +10196,7 @@
         <v>161</v>
       </c>
     </row>
-    <row r="59" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="59" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A59" t="s">
         <v>27</v>
       </c>
@@ -10080,7 +10228,7 @@
         <v>161</v>
       </c>
     </row>
-    <row r="60" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="60" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A60" t="s">
         <v>24</v>
       </c>
@@ -10115,7 +10263,7 @@
         <v>187</v>
       </c>
     </row>
-    <row r="61" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="61" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A61" t="s">
         <v>24</v>
       </c>
@@ -10150,7 +10298,7 @@
         <v>187</v>
       </c>
     </row>
-    <row r="62" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="62" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A62" t="s">
         <v>31</v>
       </c>
@@ -10177,6 +10325,146 @@
       </c>
       <c r="J62" t="s">
         <v>159</v>
+      </c>
+    </row>
+    <row r="63" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="A63" t="s">
+        <v>494</v>
+      </c>
+      <c r="B63">
+        <v>1</v>
+      </c>
+      <c r="C63" t="s">
+        <v>7</v>
+      </c>
+      <c r="D63" t="s">
+        <v>479</v>
+      </c>
+      <c r="F63" t="s">
+        <v>10</v>
+      </c>
+      <c r="G63" t="s">
+        <v>11</v>
+      </c>
+      <c r="H63" t="s">
+        <v>4</v>
+      </c>
+      <c r="I63" t="s">
+        <v>89</v>
+      </c>
+      <c r="J63" t="s">
+        <v>87</v>
+      </c>
+      <c r="K63" t="s">
+        <v>5</v>
+      </c>
+      <c r="L63" t="s">
+        <v>12</v>
+      </c>
+      <c r="M63" t="s">
+        <v>91</v>
+      </c>
+      <c r="N63" t="s">
+        <v>95</v>
+      </c>
+    </row>
+    <row r="64" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="A64" t="s">
+        <v>64</v>
+      </c>
+      <c r="B64">
+        <v>1</v>
+      </c>
+      <c r="C64" t="s">
+        <v>7</v>
+      </c>
+      <c r="D64" t="s">
+        <v>480</v>
+      </c>
+      <c r="F64" t="s">
+        <v>495</v>
+      </c>
+      <c r="G64" t="s">
+        <v>496</v>
+      </c>
+      <c r="H64" t="s">
+        <v>497</v>
+      </c>
+    </row>
+    <row r="65" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A65" t="s">
+        <v>64</v>
+      </c>
+      <c r="B65">
+        <v>2</v>
+      </c>
+      <c r="C65" t="s">
+        <v>7</v>
+      </c>
+      <c r="D65" t="s">
+        <v>477</v>
+      </c>
+      <c r="F65" t="s">
+        <v>127</v>
+      </c>
+      <c r="G65" t="s">
+        <v>132</v>
+      </c>
+      <c r="H65" t="s">
+        <v>498</v>
+      </c>
+      <c r="I65" t="s">
+        <v>499</v>
+      </c>
+      <c r="J65" t="s">
+        <v>125</v>
+      </c>
+      <c r="K65" t="s">
+        <v>141</v>
+      </c>
+      <c r="L65" t="s">
+        <v>129</v>
+      </c>
+      <c r="M65" t="s">
+        <v>500</v>
+      </c>
+    </row>
+    <row r="66" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A66" t="s">
+        <v>64</v>
+      </c>
+      <c r="B66">
+        <v>3</v>
+      </c>
+      <c r="C66" t="s">
+        <v>8</v>
+      </c>
+      <c r="D66" t="s">
+        <v>477</v>
+      </c>
+      <c r="F66" t="s">
+        <v>127</v>
+      </c>
+      <c r="G66" t="s">
+        <v>132</v>
+      </c>
+      <c r="H66" t="s">
+        <v>498</v>
+      </c>
+      <c r="I66" t="s">
+        <v>499</v>
+      </c>
+      <c r="J66" t="s">
+        <v>125</v>
+      </c>
+      <c r="K66" t="s">
+        <v>141</v>
+      </c>
+      <c r="L66" t="s">
+        <v>129</v>
+      </c>
+      <c r="M66" t="s">
+        <v>500</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
created oil by sector sheet
</commit_message>
<xml_diff>
--- a/config/master_config.xlsx
+++ b/config/master_config.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\finbar.maunsell\github\9th_edition_visualisation\config\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{95182253-812E-49D5-B3C3-D8E193DCAA78}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A2B1C39A-C273-422F-AC8B-511BA3F0DC85}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="28680" yWindow="-120" windowWidth="29040" windowHeight="15720" tabRatio="812" activeTab="6" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" tabRatio="812" activeTab="6" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="9th_EBT_schema" sheetId="7" r:id="rId1"/>
@@ -67,7 +67,6 @@
 <comments xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="xr">
   <authors>
     <author>Finbar Barton MAUNSELL</author>
-    <author>tc={781EF275-393F-4D4F-B2E9-CE751F408370}</author>
     <author>Finbar Maunsell</author>
   </authors>
   <commentList>
@@ -95,15 +94,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="A54" authorId="1" shapeId="0" xr:uid="{781EF275-393F-4D4F-B2E9-CE751F408370}">
-      <text>
-        <t>[Threaded comment]
-Your version of Excel allows you to read this threaded comment; however, any edits to it will get removed if the file is opened in a newer version of Excel. Learn more: https://go.microsoft.com/fwlink/?linkid=870924
-Comment:
-    Is lng equivalent to cng or do we need to add in a new fuel type? Should check balances</t>
-      </text>
-    </comment>
-    <comment ref="C62" authorId="2" shapeId="0" xr:uid="{89B88E45-46D2-4A21-AC6F-3EA3AEBCAB61}">
+    <comment ref="C70" authorId="1" shapeId="0" xr:uid="{89B88E45-46D2-4A21-AC6F-3EA3AEBCAB61}">
       <text>
         <r>
           <rPr>
@@ -224,7 +215,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1700" uniqueCount="499">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1757" uniqueCount="500">
   <si>
     <t>chart_type</t>
   </si>
@@ -1672,9 +1663,6 @@
     <t>aggregate</t>
   </si>
   <si>
-    <t>Gas?</t>
-  </si>
-  <si>
     <t>['2000', '2010', '2020', '2030', '2040', '2050', '2060', '2070']</t>
   </si>
   <si>
@@ -1720,7 +1708,13 @@
     <t>line_thickness</t>
   </si>
   <si>
-    <t>['FED by fuel', 'FED by sector',  'Production','Supply', 'Buildings', 'Industry', 'Transport', 'Agriculture','Fuel consumption power sector','Electricity', 'Refining',    'Renewable fuels','Non-energy','Hydrogen','Coal','TPES Coal by type', 'Crude &amp; NGL']</t>
+    <t>Other oil</t>
+  </si>
+  <si>
+    <t>Oil use by sector</t>
+  </si>
+  <si>
+    <t>['FED by fuel', 'FED by sector',  'Production','Supply', 'Buildings', 'Industry', 'Transport', 'Agriculture','Fuel consumption power sector','Electricity', 'Refining',    'Renewable fuels','Non-energy','Hydrogen','Coal','TPES Coal by type', 'Crude &amp; NGL', 'Oil use by sector']</t>
   </si>
 </sst>
 </file>
@@ -3131,20 +3125,12 @@
 </ThreadedComments>
 </file>
 
-<file path=xl/threadedComments/threadedComment2.xml><?xml version="1.0" encoding="utf-8"?>
-<ThreadedComments xmlns="http://schemas.microsoft.com/office/spreadsheetml/2018/threadedcomments" xmlns:x="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <threadedComment ref="A54" dT="2023-05-18T13:45:41.69" personId="{96FC88B6-068E-4187-B7BF-0009949FD93F}" id="{781EF275-393F-4D4F-B2E9-CE751F408370}">
-    <text>Is lng equivalent to cng or do we need to add in a new fuel type? Should check balances</text>
-  </threadedComment>
-</ThreadedComments>
-</file>
-
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{A000B41E-5923-4013-B542-E4247E89557C}">
   <dimension ref="A1:I102"/>
   <sheetViews>
-    <sheetView showGridLines="0" topLeftCell="A7" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <selection activeCell="D31" sqref="D31"/>
+    <sheetView showGridLines="0" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
+      <selection activeCell="D10" sqref="D10:D20"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -5015,10 +5001,10 @@
   <sheetPr>
     <tabColor theme="8"/>
   </sheetPr>
-  <dimension ref="A1:C224"/>
+  <dimension ref="A1:C232"/>
   <sheetViews>
-    <sheetView topLeftCell="A31" workbookViewId="0">
-      <selection activeCell="A61" sqref="A61"/>
+    <sheetView topLeftCell="A44" workbookViewId="0">
+      <selection activeCell="B76" sqref="B76"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -5384,7 +5370,7 @@
     </row>
     <row r="40" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A40" t="s">
-        <v>495</v>
+        <v>494</v>
       </c>
       <c r="B40" t="s">
         <v>92</v>
@@ -5524,7 +5510,7 @@
     </row>
     <row r="53" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A53" t="s">
-        <v>123</v>
+        <v>497</v>
       </c>
       <c r="B53" t="s">
         <v>77</v>
@@ -5534,129 +5520,129 @@
       </c>
     </row>
     <row r="54" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A54" s="4" t="s">
-        <v>482</v>
+      <c r="A54" t="s">
+        <v>497</v>
       </c>
       <c r="B54" t="s">
         <v>77</v>
       </c>
-      <c r="C54" s="4" t="s">
-        <v>125</v>
+      <c r="C54" t="s">
+        <v>127</v>
       </c>
     </row>
     <row r="55" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A55" t="s">
-        <v>126</v>
+        <v>497</v>
       </c>
       <c r="B55" t="s">
         <v>77</v>
       </c>
       <c r="C55" t="s">
-        <v>127</v>
+        <v>128</v>
       </c>
     </row>
     <row r="56" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A56" t="s">
-        <v>126</v>
+        <v>497</v>
       </c>
       <c r="B56" t="s">
         <v>77</v>
       </c>
       <c r="C56" t="s">
-        <v>128</v>
+        <v>129</v>
       </c>
     </row>
     <row r="57" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A57" t="s">
-        <v>489</v>
+        <v>497</v>
       </c>
       <c r="B57" t="s">
         <v>77</v>
       </c>
       <c r="C57" t="s">
-        <v>129</v>
+        <v>130</v>
       </c>
     </row>
     <row r="58" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A58" t="s">
-        <v>490</v>
+        <v>497</v>
       </c>
       <c r="B58" t="s">
         <v>77</v>
       </c>
       <c r="C58" t="s">
-        <v>130</v>
+        <v>131</v>
       </c>
     </row>
     <row r="59" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A59" t="s">
-        <v>135</v>
+        <v>497</v>
       </c>
       <c r="B59" t="s">
         <v>77</v>
       </c>
       <c r="C59" t="s">
-        <v>131</v>
+        <v>134</v>
       </c>
     </row>
     <row r="60" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A60" t="s">
-        <v>491</v>
+        <v>497</v>
       </c>
       <c r="B60" t="s">
         <v>77</v>
       </c>
       <c r="C60" t="s">
-        <v>134</v>
+        <v>132</v>
       </c>
     </row>
     <row r="61" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A61" s="5" t="s">
-        <v>33</v>
+      <c r="A61" t="s">
+        <v>497</v>
       </c>
       <c r="B61" t="s">
-        <v>92</v>
+        <v>77</v>
       </c>
       <c r="C61" t="s">
-        <v>117</v>
+        <v>133</v>
       </c>
     </row>
     <row r="62" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A62" s="11" t="s">
-        <v>28</v>
-      </c>
-      <c r="B62" s="11" t="s">
-        <v>92</v>
-      </c>
-      <c r="C62" s="11" t="s">
-        <v>118</v>
+      <c r="A62" t="s">
+        <v>123</v>
+      </c>
+      <c r="B62" t="s">
+        <v>77</v>
+      </c>
+      <c r="C62" t="s">
+        <v>124</v>
       </c>
     </row>
     <row r="63" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A63" t="s">
-        <v>37</v>
+        <v>126</v>
       </c>
       <c r="B63" t="s">
         <v>77</v>
       </c>
       <c r="C63" t="s">
-        <v>122</v>
+        <v>127</v>
       </c>
     </row>
     <row r="64" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A64" t="s">
-        <v>37</v>
+        <v>126</v>
       </c>
       <c r="B64" t="s">
         <v>77</v>
       </c>
       <c r="C64" t="s">
-        <v>127</v>
+        <v>128</v>
       </c>
     </row>
     <row r="65" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A65" t="s">
-        <v>37</v>
+        <v>488</v>
       </c>
       <c r="B65" t="s">
         <v>77</v>
@@ -5667,57 +5653,57 @@
     </row>
     <row r="66" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A66" t="s">
-        <v>37</v>
+        <v>489</v>
       </c>
       <c r="B66" t="s">
         <v>77</v>
       </c>
       <c r="C66" t="s">
-        <v>128</v>
+        <v>130</v>
       </c>
     </row>
     <row r="67" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A67" t="s">
-        <v>37</v>
+        <v>135</v>
       </c>
       <c r="B67" t="s">
         <v>77</v>
       </c>
       <c r="C67" t="s">
-        <v>130</v>
+        <v>131</v>
       </c>
     </row>
     <row r="68" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A68" t="s">
-        <v>37</v>
+        <v>490</v>
       </c>
       <c r="B68" t="s">
         <v>77</v>
       </c>
       <c r="C68" t="s">
-        <v>120</v>
+        <v>134</v>
       </c>
     </row>
     <row r="69" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A69" t="s">
-        <v>37</v>
+      <c r="A69" s="5" t="s">
+        <v>33</v>
       </c>
       <c r="B69" t="s">
-        <v>77</v>
+        <v>92</v>
       </c>
       <c r="C69" t="s">
-        <v>131</v>
+        <v>117</v>
       </c>
     </row>
     <row r="70" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A70" t="s">
-        <v>37</v>
-      </c>
-      <c r="B70" t="s">
-        <v>77</v>
-      </c>
-      <c r="C70" t="s">
-        <v>124</v>
+      <c r="A70" s="11" t="s">
+        <v>28</v>
+      </c>
+      <c r="B70" s="11" t="s">
+        <v>92</v>
+      </c>
+      <c r="C70" s="11" t="s">
+        <v>118</v>
       </c>
     </row>
     <row r="71" spans="1:3" x14ac:dyDescent="0.25">
@@ -5728,7 +5714,7 @@
         <v>77</v>
       </c>
       <c r="C71" t="s">
-        <v>132</v>
+        <v>122</v>
       </c>
     </row>
     <row r="72" spans="1:3" x14ac:dyDescent="0.25">
@@ -5739,7 +5725,7 @@
         <v>77</v>
       </c>
       <c r="C72" t="s">
-        <v>133</v>
+        <v>127</v>
       </c>
     </row>
     <row r="73" spans="1:3" x14ac:dyDescent="0.25">
@@ -5750,167 +5736,191 @@
         <v>77</v>
       </c>
       <c r="C73" t="s">
-        <v>134</v>
+        <v>129</v>
       </c>
     </row>
     <row r="74" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A74" t="s">
-        <v>135</v>
+        <v>37</v>
       </c>
       <c r="B74" t="s">
         <v>77</v>
       </c>
       <c r="C74" t="s">
-        <v>131</v>
+        <v>128</v>
       </c>
     </row>
     <row r="75" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A75" t="s">
-        <v>136</v>
+        <v>37</v>
       </c>
       <c r="B75" t="s">
-        <v>92</v>
+        <v>77</v>
       </c>
       <c r="C75" t="s">
-        <v>111</v>
+        <v>130</v>
       </c>
     </row>
     <row r="76" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A76" t="s">
-        <v>137</v>
+        <v>37</v>
       </c>
       <c r="B76" t="s">
-        <v>91</v>
+        <v>77</v>
+      </c>
+      <c r="C76" t="s">
+        <v>120</v>
       </c>
     </row>
     <row r="77" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A77" t="s">
-        <v>137</v>
+        <v>37</v>
       </c>
       <c r="B77" t="s">
-        <v>92</v>
+        <v>77</v>
       </c>
       <c r="C77" t="s">
-        <v>105</v>
+        <v>131</v>
       </c>
     </row>
     <row r="78" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A78" t="s">
-        <v>137</v>
+        <v>37</v>
       </c>
       <c r="B78" t="s">
-        <v>92</v>
+        <v>77</v>
       </c>
       <c r="C78" t="s">
-        <v>107</v>
+        <v>124</v>
       </c>
     </row>
     <row r="79" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A79" t="s">
-        <v>137</v>
+        <v>37</v>
       </c>
       <c r="B79" t="s">
-        <v>92</v>
+        <v>77</v>
       </c>
       <c r="C79" t="s">
-        <v>109</v>
+        <v>132</v>
       </c>
     </row>
     <row r="80" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A80" t="s">
-        <v>137</v>
+        <v>37</v>
       </c>
       <c r="B80" t="s">
-        <v>92</v>
+        <v>77</v>
       </c>
       <c r="C80" t="s">
-        <v>110</v>
+        <v>133</v>
       </c>
     </row>
     <row r="81" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A81" t="s">
-        <v>137</v>
+        <v>37</v>
       </c>
       <c r="B81" t="s">
-        <v>92</v>
+        <v>77</v>
       </c>
       <c r="C81" t="s">
-        <v>111</v>
+        <v>134</v>
       </c>
     </row>
     <row r="82" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A82" t="s">
-        <v>137</v>
+        <v>135</v>
       </c>
       <c r="B82" t="s">
-        <v>92</v>
+        <v>77</v>
       </c>
       <c r="C82" t="s">
-        <v>112</v>
+        <v>131</v>
       </c>
     </row>
     <row r="83" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A83" t="s">
-        <v>27</v>
+        <v>136</v>
       </c>
       <c r="B83" t="s">
-        <v>71</v>
+        <v>92</v>
+      </c>
+      <c r="C83" t="s">
+        <v>111</v>
       </c>
     </row>
     <row r="84" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A84" t="s">
-        <v>27</v>
+        <v>137</v>
       </c>
       <c r="B84" t="s">
-        <v>72</v>
+        <v>91</v>
       </c>
     </row>
     <row r="85" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A85" t="s">
-        <v>27</v>
+        <v>137</v>
       </c>
       <c r="B85" t="s">
-        <v>73</v>
+        <v>92</v>
+      </c>
+      <c r="C85" t="s">
+        <v>105</v>
       </c>
     </row>
     <row r="86" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A86" t="s">
-        <v>27</v>
+        <v>137</v>
       </c>
       <c r="B86" t="s">
-        <v>74</v>
+        <v>92</v>
+      </c>
+      <c r="C86" t="s">
+        <v>107</v>
       </c>
     </row>
     <row r="87" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A87" t="s">
-        <v>27</v>
+        <v>137</v>
       </c>
       <c r="B87" t="s">
-        <v>75</v>
+        <v>92</v>
+      </c>
+      <c r="C87" t="s">
+        <v>109</v>
       </c>
     </row>
     <row r="88" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A88" t="s">
-        <v>27</v>
+        <v>137</v>
       </c>
       <c r="B88" t="s">
-        <v>76</v>
+        <v>92</v>
+      </c>
+      <c r="C88" t="s">
+        <v>110</v>
       </c>
     </row>
     <row r="89" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A89" t="s">
-        <v>27</v>
+        <v>137</v>
       </c>
       <c r="B89" t="s">
-        <v>77</v>
+        <v>92</v>
+      </c>
+      <c r="C89" t="s">
+        <v>111</v>
       </c>
     </row>
     <row r="90" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A90" t="s">
-        <v>27</v>
+        <v>137</v>
       </c>
       <c r="B90" t="s">
-        <v>78</v>
+        <v>92</v>
+      </c>
+      <c r="C90" t="s">
+        <v>112</v>
       </c>
     </row>
     <row r="91" spans="1:3" x14ac:dyDescent="0.25">
@@ -5918,7 +5928,7 @@
         <v>27</v>
       </c>
       <c r="B91" t="s">
-        <v>80</v>
+        <v>71</v>
       </c>
     </row>
     <row r="92" spans="1:3" x14ac:dyDescent="0.25">
@@ -5926,7 +5936,7 @@
         <v>27</v>
       </c>
       <c r="B92" t="s">
-        <v>82</v>
+        <v>72</v>
       </c>
     </row>
     <row r="93" spans="1:3" x14ac:dyDescent="0.25">
@@ -5934,7 +5944,7 @@
         <v>27</v>
       </c>
       <c r="B93" t="s">
-        <v>84</v>
+        <v>73</v>
       </c>
     </row>
     <row r="94" spans="1:3" x14ac:dyDescent="0.25">
@@ -5942,7 +5952,7 @@
         <v>27</v>
       </c>
       <c r="B94" t="s">
-        <v>86</v>
+        <v>74</v>
       </c>
     </row>
     <row r="95" spans="1:3" x14ac:dyDescent="0.25">
@@ -5950,7 +5960,7 @@
         <v>27</v>
       </c>
       <c r="B95" t="s">
-        <v>88</v>
+        <v>75</v>
       </c>
     </row>
     <row r="96" spans="1:3" x14ac:dyDescent="0.25">
@@ -5958,7 +5968,7 @@
         <v>27</v>
       </c>
       <c r="B96" t="s">
-        <v>90</v>
+        <v>76</v>
       </c>
     </row>
     <row r="97" spans="1:2" x14ac:dyDescent="0.25">
@@ -5966,7 +5976,7 @@
         <v>27</v>
       </c>
       <c r="B97" t="s">
-        <v>91</v>
+        <v>77</v>
       </c>
     </row>
     <row r="98" spans="1:2" x14ac:dyDescent="0.25">
@@ -5974,7 +5984,7 @@
         <v>27</v>
       </c>
       <c r="B98" t="s">
-        <v>92</v>
+        <v>78</v>
       </c>
     </row>
     <row r="99" spans="1:2" x14ac:dyDescent="0.25">
@@ -5982,7 +5992,7 @@
         <v>27</v>
       </c>
       <c r="B99" t="s">
-        <v>94</v>
+        <v>80</v>
       </c>
     </row>
     <row r="100" spans="1:2" x14ac:dyDescent="0.25">
@@ -5990,71 +6000,71 @@
         <v>27</v>
       </c>
       <c r="B100" t="s">
-        <v>96</v>
+        <v>82</v>
       </c>
     </row>
     <row r="101" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A101" t="s">
-        <v>9</v>
+        <v>27</v>
       </c>
       <c r="B101" t="s">
-        <v>71</v>
+        <v>84</v>
       </c>
     </row>
     <row r="102" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A102" t="s">
-        <v>9</v>
+        <v>27</v>
       </c>
       <c r="B102" t="s">
-        <v>72</v>
+        <v>86</v>
       </c>
     </row>
     <row r="103" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A103" t="s">
-        <v>9</v>
+        <v>27</v>
       </c>
       <c r="B103" t="s">
-        <v>73</v>
+        <v>88</v>
       </c>
     </row>
     <row r="104" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A104" t="s">
-        <v>9</v>
+        <v>27</v>
       </c>
       <c r="B104" t="s">
-        <v>74</v>
+        <v>90</v>
       </c>
     </row>
     <row r="105" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A105" t="s">
-        <v>9</v>
+        <v>27</v>
       </c>
       <c r="B105" t="s">
-        <v>75</v>
+        <v>91</v>
       </c>
     </row>
     <row r="106" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A106" t="s">
-        <v>9</v>
+        <v>27</v>
       </c>
       <c r="B106" t="s">
-        <v>76</v>
+        <v>92</v>
       </c>
     </row>
     <row r="107" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A107" t="s">
-        <v>9</v>
+        <v>27</v>
       </c>
       <c r="B107" t="s">
-        <v>77</v>
+        <v>94</v>
       </c>
     </row>
     <row r="108" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A108" t="s">
-        <v>9</v>
+        <v>27</v>
       </c>
       <c r="B108" t="s">
-        <v>78</v>
+        <v>96</v>
       </c>
     </row>
     <row r="109" spans="1:2" x14ac:dyDescent="0.25">
@@ -6062,7 +6072,7 @@
         <v>9</v>
       </c>
       <c r="B109" t="s">
-        <v>80</v>
+        <v>71</v>
       </c>
     </row>
     <row r="110" spans="1:2" x14ac:dyDescent="0.25">
@@ -6070,7 +6080,7 @@
         <v>9</v>
       </c>
       <c r="B110" t="s">
-        <v>82</v>
+        <v>72</v>
       </c>
     </row>
     <row r="111" spans="1:2" x14ac:dyDescent="0.25">
@@ -6078,7 +6088,7 @@
         <v>9</v>
       </c>
       <c r="B111" t="s">
-        <v>84</v>
+        <v>73</v>
       </c>
     </row>
     <row r="112" spans="1:2" x14ac:dyDescent="0.25">
@@ -6086,7 +6096,7 @@
         <v>9</v>
       </c>
       <c r="B112" t="s">
-        <v>86</v>
+        <v>74</v>
       </c>
     </row>
     <row r="113" spans="1:2" x14ac:dyDescent="0.25">
@@ -6094,7 +6104,7 @@
         <v>9</v>
       </c>
       <c r="B113" t="s">
-        <v>88</v>
+        <v>75</v>
       </c>
     </row>
     <row r="114" spans="1:2" x14ac:dyDescent="0.25">
@@ -6102,7 +6112,7 @@
         <v>9</v>
       </c>
       <c r="B114" t="s">
-        <v>90</v>
+        <v>76</v>
       </c>
     </row>
     <row r="115" spans="1:2" x14ac:dyDescent="0.25">
@@ -6110,7 +6120,7 @@
         <v>9</v>
       </c>
       <c r="B115" t="s">
-        <v>91</v>
+        <v>77</v>
       </c>
     </row>
     <row r="116" spans="1:2" x14ac:dyDescent="0.25">
@@ -6118,7 +6128,7 @@
         <v>9</v>
       </c>
       <c r="B116" t="s">
-        <v>92</v>
+        <v>78</v>
       </c>
     </row>
     <row r="117" spans="1:2" x14ac:dyDescent="0.25">
@@ -6126,7 +6136,7 @@
         <v>9</v>
       </c>
       <c r="B117" t="s">
-        <v>94</v>
+        <v>80</v>
       </c>
     </row>
     <row r="118" spans="1:2" x14ac:dyDescent="0.25">
@@ -6134,71 +6144,71 @@
         <v>9</v>
       </c>
       <c r="B118" t="s">
-        <v>96</v>
+        <v>82</v>
       </c>
     </row>
     <row r="119" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A119" t="s">
-        <v>24</v>
+        <v>9</v>
       </c>
       <c r="B119" t="s">
-        <v>71</v>
+        <v>84</v>
       </c>
     </row>
     <row r="120" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A120" t="s">
-        <v>24</v>
+        <v>9</v>
       </c>
       <c r="B120" t="s">
-        <v>72</v>
+        <v>86</v>
       </c>
     </row>
     <row r="121" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A121" t="s">
-        <v>24</v>
+        <v>9</v>
       </c>
       <c r="B121" t="s">
-        <v>73</v>
+        <v>88</v>
       </c>
     </row>
     <row r="122" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A122" t="s">
-        <v>24</v>
+        <v>9</v>
       </c>
       <c r="B122" t="s">
-        <v>74</v>
+        <v>90</v>
       </c>
     </row>
     <row r="123" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A123" t="s">
-        <v>24</v>
+        <v>9</v>
       </c>
       <c r="B123" t="s">
-        <v>75</v>
+        <v>91</v>
       </c>
     </row>
     <row r="124" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A124" t="s">
-        <v>24</v>
+        <v>9</v>
       </c>
       <c r="B124" t="s">
-        <v>76</v>
+        <v>92</v>
       </c>
     </row>
     <row r="125" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A125" t="s">
-        <v>24</v>
+        <v>9</v>
       </c>
       <c r="B125" t="s">
-        <v>77</v>
+        <v>94</v>
       </c>
     </row>
     <row r="126" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A126" t="s">
-        <v>24</v>
+        <v>9</v>
       </c>
       <c r="B126" t="s">
-        <v>78</v>
+        <v>96</v>
       </c>
     </row>
     <row r="127" spans="1:2" x14ac:dyDescent="0.25">
@@ -6206,7 +6216,7 @@
         <v>24</v>
       </c>
       <c r="B127" t="s">
-        <v>80</v>
+        <v>71</v>
       </c>
     </row>
     <row r="128" spans="1:2" x14ac:dyDescent="0.25">
@@ -6214,7 +6224,7 @@
         <v>24</v>
       </c>
       <c r="B128" t="s">
-        <v>82</v>
+        <v>72</v>
       </c>
     </row>
     <row r="129" spans="1:2" x14ac:dyDescent="0.25">
@@ -6222,7 +6232,7 @@
         <v>24</v>
       </c>
       <c r="B129" t="s">
-        <v>84</v>
+        <v>73</v>
       </c>
     </row>
     <row r="130" spans="1:2" x14ac:dyDescent="0.25">
@@ -6230,7 +6240,7 @@
         <v>24</v>
       </c>
       <c r="B130" t="s">
-        <v>86</v>
+        <v>74</v>
       </c>
     </row>
     <row r="131" spans="1:2" x14ac:dyDescent="0.25">
@@ -6238,7 +6248,7 @@
         <v>24</v>
       </c>
       <c r="B131" t="s">
-        <v>88</v>
+        <v>75</v>
       </c>
     </row>
     <row r="132" spans="1:2" x14ac:dyDescent="0.25">
@@ -6246,7 +6256,7 @@
         <v>24</v>
       </c>
       <c r="B132" t="s">
-        <v>90</v>
+        <v>76</v>
       </c>
     </row>
     <row r="133" spans="1:2" x14ac:dyDescent="0.25">
@@ -6254,7 +6264,7 @@
         <v>24</v>
       </c>
       <c r="B133" t="s">
-        <v>91</v>
+        <v>77</v>
       </c>
     </row>
     <row r="134" spans="1:2" x14ac:dyDescent="0.25">
@@ -6262,7 +6272,7 @@
         <v>24</v>
       </c>
       <c r="B134" t="s">
-        <v>92</v>
+        <v>78</v>
       </c>
     </row>
     <row r="135" spans="1:2" x14ac:dyDescent="0.25">
@@ -6270,7 +6280,7 @@
         <v>24</v>
       </c>
       <c r="B135" t="s">
-        <v>94</v>
+        <v>80</v>
       </c>
     </row>
     <row r="136" spans="1:2" x14ac:dyDescent="0.25">
@@ -6278,71 +6288,71 @@
         <v>24</v>
       </c>
       <c r="B136" t="s">
-        <v>96</v>
+        <v>82</v>
       </c>
     </row>
     <row r="137" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A137" t="s">
-        <v>1</v>
+        <v>24</v>
       </c>
       <c r="B137" t="s">
-        <v>71</v>
+        <v>84</v>
       </c>
     </row>
     <row r="138" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A138" t="s">
-        <v>1</v>
+        <v>24</v>
       </c>
       <c r="B138" t="s">
-        <v>72</v>
+        <v>86</v>
       </c>
     </row>
     <row r="139" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A139" t="s">
-        <v>1</v>
+        <v>24</v>
       </c>
       <c r="B139" t="s">
-        <v>73</v>
+        <v>88</v>
       </c>
     </row>
     <row r="140" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A140" t="s">
-        <v>1</v>
+        <v>24</v>
       </c>
       <c r="B140" t="s">
-        <v>74</v>
+        <v>90</v>
       </c>
     </row>
     <row r="141" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A141" t="s">
-        <v>1</v>
+        <v>24</v>
       </c>
       <c r="B141" t="s">
-        <v>75</v>
+        <v>91</v>
       </c>
     </row>
     <row r="142" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A142" t="s">
-        <v>1</v>
+        <v>24</v>
       </c>
       <c r="B142" t="s">
-        <v>76</v>
+        <v>92</v>
       </c>
     </row>
     <row r="143" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A143" t="s">
-        <v>1</v>
+        <v>24</v>
       </c>
       <c r="B143" t="s">
-        <v>77</v>
+        <v>94</v>
       </c>
     </row>
     <row r="144" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A144" t="s">
-        <v>1</v>
+        <v>24</v>
       </c>
       <c r="B144" t="s">
-        <v>78</v>
+        <v>96</v>
       </c>
     </row>
     <row r="145" spans="1:2" x14ac:dyDescent="0.25">
@@ -6350,7 +6360,7 @@
         <v>1</v>
       </c>
       <c r="B145" t="s">
-        <v>80</v>
+        <v>71</v>
       </c>
     </row>
     <row r="146" spans="1:2" x14ac:dyDescent="0.25">
@@ -6358,7 +6368,7 @@
         <v>1</v>
       </c>
       <c r="B146" t="s">
-        <v>82</v>
+        <v>72</v>
       </c>
     </row>
     <row r="147" spans="1:2" x14ac:dyDescent="0.25">
@@ -6366,7 +6376,7 @@
         <v>1</v>
       </c>
       <c r="B147" t="s">
-        <v>84</v>
+        <v>73</v>
       </c>
     </row>
     <row r="148" spans="1:2" x14ac:dyDescent="0.25">
@@ -6374,7 +6384,7 @@
         <v>1</v>
       </c>
       <c r="B148" t="s">
-        <v>86</v>
+        <v>74</v>
       </c>
     </row>
     <row r="149" spans="1:2" x14ac:dyDescent="0.25">
@@ -6382,7 +6392,7 @@
         <v>1</v>
       </c>
       <c r="B149" t="s">
-        <v>88</v>
+        <v>75</v>
       </c>
     </row>
     <row r="150" spans="1:2" x14ac:dyDescent="0.25">
@@ -6390,7 +6400,7 @@
         <v>1</v>
       </c>
       <c r="B150" t="s">
-        <v>90</v>
+        <v>76</v>
       </c>
     </row>
     <row r="151" spans="1:2" x14ac:dyDescent="0.25">
@@ -6398,7 +6408,7 @@
         <v>1</v>
       </c>
       <c r="B151" t="s">
-        <v>91</v>
+        <v>77</v>
       </c>
     </row>
     <row r="152" spans="1:2" x14ac:dyDescent="0.25">
@@ -6406,7 +6416,7 @@
         <v>1</v>
       </c>
       <c r="B152" t="s">
-        <v>92</v>
+        <v>78</v>
       </c>
     </row>
     <row r="153" spans="1:2" x14ac:dyDescent="0.25">
@@ -6414,7 +6424,7 @@
         <v>1</v>
       </c>
       <c r="B153" t="s">
-        <v>94</v>
+        <v>80</v>
       </c>
     </row>
     <row r="154" spans="1:2" x14ac:dyDescent="0.25">
@@ -6422,71 +6432,71 @@
         <v>1</v>
       </c>
       <c r="B154" t="s">
-        <v>96</v>
+        <v>82</v>
       </c>
     </row>
     <row r="155" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A155" t="s">
-        <v>22</v>
+        <v>1</v>
       </c>
       <c r="B155" t="s">
-        <v>71</v>
+        <v>84</v>
       </c>
     </row>
     <row r="156" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A156" t="s">
-        <v>22</v>
+        <v>1</v>
       </c>
       <c r="B156" t="s">
-        <v>72</v>
+        <v>86</v>
       </c>
     </row>
     <row r="157" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A157" t="s">
-        <v>22</v>
+        <v>1</v>
       </c>
       <c r="B157" t="s">
-        <v>73</v>
+        <v>88</v>
       </c>
     </row>
     <row r="158" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A158" t="s">
-        <v>22</v>
+        <v>1</v>
       </c>
       <c r="B158" t="s">
-        <v>74</v>
+        <v>90</v>
       </c>
     </row>
     <row r="159" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A159" t="s">
-        <v>22</v>
+        <v>1</v>
       </c>
       <c r="B159" t="s">
-        <v>75</v>
+        <v>91</v>
       </c>
     </row>
     <row r="160" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A160" t="s">
-        <v>22</v>
+        <v>1</v>
       </c>
       <c r="B160" t="s">
-        <v>76</v>
+        <v>92</v>
       </c>
     </row>
     <row r="161" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A161" t="s">
-        <v>22</v>
+        <v>1</v>
       </c>
       <c r="B161" t="s">
-        <v>77</v>
+        <v>94</v>
       </c>
     </row>
     <row r="162" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A162" t="s">
-        <v>22</v>
+        <v>1</v>
       </c>
       <c r="B162" t="s">
-        <v>78</v>
+        <v>96</v>
       </c>
     </row>
     <row r="163" spans="1:2" x14ac:dyDescent="0.25">
@@ -6494,7 +6504,7 @@
         <v>22</v>
       </c>
       <c r="B163" t="s">
-        <v>80</v>
+        <v>71</v>
       </c>
     </row>
     <row r="164" spans="1:2" x14ac:dyDescent="0.25">
@@ -6502,7 +6512,7 @@
         <v>22</v>
       </c>
       <c r="B164" t="s">
-        <v>82</v>
+        <v>72</v>
       </c>
     </row>
     <row r="165" spans="1:2" x14ac:dyDescent="0.25">
@@ -6510,7 +6520,7 @@
         <v>22</v>
       </c>
       <c r="B165" t="s">
-        <v>84</v>
+        <v>73</v>
       </c>
     </row>
     <row r="166" spans="1:2" x14ac:dyDescent="0.25">
@@ -6518,7 +6528,7 @@
         <v>22</v>
       </c>
       <c r="B166" t="s">
-        <v>86</v>
+        <v>74</v>
       </c>
     </row>
     <row r="167" spans="1:2" x14ac:dyDescent="0.25">
@@ -6526,7 +6536,7 @@
         <v>22</v>
       </c>
       <c r="B167" t="s">
-        <v>88</v>
+        <v>75</v>
       </c>
     </row>
     <row r="168" spans="1:2" x14ac:dyDescent="0.25">
@@ -6534,7 +6544,7 @@
         <v>22</v>
       </c>
       <c r="B168" t="s">
-        <v>90</v>
+        <v>76</v>
       </c>
     </row>
     <row r="169" spans="1:2" x14ac:dyDescent="0.25">
@@ -6542,7 +6552,7 @@
         <v>22</v>
       </c>
       <c r="B169" t="s">
-        <v>91</v>
+        <v>77</v>
       </c>
     </row>
     <row r="170" spans="1:2" x14ac:dyDescent="0.25">
@@ -6550,7 +6560,7 @@
         <v>22</v>
       </c>
       <c r="B170" t="s">
-        <v>92</v>
+        <v>78</v>
       </c>
     </row>
     <row r="171" spans="1:2" x14ac:dyDescent="0.25">
@@ -6558,7 +6568,7 @@
         <v>22</v>
       </c>
       <c r="B171" t="s">
-        <v>94</v>
+        <v>80</v>
       </c>
     </row>
     <row r="172" spans="1:2" x14ac:dyDescent="0.25">
@@ -6566,71 +6576,71 @@
         <v>22</v>
       </c>
       <c r="B172" t="s">
-        <v>96</v>
+        <v>82</v>
       </c>
     </row>
     <row r="173" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A173" t="s">
-        <v>155</v>
+        <v>22</v>
       </c>
       <c r="B173" t="s">
-        <v>71</v>
+        <v>84</v>
       </c>
     </row>
     <row r="174" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A174" t="s">
-        <v>155</v>
+        <v>22</v>
       </c>
       <c r="B174" t="s">
-        <v>72</v>
+        <v>86</v>
       </c>
     </row>
     <row r="175" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A175" t="s">
-        <v>155</v>
+        <v>22</v>
       </c>
       <c r="B175" t="s">
-        <v>73</v>
+        <v>88</v>
       </c>
     </row>
     <row r="176" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A176" t="s">
-        <v>155</v>
+        <v>22</v>
       </c>
       <c r="B176" t="s">
-        <v>74</v>
+        <v>90</v>
       </c>
     </row>
     <row r="177" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A177" t="s">
-        <v>155</v>
+        <v>22</v>
       </c>
       <c r="B177" t="s">
-        <v>75</v>
+        <v>91</v>
       </c>
     </row>
     <row r="178" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A178" t="s">
-        <v>155</v>
+        <v>22</v>
       </c>
       <c r="B178" t="s">
-        <v>76</v>
+        <v>92</v>
       </c>
     </row>
     <row r="179" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A179" t="s">
-        <v>155</v>
+        <v>22</v>
       </c>
       <c r="B179" t="s">
-        <v>77</v>
+        <v>94</v>
       </c>
     </row>
     <row r="180" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A180" t="s">
-        <v>155</v>
+        <v>22</v>
       </c>
       <c r="B180" t="s">
-        <v>78</v>
+        <v>96</v>
       </c>
     </row>
     <row r="181" spans="1:2" x14ac:dyDescent="0.25">
@@ -6638,7 +6648,7 @@
         <v>155</v>
       </c>
       <c r="B181" t="s">
-        <v>80</v>
+        <v>71</v>
       </c>
     </row>
     <row r="182" spans="1:2" x14ac:dyDescent="0.25">
@@ -6646,7 +6656,7 @@
         <v>155</v>
       </c>
       <c r="B182" t="s">
-        <v>82</v>
+        <v>72</v>
       </c>
     </row>
     <row r="183" spans="1:2" x14ac:dyDescent="0.25">
@@ -6654,7 +6664,7 @@
         <v>155</v>
       </c>
       <c r="B183" t="s">
-        <v>84</v>
+        <v>73</v>
       </c>
     </row>
     <row r="184" spans="1:2" x14ac:dyDescent="0.25">
@@ -6662,7 +6672,7 @@
         <v>155</v>
       </c>
       <c r="B184" t="s">
-        <v>86</v>
+        <v>74</v>
       </c>
     </row>
     <row r="185" spans="1:2" x14ac:dyDescent="0.25">
@@ -6670,7 +6680,7 @@
         <v>155</v>
       </c>
       <c r="B185" t="s">
-        <v>88</v>
+        <v>75</v>
       </c>
     </row>
     <row r="186" spans="1:2" x14ac:dyDescent="0.25">
@@ -6678,7 +6688,7 @@
         <v>155</v>
       </c>
       <c r="B186" t="s">
-        <v>90</v>
+        <v>76</v>
       </c>
     </row>
     <row r="187" spans="1:2" x14ac:dyDescent="0.25">
@@ -6686,7 +6696,7 @@
         <v>155</v>
       </c>
       <c r="B187" t="s">
-        <v>91</v>
+        <v>77</v>
       </c>
     </row>
     <row r="188" spans="1:2" x14ac:dyDescent="0.25">
@@ -6694,7 +6704,7 @@
         <v>155</v>
       </c>
       <c r="B188" t="s">
-        <v>92</v>
+        <v>78</v>
       </c>
     </row>
     <row r="189" spans="1:2" x14ac:dyDescent="0.25">
@@ -6702,7 +6712,7 @@
         <v>155</v>
       </c>
       <c r="B189" t="s">
-        <v>94</v>
+        <v>80</v>
       </c>
     </row>
     <row r="190" spans="1:2" x14ac:dyDescent="0.25">
@@ -6710,71 +6720,71 @@
         <v>155</v>
       </c>
       <c r="B190" t="s">
-        <v>96</v>
+        <v>82</v>
       </c>
     </row>
     <row r="191" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A191" t="s">
-        <v>153</v>
+        <v>155</v>
       </c>
       <c r="B191" t="s">
-        <v>71</v>
+        <v>84</v>
       </c>
     </row>
     <row r="192" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A192" t="s">
-        <v>153</v>
+        <v>155</v>
       </c>
       <c r="B192" t="s">
-        <v>72</v>
+        <v>86</v>
       </c>
     </row>
     <row r="193" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A193" t="s">
-        <v>153</v>
+        <v>155</v>
       </c>
       <c r="B193" t="s">
-        <v>73</v>
+        <v>88</v>
       </c>
     </row>
     <row r="194" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A194" t="s">
-        <v>153</v>
+        <v>155</v>
       </c>
       <c r="B194" t="s">
-        <v>74</v>
+        <v>90</v>
       </c>
     </row>
     <row r="195" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A195" t="s">
-        <v>153</v>
+        <v>155</v>
       </c>
       <c r="B195" t="s">
-        <v>75</v>
+        <v>91</v>
       </c>
     </row>
     <row r="196" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A196" t="s">
-        <v>153</v>
+        <v>155</v>
       </c>
       <c r="B196" t="s">
-        <v>76</v>
+        <v>92</v>
       </c>
     </row>
     <row r="197" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A197" t="s">
-        <v>153</v>
+        <v>155</v>
       </c>
       <c r="B197" t="s">
-        <v>77</v>
+        <v>94</v>
       </c>
     </row>
     <row r="198" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A198" t="s">
-        <v>153</v>
+        <v>155</v>
       </c>
       <c r="B198" t="s">
-        <v>78</v>
+        <v>96</v>
       </c>
     </row>
     <row r="199" spans="1:2" x14ac:dyDescent="0.25">
@@ -6782,7 +6792,7 @@
         <v>153</v>
       </c>
       <c r="B199" t="s">
-        <v>80</v>
+        <v>71</v>
       </c>
     </row>
     <row r="200" spans="1:2" x14ac:dyDescent="0.25">
@@ -6790,7 +6800,7 @@
         <v>153</v>
       </c>
       <c r="B200" t="s">
-        <v>82</v>
+        <v>72</v>
       </c>
     </row>
     <row r="201" spans="1:2" x14ac:dyDescent="0.25">
@@ -6798,7 +6808,7 @@
         <v>153</v>
       </c>
       <c r="B201" t="s">
-        <v>84</v>
+        <v>73</v>
       </c>
     </row>
     <row r="202" spans="1:2" x14ac:dyDescent="0.25">
@@ -6806,7 +6816,7 @@
         <v>153</v>
       </c>
       <c r="B202" t="s">
-        <v>86</v>
+        <v>74</v>
       </c>
     </row>
     <row r="203" spans="1:2" x14ac:dyDescent="0.25">
@@ -6814,7 +6824,7 @@
         <v>153</v>
       </c>
       <c r="B203" t="s">
-        <v>88</v>
+        <v>75</v>
       </c>
     </row>
     <row r="204" spans="1:2" x14ac:dyDescent="0.25">
@@ -6822,7 +6832,7 @@
         <v>153</v>
       </c>
       <c r="B204" t="s">
-        <v>90</v>
+        <v>76</v>
       </c>
     </row>
     <row r="205" spans="1:2" x14ac:dyDescent="0.25">
@@ -6830,7 +6840,7 @@
         <v>153</v>
       </c>
       <c r="B205" t="s">
-        <v>91</v>
+        <v>77</v>
       </c>
     </row>
     <row r="206" spans="1:2" x14ac:dyDescent="0.25">
@@ -6838,7 +6848,7 @@
         <v>153</v>
       </c>
       <c r="B206" t="s">
-        <v>92</v>
+        <v>78</v>
       </c>
     </row>
     <row r="207" spans="1:2" x14ac:dyDescent="0.25">
@@ -6846,7 +6856,7 @@
         <v>153</v>
       </c>
       <c r="B207" t="s">
-        <v>94</v>
+        <v>80</v>
       </c>
     </row>
     <row r="208" spans="1:2" x14ac:dyDescent="0.25">
@@ -6854,44 +6864,108 @@
         <v>153</v>
       </c>
       <c r="B208" t="s">
-        <v>96</v>
+        <v>82</v>
       </c>
     </row>
     <row r="209" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A209" t="s">
-        <v>486</v>
+        <v>153</v>
       </c>
       <c r="B209" t="s">
-        <v>76</v>
-      </c>
-      <c r="C209" t="s">
-        <v>228</v>
+        <v>84</v>
       </c>
     </row>
     <row r="210" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A210" t="s">
-        <v>487</v>
+        <v>153</v>
       </c>
       <c r="B210" t="s">
-        <v>76</v>
-      </c>
-      <c r="C210" t="s">
-        <v>233</v>
+        <v>86</v>
       </c>
     </row>
     <row r="211" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A211" t="s">
-        <v>488</v>
+        <v>153</v>
       </c>
       <c r="B211" t="s">
+        <v>88</v>
+      </c>
+    </row>
+    <row r="212" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A212" t="s">
+        <v>153</v>
+      </c>
+      <c r="B212" t="s">
+        <v>90</v>
+      </c>
+    </row>
+    <row r="213" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A213" t="s">
+        <v>153</v>
+      </c>
+      <c r="B213" t="s">
+        <v>91</v>
+      </c>
+    </row>
+    <row r="214" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A214" t="s">
+        <v>153</v>
+      </c>
+      <c r="B214" t="s">
+        <v>92</v>
+      </c>
+    </row>
+    <row r="215" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A215" t="s">
+        <v>153</v>
+      </c>
+      <c r="B215" t="s">
+        <v>94</v>
+      </c>
+    </row>
+    <row r="216" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A216" t="s">
+        <v>153</v>
+      </c>
+      <c r="B216" t="s">
+        <v>96</v>
+      </c>
+    </row>
+    <row r="217" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A217" t="s">
+        <v>485</v>
+      </c>
+      <c r="B217" t="s">
         <v>76</v>
       </c>
-      <c r="C211" t="s">
+      <c r="C217" t="s">
+        <v>228</v>
+      </c>
+    </row>
+    <row r="218" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A218" t="s">
+        <v>486</v>
+      </c>
+      <c r="B218" t="s">
+        <v>76</v>
+      </c>
+      <c r="C218" t="s">
+        <v>233</v>
+      </c>
+    </row>
+    <row r="219" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A219" t="s">
+        <v>487</v>
+      </c>
+      <c r="B219" t="s">
+        <v>76</v>
+      </c>
+      <c r="C219" t="s">
         <v>238</v>
       </c>
     </row>
-    <row r="224" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="B224" s="4"/>
+    <row r="232" spans="2:2" x14ac:dyDescent="0.25">
+      <c r="B232" s="4"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
@@ -7628,7 +7702,7 @@
     </row>
     <row r="8" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A8" t="s">
-        <v>487</v>
+        <v>486</v>
       </c>
       <c r="B8" t="s">
         <v>448</v>
@@ -8020,7 +8094,7 @@
     </row>
     <row r="57" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A57" t="s">
-        <v>486</v>
+        <v>485</v>
       </c>
       <c r="B57" t="s">
         <v>460</v>
@@ -8100,10 +8174,10 @@
     </row>
     <row r="67" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A67" t="s">
-        <v>489</v>
+        <v>488</v>
       </c>
       <c r="B67" t="s">
-        <v>492</v>
+        <v>491</v>
       </c>
     </row>
     <row r="68" spans="1:2" x14ac:dyDescent="0.25">
@@ -8204,7 +8278,7 @@
     </row>
     <row r="80" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A80" t="s">
-        <v>490</v>
+        <v>489</v>
       </c>
       <c r="B80" t="s">
         <v>454</v>
@@ -8239,7 +8313,7 @@
         <v>28</v>
       </c>
       <c r="B84" t="s">
-        <v>494</v>
+        <v>493</v>
       </c>
     </row>
     <row r="85" spans="1:2" x14ac:dyDescent="0.25">
@@ -8279,7 +8353,7 @@
         <v>475</v>
       </c>
       <c r="B89" t="s">
-        <v>494</v>
+        <v>493</v>
       </c>
     </row>
     <row r="90" spans="1:2" x14ac:dyDescent="0.25">
@@ -8287,12 +8361,12 @@
         <v>472</v>
       </c>
       <c r="B90" t="s">
-        <v>494</v>
+        <v>493</v>
       </c>
     </row>
     <row r="91" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A91" t="s">
-        <v>488</v>
+        <v>487</v>
       </c>
       <c r="B91" t="s">
         <v>451</v>
@@ -8300,7 +8374,7 @@
     </row>
     <row r="92" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A92" t="s">
-        <v>491</v>
+        <v>490</v>
       </c>
       <c r="B92" t="s">
         <v>451</v>
@@ -8308,7 +8382,7 @@
     </row>
     <row r="93" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A93" t="s">
-        <v>495</v>
+        <v>494</v>
       </c>
       <c r="B93" t="s">
         <v>449</v>
@@ -8330,7 +8404,7 @@
   <dimension ref="A1:B7"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B6" sqref="B6"/>
+      <selection activeCell="N12" sqref="N12"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -8359,7 +8433,7 @@
         <v>45</v>
       </c>
       <c r="B3" t="s">
-        <v>483</v>
+        <v>482</v>
       </c>
     </row>
     <row r="4" spans="1:2" x14ac:dyDescent="0.25">
@@ -8380,15 +8454,15 @@
     </row>
     <row r="6" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
-        <v>493</v>
+        <v>492</v>
       </c>
       <c r="B6" t="s">
-        <v>498</v>
+        <v>499</v>
       </c>
     </row>
     <row r="7" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
-        <v>497</v>
+        <v>496</v>
       </c>
       <c r="B7">
         <v>3</v>
@@ -8405,12 +8479,12 @@
   <sheetPr>
     <tabColor theme="8"/>
   </sheetPr>
-  <dimension ref="A1:P44"/>
+  <dimension ref="A1:P47"/>
   <sheetViews>
     <sheetView topLeftCell="A2" zoomScale="80" zoomScaleNormal="80" workbookViewId="0">
       <pane ySplit="1" topLeftCell="A3" activePane="bottomLeft" state="frozen"/>
       <selection activeCell="E2" sqref="E2"/>
-      <selection pane="bottomLeft" activeCell="C30" sqref="C30"/>
+      <selection pane="bottomLeft" activeCell="G38" sqref="G37:G38"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -8927,7 +9001,7 @@
     </row>
     <row r="16" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A16" t="s">
-        <v>485</v>
+        <v>484</v>
       </c>
       <c r="B16">
         <v>1</v>
@@ -8957,7 +9031,7 @@
         <v>5</v>
       </c>
       <c r="L16" t="s">
-        <v>495</v>
+        <v>494</v>
       </c>
       <c r="M16" t="s">
         <v>85</v>
@@ -9285,13 +9359,13 @@
         <v>474</v>
       </c>
       <c r="F27" t="s">
+        <v>485</v>
+      </c>
+      <c r="G27" t="s">
         <v>486</v>
       </c>
-      <c r="G27" t="s">
+      <c r="H27" t="s">
         <v>487</v>
-      </c>
-      <c r="H27" t="s">
-        <v>488</v>
       </c>
     </row>
     <row r="28" spans="1:14" ht="23.25" customHeight="1" x14ac:dyDescent="0.25">
@@ -9314,10 +9388,10 @@
         <v>126</v>
       </c>
       <c r="H28" t="s">
+        <v>488</v>
+      </c>
+      <c r="I28" t="s">
         <v>489</v>
-      </c>
-      <c r="I28" t="s">
-        <v>490</v>
       </c>
       <c r="J28" t="s">
         <v>119</v>
@@ -9329,7 +9403,7 @@
         <v>123</v>
       </c>
       <c r="M28" t="s">
-        <v>491</v>
+        <v>490</v>
       </c>
     </row>
     <row r="29" spans="1:14" ht="21" customHeight="1" x14ac:dyDescent="0.25">
@@ -9352,10 +9426,10 @@
         <v>126</v>
       </c>
       <c r="H29" t="s">
+        <v>488</v>
+      </c>
+      <c r="I29" t="s">
         <v>489</v>
-      </c>
-      <c r="I29" t="s">
-        <v>490</v>
       </c>
       <c r="J29" t="s">
         <v>119</v>
@@ -9367,7 +9441,7 @@
         <v>123</v>
       </c>
       <c r="M29" t="s">
-        <v>491</v>
+        <v>490</v>
       </c>
     </row>
     <row r="30" spans="1:14" x14ac:dyDescent="0.25">
@@ -9514,7 +9588,7 @@
     </row>
     <row r="35" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A35" t="s">
-        <v>496</v>
+        <v>495</v>
       </c>
       <c r="B35">
         <v>1</v>
@@ -9561,7 +9635,7 @@
     </row>
     <row r="36" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A36" t="s">
-        <v>496</v>
+        <v>495</v>
       </c>
       <c r="B36">
         <v>2</v>
@@ -9608,7 +9682,7 @@
     </row>
     <row r="37" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A37" t="s">
-        <v>484</v>
+        <v>483</v>
       </c>
       <c r="B37">
         <v>1</v>
@@ -9631,7 +9705,7 @@
     </row>
     <row r="38" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A38" t="s">
-        <v>484</v>
+        <v>483</v>
       </c>
       <c r="B38">
         <v>2</v>
@@ -9651,7 +9725,7 @@
     </row>
     <row r="39" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A39" t="s">
-        <v>484</v>
+        <v>483</v>
       </c>
       <c r="B39">
         <v>3</v>
@@ -9826,6 +9900,120 @@
         <v>40</v>
       </c>
       <c r="K44" s="12" t="s">
+        <v>155</v>
+      </c>
+    </row>
+    <row r="45" spans="1:16" x14ac:dyDescent="0.25">
+      <c r="A45" t="s">
+        <v>498</v>
+      </c>
+      <c r="B45">
+        <v>1</v>
+      </c>
+      <c r="C45" t="s">
+        <v>2</v>
+      </c>
+      <c r="E45" t="s">
+        <v>119</v>
+      </c>
+      <c r="F45" t="s">
+        <v>3</v>
+      </c>
+      <c r="G45" t="s">
+        <v>1</v>
+      </c>
+      <c r="H45" t="s">
+        <v>9</v>
+      </c>
+      <c r="I45" t="s">
+        <v>24</v>
+      </c>
+      <c r="J45" t="s">
+        <v>25</v>
+      </c>
+      <c r="K45" t="s">
+        <v>26</v>
+      </c>
+      <c r="L45" t="s">
+        <v>27</v>
+      </c>
+      <c r="M45" t="s">
+        <v>155</v>
+      </c>
+    </row>
+    <row r="46" spans="1:16" x14ac:dyDescent="0.25">
+      <c r="A46" t="s">
+        <v>498</v>
+      </c>
+      <c r="B46">
+        <v>2</v>
+      </c>
+      <c r="C46" t="s">
+        <v>2</v>
+      </c>
+      <c r="E46" t="s">
+        <v>121</v>
+      </c>
+      <c r="F46" t="s">
+        <v>3</v>
+      </c>
+      <c r="G46" t="s">
+        <v>1</v>
+      </c>
+      <c r="H46" t="s">
+        <v>9</v>
+      </c>
+      <c r="I46" t="s">
+        <v>24</v>
+      </c>
+      <c r="J46" t="s">
+        <v>25</v>
+      </c>
+      <c r="K46" t="s">
+        <v>26</v>
+      </c>
+      <c r="L46" t="s">
+        <v>27</v>
+      </c>
+      <c r="M46" t="s">
+        <v>155</v>
+      </c>
+    </row>
+    <row r="47" spans="1:16" x14ac:dyDescent="0.25">
+      <c r="A47" t="s">
+        <v>498</v>
+      </c>
+      <c r="B47">
+        <v>3</v>
+      </c>
+      <c r="C47" t="s">
+        <v>2</v>
+      </c>
+      <c r="E47" t="s">
+        <v>497</v>
+      </c>
+      <c r="F47" t="s">
+        <v>3</v>
+      </c>
+      <c r="G47" t="s">
+        <v>1</v>
+      </c>
+      <c r="H47" t="s">
+        <v>9</v>
+      </c>
+      <c r="I47" t="s">
+        <v>24</v>
+      </c>
+      <c r="J47" t="s">
+        <v>25</v>
+      </c>
+      <c r="K47" t="s">
+        <v>26</v>
+      </c>
+      <c r="L47" t="s">
+        <v>27</v>
+      </c>
+      <c r="M47" t="s">
         <v>155</v>
       </c>
     </row>

</xml_diff>

<commit_message>
omit emissions, capacity and renewables for now
</commit_message>
<xml_diff>
--- a/config/master_config.xlsx
+++ b/config/master_config.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\hyuga.kasai\Documents\Github\9th_Visualization\9th_edition_visualisation\config\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{5C5AD227-A7D8-43F0-80C4-5BD6D7E5AEA0}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{35D34DB7-8B3B-4E95-B385-2B895062319B}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-6750" yWindow="-16320" windowWidth="29040" windowHeight="15840" tabRatio="812" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="22050" yWindow="-16395" windowWidth="29040" windowHeight="15840" tabRatio="812" firstSheet="1" activeTab="8" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="9th_EBT_schema" sheetId="7" r:id="rId1"/>
@@ -390,7 +390,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="4412" uniqueCount="557">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="4397" uniqueCount="550">
   <si>
     <t>chart_type</t>
   </si>
@@ -1991,21 +1991,6 @@
     <t>chart_title</t>
   </si>
   <si>
-    <t>intensity</t>
-  </si>
-  <si>
-    <t>energy_intensity</t>
-  </si>
-  <si>
-    <t>emissions_intensity</t>
-  </si>
-  <si>
-    <t>energy_intensity - {ECONOMY_ID} {SCENARIO} {UNIT}</t>
-  </si>
-  <si>
-    <t>emissions_intensity - {ECONOMY_ID} {SCENARIO} {UNIT}</t>
-  </si>
-  <si>
     <t>GDP_per_capita - {ECONOMY_ID} {UNIT}</t>
   </si>
   <si>
@@ -2013,12 +1998,6 @@
   </si>
   <si>
     <t>real_GDP - {ECONOMY_ID} {UNIT}</t>
-  </si>
-  <si>
-    <t>renewable_share</t>
-  </si>
-  <si>
-    <t>renewable_share - {ECONOMY_ID} {SCENARIO} {UNIT}</t>
   </si>
   <si>
     <t>10_01_13_pump_storage_plants</t>
@@ -3992,7 +3971,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{A000B41E-5923-4013-B542-E4247E89557C}">
   <dimension ref="A1:I102"/>
   <sheetViews>
-    <sheetView showGridLines="0" tabSelected="1" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
+    <sheetView showGridLines="0" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
       <selection activeCell="K8" sqref="K8"/>
     </sheetView>
   </sheetViews>
@@ -4505,7 +4484,7 @@
         <v>166</v>
       </c>
       <c r="F21" t="s">
-        <v>556</v>
+        <v>549</v>
       </c>
       <c r="G21" t="s">
         <v>291</v>
@@ -4890,7 +4869,7 @@
         <v>376</v>
       </c>
       <c r="G41" t="s">
-        <v>543</v>
+        <v>536</v>
       </c>
       <c r="H41" t="s">
         <v>377</v>
@@ -4907,7 +4886,7 @@
         <v>379</v>
       </c>
       <c r="G42" t="s">
-        <v>544</v>
+        <v>537</v>
       </c>
       <c r="H42" t="s">
         <v>380</v>
@@ -4918,7 +4897,7 @@
     </row>
     <row r="43" spans="4:9" x14ac:dyDescent="0.25">
       <c r="G43" t="s">
-        <v>545</v>
+        <v>538</v>
       </c>
       <c r="H43" t="s">
         <v>382</v>
@@ -4929,7 +4908,7 @@
     </row>
     <row r="44" spans="4:9" x14ac:dyDescent="0.25">
       <c r="G44" t="s">
-        <v>546</v>
+        <v>539</v>
       </c>
       <c r="H44" t="s">
         <v>384</v>
@@ -4940,7 +4919,7 @@
     </row>
     <row r="45" spans="4:9" x14ac:dyDescent="0.25">
       <c r="G45" t="s">
-        <v>547</v>
+        <v>540</v>
       </c>
       <c r="H45" t="s">
         <v>386</v>
@@ -4951,7 +4930,7 @@
     </row>
     <row r="46" spans="4:9" x14ac:dyDescent="0.25">
       <c r="G46" t="s">
-        <v>548</v>
+        <v>541</v>
       </c>
       <c r="H46" t="s">
         <v>388</v>
@@ -4962,7 +4941,7 @@
     </row>
     <row r="47" spans="4:9" x14ac:dyDescent="0.25">
       <c r="G47" t="s">
-        <v>549</v>
+        <v>542</v>
       </c>
       <c r="H47" t="s">
         <v>390</v>
@@ -4973,7 +4952,7 @@
     </row>
     <row r="48" spans="4:9" x14ac:dyDescent="0.25">
       <c r="G48" t="s">
-        <v>550</v>
+        <v>543</v>
       </c>
       <c r="H48" t="s">
         <v>392</v>
@@ -4984,7 +4963,7 @@
     </row>
     <row r="49" spans="7:9" x14ac:dyDescent="0.25">
       <c r="G49" t="s">
-        <v>551</v>
+        <v>544</v>
       </c>
       <c r="H49" t="s">
         <v>394</v>
@@ -4995,7 +4974,7 @@
     </row>
     <row r="50" spans="7:9" x14ac:dyDescent="0.25">
       <c r="G50" t="s">
-        <v>552</v>
+        <v>545</v>
       </c>
       <c r="H50" t="s">
         <v>396</v>
@@ -5006,7 +4985,7 @@
     </row>
     <row r="51" spans="7:9" x14ac:dyDescent="0.25">
       <c r="G51" t="s">
-        <v>553</v>
+        <v>546</v>
       </c>
       <c r="H51" t="s">
         <v>379</v>
@@ -5017,7 +4996,7 @@
     </row>
     <row r="52" spans="7:9" x14ac:dyDescent="0.25">
       <c r="G52" t="s">
-        <v>554</v>
+        <v>547</v>
       </c>
       <c r="I52" t="s">
         <v>379</v>
@@ -5030,7 +5009,7 @@
     </row>
     <row r="54" spans="7:9" x14ac:dyDescent="0.25">
       <c r="G54" t="s">
-        <v>555</v>
+        <v>548</v>
       </c>
     </row>
     <row r="55" spans="7:9" x14ac:dyDescent="0.25">
@@ -17808,9 +17787,9 @@
   <dimension ref="A1:W50"/>
   <sheetViews>
     <sheetView topLeftCell="D2" zoomScale="80" zoomScaleNormal="80" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A3" activePane="bottomLeft" state="frozen"/>
+      <pane ySplit="1" topLeftCell="A13" activePane="bottomLeft" state="frozen"/>
       <selection activeCell="E2" sqref="E2"/>
-      <selection pane="bottomLeft" activeCell="I24" sqref="I24"/>
+      <selection pane="bottomLeft" activeCell="F50" sqref="F50"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -19958,8 +19937,8 @@
   </sheetPr>
   <dimension ref="A1:F8"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="E22" sqref="E22"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="F12" sqref="F12"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -20007,7 +19986,7 @@
         <v>529</v>
       </c>
       <c r="F2" t="s">
-        <v>539</v>
+        <v>534</v>
       </c>
     </row>
     <row r="3" spans="1:6" x14ac:dyDescent="0.25">
@@ -20027,7 +20006,7 @@
         <v>530</v>
       </c>
       <c r="F3" t="s">
-        <v>540</v>
+        <v>535</v>
       </c>
     </row>
     <row r="4" spans="1:6" x14ac:dyDescent="0.25">
@@ -20047,67 +20026,7 @@
         <v>531</v>
       </c>
       <c r="F4" t="s">
-        <v>538</v>
-      </c>
-    </row>
-    <row r="5" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A5" t="s">
         <v>533</v>
-      </c>
-      <c r="B5" t="s">
-        <v>533</v>
-      </c>
-      <c r="C5">
-        <v>1</v>
-      </c>
-      <c r="D5" t="s">
-        <v>7</v>
-      </c>
-      <c r="E5" t="s">
-        <v>534</v>
-      </c>
-      <c r="F5" t="s">
-        <v>536</v>
-      </c>
-    </row>
-    <row r="6" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A6" t="s">
-        <v>533</v>
-      </c>
-      <c r="B6" t="s">
-        <v>533</v>
-      </c>
-      <c r="C6">
-        <v>2</v>
-      </c>
-      <c r="D6" t="s">
-        <v>7</v>
-      </c>
-      <c r="E6" t="s">
-        <v>535</v>
-      </c>
-      <c r="F6" t="s">
-        <v>537</v>
-      </c>
-    </row>
-    <row r="7" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A7" t="s">
-        <v>541</v>
-      </c>
-      <c r="B7" t="s">
-        <v>541</v>
-      </c>
-      <c r="C7">
-        <v>1</v>
-      </c>
-      <c r="D7" t="s">
-        <v>7</v>
-      </c>
-      <c r="E7" t="s">
-        <v>541</v>
-      </c>
-      <c r="F7" t="s">
-        <v>542</v>
       </c>
     </row>
     <row r="8" spans="1:6" x14ac:dyDescent="0.25">

</xml_diff>

<commit_message>
changed order of fuels and sectors
</commit_message>
<xml_diff>
--- a/config/master_config.xlsx
+++ b/config/master_config.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\hyuga.kasai\Documents\Github\9th_Visualization\9th_edition_visualisation\config\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A5672B59-86A1-49AD-B17F-6B62913193FA}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F6AE0D47-2134-462B-A60F-7D7AC986C225}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="22050" yWindow="-16395" windowWidth="29040" windowHeight="15840" tabRatio="812" firstSheet="6" activeTab="7" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="22050" yWindow="-16395" windowWidth="29040" windowHeight="15840" tabRatio="812" activeTab="7" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="9th_EBT_schema" sheetId="7" r:id="rId1"/>
@@ -390,7 +390,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="4398" uniqueCount="551">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="4399" uniqueCount="551">
   <si>
     <t>chart_type</t>
   </si>
@@ -6414,7 +6414,7 @@
   <dimension ref="A1:P47"/>
   <sheetViews>
     <sheetView topLeftCell="A2" zoomScale="80" zoomScaleNormal="80" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A12" activePane="bottomLeft" state="frozen"/>
+      <pane ySplit="1" topLeftCell="A3" activePane="bottomLeft" state="frozen"/>
       <selection activeCell="E2" sqref="E2"/>
       <selection pane="bottomLeft" activeCell="I49" sqref="I49"/>
     </sheetView>
@@ -8726,8 +8726,8 @@
   </sheetPr>
   <dimension ref="A1:D232"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="C8" sqref="C8"/>
+    <sheetView topLeftCell="A25" workbookViewId="0">
+      <selection activeCell="B72" sqref="B72"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -14425,7 +14425,7 @@
   </sheetPr>
   <dimension ref="A1:D219"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
+    <sheetView topLeftCell="A7" workbookViewId="0">
       <selection activeCell="B33" sqref="B33"/>
     </sheetView>
   </sheetViews>
@@ -17789,10 +17789,10 @@
   </sheetPr>
   <dimension ref="A1:W50"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="D2" zoomScale="80" zoomScaleNormal="80" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A3" activePane="bottomLeft" state="frozen"/>
+    <sheetView tabSelected="1" topLeftCell="C2" zoomScale="80" zoomScaleNormal="80" workbookViewId="0">
+      <pane ySplit="1" topLeftCell="A9" activePane="bottomLeft" state="frozen"/>
       <selection activeCell="E2" sqref="E2"/>
-      <selection pane="bottomLeft" activeCell="M39" sqref="M39"/>
+      <selection pane="bottomLeft" activeCell="H52" sqref="H52"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -17926,22 +17926,22 @@
         <v>1</v>
       </c>
       <c r="H3" t="s">
+        <v>3</v>
+      </c>
+      <c r="I3" t="s">
         <v>10</v>
       </c>
-      <c r="I3" t="s">
-        <v>11</v>
-      </c>
       <c r="J3" t="s">
-        <v>3</v>
+        <v>83</v>
       </c>
       <c r="K3" t="s">
         <v>4</v>
       </c>
       <c r="L3" t="s">
-        <v>83</v>
+        <v>5</v>
       </c>
       <c r="M3" t="s">
-        <v>5</v>
+        <v>11</v>
       </c>
       <c r="N3" t="s">
         <v>155</v>
@@ -17970,22 +17970,22 @@
         <v>1</v>
       </c>
       <c r="H4" t="s">
+        <v>3</v>
+      </c>
+      <c r="I4" t="s">
         <v>10</v>
       </c>
-      <c r="I4" t="s">
-        <v>11</v>
-      </c>
       <c r="J4" t="s">
-        <v>3</v>
+        <v>83</v>
       </c>
       <c r="K4" t="s">
         <v>4</v>
       </c>
       <c r="L4" t="s">
-        <v>83</v>
+        <v>5</v>
       </c>
       <c r="M4" t="s">
-        <v>5</v>
+        <v>11</v>
       </c>
       <c r="N4" t="s">
         <v>155</v>
@@ -18014,22 +18014,22 @@
         <v>1</v>
       </c>
       <c r="H5" t="s">
+        <v>3</v>
+      </c>
+      <c r="I5" t="s">
         <v>10</v>
       </c>
-      <c r="I5" t="s">
-        <v>11</v>
-      </c>
       <c r="J5" t="s">
-        <v>3</v>
+        <v>83</v>
       </c>
       <c r="K5" t="s">
         <v>4</v>
       </c>
       <c r="L5" t="s">
-        <v>83</v>
+        <v>5</v>
       </c>
       <c r="M5" t="s">
-        <v>5</v>
+        <v>11</v>
       </c>
       <c r="N5" t="s">
         <v>155</v>
@@ -18058,34 +18058,34 @@
         <v>9</v>
       </c>
       <c r="H6" t="s">
+        <v>95</v>
+      </c>
+      <c r="I6" t="s">
+        <v>3</v>
+      </c>
+      <c r="J6" t="s">
+        <v>28</v>
+      </c>
+      <c r="K6" t="s">
         <v>10</v>
       </c>
-      <c r="I6" t="s">
+      <c r="L6" t="s">
+        <v>85</v>
+      </c>
+      <c r="M6" t="s">
+        <v>83</v>
+      </c>
+      <c r="N6" t="s">
+        <v>12</v>
+      </c>
+      <c r="O6" t="s">
+        <v>4</v>
+      </c>
+      <c r="P6" t="s">
+        <v>5</v>
+      </c>
+      <c r="Q6" t="s">
         <v>11</v>
-      </c>
-      <c r="J6" t="s">
-        <v>3</v>
-      </c>
-      <c r="K6" t="s">
-        <v>4</v>
-      </c>
-      <c r="L6" t="s">
-        <v>83</v>
-      </c>
-      <c r="M6" t="s">
-        <v>95</v>
-      </c>
-      <c r="N6" t="s">
-        <v>28</v>
-      </c>
-      <c r="O6" t="s">
-        <v>5</v>
-      </c>
-      <c r="P6" t="s">
-        <v>12</v>
-      </c>
-      <c r="Q6" t="s">
-        <v>85</v>
       </c>
       <c r="R6" t="s">
         <v>155</v>
@@ -18114,10 +18114,10 @@
         <v>9</v>
       </c>
       <c r="H7" t="s">
+        <v>14</v>
+      </c>
+      <c r="I7" t="s">
         <v>13</v>
-      </c>
-      <c r="I7" t="s">
-        <v>14</v>
       </c>
     </row>
     <row r="8" spans="1:23" x14ac:dyDescent="0.25">
@@ -18143,16 +18143,16 @@
         <v>11</v>
       </c>
       <c r="H8" t="s">
+        <v>21</v>
+      </c>
+      <c r="I8" t="s">
         <v>18</v>
       </c>
-      <c r="I8" t="s">
+      <c r="J8" t="s">
         <v>19</v>
       </c>
-      <c r="J8" t="s">
+      <c r="K8" t="s">
         <v>20</v>
-      </c>
-      <c r="K8" t="s">
-        <v>21</v>
       </c>
       <c r="L8" t="s">
         <v>22</v>
@@ -18181,16 +18181,16 @@
         <v>11</v>
       </c>
       <c r="H9" t="s">
+        <v>21</v>
+      </c>
+      <c r="I9" t="s">
         <v>18</v>
       </c>
-      <c r="I9" t="s">
+      <c r="J9" t="s">
         <v>19</v>
       </c>
-      <c r="J9" t="s">
+      <c r="K9" t="s">
         <v>20</v>
-      </c>
-      <c r="K9" t="s">
-        <v>21</v>
       </c>
       <c r="L9" t="s">
         <v>22</v>
@@ -18219,16 +18219,16 @@
         <v>23</v>
       </c>
       <c r="H10" t="s">
+        <v>21</v>
+      </c>
+      <c r="I10" t="s">
         <v>18</v>
       </c>
-      <c r="I10" t="s">
+      <c r="J10" t="s">
         <v>19</v>
       </c>
-      <c r="J10" t="s">
+      <c r="K10" t="s">
         <v>20</v>
-      </c>
-      <c r="K10" t="s">
-        <v>21</v>
       </c>
       <c r="L10" t="s">
         <v>22</v>
@@ -18257,16 +18257,16 @@
         <v>23</v>
       </c>
       <c r="H11" t="s">
+        <v>21</v>
+      </c>
+      <c r="I11" t="s">
         <v>18</v>
       </c>
-      <c r="I11" t="s">
+      <c r="J11" t="s">
         <v>19</v>
       </c>
-      <c r="J11" t="s">
+      <c r="K11" t="s">
         <v>20</v>
-      </c>
-      <c r="K11" t="s">
-        <v>21</v>
       </c>
       <c r="L11" t="s">
         <v>22</v>
@@ -18295,22 +18295,22 @@
         <v>3</v>
       </c>
       <c r="H12" t="s">
+        <v>25</v>
+      </c>
+      <c r="I12" t="s">
         <v>1</v>
       </c>
-      <c r="I12" t="s">
+      <c r="J12" t="s">
         <v>9</v>
       </c>
-      <c r="J12" t="s">
+      <c r="K12" t="s">
+        <v>27</v>
+      </c>
+      <c r="L12" t="s">
         <v>24</v>
       </c>
-      <c r="K12" t="s">
-        <v>25</v>
-      </c>
-      <c r="L12" t="s">
+      <c r="M12" t="s">
         <v>26</v>
-      </c>
-      <c r="M12" t="s">
-        <v>27</v>
       </c>
       <c r="N12" t="s">
         <v>155</v>
@@ -18339,22 +18339,22 @@
         <v>3</v>
       </c>
       <c r="H13" t="s">
+        <v>25</v>
+      </c>
+      <c r="I13" t="s">
         <v>1</v>
       </c>
-      <c r="I13" t="s">
+      <c r="J13" t="s">
         <v>9</v>
       </c>
-      <c r="J13" t="s">
+      <c r="K13" t="s">
+        <v>27</v>
+      </c>
+      <c r="L13" t="s">
         <v>24</v>
       </c>
-      <c r="K13" t="s">
-        <v>25</v>
-      </c>
-      <c r="L13" t="s">
+      <c r="M13" t="s">
         <v>26</v>
-      </c>
-      <c r="M13" t="s">
-        <v>27</v>
       </c>
       <c r="N13" t="s">
         <v>155</v>
@@ -18383,22 +18383,22 @@
         <v>155</v>
       </c>
       <c r="H14" t="s">
+        <v>25</v>
+      </c>
+      <c r="I14" t="s">
+        <v>31</v>
+      </c>
+      <c r="J14" t="s">
         <v>1</v>
       </c>
-      <c r="I14" t="s">
+      <c r="K14" t="s">
         <v>9</v>
       </c>
-      <c r="J14" t="s">
+      <c r="L14" t="s">
+        <v>27</v>
+      </c>
+      <c r="M14" t="s">
         <v>24</v>
-      </c>
-      <c r="K14" t="s">
-        <v>27</v>
-      </c>
-      <c r="L14" t="s">
-        <v>31</v>
-      </c>
-      <c r="M14" t="s">
-        <v>25</v>
       </c>
       <c r="N14" t="s">
         <v>155</v>
@@ -18427,22 +18427,22 @@
         <v>155</v>
       </c>
       <c r="H15" t="s">
+        <v>25</v>
+      </c>
+      <c r="I15" t="s">
+        <v>31</v>
+      </c>
+      <c r="J15" t="s">
         <v>1</v>
       </c>
-      <c r="I15" t="s">
+      <c r="K15" t="s">
         <v>9</v>
       </c>
-      <c r="J15" t="s">
+      <c r="L15" t="s">
+        <v>27</v>
+      </c>
+      <c r="M15" t="s">
         <v>24</v>
-      </c>
-      <c r="K15" t="s">
-        <v>27</v>
-      </c>
-      <c r="L15" t="s">
-        <v>31</v>
-      </c>
-      <c r="M15" t="s">
-        <v>25</v>
       </c>
       <c r="N15" t="s">
         <v>155</v>
@@ -18471,31 +18471,34 @@
         <v>459</v>
       </c>
       <c r="H16" t="s">
-        <v>10</v>
+        <v>11</v>
       </c>
       <c r="I16" t="s">
-        <v>11</v>
+        <v>5</v>
       </c>
       <c r="J16" t="s">
         <v>4</v>
       </c>
       <c r="K16" t="s">
-        <v>83</v>
+        <v>79</v>
       </c>
       <c r="L16" t="s">
         <v>81</v>
       </c>
       <c r="M16" t="s">
-        <v>5</v>
+        <v>85</v>
       </c>
       <c r="N16" t="s">
+        <v>89</v>
+      </c>
+      <c r="O16" t="s">
+        <v>83</v>
+      </c>
+      <c r="P16" t="s">
+        <v>10</v>
+      </c>
+      <c r="Q16" t="s">
         <v>480</v>
-      </c>
-      <c r="O16" t="s">
-        <v>85</v>
-      </c>
-      <c r="P16" t="s">
-        <v>89</v>
       </c>
     </row>
     <row r="17" spans="1:17" x14ac:dyDescent="0.25">
@@ -18521,10 +18524,10 @@
         <v>28</v>
       </c>
       <c r="H17" t="s">
+        <v>27</v>
+      </c>
+      <c r="I17" t="s">
         <v>24</v>
-      </c>
-      <c r="I17" t="s">
-        <v>27</v>
       </c>
       <c r="J17" t="s">
         <v>155</v>
@@ -18553,10 +18556,10 @@
         <v>28</v>
       </c>
       <c r="H18" t="s">
+        <v>27</v>
+      </c>
+      <c r="I18" t="s">
         <v>24</v>
-      </c>
-      <c r="I18" t="s">
-        <v>27</v>
       </c>
       <c r="J18" t="s">
         <v>155</v>
@@ -18585,10 +18588,10 @@
         <v>28</v>
       </c>
       <c r="H19" t="s">
+        <v>27</v>
+      </c>
+      <c r="I19" t="s">
         <v>24</v>
-      </c>
-      <c r="I19" t="s">
-        <v>27</v>
       </c>
       <c r="J19" t="s">
         <v>155</v>
@@ -18617,31 +18620,31 @@
         <v>24</v>
       </c>
       <c r="H20" t="s">
+        <v>95</v>
+      </c>
+      <c r="I20" t="s">
+        <v>3</v>
+      </c>
+      <c r="J20" t="s">
+        <v>28</v>
+      </c>
+      <c r="K20" t="s">
         <v>10</v>
-      </c>
-      <c r="I20" t="s">
-        <v>11</v>
-      </c>
-      <c r="J20" t="s">
-        <v>3</v>
-      </c>
-      <c r="K20" t="s">
-        <v>4</v>
       </c>
       <c r="L20" t="s">
         <v>83</v>
       </c>
       <c r="M20" t="s">
-        <v>95</v>
+        <v>12</v>
       </c>
       <c r="N20" t="s">
-        <v>28</v>
+        <v>4</v>
       </c>
       <c r="O20" t="s">
         <v>5</v>
       </c>
       <c r="P20" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="Q20" t="s">
         <v>155</v>
@@ -18670,25 +18673,25 @@
         <v>24</v>
       </c>
       <c r="H21" t="s">
+        <v>181</v>
+      </c>
+      <c r="I21" t="s">
+        <v>179</v>
+      </c>
+      <c r="J21" t="s">
+        <v>177</v>
+      </c>
+      <c r="K21" t="s">
         <v>168</v>
       </c>
-      <c r="I21" t="s">
+      <c r="L21" t="s">
         <v>171</v>
       </c>
-      <c r="J21" t="s">
+      <c r="M21" t="s">
         <v>173</v>
       </c>
-      <c r="K21" t="s">
+      <c r="N21" t="s">
         <v>175</v>
-      </c>
-      <c r="L21" t="s">
-        <v>177</v>
-      </c>
-      <c r="M21" s="13" t="s">
-        <v>179</v>
-      </c>
-      <c r="N21" t="s">
-        <v>181</v>
       </c>
     </row>
     <row r="22" spans="1:17" x14ac:dyDescent="0.25">
@@ -18714,25 +18717,25 @@
         <v>24</v>
       </c>
       <c r="H22" t="s">
+        <v>181</v>
+      </c>
+      <c r="I22" t="s">
+        <v>179</v>
+      </c>
+      <c r="J22" t="s">
+        <v>177</v>
+      </c>
+      <c r="K22" t="s">
         <v>168</v>
       </c>
-      <c r="I22" t="s">
+      <c r="L22" t="s">
         <v>171</v>
       </c>
-      <c r="J22" t="s">
+      <c r="M22" t="s">
         <v>173</v>
       </c>
-      <c r="K22" t="s">
+      <c r="N22" t="s">
         <v>175</v>
-      </c>
-      <c r="L22" t="s">
-        <v>177</v>
-      </c>
-      <c r="M22" t="s">
-        <v>179</v>
-      </c>
-      <c r="N22" t="s">
-        <v>181</v>
       </c>
     </row>
     <row r="23" spans="1:17" x14ac:dyDescent="0.25">
@@ -18758,16 +18761,16 @@
         <v>31</v>
       </c>
       <c r="H23" t="s">
-        <v>11</v>
+        <v>28</v>
       </c>
       <c r="I23" t="s">
         <v>4</v>
       </c>
       <c r="J23" t="s">
-        <v>28</v>
+        <v>5</v>
       </c>
       <c r="K23" t="s">
-        <v>5</v>
+        <v>11</v>
       </c>
       <c r="L23" t="s">
         <v>153</v>
@@ -18796,19 +18799,19 @@
         <v>20</v>
       </c>
       <c r="H24" t="s">
+        <v>29</v>
+      </c>
+      <c r="I24" t="s">
+        <v>33</v>
+      </c>
+      <c r="J24" t="s">
+        <v>4</v>
+      </c>
+      <c r="K24" t="s">
+        <v>5</v>
+      </c>
+      <c r="L24" t="s">
         <v>11</v>
-      </c>
-      <c r="I24" t="s">
-        <v>4</v>
-      </c>
-      <c r="J24" t="s">
-        <v>5</v>
-      </c>
-      <c r="K24" t="s">
-        <v>29</v>
-      </c>
-      <c r="L24" t="s">
-        <v>33</v>
       </c>
       <c r="M24" s="4" t="s">
         <v>22</v>
@@ -18837,19 +18840,19 @@
         <v>20</v>
       </c>
       <c r="H25" t="s">
+        <v>29</v>
+      </c>
+      <c r="I25" t="s">
+        <v>33</v>
+      </c>
+      <c r="J25" t="s">
+        <v>4</v>
+      </c>
+      <c r="K25" t="s">
+        <v>5</v>
+      </c>
+      <c r="L25" t="s">
         <v>11</v>
-      </c>
-      <c r="I25" t="s">
-        <v>4</v>
-      </c>
-      <c r="J25" t="s">
-        <v>5</v>
-      </c>
-      <c r="K25" t="s">
-        <v>29</v>
-      </c>
-      <c r="L25" t="s">
-        <v>33</v>
       </c>
       <c r="M25" s="4" t="s">
         <v>22</v>
@@ -18878,19 +18881,19 @@
         <v>20</v>
       </c>
       <c r="H26" t="s">
+        <v>29</v>
+      </c>
+      <c r="I26" t="s">
+        <v>33</v>
+      </c>
+      <c r="J26" t="s">
+        <v>4</v>
+      </c>
+      <c r="K26" t="s">
+        <v>5</v>
+      </c>
+      <c r="L26" t="s">
         <v>11</v>
-      </c>
-      <c r="I26" t="s">
-        <v>4</v>
-      </c>
-      <c r="J26" t="s">
-        <v>5</v>
-      </c>
-      <c r="K26" t="s">
-        <v>29</v>
-      </c>
-      <c r="L26" t="s">
-        <v>33</v>
       </c>
       <c r="M26" s="4" t="s">
         <v>22</v>
@@ -18919,13 +18922,13 @@
         <v>460</v>
       </c>
       <c r="H27" t="s">
-        <v>471</v>
+        <v>473</v>
       </c>
       <c r="I27" t="s">
         <v>472</v>
       </c>
       <c r="J27" t="s">
-        <v>473</v>
+        <v>471</v>
       </c>
     </row>
     <row r="28" spans="1:17" ht="23.25" customHeight="1" x14ac:dyDescent="0.25">
@@ -18951,28 +18954,28 @@
         <v>457</v>
       </c>
       <c r="H28" t="s">
+        <v>476</v>
+      </c>
+      <c r="I28" t="s">
+        <v>123</v>
+      </c>
+      <c r="J28" t="s">
+        <v>135</v>
+      </c>
+      <c r="K28" t="s">
+        <v>119</v>
+      </c>
+      <c r="L28" t="s">
+        <v>475</v>
+      </c>
+      <c r="M28" t="s">
+        <v>474</v>
+      </c>
+      <c r="N28" t="s">
+        <v>126</v>
+      </c>
+      <c r="O28" t="s">
         <v>121</v>
-      </c>
-      <c r="I28" t="s">
-        <v>126</v>
-      </c>
-      <c r="J28" t="s">
-        <v>474</v>
-      </c>
-      <c r="K28" t="s">
-        <v>475</v>
-      </c>
-      <c r="L28" t="s">
-        <v>119</v>
-      </c>
-      <c r="M28" t="s">
-        <v>135</v>
-      </c>
-      <c r="N28" t="s">
-        <v>123</v>
-      </c>
-      <c r="O28" t="s">
-        <v>476</v>
       </c>
     </row>
     <row r="29" spans="1:17" ht="21" customHeight="1" x14ac:dyDescent="0.25">
@@ -18998,28 +19001,28 @@
         <v>457</v>
       </c>
       <c r="H29" t="s">
+        <v>476</v>
+      </c>
+      <c r="I29" t="s">
+        <v>123</v>
+      </c>
+      <c r="J29" t="s">
+        <v>135</v>
+      </c>
+      <c r="K29" t="s">
+        <v>119</v>
+      </c>
+      <c r="L29" t="s">
+        <v>475</v>
+      </c>
+      <c r="M29" t="s">
+        <v>474</v>
+      </c>
+      <c r="N29" t="s">
+        <v>126</v>
+      </c>
+      <c r="O29" t="s">
         <v>121</v>
-      </c>
-      <c r="I29" t="s">
-        <v>126</v>
-      </c>
-      <c r="J29" t="s">
-        <v>474</v>
-      </c>
-      <c r="K29" t="s">
-        <v>475</v>
-      </c>
-      <c r="L29" t="s">
-        <v>119</v>
-      </c>
-      <c r="M29" t="s">
-        <v>135</v>
-      </c>
-      <c r="N29" t="s">
-        <v>123</v>
-      </c>
-      <c r="O29" t="s">
-        <v>476</v>
       </c>
     </row>
     <row r="30" spans="1:17" x14ac:dyDescent="0.25">
@@ -19045,19 +19048,19 @@
         <v>104</v>
       </c>
       <c r="H30" t="s">
+        <v>21</v>
+      </c>
+      <c r="I30" t="s">
         <v>32</v>
       </c>
-      <c r="I30" t="s">
+      <c r="J30" t="s">
         <v>18</v>
       </c>
-      <c r="J30" t="s">
+      <c r="K30" t="s">
         <v>19</v>
       </c>
-      <c r="K30" t="s">
+      <c r="L30" t="s">
         <v>20</v>
-      </c>
-      <c r="L30" t="s">
-        <v>21</v>
       </c>
       <c r="M30" t="s">
         <v>22</v>
@@ -19086,19 +19089,19 @@
         <v>22</v>
       </c>
       <c r="H31" t="s">
+        <v>29</v>
+      </c>
+      <c r="I31" t="s">
+        <v>33</v>
+      </c>
+      <c r="J31" t="s">
+        <v>4</v>
+      </c>
+      <c r="K31" t="s">
+        <v>5</v>
+      </c>
+      <c r="L31" t="s">
         <v>11</v>
-      </c>
-      <c r="I31" t="s">
-        <v>4</v>
-      </c>
-      <c r="J31" t="s">
-        <v>5</v>
-      </c>
-      <c r="K31" t="s">
-        <v>29</v>
-      </c>
-      <c r="L31" t="s">
-        <v>33</v>
       </c>
       <c r="M31" t="s">
         <v>22</v>
@@ -19127,19 +19130,19 @@
         <v>22</v>
       </c>
       <c r="H32" t="s">
+        <v>29</v>
+      </c>
+      <c r="I32" t="s">
+        <v>33</v>
+      </c>
+      <c r="J32" t="s">
+        <v>4</v>
+      </c>
+      <c r="K32" t="s">
+        <v>5</v>
+      </c>
+      <c r="L32" t="s">
         <v>11</v>
-      </c>
-      <c r="I32" t="s">
-        <v>4</v>
-      </c>
-      <c r="J32" t="s">
-        <v>5</v>
-      </c>
-      <c r="K32" t="s">
-        <v>29</v>
-      </c>
-      <c r="L32" t="s">
-        <v>33</v>
       </c>
       <c r="M32" t="s">
         <v>22</v>
@@ -19197,16 +19200,16 @@
         <v>22</v>
       </c>
       <c r="H34" t="s">
+        <v>21</v>
+      </c>
+      <c r="I34" t="s">
         <v>32</v>
       </c>
-      <c r="I34" t="s">
+      <c r="J34" t="s">
         <v>35</v>
       </c>
-      <c r="J34" t="s">
+      <c r="K34" t="s">
         <v>20</v>
-      </c>
-      <c r="K34" t="s">
-        <v>21</v>
       </c>
     </row>
     <row r="35" spans="1:23" x14ac:dyDescent="0.25">
@@ -19232,34 +19235,34 @@
         <v>155</v>
       </c>
       <c r="H35" t="s">
+        <v>95</v>
+      </c>
+      <c r="I35" t="s">
+        <v>3</v>
+      </c>
+      <c r="J35" t="s">
+        <v>28</v>
+      </c>
+      <c r="K35" t="s">
         <v>10</v>
       </c>
-      <c r="I35" t="s">
+      <c r="L35" t="s">
+        <v>85</v>
+      </c>
+      <c r="M35" t="s">
+        <v>83</v>
+      </c>
+      <c r="N35" t="s">
+        <v>12</v>
+      </c>
+      <c r="O35" t="s">
+        <v>4</v>
+      </c>
+      <c r="P35" t="s">
+        <v>5</v>
+      </c>
+      <c r="Q35" t="s">
         <v>11</v>
-      </c>
-      <c r="J35" t="s">
-        <v>3</v>
-      </c>
-      <c r="K35" t="s">
-        <v>4</v>
-      </c>
-      <c r="L35" t="s">
-        <v>83</v>
-      </c>
-      <c r="M35" t="s">
-        <v>95</v>
-      </c>
-      <c r="N35" t="s">
-        <v>28</v>
-      </c>
-      <c r="O35" t="s">
-        <v>5</v>
-      </c>
-      <c r="P35" t="s">
-        <v>12</v>
-      </c>
-      <c r="Q35" t="s">
-        <v>85</v>
       </c>
       <c r="R35" t="s">
         <v>155</v>
@@ -19288,34 +19291,34 @@
         <v>155</v>
       </c>
       <c r="H36" t="s">
+        <v>95</v>
+      </c>
+      <c r="I36" t="s">
+        <v>3</v>
+      </c>
+      <c r="J36" t="s">
+        <v>28</v>
+      </c>
+      <c r="K36" t="s">
         <v>10</v>
       </c>
-      <c r="I36" t="s">
+      <c r="L36" t="s">
+        <v>85</v>
+      </c>
+      <c r="M36" t="s">
+        <v>83</v>
+      </c>
+      <c r="N36" t="s">
+        <v>12</v>
+      </c>
+      <c r="O36" t="s">
+        <v>4</v>
+      </c>
+      <c r="P36" t="s">
+        <v>5</v>
+      </c>
+      <c r="Q36" t="s">
         <v>11</v>
-      </c>
-      <c r="J36" t="s">
-        <v>3</v>
-      </c>
-      <c r="K36" t="s">
-        <v>4</v>
-      </c>
-      <c r="L36" t="s">
-        <v>83</v>
-      </c>
-      <c r="M36" t="s">
-        <v>95</v>
-      </c>
-      <c r="N36" t="s">
-        <v>28</v>
-      </c>
-      <c r="O36" t="s">
-        <v>5</v>
-      </c>
-      <c r="P36" t="s">
-        <v>12</v>
-      </c>
-      <c r="Q36" t="s">
-        <v>85</v>
       </c>
       <c r="R36" t="s">
         <v>155</v>
@@ -19344,13 +19347,13 @@
         <v>11</v>
       </c>
       <c r="H37" t="s">
+        <v>17</v>
+      </c>
+      <c r="I37" t="s">
         <v>15</v>
       </c>
-      <c r="I37" t="s">
+      <c r="J37" t="s">
         <v>16</v>
-      </c>
-      <c r="J37" t="s">
-        <v>17</v>
       </c>
     </row>
     <row r="38" spans="1:23" x14ac:dyDescent="0.25">
@@ -19376,10 +19379,10 @@
         <v>11</v>
       </c>
       <c r="H38" t="s">
+        <v>17</v>
+      </c>
+      <c r="I38" t="s">
         <v>16</v>
-      </c>
-      <c r="I38" t="s">
-        <v>17</v>
       </c>
     </row>
     <row r="39" spans="1:23" x14ac:dyDescent="0.25">
@@ -19405,10 +19408,10 @@
         <v>11</v>
       </c>
       <c r="H39" t="s">
+        <v>17</v>
+      </c>
+      <c r="I39" t="s">
         <v>16</v>
-      </c>
-      <c r="I39" t="s">
-        <v>17</v>
       </c>
     </row>
     <row r="40" spans="1:23" x14ac:dyDescent="0.25">
@@ -19434,16 +19437,16 @@
         <v>27</v>
       </c>
       <c r="H40" t="s">
+        <v>3</v>
+      </c>
+      <c r="I40" t="s">
+        <v>28</v>
+      </c>
+      <c r="J40" t="s">
         <v>104</v>
       </c>
-      <c r="I40" t="s">
-        <v>3</v>
-      </c>
-      <c r="J40" t="s">
-        <v>28</v>
-      </c>
       <c r="K40" t="s">
-        <v>4</v>
+        <v>483</v>
       </c>
       <c r="L40" t="s">
         <v>119</v>
@@ -19452,7 +19455,7 @@
         <v>121</v>
       </c>
       <c r="N40" t="s">
-        <v>483</v>
+        <v>4</v>
       </c>
       <c r="O40" t="s">
         <v>155</v>
@@ -19481,16 +19484,16 @@
         <v>27</v>
       </c>
       <c r="H41" t="s">
+        <v>3</v>
+      </c>
+      <c r="I41" t="s">
+        <v>28</v>
+      </c>
+      <c r="J41" t="s">
         <v>104</v>
       </c>
-      <c r="I41" t="s">
-        <v>3</v>
-      </c>
-      <c r="J41" t="s">
-        <v>28</v>
-      </c>
       <c r="K41" t="s">
-        <v>4</v>
+        <v>483</v>
       </c>
       <c r="L41" t="s">
         <v>119</v>
@@ -19499,7 +19502,7 @@
         <v>121</v>
       </c>
       <c r="N41" t="s">
-        <v>483</v>
+        <v>4</v>
       </c>
       <c r="O41" t="s">
         <v>155</v>
@@ -19528,16 +19531,16 @@
         <v>27</v>
       </c>
       <c r="H42" t="s">
+        <v>3</v>
+      </c>
+      <c r="I42" t="s">
+        <v>28</v>
+      </c>
+      <c r="J42" t="s">
         <v>104</v>
       </c>
-      <c r="I42" t="s">
-        <v>3</v>
-      </c>
-      <c r="J42" t="s">
-        <v>28</v>
-      </c>
       <c r="K42" t="s">
-        <v>4</v>
+        <v>483</v>
       </c>
       <c r="L42" t="s">
         <v>119</v>
@@ -19546,7 +19549,7 @@
         <v>121</v>
       </c>
       <c r="N42" t="s">
-        <v>483</v>
+        <v>4</v>
       </c>
       <c r="O42" t="s">
         <v>155</v>
@@ -19575,19 +19578,19 @@
         <v>27</v>
       </c>
       <c r="H43" t="s">
+        <v>41</v>
+      </c>
+      <c r="I43" t="s">
+        <v>40</v>
+      </c>
+      <c r="J43" s="12" t="s">
+        <v>42</v>
+      </c>
+      <c r="K43" t="s">
         <v>43</v>
       </c>
-      <c r="I43" s="12" t="s">
-        <v>42</v>
-      </c>
-      <c r="J43" t="s">
+      <c r="L43" t="s">
         <v>39</v>
-      </c>
-      <c r="K43" t="s">
-        <v>41</v>
-      </c>
-      <c r="L43" t="s">
-        <v>40</v>
       </c>
       <c r="M43" s="12" t="s">
         <v>155</v>
@@ -19616,19 +19619,19 @@
         <v>27</v>
       </c>
       <c r="H44" t="s">
+        <v>41</v>
+      </c>
+      <c r="I44" t="s">
+        <v>40</v>
+      </c>
+      <c r="J44" s="12" t="s">
+        <v>42</v>
+      </c>
+      <c r="K44" t="s">
         <v>43</v>
       </c>
-      <c r="I44" s="12" t="s">
-        <v>42</v>
-      </c>
-      <c r="J44" t="s">
+      <c r="L44" t="s">
         <v>39</v>
-      </c>
-      <c r="K44" t="s">
-        <v>41</v>
-      </c>
-      <c r="L44" t="s">
-        <v>40</v>
       </c>
       <c r="M44" s="12" t="s">
         <v>155</v>
@@ -19660,22 +19663,22 @@
         <v>3</v>
       </c>
       <c r="I45" t="s">
+        <v>25</v>
+      </c>
+      <c r="J45" t="s">
         <v>1</v>
       </c>
-      <c r="J45" t="s">
+      <c r="K45" t="s">
         <v>9</v>
       </c>
-      <c r="K45" t="s">
+      <c r="L45" t="s">
+        <v>27</v>
+      </c>
+      <c r="M45" t="s">
         <v>24</v>
       </c>
-      <c r="L45" t="s">
-        <v>25</v>
-      </c>
-      <c r="M45" t="s">
+      <c r="N45" t="s">
         <v>26</v>
-      </c>
-      <c r="N45" t="s">
-        <v>27</v>
       </c>
       <c r="O45" t="s">
         <v>155</v>
@@ -19707,22 +19710,22 @@
         <v>3</v>
       </c>
       <c r="I46" t="s">
+        <v>25</v>
+      </c>
+      <c r="J46" t="s">
         <v>1</v>
       </c>
-      <c r="J46" t="s">
+      <c r="K46" t="s">
         <v>9</v>
       </c>
-      <c r="K46" t="s">
+      <c r="L46" t="s">
+        <v>27</v>
+      </c>
+      <c r="M46" t="s">
         <v>24</v>
       </c>
-      <c r="L46" t="s">
-        <v>25</v>
-      </c>
-      <c r="M46" t="s">
+      <c r="N46" t="s">
         <v>26</v>
-      </c>
-      <c r="N46" t="s">
-        <v>27</v>
       </c>
       <c r="O46" t="s">
         <v>155</v>
@@ -19754,22 +19757,22 @@
         <v>3</v>
       </c>
       <c r="I47" t="s">
+        <v>25</v>
+      </c>
+      <c r="J47" t="s">
         <v>1</v>
       </c>
-      <c r="J47" t="s">
+      <c r="K47" t="s">
         <v>9</v>
       </c>
-      <c r="K47" t="s">
+      <c r="L47" t="s">
+        <v>27</v>
+      </c>
+      <c r="M47" t="s">
         <v>24</v>
       </c>
-      <c r="L47" t="s">
-        <v>25</v>
-      </c>
-      <c r="M47" t="s">
+      <c r="N47" t="s">
         <v>26</v>
-      </c>
-      <c r="N47" t="s">
-        <v>27</v>
       </c>
       <c r="O47" t="s">
         <v>155</v>
@@ -19901,16 +19904,16 @@
         <v>27</v>
       </c>
       <c r="H50" t="s">
+        <v>3</v>
+      </c>
+      <c r="I50" t="s">
+        <v>28</v>
+      </c>
+      <c r="J50" t="s">
         <v>104</v>
       </c>
-      <c r="I50" t="s">
-        <v>3</v>
-      </c>
-      <c r="J50" t="s">
-        <v>28</v>
-      </c>
       <c r="K50" t="s">
-        <v>4</v>
+        <v>483</v>
       </c>
       <c r="L50" t="s">
         <v>119</v>
@@ -19919,7 +19922,7 @@
         <v>121</v>
       </c>
       <c r="N50" t="s">
-        <v>483</v>
+        <v>4</v>
       </c>
       <c r="O50" t="s">
         <v>155</v>

</xml_diff>

<commit_message>
working on capacity and transport stocks
</commit_message>
<xml_diff>
--- a/config/master_config.xlsx
+++ b/config/master_config.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\hyuga.kasai\Documents\Github\9th_Visualization\9th_edition_visualisation\config\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{5DA1A0C6-A65B-400A-91FD-34EE687B3DB7}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{347784AC-7792-43B3-BE0A-13CD508B8DBB}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-6750" yWindow="-16320" windowWidth="29040" windowHeight="15840" tabRatio="812" firstSheet="1" activeTab="4" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-6750" yWindow="-16320" windowWidth="29040" windowHeight="15840" tabRatio="812" firstSheet="2" activeTab="7" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="9th_EBT_schema" sheetId="7" r:id="rId1"/>
@@ -29,7 +29,7 @@
     <sheet name="table_id_to_chart_old" sheetId="2" r:id="rId14"/>
   </sheets>
   <definedNames>
-    <definedName name="_xlnm._FilterDatabase" localSheetId="10" hidden="1">colors!$A$1:$B$97</definedName>
+    <definedName name="_xlnm._FilterDatabase" localSheetId="10" hidden="1">colors!$A$1:$B$99</definedName>
   </definedNames>
   <calcPr calcId="191029"/>
   <extLst>
@@ -390,7 +390,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="4407" uniqueCount="555">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="4426" uniqueCount="559">
   <si>
     <t>chart_type</t>
   </si>
@@ -2055,6 +2055,18 @@
   </si>
   <si>
     <t>Wind onshore</t>
+  </si>
+  <si>
+    <t>Storage Batteries</t>
+  </si>
+  <si>
+    <t>Storage</t>
+  </si>
+  <si>
+    <t>#2A615A</t>
+  </si>
+  <si>
+    <t>#AB6262</t>
   </si>
 </sst>
 </file>
@@ -2491,7 +2503,7 @@
     <xdr:to>
       <xdr:col>17</xdr:col>
       <xdr:colOff>213360</xdr:colOff>
-      <xdr:row>23</xdr:row>
+      <xdr:row>24</xdr:row>
       <xdr:rowOff>38100</xdr:rowOff>
     </xdr:to>
     <xdr:sp macro="" textlink="">
@@ -5538,10 +5550,10 @@
   <sheetPr>
     <tabColor rgb="FFFFC000"/>
   </sheetPr>
-  <dimension ref="A1:B97"/>
+  <dimension ref="A1:B99"/>
   <sheetViews>
-    <sheetView topLeftCell="A35" workbookViewId="0">
-      <selection activeCell="C43" sqref="C43"/>
+    <sheetView topLeftCell="A29" workbookViewId="0">
+      <selection activeCell="B44" sqref="B44"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -5663,55 +5675,55 @@
     </row>
     <row r="15" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A15" t="s">
-        <v>21</v>
+        <v>556</v>
       </c>
       <c r="B15" t="s">
-        <v>433</v>
+        <v>557</v>
       </c>
     </row>
     <row r="16" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A16" t="s">
-        <v>151</v>
+        <v>21</v>
       </c>
       <c r="B16" t="s">
-        <v>443</v>
+        <v>433</v>
       </c>
     </row>
     <row r="17" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A17" t="s">
-        <v>85</v>
+        <v>151</v>
       </c>
       <c r="B17" t="s">
-        <v>437</v>
+        <v>443</v>
       </c>
     </row>
     <row r="18" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A18" t="s">
-        <v>14</v>
+        <v>85</v>
       </c>
       <c r="B18" t="s">
-        <v>434</v>
+        <v>437</v>
       </c>
     </row>
     <row r="19" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A19" t="s">
-        <v>43</v>
+        <v>14</v>
       </c>
       <c r="B19" t="s">
-        <v>442</v>
+        <v>434</v>
       </c>
     </row>
     <row r="20" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A20" t="s">
-        <v>13</v>
+        <v>43</v>
       </c>
       <c r="B20" t="s">
-        <v>435</v>
+        <v>442</v>
       </c>
     </row>
     <row r="21" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A21" t="s">
-        <v>33</v>
+        <v>13</v>
       </c>
       <c r="B21" t="s">
         <v>435</v>
@@ -5719,15 +5731,15 @@
     </row>
     <row r="22" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A22" t="s">
-        <v>457</v>
+        <v>33</v>
       </c>
       <c r="B22" t="s">
-        <v>446</v>
+        <v>435</v>
       </c>
     </row>
     <row r="23" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A23" t="s">
-        <v>460</v>
+        <v>457</v>
       </c>
       <c r="B23" t="s">
         <v>446</v>
@@ -5735,7 +5747,7 @@
     </row>
     <row r="24" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A24" t="s">
-        <v>58</v>
+        <v>460</v>
       </c>
       <c r="B24" t="s">
         <v>446</v>
@@ -5743,47 +5755,47 @@
     </row>
     <row r="25" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A25" t="s">
-        <v>37</v>
+        <v>58</v>
       </c>
       <c r="B25" t="s">
-        <v>443</v>
+        <v>446</v>
       </c>
     </row>
     <row r="26" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A26" t="s">
-        <v>42</v>
+        <v>37</v>
       </c>
       <c r="B26" t="s">
-        <v>433</v>
+        <v>443</v>
       </c>
     </row>
     <row r="27" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A27" t="s">
-        <v>179</v>
+        <v>42</v>
       </c>
       <c r="B27" t="s">
-        <v>437</v>
+        <v>433</v>
       </c>
     </row>
     <row r="28" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A28" t="s">
-        <v>20</v>
+        <v>179</v>
       </c>
       <c r="B28" t="s">
-        <v>442</v>
+        <v>437</v>
       </c>
     </row>
     <row r="29" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A29" t="s">
-        <v>456</v>
+        <v>20</v>
       </c>
       <c r="B29" t="s">
-        <v>440</v>
+        <v>442</v>
       </c>
     </row>
     <row r="30" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A30" t="s">
-        <v>459</v>
+        <v>456</v>
       </c>
       <c r="B30" t="s">
         <v>440</v>
@@ -5791,7 +5803,7 @@
     </row>
     <row r="31" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A31" t="s">
-        <v>52</v>
+        <v>459</v>
       </c>
       <c r="B31" t="s">
         <v>440</v>
@@ -5799,39 +5811,39 @@
     </row>
     <row r="32" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A32" t="s">
-        <v>41</v>
+        <v>52</v>
       </c>
       <c r="B32" t="s">
-        <v>444</v>
+        <v>440</v>
       </c>
     </row>
     <row r="33" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A33" t="s">
-        <v>198</v>
+        <v>41</v>
       </c>
       <c r="B33" t="s">
-        <v>445</v>
+        <v>444</v>
       </c>
     </row>
     <row r="34" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A34" t="s">
-        <v>26</v>
+        <v>198</v>
       </c>
       <c r="B34" t="s">
-        <v>438</v>
+        <v>445</v>
       </c>
     </row>
     <row r="35" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A35" t="s">
-        <v>29</v>
+        <v>26</v>
       </c>
       <c r="B35" t="s">
-        <v>440</v>
+        <v>438</v>
       </c>
     </row>
     <row r="36" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A36" t="s">
-        <v>181</v>
+        <v>29</v>
       </c>
       <c r="B36" t="s">
         <v>440</v>
@@ -5839,15 +5851,15 @@
     </row>
     <row r="37" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A37" t="s">
-        <v>12</v>
+        <v>181</v>
       </c>
       <c r="B37" t="s">
-        <v>435</v>
+        <v>440</v>
       </c>
     </row>
     <row r="38" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A38" t="s">
-        <v>480</v>
+        <v>12</v>
       </c>
       <c r="B38" t="s">
         <v>435</v>
@@ -5855,15 +5867,15 @@
     </row>
     <row r="39" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A39" t="s">
-        <v>476</v>
+        <v>480</v>
       </c>
       <c r="B39" t="s">
-        <v>437</v>
+        <v>435</v>
       </c>
     </row>
     <row r="40" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A40" t="s">
-        <v>547</v>
+        <v>476</v>
       </c>
       <c r="B40" t="s">
         <v>437</v>
@@ -5871,7 +5883,7 @@
     </row>
     <row r="41" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A41" t="s">
-        <v>473</v>
+        <v>547</v>
       </c>
       <c r="B41" t="s">
         <v>437</v>
@@ -5879,10 +5891,10 @@
     </row>
     <row r="42" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A42" t="s">
-        <v>5</v>
+        <v>473</v>
       </c>
       <c r="B42" t="s">
-        <v>433</v>
+        <v>437</v>
       </c>
     </row>
     <row r="43" spans="1:2" x14ac:dyDescent="0.25">
@@ -5895,79 +5907,79 @@
     </row>
     <row r="44" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A44" t="s">
-        <v>87</v>
+        <v>549</v>
       </c>
       <c r="B44" t="s">
-        <v>442</v>
+        <v>558</v>
       </c>
     </row>
     <row r="45" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A45" t="s">
-        <v>79</v>
+        <v>5</v>
       </c>
       <c r="B45" t="s">
-        <v>444</v>
+        <v>433</v>
       </c>
     </row>
     <row r="46" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A46" t="s">
-        <v>200</v>
+        <v>87</v>
       </c>
       <c r="B46" t="s">
-        <v>438</v>
+        <v>442</v>
       </c>
     </row>
     <row r="47" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A47" t="s">
-        <v>187</v>
+        <v>79</v>
       </c>
       <c r="B47" t="s">
-        <v>438</v>
+        <v>444</v>
       </c>
     </row>
     <row r="48" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A48" t="s">
-        <v>25</v>
+        <v>200</v>
       </c>
       <c r="B48" t="s">
-        <v>443</v>
+        <v>438</v>
       </c>
     </row>
     <row r="49" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A49" t="s">
-        <v>177</v>
+        <v>187</v>
       </c>
       <c r="B49" t="s">
-        <v>432</v>
+        <v>438</v>
       </c>
     </row>
     <row r="50" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A50" t="s">
-        <v>31</v>
+        <v>25</v>
       </c>
       <c r="B50" t="s">
-        <v>435</v>
+        <v>443</v>
       </c>
     </row>
     <row r="51" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A51" t="s">
-        <v>102</v>
+        <v>177</v>
       </c>
       <c r="B51" t="s">
-        <v>434</v>
+        <v>432</v>
       </c>
     </row>
     <row r="52" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A52" t="s">
-        <v>472</v>
+        <v>31</v>
       </c>
       <c r="B52" t="s">
-        <v>434</v>
+        <v>435</v>
       </c>
     </row>
     <row r="53" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A53" t="s">
-        <v>35</v>
+        <v>102</v>
       </c>
       <c r="B53" t="s">
         <v>434</v>
@@ -5975,39 +5987,39 @@
     </row>
     <row r="54" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A54" t="s">
-        <v>474</v>
+        <v>472</v>
       </c>
       <c r="B54" t="s">
-        <v>477</v>
+        <v>434</v>
       </c>
     </row>
     <row r="55" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A55" t="s">
-        <v>100</v>
+        <v>35</v>
       </c>
       <c r="B55" t="s">
-        <v>437</v>
+        <v>434</v>
       </c>
     </row>
     <row r="56" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A56" t="s">
-        <v>175</v>
+        <v>474</v>
       </c>
       <c r="B56" t="s">
-        <v>435</v>
+        <v>477</v>
       </c>
     </row>
     <row r="57" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A57" t="s">
-        <v>16</v>
+        <v>100</v>
       </c>
       <c r="B57" t="s">
-        <v>435</v>
+        <v>437</v>
       </c>
     </row>
     <row r="58" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A58" t="s">
-        <v>40</v>
+        <v>175</v>
       </c>
       <c r="B58" t="s">
         <v>435</v>
@@ -6015,87 +6027,87 @@
     </row>
     <row r="59" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A59" t="s">
-        <v>123</v>
+        <v>16</v>
       </c>
       <c r="B59" t="s">
-        <v>444</v>
+        <v>435</v>
       </c>
     </row>
     <row r="60" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A60" t="s">
-        <v>137</v>
+        <v>40</v>
       </c>
       <c r="B60" t="s">
-        <v>436</v>
+        <v>435</v>
       </c>
     </row>
     <row r="61" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A61" t="s">
-        <v>15</v>
+        <v>123</v>
       </c>
       <c r="B61" t="s">
-        <v>446</v>
+        <v>444</v>
       </c>
     </row>
     <row r="62" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A62" t="s">
-        <v>475</v>
+        <v>137</v>
       </c>
       <c r="B62" t="s">
-        <v>440</v>
+        <v>436</v>
       </c>
     </row>
     <row r="63" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A63" t="s">
-        <v>126</v>
+        <v>15</v>
       </c>
       <c r="B63" t="s">
-        <v>433</v>
+        <v>446</v>
       </c>
     </row>
     <row r="64" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A64" t="s">
-        <v>173</v>
+        <v>475</v>
       </c>
       <c r="B64" t="s">
-        <v>442</v>
+        <v>440</v>
       </c>
     </row>
     <row r="65" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A65" t="s">
-        <v>24</v>
+        <v>126</v>
       </c>
       <c r="B65" t="s">
-        <v>441</v>
+        <v>433</v>
       </c>
     </row>
     <row r="66" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A66" t="s">
-        <v>19</v>
+        <v>173</v>
       </c>
       <c r="B66" t="s">
-        <v>441</v>
+        <v>442</v>
       </c>
     </row>
     <row r="67" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A67" t="s">
-        <v>458</v>
+        <v>24</v>
       </c>
       <c r="B67" t="s">
-        <v>479</v>
+        <v>441</v>
       </c>
     </row>
     <row r="68" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A68" t="s">
-        <v>461</v>
+        <v>19</v>
       </c>
       <c r="B68" t="s">
-        <v>479</v>
+        <v>441</v>
       </c>
     </row>
     <row r="69" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A69" t="s">
-        <v>28</v>
+        <v>458</v>
       </c>
       <c r="B69" t="s">
         <v>479</v>
@@ -6103,55 +6115,55 @@
     </row>
     <row r="70" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A70" t="s">
-        <v>81</v>
+        <v>461</v>
       </c>
       <c r="B70" t="s">
-        <v>445</v>
+        <v>479</v>
       </c>
     </row>
     <row r="71" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A71" t="s">
-        <v>167</v>
+        <v>28</v>
       </c>
       <c r="B71" t="s">
-        <v>439</v>
+        <v>479</v>
       </c>
     </row>
     <row r="72" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A72" t="s">
-        <v>95</v>
+        <v>81</v>
       </c>
       <c r="B72" t="s">
-        <v>439</v>
+        <v>445</v>
       </c>
     </row>
     <row r="73" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A73" t="s">
-        <v>83</v>
+        <v>167</v>
       </c>
       <c r="B73" t="s">
-        <v>442</v>
+        <v>439</v>
       </c>
     </row>
     <row r="74" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A74" t="s">
-        <v>121</v>
+        <v>95</v>
       </c>
       <c r="B74" t="s">
-        <v>443</v>
+        <v>439</v>
       </c>
     </row>
     <row r="75" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A75" t="s">
-        <v>4</v>
+        <v>83</v>
       </c>
       <c r="B75" t="s">
-        <v>434</v>
+        <v>442</v>
       </c>
     </row>
     <row r="76" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A76" t="s">
-        <v>135</v>
+        <v>121</v>
       </c>
       <c r="B76" t="s">
         <v>443</v>
@@ -6159,15 +6171,15 @@
     </row>
     <row r="77" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A77" t="s">
-        <v>195</v>
+        <v>4</v>
       </c>
       <c r="B77" t="s">
-        <v>443</v>
+        <v>434</v>
       </c>
     </row>
     <row r="78" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A78" t="s">
-        <v>18</v>
+        <v>135</v>
       </c>
       <c r="B78" t="s">
         <v>443</v>
@@ -6175,23 +6187,23 @@
     </row>
     <row r="79" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A79" t="s">
-        <v>165</v>
+        <v>195</v>
       </c>
       <c r="B79" t="s">
-        <v>438</v>
+        <v>443</v>
       </c>
     </row>
     <row r="80" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A80" t="s">
-        <v>546</v>
+        <v>18</v>
       </c>
       <c r="B80" t="s">
-        <v>438</v>
+        <v>443</v>
       </c>
     </row>
     <row r="81" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A81" t="s">
-        <v>103</v>
+        <v>165</v>
       </c>
       <c r="B81" t="s">
         <v>438</v>
@@ -6199,7 +6211,7 @@
     </row>
     <row r="82" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A82" t="s">
-        <v>3</v>
+        <v>546</v>
       </c>
       <c r="B82" t="s">
         <v>438</v>
@@ -6207,31 +6219,31 @@
     </row>
     <row r="83" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A83" t="s">
-        <v>119</v>
+        <v>103</v>
       </c>
       <c r="B83" t="s">
-        <v>432</v>
+        <v>438</v>
       </c>
     </row>
     <row r="84" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A84" t="s">
-        <v>116</v>
+        <v>3</v>
       </c>
       <c r="B84" t="s">
-        <v>446</v>
+        <v>438</v>
       </c>
     </row>
     <row r="85" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A85" t="s">
-        <v>36</v>
+        <v>119</v>
       </c>
       <c r="B85" t="s">
-        <v>446</v>
+        <v>432</v>
       </c>
     </row>
     <row r="86" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A86" t="s">
-        <v>471</v>
+        <v>116</v>
       </c>
       <c r="B86" t="s">
         <v>446</v>
@@ -6239,7 +6251,7 @@
     </row>
     <row r="87" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A87" t="s">
-        <v>189</v>
+        <v>36</v>
       </c>
       <c r="B87" t="s">
         <v>446</v>
@@ -6247,55 +6259,55 @@
     </row>
     <row r="88" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A88" t="s">
-        <v>11</v>
+        <v>471</v>
       </c>
       <c r="B88" t="s">
-        <v>432</v>
+        <v>446</v>
       </c>
     </row>
     <row r="89" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A89" t="s">
-        <v>171</v>
+        <v>189</v>
       </c>
       <c r="B89" t="s">
-        <v>434</v>
+        <v>446</v>
       </c>
     </row>
     <row r="90" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A90" t="s">
-        <v>32</v>
+        <v>11</v>
       </c>
       <c r="B90" t="s">
-        <v>435</v>
+        <v>432</v>
       </c>
     </row>
     <row r="91" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A91" t="s">
-        <v>9</v>
+        <v>171</v>
       </c>
       <c r="B91" t="s">
-        <v>433</v>
+        <v>434</v>
       </c>
     </row>
     <row r="92" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A92" t="s">
-        <v>10</v>
+        <v>32</v>
       </c>
       <c r="B92" t="s">
-        <v>436</v>
+        <v>435</v>
       </c>
     </row>
     <row r="93" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A93" t="s">
-        <v>136</v>
+        <v>9</v>
       </c>
       <c r="B93" t="s">
-        <v>440</v>
+        <v>433</v>
       </c>
     </row>
     <row r="94" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A94" t="s">
-        <v>104</v>
+        <v>10</v>
       </c>
       <c r="B94" t="s">
         <v>436</v>
@@ -6303,32 +6315,48 @@
     </row>
     <row r="95" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A95" t="s">
-        <v>39</v>
+        <v>136</v>
       </c>
       <c r="B95" t="s">
-        <v>443</v>
+        <v>440</v>
       </c>
     </row>
     <row r="96" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A96" t="s">
-        <v>168</v>
+        <v>104</v>
       </c>
       <c r="B96" t="s">
-        <v>433</v>
+        <v>436</v>
       </c>
     </row>
     <row r="97" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A97" t="s">
+        <v>39</v>
+      </c>
+      <c r="B97" t="s">
+        <v>443</v>
+      </c>
+    </row>
+    <row r="98" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A98" t="s">
+        <v>168</v>
+      </c>
+      <c r="B98" t="s">
+        <v>433</v>
+      </c>
+    </row>
+    <row r="99" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A99" t="s">
         <v>1</v>
       </c>
-      <c r="B97" t="s">
+      <c r="B99" t="s">
         <v>434</v>
       </c>
     </row>
   </sheetData>
-  <autoFilter ref="A1:B97" xr:uid="{344218C0-5C74-48AB-A8DF-7C6AE2CA916D}">
-    <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="A2:B97">
-      <sortCondition descending="1" ref="A1:A97"/>
+  <autoFilter ref="A1:B99" xr:uid="{344218C0-5C74-48AB-A8DF-7C6AE2CA916D}">
+    <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="A2:B99">
+      <sortCondition descending="1" ref="A1:A99"/>
     </sortState>
   </autoFilter>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
@@ -11846,10 +11874,10 @@
   <sheetPr>
     <tabColor theme="8"/>
   </sheetPr>
-  <dimension ref="A1:H102"/>
+  <dimension ref="A1:H103"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A79" workbookViewId="0">
-      <selection activeCell="D98" sqref="D98"/>
+    <sheetView topLeftCell="A79" workbookViewId="0">
+      <selection activeCell="C102" sqref="C102"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -14322,8 +14350,11 @@
       <c r="B100" t="s">
         <v>488</v>
       </c>
+      <c r="C100" t="s">
+        <v>556</v>
+      </c>
       <c r="D100" t="s">
-        <v>552</v>
+        <v>555</v>
       </c>
     </row>
     <row r="101" spans="1:4" x14ac:dyDescent="0.25">
@@ -14333,8 +14364,11 @@
       <c r="B101" t="s">
         <v>488</v>
       </c>
+      <c r="C101" t="s">
+        <v>556</v>
+      </c>
       <c r="D101" t="s">
-        <v>553</v>
+        <v>552</v>
       </c>
     </row>
     <row r="102" spans="1:4" x14ac:dyDescent="0.25">
@@ -14344,7 +14378,24 @@
       <c r="B102" t="s">
         <v>488</v>
       </c>
+      <c r="C102" t="s">
+        <v>89</v>
+      </c>
       <c r="D102" t="s">
+        <v>553</v>
+      </c>
+    </row>
+    <row r="103" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A103" t="s">
+        <v>487</v>
+      </c>
+      <c r="B103" t="s">
+        <v>488</v>
+      </c>
+      <c r="C103" t="s">
+        <v>89</v>
+      </c>
+      <c r="D103" t="s">
         <v>554</v>
       </c>
     </row>
@@ -17722,12 +17773,12 @@
   <sheetPr>
     <tabColor theme="9" tint="0.39997558519241921"/>
   </sheetPr>
-  <dimension ref="A1:W53"/>
+  <dimension ref="A1:W54"/>
   <sheetViews>
-    <sheetView topLeftCell="A2" zoomScale="80" zoomScaleNormal="80" workbookViewId="0">
+    <sheetView tabSelected="1" topLeftCell="E2" zoomScale="80" zoomScaleNormal="80" workbookViewId="0">
       <pane ySplit="1" topLeftCell="A13" activePane="bottomLeft" state="frozen"/>
       <selection activeCell="E2" sqref="E2"/>
-      <selection pane="bottomLeft" activeCell="O50" sqref="O50"/>
+      <selection pane="bottomLeft" activeCell="P50" sqref="P50"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -19854,6 +19905,12 @@
         <v>85</v>
       </c>
       <c r="O50" t="s">
+        <v>10</v>
+      </c>
+      <c r="P50" t="s">
+        <v>556</v>
+      </c>
+      <c r="Q50" t="s">
         <v>549</v>
       </c>
     </row>
@@ -19862,42 +19919,33 @@
         <v>487</v>
       </c>
       <c r="B51" t="s">
-        <v>489</v>
+        <v>488</v>
       </c>
       <c r="C51" t="s">
-        <v>489</v>
+        <v>488</v>
       </c>
       <c r="D51">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="E51" t="s">
-        <v>2</v>
+        <v>8</v>
       </c>
       <c r="F51" t="s">
         <v>494</v>
       </c>
       <c r="G51" t="s">
-        <v>489</v>
-      </c>
-      <c r="H51" t="s">
-        <v>518</v>
-      </c>
-      <c r="I51" t="s">
-        <v>497</v>
-      </c>
-      <c r="J51" t="s">
-        <v>517</v>
+        <v>488</v>
       </c>
     </row>
     <row r="52" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A52" t="s">
-        <v>492</v>
+        <v>487</v>
       </c>
       <c r="B52" t="s">
-        <v>491</v>
+        <v>489</v>
       </c>
       <c r="C52" t="s">
-        <v>491</v>
+        <v>489</v>
       </c>
       <c r="D52">
         <v>1</v>
@@ -19906,45 +19954,30 @@
         <v>2</v>
       </c>
       <c r="F52" t="s">
-        <v>496</v>
+        <v>494</v>
       </c>
       <c r="G52" t="s">
-        <v>27</v>
+        <v>489</v>
       </c>
       <c r="H52" t="s">
-        <v>3</v>
+        <v>518</v>
       </c>
       <c r="I52" t="s">
-        <v>28</v>
+        <v>497</v>
       </c>
       <c r="J52" t="s">
-        <v>104</v>
-      </c>
-      <c r="K52" t="s">
-        <v>483</v>
-      </c>
-      <c r="L52" t="s">
-        <v>119</v>
-      </c>
-      <c r="M52" t="s">
-        <v>121</v>
-      </c>
-      <c r="N52" t="s">
-        <v>4</v>
-      </c>
-      <c r="O52" t="s">
-        <v>155</v>
+        <v>517</v>
       </c>
     </row>
     <row r="53" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A53" t="s">
-        <v>486</v>
+        <v>492</v>
       </c>
       <c r="B53" t="s">
-        <v>546</v>
+        <v>491</v>
       </c>
       <c r="C53" t="s">
-        <v>546</v>
+        <v>491</v>
       </c>
       <c r="D53">
         <v>1</v>
@@ -19953,39 +19986,86 @@
         <v>2</v>
       </c>
       <c r="F53" t="s">
+        <v>496</v>
+      </c>
+      <c r="G53" t="s">
+        <v>27</v>
+      </c>
+      <c r="H53" t="s">
+        <v>3</v>
+      </c>
+      <c r="I53" t="s">
+        <v>28</v>
+      </c>
+      <c r="J53" t="s">
+        <v>104</v>
+      </c>
+      <c r="K53" t="s">
+        <v>483</v>
+      </c>
+      <c r="L53" t="s">
+        <v>119</v>
+      </c>
+      <c r="M53" t="s">
+        <v>121</v>
+      </c>
+      <c r="N53" t="s">
+        <v>4</v>
+      </c>
+      <c r="O53" t="s">
+        <v>155</v>
+      </c>
+    </row>
+    <row r="54" spans="1:17" x14ac:dyDescent="0.25">
+      <c r="A54" t="s">
+        <v>486</v>
+      </c>
+      <c r="B54" t="s">
+        <v>546</v>
+      </c>
+      <c r="C54" t="s">
+        <v>546</v>
+      </c>
+      <c r="D54">
+        <v>1</v>
+      </c>
+      <c r="E54" t="s">
+        <v>2</v>
+      </c>
+      <c r="F54" t="s">
         <v>49</v>
       </c>
-      <c r="G53" t="s">
+      <c r="G54" t="s">
         <v>546</v>
       </c>
-      <c r="H53" t="s">
+      <c r="H54" t="s">
         <v>11</v>
       </c>
-      <c r="I53" t="s">
+      <c r="I54" t="s">
         <v>5</v>
       </c>
-      <c r="J53" t="s">
+      <c r="J54" t="s">
         <v>4</v>
       </c>
-      <c r="K53" t="s">
+      <c r="K54" t="s">
         <v>81</v>
       </c>
-      <c r="L53" t="s">
+      <c r="L54" t="s">
         <v>83</v>
       </c>
-      <c r="M53" t="s">
+      <c r="M54" t="s">
         <v>85</v>
       </c>
-      <c r="N53" t="s">
+      <c r="N54" t="s">
         <v>89</v>
       </c>
-      <c r="O53" t="s">
+      <c r="O54" t="s">
         <v>10</v>
       </c>
-      <c r="P53" t="s">
+      <c r="P54" t="s">
         <v>547</v>
       </c>
-      <c r="Q53" t="s">
+      <c r="Q54" t="s">
         <v>3</v>
       </c>
     </row>

</xml_diff>

<commit_message>
changed order and made map_data = True
</commit_message>
<xml_diff>
--- a/config/master_config.xlsx
+++ b/config/master_config.xlsx
@@ -5,12 +5,12 @@
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\finbar.maunsell\github\9th_edition_visualisation\config\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\hyuga.kasai\Documents\Github\9th_Visualization\9th_edition_visualisation\config\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{45C1B057-EC74-460F-8E67-615DC7CC3C01}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{9AD3A407-ED00-4112-AE97-445F96A7663D}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" tabRatio="812" firstSheet="6" activeTab="11" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-6750" yWindow="-16320" windowWidth="29040" windowHeight="15840" tabRatio="812" firstSheet="6" activeTab="11" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="9th_EBT_schema" sheetId="7" r:id="rId1"/>
@@ -2123,7 +2123,7 @@
     <t>15_02_02_06_08_fuel_cell_ev</t>
   </si>
   <si>
-    <t>['Macro','Emissions', 'Generation capacity', 'FED by fuel', 'FED by sector', 'Industry', 'Transport', 'Buildings', 'Agriculture', 'Non-energy', 'Electricity', 'Oil use by sector', 'Electricity generation', 'Fuel consumption power sector', 'Refining', 'Hydrogen', 'Production', 'Supply', 'Coal', 'TPES Coal by type', 'Crude &amp; NGL', 'Renewable fuels', 'Transport stocks']</t>
+    <t>['Macro', 'FED by fuel', 'FED by sector', 'Industry', 'Transport', 'Buildings', 'Agriculture', 'Non-energy', 'Electricity', 'Oil use by sector', 'Electricity generation',  'Generation capacity', 'Fuel consumption power sector', 'Refining', 'Hydrogen', 'Production', 'Supply', 'Coal', 'TPES Coal by type', 'Crude &amp; NGL', 'Renewable fuels', 'Emissions', 'Transport stocks']</t>
   </si>
 </sst>
 </file>
@@ -6426,7 +6426,7 @@
   <dimension ref="A1:B7"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C14" sqref="C14"/>
+      <selection activeCell="B6" sqref="B6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -19055,7 +19055,7 @@
   <dimension ref="A1:W54"/>
   <sheetViews>
     <sheetView topLeftCell="E2" zoomScale="80" zoomScaleNormal="80" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A22" activePane="bottomLeft" state="frozen"/>
+      <pane ySplit="1" topLeftCell="A27" activePane="bottomLeft" state="frozen"/>
       <selection activeCell="E2" sqref="E2"/>
       <selection pane="bottomLeft" activeCell="G46" sqref="G46:N46"/>
     </sheetView>

</xml_diff>

<commit_message>
fixed issues with emissions and added emissions to tranformation
</commit_message>
<xml_diff>
--- a/config/master_config.xlsx
+++ b/config/master_config.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\finbar.maunsell\github\9th_edition_visualisation\config\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{45C1B057-EC74-460F-8E67-615DC7CC3C01}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{46287DCC-9837-4299-954D-EDF4296CB0FD}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" tabRatio="812" firstSheet="6" activeTab="11" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" tabRatio="812" firstSheet="1" activeTab="7" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="9th_EBT_schema" sheetId="7" r:id="rId1"/>
@@ -84,7 +84,7 @@
             <sz val="9"/>
             <color indexed="81"/>
             <rFont val="Tahoma"/>
-            <charset val="1"/>
+            <family val="2"/>
           </rPr>
           <t>Finbar Barton MAUNSELL:</t>
         </r>
@@ -93,7 +93,7 @@
             <sz val="9"/>
             <color indexed="81"/>
             <rFont val="Tahoma"/>
-            <charset val="1"/>
+            <family val="2"/>
           </rPr>
           <t xml:space="preserve">
 use capital to differentiate it. We need this because we need to select all 16_others and call them other renewables for power input.. At least as of octover 27</t>
@@ -142,7 +142,7 @@
             <sz val="9"/>
             <color indexed="81"/>
             <rFont val="Tahoma"/>
-            <charset val="1"/>
+            <family val="2"/>
           </rPr>
           <t>Finbar Maunsell:</t>
         </r>
@@ -151,7 +151,7 @@
             <sz val="9"/>
             <color indexed="81"/>
             <rFont val="Tahoma"/>
-            <charset val="1"/>
+            <family val="2"/>
           </rPr>
           <t xml:space="preserve">
 If input_fuel is TRUE, the vlaues will be negative, positive if output (FALSE).</t>
@@ -177,7 +177,7 @@
             <sz val="9"/>
             <color indexed="81"/>
             <rFont val="Tahoma"/>
-            <charset val="1"/>
+            <family val="2"/>
           </rPr>
           <t>Finbar Barton MAUNSELL:</t>
         </r>
@@ -186,7 +186,7 @@
             <sz val="9"/>
             <color indexed="81"/>
             <rFont val="Tahoma"/>
-            <charset val="1"/>
+            <family val="2"/>
           </rPr>
           <t xml:space="preserve">
 use capital to differentiate it. We need this because we need to select all 16_others and call them other renewables for power input.. At least as of octover 27</t>
@@ -253,7 +253,7 @@
             <sz val="9"/>
             <color indexed="81"/>
             <rFont val="Tahoma"/>
-            <charset val="1"/>
+            <family val="2"/>
           </rPr>
           <t>Finbar Maunsell:</t>
         </r>
@@ -262,7 +262,7 @@
             <sz val="9"/>
             <color indexed="81"/>
             <rFont val="Tahoma"/>
-            <charset val="1"/>
+            <family val="2"/>
           </rPr>
           <t xml:space="preserve">
 table should be used if you need/want a sepaarate table for this data. This will be needed if the data wouldn’t be available otherwise, OR if the chart is a bar chart in which case we will show it in 10 year splits, so a new table will be needed for that</t>
@@ -277,7 +277,7 @@
             <sz val="9"/>
             <color indexed="81"/>
             <rFont val="Tahoma"/>
-            <charset val="1"/>
+            <family val="2"/>
           </rPr>
           <t>Finbar Maunsell:</t>
         </r>
@@ -286,7 +286,7 @@
             <sz val="9"/>
             <color indexed="81"/>
             <rFont val="Tahoma"/>
-            <charset val="1"/>
+            <family val="2"/>
           </rPr>
           <t xml:space="preserve">
 These numbers are just placeholders, if you need more plotting names just extend the numbers to X+wahtever</t>
@@ -311,7 +311,7 @@
             <sz val="9"/>
             <color indexed="81"/>
             <rFont val="Tahoma"/>
-            <charset val="1"/>
+            <family val="2"/>
           </rPr>
           <t>Finbar Maunsell:</t>
         </r>
@@ -320,7 +320,7 @@
             <sz val="9"/>
             <color indexed="81"/>
             <rFont val="Tahoma"/>
-            <charset val="1"/>
+            <family val="2"/>
           </rPr>
           <t xml:space="preserve">
 table should be used if you need/want a sepaarate table for this data. This will be needed if the data wouldn’t be available otherwise, OR if the chart is a bar chart in which case we will show it in 10 year splits, so a new table will be needed for that</t>
@@ -345,7 +345,7 @@
             <sz val="9"/>
             <color indexed="81"/>
             <rFont val="Tahoma"/>
-            <charset val="1"/>
+            <family val="2"/>
           </rPr>
           <t>Finbar Maunsell:</t>
         </r>
@@ -354,7 +354,7 @@
             <sz val="9"/>
             <color indexed="81"/>
             <rFont val="Tahoma"/>
-            <charset val="1"/>
+            <family val="2"/>
           </rPr>
           <t xml:space="preserve">
 table should be used if you need/want a sepaarate table for this data. This will be needed if the data wouldn’t be available otherwise, OR if the chart is a bar chart in which case we will show it in 10 year splits, so a new table will be needed for that</t>
@@ -369,7 +369,7 @@
             <sz val="9"/>
             <color indexed="81"/>
             <rFont val="Tahoma"/>
-            <charset val="1"/>
+            <family val="2"/>
           </rPr>
           <t>Finbar Maunsell:</t>
         </r>
@@ -378,7 +378,7 @@
             <sz val="9"/>
             <color indexed="81"/>
             <rFont val="Tahoma"/>
-            <charset val="1"/>
+            <family val="2"/>
           </rPr>
           <t xml:space="preserve">
 These numbers are just placeholders, if you need more plotting names just extend the numbers to X+wahtever</t>
@@ -390,7 +390,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="4805" uniqueCount="578">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="4829" uniqueCount="580">
   <si>
     <t>chart_type</t>
   </si>
@@ -2124,13 +2124,19 @@
   </si>
   <si>
     <t>['Macro','Emissions', 'Generation capacity', 'FED by fuel', 'FED by sector', 'Industry', 'Transport', 'Buildings', 'Agriculture', 'Non-energy', 'Electricity', 'Oil use by sector', 'Electricity generation', 'Fuel consumption power sector', 'Refining', 'Hydrogen', 'Production', 'Supply', 'Coal', 'TPES Coal by type', 'Crude &amp; NGL', 'Renewable fuels', 'Transport stocks']</t>
+  </si>
+  <si>
+    <t>Emissions by sector</t>
+  </si>
+  <si>
+    <t>Emissions by fuel</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="10" x14ac:knownFonts="1">
+  <fonts count="8" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -2153,19 +2159,6 @@
       <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="9"/>
-      <color indexed="81"/>
-      <name val="Tahoma"/>
-      <charset val="1"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="9"/>
-      <color indexed="81"/>
-      <name val="Tahoma"/>
-      <charset val="1"/>
     </font>
     <font>
       <sz val="9"/>
@@ -2329,7 +2322,7 @@
   </borders>
   <cellStyleXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
-    <xf numFmtId="0" fontId="7" fillId="9" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="5" fillId="9" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
   <cellXfs count="20">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
@@ -2350,15 +2343,15 @@
     <xf numFmtId="0" fontId="1" fillId="6" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
     <xf numFmtId="0" fontId="1" fillId="7" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
     <xf numFmtId="0" fontId="0" fillId="8" borderId="0" xfId="0" applyFill="1"/>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" xfId="1" applyFont="1" applyFill="1"/>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="1" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="top"/>
     </xf>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="top"/>
     </xf>
-    <xf numFmtId="0" fontId="9" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
@@ -3459,8 +3452,8 @@
       </xdr:nvSpPr>
       <xdr:spPr>
         <a:xfrm>
-          <a:off x="6692900" y="2266950"/>
-          <a:ext cx="7267575" cy="2771775"/>
+          <a:off x="5267325" y="2343150"/>
+          <a:ext cx="7267575" cy="2867025"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
           <a:avLst/>
@@ -6425,8 +6418,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{8FD61665-6B06-460E-828D-1570B45BB2AE}">
   <dimension ref="A1:B7"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C14" sqref="C14"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="L21" sqref="L21"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -8121,8 +8114,8 @@
   </sheetPr>
   <dimension ref="A1:E54"/>
   <sheetViews>
-    <sheetView topLeftCell="A23" workbookViewId="0">
-      <selection activeCell="A55" sqref="A55"/>
+    <sheetView topLeftCell="A2" workbookViewId="0">
+      <selection activeCell="C42" sqref="C42"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -8882,8 +8875,8 @@
   </sheetPr>
   <dimension ref="A1:D232"/>
   <sheetViews>
-    <sheetView topLeftCell="A194" workbookViewId="0">
-      <selection activeCell="B220" sqref="B220"/>
+    <sheetView topLeftCell="A187" workbookViewId="0">
+      <selection activeCell="D208" sqref="D208"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -11530,7 +11523,7 @@
   <dimension ref="A1:D27"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="C27" sqref="C27"/>
+      <selection activeCell="D35" sqref="D35"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -15690,8 +15683,8 @@
   </sheetPr>
   <dimension ref="A1:D219"/>
   <sheetViews>
-    <sheetView topLeftCell="A7" workbookViewId="0">
-      <selection activeCell="B33" sqref="B33"/>
+    <sheetView topLeftCell="A34" workbookViewId="0">
+      <selection activeCell="I48" sqref="I48"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -18322,8 +18315,8 @@
   </sheetPr>
   <dimension ref="A1:E52"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="B1" sqref="B1"/>
+    <sheetView topLeftCell="A9" workbookViewId="0">
+      <selection activeCell="B53" sqref="B53"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -19052,16 +19045,17 @@
   <sheetPr>
     <tabColor theme="9" tint="0.39997558519241921"/>
   </sheetPr>
-  <dimension ref="A1:W54"/>
+  <dimension ref="A1:W55"/>
   <sheetViews>
-    <sheetView topLeftCell="E2" zoomScale="80" zoomScaleNormal="80" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A22" activePane="bottomLeft" state="frozen"/>
+    <sheetView tabSelected="1" topLeftCell="A2" zoomScale="80" zoomScaleNormal="80" workbookViewId="0">
+      <pane ySplit="1" topLeftCell="A18" activePane="bottomLeft" state="frozen"/>
       <selection activeCell="E2" sqref="E2"/>
-      <selection pane="bottomLeft" activeCell="G46" sqref="G46:N46"/>
+      <selection pane="bottomLeft" activeCell="F55" sqref="F55"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
+    <col min="1" max="1" width="17.5703125" customWidth="1"/>
     <col min="2" max="2" width="34.5703125" customWidth="1"/>
     <col min="3" max="3" width="25.140625" customWidth="1"/>
     <col min="4" max="7" width="25" customWidth="1"/>
@@ -21215,6 +21209,36 @@
       <c r="G51" t="s">
         <v>488</v>
       </c>
+      <c r="H51" t="s">
+        <v>11</v>
+      </c>
+      <c r="I51" t="s">
+        <v>5</v>
+      </c>
+      <c r="J51" t="s">
+        <v>4</v>
+      </c>
+      <c r="K51" t="s">
+        <v>79</v>
+      </c>
+      <c r="L51" t="s">
+        <v>81</v>
+      </c>
+      <c r="M51" t="s">
+        <v>89</v>
+      </c>
+      <c r="N51" t="s">
+        <v>85</v>
+      </c>
+      <c r="O51" t="s">
+        <v>10</v>
+      </c>
+      <c r="P51" t="s">
+        <v>555</v>
+      </c>
+      <c r="Q51" t="s">
+        <v>548</v>
+      </c>
     </row>
     <row r="52" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A52" t="s">
@@ -21262,7 +21286,7 @@
         <v>492</v>
       </c>
       <c r="B53" t="s">
-        <v>491</v>
+        <v>579</v>
       </c>
       <c r="C53" t="s">
         <v>491</v>
@@ -21280,25 +21304,25 @@
         <v>27</v>
       </c>
       <c r="H53" t="s">
+        <v>121</v>
+      </c>
+      <c r="I53" t="s">
+        <v>119</v>
+      </c>
+      <c r="J53" t="s">
+        <v>483</v>
+      </c>
+      <c r="K53" t="s">
+        <v>4</v>
+      </c>
+      <c r="L53" t="s">
+        <v>104</v>
+      </c>
+      <c r="M53" t="s">
+        <v>28</v>
+      </c>
+      <c r="N53" t="s">
         <v>3</v>
-      </c>
-      <c r="I53" t="s">
-        <v>28</v>
-      </c>
-      <c r="J53" t="s">
-        <v>104</v>
-      </c>
-      <c r="K53" t="s">
-        <v>483</v>
-      </c>
-      <c r="L53" t="s">
-        <v>119</v>
-      </c>
-      <c r="M53" t="s">
-        <v>121</v>
-      </c>
-      <c r="N53" t="s">
-        <v>4</v>
       </c>
       <c r="O53" t="s">
         <v>155</v>
@@ -21306,54 +21330,101 @@
     </row>
     <row r="54" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A54" t="s">
-        <v>486</v>
+        <v>492</v>
       </c>
       <c r="B54" t="s">
-        <v>546</v>
+        <v>578</v>
       </c>
       <c r="C54" t="s">
-        <v>546</v>
+        <v>491</v>
       </c>
       <c r="D54">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="E54" t="s">
         <v>2</v>
       </c>
       <c r="F54" t="s">
+        <v>495</v>
+      </c>
+      <c r="G54" t="s">
+        <v>153</v>
+      </c>
+      <c r="H54" t="s">
+        <v>459</v>
+      </c>
+      <c r="I54" t="s">
+        <v>25</v>
+      </c>
+      <c r="J54" t="s">
+        <v>31</v>
+      </c>
+      <c r="K54" t="s">
+        <v>1</v>
+      </c>
+      <c r="L54" t="s">
+        <v>9</v>
+      </c>
+      <c r="M54" t="s">
+        <v>27</v>
+      </c>
+      <c r="N54" t="s">
+        <v>24</v>
+      </c>
+      <c r="O54" t="s">
+        <v>153</v>
+      </c>
+    </row>
+    <row r="55" spans="1:17" x14ac:dyDescent="0.25">
+      <c r="A55" t="s">
+        <v>486</v>
+      </c>
+      <c r="B55" t="s">
+        <v>546</v>
+      </c>
+      <c r="C55" t="s">
+        <v>546</v>
+      </c>
+      <c r="D55">
+        <v>1</v>
+      </c>
+      <c r="E55" t="s">
+        <v>2</v>
+      </c>
+      <c r="F55" t="s">
         <v>49</v>
       </c>
-      <c r="G54" t="s">
+      <c r="G55" t="s">
         <v>546</v>
       </c>
-      <c r="H54" t="s">
+      <c r="H55" t="s">
         <v>11</v>
       </c>
-      <c r="I54" t="s">
+      <c r="I55" t="s">
         <v>5</v>
       </c>
-      <c r="J54" t="s">
+      <c r="J55" t="s">
         <v>4</v>
       </c>
-      <c r="K54" t="s">
+      <c r="K55" t="s">
         <v>81</v>
       </c>
-      <c r="L54" t="s">
+      <c r="L55" t="s">
         <v>83</v>
       </c>
-      <c r="M54" t="s">
+      <c r="M55" t="s">
         <v>85</v>
       </c>
-      <c r="N54" t="s">
+      <c r="N55" t="s">
         <v>89</v>
       </c>
-      <c r="O54" t="s">
+      <c r="O55" t="s">
         <v>10</v>
       </c>
-      <c r="P54" t="s">
+      <c r="P55" t="s">
         <v>547</v>
       </c>
-      <c r="Q54" t="s">
+      <c r="Q55" t="s">
         <v>3</v>
       </c>
     </row>

</xml_diff>

<commit_message>
generation capacity bar charts
</commit_message>
<xml_diff>
--- a/config/master_config.xlsx
+++ b/config/master_config.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\hyuga.kasai\Documents\Github\9th_Visualization\9th_edition_visualisation\config\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{9AD3A407-ED00-4112-AE97-445F96A7663D}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{CC790DB5-F0F7-4CF7-85A5-D60B1393C3D1}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-6750" yWindow="-16320" windowWidth="29040" windowHeight="15840" tabRatio="812" firstSheet="6" activeTab="11" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-6750" yWindow="-16320" windowWidth="29040" windowHeight="15840" tabRatio="812" firstSheet="2" activeTab="7" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="9th_EBT_schema" sheetId="7" r:id="rId1"/>
@@ -390,7 +390,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="4805" uniqueCount="578">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="4815" uniqueCount="578">
   <si>
     <t>chart_type</t>
   </si>
@@ -6425,7 +6425,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{8FD61665-6B06-460E-828D-1570B45BB2AE}">
   <dimension ref="A1:B7"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="B6" sqref="B6"/>
     </sheetView>
   </sheetViews>
@@ -19054,10 +19054,10 @@
   </sheetPr>
   <dimension ref="A1:W54"/>
   <sheetViews>
-    <sheetView topLeftCell="E2" zoomScale="80" zoomScaleNormal="80" workbookViewId="0">
+    <sheetView tabSelected="1" topLeftCell="E2" zoomScale="80" zoomScaleNormal="80" workbookViewId="0">
       <pane ySplit="1" topLeftCell="A27" activePane="bottomLeft" state="frozen"/>
       <selection activeCell="E2" sqref="E2"/>
-      <selection pane="bottomLeft" activeCell="G46" sqref="G46:N46"/>
+      <selection pane="bottomLeft" activeCell="H57" sqref="H57"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -21214,6 +21214,36 @@
       </c>
       <c r="G51" t="s">
         <v>488</v>
+      </c>
+      <c r="H51" t="s">
+        <v>11</v>
+      </c>
+      <c r="I51" t="s">
+        <v>5</v>
+      </c>
+      <c r="J51" t="s">
+        <v>4</v>
+      </c>
+      <c r="K51" t="s">
+        <v>79</v>
+      </c>
+      <c r="L51" t="s">
+        <v>81</v>
+      </c>
+      <c r="M51" t="s">
+        <v>89</v>
+      </c>
+      <c r="N51" t="s">
+        <v>85</v>
+      </c>
+      <c r="O51" t="s">
+        <v>10</v>
+      </c>
+      <c r="P51" t="s">
+        <v>555</v>
+      </c>
+      <c r="Q51" t="s">
+        <v>548</v>
       </c>
     </row>
     <row r="52" spans="1:17" x14ac:dyDescent="0.25">

</xml_diff>

<commit_message>
changed color of 'other fuel'
</commit_message>
<xml_diff>
--- a/config/master_config.xlsx
+++ b/config/master_config.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\hyuga.kasai\Documents\Github\9th_Visualization\9th_edition_visualisation\config\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B364CFC2-9EDE-4416-A7BF-96625085DEC5}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4B2778BA-4A31-4E3B-9AA8-5BA563D849B7}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-6750" yWindow="-16320" windowWidth="29040" windowHeight="15840" tabRatio="812" firstSheet="2" activeTab="7" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-6750" yWindow="-16320" windowWidth="29040" windowHeight="15840" tabRatio="812" firstSheet="2" activeTab="10" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="9th_EBT_schema" sheetId="7" r:id="rId1"/>
@@ -2337,7 +2337,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="7" fillId="9" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="21">
+  <cellXfs count="20">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="top"/>
@@ -2376,7 +2376,6 @@
     <xf numFmtId="0" fontId="2" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="top"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="Neutral" xfId="1" builtinId="28"/>
@@ -5616,8 +5615,8 @@
   </sheetPr>
   <dimension ref="A1:B99"/>
   <sheetViews>
-    <sheetView topLeftCell="A29" workbookViewId="0">
-      <selection activeCell="B44" sqref="B44"/>
+    <sheetView tabSelected="1" topLeftCell="A29" workbookViewId="0">
+      <selection activeCell="D42" sqref="D42"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -5950,7 +5949,7 @@
         <v>547</v>
       </c>
       <c r="B41" t="s">
-        <v>437</v>
+        <v>557</v>
       </c>
     </row>
     <row r="42" spans="1:2" x14ac:dyDescent="0.25">
@@ -19061,7 +19060,7 @@
   </sheetPr>
   <dimension ref="A1:W55"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A2" zoomScale="80" zoomScaleNormal="80" workbookViewId="0">
+    <sheetView topLeftCell="A2" zoomScale="80" zoomScaleNormal="80" workbookViewId="0">
       <pane ySplit="1" topLeftCell="A17" activePane="bottomLeft" state="frozen"/>
       <selection activeCell="E2" sqref="E2"/>
       <selection pane="bottomLeft" activeCell="C52" sqref="C52"/>
@@ -21342,53 +21341,51 @@
       </c>
     </row>
     <row r="54" spans="1:17" x14ac:dyDescent="0.25">
-      <c r="A54" s="20" t="s">
-        <v>492</v>
-      </c>
-      <c r="B54" s="20" t="s">
+      <c r="A54" t="s">
+        <v>492</v>
+      </c>
+      <c r="B54" t="s">
         <v>578</v>
       </c>
-      <c r="C54" s="20" t="s">
+      <c r="C54" t="s">
         <v>491</v>
       </c>
-      <c r="D54" s="20">
+      <c r="D54">
         <v>2</v>
       </c>
-      <c r="E54" s="20" t="s">
+      <c r="E54" t="s">
         <v>2</v>
       </c>
-      <c r="F54" s="20" t="s">
+      <c r="F54" t="s">
         <v>495</v>
       </c>
-      <c r="G54" s="20" t="s">
+      <c r="G54" t="s">
         <v>153</v>
       </c>
-      <c r="H54" s="20" t="s">
+      <c r="H54" t="s">
         <v>459</v>
       </c>
-      <c r="I54" s="20" t="s">
+      <c r="I54" t="s">
         <v>25</v>
       </c>
-      <c r="J54" s="20" t="s">
+      <c r="J54" t="s">
         <v>31</v>
       </c>
-      <c r="K54" s="20" t="s">
+      <c r="K54" t="s">
         <v>1</v>
       </c>
-      <c r="L54" s="20" t="s">
+      <c r="L54" t="s">
         <v>9</v>
       </c>
-      <c r="M54" s="20" t="s">
+      <c r="M54" t="s">
         <v>27</v>
       </c>
-      <c r="N54" s="20" t="s">
+      <c r="N54" t="s">
         <v>24</v>
       </c>
-      <c r="O54" s="20" t="s">
+      <c r="O54" t="s">
         <v>153</v>
       </c>
-      <c r="P54" s="20"/>
-      <c r="Q54" s="20"/>
     </row>
     <row r="55" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A55" t="s">

</xml_diff>

<commit_message>
change own use to positive values, changed GWh to TWh, added imports to electricity generations charts
</commit_message>
<xml_diff>
--- a/config/master_config.xlsx
+++ b/config/master_config.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\hyuga.kasai\Documents\Github\9th_Visualization\9th_edition_visualisation\config\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4B2778BA-4A31-4E3B-9AA8-5BA563D849B7}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{31D49311-C849-4ADB-8F2A-69D8A06F6DFC}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-6750" yWindow="-16320" windowWidth="29040" windowHeight="15840" tabRatio="812" firstSheet="2" activeTab="10" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-6750" yWindow="-16320" windowWidth="29040" windowHeight="15840" tabRatio="812" firstSheet="2" activeTab="7" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="9th_EBT_schema" sheetId="7" r:id="rId1"/>
@@ -29,7 +29,7 @@
     <sheet name="table_id_to_chart_old" sheetId="2" r:id="rId14"/>
   </sheets>
   <definedNames>
-    <definedName name="_xlnm._FilterDatabase" localSheetId="10" hidden="1">colors!$A$1:$B$99</definedName>
+    <definedName name="_xlnm._FilterDatabase" localSheetId="10" hidden="1">colors!$A$1:$B$100</definedName>
   </definedNames>
   <calcPr calcId="191029"/>
   <extLst>
@@ -390,7 +390,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="4829" uniqueCount="580">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="4839" uniqueCount="584">
   <si>
     <t>chart_type</t>
   </si>
@@ -1955,9 +1955,6 @@
     <t>Stocks (millions)</t>
   </si>
   <si>
-    <t>Gw</t>
-  </si>
-  <si>
     <t>macro</t>
   </si>
   <si>
@@ -2130,6 +2127,21 @@
   </si>
   <si>
     <t>Emissions by fuel</t>
+  </si>
+  <si>
+    <t>GW</t>
+  </si>
+  <si>
+    <t>TWh</t>
+  </si>
+  <si>
+    <t>19_imports</t>
+  </si>
+  <si>
+    <t>Electricity imports</t>
+  </si>
+  <si>
+    <t>#7C7C7C</t>
   </si>
 </sst>
 </file>
@@ -4574,7 +4586,7 @@
         <v>166</v>
       </c>
       <c r="F21" t="s">
-        <v>541</v>
+        <v>540</v>
       </c>
       <c r="G21" t="s">
         <v>291</v>
@@ -4959,7 +4971,7 @@
         <v>376</v>
       </c>
       <c r="G41" t="s">
-        <v>528</v>
+        <v>527</v>
       </c>
       <c r="H41" t="s">
         <v>377</v>
@@ -4976,7 +4988,7 @@
         <v>379</v>
       </c>
       <c r="G42" t="s">
-        <v>529</v>
+        <v>528</v>
       </c>
       <c r="H42" t="s">
         <v>380</v>
@@ -4987,7 +4999,7 @@
     </row>
     <row r="43" spans="4:9" x14ac:dyDescent="0.25">
       <c r="G43" t="s">
-        <v>530</v>
+        <v>529</v>
       </c>
       <c r="H43" t="s">
         <v>382</v>
@@ -4998,7 +5010,7 @@
     </row>
     <row r="44" spans="4:9" x14ac:dyDescent="0.25">
       <c r="G44" t="s">
-        <v>531</v>
+        <v>530</v>
       </c>
       <c r="H44" t="s">
         <v>384</v>
@@ -5009,7 +5021,7 @@
     </row>
     <row r="45" spans="4:9" x14ac:dyDescent="0.25">
       <c r="G45" t="s">
-        <v>532</v>
+        <v>531</v>
       </c>
       <c r="H45" t="s">
         <v>386</v>
@@ -5020,7 +5032,7 @@
     </row>
     <row r="46" spans="4:9" x14ac:dyDescent="0.25">
       <c r="G46" t="s">
-        <v>533</v>
+        <v>532</v>
       </c>
       <c r="H46" t="s">
         <v>388</v>
@@ -5031,7 +5043,7 @@
     </row>
     <row r="47" spans="4:9" x14ac:dyDescent="0.25">
       <c r="G47" t="s">
-        <v>534</v>
+        <v>533</v>
       </c>
       <c r="H47" t="s">
         <v>390</v>
@@ -5042,7 +5054,7 @@
     </row>
     <row r="48" spans="4:9" x14ac:dyDescent="0.25">
       <c r="G48" t="s">
-        <v>535</v>
+        <v>534</v>
       </c>
       <c r="H48" t="s">
         <v>392</v>
@@ -5053,7 +5065,7 @@
     </row>
     <row r="49" spans="7:9" x14ac:dyDescent="0.25">
       <c r="G49" t="s">
-        <v>536</v>
+        <v>535</v>
       </c>
       <c r="H49" t="s">
         <v>394</v>
@@ -5064,7 +5076,7 @@
     </row>
     <row r="50" spans="7:9" x14ac:dyDescent="0.25">
       <c r="G50" t="s">
-        <v>537</v>
+        <v>536</v>
       </c>
       <c r="H50" t="s">
         <v>396</v>
@@ -5075,7 +5087,7 @@
     </row>
     <row r="51" spans="7:9" x14ac:dyDescent="0.25">
       <c r="G51" t="s">
-        <v>538</v>
+        <v>537</v>
       </c>
       <c r="H51" t="s">
         <v>379</v>
@@ -5086,7 +5098,7 @@
     </row>
     <row r="52" spans="7:9" x14ac:dyDescent="0.25">
       <c r="G52" t="s">
-        <v>539</v>
+        <v>538</v>
       </c>
       <c r="I52" t="s">
         <v>379</v>
@@ -5099,7 +5111,7 @@
     </row>
     <row r="54" spans="7:9" x14ac:dyDescent="0.25">
       <c r="G54" t="s">
-        <v>540</v>
+        <v>539</v>
       </c>
     </row>
     <row r="55" spans="7:9" x14ac:dyDescent="0.25">
@@ -5350,10 +5362,10 @@
 
 <file path=xl/worksheets/sheet10.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{B968B52A-197D-4486-BE9F-20DC33AA9971}">
-  <dimension ref="A1:B30"/>
+  <dimension ref="A1:B31"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="H32" sqref="H32"/>
+    <sheetView topLeftCell="A3" workbookViewId="0">
+      <selection activeCell="B31" sqref="B31"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -5595,10 +5607,18 @@
     </row>
     <row r="30" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A30" t="s">
-        <v>545</v>
+        <v>544</v>
       </c>
       <c r="B30" t="s">
         <v>6</v>
+      </c>
+    </row>
+    <row r="31" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A31" t="s">
+        <v>582</v>
+      </c>
+      <c r="B31" t="s">
+        <v>19</v>
       </c>
     </row>
   </sheetData>
@@ -5613,10 +5633,10 @@
   <sheetPr>
     <tabColor rgb="FFFFC000"/>
   </sheetPr>
-  <dimension ref="A1:B99"/>
+  <dimension ref="A1:B100"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A29" workbookViewId="0">
-      <selection activeCell="D42" sqref="D42"/>
+    <sheetView topLeftCell="A61" workbookViewId="0">
+      <selection activeCell="E82" sqref="E82"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -5674,7 +5694,7 @@
     </row>
     <row r="7" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
-        <v>545</v>
+        <v>544</v>
       </c>
       <c r="B7" t="s">
         <v>432</v>
@@ -5738,10 +5758,10 @@
     </row>
     <row r="15" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A15" t="s">
+        <v>554</v>
+      </c>
+      <c r="B15" t="s">
         <v>555</v>
-      </c>
-      <c r="B15" t="s">
-        <v>556</v>
       </c>
     </row>
     <row r="16" spans="1:2" x14ac:dyDescent="0.25">
@@ -5946,10 +5966,10 @@
     </row>
     <row r="41" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A41" t="s">
-        <v>547</v>
+        <v>546</v>
       </c>
       <c r="B41" t="s">
-        <v>557</v>
+        <v>556</v>
       </c>
     </row>
     <row r="42" spans="1:2" x14ac:dyDescent="0.25">
@@ -5970,10 +5990,10 @@
     </row>
     <row r="44" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A44" t="s">
-        <v>548</v>
+        <v>547</v>
       </c>
       <c r="B44" t="s">
-        <v>557</v>
+        <v>556</v>
       </c>
     </row>
     <row r="45" spans="1:2" x14ac:dyDescent="0.25">
@@ -6274,15 +6294,15 @@
     </row>
     <row r="82" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A82" t="s">
-        <v>546</v>
+        <v>582</v>
       </c>
       <c r="B82" t="s">
-        <v>438</v>
+        <v>583</v>
       </c>
     </row>
     <row r="83" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A83" t="s">
-        <v>103</v>
+        <v>545</v>
       </c>
       <c r="B83" t="s">
         <v>438</v>
@@ -6290,7 +6310,7 @@
     </row>
     <row r="84" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A84" t="s">
-        <v>3</v>
+        <v>103</v>
       </c>
       <c r="B84" t="s">
         <v>438</v>
@@ -6298,23 +6318,23 @@
     </row>
     <row r="85" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A85" t="s">
-        <v>119</v>
+        <v>3</v>
       </c>
       <c r="B85" t="s">
-        <v>432</v>
+        <v>438</v>
       </c>
     </row>
     <row r="86" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A86" t="s">
-        <v>116</v>
+        <v>119</v>
       </c>
       <c r="B86" t="s">
-        <v>446</v>
+        <v>432</v>
       </c>
     </row>
     <row r="87" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A87" t="s">
-        <v>36</v>
+        <v>116</v>
       </c>
       <c r="B87" t="s">
         <v>446</v>
@@ -6322,7 +6342,7 @@
     </row>
     <row r="88" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A88" t="s">
-        <v>471</v>
+        <v>36</v>
       </c>
       <c r="B88" t="s">
         <v>446</v>
@@ -6330,7 +6350,7 @@
     </row>
     <row r="89" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A89" t="s">
-        <v>189</v>
+        <v>471</v>
       </c>
       <c r="B89" t="s">
         <v>446</v>
@@ -6338,88 +6358,96 @@
     </row>
     <row r="90" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A90" t="s">
-        <v>11</v>
+        <v>189</v>
       </c>
       <c r="B90" t="s">
-        <v>432</v>
+        <v>446</v>
       </c>
     </row>
     <row r="91" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A91" t="s">
-        <v>171</v>
+        <v>11</v>
       </c>
       <c r="B91" t="s">
-        <v>434</v>
+        <v>432</v>
       </c>
     </row>
     <row r="92" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A92" t="s">
-        <v>32</v>
+        <v>171</v>
       </c>
       <c r="B92" t="s">
-        <v>435</v>
+        <v>434</v>
       </c>
     </row>
     <row r="93" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A93" t="s">
-        <v>9</v>
+        <v>32</v>
       </c>
       <c r="B93" t="s">
-        <v>433</v>
+        <v>435</v>
       </c>
     </row>
     <row r="94" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A94" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="B94" t="s">
-        <v>436</v>
+        <v>433</v>
       </c>
     </row>
     <row r="95" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A95" t="s">
-        <v>136</v>
+        <v>10</v>
       </c>
       <c r="B95" t="s">
-        <v>440</v>
+        <v>436</v>
       </c>
     </row>
     <row r="96" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A96" t="s">
-        <v>104</v>
+        <v>136</v>
       </c>
       <c r="B96" t="s">
-        <v>436</v>
+        <v>440</v>
       </c>
     </row>
     <row r="97" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A97" t="s">
-        <v>39</v>
+        <v>104</v>
       </c>
       <c r="B97" t="s">
-        <v>443</v>
+        <v>436</v>
       </c>
     </row>
     <row r="98" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A98" t="s">
-        <v>168</v>
+        <v>39</v>
       </c>
       <c r="B98" t="s">
-        <v>433</v>
+        <v>443</v>
       </c>
     </row>
     <row r="99" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A99" t="s">
+        <v>168</v>
+      </c>
+      <c r="B99" t="s">
+        <v>433</v>
+      </c>
+    </row>
+    <row r="100" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A100" t="s">
         <v>1</v>
       </c>
-      <c r="B99" t="s">
+      <c r="B100" t="s">
         <v>434</v>
       </c>
     </row>
   </sheetData>
-  <autoFilter ref="A1:B99" xr:uid="{344218C0-5C74-48AB-A8DF-7C6AE2CA916D}">
-    <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="A2:B99">
-      <sortCondition descending="1" ref="A1:A99"/>
+  <autoFilter ref="A1:B100" xr:uid="{344218C0-5C74-48AB-A8DF-7C6AE2CA916D}">
+    <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="A2:B100">
+      <sortCondition descending="1" ref="A1:A100"/>
     </sortState>
   </autoFilter>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
@@ -6485,7 +6513,7 @@
         <v>478</v>
       </c>
       <c r="B6" t="s">
-        <v>577</v>
+        <v>576</v>
       </c>
     </row>
     <row r="7" spans="1:2" x14ac:dyDescent="0.25">
@@ -6505,10 +6533,10 @@
 
 <file path=xl/worksheets/sheet13.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{7A332D9E-E0E7-4510-94A6-3E3F9643D47A}">
-  <dimension ref="A1:B3"/>
+  <dimension ref="A1:B4"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="B1" sqref="B1"/>
+      <selection activeCell="A3" sqref="A3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -6534,7 +6562,15 @@
         <v>488</v>
       </c>
       <c r="B3" t="s">
-        <v>521</v>
+        <v>579</v>
+      </c>
+    </row>
+    <row r="4" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A4" t="s">
+        <v>545</v>
+      </c>
+      <c r="B4" t="s">
+        <v>580</v>
       </c>
     </row>
   </sheetData>
@@ -8128,7 +8164,7 @@
   <dimension ref="A1:E54"/>
   <sheetViews>
     <sheetView topLeftCell="A23" workbookViewId="0">
-      <selection activeCell="A55" sqref="A55"/>
+      <selection activeCell="A11" sqref="A11:XFD11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -8773,7 +8809,7 @@
         <v>486</v>
       </c>
       <c r="B46" t="s">
-        <v>545</v>
+        <v>544</v>
       </c>
       <c r="C46" t="s">
         <v>158</v>
@@ -8864,7 +8900,7 @@
         <v>486</v>
       </c>
       <c r="B54" t="s">
-        <v>546</v>
+        <v>545</v>
       </c>
       <c r="C54" t="s">
         <v>166</v>
@@ -8888,8 +8924,8 @@
   </sheetPr>
   <dimension ref="A1:D232"/>
   <sheetViews>
-    <sheetView topLeftCell="A194" workbookViewId="0">
-      <selection activeCell="B220" sqref="B220"/>
+    <sheetView topLeftCell="A193" workbookViewId="0">
+      <selection activeCell="B224" sqref="B224"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -11511,10 +11547,21 @@
         <v>486</v>
       </c>
       <c r="B220" t="s">
-        <v>547</v>
+        <v>546</v>
       </c>
       <c r="C220" t="s">
         <v>92</v>
+      </c>
+    </row>
+    <row r="221" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A221" t="s">
+        <v>486</v>
+      </c>
+      <c r="B221" t="s">
+        <v>582</v>
+      </c>
+      <c r="C221" t="s">
+        <v>581</v>
       </c>
     </row>
     <row r="232" spans="3:3" x14ac:dyDescent="0.25">
@@ -11536,7 +11583,7 @@
   <dimension ref="A1:D27"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="C27" sqref="C27"/>
+      <selection activeCell="C32" sqref="C32"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -14361,7 +14408,7 @@
         <v>85</v>
       </c>
       <c r="D96" t="s">
-        <v>549</v>
+        <v>548</v>
       </c>
     </row>
     <row r="97" spans="1:8" x14ac:dyDescent="0.25">
@@ -14372,10 +14419,10 @@
         <v>488</v>
       </c>
       <c r="C97" t="s">
-        <v>548</v>
+        <v>547</v>
       </c>
       <c r="D97" t="s">
-        <v>548</v>
+        <v>547</v>
       </c>
     </row>
     <row r="98" spans="1:8" x14ac:dyDescent="0.25">
@@ -14403,7 +14450,7 @@
         <v>10</v>
       </c>
       <c r="D99" t="s">
-        <v>550</v>
+        <v>549</v>
       </c>
     </row>
     <row r="100" spans="1:8" x14ac:dyDescent="0.25">
@@ -14414,10 +14461,10 @@
         <v>488</v>
       </c>
       <c r="C100" t="s">
-        <v>555</v>
+        <v>554</v>
       </c>
       <c r="D100" t="s">
-        <v>554</v>
+        <v>553</v>
       </c>
     </row>
     <row r="101" spans="1:8" x14ac:dyDescent="0.25">
@@ -14428,10 +14475,10 @@
         <v>488</v>
       </c>
       <c r="C101" t="s">
-        <v>555</v>
+        <v>554</v>
       </c>
       <c r="D101" t="s">
-        <v>551</v>
+        <v>550</v>
       </c>
     </row>
     <row r="102" spans="1:8" x14ac:dyDescent="0.25">
@@ -14445,7 +14492,7 @@
         <v>89</v>
       </c>
       <c r="D102" t="s">
-        <v>552</v>
+        <v>551</v>
       </c>
     </row>
     <row r="103" spans="1:8" x14ac:dyDescent="0.25">
@@ -14459,7 +14506,7 @@
         <v>89</v>
       </c>
       <c r="D103" t="s">
-        <v>553</v>
+        <v>552</v>
       </c>
     </row>
     <row r="104" spans="1:8" x14ac:dyDescent="0.25">
@@ -14470,7 +14517,7 @@
         <v>489</v>
       </c>
       <c r="C104" t="s">
-        <v>558</v>
+        <v>557</v>
       </c>
       <c r="D104" t="s">
         <v>158</v>
@@ -14496,7 +14543,7 @@
         <v>489</v>
       </c>
       <c r="C105" t="s">
-        <v>558</v>
+        <v>557</v>
       </c>
       <c r="D105" t="s">
         <v>158</v>
@@ -14522,7 +14569,7 @@
         <v>489</v>
       </c>
       <c r="C106" t="s">
-        <v>558</v>
+        <v>557</v>
       </c>
       <c r="D106" t="s">
         <v>158</v>
@@ -14548,7 +14595,7 @@
         <v>489</v>
       </c>
       <c r="C107" t="s">
-        <v>558</v>
+        <v>557</v>
       </c>
       <c r="D107" t="s">
         <v>158</v>
@@ -14574,7 +14621,7 @@
         <v>489</v>
       </c>
       <c r="C108" t="s">
-        <v>558</v>
+        <v>557</v>
       </c>
       <c r="D108" t="s">
         <v>158</v>
@@ -14600,7 +14647,7 @@
         <v>489</v>
       </c>
       <c r="C109" t="s">
-        <v>558</v>
+        <v>557</v>
       </c>
       <c r="D109" t="s">
         <v>158</v>
@@ -14626,7 +14673,7 @@
         <v>489</v>
       </c>
       <c r="C110" t="s">
-        <v>558</v>
+        <v>557</v>
       </c>
       <c r="D110" t="s">
         <v>158</v>
@@ -14652,7 +14699,7 @@
         <v>489</v>
       </c>
       <c r="C111" t="s">
-        <v>558</v>
+        <v>557</v>
       </c>
       <c r="D111" t="s">
         <v>158</v>
@@ -14678,7 +14725,7 @@
         <v>489</v>
       </c>
       <c r="C112" t="s">
-        <v>559</v>
+        <v>558</v>
       </c>
       <c r="D112" t="s">
         <v>158</v>
@@ -14704,7 +14751,7 @@
         <v>489</v>
       </c>
       <c r="C113" t="s">
-        <v>559</v>
+        <v>558</v>
       </c>
       <c r="D113" t="s">
         <v>158</v>
@@ -14730,7 +14777,7 @@
         <v>489</v>
       </c>
       <c r="C114" t="s">
-        <v>559</v>
+        <v>558</v>
       </c>
       <c r="D114" t="s">
         <v>158</v>
@@ -14756,7 +14803,7 @@
         <v>489</v>
       </c>
       <c r="C115" t="s">
-        <v>559</v>
+        <v>558</v>
       </c>
       <c r="D115" t="s">
         <v>158</v>
@@ -14782,7 +14829,7 @@
         <v>489</v>
       </c>
       <c r="C116" t="s">
-        <v>559</v>
+        <v>558</v>
       </c>
       <c r="D116" t="s">
         <v>158</v>
@@ -14808,7 +14855,7 @@
         <v>489</v>
       </c>
       <c r="C117" t="s">
-        <v>559</v>
+        <v>558</v>
       </c>
       <c r="D117" t="s">
         <v>158</v>
@@ -14834,7 +14881,7 @@
         <v>489</v>
       </c>
       <c r="C118" t="s">
-        <v>559</v>
+        <v>558</v>
       </c>
       <c r="D118" t="s">
         <v>158</v>
@@ -14860,7 +14907,7 @@
         <v>489</v>
       </c>
       <c r="C119" t="s">
-        <v>559</v>
+        <v>558</v>
       </c>
       <c r="D119" t="s">
         <v>158</v>
@@ -14886,7 +14933,7 @@
         <v>489</v>
       </c>
       <c r="C120" t="s">
-        <v>559</v>
+        <v>558</v>
       </c>
       <c r="D120" t="s">
         <v>158</v>
@@ -14912,7 +14959,7 @@
         <v>489</v>
       </c>
       <c r="C121" t="s">
-        <v>559</v>
+        <v>558</v>
       </c>
       <c r="D121" t="s">
         <v>158</v>
@@ -14938,7 +14985,7 @@
         <v>489</v>
       </c>
       <c r="C122" t="s">
-        <v>559</v>
+        <v>558</v>
       </c>
       <c r="D122" t="s">
         <v>158</v>
@@ -14964,7 +15011,7 @@
         <v>489</v>
       </c>
       <c r="C123" t="s">
-        <v>559</v>
+        <v>558</v>
       </c>
       <c r="D123" t="s">
         <v>158</v>
@@ -14990,7 +15037,7 @@
         <v>489</v>
       </c>
       <c r="C124" t="s">
-        <v>559</v>
+        <v>558</v>
       </c>
       <c r="D124" t="s">
         <v>158</v>
@@ -15016,7 +15063,7 @@
         <v>489</v>
       </c>
       <c r="C125" t="s">
-        <v>559</v>
+        <v>558</v>
       </c>
       <c r="D125" t="s">
         <v>158</v>
@@ -15042,7 +15089,7 @@
         <v>489</v>
       </c>
       <c r="C126" t="s">
-        <v>559</v>
+        <v>558</v>
       </c>
       <c r="D126" t="s">
         <v>158</v>
@@ -15068,7 +15115,7 @@
         <v>489</v>
       </c>
       <c r="C127" t="s">
-        <v>559</v>
+        <v>558</v>
       </c>
       <c r="D127" t="s">
         <v>158</v>
@@ -15094,7 +15141,7 @@
         <v>489</v>
       </c>
       <c r="C128" t="s">
-        <v>560</v>
+        <v>559</v>
       </c>
       <c r="D128" t="s">
         <v>158</v>
@@ -15109,7 +15156,7 @@
         <v>326</v>
       </c>
       <c r="H128" t="s">
-        <v>561</v>
+        <v>560</v>
       </c>
     </row>
     <row r="129" spans="1:8" x14ac:dyDescent="0.25">
@@ -15120,7 +15167,7 @@
         <v>489</v>
       </c>
       <c r="C129" t="s">
-        <v>560</v>
+        <v>559</v>
       </c>
       <c r="D129" t="s">
         <v>158</v>
@@ -15135,7 +15182,7 @@
         <v>498</v>
       </c>
       <c r="H129" t="s">
-        <v>562</v>
+        <v>561</v>
       </c>
     </row>
     <row r="130" spans="1:8" x14ac:dyDescent="0.25">
@@ -15146,7 +15193,7 @@
         <v>489</v>
       </c>
       <c r="C130" t="s">
-        <v>560</v>
+        <v>559</v>
       </c>
       <c r="D130" t="s">
         <v>158</v>
@@ -15161,7 +15208,7 @@
         <v>499</v>
       </c>
       <c r="H130" t="s">
-        <v>563</v>
+        <v>562</v>
       </c>
     </row>
     <row r="131" spans="1:8" x14ac:dyDescent="0.25">
@@ -15172,7 +15219,7 @@
         <v>489</v>
       </c>
       <c r="C131" t="s">
-        <v>560</v>
+        <v>559</v>
       </c>
       <c r="D131" t="s">
         <v>158</v>
@@ -15187,7 +15234,7 @@
         <v>500</v>
       </c>
       <c r="H131" t="s">
-        <v>564</v>
+        <v>563</v>
       </c>
     </row>
     <row r="132" spans="1:8" x14ac:dyDescent="0.25">
@@ -15198,7 +15245,7 @@
         <v>489</v>
       </c>
       <c r="C132" t="s">
-        <v>560</v>
+        <v>559</v>
       </c>
       <c r="D132" t="s">
         <v>158</v>
@@ -15213,7 +15260,7 @@
         <v>504</v>
       </c>
       <c r="H132" t="s">
-        <v>565</v>
+        <v>564</v>
       </c>
     </row>
     <row r="133" spans="1:8" x14ac:dyDescent="0.25">
@@ -15224,7 +15271,7 @@
         <v>489</v>
       </c>
       <c r="C133" t="s">
-        <v>560</v>
+        <v>559</v>
       </c>
       <c r="D133" t="s">
         <v>158</v>
@@ -15239,7 +15286,7 @@
         <v>505</v>
       </c>
       <c r="H133" t="s">
-        <v>566</v>
+        <v>565</v>
       </c>
     </row>
     <row r="134" spans="1:8" x14ac:dyDescent="0.25">
@@ -15250,7 +15297,7 @@
         <v>489</v>
       </c>
       <c r="C134" t="s">
-        <v>560</v>
+        <v>559</v>
       </c>
       <c r="D134" t="s">
         <v>158</v>
@@ -15265,7 +15312,7 @@
         <v>506</v>
       </c>
       <c r="H134" t="s">
-        <v>567</v>
+        <v>566</v>
       </c>
     </row>
     <row r="135" spans="1:8" x14ac:dyDescent="0.25">
@@ -15276,7 +15323,7 @@
         <v>489</v>
       </c>
       <c r="C135" t="s">
-        <v>560</v>
+        <v>559</v>
       </c>
       <c r="D135" t="s">
         <v>158</v>
@@ -15291,7 +15338,7 @@
         <v>354</v>
       </c>
       <c r="H135" t="s">
-        <v>568</v>
+        <v>567</v>
       </c>
     </row>
     <row r="136" spans="1:8" x14ac:dyDescent="0.25">
@@ -15499,7 +15546,7 @@
         <v>354</v>
       </c>
       <c r="H143" t="s">
-        <v>569</v>
+        <v>568</v>
       </c>
     </row>
     <row r="144" spans="1:8" x14ac:dyDescent="0.25">
@@ -15525,7 +15572,7 @@
         <v>354</v>
       </c>
       <c r="H144" t="s">
-        <v>570</v>
+        <v>569</v>
       </c>
     </row>
     <row r="145" spans="1:8" x14ac:dyDescent="0.25">
@@ -15551,7 +15598,7 @@
         <v>354</v>
       </c>
       <c r="H145" t="s">
-        <v>571</v>
+        <v>570</v>
       </c>
     </row>
     <row r="146" spans="1:8" x14ac:dyDescent="0.25">
@@ -15562,7 +15609,7 @@
         <v>489</v>
       </c>
       <c r="C146" t="s">
-        <v>558</v>
+        <v>557</v>
       </c>
       <c r="D146" t="s">
         <v>158</v>
@@ -15577,7 +15624,7 @@
         <v>354</v>
       </c>
       <c r="H146" t="s">
-        <v>572</v>
+        <v>571</v>
       </c>
     </row>
     <row r="147" spans="1:8" x14ac:dyDescent="0.25">
@@ -15588,7 +15635,7 @@
         <v>489</v>
       </c>
       <c r="C147" t="s">
-        <v>559</v>
+        <v>558</v>
       </c>
       <c r="D147" t="s">
         <v>158</v>
@@ -15603,7 +15650,7 @@
         <v>354</v>
       </c>
       <c r="H147" t="s">
-        <v>573</v>
+        <v>572</v>
       </c>
     </row>
     <row r="148" spans="1:8" x14ac:dyDescent="0.25">
@@ -15614,7 +15661,7 @@
         <v>489</v>
       </c>
       <c r="C148" t="s">
-        <v>559</v>
+        <v>558</v>
       </c>
       <c r="D148" t="s">
         <v>158</v>
@@ -15629,7 +15676,7 @@
         <v>354</v>
       </c>
       <c r="H148" t="s">
-        <v>574</v>
+        <v>573</v>
       </c>
     </row>
     <row r="149" spans="1:8" x14ac:dyDescent="0.25">
@@ -15640,7 +15687,7 @@
         <v>489</v>
       </c>
       <c r="C149" t="s">
-        <v>560</v>
+        <v>559</v>
       </c>
       <c r="D149" t="s">
         <v>158</v>
@@ -15655,7 +15702,7 @@
         <v>354</v>
       </c>
       <c r="H149" t="s">
-        <v>575</v>
+        <v>574</v>
       </c>
     </row>
     <row r="150" spans="1:8" x14ac:dyDescent="0.25">
@@ -15681,7 +15728,7 @@
         <v>354</v>
       </c>
       <c r="H150" t="s">
-        <v>576</v>
+        <v>575</v>
       </c>
     </row>
   </sheetData>
@@ -19060,10 +19107,10 @@
   </sheetPr>
   <dimension ref="A1:W55"/>
   <sheetViews>
-    <sheetView topLeftCell="A2" zoomScale="80" zoomScaleNormal="80" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A17" activePane="bottomLeft" state="frozen"/>
+    <sheetView tabSelected="1" topLeftCell="E2" zoomScale="80" zoomScaleNormal="80" workbookViewId="0">
+      <pane ySplit="1" topLeftCell="A19" activePane="bottomLeft" state="frozen"/>
       <selection activeCell="E2" sqref="E2"/>
-      <selection pane="bottomLeft" activeCell="C52" sqref="C52"/>
+      <selection pane="bottomLeft" activeCell="R55" sqref="R55"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -19108,7 +19155,7 @@
         <v>485</v>
       </c>
       <c r="B2" s="1" t="s">
-        <v>526</v>
+        <v>525</v>
       </c>
       <c r="C2" s="1" t="s">
         <v>463</v>
@@ -20970,7 +21017,7 @@
         <v>41</v>
       </c>
       <c r="M45" s="12" t="s">
-        <v>545</v>
+        <v>544</v>
       </c>
     </row>
     <row r="46" spans="1:18" x14ac:dyDescent="0.25">
@@ -21011,7 +21058,7 @@
         <v>41</v>
       </c>
       <c r="M46" s="12" t="s">
-        <v>545</v>
+        <v>544</v>
       </c>
     </row>
     <row r="47" spans="1:18" x14ac:dyDescent="0.25">
@@ -21102,7 +21149,7 @@
         <v>155</v>
       </c>
     </row>
-    <row r="49" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="49" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A49" t="s">
         <v>486</v>
       </c>
@@ -21146,7 +21193,7 @@
         <v>155</v>
       </c>
     </row>
-    <row r="50" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="50" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A50" t="s">
         <v>487</v>
       </c>
@@ -21193,13 +21240,13 @@
         <v>10</v>
       </c>
       <c r="P50" t="s">
-        <v>555</v>
+        <v>554</v>
       </c>
       <c r="Q50" t="s">
-        <v>548</v>
-      </c>
-    </row>
-    <row r="51" spans="1:17" x14ac:dyDescent="0.25">
+        <v>547</v>
+      </c>
+    </row>
+    <row r="51" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A51" t="s">
         <v>487</v>
       </c>
@@ -21246,13 +21293,13 @@
         <v>10</v>
       </c>
       <c r="P51" t="s">
-        <v>555</v>
+        <v>554</v>
       </c>
       <c r="Q51" t="s">
-        <v>548</v>
-      </c>
-    </row>
-    <row r="52" spans="1:17" x14ac:dyDescent="0.25">
+        <v>547</v>
+      </c>
+    </row>
+    <row r="52" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A52" t="s">
         <v>487</v>
       </c>
@@ -21284,21 +21331,21 @@
         <v>517</v>
       </c>
       <c r="K52" t="s">
+        <v>558</v>
+      </c>
+      <c r="L52" t="s">
         <v>559</v>
       </c>
-      <c r="L52" t="s">
-        <v>560</v>
-      </c>
       <c r="M52" t="s">
-        <v>558</v>
-      </c>
-    </row>
-    <row r="53" spans="1:17" x14ac:dyDescent="0.25">
+        <v>557</v>
+      </c>
+    </row>
+    <row r="53" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A53" t="s">
         <v>492</v>
       </c>
       <c r="B53" t="s">
-        <v>579</v>
+        <v>578</v>
       </c>
       <c r="C53" t="s">
         <v>491</v>
@@ -21340,12 +21387,12 @@
         <v>155</v>
       </c>
     </row>
-    <row r="54" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="54" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A54" t="s">
         <v>492</v>
       </c>
       <c r="B54" t="s">
-        <v>578</v>
+        <v>577</v>
       </c>
       <c r="C54" t="s">
         <v>491</v>
@@ -21387,15 +21434,15 @@
         <v>153</v>
       </c>
     </row>
-    <row r="55" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="55" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A55" t="s">
         <v>486</v>
       </c>
       <c r="B55" t="s">
-        <v>546</v>
+        <v>545</v>
       </c>
       <c r="C55" t="s">
-        <v>546</v>
+        <v>545</v>
       </c>
       <c r="D55">
         <v>1</v>
@@ -21407,7 +21454,7 @@
         <v>49</v>
       </c>
       <c r="G55" t="s">
-        <v>546</v>
+        <v>545</v>
       </c>
       <c r="H55" t="s">
         <v>11</v>
@@ -21434,10 +21481,13 @@
         <v>10</v>
       </c>
       <c r="P55" t="s">
-        <v>547</v>
+        <v>546</v>
       </c>
       <c r="Q55" t="s">
         <v>3</v>
+      </c>
+      <c r="R55" t="s">
+        <v>582</v>
       </c>
     </row>
   </sheetData>
@@ -21487,15 +21537,15 @@
         <v>452</v>
       </c>
       <c r="F1" s="15" t="s">
-        <v>526</v>
+        <v>525</v>
       </c>
     </row>
     <row r="2" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
-        <v>522</v>
+        <v>521</v>
       </c>
       <c r="B2" t="s">
-        <v>542</v>
+        <v>541</v>
       </c>
       <c r="C2">
         <v>1</v>
@@ -21504,18 +21554,18 @@
         <v>7</v>
       </c>
       <c r="E2" t="s">
-        <v>523</v>
+        <v>522</v>
       </c>
       <c r="F2" t="s">
-        <v>543</v>
+        <v>542</v>
       </c>
     </row>
     <row r="3" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
-        <v>522</v>
+        <v>521</v>
       </c>
       <c r="B3" t="s">
-        <v>542</v>
+        <v>541</v>
       </c>
       <c r="C3">
         <v>2</v>
@@ -21524,18 +21574,18 @@
         <v>7</v>
       </c>
       <c r="E3" t="s">
-        <v>524</v>
+        <v>523</v>
       </c>
       <c r="F3" t="s">
-        <v>544</v>
+        <v>543</v>
       </c>
     </row>
     <row r="4" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
-        <v>522</v>
+        <v>521</v>
       </c>
       <c r="B4" t="s">
-        <v>542</v>
+        <v>541</v>
       </c>
       <c r="C4">
         <v>3</v>
@@ -21544,10 +21594,10 @@
         <v>7</v>
       </c>
       <c r="E4" t="s">
-        <v>525</v>
+        <v>524</v>
       </c>
       <c r="F4" t="s">
-        <v>527</v>
+        <v>526</v>
       </c>
     </row>
     <row r="8" spans="1:6" x14ac:dyDescent="0.25">

</xml_diff>

<commit_message>
added gas ccs to the charts
</commit_message>
<xml_diff>
--- a/config/master_config.xlsx
+++ b/config/master_config.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\hyuga.kasai\Documents\Github\9th_Visualization\9th_edition_visualisation\config\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E7ADED9A-C90A-4B6F-922F-3022D2F4C077}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{30AB4862-2FAB-409A-9ABF-EFA4B98D1C77}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-6750" yWindow="-16320" windowWidth="29040" windowHeight="15840" tabRatio="812" firstSheet="1" activeTab="7" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-6750" yWindow="-16320" windowWidth="29040" windowHeight="15840" tabRatio="812" firstSheet="2" activeTab="10" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="9th_EBT_schema" sheetId="7" r:id="rId1"/>
@@ -29,7 +29,7 @@
     <sheet name="table_id_to_chart_old" sheetId="2" r:id="rId14"/>
   </sheets>
   <definedNames>
-    <definedName name="_xlnm._FilterDatabase" localSheetId="10" hidden="1">colors!$A$1:$B$104</definedName>
+    <definedName name="_xlnm._FilterDatabase" localSheetId="10" hidden="1">colors!$A$1:$B$106</definedName>
   </definedNames>
   <calcPr calcId="191029"/>
   <extLst>
@@ -390,7 +390,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="4430" uniqueCount="596">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="4435" uniqueCount="599">
   <si>
     <t>chart_type</t>
   </si>
@@ -2144,15 +2144,9 @@
     <t>#7C7C7C</t>
   </si>
   <si>
-    <t>Gas ccs new</t>
-  </si>
-  <si>
     <t>Gas CCS</t>
   </si>
   <si>
-    <t>#E8E8E8</t>
-  </si>
-  <si>
     <t>15_02_01_05_04_compressed_natual_gas</t>
   </si>
   <si>
@@ -2171,13 +2165,28 @@
     <t>Gas_ccs</t>
   </si>
   <si>
-    <t>18_01_02_gas_power_ccs</t>
-  </si>
-  <si>
     <t>Total_industry</t>
   </si>
   <si>
     <t>#323231</t>
+  </si>
+  <si>
+    <t>08_gas_ccs</t>
+  </si>
+  <si>
+    <t>Batteries</t>
+  </si>
+  <si>
+    <t>Pumped hydro</t>
+  </si>
+  <si>
+    <t>#C8DBEC</t>
+  </si>
+  <si>
+    <t>Gas ccs</t>
+  </si>
+  <si>
+    <t>#86539B</t>
   </si>
 </sst>
 </file>
@@ -2427,6 +2436,7 @@
     <xf numFmtId="0" fontId="9" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="top"/>
     </xf>
@@ -2436,7 +2446,6 @@
     <xf numFmtId="0" fontId="2" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="top"/>
     </xf>
-    <xf numFmtId="0" fontId="10" fillId="0" borderId="0" xfId="0" applyFont="1"/>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="Neutral" xfId="1" builtinId="28"/>
@@ -5413,7 +5422,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{B968B52A-197D-4486-BE9F-20DC33AA9971}">
   <dimension ref="A1:B35"/>
   <sheetViews>
-    <sheetView topLeftCell="A3" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="A36" sqref="A36"/>
     </sheetView>
   </sheetViews>
@@ -5672,7 +5681,7 @@
     </row>
     <row r="32" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A32" t="s">
-        <v>591</v>
+        <v>589</v>
       </c>
       <c r="B32" t="s">
         <v>4</v>
@@ -5680,15 +5689,15 @@
     </row>
     <row r="33" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A33" t="s">
-        <v>592</v>
+        <v>590</v>
       </c>
       <c r="B33" t="s">
-        <v>585</v>
+        <v>584</v>
       </c>
     </row>
     <row r="34" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A34" t="s">
-        <v>594</v>
+        <v>591</v>
       </c>
       <c r="B34" t="s">
         <v>6</v>
@@ -5714,10 +5723,10 @@
   <sheetPr>
     <tabColor rgb="FFFFC000"/>
   </sheetPr>
-  <dimension ref="A1:B104"/>
+  <dimension ref="A1:B106"/>
   <sheetViews>
-    <sheetView topLeftCell="A33" workbookViewId="0">
-      <selection activeCell="D82" sqref="D82"/>
+    <sheetView tabSelected="1" topLeftCell="A81" workbookViewId="0">
+      <selection activeCell="B103" sqref="B103"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -5786,12 +5795,12 @@
         <v>466</v>
       </c>
       <c r="B8" t="s">
-        <v>595</v>
+        <v>592</v>
       </c>
     </row>
     <row r="9" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A9" t="s">
-        <v>594</v>
+        <v>591</v>
       </c>
       <c r="B9" t="s">
         <v>432</v>
@@ -5951,31 +5960,31 @@
     </row>
     <row r="29" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A29" t="s">
-        <v>179</v>
+        <v>595</v>
       </c>
       <c r="B29" t="s">
-        <v>437</v>
+        <v>596</v>
       </c>
     </row>
     <row r="30" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A30" t="s">
-        <v>20</v>
+        <v>179</v>
       </c>
       <c r="B30" t="s">
-        <v>442</v>
+        <v>437</v>
       </c>
     </row>
     <row r="31" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A31" t="s">
-        <v>456</v>
+        <v>20</v>
       </c>
       <c r="B31" t="s">
-        <v>440</v>
+        <v>442</v>
       </c>
     </row>
     <row r="32" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A32" t="s">
-        <v>459</v>
+        <v>456</v>
       </c>
       <c r="B32" t="s">
         <v>440</v>
@@ -5983,7 +5992,7 @@
     </row>
     <row r="33" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A33" t="s">
-        <v>52</v>
+        <v>459</v>
       </c>
       <c r="B33" t="s">
         <v>440</v>
@@ -5991,39 +6000,39 @@
     </row>
     <row r="34" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A34" t="s">
-        <v>41</v>
+        <v>52</v>
       </c>
       <c r="B34" t="s">
-        <v>444</v>
+        <v>440</v>
       </c>
     </row>
     <row r="35" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A35" t="s">
-        <v>198</v>
+        <v>41</v>
       </c>
       <c r="B35" t="s">
-        <v>445</v>
+        <v>444</v>
       </c>
     </row>
     <row r="36" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A36" t="s">
-        <v>26</v>
+        <v>198</v>
       </c>
       <c r="B36" t="s">
-        <v>438</v>
+        <v>445</v>
       </c>
     </row>
     <row r="37" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A37" t="s">
-        <v>29</v>
+        <v>26</v>
       </c>
       <c r="B37" t="s">
-        <v>440</v>
+        <v>438</v>
       </c>
     </row>
     <row r="38" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A38" t="s">
-        <v>181</v>
+        <v>29</v>
       </c>
       <c r="B38" t="s">
         <v>440</v>
@@ -6031,15 +6040,15 @@
     </row>
     <row r="39" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A39" t="s">
-        <v>12</v>
+        <v>181</v>
       </c>
       <c r="B39" t="s">
-        <v>435</v>
+        <v>440</v>
       </c>
     </row>
     <row r="40" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A40" t="s">
-        <v>480</v>
+        <v>12</v>
       </c>
       <c r="B40" t="s">
         <v>435</v>
@@ -6047,31 +6056,31 @@
     </row>
     <row r="41" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A41" t="s">
-        <v>476</v>
+        <v>480</v>
       </c>
       <c r="B41" t="s">
-        <v>437</v>
+        <v>435</v>
       </c>
     </row>
     <row r="42" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A42" t="s">
-        <v>546</v>
+        <v>476</v>
       </c>
       <c r="B42" t="s">
-        <v>556</v>
+        <v>437</v>
       </c>
     </row>
     <row r="43" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A43" t="s">
-        <v>473</v>
+        <v>546</v>
       </c>
       <c r="B43" t="s">
-        <v>437</v>
+        <v>556</v>
       </c>
     </row>
     <row r="44" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A44" t="s">
-        <v>483</v>
+        <v>473</v>
       </c>
       <c r="B44" t="s">
         <v>437</v>
@@ -6079,47 +6088,47 @@
     </row>
     <row r="45" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A45" t="s">
-        <v>547</v>
+        <v>483</v>
       </c>
       <c r="B45" t="s">
-        <v>556</v>
+        <v>437</v>
       </c>
     </row>
     <row r="46" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A46" t="s">
-        <v>5</v>
+        <v>547</v>
       </c>
       <c r="B46" t="s">
-        <v>433</v>
+        <v>556</v>
       </c>
     </row>
     <row r="47" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A47" t="s">
-        <v>87</v>
+        <v>5</v>
       </c>
       <c r="B47" t="s">
-        <v>442</v>
+        <v>433</v>
       </c>
     </row>
     <row r="48" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A48" t="s">
-        <v>79</v>
+        <v>87</v>
       </c>
       <c r="B48" t="s">
-        <v>444</v>
+        <v>442</v>
       </c>
     </row>
     <row r="49" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A49" t="s">
-        <v>200</v>
+        <v>79</v>
       </c>
       <c r="B49" t="s">
-        <v>438</v>
+        <v>444</v>
       </c>
     </row>
     <row r="50" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A50" t="s">
-        <v>187</v>
+        <v>200</v>
       </c>
       <c r="B50" t="s">
         <v>438</v>
@@ -6127,39 +6136,39 @@
     </row>
     <row r="51" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A51" t="s">
-        <v>25</v>
+        <v>187</v>
       </c>
       <c r="B51" t="s">
-        <v>443</v>
+        <v>438</v>
       </c>
     </row>
     <row r="52" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A52" t="s">
-        <v>177</v>
+        <v>25</v>
       </c>
       <c r="B52" t="s">
-        <v>432</v>
+        <v>443</v>
       </c>
     </row>
     <row r="53" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A53" t="s">
-        <v>31</v>
+        <v>177</v>
       </c>
       <c r="B53" t="s">
-        <v>435</v>
+        <v>432</v>
       </c>
     </row>
     <row r="54" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A54" t="s">
-        <v>102</v>
+        <v>31</v>
       </c>
       <c r="B54" t="s">
-        <v>434</v>
+        <v>435</v>
       </c>
     </row>
     <row r="55" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A55" t="s">
-        <v>472</v>
+        <v>102</v>
       </c>
       <c r="B55" t="s">
         <v>434</v>
@@ -6167,7 +6176,7 @@
     </row>
     <row r="56" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A56" t="s">
-        <v>35</v>
+        <v>472</v>
       </c>
       <c r="B56" t="s">
         <v>434</v>
@@ -6175,31 +6184,31 @@
     </row>
     <row r="57" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A57" t="s">
-        <v>474</v>
+        <v>35</v>
       </c>
       <c r="B57" t="s">
-        <v>477</v>
+        <v>434</v>
       </c>
     </row>
     <row r="58" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A58" t="s">
-        <v>100</v>
+        <v>474</v>
       </c>
       <c r="B58" t="s">
-        <v>437</v>
+        <v>477</v>
       </c>
     </row>
     <row r="59" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A59" t="s">
-        <v>175</v>
+        <v>100</v>
       </c>
       <c r="B59" t="s">
-        <v>435</v>
+        <v>437</v>
       </c>
     </row>
     <row r="60" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A60" t="s">
-        <v>16</v>
+        <v>175</v>
       </c>
       <c r="B60" t="s">
         <v>435</v>
@@ -6207,7 +6216,7 @@
     </row>
     <row r="61" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A61" t="s">
-        <v>40</v>
+        <v>16</v>
       </c>
       <c r="B61" t="s">
         <v>435</v>
@@ -6215,63 +6224,63 @@
     </row>
     <row r="62" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A62" t="s">
-        <v>123</v>
+        <v>40</v>
       </c>
       <c r="B62" t="s">
-        <v>444</v>
+        <v>435</v>
       </c>
     </row>
     <row r="63" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A63" t="s">
-        <v>137</v>
+        <v>123</v>
       </c>
       <c r="B63" t="s">
-        <v>436</v>
+        <v>444</v>
       </c>
     </row>
     <row r="64" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A64" t="s">
-        <v>15</v>
+        <v>137</v>
       </c>
       <c r="B64" t="s">
-        <v>446</v>
+        <v>436</v>
       </c>
     </row>
     <row r="65" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A65" t="s">
-        <v>475</v>
+        <v>15</v>
       </c>
       <c r="B65" t="s">
-        <v>440</v>
+        <v>446</v>
       </c>
     </row>
     <row r="66" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A66" t="s">
-        <v>126</v>
+        <v>475</v>
       </c>
       <c r="B66" t="s">
-        <v>433</v>
+        <v>440</v>
       </c>
     </row>
     <row r="67" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A67" t="s">
-        <v>173</v>
+        <v>126</v>
       </c>
       <c r="B67" t="s">
-        <v>442</v>
+        <v>433</v>
       </c>
     </row>
     <row r="68" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A68" t="s">
-        <v>24</v>
+        <v>173</v>
       </c>
       <c r="B68" t="s">
-        <v>441</v>
+        <v>442</v>
       </c>
     </row>
     <row r="69" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A69" t="s">
-        <v>19</v>
+        <v>24</v>
       </c>
       <c r="B69" t="s">
         <v>441</v>
@@ -6279,15 +6288,15 @@
     </row>
     <row r="70" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A70" t="s">
-        <v>458</v>
+        <v>19</v>
       </c>
       <c r="B70" t="s">
-        <v>479</v>
+        <v>441</v>
       </c>
     </row>
     <row r="71" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A71" t="s">
-        <v>461</v>
+        <v>458</v>
       </c>
       <c r="B71" t="s">
         <v>479</v>
@@ -6295,7 +6304,7 @@
     </row>
     <row r="72" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A72" t="s">
-        <v>28</v>
+        <v>461</v>
       </c>
       <c r="B72" t="s">
         <v>479</v>
@@ -6303,23 +6312,23 @@
     </row>
     <row r="73" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A73" t="s">
-        <v>81</v>
+        <v>28</v>
       </c>
       <c r="B73" t="s">
-        <v>445</v>
+        <v>479</v>
       </c>
     </row>
     <row r="74" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A74" t="s">
-        <v>167</v>
+        <v>81</v>
       </c>
       <c r="B74" t="s">
-        <v>439</v>
+        <v>445</v>
       </c>
     </row>
     <row r="75" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A75" t="s">
-        <v>95</v>
+        <v>167</v>
       </c>
       <c r="B75" t="s">
         <v>439</v>
@@ -6327,31 +6336,31 @@
     </row>
     <row r="76" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A76" t="s">
-        <v>83</v>
+        <v>95</v>
       </c>
       <c r="B76" t="s">
-        <v>442</v>
+        <v>439</v>
       </c>
     </row>
     <row r="77" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A77" t="s">
-        <v>121</v>
+        <v>83</v>
       </c>
       <c r="B77" t="s">
-        <v>443</v>
+        <v>442</v>
       </c>
     </row>
     <row r="78" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A78" t="s">
-        <v>591</v>
+        <v>121</v>
       </c>
       <c r="B78" t="s">
-        <v>586</v>
+        <v>443</v>
       </c>
     </row>
     <row r="79" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A79" t="s">
-        <v>592</v>
+        <v>589</v>
       </c>
       <c r="B79" t="s">
         <v>434</v>
@@ -6359,15 +6368,15 @@
     </row>
     <row r="80" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A80" t="s">
-        <v>585</v>
+        <v>590</v>
       </c>
       <c r="B80" t="s">
-        <v>586</v>
+        <v>434</v>
       </c>
     </row>
     <row r="81" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A81" t="s">
-        <v>4</v>
+        <v>584</v>
       </c>
       <c r="B81" t="s">
         <v>434</v>
@@ -6375,15 +6384,15 @@
     </row>
     <row r="82" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A82" t="s">
-        <v>135</v>
+        <v>4</v>
       </c>
       <c r="B82" t="s">
-        <v>443</v>
+        <v>434</v>
       </c>
     </row>
     <row r="83" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A83" t="s">
-        <v>195</v>
+        <v>135</v>
       </c>
       <c r="B83" t="s">
         <v>443</v>
@@ -6391,7 +6400,7 @@
     </row>
     <row r="84" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A84" t="s">
-        <v>18</v>
+        <v>195</v>
       </c>
       <c r="B84" t="s">
         <v>443</v>
@@ -6399,31 +6408,31 @@
     </row>
     <row r="85" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A85" t="s">
-        <v>165</v>
+        <v>18</v>
       </c>
       <c r="B85" t="s">
-        <v>438</v>
+        <v>443</v>
       </c>
     </row>
     <row r="86" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A86" t="s">
-        <v>582</v>
+        <v>165</v>
       </c>
       <c r="B86" t="s">
-        <v>583</v>
+        <v>438</v>
       </c>
     </row>
     <row r="87" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A87" t="s">
-        <v>545</v>
+        <v>582</v>
       </c>
       <c r="B87" t="s">
-        <v>438</v>
+        <v>583</v>
       </c>
     </row>
     <row r="88" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A88" t="s">
-        <v>103</v>
+        <v>545</v>
       </c>
       <c r="B88" t="s">
         <v>438</v>
@@ -6431,7 +6440,7 @@
     </row>
     <row r="89" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A89" t="s">
-        <v>3</v>
+        <v>103</v>
       </c>
       <c r="B89" t="s">
         <v>438</v>
@@ -6439,23 +6448,23 @@
     </row>
     <row r="90" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A90" t="s">
-        <v>119</v>
+        <v>3</v>
       </c>
       <c r="B90" t="s">
-        <v>432</v>
+        <v>438</v>
       </c>
     </row>
     <row r="91" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A91" t="s">
-        <v>116</v>
+        <v>119</v>
       </c>
       <c r="B91" t="s">
-        <v>446</v>
+        <v>432</v>
       </c>
     </row>
     <row r="92" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A92" t="s">
-        <v>36</v>
+        <v>116</v>
       </c>
       <c r="B92" t="s">
         <v>446</v>
@@ -6463,7 +6472,7 @@
     </row>
     <row r="93" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A93" t="s">
-        <v>471</v>
+        <v>36</v>
       </c>
       <c r="B93" t="s">
         <v>446</v>
@@ -6471,7 +6480,7 @@
     </row>
     <row r="94" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A94" t="s">
-        <v>189</v>
+        <v>471</v>
       </c>
       <c r="B94" t="s">
         <v>446</v>
@@ -6479,88 +6488,104 @@
     </row>
     <row r="95" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A95" t="s">
-        <v>11</v>
+        <v>189</v>
       </c>
       <c r="B95" t="s">
-        <v>432</v>
+        <v>446</v>
       </c>
     </row>
     <row r="96" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A96" t="s">
-        <v>171</v>
+        <v>11</v>
       </c>
       <c r="B96" t="s">
-        <v>434</v>
+        <v>432</v>
       </c>
     </row>
     <row r="97" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A97" t="s">
-        <v>32</v>
+        <v>171</v>
       </c>
       <c r="B97" t="s">
-        <v>435</v>
+        <v>434</v>
       </c>
     </row>
     <row r="98" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A98" t="s">
-        <v>9</v>
+        <v>32</v>
       </c>
       <c r="B98" t="s">
-        <v>433</v>
+        <v>435</v>
       </c>
     </row>
     <row r="99" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A99" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="B99" t="s">
-        <v>436</v>
+        <v>433</v>
       </c>
     </row>
     <row r="100" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A100" t="s">
-        <v>136</v>
+        <v>10</v>
       </c>
       <c r="B100" t="s">
-        <v>440</v>
+        <v>436</v>
       </c>
     </row>
     <row r="101" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A101" t="s">
-        <v>104</v>
+        <v>136</v>
       </c>
       <c r="B101" t="s">
-        <v>436</v>
+        <v>440</v>
       </c>
     </row>
     <row r="102" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A102" t="s">
-        <v>39</v>
+        <v>104</v>
       </c>
       <c r="B102" t="s">
-        <v>443</v>
+        <v>436</v>
       </c>
     </row>
     <row r="103" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A103" t="s">
-        <v>168</v>
+        <v>594</v>
       </c>
       <c r="B103" t="s">
-        <v>433</v>
+        <v>598</v>
       </c>
     </row>
     <row r="104" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A104" t="s">
+        <v>39</v>
+      </c>
+      <c r="B104" t="s">
+        <v>443</v>
+      </c>
+    </row>
+    <row r="105" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A105" t="s">
+        <v>168</v>
+      </c>
+      <c r="B105" t="s">
+        <v>433</v>
+      </c>
+    </row>
+    <row r="106" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A106" t="s">
         <v>1</v>
       </c>
-      <c r="B104" t="s">
+      <c r="B106" t="s">
         <v>434</v>
       </c>
     </row>
   </sheetData>
-  <autoFilter ref="A1:B104" xr:uid="{344218C0-5C74-48AB-A8DF-7C6AE2CA916D}">
-    <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="A2:B104">
-      <sortCondition descending="1" ref="A1:A104"/>
+  <autoFilter ref="A1:B106" xr:uid="{344218C0-5C74-48AB-A8DF-7C6AE2CA916D}">
+    <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="A2:B106">
+      <sortCondition descending="1" ref="A1:A106"/>
     </sortState>
   </autoFilter>
   <phoneticPr fontId="11" type="noConversion"/>
@@ -6724,21 +6749,21 @@
     <row r="1" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A1" s="1"/>
       <c r="B1" s="1"/>
-      <c r="D1" s="17" t="s">
+      <c r="D1" s="18" t="s">
         <v>467</v>
       </c>
-      <c r="E1" s="19"/>
-      <c r="F1" s="17" t="s">
+      <c r="E1" s="20"/>
+      <c r="F1" s="18" t="s">
         <v>454</v>
       </c>
-      <c r="G1" s="18"/>
-      <c r="H1" s="18"/>
-      <c r="I1" s="18"/>
-      <c r="J1" s="18"/>
-      <c r="K1" s="18"/>
-      <c r="L1" s="18"/>
-      <c r="M1" s="18"/>
-      <c r="N1" s="19"/>
+      <c r="G1" s="19"/>
+      <c r="H1" s="19"/>
+      <c r="I1" s="19"/>
+      <c r="J1" s="19"/>
+      <c r="K1" s="19"/>
+      <c r="L1" s="19"/>
+      <c r="M1" s="19"/>
+      <c r="N1" s="20"/>
     </row>
     <row r="2" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A2" s="1" t="s">
@@ -8277,8 +8302,8 @@
   </sheetPr>
   <dimension ref="A1:E54"/>
   <sheetViews>
-    <sheetView topLeftCell="A13" workbookViewId="0">
-      <selection activeCell="E37" sqref="E37"/>
+    <sheetView topLeftCell="A32" workbookViewId="0">
+      <selection activeCell="A55" sqref="A55:C56"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -9011,7 +9036,7 @@
         <v>486</v>
       </c>
       <c r="B54" t="s">
-        <v>594</v>
+        <v>591</v>
       </c>
       <c r="C54" t="s">
         <v>157</v>
@@ -9032,8 +9057,8 @@
   </sheetPr>
   <dimension ref="A1:D232"/>
   <sheetViews>
-    <sheetView topLeftCell="A193" workbookViewId="0">
-      <selection activeCell="B222" sqref="B222"/>
+    <sheetView topLeftCell="A205" workbookViewId="0">
+      <selection activeCell="B240" sqref="B240"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -11677,10 +11702,10 @@
         <v>486</v>
       </c>
       <c r="B222" t="s">
-        <v>591</v>
+        <v>589</v>
       </c>
       <c r="C222" t="s">
-        <v>409</v>
+        <v>78</v>
       </c>
     </row>
     <row r="223" spans="1:4" x14ac:dyDescent="0.25">
@@ -11688,7 +11713,7 @@
         <v>486</v>
       </c>
       <c r="B223" t="s">
-        <v>592</v>
+        <v>590</v>
       </c>
       <c r="C223" t="s">
         <v>593</v>
@@ -12117,7 +12142,7 @@
   <dimension ref="A1:H96"/>
   <sheetViews>
     <sheetView topLeftCell="A71" workbookViewId="0">
-      <selection activeCell="C105" sqref="C105"/>
+      <selection activeCell="F85" sqref="F85"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -12133,2004 +12158,2004 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A1" s="20" t="s">
+      <c r="A1" s="17" t="s">
         <v>485</v>
       </c>
-      <c r="B1" s="20" t="s">
+      <c r="B1" s="17" t="s">
         <v>494</v>
       </c>
-      <c r="C1" s="20" t="s">
+      <c r="C1" s="17" t="s">
         <v>490</v>
       </c>
-      <c r="D1" s="20" t="s">
+      <c r="D1" s="17" t="s">
         <v>50</v>
       </c>
-      <c r="E1" s="20" t="s">
+      <c r="E1" s="17" t="s">
         <v>51</v>
       </c>
-      <c r="F1" s="20" t="s">
+      <c r="F1" s="17" t="s">
         <v>139</v>
       </c>
-      <c r="G1" s="20" t="s">
+      <c r="G1" s="17" t="s">
         <v>209</v>
       </c>
-      <c r="H1" s="20" t="s">
+      <c r="H1" s="17" t="s">
         <v>210</v>
       </c>
     </row>
     <row r="2" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A2" s="20" t="s">
+      <c r="A2" s="17" t="s">
         <v>487</v>
       </c>
-      <c r="B2" s="20" t="s">
+      <c r="B2" s="17" t="s">
         <v>489</v>
       </c>
-      <c r="C2" s="20" t="s">
+      <c r="C2" s="17" t="s">
         <v>497</v>
       </c>
-      <c r="D2" s="20" t="s">
+      <c r="D2" s="17" t="s">
         <v>158</v>
       </c>
-      <c r="E2" s="20" t="s">
+      <c r="E2" s="17" t="s">
         <v>196</v>
       </c>
-      <c r="F2" s="20" t="s">
+      <c r="F2" s="17" t="s">
         <v>199</v>
       </c>
-      <c r="G2" s="20" t="s">
+      <c r="G2" s="17" t="s">
         <v>326</v>
       </c>
-      <c r="H2" s="20" t="s">
+      <c r="H2" s="17" t="s">
         <v>216</v>
       </c>
     </row>
     <row r="3" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A3" s="20" t="s">
+      <c r="A3" s="17" t="s">
         <v>487</v>
       </c>
-      <c r="B3" s="20" t="s">
+      <c r="B3" s="17" t="s">
         <v>489</v>
       </c>
-      <c r="C3" s="20" t="s">
+      <c r="C3" s="17" t="s">
         <v>497</v>
       </c>
-      <c r="D3" s="20" t="s">
+      <c r="D3" s="17" t="s">
         <v>158</v>
       </c>
-      <c r="E3" s="20" t="s">
+      <c r="E3" s="17" t="s">
         <v>196</v>
       </c>
-      <c r="F3" s="20" t="s">
+      <c r="F3" s="17" t="s">
         <v>199</v>
       </c>
-      <c r="G3" s="20" t="s">
+      <c r="G3" s="17" t="s">
         <v>326</v>
       </c>
-      <c r="H3" s="20" t="s">
+      <c r="H3" s="17" t="s">
         <v>222</v>
       </c>
     </row>
     <row r="4" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A4" s="20" t="s">
+      <c r="A4" s="17" t="s">
         <v>487</v>
       </c>
-      <c r="B4" s="20" t="s">
+      <c r="B4" s="17" t="s">
         <v>489</v>
       </c>
-      <c r="C4" s="20" t="s">
+      <c r="C4" s="17" t="s">
         <v>518</v>
       </c>
-      <c r="D4" s="20" t="s">
+      <c r="D4" s="17" t="s">
         <v>158</v>
       </c>
-      <c r="E4" s="20" t="s">
+      <c r="E4" s="17" t="s">
         <v>196</v>
       </c>
-      <c r="F4" s="20" t="s">
+      <c r="F4" s="17" t="s">
         <v>199</v>
       </c>
-      <c r="G4" s="20" t="s">
+      <c r="G4" s="17" t="s">
         <v>326</v>
       </c>
-      <c r="H4" s="20" t="s">
+      <c r="H4" s="17" t="s">
         <v>226</v>
       </c>
     </row>
     <row r="5" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A5" s="20" t="s">
+      <c r="A5" s="17" t="s">
         <v>487</v>
       </c>
-      <c r="B5" s="20" t="s">
+      <c r="B5" s="17" t="s">
         <v>489</v>
       </c>
-      <c r="C5" s="20" t="s">
+      <c r="C5" s="17" t="s">
         <v>557</v>
       </c>
-      <c r="D5" s="20" t="s">
+      <c r="D5" s="17" t="s">
         <v>158</v>
       </c>
-      <c r="E5" s="20" t="s">
+      <c r="E5" s="17" t="s">
         <v>196</v>
       </c>
-      <c r="F5" s="20" t="s">
+      <c r="F5" s="17" t="s">
         <v>199</v>
       </c>
-      <c r="G5" s="20" t="s">
+      <c r="G5" s="17" t="s">
         <v>326</v>
       </c>
-      <c r="H5" s="20" t="s">
+      <c r="H5" s="17" t="s">
         <v>231</v>
       </c>
     </row>
     <row r="6" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A6" s="20" t="s">
+      <c r="A6" s="17" t="s">
         <v>487</v>
       </c>
-      <c r="B6" s="20" t="s">
+      <c r="B6" s="17" t="s">
         <v>489</v>
       </c>
-      <c r="C6" s="20" t="s">
+      <c r="C6" s="17" t="s">
         <v>558</v>
       </c>
-      <c r="D6" s="20" t="s">
+      <c r="D6" s="17" t="s">
         <v>158</v>
       </c>
-      <c r="E6" s="20" t="s">
+      <c r="E6" s="17" t="s">
         <v>196</v>
       </c>
-      <c r="F6" s="20" t="s">
+      <c r="F6" s="17" t="s">
         <v>199</v>
       </c>
-      <c r="G6" s="20" t="s">
+      <c r="G6" s="17" t="s">
         <v>326</v>
       </c>
-      <c r="H6" s="20" t="s">
+      <c r="H6" s="17" t="s">
         <v>236</v>
       </c>
     </row>
     <row r="7" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A7" s="20" t="s">
+      <c r="A7" s="17" t="s">
         <v>487</v>
       </c>
-      <c r="B7" s="20" t="s">
+      <c r="B7" s="17" t="s">
         <v>489</v>
       </c>
-      <c r="C7" s="20" t="s">
+      <c r="C7" s="17" t="s">
         <v>558</v>
       </c>
-      <c r="D7" s="20" t="s">
+      <c r="D7" s="17" t="s">
         <v>158</v>
       </c>
-      <c r="E7" s="20" t="s">
+      <c r="E7" s="17" t="s">
         <v>196</v>
       </c>
-      <c r="F7" s="20" t="s">
+      <c r="F7" s="17" t="s">
         <v>199</v>
       </c>
-      <c r="G7" s="20" t="s">
+      <c r="G7" s="17" t="s">
         <v>326</v>
       </c>
-      <c r="H7" s="20" t="s">
+      <c r="H7" s="17" t="s">
         <v>242</v>
       </c>
     </row>
     <row r="8" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A8" s="20" t="s">
+      <c r="A8" s="17" t="s">
         <v>487</v>
       </c>
-      <c r="B8" s="20" t="s">
+      <c r="B8" s="17" t="s">
         <v>489</v>
       </c>
-      <c r="C8" s="20" t="s">
+      <c r="C8" s="17" t="s">
         <v>559</v>
       </c>
-      <c r="D8" s="20" t="s">
+      <c r="D8" s="17" t="s">
         <v>158</v>
       </c>
-      <c r="E8" s="20" t="s">
+      <c r="E8" s="17" t="s">
         <v>196</v>
       </c>
-      <c r="F8" s="20" t="s">
+      <c r="F8" s="17" t="s">
         <v>199</v>
       </c>
-      <c r="G8" s="20" t="s">
+      <c r="G8" s="17" t="s">
         <v>326</v>
       </c>
-      <c r="H8" s="20" t="s">
+      <c r="H8" s="17" t="s">
         <v>560</v>
       </c>
     </row>
     <row r="9" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A9" s="20" t="s">
+      <c r="A9" s="17" t="s">
         <v>487</v>
       </c>
-      <c r="B9" s="20" t="s">
+      <c r="B9" s="17" t="s">
         <v>489</v>
       </c>
-      <c r="C9" s="20" t="s">
+      <c r="C9" s="17" t="s">
         <v>517</v>
       </c>
-      <c r="D9" s="20" t="s">
+      <c r="D9" s="17" t="s">
         <v>158</v>
       </c>
-      <c r="E9" s="20" t="s">
+      <c r="E9" s="17" t="s">
         <v>196</v>
       </c>
-      <c r="F9" s="20" t="s">
+      <c r="F9" s="17" t="s">
         <v>199</v>
       </c>
-      <c r="G9" s="20" t="s">
+      <c r="G9" s="17" t="s">
         <v>326</v>
       </c>
-      <c r="H9" s="20" t="s">
+      <c r="H9" s="17" t="s">
         <v>508</v>
       </c>
     </row>
     <row r="10" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A10" s="20" t="s">
+      <c r="A10" s="17" t="s">
         <v>487</v>
       </c>
-      <c r="B10" s="20" t="s">
+      <c r="B10" s="17" t="s">
         <v>489</v>
       </c>
-      <c r="C10" s="20" t="s">
+      <c r="C10" s="17" t="s">
         <v>497</v>
       </c>
-      <c r="D10" s="20" t="s">
+      <c r="D10" s="17" t="s">
         <v>158</v>
       </c>
-      <c r="E10" s="20" t="s">
+      <c r="E10" s="17" t="s">
         <v>196</v>
       </c>
-      <c r="F10" s="20" t="s">
+      <c r="F10" s="17" t="s">
         <v>199</v>
       </c>
-      <c r="G10" s="20" t="s">
+      <c r="G10" s="17" t="s">
         <v>498</v>
       </c>
-      <c r="H10" s="20" t="s">
+      <c r="H10" s="17" t="s">
         <v>246</v>
       </c>
     </row>
     <row r="11" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A11" s="20" t="s">
+      <c r="A11" s="17" t="s">
         <v>487</v>
       </c>
-      <c r="B11" s="20" t="s">
+      <c r="B11" s="17" t="s">
         <v>489</v>
       </c>
-      <c r="C11" s="20" t="s">
+      <c r="C11" s="17" t="s">
         <v>497</v>
       </c>
-      <c r="D11" s="20" t="s">
+      <c r="D11" s="17" t="s">
         <v>158</v>
       </c>
-      <c r="E11" s="20" t="s">
+      <c r="E11" s="17" t="s">
         <v>196</v>
       </c>
-      <c r="F11" s="20" t="s">
+      <c r="F11" s="17" t="s">
         <v>199</v>
       </c>
-      <c r="G11" s="20" t="s">
+      <c r="G11" s="17" t="s">
         <v>498</v>
       </c>
-      <c r="H11" s="20" t="s">
+      <c r="H11" s="17" t="s">
         <v>250</v>
       </c>
     </row>
     <row r="12" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A12" s="20" t="s">
+      <c r="A12" s="17" t="s">
         <v>487</v>
       </c>
-      <c r="B12" s="20" t="s">
+      <c r="B12" s="17" t="s">
         <v>489</v>
       </c>
-      <c r="C12" s="20" t="s">
+      <c r="C12" s="17" t="s">
         <v>518</v>
       </c>
-      <c r="D12" s="20" t="s">
+      <c r="D12" s="17" t="s">
         <v>158</v>
       </c>
-      <c r="E12" s="20" t="s">
+      <c r="E12" s="17" t="s">
         <v>196</v>
       </c>
-      <c r="F12" s="20" t="s">
+      <c r="F12" s="17" t="s">
         <v>199</v>
       </c>
-      <c r="G12" s="20" t="s">
+      <c r="G12" s="17" t="s">
         <v>498</v>
       </c>
-      <c r="H12" s="20" t="s">
+      <c r="H12" s="17" t="s">
         <v>254</v>
       </c>
     </row>
     <row r="13" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A13" s="20" t="s">
+      <c r="A13" s="17" t="s">
         <v>487</v>
       </c>
-      <c r="B13" s="20" t="s">
+      <c r="B13" s="17" t="s">
         <v>489</v>
       </c>
-      <c r="C13" s="20" t="s">
+      <c r="C13" s="17" t="s">
         <v>557</v>
       </c>
-      <c r="D13" s="20" t="s">
+      <c r="D13" s="17" t="s">
         <v>158</v>
       </c>
-      <c r="E13" s="20" t="s">
+      <c r="E13" s="17" t="s">
         <v>196</v>
       </c>
-      <c r="F13" s="20" t="s">
+      <c r="F13" s="17" t="s">
         <v>199</v>
       </c>
-      <c r="G13" s="20" t="s">
+      <c r="G13" s="17" t="s">
         <v>498</v>
       </c>
-      <c r="H13" s="20" t="s">
+      <c r="H13" s="17" t="s">
         <v>258</v>
       </c>
     </row>
     <row r="14" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A14" s="20" t="s">
+      <c r="A14" s="17" t="s">
         <v>487</v>
       </c>
-      <c r="B14" s="20" t="s">
+      <c r="B14" s="17" t="s">
         <v>489</v>
       </c>
-      <c r="C14" s="20" t="s">
+      <c r="C14" s="17" t="s">
         <v>558</v>
       </c>
-      <c r="D14" s="20" t="s">
+      <c r="D14" s="17" t="s">
         <v>158</v>
       </c>
-      <c r="E14" s="20" t="s">
+      <c r="E14" s="17" t="s">
         <v>196</v>
       </c>
-      <c r="F14" s="20" t="s">
+      <c r="F14" s="17" t="s">
         <v>199</v>
       </c>
-      <c r="G14" s="20" t="s">
+      <c r="G14" s="17" t="s">
         <v>498</v>
       </c>
-      <c r="H14" s="20" t="s">
+      <c r="H14" s="17" t="s">
         <v>262</v>
       </c>
     </row>
     <row r="15" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A15" s="20" t="s">
+      <c r="A15" s="17" t="s">
         <v>487</v>
       </c>
-      <c r="B15" s="20" t="s">
+      <c r="B15" s="17" t="s">
         <v>489</v>
       </c>
-      <c r="C15" s="20" t="s">
+      <c r="C15" s="17" t="s">
         <v>558</v>
       </c>
-      <c r="D15" s="20" t="s">
+      <c r="D15" s="17" t="s">
         <v>158</v>
       </c>
-      <c r="E15" s="20" t="s">
+      <c r="E15" s="17" t="s">
         <v>196</v>
       </c>
-      <c r="F15" s="20" t="s">
+      <c r="F15" s="17" t="s">
         <v>199</v>
       </c>
-      <c r="G15" s="20" t="s">
+      <c r="G15" s="17" t="s">
         <v>498</v>
       </c>
-      <c r="H15" s="20" t="s">
+      <c r="H15" s="17" t="s">
         <v>266</v>
       </c>
     </row>
     <row r="16" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A16" s="20" t="s">
+      <c r="A16" s="17" t="s">
         <v>487</v>
       </c>
-      <c r="B16" s="20" t="s">
+      <c r="B16" s="17" t="s">
         <v>489</v>
       </c>
-      <c r="C16" s="20" t="s">
+      <c r="C16" s="17" t="s">
         <v>559</v>
       </c>
-      <c r="D16" s="20" t="s">
+      <c r="D16" s="17" t="s">
         <v>158</v>
       </c>
-      <c r="E16" s="20" t="s">
+      <c r="E16" s="17" t="s">
         <v>196</v>
       </c>
-      <c r="F16" s="20" t="s">
+      <c r="F16" s="17" t="s">
         <v>199</v>
       </c>
-      <c r="G16" s="20" t="s">
+      <c r="G16" s="17" t="s">
         <v>498</v>
       </c>
-      <c r="H16" s="20" t="s">
+      <c r="H16" s="17" t="s">
         <v>561</v>
       </c>
     </row>
     <row r="17" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A17" s="20" t="s">
+      <c r="A17" s="17" t="s">
         <v>487</v>
       </c>
-      <c r="B17" s="20" t="s">
+      <c r="B17" s="17" t="s">
         <v>489</v>
       </c>
-      <c r="C17" s="20" t="s">
+      <c r="C17" s="17" t="s">
         <v>517</v>
       </c>
-      <c r="D17" s="20" t="s">
+      <c r="D17" s="17" t="s">
         <v>158</v>
       </c>
-      <c r="E17" s="20" t="s">
+      <c r="E17" s="17" t="s">
         <v>196</v>
       </c>
-      <c r="F17" s="20" t="s">
+      <c r="F17" s="17" t="s">
         <v>199</v>
       </c>
-      <c r="G17" s="20" t="s">
+      <c r="G17" s="17" t="s">
         <v>498</v>
       </c>
-      <c r="H17" s="20" t="s">
+      <c r="H17" s="17" t="s">
         <v>509</v>
       </c>
     </row>
     <row r="18" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A18" s="20" t="s">
+      <c r="A18" s="17" t="s">
         <v>487</v>
       </c>
-      <c r="B18" s="20" t="s">
+      <c r="B18" s="17" t="s">
         <v>489</v>
       </c>
-      <c r="C18" s="20" t="s">
+      <c r="C18" s="17" t="s">
         <v>497</v>
       </c>
-      <c r="D18" s="20" t="s">
+      <c r="D18" s="17" t="s">
         <v>158</v>
       </c>
-      <c r="E18" s="20" t="s">
+      <c r="E18" s="17" t="s">
         <v>196</v>
       </c>
-      <c r="F18" s="20" t="s">
+      <c r="F18" s="17" t="s">
         <v>199</v>
       </c>
-      <c r="G18" s="20" t="s">
+      <c r="G18" s="17" t="s">
         <v>499</v>
       </c>
-      <c r="H18" s="20" t="s">
+      <c r="H18" s="17" t="s">
         <v>270</v>
       </c>
     </row>
     <row r="19" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A19" s="20" t="s">
+      <c r="A19" s="17" t="s">
         <v>487</v>
       </c>
-      <c r="B19" s="20" t="s">
+      <c r="B19" s="17" t="s">
         <v>489</v>
       </c>
-      <c r="C19" s="20" t="s">
+      <c r="C19" s="17" t="s">
         <v>497</v>
       </c>
-      <c r="D19" s="20" t="s">
+      <c r="D19" s="17" t="s">
         <v>158</v>
       </c>
-      <c r="E19" s="20" t="s">
+      <c r="E19" s="17" t="s">
         <v>196</v>
       </c>
-      <c r="F19" s="20" t="s">
+      <c r="F19" s="17" t="s">
         <v>199</v>
       </c>
-      <c r="G19" s="20" t="s">
+      <c r="G19" s="17" t="s">
         <v>499</v>
       </c>
-      <c r="H19" s="20" t="s">
+      <c r="H19" s="17" t="s">
         <v>274</v>
       </c>
     </row>
     <row r="20" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A20" s="20" t="s">
+      <c r="A20" s="17" t="s">
         <v>487</v>
       </c>
-      <c r="B20" s="20" t="s">
+      <c r="B20" s="17" t="s">
         <v>489</v>
       </c>
-      <c r="C20" s="20" t="s">
+      <c r="C20" s="17" t="s">
         <v>518</v>
       </c>
-      <c r="D20" s="20" t="s">
+      <c r="D20" s="17" t="s">
         <v>158</v>
       </c>
-      <c r="E20" s="20" t="s">
+      <c r="E20" s="17" t="s">
         <v>196</v>
       </c>
-      <c r="F20" s="20" t="s">
+      <c r="F20" s="17" t="s">
         <v>199</v>
       </c>
-      <c r="G20" s="20" t="s">
+      <c r="G20" s="17" t="s">
         <v>499</v>
       </c>
-      <c r="H20" s="20" t="s">
+      <c r="H20" s="17" t="s">
         <v>278</v>
       </c>
     </row>
     <row r="21" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A21" s="20" t="s">
+      <c r="A21" s="17" t="s">
         <v>487</v>
       </c>
-      <c r="B21" s="20" t="s">
+      <c r="B21" s="17" t="s">
         <v>489</v>
       </c>
-      <c r="C21" s="20" t="s">
+      <c r="C21" s="17" t="s">
         <v>557</v>
       </c>
-      <c r="D21" s="20" t="s">
+      <c r="D21" s="17" t="s">
         <v>158</v>
       </c>
-      <c r="E21" s="20" t="s">
+      <c r="E21" s="17" t="s">
         <v>196</v>
       </c>
-      <c r="F21" s="20" t="s">
+      <c r="F21" s="17" t="s">
         <v>199</v>
       </c>
-      <c r="G21" s="20" t="s">
+      <c r="G21" s="17" t="s">
         <v>499</v>
       </c>
-      <c r="H21" s="20" t="s">
+      <c r="H21" s="17" t="s">
         <v>283</v>
       </c>
     </row>
     <row r="22" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A22" s="20" t="s">
+      <c r="A22" s="17" t="s">
         <v>487</v>
       </c>
-      <c r="B22" s="20" t="s">
+      <c r="B22" s="17" t="s">
         <v>489</v>
       </c>
-      <c r="C22" s="20" t="s">
+      <c r="C22" s="17" t="s">
         <v>558</v>
       </c>
-      <c r="D22" s="20" t="s">
+      <c r="D22" s="17" t="s">
         <v>158</v>
       </c>
-      <c r="E22" s="20" t="s">
+      <c r="E22" s="17" t="s">
         <v>196</v>
       </c>
-      <c r="F22" s="20" t="s">
+      <c r="F22" s="17" t="s">
         <v>199</v>
       </c>
-      <c r="G22" s="20" t="s">
+      <c r="G22" s="17" t="s">
         <v>499</v>
       </c>
-      <c r="H22" s="20" t="s">
+      <c r="H22" s="17" t="s">
         <v>288</v>
       </c>
     </row>
     <row r="23" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A23" s="20" t="s">
+      <c r="A23" s="17" t="s">
         <v>487</v>
       </c>
-      <c r="B23" s="20" t="s">
+      <c r="B23" s="17" t="s">
         <v>489</v>
       </c>
-      <c r="C23" s="20" t="s">
+      <c r="C23" s="17" t="s">
         <v>558</v>
       </c>
-      <c r="D23" s="20" t="s">
+      <c r="D23" s="17" t="s">
         <v>158</v>
       </c>
-      <c r="E23" s="20" t="s">
+      <c r="E23" s="17" t="s">
         <v>196</v>
       </c>
-      <c r="F23" s="20" t="s">
+      <c r="F23" s="17" t="s">
         <v>199</v>
       </c>
-      <c r="G23" s="20" t="s">
+      <c r="G23" s="17" t="s">
         <v>499</v>
       </c>
-      <c r="H23" s="20" t="s">
+      <c r="H23" s="17" t="s">
         <v>293</v>
       </c>
     </row>
     <row r="24" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A24" s="20" t="s">
+      <c r="A24" s="17" t="s">
         <v>487</v>
       </c>
-      <c r="B24" s="20" t="s">
+      <c r="B24" s="17" t="s">
         <v>489</v>
       </c>
-      <c r="C24" s="20" t="s">
+      <c r="C24" s="17" t="s">
         <v>559</v>
       </c>
-      <c r="D24" s="20" t="s">
+      <c r="D24" s="17" t="s">
         <v>158</v>
       </c>
-      <c r="E24" s="20" t="s">
+      <c r="E24" s="17" t="s">
         <v>196</v>
       </c>
-      <c r="F24" s="20" t="s">
+      <c r="F24" s="17" t="s">
         <v>199</v>
       </c>
-      <c r="G24" s="20" t="s">
+      <c r="G24" s="17" t="s">
         <v>499</v>
       </c>
-      <c r="H24" s="20" t="s">
+      <c r="H24" s="17" t="s">
         <v>562</v>
       </c>
     </row>
     <row r="25" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A25" s="20" t="s">
+      <c r="A25" s="17" t="s">
         <v>487</v>
       </c>
-      <c r="B25" s="20" t="s">
+      <c r="B25" s="17" t="s">
         <v>489</v>
       </c>
-      <c r="C25" s="20" t="s">
+      <c r="C25" s="17" t="s">
         <v>517</v>
       </c>
-      <c r="D25" s="20" t="s">
+      <c r="D25" s="17" t="s">
         <v>158</v>
       </c>
-      <c r="E25" s="20" t="s">
+      <c r="E25" s="17" t="s">
         <v>196</v>
       </c>
-      <c r="F25" s="20" t="s">
+      <c r="F25" s="17" t="s">
         <v>199</v>
       </c>
-      <c r="G25" s="20" t="s">
+      <c r="G25" s="17" t="s">
         <v>499</v>
       </c>
-      <c r="H25" s="20" t="s">
+      <c r="H25" s="17" t="s">
         <v>510</v>
       </c>
     </row>
     <row r="26" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A26" s="20" t="s">
+      <c r="A26" s="17" t="s">
         <v>487</v>
       </c>
-      <c r="B26" s="20" t="s">
+      <c r="B26" s="17" t="s">
         <v>489</v>
       </c>
-      <c r="C26" s="20" t="s">
+      <c r="C26" s="17" t="s">
         <v>497</v>
       </c>
-      <c r="D26" s="20" t="s">
+      <c r="D26" s="17" t="s">
         <v>158</v>
       </c>
-      <c r="E26" s="20" t="s">
+      <c r="E26" s="17" t="s">
         <v>196</v>
       </c>
-      <c r="F26" s="20" t="s">
+      <c r="F26" s="17" t="s">
         <v>199</v>
       </c>
-      <c r="G26" s="20" t="s">
+      <c r="G26" s="17" t="s">
         <v>500</v>
       </c>
-      <c r="H26" s="20" t="s">
+      <c r="H26" s="17" t="s">
         <v>297</v>
       </c>
     </row>
     <row r="27" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A27" s="20" t="s">
+      <c r="A27" s="17" t="s">
         <v>487</v>
       </c>
-      <c r="B27" s="20" t="s">
+      <c r="B27" s="17" t="s">
         <v>489</v>
       </c>
-      <c r="C27" s="20" t="s">
+      <c r="C27" s="17" t="s">
         <v>497</v>
       </c>
-      <c r="D27" s="20" t="s">
+      <c r="D27" s="17" t="s">
         <v>158</v>
       </c>
-      <c r="E27" s="20" t="s">
+      <c r="E27" s="17" t="s">
         <v>196</v>
       </c>
-      <c r="F27" s="20" t="s">
+      <c r="F27" s="17" t="s">
         <v>199</v>
       </c>
-      <c r="G27" s="20" t="s">
+      <c r="G27" s="17" t="s">
         <v>500</v>
       </c>
-      <c r="H27" s="20" t="s">
+      <c r="H27" s="17" t="s">
         <v>302</v>
       </c>
     </row>
     <row r="28" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A28" s="20" t="s">
+      <c r="A28" s="17" t="s">
         <v>487</v>
       </c>
-      <c r="B28" s="20" t="s">
+      <c r="B28" s="17" t="s">
         <v>489</v>
       </c>
-      <c r="C28" s="20" t="s">
+      <c r="C28" s="17" t="s">
         <v>518</v>
       </c>
-      <c r="D28" s="20" t="s">
+      <c r="D28" s="17" t="s">
         <v>158</v>
       </c>
-      <c r="E28" s="20" t="s">
+      <c r="E28" s="17" t="s">
         <v>196</v>
       </c>
-      <c r="F28" s="20" t="s">
+      <c r="F28" s="17" t="s">
         <v>199</v>
       </c>
-      <c r="G28" s="20" t="s">
+      <c r="G28" s="17" t="s">
         <v>500</v>
       </c>
-      <c r="H28" s="20" t="s">
+      <c r="H28" s="17" t="s">
         <v>307</v>
       </c>
     </row>
     <row r="29" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A29" s="20" t="s">
+      <c r="A29" s="17" t="s">
         <v>487</v>
       </c>
-      <c r="B29" s="20" t="s">
+      <c r="B29" s="17" t="s">
         <v>489</v>
       </c>
-      <c r="C29" s="20" t="s">
+      <c r="C29" s="17" t="s">
         <v>557</v>
       </c>
-      <c r="D29" s="20" t="s">
+      <c r="D29" s="17" t="s">
         <v>158</v>
       </c>
-      <c r="E29" s="20" t="s">
+      <c r="E29" s="17" t="s">
         <v>196</v>
       </c>
-      <c r="F29" s="20" t="s">
+      <c r="F29" s="17" t="s">
         <v>199</v>
       </c>
-      <c r="G29" s="20" t="s">
+      <c r="G29" s="17" t="s">
         <v>500</v>
       </c>
-      <c r="H29" s="20" t="s">
+      <c r="H29" s="17" t="s">
         <v>312</v>
       </c>
     </row>
     <row r="30" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A30" s="20" t="s">
+      <c r="A30" s="17" t="s">
         <v>487</v>
       </c>
-      <c r="B30" s="20" t="s">
+      <c r="B30" s="17" t="s">
         <v>489</v>
       </c>
-      <c r="C30" s="20" t="s">
+      <c r="C30" s="17" t="s">
         <v>558</v>
       </c>
-      <c r="D30" s="20" t="s">
+      <c r="D30" s="17" t="s">
         <v>158</v>
       </c>
-      <c r="E30" s="20" t="s">
+      <c r="E30" s="17" t="s">
         <v>196</v>
       </c>
-      <c r="F30" s="20" t="s">
+      <c r="F30" s="17" t="s">
         <v>199</v>
       </c>
-      <c r="G30" s="20" t="s">
+      <c r="G30" s="17" t="s">
         <v>500</v>
       </c>
-      <c r="H30" s="20" t="s">
+      <c r="H30" s="17" t="s">
         <v>317</v>
       </c>
     </row>
     <row r="31" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A31" s="20" t="s">
+      <c r="A31" s="17" t="s">
         <v>487</v>
       </c>
-      <c r="B31" s="20" t="s">
+      <c r="B31" s="17" t="s">
         <v>489</v>
       </c>
-      <c r="C31" s="20" t="s">
+      <c r="C31" s="17" t="s">
         <v>558</v>
       </c>
-      <c r="D31" s="20" t="s">
+      <c r="D31" s="17" t="s">
         <v>158</v>
       </c>
-      <c r="E31" s="20" t="s">
+      <c r="E31" s="17" t="s">
         <v>196</v>
       </c>
-      <c r="F31" s="20" t="s">
+      <c r="F31" s="17" t="s">
         <v>199</v>
       </c>
-      <c r="G31" s="20" t="s">
+      <c r="G31" s="17" t="s">
         <v>500</v>
       </c>
-      <c r="H31" s="20" t="s">
+      <c r="H31" s="17" t="s">
         <v>322</v>
       </c>
     </row>
     <row r="32" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A32" s="20" t="s">
+      <c r="A32" s="17" t="s">
         <v>487</v>
       </c>
-      <c r="B32" s="20" t="s">
+      <c r="B32" s="17" t="s">
         <v>489</v>
       </c>
-      <c r="C32" s="20" t="s">
+      <c r="C32" s="17" t="s">
         <v>559</v>
       </c>
-      <c r="D32" s="20" t="s">
+      <c r="D32" s="17" t="s">
         <v>158</v>
       </c>
-      <c r="E32" s="20" t="s">
+      <c r="E32" s="17" t="s">
         <v>196</v>
       </c>
-      <c r="F32" s="20" t="s">
+      <c r="F32" s="17" t="s">
         <v>199</v>
       </c>
-      <c r="G32" s="20" t="s">
+      <c r="G32" s="17" t="s">
         <v>500</v>
       </c>
-      <c r="H32" s="20" t="s">
+      <c r="H32" s="17" t="s">
         <v>563</v>
       </c>
     </row>
     <row r="33" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A33" s="20" t="s">
+      <c r="A33" s="17" t="s">
         <v>487</v>
       </c>
-      <c r="B33" s="20" t="s">
+      <c r="B33" s="17" t="s">
         <v>489</v>
       </c>
-      <c r="C33" s="20" t="s">
+      <c r="C33" s="17" t="s">
         <v>517</v>
       </c>
-      <c r="D33" s="20" t="s">
+      <c r="D33" s="17" t="s">
         <v>158</v>
       </c>
-      <c r="E33" s="20" t="s">
+      <c r="E33" s="17" t="s">
         <v>196</v>
       </c>
-      <c r="F33" s="20" t="s">
+      <c r="F33" s="17" t="s">
         <v>199</v>
       </c>
-      <c r="G33" s="20" t="s">
+      <c r="G33" s="17" t="s">
         <v>500</v>
       </c>
-      <c r="H33" s="20" t="s">
+      <c r="H33" s="17" t="s">
         <v>511</v>
       </c>
     </row>
     <row r="34" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A34" s="20" t="s">
+      <c r="A34" s="17" t="s">
         <v>487</v>
       </c>
-      <c r="B34" s="20" t="s">
+      <c r="B34" s="17" t="s">
         <v>489</v>
       </c>
-      <c r="C34" s="20" t="s">
+      <c r="C34" s="17" t="s">
         <v>497</v>
       </c>
-      <c r="D34" s="20" t="s">
+      <c r="D34" s="17" t="s">
         <v>158</v>
       </c>
-      <c r="E34" s="20" t="s">
+      <c r="E34" s="17" t="s">
         <v>196</v>
       </c>
-      <c r="F34" s="20" t="s">
+      <c r="F34" s="17" t="s">
         <v>199</v>
       </c>
-      <c r="G34" s="20" t="s">
+      <c r="G34" s="17" t="s">
         <v>501</v>
       </c>
-      <c r="H34" s="20" t="s">
+      <c r="H34" s="17" t="s">
         <v>502</v>
       </c>
     </row>
     <row r="35" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A35" s="20" t="s">
+      <c r="A35" s="17" t="s">
         <v>487</v>
       </c>
-      <c r="B35" s="20" t="s">
+      <c r="B35" s="17" t="s">
         <v>489</v>
       </c>
-      <c r="C35" s="20" t="s">
+      <c r="C35" s="17" t="s">
         <v>497</v>
       </c>
-      <c r="D35" s="20" t="s">
+      <c r="D35" s="17" t="s">
         <v>158</v>
       </c>
-      <c r="E35" s="20" t="s">
+      <c r="E35" s="17" t="s">
         <v>196</v>
       </c>
-      <c r="F35" s="20" t="s">
+      <c r="F35" s="17" t="s">
         <v>199</v>
       </c>
-      <c r="G35" s="20" t="s">
+      <c r="G35" s="17" t="s">
         <v>501</v>
       </c>
-      <c r="H35" s="20" t="s">
+      <c r="H35" s="17" t="s">
         <v>503</v>
       </c>
     </row>
     <row r="36" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A36" s="20" t="s">
+      <c r="A36" s="17" t="s">
         <v>487</v>
       </c>
-      <c r="B36" s="20" t="s">
+      <c r="B36" s="17" t="s">
         <v>489</v>
       </c>
-      <c r="C36" s="20" t="s">
+      <c r="C36" s="17" t="s">
         <v>518</v>
       </c>
-      <c r="D36" s="20" t="s">
+      <c r="D36" s="17" t="s">
         <v>158</v>
       </c>
-      <c r="E36" s="20" t="s">
+      <c r="E36" s="17" t="s">
         <v>196</v>
       </c>
-      <c r="F36" s="20" t="s">
+      <c r="F36" s="17" t="s">
         <v>199</v>
       </c>
-      <c r="G36" s="20" t="s">
+      <c r="G36" s="17" t="s">
         <v>501</v>
       </c>
-      <c r="H36" s="20" t="s">
+      <c r="H36" s="17" t="s">
         <v>507</v>
       </c>
     </row>
     <row r="37" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A37" s="20" t="s">
+      <c r="A37" s="17" t="s">
         <v>487</v>
       </c>
-      <c r="B37" s="20" t="s">
+      <c r="B37" s="17" t="s">
         <v>489</v>
       </c>
-      <c r="C37" s="20" t="s">
+      <c r="C37" s="17" t="s">
         <v>517</v>
       </c>
-      <c r="D37" s="20" t="s">
+      <c r="D37" s="17" t="s">
         <v>158</v>
       </c>
-      <c r="E37" s="20" t="s">
+      <c r="E37" s="17" t="s">
         <v>196</v>
       </c>
-      <c r="F37" s="20" t="s">
+      <c r="F37" s="17" t="s">
         <v>199</v>
       </c>
-      <c r="G37" s="20" t="s">
+      <c r="G37" s="17" t="s">
         <v>501</v>
       </c>
-      <c r="H37" s="20" t="s">
+      <c r="H37" s="17" t="s">
         <v>512</v>
       </c>
     </row>
     <row r="38" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A38" s="20" t="s">
+      <c r="A38" s="17" t="s">
         <v>487</v>
       </c>
-      <c r="B38" s="20" t="s">
+      <c r="B38" s="17" t="s">
         <v>489</v>
       </c>
-      <c r="C38" s="20" t="s">
+      <c r="C38" s="17" t="s">
         <v>497</v>
       </c>
-      <c r="D38" s="20" t="s">
+      <c r="D38" s="17" t="s">
         <v>158</v>
       </c>
-      <c r="E38" s="20" t="s">
+      <c r="E38" s="17" t="s">
         <v>196</v>
       </c>
-      <c r="F38" s="20" t="s">
+      <c r="F38" s="17" t="s">
         <v>197</v>
       </c>
-      <c r="G38" s="20" t="s">
+      <c r="G38" s="17" t="s">
         <v>504</v>
       </c>
-      <c r="H38" s="20" t="s">
+      <c r="H38" s="17" t="s">
         <v>327</v>
       </c>
     </row>
     <row r="39" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A39" s="20" t="s">
+      <c r="A39" s="17" t="s">
         <v>487</v>
       </c>
-      <c r="B39" s="20" t="s">
+      <c r="B39" s="17" t="s">
         <v>489</v>
       </c>
-      <c r="C39" s="20" t="s">
+      <c r="C39" s="17" t="s">
         <v>497</v>
       </c>
-      <c r="D39" s="20" t="s">
+      <c r="D39" s="17" t="s">
         <v>158</v>
       </c>
-      <c r="E39" s="20" t="s">
+      <c r="E39" s="17" t="s">
         <v>196</v>
       </c>
-      <c r="F39" s="20" t="s">
+      <c r="F39" s="17" t="s">
         <v>197</v>
       </c>
-      <c r="G39" s="20" t="s">
+      <c r="G39" s="17" t="s">
         <v>504</v>
       </c>
-      <c r="H39" s="20" t="s">
+      <c r="H39" s="17" t="s">
         <v>332</v>
       </c>
     </row>
     <row r="40" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A40" s="20" t="s">
+      <c r="A40" s="17" t="s">
         <v>487</v>
       </c>
-      <c r="B40" s="20" t="s">
+      <c r="B40" s="17" t="s">
         <v>489</v>
       </c>
-      <c r="C40" s="20" t="s">
+      <c r="C40" s="17" t="s">
         <v>518</v>
       </c>
-      <c r="D40" s="20" t="s">
+      <c r="D40" s="17" t="s">
         <v>158</v>
       </c>
-      <c r="E40" s="20" t="s">
+      <c r="E40" s="17" t="s">
         <v>196</v>
       </c>
-      <c r="F40" s="20" t="s">
+      <c r="F40" s="17" t="s">
         <v>197</v>
       </c>
-      <c r="G40" s="20" t="s">
+      <c r="G40" s="17" t="s">
         <v>504</v>
       </c>
-      <c r="H40" s="20" t="s">
+      <c r="H40" s="17" t="s">
         <v>337</v>
       </c>
     </row>
     <row r="41" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A41" s="20" t="s">
+      <c r="A41" s="17" t="s">
         <v>487</v>
       </c>
-      <c r="B41" s="20" t="s">
+      <c r="B41" s="17" t="s">
         <v>489</v>
       </c>
-      <c r="C41" s="20" t="s">
+      <c r="C41" s="17" t="s">
         <v>557</v>
       </c>
-      <c r="D41" s="20" t="s">
+      <c r="D41" s="17" t="s">
         <v>158</v>
       </c>
-      <c r="E41" s="20" t="s">
+      <c r="E41" s="17" t="s">
         <v>196</v>
       </c>
-      <c r="F41" s="20" t="s">
+      <c r="F41" s="17" t="s">
         <v>197</v>
       </c>
-      <c r="G41" s="20" t="s">
+      <c r="G41" s="17" t="s">
         <v>504</v>
       </c>
-      <c r="H41" s="20" t="s">
+      <c r="H41" s="17" t="s">
         <v>341</v>
       </c>
     </row>
     <row r="42" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A42" s="20" t="s">
+      <c r="A42" s="17" t="s">
         <v>487</v>
       </c>
-      <c r="B42" s="20" t="s">
+      <c r="B42" s="17" t="s">
         <v>489</v>
       </c>
-      <c r="C42" s="20" t="s">
+      <c r="C42" s="17" t="s">
         <v>558</v>
       </c>
-      <c r="D42" s="20" t="s">
+      <c r="D42" s="17" t="s">
         <v>158</v>
       </c>
-      <c r="E42" s="20" t="s">
+      <c r="E42" s="17" t="s">
         <v>196</v>
       </c>
-      <c r="F42" s="20" t="s">
+      <c r="F42" s="17" t="s">
         <v>197</v>
       </c>
-      <c r="G42" s="20" t="s">
+      <c r="G42" s="17" t="s">
         <v>504</v>
       </c>
-      <c r="H42" s="20" t="s">
+      <c r="H42" s="17" t="s">
         <v>344</v>
       </c>
     </row>
     <row r="43" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A43" s="20" t="s">
+      <c r="A43" s="17" t="s">
         <v>487</v>
       </c>
-      <c r="B43" s="20" t="s">
+      <c r="B43" s="17" t="s">
         <v>489</v>
       </c>
-      <c r="C43" s="20" t="s">
+      <c r="C43" s="17" t="s">
         <v>558</v>
       </c>
-      <c r="D43" s="20" t="s">
+      <c r="D43" s="17" t="s">
         <v>158</v>
       </c>
-      <c r="E43" s="20" t="s">
+      <c r="E43" s="17" t="s">
         <v>196</v>
       </c>
-      <c r="F43" s="20" t="s">
+      <c r="F43" s="17" t="s">
         <v>197</v>
       </c>
-      <c r="G43" s="20" t="s">
+      <c r="G43" s="17" t="s">
         <v>504</v>
       </c>
-      <c r="H43" s="20" t="s">
+      <c r="H43" s="17" t="s">
         <v>347</v>
       </c>
     </row>
     <row r="44" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A44" s="20" t="s">
+      <c r="A44" s="17" t="s">
         <v>487</v>
       </c>
-      <c r="B44" s="20" t="s">
+      <c r="B44" s="17" t="s">
         <v>489</v>
       </c>
-      <c r="C44" s="20" t="s">
+      <c r="C44" s="17" t="s">
         <v>559</v>
       </c>
-      <c r="D44" s="20" t="s">
+      <c r="D44" s="17" t="s">
         <v>158</v>
       </c>
-      <c r="E44" s="20" t="s">
+      <c r="E44" s="17" t="s">
         <v>196</v>
       </c>
-      <c r="F44" s="20" t="s">
+      <c r="F44" s="17" t="s">
         <v>197</v>
       </c>
-      <c r="G44" s="20" t="s">
+      <c r="G44" s="17" t="s">
         <v>504</v>
       </c>
-      <c r="H44" s="20" t="s">
+      <c r="H44" s="17" t="s">
         <v>564</v>
       </c>
     </row>
     <row r="45" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A45" s="20" t="s">
+      <c r="A45" s="17" t="s">
         <v>487</v>
       </c>
-      <c r="B45" s="20" t="s">
+      <c r="B45" s="17" t="s">
         <v>489</v>
       </c>
-      <c r="C45" s="20" t="s">
+      <c r="C45" s="17" t="s">
         <v>517</v>
       </c>
-      <c r="D45" s="20" t="s">
+      <c r="D45" s="17" t="s">
         <v>158</v>
       </c>
-      <c r="E45" s="20" t="s">
+      <c r="E45" s="17" t="s">
         <v>196</v>
       </c>
-      <c r="F45" s="20" t="s">
+      <c r="F45" s="17" t="s">
         <v>197</v>
       </c>
-      <c r="G45" s="20" t="s">
+      <c r="G45" s="17" t="s">
         <v>504</v>
       </c>
-      <c r="H45" s="20" t="s">
+      <c r="H45" s="17" t="s">
         <v>513</v>
       </c>
     </row>
     <row r="46" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A46" s="20" t="s">
+      <c r="A46" s="17" t="s">
         <v>487</v>
       </c>
-      <c r="B46" s="20" t="s">
+      <c r="B46" s="17" t="s">
         <v>489</v>
       </c>
-      <c r="C46" s="20" t="s">
+      <c r="C46" s="17" t="s">
         <v>497</v>
       </c>
-      <c r="D46" s="20" t="s">
+      <c r="D46" s="17" t="s">
         <v>158</v>
       </c>
-      <c r="E46" s="20" t="s">
+      <c r="E46" s="17" t="s">
         <v>196</v>
       </c>
-      <c r="F46" s="20" t="s">
+      <c r="F46" s="17" t="s">
         <v>197</v>
       </c>
-      <c r="G46" s="20" t="s">
+      <c r="G46" s="17" t="s">
         <v>505</v>
       </c>
-      <c r="H46" s="20" t="s">
+      <c r="H46" s="17" t="s">
         <v>351</v>
       </c>
     </row>
     <row r="47" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A47" s="20" t="s">
+      <c r="A47" s="17" t="s">
         <v>487</v>
       </c>
-      <c r="B47" s="20" t="s">
+      <c r="B47" s="17" t="s">
         <v>489</v>
       </c>
-      <c r="C47" s="20" t="s">
+      <c r="C47" s="17" t="s">
         <v>497</v>
       </c>
-      <c r="D47" s="20" t="s">
+      <c r="D47" s="17" t="s">
         <v>158</v>
       </c>
-      <c r="E47" s="20" t="s">
+      <c r="E47" s="17" t="s">
         <v>196</v>
       </c>
-      <c r="F47" s="20" t="s">
+      <c r="F47" s="17" t="s">
         <v>197</v>
       </c>
-      <c r="G47" s="20" t="s">
+      <c r="G47" s="17" t="s">
         <v>505</v>
       </c>
-      <c r="H47" s="20" t="s">
+      <c r="H47" s="17" t="s">
         <v>355</v>
       </c>
     </row>
     <row r="48" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A48" s="20" t="s">
+      <c r="A48" s="17" t="s">
         <v>487</v>
       </c>
-      <c r="B48" s="20" t="s">
+      <c r="B48" s="17" t="s">
         <v>489</v>
       </c>
-      <c r="C48" s="20" t="s">
+      <c r="C48" s="17" t="s">
         <v>518</v>
       </c>
-      <c r="D48" s="20" t="s">
+      <c r="D48" s="17" t="s">
         <v>158</v>
       </c>
-      <c r="E48" s="20" t="s">
+      <c r="E48" s="17" t="s">
         <v>196</v>
       </c>
-      <c r="F48" s="20" t="s">
+      <c r="F48" s="17" t="s">
         <v>197</v>
       </c>
-      <c r="G48" s="20" t="s">
+      <c r="G48" s="17" t="s">
         <v>505</v>
       </c>
-      <c r="H48" s="20" t="s">
+      <c r="H48" s="17" t="s">
         <v>359</v>
       </c>
     </row>
     <row r="49" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A49" s="20" t="s">
+      <c r="A49" s="17" t="s">
         <v>487</v>
       </c>
-      <c r="B49" s="20" t="s">
+      <c r="B49" s="17" t="s">
         <v>489</v>
       </c>
-      <c r="C49" s="20" t="s">
+      <c r="C49" s="17" t="s">
         <v>557</v>
       </c>
-      <c r="D49" s="20" t="s">
+      <c r="D49" s="17" t="s">
         <v>158</v>
       </c>
-      <c r="E49" s="20" t="s">
+      <c r="E49" s="17" t="s">
         <v>196</v>
       </c>
-      <c r="F49" s="20" t="s">
+      <c r="F49" s="17" t="s">
         <v>197</v>
       </c>
-      <c r="G49" s="20" t="s">
+      <c r="G49" s="17" t="s">
         <v>505</v>
       </c>
-      <c r="H49" s="20" t="s">
+      <c r="H49" s="17" t="s">
         <v>363</v>
       </c>
     </row>
     <row r="50" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A50" s="20" t="s">
+      <c r="A50" s="17" t="s">
         <v>487</v>
       </c>
-      <c r="B50" s="20" t="s">
+      <c r="B50" s="17" t="s">
         <v>489</v>
       </c>
-      <c r="C50" s="20" t="s">
+      <c r="C50" s="17" t="s">
         <v>558</v>
       </c>
-      <c r="D50" s="20" t="s">
+      <c r="D50" s="17" t="s">
         <v>158</v>
       </c>
-      <c r="E50" s="20" t="s">
+      <c r="E50" s="17" t="s">
         <v>196</v>
       </c>
-      <c r="F50" s="20" t="s">
+      <c r="F50" s="17" t="s">
         <v>197</v>
       </c>
-      <c r="G50" s="20" t="s">
+      <c r="G50" s="17" t="s">
         <v>505</v>
       </c>
-      <c r="H50" s="20" t="s">
+      <c r="H50" s="17" t="s">
         <v>367</v>
       </c>
     </row>
     <row r="51" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A51" s="20" t="s">
+      <c r="A51" s="17" t="s">
         <v>487</v>
       </c>
-      <c r="B51" s="20" t="s">
+      <c r="B51" s="17" t="s">
         <v>489</v>
       </c>
-      <c r="C51" s="20" t="s">
+      <c r="C51" s="17" t="s">
         <v>558</v>
       </c>
-      <c r="D51" s="20" t="s">
+      <c r="D51" s="17" t="s">
         <v>158</v>
       </c>
-      <c r="E51" s="20" t="s">
+      <c r="E51" s="17" t="s">
         <v>196</v>
       </c>
-      <c r="F51" s="20" t="s">
+      <c r="F51" s="17" t="s">
         <v>197</v>
       </c>
-      <c r="G51" s="20" t="s">
+      <c r="G51" s="17" t="s">
         <v>505</v>
       </c>
-      <c r="H51" s="20" t="s">
+      <c r="H51" s="17" t="s">
         <v>371</v>
       </c>
     </row>
     <row r="52" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A52" s="20" t="s">
+      <c r="A52" s="17" t="s">
         <v>487</v>
       </c>
-      <c r="B52" s="20" t="s">
+      <c r="B52" s="17" t="s">
         <v>489</v>
       </c>
-      <c r="C52" s="20" t="s">
+      <c r="C52" s="17" t="s">
         <v>559</v>
       </c>
-      <c r="D52" s="20" t="s">
+      <c r="D52" s="17" t="s">
         <v>158</v>
       </c>
-      <c r="E52" s="20" t="s">
+      <c r="E52" s="17" t="s">
         <v>196</v>
       </c>
-      <c r="F52" s="20" t="s">
+      <c r="F52" s="17" t="s">
         <v>197</v>
       </c>
-      <c r="G52" s="20" t="s">
+      <c r="G52" s="17" t="s">
         <v>505</v>
       </c>
-      <c r="H52" s="20" t="s">
+      <c r="H52" s="17" t="s">
         <v>565</v>
       </c>
     </row>
     <row r="53" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A53" s="20" t="s">
+      <c r="A53" s="17" t="s">
         <v>487</v>
       </c>
-      <c r="B53" s="20" t="s">
+      <c r="B53" s="17" t="s">
         <v>489</v>
       </c>
-      <c r="C53" s="20" t="s">
+      <c r="C53" s="17" t="s">
         <v>517</v>
       </c>
-      <c r="D53" s="20" t="s">
+      <c r="D53" s="17" t="s">
         <v>158</v>
       </c>
-      <c r="E53" s="20" t="s">
+      <c r="E53" s="17" t="s">
         <v>196</v>
       </c>
-      <c r="F53" s="20" t="s">
+      <c r="F53" s="17" t="s">
         <v>197</v>
       </c>
-      <c r="G53" s="20" t="s">
+      <c r="G53" s="17" t="s">
         <v>505</v>
       </c>
-      <c r="H53" s="20" t="s">
+      <c r="H53" s="17" t="s">
         <v>514</v>
       </c>
     </row>
     <row r="54" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A54" s="20" t="s">
+      <c r="A54" s="17" t="s">
         <v>487</v>
       </c>
-      <c r="B54" s="20" t="s">
+      <c r="B54" s="17" t="s">
         <v>489</v>
       </c>
-      <c r="C54" s="20" t="s">
+      <c r="C54" s="17" t="s">
         <v>497</v>
       </c>
-      <c r="D54" s="20" t="s">
+      <c r="D54" s="17" t="s">
         <v>158</v>
       </c>
-      <c r="E54" s="20" t="s">
+      <c r="E54" s="17" t="s">
         <v>196</v>
       </c>
-      <c r="F54" s="20" t="s">
+      <c r="F54" s="17" t="s">
         <v>197</v>
       </c>
-      <c r="G54" s="20" t="s">
+      <c r="G54" s="17" t="s">
         <v>506</v>
       </c>
-      <c r="H54" s="20" t="s">
+      <c r="H54" s="17" t="s">
         <v>375</v>
       </c>
     </row>
     <row r="55" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A55" s="20" t="s">
+      <c r="A55" s="17" t="s">
         <v>487</v>
       </c>
-      <c r="B55" s="20" t="s">
+      <c r="B55" s="17" t="s">
         <v>489</v>
       </c>
-      <c r="C55" s="20" t="s">
+      <c r="C55" s="17" t="s">
         <v>497</v>
       </c>
-      <c r="D55" s="20" t="s">
+      <c r="D55" s="17" t="s">
         <v>158</v>
       </c>
-      <c r="E55" s="20" t="s">
+      <c r="E55" s="17" t="s">
         <v>196</v>
       </c>
-      <c r="F55" s="20" t="s">
+      <c r="F55" s="17" t="s">
         <v>197</v>
       </c>
-      <c r="G55" s="20" t="s">
+      <c r="G55" s="17" t="s">
         <v>506</v>
       </c>
-      <c r="H55" s="20" t="s">
+      <c r="H55" s="17" t="s">
         <v>378</v>
       </c>
     </row>
     <row r="56" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A56" s="20" t="s">
+      <c r="A56" s="17" t="s">
         <v>487</v>
       </c>
-      <c r="B56" s="20" t="s">
+      <c r="B56" s="17" t="s">
         <v>489</v>
       </c>
-      <c r="C56" s="20" t="s">
+      <c r="C56" s="17" t="s">
         <v>518</v>
       </c>
-      <c r="D56" s="20" t="s">
+      <c r="D56" s="17" t="s">
         <v>158</v>
       </c>
-      <c r="E56" s="20" t="s">
+      <c r="E56" s="17" t="s">
         <v>196</v>
       </c>
-      <c r="F56" s="20" t="s">
+      <c r="F56" s="17" t="s">
         <v>197</v>
       </c>
-      <c r="G56" s="20" t="s">
+      <c r="G56" s="17" t="s">
         <v>506</v>
       </c>
-      <c r="H56" s="20" t="s">
+      <c r="H56" s="17" t="s">
         <v>381</v>
       </c>
     </row>
     <row r="57" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A57" s="20" t="s">
+      <c r="A57" s="17" t="s">
         <v>487</v>
       </c>
-      <c r="B57" s="20" t="s">
+      <c r="B57" s="17" t="s">
         <v>489</v>
       </c>
-      <c r="C57" s="20" t="s">
+      <c r="C57" s="17" t="s">
         <v>557</v>
       </c>
-      <c r="D57" s="20" t="s">
+      <c r="D57" s="17" t="s">
         <v>158</v>
       </c>
-      <c r="E57" s="20" t="s">
+      <c r="E57" s="17" t="s">
         <v>196</v>
       </c>
-      <c r="F57" s="20" t="s">
+      <c r="F57" s="17" t="s">
         <v>197</v>
       </c>
-      <c r="G57" s="20" t="s">
+      <c r="G57" s="17" t="s">
         <v>506</v>
       </c>
-      <c r="H57" s="20" t="s">
+      <c r="H57" s="17" t="s">
         <v>383</v>
       </c>
     </row>
     <row r="58" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A58" s="20" t="s">
+      <c r="A58" s="17" t="s">
         <v>487</v>
       </c>
-      <c r="B58" s="20" t="s">
+      <c r="B58" s="17" t="s">
         <v>489</v>
       </c>
-      <c r="C58" s="20" t="s">
+      <c r="C58" s="17" t="s">
         <v>558</v>
       </c>
-      <c r="D58" s="20" t="s">
+      <c r="D58" s="17" t="s">
         <v>158</v>
       </c>
-      <c r="E58" s="20" t="s">
+      <c r="E58" s="17" t="s">
         <v>196</v>
       </c>
-      <c r="F58" s="20" t="s">
+      <c r="F58" s="17" t="s">
         <v>197</v>
       </c>
-      <c r="G58" s="20" t="s">
+      <c r="G58" s="17" t="s">
         <v>506</v>
       </c>
-      <c r="H58" s="20" t="s">
+      <c r="H58" s="17" t="s">
         <v>385</v>
       </c>
     </row>
     <row r="59" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A59" s="20" t="s">
+      <c r="A59" s="17" t="s">
         <v>487</v>
       </c>
-      <c r="B59" s="20" t="s">
+      <c r="B59" s="17" t="s">
         <v>489</v>
       </c>
-      <c r="C59" s="20" t="s">
+      <c r="C59" s="17" t="s">
         <v>558</v>
       </c>
-      <c r="D59" s="20" t="s">
+      <c r="D59" s="17" t="s">
         <v>158</v>
       </c>
-      <c r="E59" s="20" t="s">
+      <c r="E59" s="17" t="s">
         <v>196</v>
       </c>
-      <c r="F59" s="20" t="s">
+      <c r="F59" s="17" t="s">
         <v>197</v>
       </c>
-      <c r="G59" s="20" t="s">
+      <c r="G59" s="17" t="s">
         <v>506</v>
       </c>
-      <c r="H59" s="20" t="s">
+      <c r="H59" s="17" t="s">
         <v>387</v>
       </c>
     </row>
     <row r="60" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A60" s="20" t="s">
+      <c r="A60" s="17" t="s">
         <v>487</v>
       </c>
-      <c r="B60" s="20" t="s">
+      <c r="B60" s="17" t="s">
         <v>489</v>
       </c>
-      <c r="C60" s="20" t="s">
+      <c r="C60" s="17" t="s">
         <v>559</v>
       </c>
-      <c r="D60" s="20" t="s">
+      <c r="D60" s="17" t="s">
         <v>158</v>
       </c>
-      <c r="E60" s="20" t="s">
+      <c r="E60" s="17" t="s">
         <v>196</v>
       </c>
-      <c r="F60" s="20" t="s">
+      <c r="F60" s="17" t="s">
         <v>197</v>
       </c>
-      <c r="G60" s="20" t="s">
+      <c r="G60" s="17" t="s">
         <v>506</v>
       </c>
-      <c r="H60" s="20" t="s">
+      <c r="H60" s="17" t="s">
         <v>566</v>
       </c>
     </row>
     <row r="61" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A61" s="20" t="s">
+      <c r="A61" s="17" t="s">
         <v>487</v>
       </c>
-      <c r="B61" s="20" t="s">
+      <c r="B61" s="17" t="s">
         <v>489</v>
       </c>
-      <c r="C61" s="20" t="s">
+      <c r="C61" s="17" t="s">
         <v>517</v>
       </c>
-      <c r="D61" s="20" t="s">
+      <c r="D61" s="17" t="s">
         <v>158</v>
       </c>
-      <c r="E61" s="20" t="s">
+      <c r="E61" s="17" t="s">
         <v>196</v>
       </c>
-      <c r="F61" s="20" t="s">
+      <c r="F61" s="17" t="s">
         <v>197</v>
       </c>
-      <c r="G61" s="20" t="s">
+      <c r="G61" s="17" t="s">
         <v>506</v>
       </c>
-      <c r="H61" s="20" t="s">
+      <c r="H61" s="17" t="s">
         <v>515</v>
       </c>
     </row>
     <row r="62" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A62" s="20" t="s">
+      <c r="A62" s="17" t="s">
         <v>487</v>
       </c>
-      <c r="B62" s="20" t="s">
+      <c r="B62" s="17" t="s">
         <v>489</v>
       </c>
-      <c r="C62" s="20" t="s">
+      <c r="C62" s="17" t="s">
         <v>497</v>
       </c>
-      <c r="D62" s="20" t="s">
+      <c r="D62" s="17" t="s">
         <v>158</v>
       </c>
-      <c r="E62" s="20" t="s">
+      <c r="E62" s="17" t="s">
         <v>196</v>
       </c>
-      <c r="F62" s="20" t="s">
+      <c r="F62" s="17" t="s">
         <v>197</v>
       </c>
-      <c r="G62" s="20" t="s">
+      <c r="G62" s="17" t="s">
         <v>354</v>
       </c>
-      <c r="H62" s="20" t="s">
+      <c r="H62" s="17" t="s">
         <v>389</v>
       </c>
     </row>
     <row r="63" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A63" s="20" t="s">
+      <c r="A63" s="17" t="s">
         <v>487</v>
       </c>
-      <c r="B63" s="20" t="s">
+      <c r="B63" s="17" t="s">
         <v>489</v>
       </c>
-      <c r="C63" s="20" t="s">
+      <c r="C63" s="17" t="s">
         <v>497</v>
       </c>
-      <c r="D63" s="20" t="s">
+      <c r="D63" s="17" t="s">
         <v>158</v>
       </c>
-      <c r="E63" s="20" t="s">
+      <c r="E63" s="17" t="s">
         <v>196</v>
       </c>
-      <c r="F63" s="20" t="s">
+      <c r="F63" s="17" t="s">
         <v>197</v>
       </c>
-      <c r="G63" s="20" t="s">
+      <c r="G63" s="17" t="s">
         <v>354</v>
       </c>
-      <c r="H63" s="20" t="s">
+      <c r="H63" s="17" t="s">
         <v>391</v>
       </c>
     </row>
     <row r="64" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A64" s="20" t="s">
+      <c r="A64" s="17" t="s">
         <v>487</v>
       </c>
-      <c r="B64" s="20" t="s">
+      <c r="B64" s="17" t="s">
         <v>489</v>
       </c>
-      <c r="C64" s="20" t="s">
+      <c r="C64" s="17" t="s">
         <v>518</v>
       </c>
-      <c r="D64" s="20" t="s">
+      <c r="D64" s="17" t="s">
         <v>158</v>
       </c>
-      <c r="E64" s="20" t="s">
+      <c r="E64" s="17" t="s">
         <v>196</v>
       </c>
-      <c r="F64" s="20" t="s">
+      <c r="F64" s="17" t="s">
         <v>197</v>
       </c>
-      <c r="G64" s="20" t="s">
+      <c r="G64" s="17" t="s">
         <v>354</v>
       </c>
-      <c r="H64" s="20" t="s">
+      <c r="H64" s="17" t="s">
         <v>393</v>
       </c>
     </row>
     <row r="65" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A65" s="20" t="s">
+      <c r="A65" s="17" t="s">
         <v>487</v>
       </c>
-      <c r="B65" s="20" t="s">
+      <c r="B65" s="17" t="s">
         <v>489</v>
       </c>
-      <c r="C65" s="20" t="s">
+      <c r="C65" s="17" t="s">
         <v>557</v>
       </c>
-      <c r="D65" s="20" t="s">
+      <c r="D65" s="17" t="s">
         <v>158</v>
       </c>
-      <c r="E65" s="20" t="s">
+      <c r="E65" s="17" t="s">
         <v>196</v>
       </c>
-      <c r="F65" s="20" t="s">
+      <c r="F65" s="17" t="s">
         <v>197</v>
       </c>
-      <c r="G65" s="20" t="s">
+      <c r="G65" s="17" t="s">
         <v>354</v>
       </c>
-      <c r="H65" s="20" t="s">
+      <c r="H65" s="17" t="s">
         <v>395</v>
       </c>
     </row>
     <row r="66" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A66" s="20" t="s">
+      <c r="A66" s="17" t="s">
         <v>487</v>
       </c>
-      <c r="B66" s="20" t="s">
+      <c r="B66" s="17" t="s">
         <v>489</v>
       </c>
-      <c r="C66" s="20" t="s">
+      <c r="C66" s="17" t="s">
         <v>558</v>
       </c>
-      <c r="D66" s="20" t="s">
+      <c r="D66" s="17" t="s">
         <v>158</v>
       </c>
-      <c r="E66" s="20" t="s">
+      <c r="E66" s="17" t="s">
         <v>196</v>
       </c>
-      <c r="F66" s="20" t="s">
+      <c r="F66" s="17" t="s">
         <v>197</v>
       </c>
-      <c r="G66" s="20" t="s">
+      <c r="G66" s="17" t="s">
         <v>354</v>
       </c>
-      <c r="H66" s="20" t="s">
+      <c r="H66" s="17" t="s">
         <v>397</v>
       </c>
     </row>
     <row r="67" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A67" s="20" t="s">
+      <c r="A67" s="17" t="s">
         <v>487</v>
       </c>
-      <c r="B67" s="20" t="s">
+      <c r="B67" s="17" t="s">
         <v>489</v>
       </c>
-      <c r="C67" s="20" t="s">
+      <c r="C67" s="17" t="s">
         <v>558</v>
       </c>
-      <c r="D67" s="20" t="s">
+      <c r="D67" s="17" t="s">
         <v>158</v>
       </c>
-      <c r="E67" s="20" t="s">
+      <c r="E67" s="17" t="s">
         <v>196</v>
       </c>
-      <c r="F67" s="20" t="s">
+      <c r="F67" s="17" t="s">
         <v>197</v>
       </c>
-      <c r="G67" s="20" t="s">
+      <c r="G67" s="17" t="s">
         <v>354</v>
       </c>
-      <c r="H67" s="20" t="s">
+      <c r="H67" s="17" t="s">
         <v>398</v>
       </c>
     </row>
     <row r="68" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A68" s="20" t="s">
+      <c r="A68" s="17" t="s">
         <v>487</v>
       </c>
-      <c r="B68" s="20" t="s">
+      <c r="B68" s="17" t="s">
         <v>489</v>
       </c>
-      <c r="C68" s="20" t="s">
+      <c r="C68" s="17" t="s">
         <v>559</v>
       </c>
-      <c r="D68" s="20" t="s">
+      <c r="D68" s="17" t="s">
         <v>158</v>
       </c>
-      <c r="E68" s="20" t="s">
+      <c r="E68" s="17" t="s">
         <v>196</v>
       </c>
-      <c r="F68" s="20" t="s">
+      <c r="F68" s="17" t="s">
         <v>197</v>
       </c>
-      <c r="G68" s="20" t="s">
+      <c r="G68" s="17" t="s">
         <v>354</v>
       </c>
-      <c r="H68" s="20" t="s">
+      <c r="H68" s="17" t="s">
         <v>567</v>
       </c>
     </row>
     <row r="69" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A69" s="20" t="s">
+      <c r="A69" s="17" t="s">
         <v>487</v>
       </c>
-      <c r="B69" s="20" t="s">
+      <c r="B69" s="17" t="s">
         <v>489</v>
       </c>
-      <c r="C69" s="20" t="s">
+      <c r="C69" s="17" t="s">
         <v>517</v>
       </c>
-      <c r="D69" s="20" t="s">
+      <c r="D69" s="17" t="s">
         <v>158</v>
       </c>
-      <c r="E69" s="20" t="s">
+      <c r="E69" s="17" t="s">
         <v>196</v>
       </c>
-      <c r="F69" s="20" t="s">
+      <c r="F69" s="17" t="s">
         <v>197</v>
       </c>
-      <c r="G69" s="20" t="s">
+      <c r="G69" s="17" t="s">
         <v>354</v>
       </c>
-      <c r="H69" s="20" t="s">
+      <c r="H69" s="17" t="s">
         <v>516</v>
       </c>
     </row>
     <row r="70" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A70" s="20" t="s">
+      <c r="A70" s="17" t="s">
         <v>487</v>
       </c>
-      <c r="B70" s="20" t="s">
+      <c r="B70" s="17" t="s">
         <v>489</v>
       </c>
-      <c r="C70" s="20" t="s">
+      <c r="C70" s="17" t="s">
         <v>497</v>
       </c>
-      <c r="D70" s="20" t="s">
+      <c r="D70" s="17" t="s">
         <v>158</v>
       </c>
-      <c r="E70" s="20" t="s">
+      <c r="E70" s="17" t="s">
         <v>196</v>
       </c>
-      <c r="F70" s="20" t="s">
+      <c r="F70" s="17" t="s">
         <v>197</v>
       </c>
-      <c r="G70" s="20" t="s">
+      <c r="G70" s="17" t="s">
         <v>354</v>
       </c>
-      <c r="H70" s="20" t="s">
+      <c r="H70" s="17" t="s">
         <v>568</v>
       </c>
     </row>
     <row r="71" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A71" s="20" t="s">
+      <c r="A71" s="17" t="s">
         <v>487</v>
       </c>
-      <c r="B71" s="20" t="s">
+      <c r="B71" s="17" t="s">
         <v>489</v>
       </c>
-      <c r="C71" s="20" t="s">
+      <c r="C71" s="17" t="s">
         <v>497</v>
       </c>
-      <c r="D71" s="20" t="s">
+      <c r="D71" s="17" t="s">
         <v>158</v>
       </c>
-      <c r="E71" s="20" t="s">
+      <c r="E71" s="17" t="s">
         <v>196</v>
       </c>
-      <c r="F71" s="20" t="s">
+      <c r="F71" s="17" t="s">
         <v>197</v>
       </c>
-      <c r="G71" s="20" t="s">
+      <c r="G71" s="17" t="s">
         <v>354</v>
       </c>
-      <c r="H71" s="20" t="s">
+      <c r="H71" s="17" t="s">
         <v>569</v>
       </c>
     </row>
     <row r="72" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A72" s="20" t="s">
+      <c r="A72" s="17" t="s">
         <v>487</v>
       </c>
-      <c r="B72" s="20" t="s">
+      <c r="B72" s="17" t="s">
         <v>489</v>
       </c>
-      <c r="C72" s="20" t="s">
+      <c r="C72" s="17" t="s">
         <v>518</v>
       </c>
-      <c r="D72" s="20" t="s">
+      <c r="D72" s="17" t="s">
         <v>158</v>
       </c>
-      <c r="E72" s="20" t="s">
+      <c r="E72" s="17" t="s">
         <v>196</v>
       </c>
-      <c r="F72" s="20" t="s">
+      <c r="F72" s="17" t="s">
         <v>197</v>
       </c>
-      <c r="G72" s="20" t="s">
+      <c r="G72" s="17" t="s">
         <v>354</v>
       </c>
-      <c r="H72" s="20" t="s">
+      <c r="H72" s="17" t="s">
         <v>570</v>
       </c>
     </row>
     <row r="73" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A73" s="20" t="s">
+      <c r="A73" s="17" t="s">
         <v>487</v>
       </c>
-      <c r="B73" s="20" t="s">
+      <c r="B73" s="17" t="s">
         <v>489</v>
       </c>
-      <c r="C73" s="20" t="s">
+      <c r="C73" s="17" t="s">
         <v>557</v>
       </c>
-      <c r="D73" s="20" t="s">
+      <c r="D73" s="17" t="s">
         <v>158</v>
       </c>
-      <c r="E73" s="20" t="s">
+      <c r="E73" s="17" t="s">
         <v>196</v>
       </c>
-      <c r="F73" s="20" t="s">
+      <c r="F73" s="17" t="s">
         <v>197</v>
       </c>
-      <c r="G73" s="20" t="s">
+      <c r="G73" s="17" t="s">
         <v>354</v>
       </c>
-      <c r="H73" s="20" t="s">
+      <c r="H73" s="17" t="s">
         <v>571</v>
       </c>
     </row>
     <row r="74" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A74" s="20" t="s">
+      <c r="A74" s="17" t="s">
         <v>487</v>
       </c>
-      <c r="B74" s="20" t="s">
+      <c r="B74" s="17" t="s">
         <v>489</v>
       </c>
-      <c r="C74" s="20" t="s">
+      <c r="C74" s="17" t="s">
         <v>558</v>
       </c>
-      <c r="D74" s="20" t="s">
+      <c r="D74" s="17" t="s">
         <v>158</v>
       </c>
-      <c r="E74" s="20" t="s">
+      <c r="E74" s="17" t="s">
         <v>196</v>
       </c>
-      <c r="F74" s="20" t="s">
+      <c r="F74" s="17" t="s">
         <v>197</v>
       </c>
-      <c r="G74" s="20" t="s">
+      <c r="G74" s="17" t="s">
         <v>354</v>
       </c>
-      <c r="H74" s="20" t="s">
+      <c r="H74" s="17" t="s">
         <v>572</v>
       </c>
     </row>
     <row r="75" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A75" s="20" t="s">
+      <c r="A75" s="17" t="s">
         <v>487</v>
       </c>
-      <c r="B75" s="20" t="s">
+      <c r="B75" s="17" t="s">
         <v>489</v>
       </c>
-      <c r="C75" s="20" t="s">
+      <c r="C75" s="17" t="s">
         <v>558</v>
       </c>
-      <c r="D75" s="20" t="s">
+      <c r="D75" s="17" t="s">
         <v>158</v>
       </c>
-      <c r="E75" s="20" t="s">
+      <c r="E75" s="17" t="s">
         <v>196</v>
       </c>
-      <c r="F75" s="20" t="s">
+      <c r="F75" s="17" t="s">
         <v>197</v>
       </c>
-      <c r="G75" s="20" t="s">
+      <c r="G75" s="17" t="s">
         <v>354</v>
       </c>
-      <c r="H75" s="20" t="s">
+      <c r="H75" s="17" t="s">
         <v>573</v>
       </c>
     </row>
     <row r="76" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A76" s="20" t="s">
+      <c r="A76" s="17" t="s">
         <v>487</v>
       </c>
-      <c r="B76" s="20" t="s">
+      <c r="B76" s="17" t="s">
         <v>489</v>
       </c>
-      <c r="C76" s="20" t="s">
+      <c r="C76" s="17" t="s">
         <v>559</v>
       </c>
-      <c r="D76" s="20" t="s">
+      <c r="D76" s="17" t="s">
         <v>158</v>
       </c>
-      <c r="E76" s="20" t="s">
+      <c r="E76" s="17" t="s">
         <v>196</v>
       </c>
-      <c r="F76" s="20" t="s">
+      <c r="F76" s="17" t="s">
         <v>197</v>
       </c>
-      <c r="G76" s="20" t="s">
+      <c r="G76" s="17" t="s">
         <v>354</v>
       </c>
-      <c r="H76" s="20" t="s">
+      <c r="H76" s="17" t="s">
         <v>574</v>
       </c>
     </row>
     <row r="77" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A77" s="20" t="s">
+      <c r="A77" s="17" t="s">
         <v>487</v>
       </c>
-      <c r="B77" s="20" t="s">
+      <c r="B77" s="17" t="s">
         <v>489</v>
       </c>
-      <c r="C77" s="20" t="s">
+      <c r="C77" s="17" t="s">
         <v>517</v>
       </c>
-      <c r="D77" s="20" t="s">
+      <c r="D77" s="17" t="s">
         <v>158</v>
       </c>
-      <c r="E77" s="20" t="s">
+      <c r="E77" s="17" t="s">
         <v>196</v>
       </c>
-      <c r="F77" s="20" t="s">
+      <c r="F77" s="17" t="s">
         <v>197</v>
       </c>
-      <c r="G77" s="20" t="s">
+      <c r="G77" s="17" t="s">
         <v>354</v>
       </c>
-      <c r="H77" s="20" t="s">
+      <c r="H77" s="17" t="s">
         <v>575</v>
       </c>
     </row>
@@ -14147,10 +14172,10 @@
       <c r="D78" t="s">
         <v>11</v>
       </c>
-      <c r="E78" s="20"/>
-      <c r="F78" s="20"/>
-      <c r="G78" s="20"/>
-      <c r="H78" s="20"/>
+      <c r="E78" s="17"/>
+      <c r="F78" s="17"/>
+      <c r="G78" s="17"/>
+      <c r="H78" s="17"/>
     </row>
     <row r="79" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A79" t="s">
@@ -14165,10 +14190,10 @@
       <c r="D79" t="s">
         <v>4</v>
       </c>
-      <c r="E79" s="20"/>
-      <c r="F79" s="20"/>
-      <c r="G79" s="20"/>
-      <c r="H79" s="20"/>
+      <c r="E79" s="17"/>
+      <c r="F79" s="17"/>
+      <c r="G79" s="17"/>
+      <c r="H79" s="17"/>
     </row>
     <row r="80" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A80" t="s">
@@ -14178,15 +14203,15 @@
         <v>488</v>
       </c>
       <c r="C80" t="s">
-        <v>585</v>
+        <v>584</v>
       </c>
       <c r="D80" t="s">
-        <v>584</v>
-      </c>
-      <c r="E80" s="20"/>
-      <c r="F80" s="20"/>
-      <c r="G80" s="20"/>
-      <c r="H80" s="20"/>
+        <v>597</v>
+      </c>
+      <c r="E80" s="17"/>
+      <c r="F80" s="17"/>
+      <c r="G80" s="17"/>
+      <c r="H80" s="17"/>
     </row>
     <row r="81" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A81" t="s">
@@ -14201,10 +14226,10 @@
       <c r="D81" t="s">
         <v>5</v>
       </c>
-      <c r="E81" s="20"/>
-      <c r="F81" s="20"/>
-      <c r="G81" s="20"/>
-      <c r="H81" s="20"/>
+      <c r="E81" s="17"/>
+      <c r="F81" s="17"/>
+      <c r="G81" s="17"/>
+      <c r="H81" s="17"/>
     </row>
     <row r="82" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A82" t="s">
@@ -14219,10 +14244,10 @@
       <c r="D82" t="s">
         <v>79</v>
       </c>
-      <c r="E82" s="20"/>
-      <c r="F82" s="20"/>
-      <c r="G82" s="20"/>
-      <c r="H82" s="20"/>
+      <c r="E82" s="17"/>
+      <c r="F82" s="17"/>
+      <c r="G82" s="17"/>
+      <c r="H82" s="17"/>
     </row>
     <row r="83" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A83" t="s">
@@ -14237,10 +14262,10 @@
       <c r="D83" t="s">
         <v>81</v>
       </c>
-      <c r="E83" s="20"/>
-      <c r="F83" s="20"/>
-      <c r="G83" s="20"/>
-      <c r="H83" s="20"/>
+      <c r="E83" s="17"/>
+      <c r="F83" s="17"/>
+      <c r="G83" s="17"/>
+      <c r="H83" s="17"/>
     </row>
     <row r="84" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A84" t="s">
@@ -14250,15 +14275,15 @@
         <v>488</v>
       </c>
       <c r="C84" t="s">
-        <v>89</v>
+        <v>595</v>
       </c>
       <c r="D84" t="s">
-        <v>89</v>
-      </c>
-      <c r="E84" s="20"/>
-      <c r="F84" s="20"/>
-      <c r="G84" s="20"/>
-      <c r="H84" s="20"/>
+        <v>550</v>
+      </c>
+      <c r="E84" s="17"/>
+      <c r="F84" s="17"/>
+      <c r="G84" s="17"/>
+      <c r="H84" s="17"/>
     </row>
     <row r="85" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A85" t="s">
@@ -14271,12 +14296,12 @@
         <v>89</v>
       </c>
       <c r="D85" t="s">
-        <v>551</v>
-      </c>
-      <c r="E85" s="20"/>
-      <c r="F85" s="20"/>
-      <c r="G85" s="20"/>
-      <c r="H85" s="20"/>
+        <v>89</v>
+      </c>
+      <c r="E85" s="17"/>
+      <c r="F85" s="17"/>
+      <c r="G85" s="17"/>
+      <c r="H85" s="17"/>
     </row>
     <row r="86" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A86" t="s">
@@ -14289,12 +14314,12 @@
         <v>89</v>
       </c>
       <c r="D86" t="s">
-        <v>552</v>
-      </c>
-      <c r="E86" s="20"/>
-      <c r="F86" s="20"/>
-      <c r="G86" s="20"/>
-      <c r="H86" s="20"/>
+        <v>551</v>
+      </c>
+      <c r="E86" s="17"/>
+      <c r="F86" s="17"/>
+      <c r="G86" s="17"/>
+      <c r="H86" s="17"/>
     </row>
     <row r="87" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A87" t="s">
@@ -14304,15 +14329,15 @@
         <v>488</v>
       </c>
       <c r="C87" t="s">
-        <v>85</v>
+        <v>89</v>
       </c>
       <c r="D87" t="s">
-        <v>548</v>
-      </c>
-      <c r="E87" s="20"/>
-      <c r="F87" s="20"/>
-      <c r="G87" s="20"/>
-      <c r="H87" s="20"/>
+        <v>552</v>
+      </c>
+      <c r="E87" s="17"/>
+      <c r="F87" s="17"/>
+      <c r="G87" s="17"/>
+      <c r="H87" s="17"/>
     </row>
     <row r="88" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A88" t="s">
@@ -14322,15 +14347,15 @@
         <v>488</v>
       </c>
       <c r="C88" t="s">
-        <v>547</v>
+        <v>85</v>
       </c>
       <c r="D88" t="s">
-        <v>547</v>
-      </c>
-      <c r="E88" s="20"/>
-      <c r="F88" s="20"/>
-      <c r="G88" s="20"/>
-      <c r="H88" s="20"/>
+        <v>548</v>
+      </c>
+      <c r="E88" s="17"/>
+      <c r="F88" s="17"/>
+      <c r="G88" s="17"/>
+      <c r="H88" s="17"/>
     </row>
     <row r="89" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A89" t="s">
@@ -14340,15 +14365,15 @@
         <v>488</v>
       </c>
       <c r="C89" t="s">
-        <v>83</v>
+        <v>547</v>
       </c>
       <c r="D89" t="s">
-        <v>83</v>
-      </c>
-      <c r="E89" s="20"/>
-      <c r="F89" s="20"/>
-      <c r="G89" s="20"/>
-      <c r="H89" s="20"/>
+        <v>547</v>
+      </c>
+      <c r="E89" s="17"/>
+      <c r="F89" s="17"/>
+      <c r="G89" s="17"/>
+      <c r="H89" s="17"/>
     </row>
     <row r="90" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A90" t="s">
@@ -14358,15 +14383,15 @@
         <v>488</v>
       </c>
       <c r="C90" t="s">
-        <v>10</v>
+        <v>83</v>
       </c>
       <c r="D90" t="s">
-        <v>549</v>
-      </c>
-      <c r="E90" s="20"/>
-      <c r="F90" s="20"/>
-      <c r="G90" s="20"/>
-      <c r="H90" s="20"/>
+        <v>83</v>
+      </c>
+      <c r="E90" s="17"/>
+      <c r="F90" s="17"/>
+      <c r="G90" s="17"/>
+      <c r="H90" s="17"/>
     </row>
     <row r="91" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A91" t="s">
@@ -14376,15 +14401,15 @@
         <v>488</v>
       </c>
       <c r="C91" t="s">
-        <v>554</v>
+        <v>10</v>
       </c>
       <c r="D91" t="s">
-        <v>553</v>
-      </c>
-      <c r="E91" s="20"/>
-      <c r="F91" s="20"/>
-      <c r="G91" s="20"/>
-      <c r="H91" s="20"/>
+        <v>549</v>
+      </c>
+      <c r="E91" s="17"/>
+      <c r="F91" s="17"/>
+      <c r="G91" s="17"/>
+      <c r="H91" s="17"/>
     </row>
     <row r="92" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A92" t="s">
@@ -14394,118 +14419,118 @@
         <v>488</v>
       </c>
       <c r="C92" t="s">
-        <v>554</v>
+        <v>594</v>
       </c>
       <c r="D92" t="s">
-        <v>550</v>
-      </c>
-      <c r="E92" s="20"/>
-      <c r="F92" s="20"/>
-      <c r="G92" s="20"/>
-      <c r="H92" s="20"/>
+        <v>553</v>
+      </c>
+      <c r="E92" s="17"/>
+      <c r="F92" s="17"/>
+      <c r="G92" s="17"/>
+      <c r="H92" s="17"/>
     </row>
     <row r="93" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A93" s="20" t="s">
+      <c r="A93" s="17" t="s">
         <v>487</v>
       </c>
-      <c r="B93" s="20" t="s">
+      <c r="B93" s="17" t="s">
         <v>489</v>
       </c>
-      <c r="C93" s="20" t="s">
+      <c r="C93" s="17" t="s">
         <v>557</v>
       </c>
-      <c r="D93" s="20" t="s">
+      <c r="D93" s="17" t="s">
         <v>158</v>
       </c>
-      <c r="E93" s="20" t="s">
+      <c r="E93" s="17" t="s">
         <v>196</v>
       </c>
-      <c r="F93" s="20" t="s">
+      <c r="F93" s="17" t="s">
         <v>199</v>
       </c>
-      <c r="G93" s="20" t="s">
+      <c r="G93" s="17" t="s">
         <v>501</v>
       </c>
-      <c r="H93" s="20" t="s">
+      <c r="H93" s="17" t="s">
+        <v>585</v>
+      </c>
+    </row>
+    <row r="94" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A94" s="17" t="s">
+        <v>487</v>
+      </c>
+      <c r="B94" s="17" t="s">
+        <v>489</v>
+      </c>
+      <c r="C94" s="17" t="s">
+        <v>558</v>
+      </c>
+      <c r="D94" s="17" t="s">
+        <v>158</v>
+      </c>
+      <c r="E94" s="17" t="s">
+        <v>196</v>
+      </c>
+      <c r="F94" s="17" t="s">
+        <v>199</v>
+      </c>
+      <c r="G94" s="17" t="s">
+        <v>501</v>
+      </c>
+      <c r="H94" s="17" t="s">
+        <v>586</v>
+      </c>
+    </row>
+    <row r="95" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A95" s="17" t="s">
+        <v>487</v>
+      </c>
+      <c r="B95" s="17" t="s">
+        <v>489</v>
+      </c>
+      <c r="C95" s="17" t="s">
+        <v>558</v>
+      </c>
+      <c r="D95" s="17" t="s">
+        <v>158</v>
+      </c>
+      <c r="E95" s="17" t="s">
+        <v>196</v>
+      </c>
+      <c r="F95" s="17" t="s">
+        <v>199</v>
+      </c>
+      <c r="G95" s="17" t="s">
+        <v>501</v>
+      </c>
+      <c r="H95" s="17" t="s">
         <v>587</v>
       </c>
     </row>
-    <row r="94" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A94" s="20" t="s">
+    <row r="96" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A96" s="17" t="s">
         <v>487</v>
       </c>
-      <c r="B94" s="20" t="s">
+      <c r="B96" s="17" t="s">
         <v>489</v>
       </c>
-      <c r="C94" s="20" t="s">
-        <v>558</v>
-      </c>
-      <c r="D94" s="20" t="s">
+      <c r="C96" s="17" t="s">
+        <v>559</v>
+      </c>
+      <c r="D96" s="17" t="s">
         <v>158</v>
       </c>
-      <c r="E94" s="20" t="s">
+      <c r="E96" s="17" t="s">
         <v>196</v>
       </c>
-      <c r="F94" s="20" t="s">
+      <c r="F96" s="17" t="s">
         <v>199</v>
       </c>
-      <c r="G94" s="20" t="s">
+      <c r="G96" s="17" t="s">
         <v>501</v>
       </c>
-      <c r="H94" s="20" t="s">
+      <c r="H96" s="17" t="s">
         <v>588</v>
-      </c>
-    </row>
-    <row r="95" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A95" s="20" t="s">
-        <v>487</v>
-      </c>
-      <c r="B95" s="20" t="s">
-        <v>489</v>
-      </c>
-      <c r="C95" s="20" t="s">
-        <v>558</v>
-      </c>
-      <c r="D95" s="20" t="s">
-        <v>158</v>
-      </c>
-      <c r="E95" s="20" t="s">
-        <v>196</v>
-      </c>
-      <c r="F95" s="20" t="s">
-        <v>199</v>
-      </c>
-      <c r="G95" s="20" t="s">
-        <v>501</v>
-      </c>
-      <c r="H95" s="20" t="s">
-        <v>589</v>
-      </c>
-    </row>
-    <row r="96" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A96" s="20" t="s">
-        <v>487</v>
-      </c>
-      <c r="B96" s="20" t="s">
-        <v>489</v>
-      </c>
-      <c r="C96" s="20" t="s">
-        <v>559</v>
-      </c>
-      <c r="D96" s="20" t="s">
-        <v>158</v>
-      </c>
-      <c r="E96" s="20" t="s">
-        <v>196</v>
-      </c>
-      <c r="F96" s="20" t="s">
-        <v>199</v>
-      </c>
-      <c r="G96" s="20" t="s">
-        <v>501</v>
-      </c>
-      <c r="H96" s="20" t="s">
-        <v>590</v>
       </c>
     </row>
   </sheetData>
@@ -17884,10 +17909,10 @@
   </sheetPr>
   <dimension ref="A1:W55"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A2" zoomScale="80" zoomScaleNormal="80" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A3" activePane="bottomLeft" state="frozen"/>
+    <sheetView topLeftCell="E2" zoomScale="80" zoomScaleNormal="80" workbookViewId="0">
+      <pane ySplit="1" topLeftCell="A27" activePane="bottomLeft" state="frozen"/>
       <selection activeCell="E2" sqref="E2"/>
-      <selection pane="bottomLeft" activeCell="E11" sqref="E11"/>
+      <selection pane="bottomLeft" activeCell="R50" sqref="R50:R51"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -17912,17 +17937,17 @@
       <c r="G1" s="14" t="s">
         <v>467</v>
       </c>
-      <c r="H1" s="17" t="s">
+      <c r="H1" s="18" t="s">
         <v>454</v>
       </c>
-      <c r="I1" s="18"/>
-      <c r="J1" s="18"/>
-      <c r="K1" s="18"/>
-      <c r="L1" s="18"/>
-      <c r="M1" s="18"/>
-      <c r="N1" s="18"/>
-      <c r="O1" s="18"/>
-      <c r="P1" s="19"/>
+      <c r="I1" s="19"/>
+      <c r="J1" s="19"/>
+      <c r="K1" s="19"/>
+      <c r="L1" s="19"/>
+      <c r="M1" s="19"/>
+      <c r="N1" s="19"/>
+      <c r="O1" s="19"/>
+      <c r="P1" s="20"/>
       <c r="W1">
         <v>15</v>
       </c>
@@ -18836,7 +18861,7 @@
         <v>181</v>
       </c>
       <c r="P22" t="s">
-        <v>594</v>
+        <v>591</v>
       </c>
     </row>
     <row r="23" spans="1:17" x14ac:dyDescent="0.25">
@@ -18886,7 +18911,7 @@
         <v>181</v>
       </c>
       <c r="P23" t="s">
-        <v>594</v>
+        <v>591</v>
       </c>
     </row>
     <row r="24" spans="1:17" x14ac:dyDescent="0.25">
@@ -20014,7 +20039,7 @@
         <v>4</v>
       </c>
       <c r="K50" t="s">
-        <v>585</v>
+        <v>584</v>
       </c>
       <c r="L50" t="s">
         <v>79</v>
@@ -20023,18 +20048,21 @@
         <v>81</v>
       </c>
       <c r="N50" t="s">
+        <v>595</v>
+      </c>
+      <c r="O50" t="s">
         <v>89</v>
       </c>
-      <c r="O50" t="s">
+      <c r="P50" t="s">
         <v>85</v>
       </c>
-      <c r="P50" t="s">
+      <c r="Q50" t="s">
         <v>10</v>
       </c>
-      <c r="Q50" t="s">
-        <v>554</v>
-      </c>
       <c r="R50" t="s">
+        <v>594</v>
+      </c>
+      <c r="S50" t="s">
         <v>547</v>
       </c>
     </row>
@@ -20070,7 +20098,7 @@
         <v>4</v>
       </c>
       <c r="K51" t="s">
-        <v>585</v>
+        <v>584</v>
       </c>
       <c r="L51" t="s">
         <v>79</v>
@@ -20079,18 +20107,21 @@
         <v>81</v>
       </c>
       <c r="N51" t="s">
+        <v>595</v>
+      </c>
+      <c r="O51" t="s">
         <v>89</v>
       </c>
-      <c r="O51" t="s">
+      <c r="P51" t="s">
         <v>85</v>
       </c>
-      <c r="P51" t="s">
+      <c r="Q51" t="s">
         <v>10</v>
       </c>
-      <c r="Q51" t="s">
-        <v>554</v>
-      </c>
       <c r="R51" t="s">
+        <v>594</v>
+      </c>
+      <c r="S51" t="s">
         <v>547</v>
       </c>
     </row>
@@ -20258,10 +20289,10 @@
         <v>5</v>
       </c>
       <c r="J55" t="s">
-        <v>591</v>
+        <v>589</v>
       </c>
       <c r="K55" t="s">
-        <v>592</v>
+        <v>590</v>
       </c>
       <c r="L55" t="s">
         <v>81</v>
@@ -20282,9 +20313,6 @@
         <v>546</v>
       </c>
       <c r="R55" t="s">
-        <v>3</v>
-      </c>
-      <c r="S55" t="s">
         <v>582</v>
       </c>
     </row>

</xml_diff>

<commit_message>
changed electricity generation to include the whole electricity output
</commit_message>
<xml_diff>
--- a/config/master_config.xlsx
+++ b/config/master_config.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\hyuga.kasai\Documents\Github\9th_Visualization\9th_edition_visualisation\config\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{30AB4862-2FAB-409A-9ABF-EFA4B98D1C77}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{1DE504A2-2EC0-4B50-A93B-EC5C9F0EC948}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-6750" yWindow="-16320" windowWidth="29040" windowHeight="15840" tabRatio="812" firstSheet="2" activeTab="10" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="22050" yWindow="-16395" windowWidth="29040" windowHeight="15840" tabRatio="812" firstSheet="1" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="9th_EBT_schema" sheetId="7" r:id="rId1"/>
@@ -390,7 +390,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="4435" uniqueCount="599">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="4434" uniqueCount="599">
   <si>
     <t>chart_type</t>
   </si>
@@ -5725,7 +5725,7 @@
   </sheetPr>
   <dimension ref="A1:B106"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A81" workbookViewId="0">
+    <sheetView topLeftCell="A81" workbookViewId="0">
       <selection activeCell="B103" sqref="B103"/>
     </sheetView>
   </sheetViews>
@@ -8302,8 +8302,8 @@
   </sheetPr>
   <dimension ref="A1:E54"/>
   <sheetViews>
-    <sheetView topLeftCell="A32" workbookViewId="0">
-      <selection activeCell="A55" sqref="A55:C56"/>
+    <sheetView tabSelected="1" topLeftCell="A32" workbookViewId="0">
+      <selection activeCell="C58" sqref="C58"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -9026,9 +9026,6 @@
       </c>
       <c r="C53" t="s">
         <v>166</v>
-      </c>
-      <c r="D53" t="s">
-        <v>364</v>
       </c>
     </row>
     <row r="54" spans="1:4" x14ac:dyDescent="0.25">

</xml_diff>

<commit_message>
added nuclear to electricity generation chart
</commit_message>
<xml_diff>
--- a/config/master_config.xlsx
+++ b/config/master_config.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\hyuga.kasai\Documents\Github\9th_Visualization\9th_edition_visualisation\config\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{1DE504A2-2EC0-4B50-A93B-EC5C9F0EC948}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{ACCE6BC9-6EDB-4643-B2FC-6B194E45412A}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="22050" yWindow="-16395" windowWidth="29040" windowHeight="15840" tabRatio="812" firstSheet="1" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="22050" yWindow="-16395" windowWidth="29040" windowHeight="15840" tabRatio="812" firstSheet="1" activeTab="7" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="9th_EBT_schema" sheetId="7" r:id="rId1"/>
@@ -390,7 +390,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="4434" uniqueCount="599">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="4435" uniqueCount="599">
   <si>
     <t>chart_type</t>
   </si>
@@ -8302,7 +8302,7 @@
   </sheetPr>
   <dimension ref="A1:E54"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A32" workbookViewId="0">
+    <sheetView topLeftCell="A32" workbookViewId="0">
       <selection activeCell="C58" sqref="C58"/>
     </sheetView>
   </sheetViews>
@@ -17906,10 +17906,10 @@
   </sheetPr>
   <dimension ref="A1:W55"/>
   <sheetViews>
-    <sheetView topLeftCell="E2" zoomScale="80" zoomScaleNormal="80" workbookViewId="0">
+    <sheetView tabSelected="1" topLeftCell="E2" zoomScale="80" zoomScaleNormal="80" workbookViewId="0">
       <pane ySplit="1" topLeftCell="A27" activePane="bottomLeft" state="frozen"/>
       <selection activeCell="E2" sqref="E2"/>
-      <selection pane="bottomLeft" activeCell="R50" sqref="R50:R51"/>
+      <selection pane="bottomLeft" activeCell="L55" sqref="L55"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -20292,24 +20292,27 @@
         <v>590</v>
       </c>
       <c r="L55" t="s">
+        <v>79</v>
+      </c>
+      <c r="M55" t="s">
         <v>81</v>
       </c>
-      <c r="M55" t="s">
+      <c r="N55" t="s">
         <v>83</v>
       </c>
-      <c r="N55" t="s">
+      <c r="O55" t="s">
         <v>85</v>
       </c>
-      <c r="O55" t="s">
+      <c r="P55" t="s">
         <v>89</v>
       </c>
-      <c r="P55" t="s">
+      <c r="Q55" t="s">
         <v>10</v>
       </c>
-      <c r="Q55" t="s">
+      <c r="R55" t="s">
         <v>546</v>
       </c>
-      <c r="R55" t="s">
+      <c r="S55" t="s">
         <v>582</v>
       </c>
     </row>

</xml_diff>

<commit_message>
final updates to handle new capacity data. added sheet_name col
</commit_message>
<xml_diff>
--- a/config/master_config.xlsx
+++ b/config/master_config.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\finbar.maunsell\github\9th_edition_visualisation\config\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E871AB24-3565-4443-B8C7-7DD456E1B89F}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{7E9AF23F-081F-4EE1-B3B9-E7C3C4ECAF73}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="28680" yWindow="-120" windowWidth="29040" windowHeight="15720" tabRatio="812" firstSheet="2" activeTab="7" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="28680" yWindow="-120" windowWidth="29040" windowHeight="15720" tabRatio="812" firstSheet="3" activeTab="4" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="9th_EBT_schema" sheetId="7" r:id="rId1"/>
@@ -402,7 +402,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="6174" uniqueCount="716">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="6174" uniqueCount="719">
   <si>
     <t>chart_type</t>
   </si>
@@ -2550,6 +2550,15 @@
   </si>
   <si>
     <t>motorcycle_freight</t>
+  </si>
+  <si>
+    <t>#323233</t>
+  </si>
+  <si>
+    <t>#323234</t>
+  </si>
+  <si>
+    <t>Transport stock shares</t>
   </si>
 </sst>
 </file>
@@ -6406,7 +6415,7 @@
   <dimension ref="A1:B172"/>
   <sheetViews>
     <sheetView topLeftCell="A160" workbookViewId="0">
-      <selection activeCell="D170" sqref="D170"/>
+      <selection activeCell="E176" sqref="E176"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -7771,7 +7780,7 @@
         <v>521</v>
       </c>
       <c r="B170" t="s">
-        <v>661</v>
+        <v>432</v>
       </c>
     </row>
     <row r="171" spans="1:2" x14ac:dyDescent="0.25">
@@ -7779,7 +7788,7 @@
         <v>522</v>
       </c>
       <c r="B171" t="s">
-        <v>661</v>
+        <v>716</v>
       </c>
     </row>
     <row r="172" spans="1:2" x14ac:dyDescent="0.25">
@@ -7787,7 +7796,7 @@
         <v>523</v>
       </c>
       <c r="B172" t="s">
-        <v>661</v>
+        <v>717</v>
       </c>
     </row>
   </sheetData>
@@ -13878,14 +13887,14 @@
   </sheetPr>
   <dimension ref="A1:I179"/>
   <sheetViews>
-    <sheetView topLeftCell="A135" workbookViewId="0">
-      <selection activeCell="D150" sqref="D150"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="C103" sqref="C103"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="2" max="2" width="29.140625" customWidth="1"/>
-    <col min="3" max="3" width="17" customWidth="1"/>
+    <col min="3" max="3" width="27.42578125" customWidth="1"/>
     <col min="4" max="4" width="25" customWidth="1"/>
     <col min="5" max="5" width="19.7109375" customWidth="1"/>
     <col min="6" max="6" width="27.5703125" customWidth="1"/>
@@ -16472,7 +16481,7 @@
         <v>572</v>
       </c>
     </row>
-    <row r="96" spans="1:9" hidden="1" x14ac:dyDescent="0.25">
+    <row r="96" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A96" t="s">
         <v>486</v>
       </c>
@@ -16480,7 +16489,7 @@
         <v>707</v>
       </c>
       <c r="C96" t="s">
-        <v>488</v>
+        <v>718</v>
       </c>
       <c r="D96" t="s">
         <v>693</v>
@@ -16501,7 +16510,7 @@
         <v>389</v>
       </c>
     </row>
-    <row r="97" spans="1:9" hidden="1" x14ac:dyDescent="0.25">
+    <row r="97" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A97" t="s">
         <v>486</v>
       </c>
@@ -16509,7 +16518,7 @@
         <v>707</v>
       </c>
       <c r="C97" t="s">
-        <v>488</v>
+        <v>718</v>
       </c>
       <c r="D97" t="s">
         <v>693</v>
@@ -16530,7 +16539,7 @@
         <v>391</v>
       </c>
     </row>
-    <row r="98" spans="1:9" hidden="1" x14ac:dyDescent="0.25">
+    <row r="98" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A98" t="s">
         <v>486</v>
       </c>
@@ -16538,7 +16547,7 @@
         <v>707</v>
       </c>
       <c r="C98" t="s">
-        <v>488</v>
+        <v>718</v>
       </c>
       <c r="D98" t="s">
         <v>694</v>
@@ -16559,7 +16568,7 @@
         <v>393</v>
       </c>
     </row>
-    <row r="99" spans="1:9" hidden="1" x14ac:dyDescent="0.25">
+    <row r="99" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A99" t="s">
         <v>486</v>
       </c>
@@ -16567,7 +16576,7 @@
         <v>707</v>
       </c>
       <c r="C99" t="s">
-        <v>488</v>
+        <v>718</v>
       </c>
       <c r="D99" t="s">
         <v>695</v>
@@ -16588,7 +16597,7 @@
         <v>395</v>
       </c>
     </row>
-    <row r="100" spans="1:9" hidden="1" x14ac:dyDescent="0.25">
+    <row r="100" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A100" t="s">
         <v>486</v>
       </c>
@@ -16596,7 +16605,7 @@
         <v>707</v>
       </c>
       <c r="C100" t="s">
-        <v>488</v>
+        <v>718</v>
       </c>
       <c r="D100" t="s">
         <v>696</v>
@@ -16617,7 +16626,7 @@
         <v>397</v>
       </c>
     </row>
-    <row r="101" spans="1:9" hidden="1" x14ac:dyDescent="0.25">
+    <row r="101" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A101" t="s">
         <v>486</v>
       </c>
@@ -16625,7 +16634,7 @@
         <v>707</v>
       </c>
       <c r="C101" t="s">
-        <v>488</v>
+        <v>718</v>
       </c>
       <c r="D101" t="s">
         <v>696</v>
@@ -16646,7 +16655,7 @@
         <v>398</v>
       </c>
     </row>
-    <row r="102" spans="1:9" hidden="1" x14ac:dyDescent="0.25">
+    <row r="102" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A102" t="s">
         <v>486</v>
       </c>
@@ -16654,7 +16663,7 @@
         <v>707</v>
       </c>
       <c r="C102" t="s">
-        <v>488</v>
+        <v>718</v>
       </c>
       <c r="D102" t="s">
         <v>697</v>
@@ -16675,7 +16684,7 @@
         <v>563</v>
       </c>
     </row>
-    <row r="103" spans="1:9" hidden="1" x14ac:dyDescent="0.25">
+    <row r="103" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A103" t="s">
         <v>486</v>
       </c>
@@ -16683,7 +16692,7 @@
         <v>707</v>
       </c>
       <c r="C103" t="s">
-        <v>488</v>
+        <v>718</v>
       </c>
       <c r="D103" t="s">
         <v>698</v>
@@ -16704,7 +16713,7 @@
         <v>515</v>
       </c>
     </row>
-    <row r="104" spans="1:9" hidden="1" x14ac:dyDescent="0.25">
+    <row r="104" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A104" t="s">
         <v>486</v>
       </c>
@@ -16712,7 +16721,7 @@
         <v>707</v>
       </c>
       <c r="C104" t="s">
-        <v>488</v>
+        <v>718</v>
       </c>
       <c r="D104" t="s">
         <v>686</v>
@@ -16733,7 +16742,7 @@
         <v>246</v>
       </c>
     </row>
-    <row r="105" spans="1:9" hidden="1" x14ac:dyDescent="0.25">
+    <row r="105" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A105" t="s">
         <v>486</v>
       </c>
@@ -16741,7 +16750,7 @@
         <v>707</v>
       </c>
       <c r="C105" t="s">
-        <v>488</v>
+        <v>718</v>
       </c>
       <c r="D105" t="s">
         <v>686</v>
@@ -16762,7 +16771,7 @@
         <v>250</v>
       </c>
     </row>
-    <row r="106" spans="1:9" hidden="1" x14ac:dyDescent="0.25">
+    <row r="106" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A106" t="s">
         <v>486</v>
       </c>
@@ -16770,7 +16779,7 @@
         <v>707</v>
       </c>
       <c r="C106" t="s">
-        <v>488</v>
+        <v>718</v>
       </c>
       <c r="D106" t="s">
         <v>687</v>
@@ -16791,7 +16800,7 @@
         <v>254</v>
       </c>
     </row>
-    <row r="107" spans="1:9" hidden="1" x14ac:dyDescent="0.25">
+    <row r="107" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A107" t="s">
         <v>486</v>
       </c>
@@ -16799,7 +16808,7 @@
         <v>707</v>
       </c>
       <c r="C107" t="s">
-        <v>488</v>
+        <v>718</v>
       </c>
       <c r="D107" t="s">
         <v>688</v>
@@ -16820,7 +16829,7 @@
         <v>258</v>
       </c>
     </row>
-    <row r="108" spans="1:9" hidden="1" x14ac:dyDescent="0.25">
+    <row r="108" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A108" t="s">
         <v>486</v>
       </c>
@@ -16828,7 +16837,7 @@
         <v>707</v>
       </c>
       <c r="C108" t="s">
-        <v>488</v>
+        <v>718</v>
       </c>
       <c r="D108" t="s">
         <v>689</v>
@@ -16849,7 +16858,7 @@
         <v>262</v>
       </c>
     </row>
-    <row r="109" spans="1:9" hidden="1" x14ac:dyDescent="0.25">
+    <row r="109" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A109" t="s">
         <v>486</v>
       </c>
@@ -16857,7 +16866,7 @@
         <v>707</v>
       </c>
       <c r="C109" t="s">
-        <v>488</v>
+        <v>718</v>
       </c>
       <c r="D109" t="s">
         <v>689</v>
@@ -16878,7 +16887,7 @@
         <v>266</v>
       </c>
     </row>
-    <row r="110" spans="1:9" hidden="1" x14ac:dyDescent="0.25">
+    <row r="110" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A110" t="s">
         <v>486</v>
       </c>
@@ -16886,7 +16895,7 @@
         <v>707</v>
       </c>
       <c r="C110" t="s">
-        <v>488</v>
+        <v>718</v>
       </c>
       <c r="D110" t="s">
         <v>690</v>
@@ -16907,7 +16916,7 @@
         <v>557</v>
       </c>
     </row>
-    <row r="111" spans="1:9" hidden="1" x14ac:dyDescent="0.25">
+    <row r="111" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A111" t="s">
         <v>486</v>
       </c>
@@ -16915,7 +16924,7 @@
         <v>707</v>
       </c>
       <c r="C111" t="s">
-        <v>488</v>
+        <v>718</v>
       </c>
       <c r="D111" t="s">
         <v>691</v>
@@ -16936,7 +16945,7 @@
         <v>508</v>
       </c>
     </row>
-    <row r="112" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="112" spans="1:9" hidden="1" x14ac:dyDescent="0.25">
       <c r="A112" t="s">
         <v>486</v>
       </c>
@@ -16965,7 +16974,7 @@
         <v>216</v>
       </c>
     </row>
-    <row r="113" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="113" spans="1:9" hidden="1" x14ac:dyDescent="0.25">
       <c r="A113" t="s">
         <v>486</v>
       </c>
@@ -16994,7 +17003,7 @@
         <v>222</v>
       </c>
     </row>
-    <row r="114" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="114" spans="1:9" hidden="1" x14ac:dyDescent="0.25">
       <c r="A114" t="s">
         <v>486</v>
       </c>
@@ -17023,7 +17032,7 @@
         <v>226</v>
       </c>
     </row>
-    <row r="115" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="115" spans="1:9" hidden="1" x14ac:dyDescent="0.25">
       <c r="A115" t="s">
         <v>486</v>
       </c>
@@ -17052,7 +17061,7 @@
         <v>231</v>
       </c>
     </row>
-    <row r="116" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="116" spans="1:9" hidden="1" x14ac:dyDescent="0.25">
       <c r="A116" t="s">
         <v>486</v>
       </c>
@@ -17081,7 +17090,7 @@
         <v>236</v>
       </c>
     </row>
-    <row r="117" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="117" spans="1:9" hidden="1" x14ac:dyDescent="0.25">
       <c r="A117" t="s">
         <v>486</v>
       </c>
@@ -17110,7 +17119,7 @@
         <v>242</v>
       </c>
     </row>
-    <row r="118" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="118" spans="1:9" hidden="1" x14ac:dyDescent="0.25">
       <c r="A118" t="s">
         <v>486</v>
       </c>
@@ -17139,7 +17148,7 @@
         <v>556</v>
       </c>
     </row>
-    <row r="119" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="119" spans="1:9" hidden="1" x14ac:dyDescent="0.25">
       <c r="A119" t="s">
         <v>486</v>
       </c>
@@ -17168,7 +17177,7 @@
         <v>507</v>
       </c>
     </row>
-    <row r="120" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="120" spans="1:9" hidden="1" x14ac:dyDescent="0.25">
       <c r="A120" t="s">
         <v>486</v>
       </c>
@@ -17197,7 +17206,7 @@
         <v>246</v>
       </c>
     </row>
-    <row r="121" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="121" spans="1:9" hidden="1" x14ac:dyDescent="0.25">
       <c r="A121" t="s">
         <v>486</v>
       </c>
@@ -17226,7 +17235,7 @@
         <v>250</v>
       </c>
     </row>
-    <row r="122" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="122" spans="1:9" hidden="1" x14ac:dyDescent="0.25">
       <c r="A122" t="s">
         <v>486</v>
       </c>
@@ -17255,7 +17264,7 @@
         <v>254</v>
       </c>
     </row>
-    <row r="123" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="123" spans="1:9" hidden="1" x14ac:dyDescent="0.25">
       <c r="A123" t="s">
         <v>486</v>
       </c>
@@ -17284,7 +17293,7 @@
         <v>258</v>
       </c>
     </row>
-    <row r="124" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="124" spans="1:9" hidden="1" x14ac:dyDescent="0.25">
       <c r="A124" t="s">
         <v>486</v>
       </c>
@@ -17313,7 +17322,7 @@
         <v>262</v>
       </c>
     </row>
-    <row r="125" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="125" spans="1:9" hidden="1" x14ac:dyDescent="0.25">
       <c r="A125" t="s">
         <v>486</v>
       </c>
@@ -17342,7 +17351,7 @@
         <v>266</v>
       </c>
     </row>
-    <row r="126" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="126" spans="1:9" hidden="1" x14ac:dyDescent="0.25">
       <c r="A126" t="s">
         <v>486</v>
       </c>
@@ -17371,7 +17380,7 @@
         <v>557</v>
       </c>
     </row>
-    <row r="127" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="127" spans="1:9" hidden="1" x14ac:dyDescent="0.25">
       <c r="A127" t="s">
         <v>486</v>
       </c>
@@ -17400,7 +17409,7 @@
         <v>508</v>
       </c>
     </row>
-    <row r="128" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="128" spans="1:9" hidden="1" x14ac:dyDescent="0.25">
       <c r="A128" t="s">
         <v>486</v>
       </c>
@@ -17429,7 +17438,7 @@
         <v>270</v>
       </c>
     </row>
-    <row r="129" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="129" spans="1:9" hidden="1" x14ac:dyDescent="0.25">
       <c r="A129" t="s">
         <v>486</v>
       </c>
@@ -17458,7 +17467,7 @@
         <v>274</v>
       </c>
     </row>
-    <row r="130" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="130" spans="1:9" hidden="1" x14ac:dyDescent="0.25">
       <c r="A130" t="s">
         <v>486</v>
       </c>
@@ -17487,7 +17496,7 @@
         <v>278</v>
       </c>
     </row>
-    <row r="131" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="131" spans="1:9" hidden="1" x14ac:dyDescent="0.25">
       <c r="A131" t="s">
         <v>486</v>
       </c>
@@ -17516,7 +17525,7 @@
         <v>283</v>
       </c>
     </row>
-    <row r="132" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="132" spans="1:9" hidden="1" x14ac:dyDescent="0.25">
       <c r="A132" t="s">
         <v>486</v>
       </c>
@@ -17545,7 +17554,7 @@
         <v>288</v>
       </c>
     </row>
-    <row r="133" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="133" spans="1:9" hidden="1" x14ac:dyDescent="0.25">
       <c r="A133" t="s">
         <v>486</v>
       </c>
@@ -17574,7 +17583,7 @@
         <v>293</v>
       </c>
     </row>
-    <row r="134" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="134" spans="1:9" hidden="1" x14ac:dyDescent="0.25">
       <c r="A134" t="s">
         <v>486</v>
       </c>
@@ -17603,7 +17612,7 @@
         <v>558</v>
       </c>
     </row>
-    <row r="135" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="135" spans="1:9" hidden="1" x14ac:dyDescent="0.25">
       <c r="A135" t="s">
         <v>486</v>
       </c>
@@ -17632,7 +17641,7 @@
         <v>509</v>
       </c>
     </row>
-    <row r="136" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="136" spans="1:9" hidden="1" x14ac:dyDescent="0.25">
       <c r="A136" t="s">
         <v>486</v>
       </c>
@@ -17661,7 +17670,7 @@
         <v>297</v>
       </c>
     </row>
-    <row r="137" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="137" spans="1:9" hidden="1" x14ac:dyDescent="0.25">
       <c r="A137" t="s">
         <v>486</v>
       </c>
@@ -17690,7 +17699,7 @@
         <v>302</v>
       </c>
     </row>
-    <row r="138" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="138" spans="1:9" hidden="1" x14ac:dyDescent="0.25">
       <c r="A138" t="s">
         <v>486</v>
       </c>
@@ -17719,7 +17728,7 @@
         <v>307</v>
       </c>
     </row>
-    <row r="139" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="139" spans="1:9" hidden="1" x14ac:dyDescent="0.25">
       <c r="A139" t="s">
         <v>486</v>
       </c>
@@ -17748,7 +17757,7 @@
         <v>312</v>
       </c>
     </row>
-    <row r="140" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="140" spans="1:9" hidden="1" x14ac:dyDescent="0.25">
       <c r="A140" t="s">
         <v>486</v>
       </c>
@@ -17777,7 +17786,7 @@
         <v>317</v>
       </c>
     </row>
-    <row r="141" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="141" spans="1:9" hidden="1" x14ac:dyDescent="0.25">
       <c r="A141" t="s">
         <v>486</v>
       </c>
@@ -17806,7 +17815,7 @@
         <v>322</v>
       </c>
     </row>
-    <row r="142" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="142" spans="1:9" hidden="1" x14ac:dyDescent="0.25">
       <c r="A142" t="s">
         <v>486</v>
       </c>
@@ -17835,7 +17844,7 @@
         <v>559</v>
       </c>
     </row>
-    <row r="143" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="143" spans="1:9" hidden="1" x14ac:dyDescent="0.25">
       <c r="A143" t="s">
         <v>486</v>
       </c>
@@ -17864,7 +17873,7 @@
         <v>510</v>
       </c>
     </row>
-    <row r="144" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="144" spans="1:9" hidden="1" x14ac:dyDescent="0.25">
       <c r="A144" t="s">
         <v>486</v>
       </c>
@@ -17893,7 +17902,7 @@
         <v>501</v>
       </c>
     </row>
-    <row r="145" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="145" spans="1:9" hidden="1" x14ac:dyDescent="0.25">
       <c r="A145" t="s">
         <v>486</v>
       </c>
@@ -17922,7 +17931,7 @@
         <v>502</v>
       </c>
     </row>
-    <row r="146" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="146" spans="1:9" hidden="1" x14ac:dyDescent="0.25">
       <c r="A146" t="s">
         <v>486</v>
       </c>
@@ -17951,7 +17960,7 @@
         <v>506</v>
       </c>
     </row>
-    <row r="147" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="147" spans="1:9" hidden="1" x14ac:dyDescent="0.25">
       <c r="A147" t="s">
         <v>486</v>
       </c>
@@ -17980,7 +17989,7 @@
         <v>511</v>
       </c>
     </row>
-    <row r="148" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="148" spans="1:9" hidden="1" x14ac:dyDescent="0.25">
       <c r="A148" t="s">
         <v>486</v>
       </c>
@@ -18009,7 +18018,7 @@
         <v>327</v>
       </c>
     </row>
-    <row r="149" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="149" spans="1:9" hidden="1" x14ac:dyDescent="0.25">
       <c r="A149" t="s">
         <v>486</v>
       </c>
@@ -18038,7 +18047,7 @@
         <v>332</v>
       </c>
     </row>
-    <row r="150" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="150" spans="1:9" hidden="1" x14ac:dyDescent="0.25">
       <c r="A150" t="s">
         <v>486</v>
       </c>
@@ -18067,7 +18076,7 @@
         <v>337</v>
       </c>
     </row>
-    <row r="151" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="151" spans="1:9" hidden="1" x14ac:dyDescent="0.25">
       <c r="A151" t="s">
         <v>486</v>
       </c>
@@ -18096,7 +18105,7 @@
         <v>341</v>
       </c>
     </row>
-    <row r="152" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="152" spans="1:9" hidden="1" x14ac:dyDescent="0.25">
       <c r="A152" t="s">
         <v>486</v>
       </c>
@@ -18125,7 +18134,7 @@
         <v>344</v>
       </c>
     </row>
-    <row r="153" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="153" spans="1:9" hidden="1" x14ac:dyDescent="0.25">
       <c r="A153" t="s">
         <v>486</v>
       </c>
@@ -18154,7 +18163,7 @@
         <v>347</v>
       </c>
     </row>
-    <row r="154" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="154" spans="1:9" hidden="1" x14ac:dyDescent="0.25">
       <c r="A154" t="s">
         <v>486</v>
       </c>
@@ -18183,7 +18192,7 @@
         <v>560</v>
       </c>
     </row>
-    <row r="155" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="155" spans="1:9" hidden="1" x14ac:dyDescent="0.25">
       <c r="A155" t="s">
         <v>486</v>
       </c>
@@ -18212,7 +18221,7 @@
         <v>512</v>
       </c>
     </row>
-    <row r="156" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="156" spans="1:9" hidden="1" x14ac:dyDescent="0.25">
       <c r="A156" t="s">
         <v>486</v>
       </c>
@@ -18241,7 +18250,7 @@
         <v>351</v>
       </c>
     </row>
-    <row r="157" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="157" spans="1:9" hidden="1" x14ac:dyDescent="0.25">
       <c r="A157" t="s">
         <v>486</v>
       </c>
@@ -18270,7 +18279,7 @@
         <v>355</v>
       </c>
     </row>
-    <row r="158" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="158" spans="1:9" hidden="1" x14ac:dyDescent="0.25">
       <c r="A158" t="s">
         <v>486</v>
       </c>
@@ -18299,7 +18308,7 @@
         <v>359</v>
       </c>
     </row>
-    <row r="159" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="159" spans="1:9" hidden="1" x14ac:dyDescent="0.25">
       <c r="A159" t="s">
         <v>486</v>
       </c>
@@ -18328,7 +18337,7 @@
         <v>363</v>
       </c>
     </row>
-    <row r="160" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="160" spans="1:9" hidden="1" x14ac:dyDescent="0.25">
       <c r="A160" t="s">
         <v>486</v>
       </c>
@@ -18357,7 +18366,7 @@
         <v>367</v>
       </c>
     </row>
-    <row r="161" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="161" spans="1:9" hidden="1" x14ac:dyDescent="0.25">
       <c r="A161" t="s">
         <v>486</v>
       </c>
@@ -18386,7 +18395,7 @@
         <v>371</v>
       </c>
     </row>
-    <row r="162" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="162" spans="1:9" hidden="1" x14ac:dyDescent="0.25">
       <c r="A162" t="s">
         <v>486</v>
       </c>
@@ -18415,7 +18424,7 @@
         <v>561</v>
       </c>
     </row>
-    <row r="163" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="163" spans="1:9" hidden="1" x14ac:dyDescent="0.25">
       <c r="A163" t="s">
         <v>486</v>
       </c>
@@ -18444,7 +18453,7 @@
         <v>513</v>
       </c>
     </row>
-    <row r="164" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="164" spans="1:9" hidden="1" x14ac:dyDescent="0.25">
       <c r="A164" t="s">
         <v>486</v>
       </c>
@@ -18473,7 +18482,7 @@
         <v>375</v>
       </c>
     </row>
-    <row r="165" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="165" spans="1:9" hidden="1" x14ac:dyDescent="0.25">
       <c r="A165" t="s">
         <v>486</v>
       </c>
@@ -18502,7 +18511,7 @@
         <v>378</v>
       </c>
     </row>
-    <row r="166" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="166" spans="1:9" hidden="1" x14ac:dyDescent="0.25">
       <c r="A166" t="s">
         <v>486</v>
       </c>
@@ -18531,7 +18540,7 @@
         <v>381</v>
       </c>
     </row>
-    <row r="167" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="167" spans="1:9" hidden="1" x14ac:dyDescent="0.25">
       <c r="A167" t="s">
         <v>486</v>
       </c>
@@ -18560,7 +18569,7 @@
         <v>383</v>
       </c>
     </row>
-    <row r="168" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="168" spans="1:9" hidden="1" x14ac:dyDescent="0.25">
       <c r="A168" t="s">
         <v>486</v>
       </c>
@@ -18589,7 +18598,7 @@
         <v>385</v>
       </c>
     </row>
-    <row r="169" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="169" spans="1:9" hidden="1" x14ac:dyDescent="0.25">
       <c r="A169" t="s">
         <v>486</v>
       </c>
@@ -18618,7 +18627,7 @@
         <v>387</v>
       </c>
     </row>
-    <row r="170" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="170" spans="1:9" hidden="1" x14ac:dyDescent="0.25">
       <c r="A170" t="s">
         <v>486</v>
       </c>
@@ -18647,7 +18656,7 @@
         <v>562</v>
       </c>
     </row>
-    <row r="171" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="171" spans="1:9" hidden="1" x14ac:dyDescent="0.25">
       <c r="A171" t="s">
         <v>486</v>
       </c>
@@ -18676,7 +18685,7 @@
         <v>514</v>
       </c>
     </row>
-    <row r="172" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="172" spans="1:9" hidden="1" x14ac:dyDescent="0.25">
       <c r="A172" t="s">
         <v>486</v>
       </c>
@@ -18705,7 +18714,7 @@
         <v>389</v>
       </c>
     </row>
-    <row r="173" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="173" spans="1:9" hidden="1" x14ac:dyDescent="0.25">
       <c r="A173" t="s">
         <v>486</v>
       </c>
@@ -18734,7 +18743,7 @@
         <v>391</v>
       </c>
     </row>
-    <row r="174" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="174" spans="1:9" hidden="1" x14ac:dyDescent="0.25">
       <c r="A174" t="s">
         <v>486</v>
       </c>
@@ -18763,7 +18772,7 @@
         <v>393</v>
       </c>
     </row>
-    <row r="175" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="175" spans="1:9" hidden="1" x14ac:dyDescent="0.25">
       <c r="A175" t="s">
         <v>486</v>
       </c>
@@ -18792,7 +18801,7 @@
         <v>395</v>
       </c>
     </row>
-    <row r="176" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="176" spans="1:9" hidden="1" x14ac:dyDescent="0.25">
       <c r="A176" t="s">
         <v>486</v>
       </c>
@@ -18821,7 +18830,7 @@
         <v>397</v>
       </c>
     </row>
-    <row r="177" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="177" spans="1:9" hidden="1" x14ac:dyDescent="0.25">
       <c r="A177" t="s">
         <v>486</v>
       </c>
@@ -18850,7 +18859,7 @@
         <v>398</v>
       </c>
     </row>
-    <row r="178" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="178" spans="1:9" hidden="1" x14ac:dyDescent="0.25">
       <c r="A178" t="s">
         <v>486</v>
       </c>
@@ -18879,7 +18888,7 @@
         <v>563</v>
       </c>
     </row>
-    <row r="179" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="179" spans="1:9" hidden="1" x14ac:dyDescent="0.25">
       <c r="A179" t="s">
         <v>486</v>
       </c>
@@ -18912,7 +18921,7 @@
   <autoFilter ref="A1:I179" xr:uid="{57DE5463-B504-41DB-9442-85F0E395C61E}">
     <filterColumn colId="1">
       <filters>
-        <filter val="transport_activity"/>
+        <filter val="transport_stock_shares"/>
       </filters>
     </filterColumn>
   </autoFilter>
@@ -22471,8 +22480,8 @@
   </sheetPr>
   <dimension ref="A1:W80"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A39" zoomScale="80" zoomScaleNormal="80" workbookViewId="0">
-      <selection activeCell="E80" sqref="E80"/>
+    <sheetView topLeftCell="A38" zoomScale="80" zoomScaleNormal="80" workbookViewId="0">
+      <selection activeCell="E72" sqref="E72"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -25775,7 +25784,7 @@
         <v>493</v>
       </c>
       <c r="G72" t="s">
-        <v>488</v>
+        <v>718</v>
       </c>
       <c r="H72" t="s">
         <v>686</v>
@@ -25816,7 +25825,7 @@
         <v>493</v>
       </c>
       <c r="G73" t="s">
-        <v>488</v>
+        <v>718</v>
       </c>
       <c r="H73" t="s">
         <v>693</v>

</xml_diff>

<commit_message>
added spec by economy
</commit_message>
<xml_diff>
--- a/config/master_config.xlsx
+++ b/config/master_config.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\finbar.maunsell\github\9th_edition_visualisation\config\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{7E9AF23F-081F-4EE1-B3B9-E7C3C4ECAF73}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{661377D0-DEC2-45E4-B508-A66ECC0B407E}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="28680" yWindow="-120" windowWidth="29040" windowHeight="15720" tabRatio="812" firstSheet="3" activeTab="4" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="28680" yWindow="-120" windowWidth="29040" windowHeight="15720" tabRatio="812" firstSheet="3" activeTab="8" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="9th_EBT_schema" sheetId="7" r:id="rId1"/>
@@ -21,7 +21,7 @@
     <sheet name="emissions_fuels_plotting" sheetId="13" r:id="rId6"/>
     <sheet name="emissions_sectors_plotting" sheetId="14" r:id="rId7"/>
     <sheet name="two_dimensional_plots" sheetId="18" r:id="rId8"/>
-    <sheet name="economy_specific" sheetId="22" r:id="rId9"/>
+    <sheet name="economy_specific_2d" sheetId="22" r:id="rId9"/>
     <sheet name="one_dimensional_plots" sheetId="16" r:id="rId10"/>
     <sheet name="plotting_name_to_label" sheetId="10" r:id="rId11"/>
     <sheet name="colors" sheetId="9" r:id="rId12"/>
@@ -315,6 +315,64 @@
     <author>Finbar Maunsell</author>
   </authors>
   <commentList>
+    <comment ref="E1" authorId="0" shapeId="0" xr:uid="{AD810412-828F-4728-BB16-5FD24C46A520}">
+      <text>
+        <r>
+          <rPr>
+            <b/>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <charset val="1"/>
+          </rPr>
+          <t>Finbar Maunsell:</t>
+        </r>
+        <r>
+          <rPr>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <charset val="1"/>
+          </rPr>
+          <t xml:space="preserve">
+table should be used if you need/want a sepaarate table for this data. This will be needed if the data wouldn’t be available otherwise, OR if the chart is a bar chart in which case we will show it in 10 year splits, so a new table will be needed for that</t>
+        </r>
+      </text>
+    </comment>
+    <comment ref="I1" authorId="0" shapeId="0" xr:uid="{03F3F105-5ABC-4D70-AD22-878D910AF562}">
+      <text>
+        <r>
+          <rPr>
+            <b/>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <charset val="1"/>
+          </rPr>
+          <t>Finbar Maunsell:</t>
+        </r>
+        <r>
+          <rPr>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <charset val="1"/>
+          </rPr>
+          <t xml:space="preserve">
+These numbers are just placeholders, if you need more plotting names just extend the numbers to X+wahtever</t>
+        </r>
+      </text>
+    </comment>
+  </commentList>
+</comments>
+</file>
+
+<file path=xl/comments8.xml><?xml version="1.0" encoding="utf-8"?>
+<comments xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="xr">
+  <authors>
+    <author>Finbar Maunsell</author>
+  </authors>
+  <commentList>
     <comment ref="C1" authorId="0" shapeId="0" xr:uid="{1258B623-61DE-4825-BC11-55DF89ECC451}">
       <text>
         <r>
@@ -343,7 +401,7 @@
 </comments>
 </file>
 
-<file path=xl/comments8.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/comments9.xml><?xml version="1.0" encoding="utf-8"?>
 <comments xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="xr">
   <authors>
     <author>Finbar Maunsell</author>
@@ -402,7 +460,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="6174" uniqueCount="719">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="6182" uniqueCount="719">
   <si>
     <t>chart_type</t>
   </si>
@@ -2696,7 +2754,7 @@
       </patternFill>
     </fill>
   </fills>
-  <borders count="6">
+  <borders count="7">
     <border>
       <left/>
       <right/>
@@ -2767,12 +2825,23 @@
       <bottom/>
       <diagonal/>
     </border>
+    <border>
+      <left/>
+      <right style="thin">
+        <color auto="1"/>
+      </right>
+      <top/>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="7" fillId="9" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="20">
+  <cellXfs count="21">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="top"/>
@@ -2809,6 +2878,7 @@
     <xf numFmtId="0" fontId="2" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="top"/>
     </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="Neutral" xfId="1" builtinId="28"/>
@@ -13887,8 +13957,8 @@
   </sheetPr>
   <dimension ref="A1:I179"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C103" sqref="C103"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="D181" sqref="D181"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -22480,8 +22550,8 @@
   </sheetPr>
   <dimension ref="A1:W80"/>
   <sheetViews>
-    <sheetView topLeftCell="A38" zoomScale="80" zoomScaleNormal="80" workbookViewId="0">
-      <selection activeCell="E72" sqref="E72"/>
+    <sheetView zoomScale="80" zoomScaleNormal="80" workbookViewId="0">
+      <selection sqref="A1:W1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -26078,708 +26148,779 @@
 </file>
 
 <file path=xl/worksheets/sheet9.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{1FB41151-CF9C-4A5D-8C89-4DDD65A34550}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{1FB41151-CF9C-4A5D-8C89-4DDD65A34550}">
   <sheetPr>
     <tabColor theme="9" tint="0.39997558519241921"/>
   </sheetPr>
-  <dimension ref="A1:T19"/>
+  <dimension ref="A1:X13"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection sqref="A1:U4"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="C10" sqref="C10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <sheetData>
-    <row r="1" spans="1:20" x14ac:dyDescent="0.25">
-      <c r="A1" t="s">
-        <v>485</v>
-      </c>
-      <c r="B1" t="s">
-        <v>24</v>
-      </c>
-      <c r="C1" t="s">
-        <v>24</v>
-      </c>
-      <c r="D1">
+    <row r="1" spans="1:24" x14ac:dyDescent="0.25">
+      <c r="A1" s="20" t="s">
+        <v>208</v>
+      </c>
+      <c r="B1" s="1" t="s">
+        <v>484</v>
+      </c>
+      <c r="C1" s="1" t="s">
+        <v>524</v>
+      </c>
+      <c r="D1" s="1" t="s">
+        <v>463</v>
+      </c>
+      <c r="E1" s="1" t="s">
+        <v>462</v>
+      </c>
+      <c r="F1" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="G1" s="1" t="s">
+        <v>492</v>
+      </c>
+      <c r="H1" s="1" t="s">
+        <v>493</v>
+      </c>
+      <c r="I1" s="1">
+        <v>0</v>
+      </c>
+      <c r="J1" s="1">
         <v>1</v>
       </c>
-      <c r="E1" t="s">
+      <c r="K1" s="1">
         <v>2</v>
       </c>
-      <c r="F1" t="s">
-        <v>49</v>
-      </c>
-      <c r="G1" t="s">
-        <v>24</v>
-      </c>
-      <c r="H1" t="s">
+      <c r="L1" s="1">
+        <v>3</v>
+      </c>
+      <c r="M1" s="1">
+        <v>4</v>
+      </c>
+      <c r="N1" s="1">
+        <v>5</v>
+      </c>
+      <c r="O1" s="1">
+        <v>6</v>
+      </c>
+      <c r="P1" s="1">
+        <v>7</v>
+      </c>
+      <c r="Q1" s="1">
+        <v>8</v>
+      </c>
+      <c r="R1" s="1">
+        <v>9</v>
+      </c>
+      <c r="S1" s="1">
+        <v>10</v>
+      </c>
+      <c r="T1" s="14">
         <v>11</v>
       </c>
-      <c r="I1" t="s">
-        <v>5</v>
-      </c>
-      <c r="J1" t="s">
-        <v>4</v>
-      </c>
-      <c r="K1" t="s">
+      <c r="U1" s="14">
         <v>12</v>
       </c>
-      <c r="L1" t="s">
-        <v>83</v>
-      </c>
-      <c r="M1" t="s">
-        <v>10</v>
-      </c>
-      <c r="N1" t="s">
-        <v>28</v>
-      </c>
-      <c r="O1" t="s">
-        <v>3</v>
-      </c>
-      <c r="P1" t="s">
-        <v>95</v>
-      </c>
-      <c r="Q1" t="s">
-        <v>155</v>
-      </c>
-    </row>
-    <row r="2" spans="1:20" x14ac:dyDescent="0.25">
+      <c r="V1" s="14">
+        <v>13</v>
+      </c>
+      <c r="W1" s="14">
+        <v>14</v>
+      </c>
+      <c r="X1" s="14">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="2" spans="1:24" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
-        <v>485</v>
+        <v>212</v>
       </c>
       <c r="B2" t="s">
-        <v>24</v>
+        <v>485</v>
       </c>
       <c r="C2" t="s">
         <v>24</v>
       </c>
-      <c r="D2">
+      <c r="D2" t="s">
+        <v>24</v>
+      </c>
+      <c r="E2">
         <v>1</v>
       </c>
-      <c r="E2" t="s">
-        <v>7</v>
-      </c>
       <c r="F2" t="s">
+        <v>2</v>
+      </c>
+      <c r="G2" t="s">
         <v>49</v>
       </c>
-      <c r="G2" t="s">
+      <c r="H2" t="s">
         <v>24</v>
       </c>
-      <c r="H2" t="s">
+      <c r="I2" t="s">
         <v>11</v>
       </c>
-      <c r="I2" t="s">
+      <c r="J2" t="s">
         <v>5</v>
       </c>
-      <c r="J2" t="s">
+      <c r="K2" t="s">
         <v>4</v>
       </c>
-      <c r="K2" t="s">
+      <c r="L2" t="s">
         <v>12</v>
       </c>
-      <c r="L2" t="s">
+      <c r="M2" t="s">
         <v>83</v>
       </c>
-      <c r="M2" t="s">
+      <c r="N2" t="s">
         <v>10</v>
       </c>
-      <c r="N2" t="s">
+      <c r="O2" t="s">
         <v>28</v>
       </c>
-      <c r="O2" t="s">
+      <c r="P2" t="s">
         <v>3</v>
       </c>
-      <c r="P2" t="s">
+      <c r="Q2" t="s">
         <v>95</v>
       </c>
-      <c r="Q2" t="s">
+      <c r="R2" t="s">
         <v>155</v>
       </c>
     </row>
-    <row r="3" spans="1:20" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:24" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
-        <v>485</v>
+        <v>212</v>
       </c>
       <c r="B3" t="s">
-        <v>24</v>
+        <v>485</v>
       </c>
       <c r="C3" t="s">
         <v>24</v>
       </c>
-      <c r="D3">
-        <v>2</v>
-      </c>
-      <c r="E3" t="s">
-        <v>2</v>
+      <c r="D3" t="s">
+        <v>24</v>
+      </c>
+      <c r="E3">
+        <v>1</v>
       </c>
       <c r="F3" t="s">
-        <v>68</v>
+        <v>7</v>
       </c>
       <c r="G3" t="s">
+        <v>49</v>
+      </c>
+      <c r="H3" t="s">
         <v>24</v>
       </c>
-      <c r="H3" t="s">
-        <v>175</v>
-      </c>
       <c r="I3" t="s">
-        <v>189</v>
+        <v>11</v>
       </c>
       <c r="J3" t="s">
-        <v>173</v>
+        <v>5</v>
       </c>
       <c r="K3" t="s">
-        <v>171</v>
+        <v>4</v>
       </c>
       <c r="L3" t="s">
-        <v>583</v>
+        <v>12</v>
       </c>
       <c r="M3" t="s">
-        <v>177</v>
+        <v>83</v>
       </c>
       <c r="N3" t="s">
-        <v>179</v>
+        <v>10</v>
       </c>
       <c r="O3" t="s">
-        <v>181</v>
+        <v>28</v>
       </c>
       <c r="P3" t="s">
-        <v>575</v>
-      </c>
-    </row>
-    <row r="4" spans="1:20" x14ac:dyDescent="0.25">
+        <v>3</v>
+      </c>
+      <c r="Q3" t="s">
+        <v>95</v>
+      </c>
+      <c r="R3" t="s">
+        <v>155</v>
+      </c>
+    </row>
+    <row r="4" spans="1:24" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
-        <v>485</v>
+        <v>212</v>
       </c>
       <c r="B4" t="s">
-        <v>24</v>
+        <v>485</v>
       </c>
       <c r="C4" t="s">
         <v>24</v>
       </c>
-      <c r="D4">
+      <c r="D4" t="s">
+        <v>24</v>
+      </c>
+      <c r="E4">
+        <v>2</v>
+      </c>
+      <c r="F4" t="s">
+        <v>2</v>
+      </c>
+      <c r="G4" t="s">
+        <v>68</v>
+      </c>
+      <c r="H4" t="s">
+        <v>24</v>
+      </c>
+      <c r="I4" t="s">
+        <v>175</v>
+      </c>
+      <c r="J4" t="s">
+        <v>189</v>
+      </c>
+      <c r="K4" t="s">
+        <v>173</v>
+      </c>
+      <c r="L4" t="s">
+        <v>171</v>
+      </c>
+      <c r="M4" t="s">
+        <v>583</v>
+      </c>
+      <c r="N4" t="s">
+        <v>177</v>
+      </c>
+      <c r="O4" t="s">
+        <v>179</v>
+      </c>
+      <c r="P4" t="s">
+        <v>181</v>
+      </c>
+      <c r="Q4" t="s">
+        <v>575</v>
+      </c>
+    </row>
+    <row r="5" spans="1:24" x14ac:dyDescent="0.25">
+      <c r="A5" t="s">
+        <v>212</v>
+      </c>
+      <c r="B5" t="s">
+        <v>485</v>
+      </c>
+      <c r="C5" t="s">
+        <v>24</v>
+      </c>
+      <c r="D5" t="s">
+        <v>24</v>
+      </c>
+      <c r="E5">
         <v>3</v>
       </c>
-      <c r="E4" t="s">
+      <c r="F5" t="s">
         <v>8</v>
       </c>
-      <c r="F4" t="s">
+      <c r="G5" t="s">
         <v>68</v>
       </c>
-      <c r="G4" t="s">
+      <c r="H5" t="s">
         <v>24</v>
       </c>
-      <c r="H4" t="s">
+      <c r="I5" t="s">
         <v>175</v>
       </c>
-      <c r="I4" t="s">
+      <c r="J5" t="s">
         <v>189</v>
       </c>
-      <c r="J4" t="s">
+      <c r="K5" t="s">
         <v>173</v>
       </c>
-      <c r="K4" t="s">
+      <c r="L5" t="s">
         <v>171</v>
       </c>
-      <c r="L4" t="s">
+      <c r="M5" t="s">
         <v>583</v>
       </c>
-      <c r="M4" t="s">
+      <c r="N5" t="s">
         <v>177</v>
       </c>
-      <c r="N4" t="s">
+      <c r="O5" t="s">
         <v>179</v>
       </c>
-      <c r="O4" t="s">
+      <c r="P5" t="s">
         <v>181</v>
       </c>
-      <c r="P4" t="s">
+      <c r="Q5" t="s">
         <v>575</v>
       </c>
     </row>
-    <row r="6" spans="1:20" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:24" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
-        <v>485</v>
+        <v>289</v>
       </c>
       <c r="B6" t="s">
-        <v>673</v>
+        <v>485</v>
       </c>
       <c r="C6" t="s">
         <v>673</v>
       </c>
-      <c r="D6">
+      <c r="D6" t="s">
+        <v>673</v>
+      </c>
+      <c r="E6">
         <v>1</v>
       </c>
-      <c r="E6" t="s">
+      <c r="F6" t="s">
         <v>2</v>
       </c>
-      <c r="F6" t="s">
+      <c r="G6" t="s">
         <v>49</v>
       </c>
-      <c r="G6" t="s">
+      <c r="H6" t="s">
         <v>24</v>
       </c>
-      <c r="H6" t="s">
+      <c r="I6" t="s">
         <v>11</v>
       </c>
-      <c r="I6" t="s">
+      <c r="J6" t="s">
         <v>5</v>
       </c>
-      <c r="J6" t="s">
+      <c r="K6" t="s">
         <v>4</v>
       </c>
-      <c r="K6" t="s">
+      <c r="L6" t="s">
         <v>12</v>
       </c>
-      <c r="L6" t="s">
+      <c r="M6" t="s">
         <v>83</v>
       </c>
-      <c r="M6" t="s">
+      <c r="N6" t="s">
         <v>10</v>
       </c>
-      <c r="N6" t="s">
+      <c r="O6" t="s">
         <v>28</v>
       </c>
-      <c r="O6" t="s">
+      <c r="P6" t="s">
         <v>3</v>
       </c>
-      <c r="P6" t="s">
+      <c r="Q6" t="s">
         <v>95</v>
       </c>
-      <c r="Q6" t="s">
+      <c r="R6" t="s">
         <v>155</v>
       </c>
     </row>
-    <row r="7" spans="1:20" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:24" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
-        <v>485</v>
+        <v>289</v>
       </c>
       <c r="B7" t="s">
-        <v>673</v>
+        <v>485</v>
       </c>
       <c r="C7" t="s">
         <v>673</v>
       </c>
-      <c r="D7">
+      <c r="D7" t="s">
+        <v>673</v>
+      </c>
+      <c r="E7">
         <v>1</v>
       </c>
-      <c r="E7" t="s">
+      <c r="F7" t="s">
         <v>7</v>
       </c>
-      <c r="F7" t="s">
+      <c r="G7" t="s">
         <v>49</v>
       </c>
-      <c r="G7" t="s">
+      <c r="H7" t="s">
         <v>24</v>
       </c>
-      <c r="H7" t="s">
+      <c r="I7" t="s">
         <v>11</v>
       </c>
-      <c r="I7" t="s">
+      <c r="J7" t="s">
         <v>5</v>
       </c>
-      <c r="J7" t="s">
+      <c r="K7" t="s">
         <v>4</v>
       </c>
-      <c r="K7" t="s">
+      <c r="L7" t="s">
         <v>12</v>
       </c>
-      <c r="L7" t="s">
+      <c r="M7" t="s">
         <v>83</v>
       </c>
-      <c r="M7" t="s">
+      <c r="N7" t="s">
         <v>10</v>
       </c>
-      <c r="N7" t="s">
+      <c r="O7" t="s">
         <v>28</v>
       </c>
-      <c r="O7" t="s">
+      <c r="P7" t="s">
         <v>3</v>
       </c>
-      <c r="P7" t="s">
+      <c r="Q7" t="s">
         <v>95</v>
       </c>
-      <c r="Q7" t="s">
+      <c r="R7" t="s">
         <v>155</v>
       </c>
     </row>
-    <row r="8" spans="1:20" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:24" x14ac:dyDescent="0.25">
       <c r="A8" t="s">
-        <v>485</v>
+        <v>289</v>
       </c>
       <c r="B8" t="s">
-        <v>673</v>
+        <v>485</v>
       </c>
       <c r="C8" t="s">
         <v>673</v>
       </c>
-      <c r="D8">
+      <c r="D8" t="s">
+        <v>673</v>
+      </c>
+      <c r="E8">
         <v>2</v>
       </c>
-      <c r="E8" t="s">
+      <c r="F8" t="s">
         <v>2</v>
       </c>
-      <c r="F8" t="s">
+      <c r="G8" t="s">
         <v>68</v>
       </c>
-      <c r="G8" t="s">
+      <c r="H8" t="s">
         <v>24</v>
       </c>
-      <c r="H8" t="s">
+      <c r="I8" t="s">
         <v>175</v>
       </c>
-      <c r="I8" t="s">
+      <c r="J8" t="s">
         <v>189</v>
       </c>
-      <c r="J8" t="s">
+      <c r="K8" t="s">
         <v>173</v>
       </c>
-      <c r="K8" t="s">
+      <c r="L8" t="s">
         <v>171</v>
       </c>
-      <c r="L8" t="s">
+      <c r="M8" t="s">
         <v>583</v>
       </c>
-      <c r="M8" t="s">
+      <c r="N8" t="s">
         <v>177</v>
       </c>
-      <c r="N8" t="s">
+      <c r="O8" t="s">
         <v>674</v>
       </c>
-      <c r="O8" t="s">
+      <c r="P8" t="s">
         <v>179</v>
       </c>
-      <c r="P8" t="s">
+      <c r="Q8" t="s">
         <v>675</v>
       </c>
-      <c r="Q8" t="s">
+      <c r="R8" t="s">
         <v>575</v>
       </c>
     </row>
-    <row r="9" spans="1:20" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:24" x14ac:dyDescent="0.25">
       <c r="A9" t="s">
-        <v>485</v>
+        <v>289</v>
       </c>
       <c r="B9" t="s">
-        <v>673</v>
+        <v>485</v>
       </c>
       <c r="C9" t="s">
         <v>673</v>
       </c>
-      <c r="D9">
+      <c r="D9" t="s">
+        <v>673</v>
+      </c>
+      <c r="E9">
         <v>3</v>
       </c>
-      <c r="E9" t="s">
+      <c r="F9" t="s">
         <v>8</v>
       </c>
-      <c r="F9" t="s">
+      <c r="G9" t="s">
         <v>68</v>
       </c>
-      <c r="G9" t="s">
+      <c r="H9" t="s">
         <v>24</v>
       </c>
-      <c r="H9" t="s">
+      <c r="I9" t="s">
         <v>175</v>
       </c>
-      <c r="I9" t="s">
+      <c r="J9" t="s">
         <v>189</v>
       </c>
-      <c r="J9" t="s">
+      <c r="K9" t="s">
         <v>173</v>
       </c>
-      <c r="K9" t="s">
+      <c r="L9" t="s">
         <v>171</v>
       </c>
-      <c r="L9" t="s">
+      <c r="M9" t="s">
         <v>583</v>
       </c>
-      <c r="M9" t="s">
+      <c r="N9" t="s">
         <v>177</v>
       </c>
-      <c r="N9" t="s">
+      <c r="O9" t="s">
         <v>674</v>
       </c>
-      <c r="O9" t="s">
+      <c r="P9" t="s">
         <v>179</v>
       </c>
-      <c r="P9" t="s">
+      <c r="Q9" t="s">
         <v>675</v>
       </c>
-      <c r="Q9" t="s">
+      <c r="R9" t="s">
         <v>575</v>
       </c>
     </row>
-    <row r="11" spans="1:20" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:24" x14ac:dyDescent="0.25">
+      <c r="A10" t="s">
+        <v>251</v>
+      </c>
+      <c r="B10" t="s">
+        <v>485</v>
+      </c>
+      <c r="C10" t="s">
+        <v>678</v>
+      </c>
+      <c r="D10" t="s">
+        <v>678</v>
+      </c>
+      <c r="E10">
+        <v>1</v>
+      </c>
+      <c r="F10" t="s">
+        <v>2</v>
+      </c>
+      <c r="G10" t="s">
+        <v>49</v>
+      </c>
+      <c r="H10" t="s">
+        <v>24</v>
+      </c>
+      <c r="I10" t="s">
+        <v>11</v>
+      </c>
+      <c r="J10" t="s">
+        <v>5</v>
+      </c>
+      <c r="K10" t="s">
+        <v>4</v>
+      </c>
+      <c r="L10" t="s">
+        <v>12</v>
+      </c>
+      <c r="M10" t="s">
+        <v>83</v>
+      </c>
+      <c r="N10" t="s">
+        <v>10</v>
+      </c>
+      <c r="O10" t="s">
+        <v>28</v>
+      </c>
+      <c r="P10" t="s">
+        <v>3</v>
+      </c>
+      <c r="Q10" t="s">
+        <v>95</v>
+      </c>
+      <c r="R10" t="s">
+        <v>155</v>
+      </c>
+    </row>
+    <row r="11" spans="1:24" x14ac:dyDescent="0.25">
       <c r="A11" t="s">
-        <v>485</v>
+        <v>251</v>
       </c>
       <c r="B11" t="s">
-        <v>678</v>
+        <v>485</v>
       </c>
       <c r="C11" t="s">
         <v>678</v>
       </c>
-      <c r="D11">
+      <c r="D11" t="s">
+        <v>678</v>
+      </c>
+      <c r="E11">
         <v>1</v>
       </c>
-      <c r="E11" t="s">
-        <v>2</v>
-      </c>
       <c r="F11" t="s">
+        <v>7</v>
+      </c>
+      <c r="G11" t="s">
         <v>49</v>
       </c>
-      <c r="G11" t="s">
+      <c r="H11" t="s">
         <v>24</v>
       </c>
-      <c r="H11" t="s">
+      <c r="I11" t="s">
         <v>11</v>
       </c>
-      <c r="I11" t="s">
+      <c r="J11" t="s">
         <v>5</v>
       </c>
-      <c r="J11" t="s">
+      <c r="K11" t="s">
         <v>4</v>
       </c>
-      <c r="K11" t="s">
+      <c r="L11" t="s">
         <v>12</v>
       </c>
-      <c r="L11" t="s">
+      <c r="M11" t="s">
         <v>83</v>
       </c>
-      <c r="M11" t="s">
+      <c r="N11" t="s">
         <v>10</v>
       </c>
-      <c r="N11" t="s">
+      <c r="O11" t="s">
         <v>28</v>
       </c>
-      <c r="O11" t="s">
+      <c r="P11" t="s">
         <v>3</v>
       </c>
-      <c r="P11" t="s">
+      <c r="Q11" t="s">
         <v>95</v>
       </c>
-      <c r="Q11" t="s">
+      <c r="R11" t="s">
         <v>155</v>
       </c>
     </row>
-    <row r="12" spans="1:20" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:24" x14ac:dyDescent="0.25">
       <c r="A12" t="s">
-        <v>485</v>
+        <v>251</v>
       </c>
       <c r="B12" t="s">
-        <v>678</v>
+        <v>485</v>
       </c>
       <c r="C12" t="s">
         <v>678</v>
       </c>
-      <c r="D12">
-        <v>1</v>
-      </c>
-      <c r="E12" t="s">
-        <v>7</v>
+      <c r="D12" t="s">
+        <v>678</v>
+      </c>
+      <c r="E12">
+        <v>2</v>
       </c>
       <c r="F12" t="s">
-        <v>49</v>
+        <v>2</v>
       </c>
       <c r="G12" t="s">
+        <v>68</v>
+      </c>
+      <c r="H12" t="s">
         <v>24</v>
       </c>
-      <c r="H12" t="s">
-        <v>11</v>
-      </c>
       <c r="I12" t="s">
-        <v>5</v>
+        <v>175</v>
       </c>
       <c r="J12" t="s">
-        <v>4</v>
+        <v>189</v>
       </c>
       <c r="K12" t="s">
-        <v>12</v>
+        <v>173</v>
       </c>
       <c r="L12" t="s">
-        <v>83</v>
+        <v>171</v>
       </c>
       <c r="M12" t="s">
-        <v>10</v>
+        <v>583</v>
       </c>
       <c r="N12" t="s">
-        <v>28</v>
+        <v>177</v>
       </c>
       <c r="O12" t="s">
-        <v>3</v>
+        <v>680</v>
       </c>
       <c r="P12" t="s">
-        <v>95</v>
+        <v>674</v>
       </c>
       <c r="Q12" t="s">
-        <v>155</v>
-      </c>
-    </row>
-    <row r="13" spans="1:20" x14ac:dyDescent="0.25">
+        <v>681</v>
+      </c>
+      <c r="R12" t="s">
+        <v>179</v>
+      </c>
+      <c r="S12" t="s">
+        <v>682</v>
+      </c>
+      <c r="T12" t="s">
+        <v>679</v>
+      </c>
+      <c r="U12" t="s">
+        <v>575</v>
+      </c>
+    </row>
+    <row r="13" spans="1:24" x14ac:dyDescent="0.25">
       <c r="A13" t="s">
-        <v>485</v>
+        <v>251</v>
       </c>
       <c r="B13" t="s">
-        <v>678</v>
+        <v>485</v>
       </c>
       <c r="C13" t="s">
         <v>678</v>
       </c>
-      <c r="D13">
-        <v>2</v>
-      </c>
-      <c r="E13" t="s">
-        <v>2</v>
+      <c r="D13" t="s">
+        <v>678</v>
+      </c>
+      <c r="E13">
+        <v>3</v>
       </c>
       <c r="F13" t="s">
+        <v>8</v>
+      </c>
+      <c r="G13" t="s">
         <v>68</v>
       </c>
-      <c r="G13" t="s">
+      <c r="H13" t="s">
         <v>24</v>
       </c>
-      <c r="H13" t="s">
+      <c r="I13" t="s">
         <v>175</v>
       </c>
-      <c r="I13" t="s">
+      <c r="J13" t="s">
         <v>189</v>
       </c>
-      <c r="J13" t="s">
+      <c r="K13" t="s">
         <v>173</v>
       </c>
-      <c r="K13" t="s">
+      <c r="L13" t="s">
         <v>171</v>
       </c>
-      <c r="L13" t="s">
+      <c r="M13" t="s">
         <v>583</v>
       </c>
-      <c r="M13" t="s">
+      <c r="N13" t="s">
         <v>177</v>
       </c>
-      <c r="N13" t="s">
+      <c r="O13" t="s">
         <v>680</v>
       </c>
-      <c r="O13" t="s">
+      <c r="P13" t="s">
         <v>674</v>
       </c>
-      <c r="P13" t="s">
+      <c r="Q13" t="s">
         <v>681</v>
       </c>
-      <c r="Q13" t="s">
+      <c r="R13" t="s">
         <v>179</v>
       </c>
-      <c r="R13" t="s">
+      <c r="S13" t="s">
         <v>682</v>
       </c>
-      <c r="S13" t="s">
+      <c r="T13" t="s">
         <v>679</v>
       </c>
-      <c r="T13" t="s">
+      <c r="U13" t="s">
         <v>575</v>
-      </c>
-    </row>
-    <row r="14" spans="1:20" x14ac:dyDescent="0.25">
-      <c r="A14" t="s">
-        <v>485</v>
-      </c>
-      <c r="B14" t="s">
-        <v>678</v>
-      </c>
-      <c r="C14" t="s">
-        <v>678</v>
-      </c>
-      <c r="D14">
-        <v>3</v>
-      </c>
-      <c r="E14" t="s">
-        <v>8</v>
-      </c>
-      <c r="F14" t="s">
-        <v>68</v>
-      </c>
-      <c r="G14" t="s">
-        <v>24</v>
-      </c>
-      <c r="H14" t="s">
-        <v>175</v>
-      </c>
-      <c r="I14" t="s">
-        <v>189</v>
-      </c>
-      <c r="J14" t="s">
-        <v>173</v>
-      </c>
-      <c r="K14" t="s">
-        <v>171</v>
-      </c>
-      <c r="L14" t="s">
-        <v>583</v>
-      </c>
-      <c r="M14" t="s">
-        <v>177</v>
-      </c>
-      <c r="N14" t="s">
-        <v>680</v>
-      </c>
-      <c r="O14" t="s">
-        <v>674</v>
-      </c>
-      <c r="P14" t="s">
-        <v>681</v>
-      </c>
-      <c r="Q14" t="s">
-        <v>179</v>
-      </c>
-      <c r="R14" t="s">
-        <v>682</v>
-      </c>
-      <c r="S14" t="s">
-        <v>679</v>
-      </c>
-      <c r="T14" t="s">
-        <v>575</v>
-      </c>
-    </row>
-    <row r="19" spans="1:13" x14ac:dyDescent="0.25">
-      <c r="A19" t="s">
-        <v>486</v>
-      </c>
-      <c r="B19" t="s">
-        <v>488</v>
-      </c>
-      <c r="C19" t="s">
-        <v>488</v>
-      </c>
-      <c r="D19">
-        <v>1</v>
-      </c>
-      <c r="E19" t="s">
-        <v>2</v>
-      </c>
-      <c r="F19" t="s">
-        <v>493</v>
-      </c>
-      <c r="G19" t="s">
-        <v>488</v>
-      </c>
-      <c r="H19" t="s">
-        <v>517</v>
-      </c>
-      <c r="I19" t="s">
-        <v>496</v>
-      </c>
-      <c r="J19" t="s">
-        <v>516</v>
-      </c>
-      <c r="K19" t="s">
-        <v>554</v>
-      </c>
-      <c r="L19" t="s">
-        <v>555</v>
-      </c>
-      <c r="M19" t="s">
-        <v>553</v>
       </c>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
+  <legacyDrawing r:id="rId2"/>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
updated master config to automatically change charts economy specific
</commit_message>
<xml_diff>
--- a/config/master_config.xlsx
+++ b/config/master_config.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\finbar.maunsell\github\9th_edition_visualisation\config\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{7E9AF23F-081F-4EE1-B3B9-E7C3C4ECAF73}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{661377D0-DEC2-45E4-B508-A66ECC0B407E}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="28680" yWindow="-120" windowWidth="29040" windowHeight="15720" tabRatio="812" firstSheet="3" activeTab="4" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="28680" yWindow="-120" windowWidth="29040" windowHeight="15720" tabRatio="812" firstSheet="3" activeTab="8" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="9th_EBT_schema" sheetId="7" r:id="rId1"/>
@@ -21,7 +21,7 @@
     <sheet name="emissions_fuels_plotting" sheetId="13" r:id="rId6"/>
     <sheet name="emissions_sectors_plotting" sheetId="14" r:id="rId7"/>
     <sheet name="two_dimensional_plots" sheetId="18" r:id="rId8"/>
-    <sheet name="economy_specific" sheetId="22" r:id="rId9"/>
+    <sheet name="economy_specific_2d" sheetId="22" r:id="rId9"/>
     <sheet name="one_dimensional_plots" sheetId="16" r:id="rId10"/>
     <sheet name="plotting_name_to_label" sheetId="10" r:id="rId11"/>
     <sheet name="colors" sheetId="9" r:id="rId12"/>
@@ -315,6 +315,64 @@
     <author>Finbar Maunsell</author>
   </authors>
   <commentList>
+    <comment ref="E1" authorId="0" shapeId="0" xr:uid="{AD810412-828F-4728-BB16-5FD24C46A520}">
+      <text>
+        <r>
+          <rPr>
+            <b/>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <charset val="1"/>
+          </rPr>
+          <t>Finbar Maunsell:</t>
+        </r>
+        <r>
+          <rPr>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <charset val="1"/>
+          </rPr>
+          <t xml:space="preserve">
+table should be used if you need/want a sepaarate table for this data. This will be needed if the data wouldn’t be available otherwise, OR if the chart is a bar chart in which case we will show it in 10 year splits, so a new table will be needed for that</t>
+        </r>
+      </text>
+    </comment>
+    <comment ref="I1" authorId="0" shapeId="0" xr:uid="{03F3F105-5ABC-4D70-AD22-878D910AF562}">
+      <text>
+        <r>
+          <rPr>
+            <b/>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <charset val="1"/>
+          </rPr>
+          <t>Finbar Maunsell:</t>
+        </r>
+        <r>
+          <rPr>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <charset val="1"/>
+          </rPr>
+          <t xml:space="preserve">
+These numbers are just placeholders, if you need more plotting names just extend the numbers to X+wahtever</t>
+        </r>
+      </text>
+    </comment>
+  </commentList>
+</comments>
+</file>
+
+<file path=xl/comments8.xml><?xml version="1.0" encoding="utf-8"?>
+<comments xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="xr">
+  <authors>
+    <author>Finbar Maunsell</author>
+  </authors>
+  <commentList>
     <comment ref="C1" authorId="0" shapeId="0" xr:uid="{1258B623-61DE-4825-BC11-55DF89ECC451}">
       <text>
         <r>
@@ -343,7 +401,7 @@
 </comments>
 </file>
 
-<file path=xl/comments8.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/comments9.xml><?xml version="1.0" encoding="utf-8"?>
 <comments xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="xr">
   <authors>
     <author>Finbar Maunsell</author>
@@ -402,7 +460,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="6174" uniqueCount="719">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="6182" uniqueCount="719">
   <si>
     <t>chart_type</t>
   </si>
@@ -2696,7 +2754,7 @@
       </patternFill>
     </fill>
   </fills>
-  <borders count="6">
+  <borders count="7">
     <border>
       <left/>
       <right/>
@@ -2767,12 +2825,23 @@
       <bottom/>
       <diagonal/>
     </border>
+    <border>
+      <left/>
+      <right style="thin">
+        <color auto="1"/>
+      </right>
+      <top/>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="7" fillId="9" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="20">
+  <cellXfs count="21">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="top"/>
@@ -2809,6 +2878,7 @@
     <xf numFmtId="0" fontId="2" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="top"/>
     </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="Neutral" xfId="1" builtinId="28"/>
@@ -13887,8 +13957,8 @@
   </sheetPr>
   <dimension ref="A1:I179"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C103" sqref="C103"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="D181" sqref="D181"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -22480,8 +22550,8 @@
   </sheetPr>
   <dimension ref="A1:W80"/>
   <sheetViews>
-    <sheetView topLeftCell="A38" zoomScale="80" zoomScaleNormal="80" workbookViewId="0">
-      <selection activeCell="E72" sqref="E72"/>
+    <sheetView zoomScale="80" zoomScaleNormal="80" workbookViewId="0">
+      <selection sqref="A1:W1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -26078,708 +26148,779 @@
 </file>
 
 <file path=xl/worksheets/sheet9.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{1FB41151-CF9C-4A5D-8C89-4DDD65A34550}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{1FB41151-CF9C-4A5D-8C89-4DDD65A34550}">
   <sheetPr>
     <tabColor theme="9" tint="0.39997558519241921"/>
   </sheetPr>
-  <dimension ref="A1:T19"/>
+  <dimension ref="A1:X13"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection sqref="A1:U4"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="C10" sqref="C10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <sheetData>
-    <row r="1" spans="1:20" x14ac:dyDescent="0.25">
-      <c r="A1" t="s">
-        <v>485</v>
-      </c>
-      <c r="B1" t="s">
-        <v>24</v>
-      </c>
-      <c r="C1" t="s">
-        <v>24</v>
-      </c>
-      <c r="D1">
+    <row r="1" spans="1:24" x14ac:dyDescent="0.25">
+      <c r="A1" s="20" t="s">
+        <v>208</v>
+      </c>
+      <c r="B1" s="1" t="s">
+        <v>484</v>
+      </c>
+      <c r="C1" s="1" t="s">
+        <v>524</v>
+      </c>
+      <c r="D1" s="1" t="s">
+        <v>463</v>
+      </c>
+      <c r="E1" s="1" t="s">
+        <v>462</v>
+      </c>
+      <c r="F1" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="G1" s="1" t="s">
+        <v>492</v>
+      </c>
+      <c r="H1" s="1" t="s">
+        <v>493</v>
+      </c>
+      <c r="I1" s="1">
+        <v>0</v>
+      </c>
+      <c r="J1" s="1">
         <v>1</v>
       </c>
-      <c r="E1" t="s">
+      <c r="K1" s="1">
         <v>2</v>
       </c>
-      <c r="F1" t="s">
-        <v>49</v>
-      </c>
-      <c r="G1" t="s">
-        <v>24</v>
-      </c>
-      <c r="H1" t="s">
+      <c r="L1" s="1">
+        <v>3</v>
+      </c>
+      <c r="M1" s="1">
+        <v>4</v>
+      </c>
+      <c r="N1" s="1">
+        <v>5</v>
+      </c>
+      <c r="O1" s="1">
+        <v>6</v>
+      </c>
+      <c r="P1" s="1">
+        <v>7</v>
+      </c>
+      <c r="Q1" s="1">
+        <v>8</v>
+      </c>
+      <c r="R1" s="1">
+        <v>9</v>
+      </c>
+      <c r="S1" s="1">
+        <v>10</v>
+      </c>
+      <c r="T1" s="14">
         <v>11</v>
       </c>
-      <c r="I1" t="s">
-        <v>5</v>
-      </c>
-      <c r="J1" t="s">
-        <v>4</v>
-      </c>
-      <c r="K1" t="s">
+      <c r="U1" s="14">
         <v>12</v>
       </c>
-      <c r="L1" t="s">
-        <v>83</v>
-      </c>
-      <c r="M1" t="s">
-        <v>10</v>
-      </c>
-      <c r="N1" t="s">
-        <v>28</v>
-      </c>
-      <c r="O1" t="s">
-        <v>3</v>
-      </c>
-      <c r="P1" t="s">
-        <v>95</v>
-      </c>
-      <c r="Q1" t="s">
-        <v>155</v>
-      </c>
-    </row>
-    <row r="2" spans="1:20" x14ac:dyDescent="0.25">
+      <c r="V1" s="14">
+        <v>13</v>
+      </c>
+      <c r="W1" s="14">
+        <v>14</v>
+      </c>
+      <c r="X1" s="14">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="2" spans="1:24" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
-        <v>485</v>
+        <v>212</v>
       </c>
       <c r="B2" t="s">
-        <v>24</v>
+        <v>485</v>
       </c>
       <c r="C2" t="s">
         <v>24</v>
       </c>
-      <c r="D2">
+      <c r="D2" t="s">
+        <v>24</v>
+      </c>
+      <c r="E2">
         <v>1</v>
       </c>
-      <c r="E2" t="s">
-        <v>7</v>
-      </c>
       <c r="F2" t="s">
+        <v>2</v>
+      </c>
+      <c r="G2" t="s">
         <v>49</v>
       </c>
-      <c r="G2" t="s">
+      <c r="H2" t="s">
         <v>24</v>
       </c>
-      <c r="H2" t="s">
+      <c r="I2" t="s">
         <v>11</v>
       </c>
-      <c r="I2" t="s">
+      <c r="J2" t="s">
         <v>5</v>
       </c>
-      <c r="J2" t="s">
+      <c r="K2" t="s">
         <v>4</v>
       </c>
-      <c r="K2" t="s">
+      <c r="L2" t="s">
         <v>12</v>
       </c>
-      <c r="L2" t="s">
+      <c r="M2" t="s">
         <v>83</v>
       </c>
-      <c r="M2" t="s">
+      <c r="N2" t="s">
         <v>10</v>
       </c>
-      <c r="N2" t="s">
+      <c r="O2" t="s">
         <v>28</v>
       </c>
-      <c r="O2" t="s">
+      <c r="P2" t="s">
         <v>3</v>
       </c>
-      <c r="P2" t="s">
+      <c r="Q2" t="s">
         <v>95</v>
       </c>
-      <c r="Q2" t="s">
+      <c r="R2" t="s">
         <v>155</v>
       </c>
     </row>
-    <row r="3" spans="1:20" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:24" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
-        <v>485</v>
+        <v>212</v>
       </c>
       <c r="B3" t="s">
-        <v>24</v>
+        <v>485</v>
       </c>
       <c r="C3" t="s">
         <v>24</v>
       </c>
-      <c r="D3">
-        <v>2</v>
-      </c>
-      <c r="E3" t="s">
-        <v>2</v>
+      <c r="D3" t="s">
+        <v>24</v>
+      </c>
+      <c r="E3">
+        <v>1</v>
       </c>
       <c r="F3" t="s">
-        <v>68</v>
+        <v>7</v>
       </c>
       <c r="G3" t="s">
+        <v>49</v>
+      </c>
+      <c r="H3" t="s">
         <v>24</v>
       </c>
-      <c r="H3" t="s">
-        <v>175</v>
-      </c>
       <c r="I3" t="s">
-        <v>189</v>
+        <v>11</v>
       </c>
       <c r="J3" t="s">
-        <v>173</v>
+        <v>5</v>
       </c>
       <c r="K3" t="s">
-        <v>171</v>
+        <v>4</v>
       </c>
       <c r="L3" t="s">
-        <v>583</v>
+        <v>12</v>
       </c>
       <c r="M3" t="s">
-        <v>177</v>
+        <v>83</v>
       </c>
       <c r="N3" t="s">
-        <v>179</v>
+        <v>10</v>
       </c>
       <c r="O3" t="s">
-        <v>181</v>
+        <v>28</v>
       </c>
       <c r="P3" t="s">
-        <v>575</v>
-      </c>
-    </row>
-    <row r="4" spans="1:20" x14ac:dyDescent="0.25">
+        <v>3</v>
+      </c>
+      <c r="Q3" t="s">
+        <v>95</v>
+      </c>
+      <c r="R3" t="s">
+        <v>155</v>
+      </c>
+    </row>
+    <row r="4" spans="1:24" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
-        <v>485</v>
+        <v>212</v>
       </c>
       <c r="B4" t="s">
-        <v>24</v>
+        <v>485</v>
       </c>
       <c r="C4" t="s">
         <v>24</v>
       </c>
-      <c r="D4">
+      <c r="D4" t="s">
+        <v>24</v>
+      </c>
+      <c r="E4">
+        <v>2</v>
+      </c>
+      <c r="F4" t="s">
+        <v>2</v>
+      </c>
+      <c r="G4" t="s">
+        <v>68</v>
+      </c>
+      <c r="H4" t="s">
+        <v>24</v>
+      </c>
+      <c r="I4" t="s">
+        <v>175</v>
+      </c>
+      <c r="J4" t="s">
+        <v>189</v>
+      </c>
+      <c r="K4" t="s">
+        <v>173</v>
+      </c>
+      <c r="L4" t="s">
+        <v>171</v>
+      </c>
+      <c r="M4" t="s">
+        <v>583</v>
+      </c>
+      <c r="N4" t="s">
+        <v>177</v>
+      </c>
+      <c r="O4" t="s">
+        <v>179</v>
+      </c>
+      <c r="P4" t="s">
+        <v>181</v>
+      </c>
+      <c r="Q4" t="s">
+        <v>575</v>
+      </c>
+    </row>
+    <row r="5" spans="1:24" x14ac:dyDescent="0.25">
+      <c r="A5" t="s">
+        <v>212</v>
+      </c>
+      <c r="B5" t="s">
+        <v>485</v>
+      </c>
+      <c r="C5" t="s">
+        <v>24</v>
+      </c>
+      <c r="D5" t="s">
+        <v>24</v>
+      </c>
+      <c r="E5">
         <v>3</v>
       </c>
-      <c r="E4" t="s">
+      <c r="F5" t="s">
         <v>8</v>
       </c>
-      <c r="F4" t="s">
+      <c r="G5" t="s">
         <v>68</v>
       </c>
-      <c r="G4" t="s">
+      <c r="H5" t="s">
         <v>24</v>
       </c>
-      <c r="H4" t="s">
+      <c r="I5" t="s">
         <v>175</v>
       </c>
-      <c r="I4" t="s">
+      <c r="J5" t="s">
         <v>189</v>
       </c>
-      <c r="J4" t="s">
+      <c r="K5" t="s">
         <v>173</v>
       </c>
-      <c r="K4" t="s">
+      <c r="L5" t="s">
         <v>171</v>
       </c>
-      <c r="L4" t="s">
+      <c r="M5" t="s">
         <v>583</v>
       </c>
-      <c r="M4" t="s">
+      <c r="N5" t="s">
         <v>177</v>
       </c>
-      <c r="N4" t="s">
+      <c r="O5" t="s">
         <v>179</v>
       </c>
-      <c r="O4" t="s">
+      <c r="P5" t="s">
         <v>181</v>
       </c>
-      <c r="P4" t="s">
+      <c r="Q5" t="s">
         <v>575</v>
       </c>
     </row>
-    <row r="6" spans="1:20" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:24" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
-        <v>485</v>
+        <v>289</v>
       </c>
       <c r="B6" t="s">
-        <v>673</v>
+        <v>485</v>
       </c>
       <c r="C6" t="s">
         <v>673</v>
       </c>
-      <c r="D6">
+      <c r="D6" t="s">
+        <v>673</v>
+      </c>
+      <c r="E6">
         <v>1</v>
       </c>
-      <c r="E6" t="s">
+      <c r="F6" t="s">
         <v>2</v>
       </c>
-      <c r="F6" t="s">
+      <c r="G6" t="s">
         <v>49</v>
       </c>
-      <c r="G6" t="s">
+      <c r="H6" t="s">
         <v>24</v>
       </c>
-      <c r="H6" t="s">
+      <c r="I6" t="s">
         <v>11</v>
       </c>
-      <c r="I6" t="s">
+      <c r="J6" t="s">
         <v>5</v>
       </c>
-      <c r="J6" t="s">
+      <c r="K6" t="s">
         <v>4</v>
       </c>
-      <c r="K6" t="s">
+      <c r="L6" t="s">
         <v>12</v>
       </c>
-      <c r="L6" t="s">
+      <c r="M6" t="s">
         <v>83</v>
       </c>
-      <c r="M6" t="s">
+      <c r="N6" t="s">
         <v>10</v>
       </c>
-      <c r="N6" t="s">
+      <c r="O6" t="s">
         <v>28</v>
       </c>
-      <c r="O6" t="s">
+      <c r="P6" t="s">
         <v>3</v>
       </c>
-      <c r="P6" t="s">
+      <c r="Q6" t="s">
         <v>95</v>
       </c>
-      <c r="Q6" t="s">
+      <c r="R6" t="s">
         <v>155</v>
       </c>
     </row>
-    <row r="7" spans="1:20" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:24" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
-        <v>485</v>
+        <v>289</v>
       </c>
       <c r="B7" t="s">
-        <v>673</v>
+        <v>485</v>
       </c>
       <c r="C7" t="s">
         <v>673</v>
       </c>
-      <c r="D7">
+      <c r="D7" t="s">
+        <v>673</v>
+      </c>
+      <c r="E7">
         <v>1</v>
       </c>
-      <c r="E7" t="s">
+      <c r="F7" t="s">
         <v>7</v>
       </c>
-      <c r="F7" t="s">
+      <c r="G7" t="s">
         <v>49</v>
       </c>
-      <c r="G7" t="s">
+      <c r="H7" t="s">
         <v>24</v>
       </c>
-      <c r="H7" t="s">
+      <c r="I7" t="s">
         <v>11</v>
       </c>
-      <c r="I7" t="s">
+      <c r="J7" t="s">
         <v>5</v>
       </c>
-      <c r="J7" t="s">
+      <c r="K7" t="s">
         <v>4</v>
       </c>
-      <c r="K7" t="s">
+      <c r="L7" t="s">
         <v>12</v>
       </c>
-      <c r="L7" t="s">
+      <c r="M7" t="s">
         <v>83</v>
       </c>
-      <c r="M7" t="s">
+      <c r="N7" t="s">
         <v>10</v>
       </c>
-      <c r="N7" t="s">
+      <c r="O7" t="s">
         <v>28</v>
       </c>
-      <c r="O7" t="s">
+      <c r="P7" t="s">
         <v>3</v>
       </c>
-      <c r="P7" t="s">
+      <c r="Q7" t="s">
         <v>95</v>
       </c>
-      <c r="Q7" t="s">
+      <c r="R7" t="s">
         <v>155</v>
       </c>
     </row>
-    <row r="8" spans="1:20" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:24" x14ac:dyDescent="0.25">
       <c r="A8" t="s">
-        <v>485</v>
+        <v>289</v>
       </c>
       <c r="B8" t="s">
-        <v>673</v>
+        <v>485</v>
       </c>
       <c r="C8" t="s">
         <v>673</v>
       </c>
-      <c r="D8">
+      <c r="D8" t="s">
+        <v>673</v>
+      </c>
+      <c r="E8">
         <v>2</v>
       </c>
-      <c r="E8" t="s">
+      <c r="F8" t="s">
         <v>2</v>
       </c>
-      <c r="F8" t="s">
+      <c r="G8" t="s">
         <v>68</v>
       </c>
-      <c r="G8" t="s">
+      <c r="H8" t="s">
         <v>24</v>
       </c>
-      <c r="H8" t="s">
+      <c r="I8" t="s">
         <v>175</v>
       </c>
-      <c r="I8" t="s">
+      <c r="J8" t="s">
         <v>189</v>
       </c>
-      <c r="J8" t="s">
+      <c r="K8" t="s">
         <v>173</v>
       </c>
-      <c r="K8" t="s">
+      <c r="L8" t="s">
         <v>171</v>
       </c>
-      <c r="L8" t="s">
+      <c r="M8" t="s">
         <v>583</v>
       </c>
-      <c r="M8" t="s">
+      <c r="N8" t="s">
         <v>177</v>
       </c>
-      <c r="N8" t="s">
+      <c r="O8" t="s">
         <v>674</v>
       </c>
-      <c r="O8" t="s">
+      <c r="P8" t="s">
         <v>179</v>
       </c>
-      <c r="P8" t="s">
+      <c r="Q8" t="s">
         <v>675</v>
       </c>
-      <c r="Q8" t="s">
+      <c r="R8" t="s">
         <v>575</v>
       </c>
     </row>
-    <row r="9" spans="1:20" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:24" x14ac:dyDescent="0.25">
       <c r="A9" t="s">
-        <v>485</v>
+        <v>289</v>
       </c>
       <c r="B9" t="s">
-        <v>673</v>
+        <v>485</v>
       </c>
       <c r="C9" t="s">
         <v>673</v>
       </c>
-      <c r="D9">
+      <c r="D9" t="s">
+        <v>673</v>
+      </c>
+      <c r="E9">
         <v>3</v>
       </c>
-      <c r="E9" t="s">
+      <c r="F9" t="s">
         <v>8</v>
       </c>
-      <c r="F9" t="s">
+      <c r="G9" t="s">
         <v>68</v>
       </c>
-      <c r="G9" t="s">
+      <c r="H9" t="s">
         <v>24</v>
       </c>
-      <c r="H9" t="s">
+      <c r="I9" t="s">
         <v>175</v>
       </c>
-      <c r="I9" t="s">
+      <c r="J9" t="s">
         <v>189</v>
       </c>
-      <c r="J9" t="s">
+      <c r="K9" t="s">
         <v>173</v>
       </c>
-      <c r="K9" t="s">
+      <c r="L9" t="s">
         <v>171</v>
       </c>
-      <c r="L9" t="s">
+      <c r="M9" t="s">
         <v>583</v>
       </c>
-      <c r="M9" t="s">
+      <c r="N9" t="s">
         <v>177</v>
       </c>
-      <c r="N9" t="s">
+      <c r="O9" t="s">
         <v>674</v>
       </c>
-      <c r="O9" t="s">
+      <c r="P9" t="s">
         <v>179</v>
       </c>
-      <c r="P9" t="s">
+      <c r="Q9" t="s">
         <v>675</v>
       </c>
-      <c r="Q9" t="s">
+      <c r="R9" t="s">
         <v>575</v>
       </c>
     </row>
-    <row r="11" spans="1:20" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:24" x14ac:dyDescent="0.25">
+      <c r="A10" t="s">
+        <v>251</v>
+      </c>
+      <c r="B10" t="s">
+        <v>485</v>
+      </c>
+      <c r="C10" t="s">
+        <v>678</v>
+      </c>
+      <c r="D10" t="s">
+        <v>678</v>
+      </c>
+      <c r="E10">
+        <v>1</v>
+      </c>
+      <c r="F10" t="s">
+        <v>2</v>
+      </c>
+      <c r="G10" t="s">
+        <v>49</v>
+      </c>
+      <c r="H10" t="s">
+        <v>24</v>
+      </c>
+      <c r="I10" t="s">
+        <v>11</v>
+      </c>
+      <c r="J10" t="s">
+        <v>5</v>
+      </c>
+      <c r="K10" t="s">
+        <v>4</v>
+      </c>
+      <c r="L10" t="s">
+        <v>12</v>
+      </c>
+      <c r="M10" t="s">
+        <v>83</v>
+      </c>
+      <c r="N10" t="s">
+        <v>10</v>
+      </c>
+      <c r="O10" t="s">
+        <v>28</v>
+      </c>
+      <c r="P10" t="s">
+        <v>3</v>
+      </c>
+      <c r="Q10" t="s">
+        <v>95</v>
+      </c>
+      <c r="R10" t="s">
+        <v>155</v>
+      </c>
+    </row>
+    <row r="11" spans="1:24" x14ac:dyDescent="0.25">
       <c r="A11" t="s">
-        <v>485</v>
+        <v>251</v>
       </c>
       <c r="B11" t="s">
-        <v>678</v>
+        <v>485</v>
       </c>
       <c r="C11" t="s">
         <v>678</v>
       </c>
-      <c r="D11">
+      <c r="D11" t="s">
+        <v>678</v>
+      </c>
+      <c r="E11">
         <v>1</v>
       </c>
-      <c r="E11" t="s">
-        <v>2</v>
-      </c>
       <c r="F11" t="s">
+        <v>7</v>
+      </c>
+      <c r="G11" t="s">
         <v>49</v>
       </c>
-      <c r="G11" t="s">
+      <c r="H11" t="s">
         <v>24</v>
       </c>
-      <c r="H11" t="s">
+      <c r="I11" t="s">
         <v>11</v>
       </c>
-      <c r="I11" t="s">
+      <c r="J11" t="s">
         <v>5</v>
       </c>
-      <c r="J11" t="s">
+      <c r="K11" t="s">
         <v>4</v>
       </c>
-      <c r="K11" t="s">
+      <c r="L11" t="s">
         <v>12</v>
       </c>
-      <c r="L11" t="s">
+      <c r="M11" t="s">
         <v>83</v>
       </c>
-      <c r="M11" t="s">
+      <c r="N11" t="s">
         <v>10</v>
       </c>
-      <c r="N11" t="s">
+      <c r="O11" t="s">
         <v>28</v>
       </c>
-      <c r="O11" t="s">
+      <c r="P11" t="s">
         <v>3</v>
       </c>
-      <c r="P11" t="s">
+      <c r="Q11" t="s">
         <v>95</v>
       </c>
-      <c r="Q11" t="s">
+      <c r="R11" t="s">
         <v>155</v>
       </c>
     </row>
-    <row r="12" spans="1:20" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:24" x14ac:dyDescent="0.25">
       <c r="A12" t="s">
-        <v>485</v>
+        <v>251</v>
       </c>
       <c r="B12" t="s">
-        <v>678</v>
+        <v>485</v>
       </c>
       <c r="C12" t="s">
         <v>678</v>
       </c>
-      <c r="D12">
-        <v>1</v>
-      </c>
-      <c r="E12" t="s">
-        <v>7</v>
+      <c r="D12" t="s">
+        <v>678</v>
+      </c>
+      <c r="E12">
+        <v>2</v>
       </c>
       <c r="F12" t="s">
-        <v>49</v>
+        <v>2</v>
       </c>
       <c r="G12" t="s">
+        <v>68</v>
+      </c>
+      <c r="H12" t="s">
         <v>24</v>
       </c>
-      <c r="H12" t="s">
-        <v>11</v>
-      </c>
       <c r="I12" t="s">
-        <v>5</v>
+        <v>175</v>
       </c>
       <c r="J12" t="s">
-        <v>4</v>
+        <v>189</v>
       </c>
       <c r="K12" t="s">
-        <v>12</v>
+        <v>173</v>
       </c>
       <c r="L12" t="s">
-        <v>83</v>
+        <v>171</v>
       </c>
       <c r="M12" t="s">
-        <v>10</v>
+        <v>583</v>
       </c>
       <c r="N12" t="s">
-        <v>28</v>
+        <v>177</v>
       </c>
       <c r="O12" t="s">
-        <v>3</v>
+        <v>680</v>
       </c>
       <c r="P12" t="s">
-        <v>95</v>
+        <v>674</v>
       </c>
       <c r="Q12" t="s">
-        <v>155</v>
-      </c>
-    </row>
-    <row r="13" spans="1:20" x14ac:dyDescent="0.25">
+        <v>681</v>
+      </c>
+      <c r="R12" t="s">
+        <v>179</v>
+      </c>
+      <c r="S12" t="s">
+        <v>682</v>
+      </c>
+      <c r="T12" t="s">
+        <v>679</v>
+      </c>
+      <c r="U12" t="s">
+        <v>575</v>
+      </c>
+    </row>
+    <row r="13" spans="1:24" x14ac:dyDescent="0.25">
       <c r="A13" t="s">
-        <v>485</v>
+        <v>251</v>
       </c>
       <c r="B13" t="s">
-        <v>678</v>
+        <v>485</v>
       </c>
       <c r="C13" t="s">
         <v>678</v>
       </c>
-      <c r="D13">
-        <v>2</v>
-      </c>
-      <c r="E13" t="s">
-        <v>2</v>
+      <c r="D13" t="s">
+        <v>678</v>
+      </c>
+      <c r="E13">
+        <v>3</v>
       </c>
       <c r="F13" t="s">
+        <v>8</v>
+      </c>
+      <c r="G13" t="s">
         <v>68</v>
       </c>
-      <c r="G13" t="s">
+      <c r="H13" t="s">
         <v>24</v>
       </c>
-      <c r="H13" t="s">
+      <c r="I13" t="s">
         <v>175</v>
       </c>
-      <c r="I13" t="s">
+      <c r="J13" t="s">
         <v>189</v>
       </c>
-      <c r="J13" t="s">
+      <c r="K13" t="s">
         <v>173</v>
       </c>
-      <c r="K13" t="s">
+      <c r="L13" t="s">
         <v>171</v>
       </c>
-      <c r="L13" t="s">
+      <c r="M13" t="s">
         <v>583</v>
       </c>
-      <c r="M13" t="s">
+      <c r="N13" t="s">
         <v>177</v>
       </c>
-      <c r="N13" t="s">
+      <c r="O13" t="s">
         <v>680</v>
       </c>
-      <c r="O13" t="s">
+      <c r="P13" t="s">
         <v>674</v>
       </c>
-      <c r="P13" t="s">
+      <c r="Q13" t="s">
         <v>681</v>
       </c>
-      <c r="Q13" t="s">
+      <c r="R13" t="s">
         <v>179</v>
       </c>
-      <c r="R13" t="s">
+      <c r="S13" t="s">
         <v>682</v>
       </c>
-      <c r="S13" t="s">
+      <c r="T13" t="s">
         <v>679</v>
       </c>
-      <c r="T13" t="s">
+      <c r="U13" t="s">
         <v>575</v>
-      </c>
-    </row>
-    <row r="14" spans="1:20" x14ac:dyDescent="0.25">
-      <c r="A14" t="s">
-        <v>485</v>
-      </c>
-      <c r="B14" t="s">
-        <v>678</v>
-      </c>
-      <c r="C14" t="s">
-        <v>678</v>
-      </c>
-      <c r="D14">
-        <v>3</v>
-      </c>
-      <c r="E14" t="s">
-        <v>8</v>
-      </c>
-      <c r="F14" t="s">
-        <v>68</v>
-      </c>
-      <c r="G14" t="s">
-        <v>24</v>
-      </c>
-      <c r="H14" t="s">
-        <v>175</v>
-      </c>
-      <c r="I14" t="s">
-        <v>189</v>
-      </c>
-      <c r="J14" t="s">
-        <v>173</v>
-      </c>
-      <c r="K14" t="s">
-        <v>171</v>
-      </c>
-      <c r="L14" t="s">
-        <v>583</v>
-      </c>
-      <c r="M14" t="s">
-        <v>177</v>
-      </c>
-      <c r="N14" t="s">
-        <v>680</v>
-      </c>
-      <c r="O14" t="s">
-        <v>674</v>
-      </c>
-      <c r="P14" t="s">
-        <v>681</v>
-      </c>
-      <c r="Q14" t="s">
-        <v>179</v>
-      </c>
-      <c r="R14" t="s">
-        <v>682</v>
-      </c>
-      <c r="S14" t="s">
-        <v>679</v>
-      </c>
-      <c r="T14" t="s">
-        <v>575</v>
-      </c>
-    </row>
-    <row r="19" spans="1:13" x14ac:dyDescent="0.25">
-      <c r="A19" t="s">
-        <v>486</v>
-      </c>
-      <c r="B19" t="s">
-        <v>488</v>
-      </c>
-      <c r="C19" t="s">
-        <v>488</v>
-      </c>
-      <c r="D19">
-        <v>1</v>
-      </c>
-      <c r="E19" t="s">
-        <v>2</v>
-      </c>
-      <c r="F19" t="s">
-        <v>493</v>
-      </c>
-      <c r="G19" t="s">
-        <v>488</v>
-      </c>
-      <c r="H19" t="s">
-        <v>517</v>
-      </c>
-      <c r="I19" t="s">
-        <v>496</v>
-      </c>
-      <c r="J19" t="s">
-        <v>516</v>
-      </c>
-      <c r="K19" t="s">
-        <v>554</v>
-      </c>
-      <c r="L19" t="s">
-        <v>555</v>
-      </c>
-      <c r="M19" t="s">
-        <v>553</v>
       </c>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
+  <legacyDrawing r:id="rId2"/>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
changed order of sheets
</commit_message>
<xml_diff>
--- a/config/master_config.xlsx
+++ b/config/master_config.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\hyuga.kasai\Documents\Github\9th_Visualization\9th_edition_visualisation\config\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{AF62A223-63DB-4E5E-A915-5E4F5E84B50B}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{12DE9BB4-CE62-4700-9093-36945D07037B}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-6750" yWindow="-16320" windowWidth="29040" windowHeight="15840" tabRatio="812" firstSheet="4" activeTab="11" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-6750" yWindow="-16320" windowWidth="29040" windowHeight="15840" tabRatio="812" firstSheet="5" activeTab="12" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="9th_EBT_schema" sheetId="7" r:id="rId1"/>
@@ -2496,9 +2496,6 @@
     <t>#708090</t>
   </si>
   <si>
-    <t>['Macro', 'TFC by fuel', 'TFC by sector', 'FED by fuel', 'FED by sector', 'Industry', '09_ROK Industry', '18_CT Industry', 'Transport', 'Buildings', 'Agriculture', 'Non-energy', 'Electricity', 'Oil use by sector', 'Renewables consumption', 'Electricity generation',  'Generation capacity', 'Fuel consumption power sector', 'Refining', 'Hydrogen', 'Production', 'Supply', 'Exports', 'Coal',  'TPES Coal by type', 'Natural gas', 'Crude oil &amp; NGL', 'Refined products', 'Renewable fuels', 'Emissions', 'Transport stocks', 'Intensity', 'Renewables share', 'CO2 emissions components']</t>
-  </si>
-  <si>
     <t>Passenger stock shares</t>
   </si>
   <si>
@@ -2638,6 +2635,9 @@
   </si>
   <si>
     <t>Freight activity by drive</t>
+  </si>
+  <si>
+    <t>['Macro', 'TFC by fuel', 'TFC by sector', 'FED by fuel', 'FED by sector', 'Industry', '09_ROK Industry', '18_CT Industry', 'Transport', 'Buildings', 'Agriculture', 'Non-energy', 'Electricity', 'Oil use by sector', 'Renewables consumption', 'Electricity generation',  'Generation capacity', 'Fuel consumption power sector', 'Refining', 'Hydrogen', 'Production', 'Supply', 'Exports', 'Coal',  'TPES Coal by type', 'Natural gas', 'Crude oil &amp; NGL', 'Refined products', 'Renewable fuels', 'Emissions', 'Intensity', 'Renewables share', 'CO2 emissions components', 'Transport stocks', 'Transport activity']</t>
   </si>
 </sst>
 </file>
@@ -6505,7 +6505,7 @@
   </sheetPr>
   <dimension ref="A1:B173"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A41" workbookViewId="0">
+    <sheetView topLeftCell="A41" workbookViewId="0">
       <selection activeCell="E60" sqref="E60"/>
     </sheetView>
   </sheetViews>
@@ -6807,7 +6807,7 @@
         <v>647</v>
       </c>
       <c r="B37" t="s">
-        <v>713</v>
+        <v>712</v>
       </c>
     </row>
     <row r="38" spans="1:2" x14ac:dyDescent="0.25">
@@ -6924,7 +6924,7 @@
     </row>
     <row r="52" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A52" t="s">
-        <v>683</v>
+        <v>682</v>
       </c>
       <c r="B52" t="s">
         <v>437</v>
@@ -6932,7 +6932,7 @@
     </row>
     <row r="53" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A53" t="s">
-        <v>690</v>
+        <v>689</v>
       </c>
       <c r="B53" t="s">
         <v>437</v>
@@ -6972,7 +6972,7 @@
     </row>
     <row r="58" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A58" t="s">
-        <v>724</v>
+        <v>723</v>
       </c>
       <c r="B58" t="s">
         <v>433</v>
@@ -6999,7 +6999,7 @@
         <v>119</v>
       </c>
       <c r="B61" t="s">
-        <v>716</v>
+        <v>715</v>
       </c>
     </row>
     <row r="62" spans="1:2" x14ac:dyDescent="0.25">
@@ -7167,7 +7167,7 @@
         <v>649</v>
       </c>
       <c r="B82" t="s">
-        <v>720</v>
+        <v>719</v>
       </c>
     </row>
     <row r="83" spans="1:2" x14ac:dyDescent="0.25">
@@ -7220,7 +7220,7 @@
     </row>
     <row r="89" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A89" t="s">
-        <v>684</v>
+        <v>683</v>
       </c>
       <c r="B89" t="s">
         <v>444</v>
@@ -7228,7 +7228,7 @@
     </row>
     <row r="90" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A90" t="s">
-        <v>691</v>
+        <v>690</v>
       </c>
       <c r="B90" t="s">
         <v>444</v>
@@ -7239,7 +7239,7 @@
         <v>135</v>
       </c>
       <c r="B91" t="s">
-        <v>717</v>
+        <v>716</v>
       </c>
     </row>
     <row r="92" spans="1:2" x14ac:dyDescent="0.25">
@@ -7263,7 +7263,7 @@
         <v>121</v>
       </c>
       <c r="B94" t="s">
-        <v>712</v>
+        <v>711</v>
       </c>
     </row>
     <row r="95" spans="1:2" x14ac:dyDescent="0.25">
@@ -7271,7 +7271,7 @@
         <v>126</v>
       </c>
       <c r="B95" t="s">
-        <v>721</v>
+        <v>720</v>
       </c>
     </row>
     <row r="96" spans="1:2" x14ac:dyDescent="0.25">
@@ -7340,7 +7340,7 @@
     </row>
     <row r="104" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A104" t="s">
-        <v>680</v>
+        <v>679</v>
       </c>
       <c r="B104" t="s">
         <v>432</v>
@@ -7348,7 +7348,7 @@
     </row>
     <row r="105" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A105" t="s">
-        <v>687</v>
+        <v>686</v>
       </c>
       <c r="B105" t="s">
         <v>432</v>
@@ -7415,7 +7415,7 @@
         <v>475</v>
       </c>
       <c r="B113" t="s">
-        <v>715</v>
+        <v>714</v>
       </c>
     </row>
     <row r="114" spans="1:2" x14ac:dyDescent="0.25">
@@ -7455,7 +7455,7 @@
         <v>123</v>
       </c>
       <c r="B118" t="s">
-        <v>718</v>
+        <v>717</v>
       </c>
     </row>
     <row r="119" spans="1:2" x14ac:dyDescent="0.25">
@@ -7468,7 +7468,7 @@
     </row>
     <row r="120" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A120" t="s">
-        <v>685</v>
+        <v>684</v>
       </c>
       <c r="B120" t="s">
         <v>478</v>
@@ -7476,7 +7476,7 @@
     </row>
     <row r="121" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A121" t="s">
-        <v>692</v>
+        <v>691</v>
       </c>
       <c r="B121" t="s">
         <v>478</v>
@@ -7519,7 +7519,7 @@
         <v>474</v>
       </c>
       <c r="B126" t="s">
-        <v>714</v>
+        <v>713</v>
       </c>
     </row>
     <row r="127" spans="1:2" x14ac:dyDescent="0.25">
@@ -7607,7 +7607,7 @@
         <v>476</v>
       </c>
       <c r="B137" t="s">
-        <v>722</v>
+        <v>721</v>
       </c>
     </row>
     <row r="138" spans="1:2" x14ac:dyDescent="0.25">
@@ -7668,7 +7668,7 @@
     </row>
     <row r="145" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A145" t="s">
-        <v>682</v>
+        <v>681</v>
       </c>
       <c r="B145" t="s">
         <v>434</v>
@@ -7676,7 +7676,7 @@
     </row>
     <row r="146" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A146" t="s">
-        <v>689</v>
+        <v>688</v>
       </c>
       <c r="B146" t="s">
         <v>434</v>
@@ -7748,7 +7748,7 @@
     </row>
     <row r="155" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A155" t="s">
-        <v>681</v>
+        <v>680</v>
       </c>
       <c r="B155" t="s">
         <v>438</v>
@@ -7756,7 +7756,7 @@
     </row>
     <row r="156" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A156" t="s">
-        <v>688</v>
+        <v>687</v>
       </c>
       <c r="B156" t="s">
         <v>438</v>
@@ -7783,7 +7783,7 @@
         <v>648</v>
       </c>
       <c r="B159" t="s">
-        <v>719</v>
+        <v>718</v>
       </c>
     </row>
     <row r="160" spans="1:2" x14ac:dyDescent="0.25">
@@ -7812,7 +7812,7 @@
     </row>
     <row r="163" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A163" t="s">
-        <v>696</v>
+        <v>695</v>
       </c>
       <c r="B163" t="s">
         <v>650</v>
@@ -7820,15 +7820,15 @@
     </row>
     <row r="164" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A164" t="s">
-        <v>698</v>
+        <v>697</v>
       </c>
       <c r="B164" t="s">
-        <v>705</v>
+        <v>704</v>
       </c>
     </row>
     <row r="165" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A165" t="s">
-        <v>695</v>
+        <v>694</v>
       </c>
       <c r="B165" t="s">
         <v>652</v>
@@ -7836,7 +7836,7 @@
     </row>
     <row r="166" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A166" t="s">
-        <v>704</v>
+        <v>703</v>
       </c>
       <c r="B166" t="s">
         <v>653</v>
@@ -7844,10 +7844,10 @@
     </row>
     <row r="167" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A167" t="s">
-        <v>703</v>
+        <v>702</v>
       </c>
       <c r="B167" t="s">
-        <v>706</v>
+        <v>705</v>
       </c>
     </row>
     <row r="168" spans="1:2" x14ac:dyDescent="0.25">
@@ -7887,7 +7887,7 @@
         <v>522</v>
       </c>
       <c r="B172" t="s">
-        <v>709</v>
+        <v>708</v>
       </c>
     </row>
     <row r="173" spans="1:2" x14ac:dyDescent="0.25">
@@ -7895,7 +7895,7 @@
         <v>523</v>
       </c>
       <c r="B173" t="s">
-        <v>710</v>
+        <v>709</v>
       </c>
     </row>
   </sheetData>
@@ -7914,8 +7914,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{8FD61665-6B06-460E-828D-1570B45BB2AE}">
   <dimension ref="A1:B7"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="B6" sqref="B6"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="B7" sqref="B7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -7968,7 +7968,7 @@
         <v>477</v>
       </c>
       <c r="B6" t="s">
-        <v>678</v>
+        <v>725</v>
       </c>
     </row>
     <row r="7" spans="1:2" x14ac:dyDescent="0.25">
@@ -14007,7 +14007,7 @@
         <v>484</v>
       </c>
       <c r="B1" s="15" t="s">
-        <v>699</v>
+        <v>698</v>
       </c>
       <c r="C1" s="15" t="s">
         <v>493</v>
@@ -14036,7 +14036,7 @@
         <v>486</v>
       </c>
       <c r="B2" t="s">
-        <v>700</v>
+        <v>699</v>
       </c>
       <c r="C2" t="s">
         <v>488</v>
@@ -14065,7 +14065,7 @@
         <v>486</v>
       </c>
       <c r="B3" t="s">
-        <v>700</v>
+        <v>699</v>
       </c>
       <c r="C3" t="s">
         <v>488</v>
@@ -14094,7 +14094,7 @@
         <v>486</v>
       </c>
       <c r="B4" t="s">
-        <v>700</v>
+        <v>699</v>
       </c>
       <c r="C4" t="s">
         <v>488</v>
@@ -14123,7 +14123,7 @@
         <v>486</v>
       </c>
       <c r="B5" t="s">
-        <v>700</v>
+        <v>699</v>
       </c>
       <c r="C5" t="s">
         <v>488</v>
@@ -14152,7 +14152,7 @@
         <v>486</v>
       </c>
       <c r="B6" t="s">
-        <v>700</v>
+        <v>699</v>
       </c>
       <c r="C6" t="s">
         <v>488</v>
@@ -14181,7 +14181,7 @@
         <v>486</v>
       </c>
       <c r="B7" t="s">
-        <v>700</v>
+        <v>699</v>
       </c>
       <c r="C7" t="s">
         <v>488</v>
@@ -14210,7 +14210,7 @@
         <v>486</v>
       </c>
       <c r="B8" t="s">
-        <v>700</v>
+        <v>699</v>
       </c>
       <c r="C8" t="s">
         <v>488</v>
@@ -14239,7 +14239,7 @@
         <v>486</v>
       </c>
       <c r="B9" t="s">
-        <v>700</v>
+        <v>699</v>
       </c>
       <c r="C9" t="s">
         <v>488</v>
@@ -14268,7 +14268,7 @@
         <v>486</v>
       </c>
       <c r="B10" t="s">
-        <v>700</v>
+        <v>699</v>
       </c>
       <c r="C10" t="s">
         <v>488</v>
@@ -14297,7 +14297,7 @@
         <v>486</v>
       </c>
       <c r="B11" t="s">
-        <v>700</v>
+        <v>699</v>
       </c>
       <c r="C11" t="s">
         <v>488</v>
@@ -14326,7 +14326,7 @@
         <v>486</v>
       </c>
       <c r="B12" t="s">
-        <v>700</v>
+        <v>699</v>
       </c>
       <c r="C12" t="s">
         <v>488</v>
@@ -14355,7 +14355,7 @@
         <v>486</v>
       </c>
       <c r="B13" t="s">
-        <v>700</v>
+        <v>699</v>
       </c>
       <c r="C13" t="s">
         <v>488</v>
@@ -14384,7 +14384,7 @@
         <v>486</v>
       </c>
       <c r="B14" t="s">
-        <v>700</v>
+        <v>699</v>
       </c>
       <c r="C14" t="s">
         <v>488</v>
@@ -14413,7 +14413,7 @@
         <v>486</v>
       </c>
       <c r="B15" t="s">
-        <v>700</v>
+        <v>699</v>
       </c>
       <c r="C15" t="s">
         <v>488</v>
@@ -14442,7 +14442,7 @@
         <v>486</v>
       </c>
       <c r="B16" t="s">
-        <v>700</v>
+        <v>699</v>
       </c>
       <c r="C16" t="s">
         <v>488</v>
@@ -14471,7 +14471,7 @@
         <v>486</v>
       </c>
       <c r="B17" t="s">
-        <v>700</v>
+        <v>699</v>
       </c>
       <c r="C17" t="s">
         <v>488</v>
@@ -14500,7 +14500,7 @@
         <v>486</v>
       </c>
       <c r="B18" t="s">
-        <v>700</v>
+        <v>699</v>
       </c>
       <c r="C18" t="s">
         <v>488</v>
@@ -14529,7 +14529,7 @@
         <v>486</v>
       </c>
       <c r="B19" t="s">
-        <v>700</v>
+        <v>699</v>
       </c>
       <c r="C19" t="s">
         <v>488</v>
@@ -14558,7 +14558,7 @@
         <v>486</v>
       </c>
       <c r="B20" t="s">
-        <v>700</v>
+        <v>699</v>
       </c>
       <c r="C20" t="s">
         <v>488</v>
@@ -14587,7 +14587,7 @@
         <v>486</v>
       </c>
       <c r="B21" t="s">
-        <v>700</v>
+        <v>699</v>
       </c>
       <c r="C21" t="s">
         <v>488</v>
@@ -14616,7 +14616,7 @@
         <v>486</v>
       </c>
       <c r="B22" t="s">
-        <v>700</v>
+        <v>699</v>
       </c>
       <c r="C22" t="s">
         <v>488</v>
@@ -14645,7 +14645,7 @@
         <v>486</v>
       </c>
       <c r="B23" t="s">
-        <v>700</v>
+        <v>699</v>
       </c>
       <c r="C23" t="s">
         <v>488</v>
@@ -14674,7 +14674,7 @@
         <v>486</v>
       </c>
       <c r="B24" t="s">
-        <v>700</v>
+        <v>699</v>
       </c>
       <c r="C24" t="s">
         <v>488</v>
@@ -14703,7 +14703,7 @@
         <v>486</v>
       </c>
       <c r="B25" t="s">
-        <v>700</v>
+        <v>699</v>
       </c>
       <c r="C25" t="s">
         <v>488</v>
@@ -14732,7 +14732,7 @@
         <v>486</v>
       </c>
       <c r="B26" t="s">
-        <v>700</v>
+        <v>699</v>
       </c>
       <c r="C26" t="s">
         <v>488</v>
@@ -14761,7 +14761,7 @@
         <v>486</v>
       </c>
       <c r="B27" t="s">
-        <v>700</v>
+        <v>699</v>
       </c>
       <c r="C27" t="s">
         <v>488</v>
@@ -14790,7 +14790,7 @@
         <v>486</v>
       </c>
       <c r="B28" t="s">
-        <v>700</v>
+        <v>699</v>
       </c>
       <c r="C28" t="s">
         <v>488</v>
@@ -14819,7 +14819,7 @@
         <v>486</v>
       </c>
       <c r="B29" t="s">
-        <v>700</v>
+        <v>699</v>
       </c>
       <c r="C29" t="s">
         <v>488</v>
@@ -14848,7 +14848,7 @@
         <v>486</v>
       </c>
       <c r="B30" t="s">
-        <v>700</v>
+        <v>699</v>
       </c>
       <c r="C30" t="s">
         <v>488</v>
@@ -14877,7 +14877,7 @@
         <v>486</v>
       </c>
       <c r="B31" t="s">
-        <v>700</v>
+        <v>699</v>
       </c>
       <c r="C31" t="s">
         <v>488</v>
@@ -14906,7 +14906,7 @@
         <v>486</v>
       </c>
       <c r="B32" t="s">
-        <v>700</v>
+        <v>699</v>
       </c>
       <c r="C32" t="s">
         <v>488</v>
@@ -14935,7 +14935,7 @@
         <v>486</v>
       </c>
       <c r="B33" t="s">
-        <v>700</v>
+        <v>699</v>
       </c>
       <c r="C33" t="s">
         <v>488</v>
@@ -14964,7 +14964,7 @@
         <v>486</v>
       </c>
       <c r="B34" t="s">
-        <v>700</v>
+        <v>699</v>
       </c>
       <c r="C34" t="s">
         <v>488</v>
@@ -14993,7 +14993,7 @@
         <v>486</v>
       </c>
       <c r="B35" t="s">
-        <v>700</v>
+        <v>699</v>
       </c>
       <c r="C35" t="s">
         <v>488</v>
@@ -15022,7 +15022,7 @@
         <v>486</v>
       </c>
       <c r="B36" t="s">
-        <v>700</v>
+        <v>699</v>
       </c>
       <c r="C36" t="s">
         <v>488</v>
@@ -15051,7 +15051,7 @@
         <v>486</v>
       </c>
       <c r="B37" t="s">
-        <v>700</v>
+        <v>699</v>
       </c>
       <c r="C37" t="s">
         <v>488</v>
@@ -15080,7 +15080,7 @@
         <v>486</v>
       </c>
       <c r="B38" t="s">
-        <v>700</v>
+        <v>699</v>
       </c>
       <c r="C38" t="s">
         <v>488</v>
@@ -15109,7 +15109,7 @@
         <v>486</v>
       </c>
       <c r="B39" t="s">
-        <v>700</v>
+        <v>699</v>
       </c>
       <c r="C39" t="s">
         <v>488</v>
@@ -15138,7 +15138,7 @@
         <v>486</v>
       </c>
       <c r="B40" t="s">
-        <v>700</v>
+        <v>699</v>
       </c>
       <c r="C40" t="s">
         <v>488</v>
@@ -15167,7 +15167,7 @@
         <v>486</v>
       </c>
       <c r="B41" t="s">
-        <v>700</v>
+        <v>699</v>
       </c>
       <c r="C41" t="s">
         <v>488</v>
@@ -15196,7 +15196,7 @@
         <v>486</v>
       </c>
       <c r="B42" t="s">
-        <v>700</v>
+        <v>699</v>
       </c>
       <c r="C42" t="s">
         <v>488</v>
@@ -15225,7 +15225,7 @@
         <v>486</v>
       </c>
       <c r="B43" t="s">
-        <v>700</v>
+        <v>699</v>
       </c>
       <c r="C43" t="s">
         <v>488</v>
@@ -15254,7 +15254,7 @@
         <v>486</v>
       </c>
       <c r="B44" t="s">
-        <v>700</v>
+        <v>699</v>
       </c>
       <c r="C44" t="s">
         <v>488</v>
@@ -15283,7 +15283,7 @@
         <v>486</v>
       </c>
       <c r="B45" t="s">
-        <v>700</v>
+        <v>699</v>
       </c>
       <c r="C45" t="s">
         <v>488</v>
@@ -15312,7 +15312,7 @@
         <v>486</v>
       </c>
       <c r="B46" t="s">
-        <v>700</v>
+        <v>699</v>
       </c>
       <c r="C46" t="s">
         <v>488</v>
@@ -15341,7 +15341,7 @@
         <v>486</v>
       </c>
       <c r="B47" t="s">
-        <v>700</v>
+        <v>699</v>
       </c>
       <c r="C47" t="s">
         <v>488</v>
@@ -15370,7 +15370,7 @@
         <v>486</v>
       </c>
       <c r="B48" t="s">
-        <v>700</v>
+        <v>699</v>
       </c>
       <c r="C48" t="s">
         <v>488</v>
@@ -15399,7 +15399,7 @@
         <v>486</v>
       </c>
       <c r="B49" t="s">
-        <v>700</v>
+        <v>699</v>
       </c>
       <c r="C49" t="s">
         <v>488</v>
@@ -15428,7 +15428,7 @@
         <v>486</v>
       </c>
       <c r="B50" t="s">
-        <v>700</v>
+        <v>699</v>
       </c>
       <c r="C50" t="s">
         <v>488</v>
@@ -15457,7 +15457,7 @@
         <v>486</v>
       </c>
       <c r="B51" t="s">
-        <v>700</v>
+        <v>699</v>
       </c>
       <c r="C51" t="s">
         <v>488</v>
@@ -15486,7 +15486,7 @@
         <v>486</v>
       </c>
       <c r="B52" t="s">
-        <v>700</v>
+        <v>699</v>
       </c>
       <c r="C52" t="s">
         <v>488</v>
@@ -15515,7 +15515,7 @@
         <v>486</v>
       </c>
       <c r="B53" t="s">
-        <v>700</v>
+        <v>699</v>
       </c>
       <c r="C53" t="s">
         <v>488</v>
@@ -15544,7 +15544,7 @@
         <v>486</v>
       </c>
       <c r="B54" t="s">
-        <v>700</v>
+        <v>699</v>
       </c>
       <c r="C54" t="s">
         <v>488</v>
@@ -15573,7 +15573,7 @@
         <v>486</v>
       </c>
       <c r="B55" t="s">
-        <v>700</v>
+        <v>699</v>
       </c>
       <c r="C55" t="s">
         <v>488</v>
@@ -15602,7 +15602,7 @@
         <v>486</v>
       </c>
       <c r="B56" t="s">
-        <v>700</v>
+        <v>699</v>
       </c>
       <c r="C56" t="s">
         <v>488</v>
@@ -15631,7 +15631,7 @@
         <v>486</v>
       </c>
       <c r="B57" t="s">
-        <v>700</v>
+        <v>699</v>
       </c>
       <c r="C57" t="s">
         <v>488</v>
@@ -15660,7 +15660,7 @@
         <v>486</v>
       </c>
       <c r="B58" t="s">
-        <v>700</v>
+        <v>699</v>
       </c>
       <c r="C58" t="s">
         <v>488</v>
@@ -15689,7 +15689,7 @@
         <v>486</v>
       </c>
       <c r="B59" t="s">
-        <v>700</v>
+        <v>699</v>
       </c>
       <c r="C59" t="s">
         <v>488</v>
@@ -15718,7 +15718,7 @@
         <v>486</v>
       </c>
       <c r="B60" t="s">
-        <v>700</v>
+        <v>699</v>
       </c>
       <c r="C60" t="s">
         <v>488</v>
@@ -15747,7 +15747,7 @@
         <v>486</v>
       </c>
       <c r="B61" t="s">
-        <v>700</v>
+        <v>699</v>
       </c>
       <c r="C61" t="s">
         <v>488</v>
@@ -15776,7 +15776,7 @@
         <v>486</v>
       </c>
       <c r="B62" t="s">
-        <v>700</v>
+        <v>699</v>
       </c>
       <c r="C62" t="s">
         <v>488</v>
@@ -15805,7 +15805,7 @@
         <v>486</v>
       </c>
       <c r="B63" t="s">
-        <v>700</v>
+        <v>699</v>
       </c>
       <c r="C63" t="s">
         <v>488</v>
@@ -15834,7 +15834,7 @@
         <v>486</v>
       </c>
       <c r="B64" t="s">
-        <v>700</v>
+        <v>699</v>
       </c>
       <c r="C64" t="s">
         <v>488</v>
@@ -15863,7 +15863,7 @@
         <v>486</v>
       </c>
       <c r="B65" t="s">
-        <v>700</v>
+        <v>699</v>
       </c>
       <c r="C65" t="s">
         <v>488</v>
@@ -15892,7 +15892,7 @@
         <v>486</v>
       </c>
       <c r="B66" t="s">
-        <v>700</v>
+        <v>699</v>
       </c>
       <c r="C66" t="s">
         <v>488</v>
@@ -15921,7 +15921,7 @@
         <v>486</v>
       </c>
       <c r="B67" t="s">
-        <v>700</v>
+        <v>699</v>
       </c>
       <c r="C67" t="s">
         <v>488</v>
@@ -15950,7 +15950,7 @@
         <v>486</v>
       </c>
       <c r="B68" t="s">
-        <v>700</v>
+        <v>699</v>
       </c>
       <c r="C68" t="s">
         <v>488</v>
@@ -15979,7 +15979,7 @@
         <v>486</v>
       </c>
       <c r="B69" t="s">
-        <v>700</v>
+        <v>699</v>
       </c>
       <c r="C69" t="s">
         <v>488</v>
@@ -16008,7 +16008,7 @@
         <v>486</v>
       </c>
       <c r="B70" t="s">
-        <v>707</v>
+        <v>706</v>
       </c>
       <c r="C70" t="s">
         <v>487</v>
@@ -16029,7 +16029,7 @@
         <v>486</v>
       </c>
       <c r="B71" t="s">
-        <v>707</v>
+        <v>706</v>
       </c>
       <c r="C71" t="s">
         <v>487</v>
@@ -16050,7 +16050,7 @@
         <v>486</v>
       </c>
       <c r="B72" t="s">
-        <v>707</v>
+        <v>706</v>
       </c>
       <c r="C72" t="s">
         <v>487</v>
@@ -16071,7 +16071,7 @@
         <v>486</v>
       </c>
       <c r="B73" t="s">
-        <v>707</v>
+        <v>706</v>
       </c>
       <c r="C73" t="s">
         <v>487</v>
@@ -16092,7 +16092,7 @@
         <v>486</v>
       </c>
       <c r="B74" t="s">
-        <v>707</v>
+        <v>706</v>
       </c>
       <c r="C74" t="s">
         <v>487</v>
@@ -16113,7 +16113,7 @@
         <v>486</v>
       </c>
       <c r="B75" t="s">
-        <v>707</v>
+        <v>706</v>
       </c>
       <c r="C75" t="s">
         <v>487</v>
@@ -16134,7 +16134,7 @@
         <v>486</v>
       </c>
       <c r="B76" t="s">
-        <v>707</v>
+        <v>706</v>
       </c>
       <c r="C76" t="s">
         <v>487</v>
@@ -16155,7 +16155,7 @@
         <v>486</v>
       </c>
       <c r="B77" t="s">
-        <v>707</v>
+        <v>706</v>
       </c>
       <c r="C77" t="s">
         <v>487</v>
@@ -16176,7 +16176,7 @@
         <v>486</v>
       </c>
       <c r="B78" t="s">
-        <v>707</v>
+        <v>706</v>
       </c>
       <c r="C78" t="s">
         <v>487</v>
@@ -16197,7 +16197,7 @@
         <v>486</v>
       </c>
       <c r="B79" t="s">
-        <v>707</v>
+        <v>706</v>
       </c>
       <c r="C79" t="s">
         <v>487</v>
@@ -16218,7 +16218,7 @@
         <v>486</v>
       </c>
       <c r="B80" t="s">
-        <v>707</v>
+        <v>706</v>
       </c>
       <c r="C80" t="s">
         <v>487</v>
@@ -16239,7 +16239,7 @@
         <v>486</v>
       </c>
       <c r="B81" t="s">
-        <v>707</v>
+        <v>706</v>
       </c>
       <c r="C81" t="s">
         <v>487</v>
@@ -16260,7 +16260,7 @@
         <v>486</v>
       </c>
       <c r="B82" t="s">
-        <v>707</v>
+        <v>706</v>
       </c>
       <c r="C82" t="s">
         <v>487</v>
@@ -16281,7 +16281,7 @@
         <v>486</v>
       </c>
       <c r="B83" t="s">
-        <v>707</v>
+        <v>706</v>
       </c>
       <c r="C83" t="s">
         <v>487</v>
@@ -16302,7 +16302,7 @@
         <v>486</v>
       </c>
       <c r="B84" t="s">
-        <v>707</v>
+        <v>706</v>
       </c>
       <c r="C84" t="s">
         <v>487</v>
@@ -16323,7 +16323,7 @@
         <v>486</v>
       </c>
       <c r="B85" t="s">
-        <v>707</v>
+        <v>706</v>
       </c>
       <c r="C85" t="s">
         <v>487</v>
@@ -16344,7 +16344,7 @@
         <v>486</v>
       </c>
       <c r="B86" t="s">
-        <v>707</v>
+        <v>706</v>
       </c>
       <c r="C86" t="s">
         <v>487</v>
@@ -16365,7 +16365,7 @@
         <v>486</v>
       </c>
       <c r="B87" t="s">
-        <v>707</v>
+        <v>706</v>
       </c>
       <c r="C87" t="s">
         <v>487</v>
@@ -16386,7 +16386,7 @@
         <v>486</v>
       </c>
       <c r="B88" t="s">
-        <v>707</v>
+        <v>706</v>
       </c>
       <c r="C88" t="s">
         <v>487</v>
@@ -16407,7 +16407,7 @@
         <v>486</v>
       </c>
       <c r="B89" t="s">
-        <v>707</v>
+        <v>706</v>
       </c>
       <c r="C89" t="s">
         <v>487</v>
@@ -16428,7 +16428,7 @@
         <v>486</v>
       </c>
       <c r="B90" t="s">
-        <v>707</v>
+        <v>706</v>
       </c>
       <c r="C90" t="s">
         <v>487</v>
@@ -16449,7 +16449,7 @@
         <v>486</v>
       </c>
       <c r="B91" t="s">
-        <v>707</v>
+        <v>706</v>
       </c>
       <c r="C91" t="s">
         <v>487</v>
@@ -16470,7 +16470,7 @@
         <v>486</v>
       </c>
       <c r="B92" t="s">
-        <v>700</v>
+        <v>699</v>
       </c>
       <c r="C92" t="s">
         <v>488</v>
@@ -16499,7 +16499,7 @@
         <v>486</v>
       </c>
       <c r="B93" t="s">
-        <v>700</v>
+        <v>699</v>
       </c>
       <c r="C93" t="s">
         <v>488</v>
@@ -16528,7 +16528,7 @@
         <v>486</v>
       </c>
       <c r="B94" t="s">
-        <v>700</v>
+        <v>699</v>
       </c>
       <c r="C94" t="s">
         <v>488</v>
@@ -16557,7 +16557,7 @@
         <v>486</v>
       </c>
       <c r="B95" t="s">
-        <v>700</v>
+        <v>699</v>
       </c>
       <c r="C95" t="s">
         <v>488</v>
@@ -16586,13 +16586,13 @@
         <v>486</v>
       </c>
       <c r="B96" t="s">
-        <v>701</v>
+        <v>700</v>
       </c>
       <c r="C96" t="s">
-        <v>711</v>
+        <v>710</v>
       </c>
       <c r="D96" t="s">
-        <v>687</v>
+        <v>686</v>
       </c>
       <c r="E96" t="s">
         <v>158</v>
@@ -16615,13 +16615,13 @@
         <v>486</v>
       </c>
       <c r="B97" t="s">
-        <v>701</v>
+        <v>700</v>
       </c>
       <c r="C97" t="s">
-        <v>711</v>
+        <v>710</v>
       </c>
       <c r="D97" t="s">
-        <v>687</v>
+        <v>686</v>
       </c>
       <c r="E97" t="s">
         <v>158</v>
@@ -16644,13 +16644,13 @@
         <v>486</v>
       </c>
       <c r="B98" t="s">
-        <v>701</v>
+        <v>700</v>
       </c>
       <c r="C98" t="s">
-        <v>711</v>
+        <v>710</v>
       </c>
       <c r="D98" t="s">
-        <v>688</v>
+        <v>687</v>
       </c>
       <c r="E98" t="s">
         <v>158</v>
@@ -16673,13 +16673,13 @@
         <v>486</v>
       </c>
       <c r="B99" t="s">
-        <v>701</v>
+        <v>700</v>
       </c>
       <c r="C99" t="s">
-        <v>711</v>
+        <v>710</v>
       </c>
       <c r="D99" t="s">
-        <v>689</v>
+        <v>688</v>
       </c>
       <c r="E99" t="s">
         <v>158</v>
@@ -16702,13 +16702,13 @@
         <v>486</v>
       </c>
       <c r="B100" t="s">
-        <v>701</v>
+        <v>700</v>
       </c>
       <c r="C100" t="s">
-        <v>711</v>
+        <v>710</v>
       </c>
       <c r="D100" t="s">
-        <v>690</v>
+        <v>689</v>
       </c>
       <c r="E100" t="s">
         <v>158</v>
@@ -16731,13 +16731,13 @@
         <v>486</v>
       </c>
       <c r="B101" t="s">
-        <v>701</v>
+        <v>700</v>
       </c>
       <c r="C101" t="s">
-        <v>711</v>
+        <v>710</v>
       </c>
       <c r="D101" t="s">
-        <v>690</v>
+        <v>689</v>
       </c>
       <c r="E101" t="s">
         <v>158</v>
@@ -16760,13 +16760,13 @@
         <v>486</v>
       </c>
       <c r="B102" t="s">
-        <v>701</v>
+        <v>700</v>
       </c>
       <c r="C102" t="s">
-        <v>711</v>
+        <v>710</v>
       </c>
       <c r="D102" t="s">
-        <v>691</v>
+        <v>690</v>
       </c>
       <c r="E102" t="s">
         <v>158</v>
@@ -16789,13 +16789,13 @@
         <v>486</v>
       </c>
       <c r="B103" t="s">
-        <v>701</v>
+        <v>700</v>
       </c>
       <c r="C103" t="s">
-        <v>711</v>
+        <v>710</v>
       </c>
       <c r="D103" t="s">
-        <v>692</v>
+        <v>691</v>
       </c>
       <c r="E103" t="s">
         <v>158</v>
@@ -16818,13 +16818,13 @@
         <v>486</v>
       </c>
       <c r="B104" t="s">
-        <v>701</v>
+        <v>700</v>
       </c>
       <c r="C104" t="s">
-        <v>711</v>
+        <v>710</v>
       </c>
       <c r="D104" t="s">
-        <v>680</v>
+        <v>679</v>
       </c>
       <c r="E104" t="s">
         <v>158</v>
@@ -16847,13 +16847,13 @@
         <v>486</v>
       </c>
       <c r="B105" t="s">
-        <v>701</v>
+        <v>700</v>
       </c>
       <c r="C105" t="s">
-        <v>711</v>
+        <v>710</v>
       </c>
       <c r="D105" t="s">
-        <v>680</v>
+        <v>679</v>
       </c>
       <c r="E105" t="s">
         <v>158</v>
@@ -16876,13 +16876,13 @@
         <v>486</v>
       </c>
       <c r="B106" t="s">
-        <v>701</v>
+        <v>700</v>
       </c>
       <c r="C106" t="s">
-        <v>711</v>
+        <v>710</v>
       </c>
       <c r="D106" t="s">
-        <v>681</v>
+        <v>680</v>
       </c>
       <c r="E106" t="s">
         <v>158</v>
@@ -16905,13 +16905,13 @@
         <v>486</v>
       </c>
       <c r="B107" t="s">
-        <v>701</v>
+        <v>700</v>
       </c>
       <c r="C107" t="s">
-        <v>711</v>
+        <v>710</v>
       </c>
       <c r="D107" t="s">
-        <v>682</v>
+        <v>681</v>
       </c>
       <c r="E107" t="s">
         <v>158</v>
@@ -16934,13 +16934,13 @@
         <v>486</v>
       </c>
       <c r="B108" t="s">
-        <v>701</v>
+        <v>700</v>
       </c>
       <c r="C108" t="s">
-        <v>711</v>
+        <v>710</v>
       </c>
       <c r="D108" t="s">
-        <v>683</v>
+        <v>682</v>
       </c>
       <c r="E108" t="s">
         <v>158</v>
@@ -16963,13 +16963,13 @@
         <v>486</v>
       </c>
       <c r="B109" t="s">
-        <v>701</v>
+        <v>700</v>
       </c>
       <c r="C109" t="s">
-        <v>711</v>
+        <v>710</v>
       </c>
       <c r="D109" t="s">
-        <v>683</v>
+        <v>682</v>
       </c>
       <c r="E109" t="s">
         <v>158</v>
@@ -16992,13 +16992,13 @@
         <v>486</v>
       </c>
       <c r="B110" t="s">
-        <v>701</v>
+        <v>700</v>
       </c>
       <c r="C110" t="s">
-        <v>711</v>
+        <v>710</v>
       </c>
       <c r="D110" t="s">
-        <v>684</v>
+        <v>683</v>
       </c>
       <c r="E110" t="s">
         <v>158</v>
@@ -17021,13 +17021,13 @@
         <v>486</v>
       </c>
       <c r="B111" t="s">
-        <v>701</v>
+        <v>700</v>
       </c>
       <c r="C111" t="s">
-        <v>711</v>
+        <v>710</v>
       </c>
       <c r="D111" t="s">
-        <v>685</v>
+        <v>684</v>
       </c>
       <c r="E111" t="s">
         <v>158</v>
@@ -17050,13 +17050,13 @@
         <v>486</v>
       </c>
       <c r="B112" t="s">
-        <v>702</v>
+        <v>701</v>
       </c>
       <c r="C112" t="s">
+        <v>693</v>
+      </c>
+      <c r="D112" t="s">
         <v>694</v>
-      </c>
-      <c r="D112" t="s">
-        <v>695</v>
       </c>
       <c r="E112" t="s">
         <v>158</v>
@@ -17079,13 +17079,13 @@
         <v>486</v>
       </c>
       <c r="B113" t="s">
-        <v>702</v>
+        <v>701</v>
       </c>
       <c r="C113" t="s">
+        <v>693</v>
+      </c>
+      <c r="D113" t="s">
         <v>694</v>
-      </c>
-      <c r="D113" t="s">
-        <v>695</v>
       </c>
       <c r="E113" t="s">
         <v>158</v>
@@ -17108,13 +17108,13 @@
         <v>486</v>
       </c>
       <c r="B114" t="s">
-        <v>702</v>
+        <v>701</v>
       </c>
       <c r="C114" t="s">
+        <v>693</v>
+      </c>
+      <c r="D114" t="s">
         <v>694</v>
-      </c>
-      <c r="D114" t="s">
-        <v>695</v>
       </c>
       <c r="E114" t="s">
         <v>158</v>
@@ -17137,13 +17137,13 @@
         <v>486</v>
       </c>
       <c r="B115" t="s">
-        <v>702</v>
+        <v>701</v>
       </c>
       <c r="C115" t="s">
+        <v>693</v>
+      </c>
+      <c r="D115" t="s">
         <v>694</v>
-      </c>
-      <c r="D115" t="s">
-        <v>695</v>
       </c>
       <c r="E115" t="s">
         <v>158</v>
@@ -17166,13 +17166,13 @@
         <v>486</v>
       </c>
       <c r="B116" t="s">
-        <v>702</v>
+        <v>701</v>
       </c>
       <c r="C116" t="s">
+        <v>693</v>
+      </c>
+      <c r="D116" t="s">
         <v>694</v>
-      </c>
-      <c r="D116" t="s">
-        <v>695</v>
       </c>
       <c r="E116" t="s">
         <v>158</v>
@@ -17195,13 +17195,13 @@
         <v>486</v>
       </c>
       <c r="B117" t="s">
-        <v>702</v>
+        <v>701</v>
       </c>
       <c r="C117" t="s">
+        <v>693</v>
+      </c>
+      <c r="D117" t="s">
         <v>694</v>
-      </c>
-      <c r="D117" t="s">
-        <v>695</v>
       </c>
       <c r="E117" t="s">
         <v>158</v>
@@ -17224,13 +17224,13 @@
         <v>486</v>
       </c>
       <c r="B118" t="s">
-        <v>702</v>
+        <v>701</v>
       </c>
       <c r="C118" t="s">
+        <v>693</v>
+      </c>
+      <c r="D118" t="s">
         <v>694</v>
-      </c>
-      <c r="D118" t="s">
-        <v>695</v>
       </c>
       <c r="E118" t="s">
         <v>158</v>
@@ -17253,13 +17253,13 @@
         <v>486</v>
       </c>
       <c r="B119" t="s">
-        <v>702</v>
+        <v>701</v>
       </c>
       <c r="C119" t="s">
+        <v>693</v>
+      </c>
+      <c r="D119" t="s">
         <v>694</v>
-      </c>
-      <c r="D119" t="s">
-        <v>695</v>
       </c>
       <c r="E119" t="s">
         <v>158</v>
@@ -17282,13 +17282,13 @@
         <v>486</v>
       </c>
       <c r="B120" t="s">
-        <v>702</v>
+        <v>701</v>
       </c>
       <c r="C120" t="s">
-        <v>694</v>
+        <v>693</v>
       </c>
       <c r="D120" t="s">
-        <v>696</v>
+        <v>695</v>
       </c>
       <c r="E120" t="s">
         <v>158</v>
@@ -17311,13 +17311,13 @@
         <v>486</v>
       </c>
       <c r="B121" t="s">
-        <v>702</v>
+        <v>701</v>
       </c>
       <c r="C121" t="s">
-        <v>694</v>
+        <v>693</v>
       </c>
       <c r="D121" t="s">
-        <v>696</v>
+        <v>695</v>
       </c>
       <c r="E121" t="s">
         <v>158</v>
@@ -17340,13 +17340,13 @@
         <v>486</v>
       </c>
       <c r="B122" t="s">
-        <v>702</v>
+        <v>701</v>
       </c>
       <c r="C122" t="s">
-        <v>694</v>
+        <v>693</v>
       </c>
       <c r="D122" t="s">
-        <v>696</v>
+        <v>695</v>
       </c>
       <c r="E122" t="s">
         <v>158</v>
@@ -17369,13 +17369,13 @@
         <v>486</v>
       </c>
       <c r="B123" t="s">
-        <v>702</v>
+        <v>701</v>
       </c>
       <c r="C123" t="s">
-        <v>694</v>
+        <v>693</v>
       </c>
       <c r="D123" t="s">
-        <v>696</v>
+        <v>695</v>
       </c>
       <c r="E123" t="s">
         <v>158</v>
@@ -17398,13 +17398,13 @@
         <v>486</v>
       </c>
       <c r="B124" t="s">
-        <v>702</v>
+        <v>701</v>
       </c>
       <c r="C124" t="s">
-        <v>694</v>
+        <v>693</v>
       </c>
       <c r="D124" t="s">
-        <v>696</v>
+        <v>695</v>
       </c>
       <c r="E124" t="s">
         <v>158</v>
@@ -17427,13 +17427,13 @@
         <v>486</v>
       </c>
       <c r="B125" t="s">
-        <v>702</v>
+        <v>701</v>
       </c>
       <c r="C125" t="s">
-        <v>694</v>
+        <v>693</v>
       </c>
       <c r="D125" t="s">
-        <v>696</v>
+        <v>695</v>
       </c>
       <c r="E125" t="s">
         <v>158</v>
@@ -17456,13 +17456,13 @@
         <v>486</v>
       </c>
       <c r="B126" t="s">
-        <v>702</v>
+        <v>701</v>
       </c>
       <c r="C126" t="s">
-        <v>694</v>
+        <v>693</v>
       </c>
       <c r="D126" t="s">
-        <v>696</v>
+        <v>695</v>
       </c>
       <c r="E126" t="s">
         <v>158</v>
@@ -17485,13 +17485,13 @@
         <v>486</v>
       </c>
       <c r="B127" t="s">
-        <v>702</v>
+        <v>701</v>
       </c>
       <c r="C127" t="s">
-        <v>694</v>
+        <v>693</v>
       </c>
       <c r="D127" t="s">
-        <v>696</v>
+        <v>695</v>
       </c>
       <c r="E127" t="s">
         <v>158</v>
@@ -17514,13 +17514,13 @@
         <v>486</v>
       </c>
       <c r="B128" t="s">
-        <v>702</v>
+        <v>701</v>
       </c>
       <c r="C128" t="s">
-        <v>694</v>
+        <v>693</v>
       </c>
       <c r="D128" t="s">
-        <v>696</v>
+        <v>695</v>
       </c>
       <c r="E128" t="s">
         <v>158</v>
@@ -17543,13 +17543,13 @@
         <v>486</v>
       </c>
       <c r="B129" t="s">
-        <v>702</v>
+        <v>701</v>
       </c>
       <c r="C129" t="s">
-        <v>694</v>
+        <v>693</v>
       </c>
       <c r="D129" t="s">
-        <v>696</v>
+        <v>695</v>
       </c>
       <c r="E129" t="s">
         <v>158</v>
@@ -17572,13 +17572,13 @@
         <v>486</v>
       </c>
       <c r="B130" t="s">
-        <v>702</v>
+        <v>701</v>
       </c>
       <c r="C130" t="s">
-        <v>694</v>
+        <v>693</v>
       </c>
       <c r="D130" t="s">
-        <v>696</v>
+        <v>695</v>
       </c>
       <c r="E130" t="s">
         <v>158</v>
@@ -17601,13 +17601,13 @@
         <v>486</v>
       </c>
       <c r="B131" t="s">
-        <v>702</v>
+        <v>701</v>
       </c>
       <c r="C131" t="s">
-        <v>694</v>
+        <v>693</v>
       </c>
       <c r="D131" t="s">
-        <v>696</v>
+        <v>695</v>
       </c>
       <c r="E131" t="s">
         <v>158</v>
@@ -17630,13 +17630,13 @@
         <v>486</v>
       </c>
       <c r="B132" t="s">
-        <v>702</v>
+        <v>701</v>
       </c>
       <c r="C132" t="s">
-        <v>694</v>
+        <v>693</v>
       </c>
       <c r="D132" t="s">
-        <v>696</v>
+        <v>695</v>
       </c>
       <c r="E132" t="s">
         <v>158</v>
@@ -17659,13 +17659,13 @@
         <v>486</v>
       </c>
       <c r="B133" t="s">
-        <v>702</v>
+        <v>701</v>
       </c>
       <c r="C133" t="s">
-        <v>694</v>
+        <v>693</v>
       </c>
       <c r="D133" t="s">
-        <v>696</v>
+        <v>695</v>
       </c>
       <c r="E133" t="s">
         <v>158</v>
@@ -17688,13 +17688,13 @@
         <v>486</v>
       </c>
       <c r="B134" t="s">
-        <v>702</v>
+        <v>701</v>
       </c>
       <c r="C134" t="s">
-        <v>694</v>
+        <v>693</v>
       </c>
       <c r="D134" t="s">
-        <v>696</v>
+        <v>695</v>
       </c>
       <c r="E134" t="s">
         <v>158</v>
@@ -17717,13 +17717,13 @@
         <v>486</v>
       </c>
       <c r="B135" t="s">
-        <v>702</v>
+        <v>701</v>
       </c>
       <c r="C135" t="s">
-        <v>694</v>
+        <v>693</v>
       </c>
       <c r="D135" t="s">
-        <v>696</v>
+        <v>695</v>
       </c>
       <c r="E135" t="s">
         <v>158</v>
@@ -17746,13 +17746,13 @@
         <v>486</v>
       </c>
       <c r="B136" t="s">
-        <v>702</v>
+        <v>701</v>
       </c>
       <c r="C136" t="s">
-        <v>694</v>
+        <v>693</v>
       </c>
       <c r="D136" t="s">
-        <v>696</v>
+        <v>695</v>
       </c>
       <c r="E136" t="s">
         <v>158</v>
@@ -17775,13 +17775,13 @@
         <v>486</v>
       </c>
       <c r="B137" t="s">
-        <v>702</v>
+        <v>701</v>
       </c>
       <c r="C137" t="s">
-        <v>694</v>
+        <v>693</v>
       </c>
       <c r="D137" t="s">
-        <v>696</v>
+        <v>695</v>
       </c>
       <c r="E137" t="s">
         <v>158</v>
@@ -17804,13 +17804,13 @@
         <v>486</v>
       </c>
       <c r="B138" t="s">
-        <v>702</v>
+        <v>701</v>
       </c>
       <c r="C138" t="s">
-        <v>694</v>
+        <v>693</v>
       </c>
       <c r="D138" t="s">
-        <v>696</v>
+        <v>695</v>
       </c>
       <c r="E138" t="s">
         <v>158</v>
@@ -17833,13 +17833,13 @@
         <v>486</v>
       </c>
       <c r="B139" t="s">
-        <v>702</v>
+        <v>701</v>
       </c>
       <c r="C139" t="s">
-        <v>694</v>
+        <v>693</v>
       </c>
       <c r="D139" t="s">
-        <v>696</v>
+        <v>695</v>
       </c>
       <c r="E139" t="s">
         <v>158</v>
@@ -17862,13 +17862,13 @@
         <v>486</v>
       </c>
       <c r="B140" t="s">
-        <v>702</v>
+        <v>701</v>
       </c>
       <c r="C140" t="s">
-        <v>694</v>
+        <v>693</v>
       </c>
       <c r="D140" t="s">
-        <v>696</v>
+        <v>695</v>
       </c>
       <c r="E140" t="s">
         <v>158</v>
@@ -17891,13 +17891,13 @@
         <v>486</v>
       </c>
       <c r="B141" t="s">
-        <v>702</v>
+        <v>701</v>
       </c>
       <c r="C141" t="s">
-        <v>694</v>
+        <v>693</v>
       </c>
       <c r="D141" t="s">
-        <v>696</v>
+        <v>695</v>
       </c>
       <c r="E141" t="s">
         <v>158</v>
@@ -17920,13 +17920,13 @@
         <v>486</v>
       </c>
       <c r="B142" t="s">
-        <v>702</v>
+        <v>701</v>
       </c>
       <c r="C142" t="s">
-        <v>694</v>
+        <v>693</v>
       </c>
       <c r="D142" t="s">
-        <v>696</v>
+        <v>695</v>
       </c>
       <c r="E142" t="s">
         <v>158</v>
@@ -17949,13 +17949,13 @@
         <v>486</v>
       </c>
       <c r="B143" t="s">
-        <v>702</v>
+        <v>701</v>
       </c>
       <c r="C143" t="s">
-        <v>694</v>
+        <v>693</v>
       </c>
       <c r="D143" t="s">
-        <v>696</v>
+        <v>695</v>
       </c>
       <c r="E143" t="s">
         <v>158</v>
@@ -17978,13 +17978,13 @@
         <v>486</v>
       </c>
       <c r="B144" t="s">
+        <v>701</v>
+      </c>
+      <c r="C144" t="s">
+        <v>693</v>
+      </c>
+      <c r="D144" t="s">
         <v>702</v>
-      </c>
-      <c r="C144" t="s">
-        <v>694</v>
-      </c>
-      <c r="D144" t="s">
-        <v>703</v>
       </c>
       <c r="E144" t="s">
         <v>158</v>
@@ -18007,13 +18007,13 @@
         <v>486</v>
       </c>
       <c r="B145" t="s">
+        <v>701</v>
+      </c>
+      <c r="C145" t="s">
+        <v>693</v>
+      </c>
+      <c r="D145" t="s">
         <v>702</v>
-      </c>
-      <c r="C145" t="s">
-        <v>694</v>
-      </c>
-      <c r="D145" t="s">
-        <v>703</v>
       </c>
       <c r="E145" t="s">
         <v>158</v>
@@ -18036,13 +18036,13 @@
         <v>486</v>
       </c>
       <c r="B146" t="s">
+        <v>701</v>
+      </c>
+      <c r="C146" t="s">
+        <v>693</v>
+      </c>
+      <c r="D146" t="s">
         <v>702</v>
-      </c>
-      <c r="C146" t="s">
-        <v>694</v>
-      </c>
-      <c r="D146" t="s">
-        <v>703</v>
       </c>
       <c r="E146" t="s">
         <v>158</v>
@@ -18065,13 +18065,13 @@
         <v>486</v>
       </c>
       <c r="B147" t="s">
+        <v>701</v>
+      </c>
+      <c r="C147" t="s">
+        <v>693</v>
+      </c>
+      <c r="D147" t="s">
         <v>702</v>
-      </c>
-      <c r="C147" t="s">
-        <v>694</v>
-      </c>
-      <c r="D147" t="s">
-        <v>703</v>
       </c>
       <c r="E147" t="s">
         <v>158</v>
@@ -18094,13 +18094,13 @@
         <v>486</v>
       </c>
       <c r="B148" t="s">
-        <v>702</v>
+        <v>701</v>
       </c>
       <c r="C148" t="s">
-        <v>694</v>
+        <v>693</v>
       </c>
       <c r="D148" t="s">
-        <v>708</v>
+        <v>707</v>
       </c>
       <c r="E148" t="s">
         <v>158</v>
@@ -18123,13 +18123,13 @@
         <v>486</v>
       </c>
       <c r="B149" t="s">
-        <v>702</v>
+        <v>701</v>
       </c>
       <c r="C149" t="s">
-        <v>694</v>
+        <v>693</v>
       </c>
       <c r="D149" t="s">
-        <v>708</v>
+        <v>707</v>
       </c>
       <c r="E149" t="s">
         <v>158</v>
@@ -18152,13 +18152,13 @@
         <v>486</v>
       </c>
       <c r="B150" t="s">
-        <v>702</v>
+        <v>701</v>
       </c>
       <c r="C150" t="s">
-        <v>694</v>
+        <v>693</v>
       </c>
       <c r="D150" t="s">
-        <v>708</v>
+        <v>707</v>
       </c>
       <c r="E150" t="s">
         <v>158</v>
@@ -18181,13 +18181,13 @@
         <v>486</v>
       </c>
       <c r="B151" t="s">
-        <v>702</v>
+        <v>701</v>
       </c>
       <c r="C151" t="s">
-        <v>694</v>
+        <v>693</v>
       </c>
       <c r="D151" t="s">
-        <v>708</v>
+        <v>707</v>
       </c>
       <c r="E151" t="s">
         <v>158</v>
@@ -18210,13 +18210,13 @@
         <v>486</v>
       </c>
       <c r="B152" t="s">
-        <v>702</v>
+        <v>701</v>
       </c>
       <c r="C152" t="s">
-        <v>694</v>
+        <v>693</v>
       </c>
       <c r="D152" t="s">
-        <v>708</v>
+        <v>707</v>
       </c>
       <c r="E152" t="s">
         <v>158</v>
@@ -18239,13 +18239,13 @@
         <v>486</v>
       </c>
       <c r="B153" t="s">
-        <v>702</v>
+        <v>701</v>
       </c>
       <c r="C153" t="s">
-        <v>694</v>
+        <v>693</v>
       </c>
       <c r="D153" t="s">
-        <v>708</v>
+        <v>707</v>
       </c>
       <c r="E153" t="s">
         <v>158</v>
@@ -18268,13 +18268,13 @@
         <v>486</v>
       </c>
       <c r="B154" t="s">
-        <v>702</v>
+        <v>701</v>
       </c>
       <c r="C154" t="s">
-        <v>694</v>
+        <v>693</v>
       </c>
       <c r="D154" t="s">
-        <v>708</v>
+        <v>707</v>
       </c>
       <c r="E154" t="s">
         <v>158</v>
@@ -18297,13 +18297,13 @@
         <v>486</v>
       </c>
       <c r="B155" t="s">
-        <v>702</v>
+        <v>701</v>
       </c>
       <c r="C155" t="s">
-        <v>694</v>
+        <v>693</v>
       </c>
       <c r="D155" t="s">
-        <v>708</v>
+        <v>707</v>
       </c>
       <c r="E155" t="s">
         <v>158</v>
@@ -18326,13 +18326,13 @@
         <v>486</v>
       </c>
       <c r="B156" t="s">
-        <v>702</v>
+        <v>701</v>
       </c>
       <c r="C156" t="s">
-        <v>694</v>
+        <v>693</v>
       </c>
       <c r="D156" t="s">
-        <v>698</v>
+        <v>697</v>
       </c>
       <c r="E156" t="s">
         <v>158</v>
@@ -18355,13 +18355,13 @@
         <v>486</v>
       </c>
       <c r="B157" t="s">
-        <v>702</v>
+        <v>701</v>
       </c>
       <c r="C157" t="s">
-        <v>694</v>
+        <v>693</v>
       </c>
       <c r="D157" t="s">
-        <v>698</v>
+        <v>697</v>
       </c>
       <c r="E157" t="s">
         <v>158</v>
@@ -18384,13 +18384,13 @@
         <v>486</v>
       </c>
       <c r="B158" t="s">
-        <v>702</v>
+        <v>701</v>
       </c>
       <c r="C158" t="s">
-        <v>694</v>
+        <v>693</v>
       </c>
       <c r="D158" t="s">
-        <v>698</v>
+        <v>697</v>
       </c>
       <c r="E158" t="s">
         <v>158</v>
@@ -18413,13 +18413,13 @@
         <v>486</v>
       </c>
       <c r="B159" t="s">
-        <v>702</v>
+        <v>701</v>
       </c>
       <c r="C159" t="s">
-        <v>694</v>
+        <v>693</v>
       </c>
       <c r="D159" t="s">
-        <v>698</v>
+        <v>697</v>
       </c>
       <c r="E159" t="s">
         <v>158</v>
@@ -18442,13 +18442,13 @@
         <v>486</v>
       </c>
       <c r="B160" t="s">
-        <v>702</v>
+        <v>701</v>
       </c>
       <c r="C160" t="s">
-        <v>694</v>
+        <v>693</v>
       </c>
       <c r="D160" t="s">
-        <v>698</v>
+        <v>697</v>
       </c>
       <c r="E160" t="s">
         <v>158</v>
@@ -18471,13 +18471,13 @@
         <v>486</v>
       </c>
       <c r="B161" t="s">
-        <v>702</v>
+        <v>701</v>
       </c>
       <c r="C161" t="s">
-        <v>694</v>
+        <v>693</v>
       </c>
       <c r="D161" t="s">
-        <v>698</v>
+        <v>697</v>
       </c>
       <c r="E161" t="s">
         <v>158</v>
@@ -18500,13 +18500,13 @@
         <v>486</v>
       </c>
       <c r="B162" t="s">
-        <v>702</v>
+        <v>701</v>
       </c>
       <c r="C162" t="s">
-        <v>694</v>
+        <v>693</v>
       </c>
       <c r="D162" t="s">
-        <v>698</v>
+        <v>697</v>
       </c>
       <c r="E162" t="s">
         <v>158</v>
@@ -18529,13 +18529,13 @@
         <v>486</v>
       </c>
       <c r="B163" t="s">
-        <v>702</v>
+        <v>701</v>
       </c>
       <c r="C163" t="s">
-        <v>694</v>
+        <v>693</v>
       </c>
       <c r="D163" t="s">
-        <v>698</v>
+        <v>697</v>
       </c>
       <c r="E163" t="s">
         <v>158</v>
@@ -18558,13 +18558,13 @@
         <v>486</v>
       </c>
       <c r="B164" t="s">
-        <v>702</v>
+        <v>701</v>
       </c>
       <c r="C164" t="s">
-        <v>694</v>
+        <v>693</v>
       </c>
       <c r="D164" t="s">
-        <v>704</v>
+        <v>703</v>
       </c>
       <c r="E164" t="s">
         <v>158</v>
@@ -18587,13 +18587,13 @@
         <v>486</v>
       </c>
       <c r="B165" t="s">
-        <v>702</v>
+        <v>701</v>
       </c>
       <c r="C165" t="s">
-        <v>694</v>
+        <v>693</v>
       </c>
       <c r="D165" t="s">
-        <v>704</v>
+        <v>703</v>
       </c>
       <c r="E165" t="s">
         <v>158</v>
@@ -18616,13 +18616,13 @@
         <v>486</v>
       </c>
       <c r="B166" t="s">
-        <v>702</v>
+        <v>701</v>
       </c>
       <c r="C166" t="s">
-        <v>694</v>
+        <v>693</v>
       </c>
       <c r="D166" t="s">
-        <v>704</v>
+        <v>703</v>
       </c>
       <c r="E166" t="s">
         <v>158</v>
@@ -18645,13 +18645,13 @@
         <v>486</v>
       </c>
       <c r="B167" t="s">
-        <v>702</v>
+        <v>701</v>
       </c>
       <c r="C167" t="s">
-        <v>694</v>
+        <v>693</v>
       </c>
       <c r="D167" t="s">
-        <v>704</v>
+        <v>703</v>
       </c>
       <c r="E167" t="s">
         <v>158</v>
@@ -18674,13 +18674,13 @@
         <v>486</v>
       </c>
       <c r="B168" t="s">
-        <v>702</v>
+        <v>701</v>
       </c>
       <c r="C168" t="s">
-        <v>694</v>
+        <v>693</v>
       </c>
       <c r="D168" t="s">
-        <v>704</v>
+        <v>703</v>
       </c>
       <c r="E168" t="s">
         <v>158</v>
@@ -18703,13 +18703,13 @@
         <v>486</v>
       </c>
       <c r="B169" t="s">
-        <v>702</v>
+        <v>701</v>
       </c>
       <c r="C169" t="s">
-        <v>694</v>
+        <v>693</v>
       </c>
       <c r="D169" t="s">
-        <v>704</v>
+        <v>703</v>
       </c>
       <c r="E169" t="s">
         <v>158</v>
@@ -18732,13 +18732,13 @@
         <v>486</v>
       </c>
       <c r="B170" t="s">
-        <v>702</v>
+        <v>701</v>
       </c>
       <c r="C170" t="s">
-        <v>694</v>
+        <v>693</v>
       </c>
       <c r="D170" t="s">
-        <v>704</v>
+        <v>703</v>
       </c>
       <c r="E170" t="s">
         <v>158</v>
@@ -18761,13 +18761,13 @@
         <v>486</v>
       </c>
       <c r="B171" t="s">
-        <v>702</v>
+        <v>701</v>
       </c>
       <c r="C171" t="s">
-        <v>694</v>
+        <v>693</v>
       </c>
       <c r="D171" t="s">
-        <v>704</v>
+        <v>703</v>
       </c>
       <c r="E171" t="s">
         <v>158</v>
@@ -18790,13 +18790,13 @@
         <v>486</v>
       </c>
       <c r="B172" t="s">
-        <v>702</v>
+        <v>701</v>
       </c>
       <c r="C172" t="s">
-        <v>694</v>
+        <v>693</v>
       </c>
       <c r="D172" t="s">
-        <v>704</v>
+        <v>703</v>
       </c>
       <c r="E172" t="s">
         <v>158</v>
@@ -18819,13 +18819,13 @@
         <v>486</v>
       </c>
       <c r="B173" t="s">
-        <v>702</v>
+        <v>701</v>
       </c>
       <c r="C173" t="s">
-        <v>694</v>
+        <v>693</v>
       </c>
       <c r="D173" t="s">
-        <v>704</v>
+        <v>703</v>
       </c>
       <c r="E173" t="s">
         <v>158</v>
@@ -18848,13 +18848,13 @@
         <v>486</v>
       </c>
       <c r="B174" t="s">
-        <v>702</v>
+        <v>701</v>
       </c>
       <c r="C174" t="s">
-        <v>694</v>
+        <v>693</v>
       </c>
       <c r="D174" t="s">
-        <v>704</v>
+        <v>703</v>
       </c>
       <c r="E174" t="s">
         <v>158</v>
@@ -18877,13 +18877,13 @@
         <v>486</v>
       </c>
       <c r="B175" t="s">
-        <v>702</v>
+        <v>701</v>
       </c>
       <c r="C175" t="s">
-        <v>694</v>
+        <v>693</v>
       </c>
       <c r="D175" t="s">
-        <v>704</v>
+        <v>703</v>
       </c>
       <c r="E175" t="s">
         <v>158</v>
@@ -18906,13 +18906,13 @@
         <v>486</v>
       </c>
       <c r="B176" t="s">
-        <v>702</v>
+        <v>701</v>
       </c>
       <c r="C176" t="s">
-        <v>694</v>
+        <v>693</v>
       </c>
       <c r="D176" t="s">
-        <v>704</v>
+        <v>703</v>
       </c>
       <c r="E176" t="s">
         <v>158</v>
@@ -18935,13 +18935,13 @@
         <v>486</v>
       </c>
       <c r="B177" t="s">
-        <v>702</v>
+        <v>701</v>
       </c>
       <c r="C177" t="s">
-        <v>694</v>
+        <v>693</v>
       </c>
       <c r="D177" t="s">
-        <v>704</v>
+        <v>703</v>
       </c>
       <c r="E177" t="s">
         <v>158</v>
@@ -18964,13 +18964,13 @@
         <v>486</v>
       </c>
       <c r="B178" t="s">
-        <v>702</v>
+        <v>701</v>
       </c>
       <c r="C178" t="s">
-        <v>694</v>
+        <v>693</v>
       </c>
       <c r="D178" t="s">
-        <v>704</v>
+        <v>703</v>
       </c>
       <c r="E178" t="s">
         <v>158</v>
@@ -18993,13 +18993,13 @@
         <v>486</v>
       </c>
       <c r="B179" t="s">
-        <v>702</v>
+        <v>701</v>
       </c>
       <c r="C179" t="s">
-        <v>694</v>
+        <v>693</v>
       </c>
       <c r="D179" t="s">
-        <v>704</v>
+        <v>703</v>
       </c>
       <c r="E179" t="s">
         <v>158</v>
@@ -19022,10 +19022,10 @@
         <v>486</v>
       </c>
       <c r="B180" t="s">
-        <v>702</v>
+        <v>701</v>
       </c>
       <c r="C180" t="s">
-        <v>694</v>
+        <v>693</v>
       </c>
       <c r="D180" t="s">
         <v>496</v>
@@ -19051,10 +19051,10 @@
         <v>486</v>
       </c>
       <c r="B181" t="s">
-        <v>702</v>
+        <v>701</v>
       </c>
       <c r="C181" t="s">
-        <v>694</v>
+        <v>693</v>
       </c>
       <c r="D181" t="s">
         <v>496</v>
@@ -19080,10 +19080,10 @@
         <v>486</v>
       </c>
       <c r="B182" t="s">
-        <v>702</v>
+        <v>701</v>
       </c>
       <c r="C182" t="s">
-        <v>694</v>
+        <v>693</v>
       </c>
       <c r="D182" t="s">
         <v>517</v>
@@ -19109,13 +19109,13 @@
         <v>486</v>
       </c>
       <c r="B183" t="s">
-        <v>702</v>
+        <v>701</v>
       </c>
       <c r="C183" t="s">
-        <v>694</v>
+        <v>693</v>
       </c>
       <c r="D183" t="s">
-        <v>724</v>
+        <v>723</v>
       </c>
       <c r="E183" t="s">
         <v>158</v>
@@ -19138,13 +19138,13 @@
         <v>486</v>
       </c>
       <c r="B184" t="s">
-        <v>702</v>
+        <v>701</v>
       </c>
       <c r="C184" t="s">
-        <v>694</v>
+        <v>693</v>
       </c>
       <c r="D184" t="s">
-        <v>724</v>
+        <v>723</v>
       </c>
       <c r="E184" t="s">
         <v>158</v>
@@ -19167,13 +19167,13 @@
         <v>486</v>
       </c>
       <c r="B185" t="s">
-        <v>702</v>
+        <v>701</v>
       </c>
       <c r="C185" t="s">
-        <v>694</v>
+        <v>693</v>
       </c>
       <c r="D185" t="s">
-        <v>724</v>
+        <v>723</v>
       </c>
       <c r="E185" t="s">
         <v>158</v>
@@ -19196,13 +19196,13 @@
         <v>486</v>
       </c>
       <c r="B186" t="s">
-        <v>702</v>
+        <v>701</v>
       </c>
       <c r="C186" t="s">
-        <v>694</v>
+        <v>693</v>
       </c>
       <c r="D186" t="s">
-        <v>724</v>
+        <v>723</v>
       </c>
       <c r="E186" t="s">
         <v>158</v>
@@ -19225,10 +19225,10 @@
         <v>486</v>
       </c>
       <c r="B187" t="s">
-        <v>702</v>
+        <v>701</v>
       </c>
       <c r="C187" t="s">
-        <v>694</v>
+        <v>693</v>
       </c>
       <c r="D187" t="s">
         <v>516</v>
@@ -19254,10 +19254,10 @@
         <v>486</v>
       </c>
       <c r="B188" t="s">
-        <v>702</v>
+        <v>701</v>
       </c>
       <c r="C188" t="s">
-        <v>694</v>
+        <v>693</v>
       </c>
       <c r="D188" t="s">
         <v>496</v>
@@ -19283,10 +19283,10 @@
         <v>486</v>
       </c>
       <c r="B189" t="s">
-        <v>702</v>
+        <v>701</v>
       </c>
       <c r="C189" t="s">
-        <v>694</v>
+        <v>693</v>
       </c>
       <c r="D189" t="s">
         <v>496</v>
@@ -19312,10 +19312,10 @@
         <v>486</v>
       </c>
       <c r="B190" t="s">
-        <v>702</v>
+        <v>701</v>
       </c>
       <c r="C190" t="s">
-        <v>694</v>
+        <v>693</v>
       </c>
       <c r="D190" t="s">
         <v>517</v>
@@ -19341,13 +19341,13 @@
         <v>486</v>
       </c>
       <c r="B191" t="s">
-        <v>702</v>
+        <v>701</v>
       </c>
       <c r="C191" t="s">
-        <v>694</v>
+        <v>693</v>
       </c>
       <c r="D191" t="s">
-        <v>724</v>
+        <v>723</v>
       </c>
       <c r="E191" t="s">
         <v>158</v>
@@ -19370,13 +19370,13 @@
         <v>486</v>
       </c>
       <c r="B192" t="s">
-        <v>702</v>
+        <v>701</v>
       </c>
       <c r="C192" t="s">
-        <v>694</v>
+        <v>693</v>
       </c>
       <c r="D192" t="s">
-        <v>724</v>
+        <v>723</v>
       </c>
       <c r="E192" t="s">
         <v>158</v>
@@ -19399,13 +19399,13 @@
         <v>486</v>
       </c>
       <c r="B193" t="s">
-        <v>702</v>
+        <v>701</v>
       </c>
       <c r="C193" t="s">
-        <v>694</v>
+        <v>693</v>
       </c>
       <c r="D193" t="s">
-        <v>724</v>
+        <v>723</v>
       </c>
       <c r="E193" t="s">
         <v>158</v>
@@ -19428,13 +19428,13 @@
         <v>486</v>
       </c>
       <c r="B194" t="s">
-        <v>702</v>
+        <v>701</v>
       </c>
       <c r="C194" t="s">
-        <v>694</v>
+        <v>693</v>
       </c>
       <c r="D194" t="s">
-        <v>724</v>
+        <v>723</v>
       </c>
       <c r="E194" t="s">
         <v>158</v>
@@ -19457,10 +19457,10 @@
         <v>486</v>
       </c>
       <c r="B195" t="s">
-        <v>702</v>
+        <v>701</v>
       </c>
       <c r="C195" t="s">
-        <v>694</v>
+        <v>693</v>
       </c>
       <c r="D195" t="s">
         <v>516</v>
@@ -19486,10 +19486,10 @@
         <v>486</v>
       </c>
       <c r="B196" t="s">
-        <v>702</v>
+        <v>701</v>
       </c>
       <c r="C196" t="s">
-        <v>694</v>
+        <v>693</v>
       </c>
       <c r="D196" t="s">
         <v>496</v>
@@ -19515,10 +19515,10 @@
         <v>486</v>
       </c>
       <c r="B197" t="s">
-        <v>702</v>
+        <v>701</v>
       </c>
       <c r="C197" t="s">
-        <v>694</v>
+        <v>693</v>
       </c>
       <c r="D197" t="s">
         <v>496</v>
@@ -19544,10 +19544,10 @@
         <v>486</v>
       </c>
       <c r="B198" t="s">
-        <v>702</v>
+        <v>701</v>
       </c>
       <c r="C198" t="s">
-        <v>694</v>
+        <v>693</v>
       </c>
       <c r="D198" t="s">
         <v>517</v>
@@ -19573,13 +19573,13 @@
         <v>486</v>
       </c>
       <c r="B199" t="s">
-        <v>702</v>
+        <v>701</v>
       </c>
       <c r="C199" t="s">
-        <v>694</v>
+        <v>693</v>
       </c>
       <c r="D199" t="s">
-        <v>724</v>
+        <v>723</v>
       </c>
       <c r="E199" t="s">
         <v>158</v>
@@ -19602,13 +19602,13 @@
         <v>486</v>
       </c>
       <c r="B200" t="s">
-        <v>702</v>
+        <v>701</v>
       </c>
       <c r="C200" t="s">
-        <v>694</v>
+        <v>693</v>
       </c>
       <c r="D200" t="s">
-        <v>724</v>
+        <v>723</v>
       </c>
       <c r="E200" t="s">
         <v>158</v>
@@ -19631,13 +19631,13 @@
         <v>486</v>
       </c>
       <c r="B201" t="s">
-        <v>702</v>
+        <v>701</v>
       </c>
       <c r="C201" t="s">
-        <v>694</v>
+        <v>693</v>
       </c>
       <c r="D201" t="s">
-        <v>724</v>
+        <v>723</v>
       </c>
       <c r="E201" t="s">
         <v>158</v>
@@ -19660,13 +19660,13 @@
         <v>486</v>
       </c>
       <c r="B202" t="s">
-        <v>702</v>
+        <v>701</v>
       </c>
       <c r="C202" t="s">
-        <v>694</v>
+        <v>693</v>
       </c>
       <c r="D202" t="s">
-        <v>724</v>
+        <v>723</v>
       </c>
       <c r="E202" t="s">
         <v>158</v>
@@ -19689,10 +19689,10 @@
         <v>486</v>
       </c>
       <c r="B203" t="s">
-        <v>702</v>
+        <v>701</v>
       </c>
       <c r="C203" t="s">
-        <v>694</v>
+        <v>693</v>
       </c>
       <c r="D203" t="s">
         <v>516</v>
@@ -19718,10 +19718,10 @@
         <v>486</v>
       </c>
       <c r="B204" t="s">
-        <v>702</v>
+        <v>701</v>
       </c>
       <c r="C204" t="s">
-        <v>694</v>
+        <v>693</v>
       </c>
       <c r="D204" t="s">
         <v>496</v>
@@ -19747,10 +19747,10 @@
         <v>486</v>
       </c>
       <c r="B205" t="s">
-        <v>702</v>
+        <v>701</v>
       </c>
       <c r="C205" t="s">
-        <v>694</v>
+        <v>693</v>
       </c>
       <c r="D205" t="s">
         <v>496</v>
@@ -19776,10 +19776,10 @@
         <v>486</v>
       </c>
       <c r="B206" t="s">
-        <v>702</v>
+        <v>701</v>
       </c>
       <c r="C206" t="s">
-        <v>694</v>
+        <v>693</v>
       </c>
       <c r="D206" t="s">
         <v>517</v>
@@ -19805,13 +19805,13 @@
         <v>486</v>
       </c>
       <c r="B207" t="s">
-        <v>702</v>
+        <v>701</v>
       </c>
       <c r="C207" t="s">
-        <v>694</v>
+        <v>693</v>
       </c>
       <c r="D207" t="s">
-        <v>724</v>
+        <v>723</v>
       </c>
       <c r="E207" t="s">
         <v>158</v>
@@ -19834,13 +19834,13 @@
         <v>486</v>
       </c>
       <c r="B208" t="s">
-        <v>702</v>
+        <v>701</v>
       </c>
       <c r="C208" t="s">
-        <v>694</v>
+        <v>693</v>
       </c>
       <c r="D208" t="s">
-        <v>724</v>
+        <v>723</v>
       </c>
       <c r="E208" t="s">
         <v>158</v>
@@ -19863,13 +19863,13 @@
         <v>486</v>
       </c>
       <c r="B209" t="s">
-        <v>702</v>
+        <v>701</v>
       </c>
       <c r="C209" t="s">
-        <v>694</v>
+        <v>693</v>
       </c>
       <c r="D209" t="s">
-        <v>724</v>
+        <v>723</v>
       </c>
       <c r="E209" t="s">
         <v>158</v>
@@ -19892,13 +19892,13 @@
         <v>486</v>
       </c>
       <c r="B210" t="s">
-        <v>702</v>
+        <v>701</v>
       </c>
       <c r="C210" t="s">
-        <v>694</v>
+        <v>693</v>
       </c>
       <c r="D210" t="s">
-        <v>724</v>
+        <v>723</v>
       </c>
       <c r="E210" t="s">
         <v>158</v>
@@ -19921,10 +19921,10 @@
         <v>486</v>
       </c>
       <c r="B211" t="s">
-        <v>702</v>
+        <v>701</v>
       </c>
       <c r="C211" t="s">
-        <v>694</v>
+        <v>693</v>
       </c>
       <c r="D211" t="s">
         <v>516</v>
@@ -19950,10 +19950,10 @@
         <v>486</v>
       </c>
       <c r="B212" t="s">
-        <v>702</v>
+        <v>701</v>
       </c>
       <c r="C212" t="s">
-        <v>694</v>
+        <v>693</v>
       </c>
       <c r="D212" t="s">
         <v>496</v>
@@ -19979,10 +19979,10 @@
         <v>486</v>
       </c>
       <c r="B213" t="s">
-        <v>702</v>
+        <v>701</v>
       </c>
       <c r="C213" t="s">
-        <v>694</v>
+        <v>693</v>
       </c>
       <c r="D213" t="s">
         <v>496</v>
@@ -20008,10 +20008,10 @@
         <v>486</v>
       </c>
       <c r="B214" t="s">
-        <v>702</v>
+        <v>701</v>
       </c>
       <c r="C214" t="s">
-        <v>694</v>
+        <v>693</v>
       </c>
       <c r="D214" t="s">
         <v>517</v>
@@ -20037,10 +20037,10 @@
         <v>486</v>
       </c>
       <c r="B215" t="s">
-        <v>702</v>
+        <v>701</v>
       </c>
       <c r="C215" t="s">
-        <v>694</v>
+        <v>693</v>
       </c>
       <c r="D215" t="s">
         <v>516</v>
@@ -20066,10 +20066,10 @@
         <v>486</v>
       </c>
       <c r="B216" t="s">
-        <v>702</v>
+        <v>701</v>
       </c>
       <c r="C216" t="s">
-        <v>694</v>
+        <v>693</v>
       </c>
       <c r="D216" t="s">
         <v>496</v>
@@ -20095,10 +20095,10 @@
         <v>486</v>
       </c>
       <c r="B217" t="s">
-        <v>702</v>
+        <v>701</v>
       </c>
       <c r="C217" t="s">
-        <v>694</v>
+        <v>693</v>
       </c>
       <c r="D217" t="s">
         <v>496</v>
@@ -20124,10 +20124,10 @@
         <v>486</v>
       </c>
       <c r="B218" t="s">
-        <v>702</v>
+        <v>701</v>
       </c>
       <c r="C218" t="s">
-        <v>694</v>
+        <v>693</v>
       </c>
       <c r="D218" t="s">
         <v>517</v>
@@ -20153,13 +20153,13 @@
         <v>486</v>
       </c>
       <c r="B219" t="s">
-        <v>702</v>
+        <v>701</v>
       </c>
       <c r="C219" t="s">
-        <v>694</v>
+        <v>693</v>
       </c>
       <c r="D219" t="s">
-        <v>724</v>
+        <v>723</v>
       </c>
       <c r="E219" t="s">
         <v>158</v>
@@ -20182,13 +20182,13 @@
         <v>486</v>
       </c>
       <c r="B220" t="s">
-        <v>702</v>
+        <v>701</v>
       </c>
       <c r="C220" t="s">
-        <v>694</v>
+        <v>693</v>
       </c>
       <c r="D220" t="s">
-        <v>724</v>
+        <v>723</v>
       </c>
       <c r="E220" t="s">
         <v>158</v>
@@ -20211,13 +20211,13 @@
         <v>486</v>
       </c>
       <c r="B221" t="s">
-        <v>702</v>
+        <v>701</v>
       </c>
       <c r="C221" t="s">
-        <v>694</v>
+        <v>693</v>
       </c>
       <c r="D221" t="s">
-        <v>724</v>
+        <v>723</v>
       </c>
       <c r="E221" t="s">
         <v>158</v>
@@ -20240,13 +20240,13 @@
         <v>486</v>
       </c>
       <c r="B222" t="s">
-        <v>702</v>
+        <v>701</v>
       </c>
       <c r="C222" t="s">
-        <v>694</v>
+        <v>693</v>
       </c>
       <c r="D222" t="s">
-        <v>724</v>
+        <v>723</v>
       </c>
       <c r="E222" t="s">
         <v>158</v>
@@ -20269,10 +20269,10 @@
         <v>486</v>
       </c>
       <c r="B223" t="s">
-        <v>702</v>
+        <v>701</v>
       </c>
       <c r="C223" t="s">
-        <v>694</v>
+        <v>693</v>
       </c>
       <c r="D223" t="s">
         <v>516</v>
@@ -20298,10 +20298,10 @@
         <v>486</v>
       </c>
       <c r="B224" t="s">
-        <v>702</v>
+        <v>701</v>
       </c>
       <c r="C224" t="s">
-        <v>694</v>
+        <v>693</v>
       </c>
       <c r="D224" t="s">
         <v>496</v>
@@ -20327,10 +20327,10 @@
         <v>486</v>
       </c>
       <c r="B225" t="s">
-        <v>702</v>
+        <v>701</v>
       </c>
       <c r="C225" t="s">
-        <v>694</v>
+        <v>693</v>
       </c>
       <c r="D225" t="s">
         <v>496</v>
@@ -20356,10 +20356,10 @@
         <v>486</v>
       </c>
       <c r="B226" t="s">
-        <v>702</v>
+        <v>701</v>
       </c>
       <c r="C226" t="s">
-        <v>694</v>
+        <v>693</v>
       </c>
       <c r="D226" t="s">
         <v>517</v>
@@ -20385,13 +20385,13 @@
         <v>486</v>
       </c>
       <c r="B227" t="s">
-        <v>702</v>
+        <v>701</v>
       </c>
       <c r="C227" t="s">
-        <v>694</v>
+        <v>693</v>
       </c>
       <c r="D227" t="s">
-        <v>724</v>
+        <v>723</v>
       </c>
       <c r="E227" t="s">
         <v>158</v>
@@ -20414,13 +20414,13 @@
         <v>486</v>
       </c>
       <c r="B228" t="s">
-        <v>702</v>
+        <v>701</v>
       </c>
       <c r="C228" t="s">
-        <v>694</v>
+        <v>693</v>
       </c>
       <c r="D228" t="s">
-        <v>724</v>
+        <v>723</v>
       </c>
       <c r="E228" t="s">
         <v>158</v>
@@ -20443,13 +20443,13 @@
         <v>486</v>
       </c>
       <c r="B229" t="s">
-        <v>702</v>
+        <v>701</v>
       </c>
       <c r="C229" t="s">
-        <v>694</v>
+        <v>693</v>
       </c>
       <c r="D229" t="s">
-        <v>724</v>
+        <v>723</v>
       </c>
       <c r="E229" t="s">
         <v>158</v>
@@ -20472,13 +20472,13 @@
         <v>486</v>
       </c>
       <c r="B230" t="s">
-        <v>702</v>
+        <v>701</v>
       </c>
       <c r="C230" t="s">
-        <v>694</v>
+        <v>693</v>
       </c>
       <c r="D230" t="s">
-        <v>724</v>
+        <v>723</v>
       </c>
       <c r="E230" t="s">
         <v>158</v>
@@ -20501,10 +20501,10 @@
         <v>486</v>
       </c>
       <c r="B231" t="s">
-        <v>702</v>
+        <v>701</v>
       </c>
       <c r="C231" t="s">
-        <v>694</v>
+        <v>693</v>
       </c>
       <c r="D231" t="s">
         <v>516</v>
@@ -20530,10 +20530,10 @@
         <v>486</v>
       </c>
       <c r="B232" t="s">
-        <v>702</v>
+        <v>701</v>
       </c>
       <c r="C232" t="s">
-        <v>694</v>
+        <v>693</v>
       </c>
       <c r="D232" t="s">
         <v>496</v>
@@ -20559,10 +20559,10 @@
         <v>486</v>
       </c>
       <c r="B233" t="s">
-        <v>702</v>
+        <v>701</v>
       </c>
       <c r="C233" t="s">
-        <v>694</v>
+        <v>693</v>
       </c>
       <c r="D233" t="s">
         <v>496</v>
@@ -20588,10 +20588,10 @@
         <v>486</v>
       </c>
       <c r="B234" t="s">
-        <v>702</v>
+        <v>701</v>
       </c>
       <c r="C234" t="s">
-        <v>694</v>
+        <v>693</v>
       </c>
       <c r="D234" t="s">
         <v>517</v>
@@ -20617,13 +20617,13 @@
         <v>486</v>
       </c>
       <c r="B235" t="s">
-        <v>702</v>
+        <v>701</v>
       </c>
       <c r="C235" t="s">
-        <v>694</v>
+        <v>693</v>
       </c>
       <c r="D235" t="s">
-        <v>724</v>
+        <v>723</v>
       </c>
       <c r="E235" t="s">
         <v>158</v>
@@ -20646,13 +20646,13 @@
         <v>486</v>
       </c>
       <c r="B236" t="s">
-        <v>702</v>
+        <v>701</v>
       </c>
       <c r="C236" t="s">
-        <v>694</v>
+        <v>693</v>
       </c>
       <c r="D236" t="s">
-        <v>724</v>
+        <v>723</v>
       </c>
       <c r="E236" t="s">
         <v>158</v>
@@ -20675,13 +20675,13 @@
         <v>486</v>
       </c>
       <c r="B237" t="s">
-        <v>702</v>
+        <v>701</v>
       </c>
       <c r="C237" t="s">
-        <v>694</v>
+        <v>693</v>
       </c>
       <c r="D237" t="s">
-        <v>724</v>
+        <v>723</v>
       </c>
       <c r="E237" t="s">
         <v>158</v>
@@ -20704,13 +20704,13 @@
         <v>486</v>
       </c>
       <c r="B238" t="s">
-        <v>702</v>
+        <v>701</v>
       </c>
       <c r="C238" t="s">
-        <v>694</v>
+        <v>693</v>
       </c>
       <c r="D238" t="s">
-        <v>724</v>
+        <v>723</v>
       </c>
       <c r="E238" t="s">
         <v>158</v>
@@ -20733,10 +20733,10 @@
         <v>486</v>
       </c>
       <c r="B239" t="s">
-        <v>702</v>
+        <v>701</v>
       </c>
       <c r="C239" t="s">
-        <v>694</v>
+        <v>693</v>
       </c>
       <c r="D239" t="s">
         <v>516</v>
@@ -20762,10 +20762,10 @@
         <v>486</v>
       </c>
       <c r="B240" t="s">
-        <v>702</v>
+        <v>701</v>
       </c>
       <c r="C240" t="s">
-        <v>694</v>
+        <v>693</v>
       </c>
       <c r="D240" t="s">
         <v>496</v>
@@ -20791,10 +20791,10 @@
         <v>486</v>
       </c>
       <c r="B241" t="s">
-        <v>702</v>
+        <v>701</v>
       </c>
       <c r="C241" t="s">
-        <v>694</v>
+        <v>693</v>
       </c>
       <c r="D241" t="s">
         <v>496</v>
@@ -20820,10 +20820,10 @@
         <v>486</v>
       </c>
       <c r="B242" t="s">
-        <v>702</v>
+        <v>701</v>
       </c>
       <c r="C242" t="s">
-        <v>694</v>
+        <v>693</v>
       </c>
       <c r="D242" t="s">
         <v>517</v>
@@ -20849,13 +20849,13 @@
         <v>486</v>
       </c>
       <c r="B243" t="s">
-        <v>702</v>
+        <v>701</v>
       </c>
       <c r="C243" t="s">
-        <v>694</v>
+        <v>693</v>
       </c>
       <c r="D243" t="s">
-        <v>724</v>
+        <v>723</v>
       </c>
       <c r="E243" t="s">
         <v>158</v>
@@ -20878,13 +20878,13 @@
         <v>486</v>
       </c>
       <c r="B244" t="s">
-        <v>702</v>
+        <v>701</v>
       </c>
       <c r="C244" t="s">
-        <v>694</v>
+        <v>693</v>
       </c>
       <c r="D244" t="s">
-        <v>724</v>
+        <v>723</v>
       </c>
       <c r="E244" t="s">
         <v>158</v>
@@ -20907,13 +20907,13 @@
         <v>486</v>
       </c>
       <c r="B245" t="s">
-        <v>702</v>
+        <v>701</v>
       </c>
       <c r="C245" t="s">
-        <v>694</v>
+        <v>693</v>
       </c>
       <c r="D245" t="s">
-        <v>724</v>
+        <v>723</v>
       </c>
       <c r="E245" t="s">
         <v>158</v>
@@ -20936,13 +20936,13 @@
         <v>486</v>
       </c>
       <c r="B246" t="s">
-        <v>702</v>
+        <v>701</v>
       </c>
       <c r="C246" t="s">
-        <v>694</v>
+        <v>693</v>
       </c>
       <c r="D246" t="s">
-        <v>724</v>
+        <v>723</v>
       </c>
       <c r="E246" t="s">
         <v>158</v>
@@ -20965,10 +20965,10 @@
         <v>486</v>
       </c>
       <c r="B247" t="s">
-        <v>702</v>
+        <v>701</v>
       </c>
       <c r="C247" t="s">
-        <v>694</v>
+        <v>693</v>
       </c>
       <c r="D247" t="s">
         <v>516</v>
@@ -24552,7 +24552,7 @@
   </sheetPr>
   <dimension ref="A1:W78"/>
   <sheetViews>
-    <sheetView zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
+    <sheetView topLeftCell="A42" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
       <selection activeCell="I71" sqref="I71"/>
     </sheetView>
   </sheetViews>
@@ -27841,7 +27841,7 @@
         <v>486</v>
       </c>
       <c r="B72" t="s">
-        <v>679</v>
+        <v>678</v>
       </c>
       <c r="C72" t="s">
         <v>488</v>
@@ -27856,25 +27856,25 @@
         <v>493</v>
       </c>
       <c r="G72" t="s">
-        <v>711</v>
+        <v>710</v>
       </c>
       <c r="H72" t="s">
+        <v>679</v>
+      </c>
+      <c r="I72" t="s">
         <v>680</v>
       </c>
-      <c r="I72" t="s">
+      <c r="J72" t="s">
         <v>681</v>
       </c>
-      <c r="J72" t="s">
+      <c r="K72" t="s">
         <v>682</v>
       </c>
-      <c r="K72" t="s">
+      <c r="L72" t="s">
         <v>683</v>
       </c>
-      <c r="L72" t="s">
+      <c r="M72" t="s">
         <v>684</v>
-      </c>
-      <c r="M72" t="s">
-        <v>685</v>
       </c>
     </row>
     <row r="73" spans="1:22" x14ac:dyDescent="0.25">
@@ -27882,7 +27882,7 @@
         <v>486</v>
       </c>
       <c r="B73" t="s">
-        <v>686</v>
+        <v>685</v>
       </c>
       <c r="C73" t="s">
         <v>488</v>
@@ -27897,25 +27897,25 @@
         <v>493</v>
       </c>
       <c r="G73" t="s">
-        <v>711</v>
+        <v>710</v>
       </c>
       <c r="H73" t="s">
+        <v>686</v>
+      </c>
+      <c r="I73" t="s">
         <v>687</v>
       </c>
-      <c r="I73" t="s">
+      <c r="J73" t="s">
         <v>688</v>
       </c>
-      <c r="J73" t="s">
+      <c r="K73" t="s">
         <v>689</v>
       </c>
-      <c r="K73" t="s">
+      <c r="L73" t="s">
         <v>690</v>
       </c>
-      <c r="L73" t="s">
+      <c r="M73" t="s">
         <v>691</v>
-      </c>
-      <c r="M73" t="s">
-        <v>692</v>
       </c>
     </row>
     <row r="74" spans="1:22" x14ac:dyDescent="0.25">
@@ -27964,10 +27964,10 @@
         <v>486</v>
       </c>
       <c r="B75" t="s">
+        <v>692</v>
+      </c>
+      <c r="C75" t="s">
         <v>693</v>
-      </c>
-      <c r="C75" t="s">
-        <v>694</v>
       </c>
       <c r="D75">
         <v>1</v>
@@ -27979,16 +27979,16 @@
         <v>493</v>
       </c>
       <c r="G75" t="s">
+        <v>693</v>
+      </c>
+      <c r="H75" t="s">
         <v>694</v>
       </c>
-      <c r="H75" t="s">
+      <c r="I75" t="s">
         <v>695</v>
       </c>
-      <c r="I75" t="s">
-        <v>696</v>
-      </c>
       <c r="J75" t="s">
-        <v>703</v>
+        <v>702</v>
       </c>
     </row>
     <row r="76" spans="1:22" x14ac:dyDescent="0.25">
@@ -27996,10 +27996,10 @@
         <v>486</v>
       </c>
       <c r="B76" t="s">
-        <v>697</v>
+        <v>696</v>
       </c>
       <c r="C76" t="s">
-        <v>694</v>
+        <v>693</v>
       </c>
       <c r="D76">
         <v>2</v>
@@ -28011,13 +28011,13 @@
         <v>493</v>
       </c>
       <c r="G76" t="s">
-        <v>694</v>
+        <v>693</v>
       </c>
       <c r="H76" t="s">
-        <v>704</v>
+        <v>703</v>
       </c>
       <c r="I76" t="s">
-        <v>698</v>
+        <v>697</v>
       </c>
     </row>
     <row r="77" spans="1:22" x14ac:dyDescent="0.25">
@@ -28025,10 +28025,10 @@
         <v>486</v>
       </c>
       <c r="B77" t="s">
-        <v>723</v>
+        <v>722</v>
       </c>
       <c r="C77" t="s">
-        <v>694</v>
+        <v>693</v>
       </c>
       <c r="D77">
         <v>3</v>
@@ -28040,7 +28040,7 @@
         <v>493</v>
       </c>
       <c r="G77" t="s">
-        <v>694</v>
+        <v>693</v>
       </c>
       <c r="H77" t="s">
         <v>517</v>
@@ -28049,7 +28049,7 @@
         <v>496</v>
       </c>
       <c r="J77" t="s">
-        <v>724</v>
+        <v>723</v>
       </c>
     </row>
     <row r="78" spans="1:22" x14ac:dyDescent="0.25">
@@ -28057,10 +28057,10 @@
         <v>486</v>
       </c>
       <c r="B78" t="s">
-        <v>725</v>
+        <v>724</v>
       </c>
       <c r="C78" t="s">
-        <v>694</v>
+        <v>693</v>
       </c>
       <c r="D78">
         <v>4</v>
@@ -28072,7 +28072,7 @@
         <v>493</v>
       </c>
       <c r="G78" t="s">
-        <v>694</v>
+        <v>693</v>
       </c>
       <c r="H78" t="s">
         <v>517</v>
@@ -28084,7 +28084,7 @@
         <v>516</v>
       </c>
       <c r="K78" t="s">
-        <v>724</v>
+        <v>723</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
temp macro file reading fix
</commit_message>
<xml_diff>
--- a/config/master_config.xlsx
+++ b/config/master_config.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\finbar.maunsell\github\9th_edition_visualisation\config\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{1328866A-3779-4DCB-930E-187E33E0C505}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{5589BE36-2033-48C1-9F6F-3A48D648E487}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="28680" yWindow="-120" windowWidth="29040" windowHeight="15720" tabRatio="844" xr2:uid="{E1808A28-6E92-43AB-8411-89A0CBB0B83A}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" tabRatio="844" activeTab="5" xr2:uid="{E1808A28-6E92-43AB-8411-89A0CBB0B83A}"/>
   </bookViews>
   <sheets>
     <sheet name="9th_EBT_schema" sheetId="7" r:id="rId1"/>
@@ -382,7 +382,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="6209" uniqueCount="819">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="6207" uniqueCount="820">
   <si>
     <t>Variables (fuels and sectors 'lined-up' in subsequent sheets)</t>
   </si>
@@ -2704,6 +2704,9 @@
   </si>
   <si>
     <t>Datacentres</t>
+  </si>
+  <si>
+    <t>16_01_03_traditional_data_centres</t>
   </si>
   <si>
     <t>Ai training</t>
@@ -4871,10 +4874,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{A000B41E-5923-4013-B542-E4247E89557C}">
-  <dimension ref="A1:I104"/>
+  <dimension ref="A1:I102"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A89" workbookViewId="0">
-      <selection activeCell="G103" sqref="G103:G104"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="F42" sqref="F42"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -5435,7 +5438,7 @@
         <v>166</v>
       </c>
       <c r="E23" s="19" t="s">
-        <v>800</v>
+        <v>801</v>
       </c>
       <c r="F23" t="s">
         <v>167</v>
@@ -5478,7 +5481,7 @@
         <v>178</v>
       </c>
       <c r="C25" s="19" t="s">
-        <v>804</v>
+        <v>805</v>
       </c>
       <c r="D25" t="s">
         <v>179</v>
@@ -6158,16 +6161,6 @@
     <row r="102" spans="7:7" x14ac:dyDescent="0.25">
       <c r="G102" t="s">
         <v>270</v>
-      </c>
-    </row>
-    <row r="103" spans="7:7" x14ac:dyDescent="0.25">
-      <c r="G103" t="s">
-        <v>779</v>
-      </c>
-    </row>
-    <row r="104" spans="7:7" x14ac:dyDescent="0.25">
-      <c r="G104" t="s">
-        <v>778</v>
       </c>
     </row>
   </sheetData>
@@ -7710,7 +7703,7 @@
         <v>743</v>
       </c>
       <c r="B190" t="s">
-        <v>797</v>
+        <v>798</v>
       </c>
     </row>
     <row r="191" spans="1:2" x14ac:dyDescent="0.25">
@@ -7739,18 +7732,18 @@
     </row>
     <row r="194" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A194" t="s">
-        <v>774</v>
+        <v>775</v>
       </c>
       <c r="B194" t="s">
-        <v>776</v>
+        <v>777</v>
       </c>
     </row>
     <row r="195" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A195" t="s">
-        <v>775</v>
+        <v>776</v>
       </c>
       <c r="B195" t="s">
-        <v>777</v>
+        <v>778</v>
       </c>
     </row>
   </sheetData>
@@ -7824,7 +7817,7 @@
         <v>698</v>
       </c>
       <c r="B6" s="22" t="s">
-        <v>803</v>
+        <v>804</v>
       </c>
     </row>
     <row r="7" spans="1:2" x14ac:dyDescent="0.25">
@@ -7927,7 +7920,7 @@
         <v>364</v>
       </c>
       <c r="C6" t="s">
-        <v>780</v>
+        <v>781</v>
       </c>
     </row>
     <row r="7" spans="1:3" x14ac:dyDescent="0.25">
@@ -7938,7 +7931,7 @@
         <v>363</v>
       </c>
       <c r="C7" t="s">
-        <v>780</v>
+        <v>781</v>
       </c>
     </row>
     <row r="8" spans="1:3" x14ac:dyDescent="0.25">
@@ -7949,7 +7942,7 @@
         <v>364</v>
       </c>
       <c r="C8" t="s">
-        <v>781</v>
+        <v>782</v>
       </c>
     </row>
     <row r="9" spans="1:3" x14ac:dyDescent="0.25">
@@ -7960,7 +7953,7 @@
         <v>364</v>
       </c>
       <c r="C9" t="s">
-        <v>781</v>
+        <v>782</v>
       </c>
     </row>
     <row r="10" spans="1:3" x14ac:dyDescent="0.25">
@@ -7971,7 +7964,7 @@
         <v>364</v>
       </c>
       <c r="C10" t="s">
-        <v>781</v>
+        <v>782</v>
       </c>
     </row>
     <row r="11" spans="1:3" x14ac:dyDescent="0.25">
@@ -7982,7 +7975,7 @@
         <v>364</v>
       </c>
       <c r="C11" t="s">
-        <v>781</v>
+        <v>782</v>
       </c>
     </row>
   </sheetData>
@@ -9572,7 +9565,7 @@
   <dimension ref="A1:D94"/>
   <sheetViews>
     <sheetView topLeftCell="A67" workbookViewId="0">
-      <selection activeCell="I85" sqref="H85:I87"/>
+      <selection activeCell="B75" sqref="B75"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -10367,7 +10360,7 @@
         <v>216</v>
       </c>
       <c r="D70" t="s">
-        <v>779</v>
+        <v>774</v>
       </c>
     </row>
     <row r="71" spans="1:4" x14ac:dyDescent="0.25">
@@ -10381,12 +10374,12 @@
         <v>216</v>
       </c>
       <c r="D71" t="s">
-        <v>778</v>
+        <v>779</v>
       </c>
     </row>
     <row r="72" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A72" t="s">
-        <v>782</v>
+        <v>783</v>
       </c>
       <c r="B72" t="s">
         <v>135</v>
@@ -10395,12 +10388,12 @@
         <v>216</v>
       </c>
       <c r="D72" t="s">
-        <v>778</v>
+        <v>779</v>
       </c>
     </row>
     <row r="73" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A73" t="s">
-        <v>775</v>
+        <v>776</v>
       </c>
       <c r="B73" t="s">
         <v>135</v>
@@ -10409,7 +10402,7 @@
         <v>216</v>
       </c>
       <c r="D73" t="s">
-        <v>779</v>
+        <v>780</v>
       </c>
     </row>
     <row r="74" spans="1:4" x14ac:dyDescent="0.25">
@@ -10417,7 +10410,7 @@
         <v>564</v>
       </c>
       <c r="B74" s="18" t="s">
-        <v>807</v>
+        <v>808</v>
       </c>
       <c r="C74" s="18"/>
     </row>
@@ -10426,7 +10419,7 @@
         <v>565</v>
       </c>
       <c r="B75" s="18" t="s">
-        <v>808</v>
+        <v>809</v>
       </c>
       <c r="C75" s="18"/>
     </row>
@@ -10435,22 +10428,22 @@
         <v>570</v>
       </c>
       <c r="B76" s="18" t="s">
-        <v>806</v>
+        <v>807</v>
       </c>
       <c r="C76" s="18"/>
     </row>
     <row r="77" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A77" s="18" t="s">
+        <v>802</v>
+      </c>
+      <c r="B77" s="20" t="s">
         <v>801</v>
-      </c>
-      <c r="B77" s="20" t="s">
-        <v>800</v>
       </c>
       <c r="C77" s="18"/>
     </row>
     <row r="78" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A78" t="s">
-        <v>798</v>
+        <v>799</v>
       </c>
       <c r="B78" t="s">
         <v>87</v>
@@ -10461,7 +10454,7 @@
     </row>
     <row r="79" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A79" t="s">
-        <v>799</v>
+        <v>800</v>
       </c>
       <c r="B79" t="s">
         <v>87</v>
@@ -10641,8 +10634,8 @@
   </sheetPr>
   <dimension ref="A1:C345"/>
   <sheetViews>
-    <sheetView topLeftCell="A67" workbookViewId="0">
-      <selection activeCell="B96" sqref="B96"/>
+    <sheetView topLeftCell="A331" workbookViewId="0">
+      <selection activeCell="A343" sqref="A343:A344"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -13771,7 +13764,7 @@
     </row>
     <row r="334" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A334" t="s">
-        <v>791</v>
+        <v>792</v>
       </c>
       <c r="B334" t="s">
         <v>133</v>
@@ -13782,10 +13775,10 @@
     </row>
     <row r="335" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A335" s="18" t="s">
-        <v>801</v>
+        <v>802</v>
       </c>
       <c r="B335" s="18" t="s">
-        <v>804</v>
+        <v>805</v>
       </c>
     </row>
     <row r="336" spans="1:3" x14ac:dyDescent="0.25">
@@ -13793,7 +13786,7 @@
         <v>570</v>
       </c>
       <c r="B336" s="18" t="s">
-        <v>805</v>
+        <v>806</v>
       </c>
     </row>
     <row r="337" spans="1:3" x14ac:dyDescent="0.25">
@@ -13809,7 +13802,7 @@
     </row>
     <row r="338" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A338" t="s">
-        <v>810</v>
+        <v>811</v>
       </c>
       <c r="B338" t="s">
         <v>133</v>
@@ -13842,7 +13835,7 @@
     </row>
     <row r="341" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A341" t="s">
-        <v>811</v>
+        <v>812</v>
       </c>
       <c r="B341" t="s">
         <v>133</v>
@@ -13853,7 +13846,7 @@
     </row>
     <row r="342" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A342" t="s">
-        <v>813</v>
+        <v>814</v>
       </c>
       <c r="B342" t="s">
         <v>69</v>
@@ -13864,26 +13857,26 @@
     </row>
     <row r="343" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A343" t="s">
-        <v>814</v>
+        <v>815</v>
       </c>
       <c r="B343" t="s">
-        <v>815</v>
+        <v>816</v>
       </c>
     </row>
     <row r="344" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A344" t="s">
-        <v>816</v>
+        <v>817</v>
       </c>
       <c r="B344" t="s">
-        <v>817</v>
+        <v>818</v>
       </c>
     </row>
     <row r="345" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A345" t="s">
-        <v>816</v>
+        <v>817</v>
       </c>
       <c r="B345" t="s">
-        <v>818</v>
+        <v>819</v>
       </c>
     </row>
   </sheetData>
@@ -13902,7 +13895,7 @@
   <dimension ref="A1:D28"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="D35" sqref="D35"/>
+      <selection activeCell="C51" sqref="C51"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -21400,8 +21393,8 @@
   </sheetPr>
   <dimension ref="A1:W89"/>
   <sheetViews>
-    <sheetView topLeftCell="A55" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="G85" sqref="G85"/>
+    <sheetView tabSelected="1" topLeftCell="G33" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="L71" sqref="L71:O71"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -21771,10 +21764,10 @@
         <v>368</v>
       </c>
       <c r="J7" t="s">
-        <v>782</v>
+        <v>783</v>
       </c>
       <c r="K7" t="s">
-        <v>775</v>
+        <v>776</v>
       </c>
     </row>
     <row r="8" spans="1:23" x14ac:dyDescent="0.25">
@@ -21806,10 +21799,10 @@
         <v>368</v>
       </c>
       <c r="J8" t="s">
-        <v>782</v>
+        <v>783</v>
       </c>
       <c r="K8" t="s">
-        <v>775</v>
+        <v>776</v>
       </c>
     </row>
     <row r="9" spans="1:23" x14ac:dyDescent="0.25">
@@ -23946,7 +23939,7 @@
         <v>352</v>
       </c>
       <c r="B52" t="s">
-        <v>812</v>
+        <v>813</v>
       </c>
       <c r="C52" t="s">
         <v>588</v>
@@ -23961,7 +23954,7 @@
         <v>411</v>
       </c>
       <c r="G52" t="s">
-        <v>813</v>
+        <v>814</v>
       </c>
       <c r="H52" t="s">
         <v>353</v>
@@ -24542,7 +24535,7 @@
         <v>734</v>
       </c>
       <c r="B65" t="s">
-        <v>783</v>
+        <v>784</v>
       </c>
       <c r="C65" s="16" t="s">
         <v>735</v>
@@ -24557,7 +24550,7 @@
         <v>561</v>
       </c>
       <c r="G65" t="s">
-        <v>801</v>
+        <v>802</v>
       </c>
       <c r="H65" t="s">
         <v>398</v>
@@ -24572,13 +24565,13 @@
         <v>422</v>
       </c>
       <c r="L65" t="s">
-        <v>814</v>
+        <v>815</v>
       </c>
       <c r="M65" t="s">
-        <v>816</v>
+        <v>817</v>
       </c>
       <c r="N65" t="s">
-        <v>801</v>
+        <v>802</v>
       </c>
       <c r="O65" t="s">
         <v>570</v>
@@ -24604,7 +24597,7 @@
         <v>559</v>
       </c>
       <c r="G66" t="s">
-        <v>801</v>
+        <v>802</v>
       </c>
       <c r="H66" t="s">
         <v>565</v>
@@ -24613,7 +24606,7 @@
         <v>564</v>
       </c>
       <c r="J66" t="s">
-        <v>798</v>
+        <v>799</v>
       </c>
       <c r="K66" t="s">
         <v>365</v>
@@ -24637,7 +24630,7 @@
         <v>437</v>
       </c>
       <c r="R66" t="s">
-        <v>801</v>
+        <v>802</v>
       </c>
       <c r="S66" t="s">
         <v>570</v>
@@ -24648,7 +24641,7 @@
         <v>737</v>
       </c>
       <c r="B67" t="s">
-        <v>784</v>
+        <v>785</v>
       </c>
       <c r="C67" s="16" t="s">
         <v>738</v>
@@ -24663,7 +24656,7 @@
         <v>561</v>
       </c>
       <c r="G67" t="s">
-        <v>801</v>
+        <v>802</v>
       </c>
       <c r="H67" t="s">
         <v>398</v>
@@ -24678,13 +24671,13 @@
         <v>422</v>
       </c>
       <c r="L67" t="s">
-        <v>814</v>
+        <v>815</v>
       </c>
       <c r="M67" t="s">
-        <v>816</v>
+        <v>817</v>
       </c>
       <c r="N67" t="s">
-        <v>801</v>
+        <v>802</v>
       </c>
       <c r="O67" t="s">
         <v>570</v>
@@ -24695,7 +24688,7 @@
         <v>737</v>
       </c>
       <c r="B68" t="s">
-        <v>785</v>
+        <v>786</v>
       </c>
       <c r="C68" s="16" t="s">
         <v>738</v>
@@ -24710,7 +24703,7 @@
         <v>559</v>
       </c>
       <c r="G68" t="s">
-        <v>801</v>
+        <v>802</v>
       </c>
       <c r="H68" t="s">
         <v>565</v>
@@ -24719,7 +24712,7 @@
         <v>564</v>
       </c>
       <c r="J68" t="s">
-        <v>798</v>
+        <v>799</v>
       </c>
       <c r="K68" t="s">
         <v>365</v>
@@ -24743,7 +24736,7 @@
         <v>437</v>
       </c>
       <c r="R68" t="s">
-        <v>801</v>
+        <v>802</v>
       </c>
       <c r="S68" t="s">
         <v>570</v>
@@ -24754,7 +24747,7 @@
         <v>739</v>
       </c>
       <c r="B69" t="s">
-        <v>786</v>
+        <v>787</v>
       </c>
       <c r="C69" s="16" t="s">
         <v>738</v>
@@ -24769,7 +24762,7 @@
         <v>561</v>
       </c>
       <c r="G69" t="s">
-        <v>801</v>
+        <v>802</v>
       </c>
       <c r="H69" t="s">
         <v>398</v>
@@ -24784,13 +24777,13 @@
         <v>422</v>
       </c>
       <c r="L69" t="s">
-        <v>814</v>
+        <v>815</v>
       </c>
       <c r="M69" t="s">
-        <v>816</v>
+        <v>817</v>
       </c>
       <c r="N69" t="s">
-        <v>801</v>
+        <v>802</v>
       </c>
       <c r="O69" t="s">
         <v>570</v>
@@ -24801,7 +24794,7 @@
         <v>739</v>
       </c>
       <c r="B70" t="s">
-        <v>787</v>
+        <v>788</v>
       </c>
       <c r="C70" s="16" t="s">
         <v>738</v>
@@ -24816,7 +24809,7 @@
         <v>559</v>
       </c>
       <c r="G70" t="s">
-        <v>801</v>
+        <v>802</v>
       </c>
       <c r="H70" t="s">
         <v>565</v>
@@ -24825,7 +24818,7 @@
         <v>564</v>
       </c>
       <c r="J70" t="s">
-        <v>798</v>
+        <v>799</v>
       </c>
       <c r="K70" t="s">
         <v>365</v>
@@ -24849,7 +24842,7 @@
         <v>437</v>
       </c>
       <c r="R70" t="s">
-        <v>801</v>
+        <v>802</v>
       </c>
       <c r="S70" t="s">
         <v>570</v>
@@ -24860,7 +24853,7 @@
         <v>740</v>
       </c>
       <c r="B71" t="s">
-        <v>788</v>
+        <v>789</v>
       </c>
       <c r="C71" s="16" t="s">
         <v>738</v>
@@ -24875,7 +24868,7 @@
         <v>561</v>
       </c>
       <c r="G71" t="s">
-        <v>801</v>
+        <v>802</v>
       </c>
       <c r="H71" t="s">
         <v>398</v>
@@ -24890,13 +24883,13 @@
         <v>422</v>
       </c>
       <c r="L71" t="s">
-        <v>814</v>
+        <v>815</v>
       </c>
       <c r="M71" t="s">
-        <v>816</v>
+        <v>817</v>
       </c>
       <c r="N71" t="s">
-        <v>801</v>
+        <v>802</v>
       </c>
       <c r="O71" t="s">
         <v>570</v>
@@ -24907,7 +24900,7 @@
         <v>740</v>
       </c>
       <c r="B72" t="s">
-        <v>789</v>
+        <v>790</v>
       </c>
       <c r="C72" s="16" t="s">
         <v>738</v>
@@ -24922,7 +24915,7 @@
         <v>559</v>
       </c>
       <c r="G72" t="s">
-        <v>801</v>
+        <v>802</v>
       </c>
       <c r="H72" t="s">
         <v>565</v>
@@ -24931,7 +24924,7 @@
         <v>564</v>
       </c>
       <c r="J72" t="s">
-        <v>798</v>
+        <v>799</v>
       </c>
       <c r="K72" t="s">
         <v>365</v>
@@ -24952,7 +24945,7 @@
         <v>622</v>
       </c>
       <c r="Q72" t="s">
-        <v>801</v>
+        <v>802</v>
       </c>
       <c r="R72" t="s">
         <v>570</v>
@@ -24963,7 +24956,7 @@
         <v>352</v>
       </c>
       <c r="B73" t="s">
-        <v>795</v>
+        <v>796</v>
       </c>
       <c r="C73" t="s">
         <v>437</v>
@@ -24984,7 +24977,7 @@
         <v>708</v>
       </c>
       <c r="I73" t="s">
-        <v>791</v>
+        <v>792</v>
       </c>
       <c r="J73" t="s">
         <v>437</v>
@@ -24995,7 +24988,7 @@
         <v>352</v>
       </c>
       <c r="B74" t="s">
-        <v>796</v>
+        <v>797</v>
       </c>
       <c r="C74" t="s">
         <v>437</v>
@@ -25039,7 +25032,7 @@
         <v>352</v>
       </c>
       <c r="B75" t="s">
-        <v>793</v>
+        <v>794</v>
       </c>
       <c r="C75" t="s">
         <v>437</v>
@@ -25083,7 +25076,7 @@
         <v>352</v>
       </c>
       <c r="B76" t="s">
-        <v>794</v>
+        <v>795</v>
       </c>
       <c r="C76" t="s">
         <v>749</v>
@@ -25127,7 +25120,7 @@
         <v>352</v>
       </c>
       <c r="B77" t="s">
-        <v>790</v>
+        <v>791</v>
       </c>
       <c r="C77" t="s">
         <v>749</v>
@@ -25162,7 +25155,7 @@
         <v>352</v>
       </c>
       <c r="B78" t="s">
-        <v>802</v>
+        <v>803</v>
       </c>
       <c r="C78" t="s">
         <v>749</v>
@@ -25244,7 +25237,7 @@
         <v>352</v>
       </c>
       <c r="B80" t="s">
-        <v>809</v>
+        <v>810</v>
       </c>
       <c r="C80" t="s">
         <v>749</v>
@@ -25332,7 +25325,7 @@
         <v>352</v>
       </c>
       <c r="B82" t="s">
-        <v>792</v>
+        <v>793</v>
       </c>
       <c r="C82" t="s">
         <v>741</v>
@@ -25359,7 +25352,7 @@
         <v>708</v>
       </c>
       <c r="K82" t="s">
-        <v>791</v>
+        <v>792</v>
       </c>
       <c r="L82" t="s">
         <v>437</v>
@@ -25368,7 +25361,7 @@
         <v>742</v>
       </c>
       <c r="N82" t="s">
-        <v>810</v>
+        <v>811</v>
       </c>
       <c r="O82" t="s">
         <v>725</v>
@@ -25377,7 +25370,7 @@
         <v>453</v>
       </c>
       <c r="Q82" t="s">
-        <v>811</v>
+        <v>812</v>
       </c>
       <c r="R82" t="s">
         <v>363</v>

</xml_diff>

<commit_message>
LNG updates and fixes to kaya
</commit_message>
<xml_diff>
--- a/config/master_config.xlsx
+++ b/config/master_config.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\finbar.maunsell\github\9th_edition_visualisation\config\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{AC76D7ED-7395-41AE-8707-AECECA95528D}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D38E483A-B4F5-4AD4-9A89-1C941FC0000D}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" tabRatio="844" firstSheet="2" activeTab="4" xr2:uid="{E1808A28-6E92-43AB-8411-89A0CBB0B83A}"/>
+    <workbookView xWindow="-75" yWindow="180" windowWidth="57315" windowHeight="15435" tabRatio="844" firstSheet="2" activeTab="5" xr2:uid="{E1808A28-6E92-43AB-8411-89A0CBB0B83A}"/>
   </bookViews>
   <sheets>
     <sheet name="9th_EBT_schema" sheetId="7" r:id="rId1"/>
@@ -382,7 +382,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="6220" uniqueCount="831">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="6219" uniqueCount="831">
   <si>
     <t>Variables (fuels and sectors 'lined-up' in subsequent sheets)</t>
   </si>
@@ -14401,7 +14401,7 @@
   </sheetPr>
   <dimension ref="A1:I249"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="C195" sqref="C195"/>
     </sheetView>
   </sheetViews>
@@ -21474,8 +21474,8 @@
   </sheetPr>
   <dimension ref="A1:W89"/>
   <sheetViews>
-    <sheetView topLeftCell="A44" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="G78" sqref="G78"/>
+    <sheetView tabSelected="1" topLeftCell="A44" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
+      <selection activeCell="J91" sqref="J91"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -23027,12 +23027,9 @@
         <v>355</v>
       </c>
       <c r="K31" t="s">
-        <v>356</v>
+        <v>357</v>
       </c>
       <c r="L31" t="s">
-        <v>357</v>
-      </c>
-      <c r="M31" t="s">
         <v>358</v>
       </c>
     </row>
@@ -23926,6 +23923,9 @@
       <c r="O49" t="s">
         <v>469</v>
       </c>
+      <c r="P49" t="s">
+        <v>356</v>
+      </c>
     </row>
     <row r="50" spans="1:22" x14ac:dyDescent="0.25">
       <c r="A50" t="s">
@@ -23973,6 +23973,9 @@
       <c r="O50" t="s">
         <v>469</v>
       </c>
+      <c r="P50" t="s">
+        <v>356</v>
+      </c>
     </row>
     <row r="51" spans="1:22" x14ac:dyDescent="0.25">
       <c r="A51" t="s">
@@ -24006,12 +24009,9 @@
         <v>355</v>
       </c>
       <c r="K51" t="s">
-        <v>356</v>
+        <v>357</v>
       </c>
       <c r="L51" t="s">
-        <v>357</v>
-      </c>
-      <c r="M51" t="s">
         <v>358</v>
       </c>
     </row>
@@ -24047,12 +24047,9 @@
         <v>355</v>
       </c>
       <c r="K52" t="s">
-        <v>356</v>
+        <v>357</v>
       </c>
       <c r="L52" t="s">
-        <v>357</v>
-      </c>
-      <c r="M52" t="s">
         <v>358</v>
       </c>
     </row>
@@ -25105,12 +25102,9 @@
         <v>355</v>
       </c>
       <c r="L74" t="s">
-        <v>356</v>
+        <v>357</v>
       </c>
       <c r="M74" t="s">
-        <v>357</v>
-      </c>
-      <c r="N74" t="s">
         <v>358</v>
       </c>
     </row>
@@ -25157,6 +25151,9 @@
       <c r="N75" t="s">
         <v>467</v>
       </c>
+      <c r="O75" t="s">
+        <v>356</v>
+      </c>
     </row>
     <row r="76" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A76" t="s">
@@ -25201,6 +25198,9 @@
       <c r="N76" t="s">
         <v>467</v>
       </c>
+      <c r="O76" t="s">
+        <v>356</v>
+      </c>
     </row>
     <row r="77" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A77" t="s">
@@ -25269,12 +25269,9 @@
         <v>355</v>
       </c>
       <c r="K78" t="s">
-        <v>356</v>
+        <v>357</v>
       </c>
       <c r="L78" t="s">
-        <v>357</v>
-      </c>
-      <c r="M78" t="s">
         <v>358</v>
       </c>
     </row>
@@ -25310,12 +25307,9 @@
         <v>355</v>
       </c>
       <c r="K79" t="s">
-        <v>356</v>
+        <v>357</v>
       </c>
       <c r="L79" t="s">
-        <v>357</v>
-      </c>
-      <c r="M79" t="s">
         <v>358</v>
       </c>
     </row>
@@ -25362,6 +25356,9 @@
       <c r="N80" t="s">
         <v>467</v>
       </c>
+      <c r="O80" t="s">
+        <v>356</v>
+      </c>
     </row>
     <row r="81" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A81" t="s">
@@ -25506,6 +25503,9 @@
       <c r="N83" t="s">
         <v>467</v>
       </c>
+      <c r="O83" t="s">
+        <v>356</v>
+      </c>
     </row>
     <row r="84" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A84" t="s">
@@ -25592,9 +25592,6 @@
         <v>355</v>
       </c>
       <c r="K85" t="s">
-        <v>356</v>
-      </c>
-      <c r="L85" t="s">
         <v>357</v>
       </c>
     </row>

</xml_diff>

<commit_message>
update bunkers in master config
</commit_message>
<xml_diff>
--- a/config/master_config.xlsx
+++ b/config/master_config.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="28227"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="28324"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\finbar.maunsell\github\9th_edition_visualisation\config\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\hyuga.kasai\Documents\Github\9th_Visualization\9th_edition_visualisation\config\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{AC76D7ED-7395-41AE-8707-AECECA95528D}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{88E004B2-A43B-49A0-9E81-51A0DC121AC6}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" tabRatio="844" firstSheet="2" activeTab="4" xr2:uid="{E1808A28-6E92-43AB-8411-89A0CBB0B83A}"/>
+    <workbookView xWindow="22050" yWindow="-16395" windowWidth="29040" windowHeight="15720" tabRatio="844" firstSheet="2" activeTab="5" xr2:uid="{E1808A28-6E92-43AB-8411-89A0CBB0B83A}"/>
   </bookViews>
   <sheets>
     <sheet name="9th_EBT_schema" sheetId="7" r:id="rId1"/>
@@ -179,7 +179,7 @@
     <author>Finbar Maunsell</author>
   </authors>
   <commentList>
-    <comment ref="D1" authorId="0" shapeId="0" xr:uid="{B1D5F555-88D3-4D14-A6EE-A54EA1CCEE41}">
+    <comment ref="D1" authorId="0" shapeId="0" xr:uid="{015AC340-F00B-4C80-8FD7-31207E662310}">
       <text>
         <r>
           <rPr>
@@ -203,7 +203,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="H1" authorId="0" shapeId="0" xr:uid="{66B2255A-AC70-44D7-9495-55BB5730927F}">
+    <comment ref="H1" authorId="0" shapeId="0" xr:uid="{BC2267C3-B75B-4EB2-84C7-525C5856F82A}">
       <text>
         <r>
           <rPr>
@@ -382,7 +382,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="6220" uniqueCount="831">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="6219" uniqueCount="831">
   <si>
     <t>Variables (fuels and sectors 'lined-up' in subsequent sheets)</t>
   </si>
@@ -4236,6 +4236,172 @@
     </xdr:sp>
     <xdr:clientData/>
   </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>18</xdr:col>
+      <xdr:colOff>115166</xdr:colOff>
+      <xdr:row>1</xdr:row>
+      <xdr:rowOff>0</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>23</xdr:col>
+      <xdr:colOff>29441</xdr:colOff>
+      <xdr:row>14</xdr:row>
+      <xdr:rowOff>73602</xdr:rowOff>
+    </xdr:to>
+    <xdr:sp macro="" textlink="">
+      <xdr:nvSpPr>
+        <xdr:cNvPr id="4" name="TextBox 3">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{764EE781-9FC0-4C8D-972C-64D83CF1B438}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvSpPr txBox="1"/>
+      </xdr:nvSpPr>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="27766241" y="190500"/>
+          <a:ext cx="2962275" cy="2550102"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+        <a:solidFill>
+          <a:schemeClr val="accent2"/>
+        </a:solidFill>
+        <a:ln w="9525" cmpd="sng">
+          <a:solidFill>
+            <a:schemeClr val="lt1">
+              <a:shade val="50000"/>
+            </a:schemeClr>
+          </a:solidFill>
+        </a:ln>
+      </xdr:spPr>
+      <xdr:style>
+        <a:lnRef idx="0">
+          <a:scrgbClr r="0" g="0" b="0"/>
+        </a:lnRef>
+        <a:fillRef idx="0">
+          <a:scrgbClr r="0" g="0" b="0"/>
+        </a:fillRef>
+        <a:effectRef idx="0">
+          <a:scrgbClr r="0" g="0" b="0"/>
+        </a:effectRef>
+        <a:fontRef idx="minor">
+          <a:schemeClr val="dk1"/>
+        </a:fontRef>
+      </xdr:style>
+      <xdr:txBody>
+        <a:bodyPr vertOverflow="clip" horzOverflow="clip" wrap="square" rtlCol="0" anchor="t"/>
+        <a:lstStyle/>
+        <a:p>
+          <a:r>
+            <a:rPr lang="en-US" sz="1100"/>
+            <a:t>If you add want to</a:t>
+          </a:r>
+          <a:r>
+            <a:rPr lang="en-US" sz="1100" baseline="0"/>
+            <a:t> add n</a:t>
+          </a:r>
+          <a:r>
+            <a:rPr lang="en-US" sz="1100"/>
+            <a:t>ew Plotting names, for</a:t>
+          </a:r>
+          <a:r>
+            <a:rPr lang="en-US" sz="1100" baseline="0"/>
+            <a:t> example 'fossil fuels' then you would add that in the related sheet, which would be one of ['sectors_plotting', 'fuels_plotting', 'transformation_sector_mappings'] and it's associated fuels (which for fossil fuels would be a lot!). Then also, add it to colors dict, which is the color to use for that plotting name!</a:t>
+          </a:r>
+          <a:endParaRPr lang="en-US" sz="1100"/>
+        </a:p>
+      </xdr:txBody>
+    </xdr:sp>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>18</xdr:col>
+      <xdr:colOff>115166</xdr:colOff>
+      <xdr:row>2</xdr:row>
+      <xdr:rowOff>121227</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>23</xdr:col>
+      <xdr:colOff>29441</xdr:colOff>
+      <xdr:row>16</xdr:row>
+      <xdr:rowOff>73602</xdr:rowOff>
+    </xdr:to>
+    <xdr:sp macro="" textlink="">
+      <xdr:nvSpPr>
+        <xdr:cNvPr id="5" name="TextBox 4">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{669B984E-C78F-47D6-9826-A8B2D57D94FA}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvSpPr txBox="1"/>
+      </xdr:nvSpPr>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="27766241" y="502227"/>
+          <a:ext cx="2962275" cy="2619375"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+        <a:solidFill>
+          <a:schemeClr val="accent2"/>
+        </a:solidFill>
+        <a:ln w="9525" cmpd="sng">
+          <a:solidFill>
+            <a:schemeClr val="lt1">
+              <a:shade val="50000"/>
+            </a:schemeClr>
+          </a:solidFill>
+        </a:ln>
+      </xdr:spPr>
+      <xdr:style>
+        <a:lnRef idx="0">
+          <a:scrgbClr r="0" g="0" b="0"/>
+        </a:lnRef>
+        <a:fillRef idx="0">
+          <a:scrgbClr r="0" g="0" b="0"/>
+        </a:fillRef>
+        <a:effectRef idx="0">
+          <a:scrgbClr r="0" g="0" b="0"/>
+        </a:effectRef>
+        <a:fontRef idx="minor">
+          <a:schemeClr val="dk1"/>
+        </a:fontRef>
+      </xdr:style>
+      <xdr:txBody>
+        <a:bodyPr vertOverflow="clip" horzOverflow="clip" wrap="square" rtlCol="0" anchor="t"/>
+        <a:lstStyle/>
+        <a:p>
+          <a:r>
+            <a:rPr lang="en-US" sz="1100"/>
+            <a:t>If you add want to</a:t>
+          </a:r>
+          <a:r>
+            <a:rPr lang="en-US" sz="1100" baseline="0"/>
+            <a:t> add n</a:t>
+          </a:r>
+          <a:r>
+            <a:rPr lang="en-US" sz="1100"/>
+            <a:t>ew Plotting names, for</a:t>
+          </a:r>
+          <a:r>
+            <a:rPr lang="en-US" sz="1100" baseline="0"/>
+            <a:t> example 'fossil fuels' then you would add that in the related sheet, which would be one of ['sectors_plotting', 'fuels_plotting', 'transformation_sector_mappings'] and it's associated fuels (which for fossil fuels would be a lot!). Then also, add it to colors dict, which is the color to use for that plotting name!</a:t>
+          </a:r>
+          <a:endParaRPr lang="en-US" sz="1100"/>
+        </a:p>
+      </xdr:txBody>
+    </xdr:sp>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
 </xdr:wsDr>
 </file>
 
@@ -14401,7 +14567,7 @@
   </sheetPr>
   <dimension ref="A1:I249"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="C195" sqref="C195"/>
     </sheetView>
   </sheetViews>
@@ -21474,7 +21640,7 @@
   </sheetPr>
   <dimension ref="A1:W89"/>
   <sheetViews>
-    <sheetView topLeftCell="A44" zoomScaleNormal="100" workbookViewId="0">
+    <sheetView tabSelected="1" topLeftCell="A60" zoomScaleNormal="100" workbookViewId="0">
       <selection activeCell="G78" sqref="G78"/>
     </sheetView>
   </sheetViews>
@@ -23027,12 +23193,9 @@
         <v>355</v>
       </c>
       <c r="K31" t="s">
-        <v>356</v>
+        <v>357</v>
       </c>
       <c r="L31" t="s">
-        <v>357</v>
-      </c>
-      <c r="M31" t="s">
         <v>358</v>
       </c>
     </row>
@@ -23926,6 +24089,9 @@
       <c r="O49" t="s">
         <v>469</v>
       </c>
+      <c r="P49" t="s">
+        <v>356</v>
+      </c>
     </row>
     <row r="50" spans="1:22" x14ac:dyDescent="0.25">
       <c r="A50" t="s">
@@ -23973,6 +24139,9 @@
       <c r="O50" t="s">
         <v>469</v>
       </c>
+      <c r="P50" t="s">
+        <v>356</v>
+      </c>
     </row>
     <row r="51" spans="1:22" x14ac:dyDescent="0.25">
       <c r="A51" t="s">
@@ -24006,12 +24175,9 @@
         <v>355</v>
       </c>
       <c r="K51" t="s">
-        <v>356</v>
+        <v>357</v>
       </c>
       <c r="L51" t="s">
-        <v>357</v>
-      </c>
-      <c r="M51" t="s">
         <v>358</v>
       </c>
     </row>
@@ -24047,12 +24213,9 @@
         <v>355</v>
       </c>
       <c r="K52" t="s">
-        <v>356</v>
+        <v>357</v>
       </c>
       <c r="L52" t="s">
-        <v>357</v>
-      </c>
-      <c r="M52" t="s">
         <v>358</v>
       </c>
     </row>
@@ -25105,12 +25268,9 @@
         <v>355</v>
       </c>
       <c r="L74" t="s">
-        <v>356</v>
+        <v>357</v>
       </c>
       <c r="M74" t="s">
-        <v>357</v>
-      </c>
-      <c r="N74" t="s">
         <v>358</v>
       </c>
     </row>
@@ -25157,6 +25317,9 @@
       <c r="N75" t="s">
         <v>467</v>
       </c>
+      <c r="O75" t="s">
+        <v>356</v>
+      </c>
     </row>
     <row r="76" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A76" t="s">
@@ -25201,6 +25364,9 @@
       <c r="N76" t="s">
         <v>467</v>
       </c>
+      <c r="O76" t="s">
+        <v>356</v>
+      </c>
     </row>
     <row r="77" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A77" t="s">
@@ -25269,12 +25435,9 @@
         <v>355</v>
       </c>
       <c r="K78" t="s">
-        <v>356</v>
+        <v>357</v>
       </c>
       <c r="L78" t="s">
-        <v>357</v>
-      </c>
-      <c r="M78" t="s">
         <v>358</v>
       </c>
     </row>
@@ -25310,12 +25473,9 @@
         <v>355</v>
       </c>
       <c r="K79" t="s">
-        <v>356</v>
+        <v>357</v>
       </c>
       <c r="L79" t="s">
-        <v>357</v>
-      </c>
-      <c r="M79" t="s">
         <v>358</v>
       </c>
     </row>
@@ -25362,6 +25522,9 @@
       <c r="N80" t="s">
         <v>467</v>
       </c>
+      <c r="O80" t="s">
+        <v>356</v>
+      </c>
     </row>
     <row r="81" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A81" t="s">
@@ -25506,6 +25669,9 @@
       <c r="N83" t="s">
         <v>467</v>
       </c>
+      <c r="O83" t="s">
+        <v>356</v>
+      </c>
     </row>
     <row r="84" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A84" t="s">
@@ -25592,9 +25758,6 @@
         <v>355</v>
       </c>
       <c r="K85" t="s">
-        <v>356</v>
-      </c>
-      <c r="L85" t="s">
         <v>357</v>
       </c>
     </row>

</xml_diff>

<commit_message>
changed to hydrogen based fuels in power input
</commit_message>
<xml_diff>
--- a/config/master_config.xlsx
+++ b/config/master_config.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\hyuga.kasai\Documents\Github\9th_Visualization\9th_edition_visualisation\config\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{88E004B2-A43B-49A0-9E81-51A0DC121AC6}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{6B385639-CE67-4DA6-8D82-077D4731B663}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="22050" yWindow="-16395" windowWidth="29040" windowHeight="15720" tabRatio="844" firstSheet="2" activeTab="5" xr2:uid="{E1808A28-6E92-43AB-8411-89A0CBB0B83A}"/>
+    <workbookView xWindow="22050" yWindow="-16395" windowWidth="29040" windowHeight="15720" tabRatio="844" activeTab="5" xr2:uid="{E1808A28-6E92-43AB-8411-89A0CBB0B83A}"/>
   </bookViews>
   <sheets>
     <sheet name="9th_EBT_schema" sheetId="7" r:id="rId1"/>
@@ -9818,8 +9818,8 @@
   </sheetPr>
   <dimension ref="A1:D94"/>
   <sheetViews>
-    <sheetView topLeftCell="A67" workbookViewId="0">
-      <selection activeCell="B75" sqref="B75"/>
+    <sheetView topLeftCell="A35" workbookViewId="0">
+      <selection activeCell="A52" sqref="A52"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -10888,8 +10888,8 @@
   </sheetPr>
   <dimension ref="A1:C345"/>
   <sheetViews>
-    <sheetView topLeftCell="A331" workbookViewId="0">
-      <selection activeCell="A343" sqref="A343:A344"/>
+    <sheetView topLeftCell="A31" workbookViewId="0">
+      <selection activeCell="A52" sqref="A52:XFD52"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -21640,8 +21640,8 @@
   </sheetPr>
   <dimension ref="A1:W89"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A60" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="G78" sqref="G78"/>
+    <sheetView tabSelected="1" topLeftCell="I19" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="Q45" sqref="Q45"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -23697,10 +23697,10 @@
         <v>421</v>
       </c>
       <c r="Q40" t="s">
-        <v>437</v>
+        <v>716</v>
       </c>
       <c r="R40" t="s">
-        <v>435</v>
+        <v>436</v>
       </c>
     </row>
     <row r="41" spans="1:22" x14ac:dyDescent="0.25">

</xml_diff>